<commit_message>
Cleaned out trash (v0.12)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\OneDrive\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A4707C-315F-480A-B6E8-C1F3352CA811}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285A0BD-C9BE-420F-A9F6-4110112CC052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
   <si>
     <t>WBS</t>
   </si>
@@ -742,25 +742,34 @@
     <t>Begin Theory for Structural Framework</t>
   </si>
   <si>
-    <t>Create Framework for Qualitative Forecasts</t>
+    <t>Toy Structural Model &amp; Improve Nowcasts</t>
   </si>
   <si>
-    <t>Create Framework for Structural Equations</t>
+    <t>Add Nowcasts to Front Page</t>
   </si>
   <si>
-    <t>Create Forecasting Code &amp; Graphics</t>
+    <t>Improve Forecasts &amp; Fix Bugs</t>
+  </si>
+  <si>
+    <t>Update JS Depencies</t>
+  </si>
+  <si>
+    <t>Fix Asset Contagion Bug</t>
+  </si>
+  <si>
+    <t>Clean Nowcasts</t>
+  </si>
+  <si>
+    <t>Add Motivation Page</t>
   </si>
   <si>
     <t>Create IRF Code &amp; Graphics</t>
   </si>
   <si>
-    <t>Toy Structural Model &amp; Improve Nowcasts</t>
-  </si>
-  <si>
     <t>Add Nowcasted HPI, Other Variables</t>
   </si>
   <si>
-    <t>Add Nowcasts to Front Page</t>
+    <t>Create "Forecast Quality" Measure of Different Variables</t>
   </si>
 </sst>
 </file>
@@ -773,7 +782,7 @@
     <numFmt numFmtId="166" formatCode="d"/>
     <numFmt numFmtId="167" formatCode="d\ mmm\ yyyy"/>
   </numFmts>
-  <fonts count="44" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1053,6 +1062,13 @@
       <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="24">
@@ -1474,7 +1490,7 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -1708,6 +1724,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1755,7 +1774,82 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="80">
+  <dxfs count="90">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -2452,21 +2546,21 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="8"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="20"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>80433</xdr:rowOff>
     </xdr:to>
@@ -2863,13 +2957,13 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E91" sqref="E91"/>
+      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="38" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" style="6" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="6" bestFit="1" customWidth="1"/>
@@ -2969,13 +3063,13 @@
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
       <c r="L4" s="77" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 8</v>
+        <v>Week 20</v>
       </c>
       <c r="M4" s="78"/>
       <c r="N4" s="78"/>
@@ -2985,7 +3079,7 @@
       <c r="R4" s="79"/>
       <c r="S4" s="77" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 9</v>
+        <v>Week 21</v>
       </c>
       <c r="T4" s="78"/>
       <c r="U4" s="78"/>
@@ -2995,7 +3089,7 @@
       <c r="Y4" s="79"/>
       <c r="Z4" s="77" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 10</v>
+        <v>Week 22</v>
       </c>
       <c r="AA4" s="78"/>
       <c r="AB4" s="78"/>
@@ -3005,7 +3099,7 @@
       <c r="AF4" s="79"/>
       <c r="AG4" s="77" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 11</v>
+        <v>Week 23</v>
       </c>
       <c r="AH4" s="78"/>
       <c r="AI4" s="78"/>
@@ -3015,7 +3109,7 @@
       <c r="AM4" s="79"/>
       <c r="AN4" s="77" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 12</v>
+        <v>Week 24</v>
       </c>
       <c r="AO4" s="78"/>
       <c r="AP4" s="78"/>
@@ -3025,7 +3119,7 @@
       <c r="AT4" s="79"/>
       <c r="AU4" s="77" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 13</v>
+        <v>Week 25</v>
       </c>
       <c r="AV4" s="78"/>
       <c r="AW4" s="78"/>
@@ -3035,7 +3129,7 @@
       <c r="BA4" s="79"/>
       <c r="BB4" s="77" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 14</v>
+        <v>Week 26</v>
       </c>
       <c r="BC4" s="78"/>
       <c r="BD4" s="78"/>
@@ -3045,7 +3139,7 @@
       <c r="BH4" s="79"/>
       <c r="BI4" s="77" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 15</v>
+        <v>Week 27</v>
       </c>
       <c r="BJ4" s="78"/>
       <c r="BK4" s="78"/>
@@ -3072,7 +3166,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="80">
         <f>L6</f>
-        <v>44242</v>
+        <v>44326</v>
       </c>
       <c r="M5" s="81"/>
       <c r="N5" s="81"/>
@@ -3082,7 +3176,7 @@
       <c r="R5" s="82"/>
       <c r="S5" s="80">
         <f>S6</f>
-        <v>44249</v>
+        <v>44333</v>
       </c>
       <c r="T5" s="81"/>
       <c r="U5" s="81"/>
@@ -3092,7 +3186,7 @@
       <c r="Y5" s="82"/>
       <c r="Z5" s="80">
         <f>Z6</f>
-        <v>44256</v>
+        <v>44340</v>
       </c>
       <c r="AA5" s="81"/>
       <c r="AB5" s="81"/>
@@ -3102,7 +3196,7 @@
       <c r="AF5" s="82"/>
       <c r="AG5" s="80">
         <f>AG6</f>
-        <v>44263</v>
+        <v>44347</v>
       </c>
       <c r="AH5" s="81"/>
       <c r="AI5" s="81"/>
@@ -3112,7 +3206,7 @@
       <c r="AM5" s="82"/>
       <c r="AN5" s="80">
         <f>AN6</f>
-        <v>44270</v>
+        <v>44354</v>
       </c>
       <c r="AO5" s="81"/>
       <c r="AP5" s="81"/>
@@ -3122,7 +3216,7 @@
       <c r="AT5" s="82"/>
       <c r="AU5" s="80">
         <f>AU6</f>
-        <v>44277</v>
+        <v>44361</v>
       </c>
       <c r="AV5" s="81"/>
       <c r="AW5" s="81"/>
@@ -3132,7 +3226,7 @@
       <c r="BA5" s="82"/>
       <c r="BB5" s="80">
         <f>BB6</f>
-        <v>44284</v>
+        <v>44368</v>
       </c>
       <c r="BC5" s="81"/>
       <c r="BD5" s="81"/>
@@ -3142,7 +3236,7 @@
       <c r="BH5" s="82"/>
       <c r="BI5" s="80">
         <f>BI6</f>
-        <v>44291</v>
+        <v>44375</v>
       </c>
       <c r="BJ5" s="81"/>
       <c r="BK5" s="81"/>
@@ -3165,227 +3259,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44242</v>
+        <v>44326</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44243</v>
+        <v>44327</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44244</v>
+        <v>44328</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44245</v>
+        <v>44329</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44246</v>
+        <v>44330</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44247</v>
+        <v>44331</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44248</v>
+        <v>44332</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44249</v>
+        <v>44333</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44250</v>
+        <v>44334</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44251</v>
+        <v>44335</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44252</v>
+        <v>44336</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44253</v>
+        <v>44337</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44254</v>
+        <v>44338</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44255</v>
+        <v>44339</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44256</v>
+        <v>44340</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44257</v>
+        <v>44341</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44258</v>
+        <v>44342</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44259</v>
+        <v>44343</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44260</v>
+        <v>44344</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44261</v>
+        <v>44345</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44262</v>
+        <v>44346</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44263</v>
+        <v>44347</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44264</v>
+        <v>44348</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44265</v>
+        <v>44349</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44266</v>
+        <v>44350</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44267</v>
+        <v>44351</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44268</v>
+        <v>44352</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44269</v>
+        <v>44353</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44270</v>
+        <v>44354</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44271</v>
+        <v>44355</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44272</v>
+        <v>44356</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44273</v>
+        <v>44357</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44274</v>
+        <v>44358</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44275</v>
+        <v>44359</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44276</v>
+        <v>44360</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44277</v>
+        <v>44361</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44278</v>
+        <v>44362</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44279</v>
+        <v>44363</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44280</v>
+        <v>44364</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44281</v>
+        <v>44365</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44282</v>
+        <v>44366</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44283</v>
+        <v>44367</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44284</v>
+        <v>44368</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44285</v>
+        <v>44369</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44286</v>
+        <v>44370</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44287</v>
+        <v>44371</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44288</v>
+        <v>44372</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44289</v>
+        <v>44373</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44290</v>
+        <v>44374</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44291</v>
+        <v>44375</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44292</v>
+        <v>44376</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44293</v>
+        <v>44377</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44294</v>
+        <v>44378</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44295</v>
+        <v>44379</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44296</v>
+        <v>44380</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44297</v>
+        <v>44381</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8307,7 +8401,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A94" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A95" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10039,7 +10133,7 @@
         <v>7</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D85" s="19"/>
       <c r="E85" s="19"/>
@@ -10196,110 +10290,111 @@
       <c r="BN86" s="46"/>
       <c r="BO86" s="46"/>
     </row>
-    <row r="87" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>7.2</v>
-      </c>
-      <c r="B87" s="65" t="s">
-        <v>104</v>
-      </c>
-      <c r="D87" s="66"/>
-      <c r="E87" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F87" s="42">
-        <v>44286</v>
-      </c>
-      <c r="G87" s="43">
-        <v>44291</v>
-      </c>
-      <c r="H87" s="25"/>
-      <c r="I87" s="26">
-        <v>0</v>
-      </c>
-      <c r="J87" s="27"/>
-      <c r="K87" s="40"/>
-      <c r="L87" s="46"/>
-      <c r="M87" s="46"/>
-      <c r="N87" s="46"/>
-      <c r="O87" s="46"/>
-      <c r="P87" s="46"/>
-      <c r="Q87" s="46"/>
-      <c r="R87" s="46"/>
-      <c r="S87" s="46"/>
-      <c r="T87" s="46"/>
-      <c r="U87" s="46"/>
-      <c r="V87" s="46"/>
-      <c r="W87" s="46"/>
-      <c r="X87" s="46"/>
-      <c r="Y87" s="46"/>
-      <c r="Z87" s="46"/>
-      <c r="AA87" s="46"/>
-      <c r="AB87" s="46"/>
-      <c r="AC87" s="46"/>
-      <c r="AD87" s="46"/>
-      <c r="AE87" s="46"/>
-      <c r="AF87" s="46"/>
-      <c r="AG87" s="46"/>
-      <c r="AH87" s="46"/>
-      <c r="AI87" s="46"/>
-      <c r="AJ87" s="46"/>
-      <c r="AK87" s="46"/>
-      <c r="AL87" s="46"/>
-      <c r="AM87" s="46"/>
-      <c r="AN87" s="46"/>
-      <c r="AO87" s="46"/>
-      <c r="AP87" s="46"/>
-      <c r="AQ87" s="46"/>
-      <c r="AR87" s="46"/>
-      <c r="AS87" s="46"/>
-      <c r="AT87" s="46"/>
-      <c r="AU87" s="46"/>
-      <c r="AV87" s="46"/>
-      <c r="AW87" s="46"/>
-      <c r="AX87" s="46"/>
-      <c r="AY87" s="46"/>
-      <c r="AZ87" s="46"/>
-      <c r="BA87" s="46"/>
-      <c r="BB87" s="46"/>
-      <c r="BC87" s="46"/>
-      <c r="BD87" s="46"/>
-      <c r="BE87" s="46"/>
-      <c r="BF87" s="46"/>
-      <c r="BG87" s="46"/>
-      <c r="BH87" s="46"/>
-      <c r="BI87" s="46"/>
-      <c r="BJ87" s="46"/>
-      <c r="BK87" s="46"/>
-      <c r="BL87" s="46"/>
-      <c r="BM87" s="46"/>
-      <c r="BN87" s="46"/>
-      <c r="BO87" s="46"/>
+    <row r="87" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>8</v>
+      </c>
+      <c r="B87" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D87" s="19"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44" t="str">
+        <f t="shared" ref="G87" si="14">IF(ISBLANK(F87)," - ",IF(H87=0,F87,F87+H87-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H87" s="20"/>
+      <c r="I87" s="21"/>
+      <c r="J87" s="22" t="str">
+        <f t="shared" ref="J87:J88" si="15">IF(OR(G87=0,F87=0)," - ",NETWORKDAYS(F87,G87))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K87" s="41"/>
+      <c r="L87" s="48"/>
+      <c r="M87" s="48"/>
+      <c r="N87" s="48"/>
+      <c r="O87" s="48"/>
+      <c r="P87" s="48"/>
+      <c r="Q87" s="48"/>
+      <c r="R87" s="48"/>
+      <c r="S87" s="48"/>
+      <c r="T87" s="48"/>
+      <c r="U87" s="48"/>
+      <c r="V87" s="48"/>
+      <c r="W87" s="48"/>
+      <c r="X87" s="48"/>
+      <c r="Y87" s="48"/>
+      <c r="Z87" s="48"/>
+      <c r="AA87" s="48"/>
+      <c r="AB87" s="48"/>
+      <c r="AC87" s="48"/>
+      <c r="AD87" s="48"/>
+      <c r="AE87" s="48"/>
+      <c r="AF87" s="48"/>
+      <c r="AG87" s="48"/>
+      <c r="AH87" s="48"/>
+      <c r="AI87" s="48"/>
+      <c r="AJ87" s="48"/>
+      <c r="AK87" s="48"/>
+      <c r="AL87" s="48"/>
+      <c r="AM87" s="48"/>
+      <c r="AN87" s="48"/>
+      <c r="AO87" s="48"/>
+      <c r="AP87" s="48"/>
+      <c r="AQ87" s="48"/>
+      <c r="AR87" s="48"/>
+      <c r="AS87" s="48"/>
+      <c r="AT87" s="48"/>
+      <c r="AU87" s="48"/>
+      <c r="AV87" s="48"/>
+      <c r="AW87" s="48"/>
+      <c r="AX87" s="48"/>
+      <c r="AY87" s="48"/>
+      <c r="AZ87" s="48"/>
+      <c r="BA87" s="48"/>
+      <c r="BB87" s="48"/>
+      <c r="BC87" s="48"/>
+      <c r="BD87" s="48"/>
+      <c r="BE87" s="48"/>
+      <c r="BF87" s="48"/>
+      <c r="BG87" s="48"/>
+      <c r="BH87" s="48"/>
+      <c r="BI87" s="48"/>
+      <c r="BJ87" s="48"/>
+      <c r="BK87" s="48"/>
+      <c r="BL87" s="48"/>
+      <c r="BM87" s="48"/>
+      <c r="BN87" s="48"/>
+      <c r="BO87" s="48"/>
     </row>
     <row r="88" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.3</v>
+        <v>8.1</v>
       </c>
       <c r="B88" s="65" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D88" s="66"/>
       <c r="E88" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F88" s="42">
-        <v>44285</v>
+        <v>44325</v>
       </c>
       <c r="G88" s="43">
-        <v>44286</v>
+        <v>44328</v>
       </c>
       <c r="H88" s="25"/>
       <c r="I88" s="26">
-        <v>0.5</v>
-      </c>
-      <c r="J88" s="27"/>
+        <v>1</v>
+      </c>
+      <c r="J88" s="27">
+        <f t="shared" si="15"/>
+        <v>3</v>
+      </c>
       <c r="K88" s="40"/>
       <c r="L88" s="46"/>
       <c r="M88" s="46"/>
@@ -10361,17 +10456,17 @@
     <row r="89" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.4</v>
+        <v>8.2</v>
       </c>
       <c r="B89" s="65" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D89" s="66"/>
       <c r="E89" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F89" s="42">
-        <v>44286</v>
+        <v>44326</v>
       </c>
       <c r="G89" s="43"/>
       <c r="H89" s="25"/>
@@ -10438,17 +10533,17 @@
     <row r="90" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.5</v>
+        <v>8.3</v>
       </c>
       <c r="B90" s="65" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D90" s="66"/>
       <c r="E90" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F90" s="42">
-        <v>44286</v>
+        <v>44336</v>
       </c>
       <c r="G90" s="43"/>
       <c r="H90" s="25"/>
@@ -10515,17 +10610,17 @@
     <row r="91" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.6</v>
+        <v>8.4</v>
       </c>
       <c r="B91" s="65" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D91" s="70"/>
       <c r="E91" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F91" s="42">
-        <v>44286</v>
+        <v>44336</v>
       </c>
       <c r="G91" s="43"/>
       <c r="H91" s="25"/>
@@ -10592,17 +10687,17 @@
     <row r="92" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.7</v>
+        <v>8.5</v>
       </c>
       <c r="B92" s="65" t="s">
         <v>110</v>
       </c>
       <c r="D92" s="70"/>
       <c r="E92" s="66" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F92" s="42">
-        <v>44286</v>
+        <v>44338</v>
       </c>
       <c r="G92" s="43"/>
       <c r="H92" s="25"/>
@@ -10669,12 +10764,18 @@
     <row r="93" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.8</v>
-      </c>
-      <c r="B93" s="65"/>
+        <v>8.6</v>
+      </c>
+      <c r="B93" s="65" t="s">
+        <v>111</v>
+      </c>
       <c r="D93" s="70"/>
-      <c r="E93" s="66"/>
-      <c r="F93" s="42"/>
+      <c r="E93" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F93" s="42">
+        <v>44348</v>
+      </c>
       <c r="G93" s="43"/>
       <c r="H93" s="25"/>
       <c r="I93" s="26"/>
@@ -10740,12 +10841,18 @@
     <row r="94" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>7.9</v>
-      </c>
-      <c r="B94" s="65"/>
+        <v>8.7</v>
+      </c>
+      <c r="B94" s="65" t="s">
+        <v>112</v>
+      </c>
       <c r="D94" s="70"/>
-      <c r="E94" s="66"/>
-      <c r="F94" s="42"/>
+      <c r="E94" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F94" s="42">
+        <v>44348</v>
+      </c>
       <c r="G94" s="43"/>
       <c r="H94" s="25"/>
       <c r="I94" s="26"/>
@@ -10809,11 +10916,20 @@
       <c r="BO94" s="46"/>
     </row>
     <row r="95" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="23"/>
-      <c r="B95" s="65"/>
+      <c r="A95" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.8</v>
+      </c>
+      <c r="B95" s="86" t="s">
+        <v>113</v>
+      </c>
       <c r="D95" s="66"/>
-      <c r="E95" s="66"/>
-      <c r="F95" s="42"/>
+      <c r="E95" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F95" s="42">
+        <v>44348</v>
+      </c>
       <c r="G95" s="43"/>
       <c r="H95" s="25"/>
       <c r="I95" s="26"/>
@@ -13281,7 +13397,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73">
-    <cfRule type="dataBar" priority="170">
+    <cfRule type="dataBar" priority="181">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13295,66 +13411,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="79" priority="213">
+    <cfRule type="expression" dxfId="89" priority="224">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L95:BO97 M98:BN103 BO101:BO103 L104:BO106 M107:BN112 BO110:BO112 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L85:BO89 M90:BN94 BO93:BO94">
-    <cfRule type="expression" dxfId="78" priority="216">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L95:BO97 M98:BN103 BO101:BO103 L104:BO106 M107:BN112 BO110:BO112 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L85:BO86 M90:BN94 BO93:BO94 L89:BO89">
+    <cfRule type="expression" dxfId="88" priority="227">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="77" priority="217">
+    <cfRule type="expression" dxfId="87" priority="228">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO62">
-    <cfRule type="expression" dxfId="76" priority="176">
+    <cfRule type="expression" dxfId="86" priority="187">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="75" priority="166">
+    <cfRule type="expression" dxfId="85" priority="177">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E73 E131:E1048576">
-    <cfRule type="cellIs" dxfId="74" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="168" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="170" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="172" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="173" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="174" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="175" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="67" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="169" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="66" priority="222">
+    <cfRule type="expression" dxfId="76" priority="233">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="65" priority="223">
+    <cfRule type="expression" dxfId="75" priority="234">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I84">
-    <cfRule type="dataBar" priority="152">
+    <cfRule type="dataBar" priority="163">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13368,51 +13484,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="64" priority="153">
+    <cfRule type="expression" dxfId="74" priority="164">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="154">
+    <cfRule type="expression" dxfId="73" priority="165">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="62" priority="151">
+    <cfRule type="expression" dxfId="72" priority="162">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="61" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="155" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="156" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="157" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="158" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="159" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="160" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="161" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="54" priority="155">
+    <cfRule type="expression" dxfId="64" priority="166">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="156">
+    <cfRule type="expression" dxfId="63" priority="167">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I95:I103">
-    <cfRule type="dataBar" priority="61">
+    <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13426,43 +13542,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L95:BO103">
-    <cfRule type="expression" dxfId="52" priority="60">
+    <cfRule type="expression" dxfId="62" priority="71">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95:E103">
-    <cfRule type="cellIs" dxfId="51" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="64" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="65" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="67" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="68" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="69" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="70" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L98:BO103">
-    <cfRule type="expression" dxfId="44" priority="64">
+    <cfRule type="expression" dxfId="54" priority="75">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="65">
+    <cfRule type="expression" dxfId="53" priority="76">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I104:I112">
-    <cfRule type="dataBar" priority="48">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13476,43 +13592,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L104:BO112">
-    <cfRule type="expression" dxfId="42" priority="47">
+    <cfRule type="expression" dxfId="52" priority="58">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E104:E112">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L107:BO112">
-    <cfRule type="expression" dxfId="34" priority="51">
+    <cfRule type="expression" dxfId="44" priority="62">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="52">
+    <cfRule type="expression" dxfId="43" priority="63">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I113:I121">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13526,43 +13642,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L113:BO121">
-    <cfRule type="expression" dxfId="32" priority="34">
+    <cfRule type="expression" dxfId="42" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E113:E121">
-    <cfRule type="cellIs" dxfId="31" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="38" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="42" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L116:BO121">
-    <cfRule type="expression" dxfId="24" priority="38">
+    <cfRule type="expression" dxfId="34" priority="49">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="39">
+    <cfRule type="expression" dxfId="33" priority="50">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I122:I130">
-    <cfRule type="dataBar" priority="22">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13576,43 +13692,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L122:BO130">
-    <cfRule type="expression" dxfId="22" priority="21">
+    <cfRule type="expression" dxfId="32" priority="32">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E122:E130">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L125:BO130">
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="24" priority="36">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="26">
+    <cfRule type="expression" dxfId="23" priority="37">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I85:I94">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="I85:I86 I89:I94">
+    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13625,40 +13741,90 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L85:BO94">
-    <cfRule type="expression" dxfId="12" priority="8">
+  <conditionalFormatting sqref="L85:BO86 L89:BO94">
+    <cfRule type="expression" dxfId="22" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E94">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+  <conditionalFormatting sqref="E85:E86 E89:E94">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L90:BO94">
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="14" priority="23">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="13">
+    <cfRule type="expression" dxfId="13" priority="24">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO88">
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87:I88">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO88">
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E87:E88">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+      <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -13807,7 +13973,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I85:I94</xm:sqref>
+          <xm:sqref>I85:I86 I89:I94</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I87:I88</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added release dates import (v0.13)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9285A0BD-C9BE-420F-A9F6-4110112CC052}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15C62A4-9DBE-4E08-9604-8FFA4E12BC08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="116">
   <si>
     <t>WBS</t>
   </si>
@@ -751,15 +751,6 @@
     <t>Improve Forecasts &amp; Fix Bugs</t>
   </si>
   <si>
-    <t>Update JS Depencies</t>
-  </si>
-  <si>
-    <t>Fix Asset Contagion Bug</t>
-  </si>
-  <si>
-    <t>Clean Nowcasts</t>
-  </si>
-  <si>
     <t>Add Motivation Page</t>
   </si>
   <si>
@@ -770,6 +761,21 @@
   </si>
   <si>
     <t>Create "Forecast Quality" Measure of Different Variables</t>
+  </si>
+  <si>
+    <t>Update JS Dependencies</t>
+  </si>
+  <si>
+    <t>Improve Nowcast Quality</t>
+  </si>
+  <si>
+    <t>Fix Treasury Yield Forecasts</t>
+  </si>
+  <si>
+    <t>Fix Asset Contagion</t>
+  </si>
+  <si>
+    <t>Scrape &amp; Store Nowcast Releases</t>
   </si>
 </sst>
 </file>
@@ -1695,6 +1701,16 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1704,6 +1720,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1712,20 +1732,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1774,7 +1780,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="88">
     <dxf>
       <border>
         <left style="thin">
@@ -1861,20 +1867,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2953,11 +2945,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO130"/>
+  <dimension ref="A1:BO132"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
+      <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2987,27 +2979,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3052,12 +3044,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3067,183 +3059,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="77" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="77" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="77" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="78"/>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="77" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="78"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="77" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="77" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="78"/>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="77" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="78"/>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="77" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="78"/>
-      <c r="BM4" s="78"/>
-      <c r="BN4" s="78"/>
-      <c r="BO4" s="79"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="80">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="80">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="80">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="82"/>
-      <c r="AG5" s="80">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="82"/>
-      <c r="AN5" s="80">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AT5" s="82"/>
-      <c r="AU5" s="80">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="82"/>
-      <c r="BB5" s="80">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BH5" s="82"/>
-      <c r="BI5" s="80">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="82"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8401,7 +8393,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A95" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A97" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10375,17 +10367,17 @@
         <v>8.1</v>
       </c>
       <c r="B88" s="65" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="D88" s="66"/>
       <c r="E88" s="66" t="s">
         <v>69</v>
       </c>
       <c r="F88" s="42">
-        <v>44325</v>
+        <v>44323</v>
       </c>
       <c r="G88" s="43">
-        <v>44328</v>
+        <v>44324</v>
       </c>
       <c r="H88" s="25"/>
       <c r="I88" s="26">
@@ -10393,7 +10385,7 @@
       </c>
       <c r="J88" s="27">
         <f t="shared" si="15"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K88" s="40"/>
       <c r="L88" s="46"/>
@@ -10459,14 +10451,14 @@
         <v>8.2</v>
       </c>
       <c r="B89" s="65" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D89" s="66"/>
       <c r="E89" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F89" s="42">
-        <v>44326</v>
+        <v>44324</v>
       </c>
       <c r="G89" s="43"/>
       <c r="H89" s="25"/>
@@ -10536,18 +10528,22 @@
         <v>8.3</v>
       </c>
       <c r="B90" s="65" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D90" s="66"/>
       <c r="E90" s="66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F90" s="42">
-        <v>44336</v>
-      </c>
-      <c r="G90" s="43"/>
+        <v>44324</v>
+      </c>
+      <c r="G90" s="43">
+        <v>44324</v>
+      </c>
       <c r="H90" s="25"/>
-      <c r="I90" s="26"/>
+      <c r="I90" s="26">
+        <v>1</v>
+      </c>
       <c r="J90" s="27"/>
       <c r="K90" s="40"/>
       <c r="L90" s="46"/>
@@ -10613,15 +10609,13 @@
         <v>8.4</v>
       </c>
       <c r="B91" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D91" s="70"/>
+        <v>113</v>
+      </c>
+      <c r="D91" s="66"/>
       <c r="E91" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F91" s="42">
-        <v>44336</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F91" s="42"/>
       <c r="G91" s="43"/>
       <c r="H91" s="25"/>
       <c r="I91" s="26"/>
@@ -10690,14 +10684,14 @@
         <v>8.5</v>
       </c>
       <c r="B92" s="65" t="s">
-        <v>110</v>
-      </c>
-      <c r="D92" s="70"/>
+        <v>114</v>
+      </c>
+      <c r="D92" s="66"/>
       <c r="E92" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F92" s="42">
-        <v>44338</v>
+        <v>44326</v>
       </c>
       <c r="G92" s="43"/>
       <c r="H92" s="25"/>
@@ -10767,14 +10761,14 @@
         <v>8.6</v>
       </c>
       <c r="B93" s="65" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D93" s="70"/>
       <c r="E93" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F93" s="42">
-        <v>44348</v>
+        <v>44336</v>
       </c>
       <c r="G93" s="43"/>
       <c r="H93" s="25"/>
@@ -10844,14 +10838,14 @@
         <v>8.7</v>
       </c>
       <c r="B94" s="65" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D94" s="70"/>
       <c r="E94" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F94" s="42">
-        <v>44348</v>
+        <v>44338</v>
       </c>
       <c r="G94" s="43"/>
       <c r="H94" s="25"/>
@@ -10920,10 +10914,10 @@
         <f t="shared" si="9"/>
         <v>8.8</v>
       </c>
-      <c r="B95" s="86" t="s">
-        <v>113</v>
-      </c>
-      <c r="D95" s="66"/>
+      <c r="B95" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D95" s="70"/>
       <c r="E95" s="66" t="s">
         <v>67</v>
       </c>
@@ -10993,11 +10987,20 @@
       <c r="BO95" s="46"/>
     </row>
     <row r="96" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="23"/>
-      <c r="B96" s="65"/>
-      <c r="D96" s="66"/>
-      <c r="E96" s="66"/>
-      <c r="F96" s="42"/>
+      <c r="A96" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.9</v>
+      </c>
+      <c r="B96" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D96" s="70"/>
+      <c r="E96" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F96" s="42">
+        <v>44348</v>
+      </c>
       <c r="G96" s="43"/>
       <c r="H96" s="25"/>
       <c r="I96" s="26"/>
@@ -11061,11 +11064,20 @@
       <c r="BO96" s="46"/>
     </row>
     <row r="97" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="23"/>
-      <c r="B97" s="65"/>
+      <c r="A97" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.10</v>
+      </c>
+      <c r="B97" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D97" s="66"/>
-      <c r="E97" s="66"/>
-      <c r="F97" s="42"/>
+      <c r="E97" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F97" s="42">
+        <v>44348</v>
+      </c>
       <c r="G97" s="43"/>
       <c r="H97" s="25"/>
       <c r="I97" s="26"/>
@@ -11199,7 +11211,7 @@
     <row r="99" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="23"/>
       <c r="B99" s="65"/>
-      <c r="D99" s="70"/>
+      <c r="D99" s="66"/>
       <c r="E99" s="66"/>
       <c r="F99" s="42"/>
       <c r="G99" s="43"/>
@@ -11267,7 +11279,7 @@
     <row r="100" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="23"/>
       <c r="B100" s="65"/>
-      <c r="D100" s="70"/>
+      <c r="D100" s="66"/>
       <c r="E100" s="66"/>
       <c r="F100" s="42"/>
       <c r="G100" s="43"/>
@@ -11539,7 +11551,7 @@
     <row r="104" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="23"/>
       <c r="B104" s="65"/>
-      <c r="D104" s="66"/>
+      <c r="D104" s="70"/>
       <c r="E104" s="66"/>
       <c r="F104" s="42"/>
       <c r="G104" s="43"/>
@@ -11607,7 +11619,7 @@
     <row r="105" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="23"/>
       <c r="B105" s="65"/>
-      <c r="D105" s="66"/>
+      <c r="D105" s="70"/>
       <c r="E105" s="66"/>
       <c r="F105" s="42"/>
       <c r="G105" s="43"/>
@@ -11811,7 +11823,7 @@
     <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="23"/>
       <c r="B108" s="65"/>
-      <c r="D108" s="70"/>
+      <c r="D108" s="66"/>
       <c r="E108" s="66"/>
       <c r="F108" s="42"/>
       <c r="G108" s="43"/>
@@ -11879,7 +11891,7 @@
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="23"/>
       <c r="B109" s="65"/>
-      <c r="D109" s="70"/>
+      <c r="D109" s="66"/>
       <c r="E109" s="66"/>
       <c r="F109" s="42"/>
       <c r="G109" s="43"/>
@@ -12151,7 +12163,7 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23"/>
       <c r="B113" s="65"/>
-      <c r="D113" s="66"/>
+      <c r="D113" s="70"/>
       <c r="E113" s="66"/>
       <c r="F113" s="42"/>
       <c r="G113" s="43"/>
@@ -12219,7 +12231,7 @@
     <row r="114" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="23"/>
       <c r="B114" s="65"/>
-      <c r="D114" s="66"/>
+      <c r="D114" s="70"/>
       <c r="E114" s="66"/>
       <c r="F114" s="42"/>
       <c r="G114" s="43"/>
@@ -12423,7 +12435,7 @@
     <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="23"/>
       <c r="B117" s="65"/>
-      <c r="D117" s="70"/>
+      <c r="D117" s="66"/>
       <c r="E117" s="66"/>
       <c r="F117" s="42"/>
       <c r="G117" s="43"/>
@@ -12491,7 +12503,7 @@
     <row r="118" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="23"/>
       <c r="B118" s="65"/>
-      <c r="D118" s="70"/>
+      <c r="D118" s="66"/>
       <c r="E118" s="66"/>
       <c r="F118" s="42"/>
       <c r="G118" s="43"/>
@@ -12763,7 +12775,7 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
       <c r="B122" s="65"/>
-      <c r="D122" s="66"/>
+      <c r="D122" s="70"/>
       <c r="E122" s="66"/>
       <c r="F122" s="42"/>
       <c r="G122" s="43"/>
@@ -12831,7 +12843,7 @@
     <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="23"/>
       <c r="B123" s="65"/>
-      <c r="D123" s="66"/>
+      <c r="D123" s="70"/>
       <c r="E123" s="66"/>
       <c r="F123" s="42"/>
       <c r="G123" s="43"/>
@@ -13035,7 +13047,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="70"/>
+      <c r="D126" s="66"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -13103,7 +13115,7 @@
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23"/>
       <c r="B127" s="65"/>
-      <c r="D127" s="70"/>
+      <c r="D127" s="66"/>
       <c r="E127" s="66"/>
       <c r="F127" s="42"/>
       <c r="G127" s="43"/>
@@ -13372,18 +13384,145 @@
       <c r="BN130" s="46"/>
       <c r="BO130" s="46"/>
     </row>
+    <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="23"/>
+      <c r="B131" s="65"/>
+      <c r="D131" s="70"/>
+      <c r="E131" s="66"/>
+      <c r="F131" s="42"/>
+      <c r="G131" s="43"/>
+      <c r="H131" s="25"/>
+      <c r="I131" s="26"/>
+      <c r="J131" s="27"/>
+      <c r="K131" s="40"/>
+      <c r="L131" s="46"/>
+      <c r="M131" s="46"/>
+      <c r="N131" s="46"/>
+      <c r="O131" s="46"/>
+      <c r="P131" s="46"/>
+      <c r="Q131" s="46"/>
+      <c r="R131" s="46"/>
+      <c r="S131" s="46"/>
+      <c r="T131" s="46"/>
+      <c r="U131" s="46"/>
+      <c r="V131" s="46"/>
+      <c r="W131" s="46"/>
+      <c r="X131" s="46"/>
+      <c r="Y131" s="46"/>
+      <c r="Z131" s="46"/>
+      <c r="AA131" s="46"/>
+      <c r="AB131" s="46"/>
+      <c r="AC131" s="46"/>
+      <c r="AD131" s="46"/>
+      <c r="AE131" s="46"/>
+      <c r="AF131" s="46"/>
+      <c r="AG131" s="46"/>
+      <c r="AH131" s="46"/>
+      <c r="AI131" s="46"/>
+      <c r="AJ131" s="46"/>
+      <c r="AK131" s="46"/>
+      <c r="AL131" s="46"/>
+      <c r="AM131" s="46"/>
+      <c r="AN131" s="46"/>
+      <c r="AO131" s="46"/>
+      <c r="AP131" s="46"/>
+      <c r="AQ131" s="46"/>
+      <c r="AR131" s="46"/>
+      <c r="AS131" s="46"/>
+      <c r="AT131" s="46"/>
+      <c r="AU131" s="46"/>
+      <c r="AV131" s="46"/>
+      <c r="AW131" s="46"/>
+      <c r="AX131" s="46"/>
+      <c r="AY131" s="46"/>
+      <c r="AZ131" s="46"/>
+      <c r="BA131" s="46"/>
+      <c r="BB131" s="46"/>
+      <c r="BC131" s="46"/>
+      <c r="BD131" s="46"/>
+      <c r="BE131" s="46"/>
+      <c r="BF131" s="46"/>
+      <c r="BG131" s="46"/>
+      <c r="BH131" s="46"/>
+      <c r="BI131" s="46"/>
+      <c r="BJ131" s="46"/>
+      <c r="BK131" s="46"/>
+      <c r="BL131" s="46"/>
+      <c r="BM131" s="46"/>
+      <c r="BN131" s="46"/>
+      <c r="BO131" s="46"/>
+    </row>
+    <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="23"/>
+      <c r="B132" s="65"/>
+      <c r="D132" s="70"/>
+      <c r="E132" s="66"/>
+      <c r="F132" s="42"/>
+      <c r="G132" s="43"/>
+      <c r="H132" s="25"/>
+      <c r="I132" s="26"/>
+      <c r="J132" s="27"/>
+      <c r="K132" s="40"/>
+      <c r="L132" s="46"/>
+      <c r="M132" s="46"/>
+      <c r="N132" s="46"/>
+      <c r="O132" s="46"/>
+      <c r="P132" s="46"/>
+      <c r="Q132" s="46"/>
+      <c r="R132" s="46"/>
+      <c r="S132" s="46"/>
+      <c r="T132" s="46"/>
+      <c r="U132" s="46"/>
+      <c r="V132" s="46"/>
+      <c r="W132" s="46"/>
+      <c r="X132" s="46"/>
+      <c r="Y132" s="46"/>
+      <c r="Z132" s="46"/>
+      <c r="AA132" s="46"/>
+      <c r="AB132" s="46"/>
+      <c r="AC132" s="46"/>
+      <c r="AD132" s="46"/>
+      <c r="AE132" s="46"/>
+      <c r="AF132" s="46"/>
+      <c r="AG132" s="46"/>
+      <c r="AH132" s="46"/>
+      <c r="AI132" s="46"/>
+      <c r="AJ132" s="46"/>
+      <c r="AK132" s="46"/>
+      <c r="AL132" s="46"/>
+      <c r="AM132" s="46"/>
+      <c r="AN132" s="46"/>
+      <c r="AO132" s="46"/>
+      <c r="AP132" s="46"/>
+      <c r="AQ132" s="46"/>
+      <c r="AR132" s="46"/>
+      <c r="AS132" s="46"/>
+      <c r="AT132" s="46"/>
+      <c r="AU132" s="46"/>
+      <c r="AV132" s="46"/>
+      <c r="AW132" s="46"/>
+      <c r="AX132" s="46"/>
+      <c r="AY132" s="46"/>
+      <c r="AZ132" s="46"/>
+      <c r="BA132" s="46"/>
+      <c r="BB132" s="46"/>
+      <c r="BC132" s="46"/>
+      <c r="BD132" s="46"/>
+      <c r="BE132" s="46"/>
+      <c r="BF132" s="46"/>
+      <c r="BG132" s="46"/>
+      <c r="BH132" s="46"/>
+      <c r="BI132" s="46"/>
+      <c r="BJ132" s="46"/>
+      <c r="BK132" s="46"/>
+      <c r="BL132" s="46"/>
+      <c r="BM132" s="46"/>
+      <c r="BN132" s="46"/>
+      <c r="BO132" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -13394,9 +13533,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73">
+  <conditionalFormatting sqref="I8:I73 I92:I96">
     <cfRule type="dataBar" priority="181">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13411,61 +13559,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="89" priority="224">
+    <cfRule type="expression" dxfId="87" priority="224">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L95:BO97 M98:BN103 BO101:BO103 L104:BO106 M107:BN112 BO110:BO112 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L85:BO86 M90:BN94 BO93:BO94 L89:BO89">
-    <cfRule type="expression" dxfId="88" priority="227">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L92:BO92 L97:BO99 M100:BN105 BO103:BO105 L106:BO108 M109:BN114 BO112:BO114 L115:BO117 M118:BN123 BO121:BO123 L124:BO126 M127:BN132 BO130:BO132 M93:BN96 BO95:BO96">
+    <cfRule type="expression" dxfId="86" priority="227">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="228">
+    <cfRule type="expression" dxfId="85" priority="228">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62">
-    <cfRule type="expression" dxfId="86" priority="187">
+  <conditionalFormatting sqref="L6:BO62 L92:BO96">
+    <cfRule type="expression" dxfId="84" priority="187">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="85" priority="177">
+    <cfRule type="expression" dxfId="83" priority="177">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E131:E1048576">
-    <cfRule type="cellIs" dxfId="84" priority="168" operator="equal">
+  <conditionalFormatting sqref="E1:E73 E133:E1048576 E92:E96">
+    <cfRule type="cellIs" dxfId="82" priority="168" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="170" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="171" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="172" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="173" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="174" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="175" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="77" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="169" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="76" priority="233">
+    <cfRule type="expression" dxfId="74" priority="233">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="234">
+    <cfRule type="expression" dxfId="73" priority="234">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13484,50 +13632,50 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="74" priority="164">
+    <cfRule type="expression" dxfId="72" priority="164">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="165">
+    <cfRule type="expression" dxfId="71" priority="165">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="72" priority="162">
+    <cfRule type="expression" dxfId="70" priority="162">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="71" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="155" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="156" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="157" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="158" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="159" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="160" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="161" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="64" priority="166">
+    <cfRule type="expression" dxfId="62" priority="166">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="167">
+    <cfRule type="expression" dxfId="61" priority="167">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I95:I103">
+  <conditionalFormatting sqref="I97:I105">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13541,43 +13689,43 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L95:BO103">
-    <cfRule type="expression" dxfId="62" priority="71">
+  <conditionalFormatting sqref="L97:BO105">
+    <cfRule type="expression" dxfId="60" priority="71">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95:E103">
-    <cfRule type="cellIs" dxfId="61" priority="64" operator="equal">
+  <conditionalFormatting sqref="E97:E105">
+    <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="68" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="70" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L98:BO103">
-    <cfRule type="expression" dxfId="54" priority="75">
+  <conditionalFormatting sqref="L100:BO105 L93:BO96">
+    <cfRule type="expression" dxfId="52" priority="75">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="76">
+    <cfRule type="expression" dxfId="51" priority="76">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I104:I112">
+  <conditionalFormatting sqref="I106:I114">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13591,43 +13739,43 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L104:BO112">
-    <cfRule type="expression" dxfId="52" priority="58">
+  <conditionalFormatting sqref="L106:BO114">
+    <cfRule type="expression" dxfId="50" priority="58">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E104:E112">
-    <cfRule type="cellIs" dxfId="51" priority="51" operator="equal">
+  <conditionalFormatting sqref="E106:E114">
+    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L107:BO112">
-    <cfRule type="expression" dxfId="44" priority="62">
+  <conditionalFormatting sqref="L109:BO114">
+    <cfRule type="expression" dxfId="42" priority="62">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="63">
+    <cfRule type="expression" dxfId="41" priority="63">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I113:I121">
+  <conditionalFormatting sqref="I115:I123">
     <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13641,43 +13789,43 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L113:BO121">
-    <cfRule type="expression" dxfId="42" priority="45">
+  <conditionalFormatting sqref="L115:BO123">
+    <cfRule type="expression" dxfId="40" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113:E121">
-    <cfRule type="cellIs" dxfId="41" priority="38" operator="equal">
+  <conditionalFormatting sqref="E115:E123">
+    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L116:BO121">
-    <cfRule type="expression" dxfId="34" priority="49">
+  <conditionalFormatting sqref="L118:BO123">
+    <cfRule type="expression" dxfId="32" priority="49">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="50">
+    <cfRule type="expression" dxfId="31" priority="50">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122:I130">
+  <conditionalFormatting sqref="I124:I132">
     <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13691,43 +13839,43 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L122:BO130">
-    <cfRule type="expression" dxfId="32" priority="32">
+  <conditionalFormatting sqref="L124:BO132">
+    <cfRule type="expression" dxfId="30" priority="32">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122:E130">
-    <cfRule type="cellIs" dxfId="31" priority="25" operator="equal">
+  <conditionalFormatting sqref="E124:E132">
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO130">
-    <cfRule type="expression" dxfId="24" priority="36">
+  <conditionalFormatting sqref="L127:BO132">
+    <cfRule type="expression" dxfId="22" priority="36">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="37">
+    <cfRule type="expression" dxfId="21" priority="37">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I85:I86 I89:I94">
+  <conditionalFormatting sqref="I85:I86">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13741,43 +13889,35 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L85:BO86 L89:BO94">
-    <cfRule type="expression" dxfId="22" priority="19">
+  <conditionalFormatting sqref="L85:BO86">
+    <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E86 E89:E94">
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+  <conditionalFormatting sqref="E85:E86">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L90:BO94">
-    <cfRule type="expression" dxfId="14" priority="23">
-      <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="24">
-      <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO88">
+  <conditionalFormatting sqref="L87:BO91">
     <cfRule type="expression" dxfId="12" priority="10">
       <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
     </cfRule>
@@ -13785,7 +13925,7 @@
       <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I88">
+  <conditionalFormatting sqref="I87:I91">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13799,12 +13939,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO88">
+  <conditionalFormatting sqref="L87:BO91">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E88">
+  <conditionalFormatting sqref="E87:E91">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13883,7 +14023,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73</xm:sqref>
+          <xm:sqref>I8:I73 I92:I96</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -13913,7 +14053,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I95:I103</xm:sqref>
+          <xm:sqref>I97:I105</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -13928,7 +14068,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I104:I112</xm:sqref>
+          <xm:sqref>I106:I114</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -13943,7 +14083,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I113:I121</xm:sqref>
+          <xm:sqref>I115:I123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -13958,7 +14098,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I122:I130</xm:sqref>
+          <xm:sqref>I124:I132</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -13973,7 +14113,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I85:I86 I89:I94</xm:sqref>
+          <xm:sqref>I85:I86</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}">
@@ -13988,7 +14128,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I87:I88</xm:sqref>
+          <xm:sqref>I87:I91</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Moved rundates in backtest to only weekdays
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A15C62A4-9DBE-4E08-9604-8FFA4E12BC08}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F016CA-0501-425F-9897-21B038FCF55B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31470" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="117">
   <si>
     <t>WBS</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>Scrape &amp; Store Nowcast Releases</t>
+  </si>
+  <si>
+    <t>Added Cleanup Code</t>
   </si>
 </sst>
 </file>
@@ -1704,13 +1707,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1720,10 +1716,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1732,6 +1724,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2945,11 +2948,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO132"/>
+  <dimension ref="A1:BO133"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G91" sqref="G91"/>
+      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2979,27 +2982,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3044,12 +3047,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3059,183 +3062,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8393,7 +8396,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A97" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A98" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10460,9 +10463,13 @@
       <c r="F89" s="42">
         <v>44324</v>
       </c>
-      <c r="G89" s="43"/>
+      <c r="G89" s="43">
+        <v>44324</v>
+      </c>
       <c r="H89" s="25"/>
-      <c r="I89" s="26"/>
+      <c r="I89" s="26">
+        <v>1</v>
+      </c>
       <c r="J89" s="27"/>
       <c r="K89" s="40"/>
       <c r="L89" s="46"/>
@@ -10609,16 +10616,22 @@
         <v>8.4</v>
       </c>
       <c r="B91" s="65" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D91" s="66"/>
       <c r="E91" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F91" s="42"/>
-      <c r="G91" s="43"/>
+      <c r="F91" s="42">
+        <v>44324</v>
+      </c>
+      <c r="G91" s="43">
+        <v>44324</v>
+      </c>
       <c r="H91" s="25"/>
-      <c r="I91" s="26"/>
+      <c r="I91" s="26">
+        <v>1</v>
+      </c>
       <c r="J91" s="27"/>
       <c r="K91" s="40"/>
       <c r="L91" s="46"/>
@@ -10684,15 +10697,13 @@
         <v>8.5</v>
       </c>
       <c r="B92" s="65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D92" s="66"/>
       <c r="E92" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F92" s="42">
-        <v>44326</v>
-      </c>
+      <c r="F92" s="42"/>
       <c r="G92" s="43"/>
       <c r="H92" s="25"/>
       <c r="I92" s="26"/>
@@ -10761,14 +10772,14 @@
         <v>8.6</v>
       </c>
       <c r="B93" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D93" s="70"/>
+        <v>114</v>
+      </c>
+      <c r="D93" s="66"/>
       <c r="E93" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F93" s="42">
-        <v>44336</v>
+        <v>44326</v>
       </c>
       <c r="G93" s="43"/>
       <c r="H93" s="25"/>
@@ -10838,14 +10849,14 @@
         <v>8.7</v>
       </c>
       <c r="B94" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D94" s="70"/>
       <c r="E94" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F94" s="42">
-        <v>44338</v>
+        <v>44336</v>
       </c>
       <c r="G94" s="43"/>
       <c r="H94" s="25"/>
@@ -10915,14 +10926,14 @@
         <v>8.8</v>
       </c>
       <c r="B95" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D95" s="70"/>
       <c r="E95" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F95" s="42">
-        <v>44348</v>
+        <v>44338</v>
       </c>
       <c r="G95" s="43"/>
       <c r="H95" s="25"/>
@@ -10992,7 +11003,7 @@
         <v>8.9</v>
       </c>
       <c r="B96" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D96" s="70"/>
       <c r="E96" s="66" t="s">
@@ -11068,10 +11079,10 @@
         <f t="shared" si="9"/>
         <v>8.10</v>
       </c>
-      <c r="B97" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D97" s="66"/>
+      <c r="B97" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D97" s="70"/>
       <c r="E97" s="66" t="s">
         <v>67</v>
       </c>
@@ -11141,11 +11152,20 @@
       <c r="BO97" s="46"/>
     </row>
     <row r="98" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="23"/>
-      <c r="B98" s="65"/>
+      <c r="A98" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.11</v>
+      </c>
+      <c r="B98" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D98" s="66"/>
-      <c r="E98" s="66"/>
-      <c r="F98" s="42"/>
+      <c r="E98" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F98" s="42">
+        <v>44348</v>
+      </c>
       <c r="G98" s="43"/>
       <c r="H98" s="25"/>
       <c r="I98" s="26"/>
@@ -11347,7 +11367,7 @@
     <row r="101" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="23"/>
       <c r="B101" s="65"/>
-      <c r="D101" s="70"/>
+      <c r="D101" s="66"/>
       <c r="E101" s="66"/>
       <c r="F101" s="42"/>
       <c r="G101" s="43"/>
@@ -11687,7 +11707,7 @@
     <row r="106" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="23"/>
       <c r="B106" s="65"/>
-      <c r="D106" s="66"/>
+      <c r="D106" s="70"/>
       <c r="E106" s="66"/>
       <c r="F106" s="42"/>
       <c r="G106" s="43"/>
@@ -11959,7 +11979,7 @@
     <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="23"/>
       <c r="B110" s="65"/>
-      <c r="D110" s="70"/>
+      <c r="D110" s="66"/>
       <c r="E110" s="66"/>
       <c r="F110" s="42"/>
       <c r="G110" s="43"/>
@@ -12299,7 +12319,7 @@
     <row r="115" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="23"/>
       <c r="B115" s="65"/>
-      <c r="D115" s="66"/>
+      <c r="D115" s="70"/>
       <c r="E115" s="66"/>
       <c r="F115" s="42"/>
       <c r="G115" s="43"/>
@@ -12571,7 +12591,7 @@
     <row r="119" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="23"/>
       <c r="B119" s="65"/>
-      <c r="D119" s="70"/>
+      <c r="D119" s="66"/>
       <c r="E119" s="66"/>
       <c r="F119" s="42"/>
       <c r="G119" s="43"/>
@@ -12911,7 +12931,7 @@
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
       <c r="B124" s="65"/>
-      <c r="D124" s="66"/>
+      <c r="D124" s="70"/>
       <c r="E124" s="66"/>
       <c r="F124" s="42"/>
       <c r="G124" s="43"/>
@@ -13183,7 +13203,7 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23"/>
       <c r="B128" s="65"/>
-      <c r="D128" s="70"/>
+      <c r="D128" s="66"/>
       <c r="E128" s="66"/>
       <c r="F128" s="42"/>
       <c r="G128" s="43"/>
@@ -13520,9 +13540,86 @@
       <c r="BN132" s="46"/>
       <c r="BO132" s="46"/>
     </row>
+    <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="23"/>
+      <c r="B133" s="65"/>
+      <c r="D133" s="70"/>
+      <c r="E133" s="66"/>
+      <c r="F133" s="42"/>
+      <c r="G133" s="43"/>
+      <c r="H133" s="25"/>
+      <c r="I133" s="26"/>
+      <c r="J133" s="27"/>
+      <c r="K133" s="40"/>
+      <c r="L133" s="46"/>
+      <c r="M133" s="46"/>
+      <c r="N133" s="46"/>
+      <c r="O133" s="46"/>
+      <c r="P133" s="46"/>
+      <c r="Q133" s="46"/>
+      <c r="R133" s="46"/>
+      <c r="S133" s="46"/>
+      <c r="T133" s="46"/>
+      <c r="U133" s="46"/>
+      <c r="V133" s="46"/>
+      <c r="W133" s="46"/>
+      <c r="X133" s="46"/>
+      <c r="Y133" s="46"/>
+      <c r="Z133" s="46"/>
+      <c r="AA133" s="46"/>
+      <c r="AB133" s="46"/>
+      <c r="AC133" s="46"/>
+      <c r="AD133" s="46"/>
+      <c r="AE133" s="46"/>
+      <c r="AF133" s="46"/>
+      <c r="AG133" s="46"/>
+      <c r="AH133" s="46"/>
+      <c r="AI133" s="46"/>
+      <c r="AJ133" s="46"/>
+      <c r="AK133" s="46"/>
+      <c r="AL133" s="46"/>
+      <c r="AM133" s="46"/>
+      <c r="AN133" s="46"/>
+      <c r="AO133" s="46"/>
+      <c r="AP133" s="46"/>
+      <c r="AQ133" s="46"/>
+      <c r="AR133" s="46"/>
+      <c r="AS133" s="46"/>
+      <c r="AT133" s="46"/>
+      <c r="AU133" s="46"/>
+      <c r="AV133" s="46"/>
+      <c r="AW133" s="46"/>
+      <c r="AX133" s="46"/>
+      <c r="AY133" s="46"/>
+      <c r="AZ133" s="46"/>
+      <c r="BA133" s="46"/>
+      <c r="BB133" s="46"/>
+      <c r="BC133" s="46"/>
+      <c r="BD133" s="46"/>
+      <c r="BE133" s="46"/>
+      <c r="BF133" s="46"/>
+      <c r="BG133" s="46"/>
+      <c r="BH133" s="46"/>
+      <c r="BI133" s="46"/>
+      <c r="BJ133" s="46"/>
+      <c r="BK133" s="46"/>
+      <c r="BL133" s="46"/>
+      <c r="BM133" s="46"/>
+      <c r="BN133" s="46"/>
+      <c r="BO133" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -13533,18 +13630,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I92:I96">
+  <conditionalFormatting sqref="I8:I73 I93:I97">
     <cfRule type="dataBar" priority="181">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13563,7 +13651,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L92:BO92 L97:BO99 M100:BN105 BO103:BO105 L106:BO108 M109:BN114 BO112:BO114 L115:BO117 M118:BN123 BO121:BO123 L124:BO126 M127:BN132 BO130:BO132 M93:BN96 BO95:BO96">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L93:BO93 L98:BO100 M101:BN106 BO104:BO106 L107:BO109 M110:BN115 BO113:BO115 L116:BO118 M119:BN124 BO122:BO124 L125:BO127 M128:BN133 BO131:BO133 M94:BN97 BO96:BO97">
     <cfRule type="expression" dxfId="86" priority="227">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -13571,7 +13659,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L92:BO96">
+  <conditionalFormatting sqref="L6:BO62 L93:BO97">
     <cfRule type="expression" dxfId="84" priority="187">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -13581,7 +13669,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E133:E1048576 E92:E96">
+  <conditionalFormatting sqref="E1:E73 E134:E1048576 E93:E97">
     <cfRule type="cellIs" dxfId="82" priority="168" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13675,7 +13763,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I97:I105">
+  <conditionalFormatting sqref="I98:I106">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13689,12 +13777,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO105">
+  <conditionalFormatting sqref="L98:BO106">
     <cfRule type="expression" dxfId="60" priority="71">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E97:E105">
+  <conditionalFormatting sqref="E98:E106">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13717,7 +13805,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L100:BO105 L93:BO96">
+  <conditionalFormatting sqref="L101:BO106 L94:BO97">
     <cfRule type="expression" dxfId="52" priority="75">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13725,7 +13813,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I106:I114">
+  <conditionalFormatting sqref="I107:I115">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13739,12 +13827,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L106:BO114">
+  <conditionalFormatting sqref="L107:BO115">
     <cfRule type="expression" dxfId="50" priority="58">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106:E114">
+  <conditionalFormatting sqref="E107:E115">
     <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13767,7 +13855,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L109:BO114">
+  <conditionalFormatting sqref="L110:BO115">
     <cfRule type="expression" dxfId="42" priority="62">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13775,7 +13863,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I115:I123">
+  <conditionalFormatting sqref="I116:I124">
     <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13789,12 +13877,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L115:BO123">
+  <conditionalFormatting sqref="L116:BO124">
     <cfRule type="expression" dxfId="40" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E115:E123">
+  <conditionalFormatting sqref="E116:E124">
     <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13817,7 +13905,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L118:BO123">
+  <conditionalFormatting sqref="L119:BO124">
     <cfRule type="expression" dxfId="32" priority="49">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13825,7 +13913,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I124:I132">
+  <conditionalFormatting sqref="I125:I133">
     <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13839,12 +13927,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L124:BO132">
+  <conditionalFormatting sqref="L125:BO133">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E124:E132">
+  <conditionalFormatting sqref="E125:E133">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13867,7 +13955,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L127:BO132">
+  <conditionalFormatting sqref="L128:BO133">
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13917,7 +14005,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO91">
+  <conditionalFormatting sqref="L87:BO92">
     <cfRule type="expression" dxfId="12" priority="10">
       <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
     </cfRule>
@@ -13925,7 +14013,7 @@
       <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I91">
+  <conditionalFormatting sqref="I87:I92">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13939,12 +14027,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO91">
+  <conditionalFormatting sqref="L87:BO92">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E91">
+  <conditionalFormatting sqref="E87:E92">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14023,7 +14111,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I92:I96</xm:sqref>
+          <xm:sqref>I8:I73 I93:I97</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14053,7 +14141,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I97:I105</xm:sqref>
+          <xm:sqref>I98:I106</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14068,7 +14156,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I106:I114</xm:sqref>
+          <xm:sqref>I107:I115</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14083,7 +14171,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I115:I123</xm:sqref>
+          <xm:sqref>I116:I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14098,7 +14186,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I124:I132</xm:sqref>
+          <xm:sqref>I125:I133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -14128,7 +14216,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I87:I91</xm:sqref>
+          <xm:sqref>I87:I92</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added data release dates (v0.13)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F016CA-0501-425F-9897-21B038FCF55B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE7A265-6943-41BE-8B41-5E0CC4809AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31470" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
   <si>
     <t>WBS</t>
   </si>
@@ -778,7 +778,10 @@
     <t>Scrape &amp; Store Nowcast Releases</t>
   </si>
   <si>
-    <t>Added Cleanup Code</t>
+    <t>Add Cleanup Code</t>
+  </si>
+  <si>
+    <t>Add Nowcast Releases to UI</t>
   </si>
 </sst>
 </file>
@@ -1707,6 +1710,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1716,6 +1726,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1724,17 +1738,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2948,11 +2951,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO133"/>
+  <dimension ref="A1:BO134"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G94" sqref="G94"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2982,27 +2985,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3047,12 +3050,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3062,183 +3065,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8396,7 +8399,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A98" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A99" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10697,16 +10700,22 @@
         <v>8.5</v>
       </c>
       <c r="B92" s="65" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="D92" s="66"/>
       <c r="E92" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F92" s="42"/>
-      <c r="G92" s="43"/>
+        <v>69</v>
+      </c>
+      <c r="F92" s="42">
+        <v>44324</v>
+      </c>
+      <c r="G92" s="43">
+        <v>44324</v>
+      </c>
       <c r="H92" s="25"/>
-      <c r="I92" s="26"/>
+      <c r="I92" s="26">
+        <v>1</v>
+      </c>
       <c r="J92" s="27"/>
       <c r="K92" s="40"/>
       <c r="L92" s="46"/>
@@ -10772,15 +10781,13 @@
         <v>8.6</v>
       </c>
       <c r="B93" s="65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D93" s="66"/>
       <c r="E93" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F93" s="42">
-        <v>44326</v>
-      </c>
+      <c r="F93" s="42"/>
       <c r="G93" s="43"/>
       <c r="H93" s="25"/>
       <c r="I93" s="26"/>
@@ -10849,14 +10856,14 @@
         <v>8.7</v>
       </c>
       <c r="B94" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D94" s="70"/>
+        <v>114</v>
+      </c>
+      <c r="D94" s="66"/>
       <c r="E94" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F94" s="42">
-        <v>44336</v>
+        <v>44326</v>
       </c>
       <c r="G94" s="43"/>
       <c r="H94" s="25"/>
@@ -10926,14 +10933,14 @@
         <v>8.8</v>
       </c>
       <c r="B95" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D95" s="70"/>
       <c r="E95" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F95" s="42">
-        <v>44338</v>
+        <v>44336</v>
       </c>
       <c r="G95" s="43"/>
       <c r="H95" s="25"/>
@@ -11003,14 +11010,14 @@
         <v>8.9</v>
       </c>
       <c r="B96" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D96" s="70"/>
       <c r="E96" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F96" s="42">
-        <v>44348</v>
+        <v>44338</v>
       </c>
       <c r="G96" s="43"/>
       <c r="H96" s="25"/>
@@ -11080,7 +11087,7 @@
         <v>8.10</v>
       </c>
       <c r="B97" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D97" s="70"/>
       <c r="E97" s="66" t="s">
@@ -11156,10 +11163,10 @@
         <f t="shared" si="9"/>
         <v>8.11</v>
       </c>
-      <c r="B98" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D98" s="66"/>
+      <c r="B98" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D98" s="70"/>
       <c r="E98" s="66" t="s">
         <v>67</v>
       </c>
@@ -11229,11 +11236,20 @@
       <c r="BO98" s="46"/>
     </row>
     <row r="99" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="23"/>
-      <c r="B99" s="65"/>
+      <c r="A99" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.12</v>
+      </c>
+      <c r="B99" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D99" s="66"/>
-      <c r="E99" s="66"/>
-      <c r="F99" s="42"/>
+      <c r="E99" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F99" s="42">
+        <v>44348</v>
+      </c>
       <c r="G99" s="43"/>
       <c r="H99" s="25"/>
       <c r="I99" s="26"/>
@@ -11435,7 +11451,7 @@
     <row r="102" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="23"/>
       <c r="B102" s="65"/>
-      <c r="D102" s="70"/>
+      <c r="D102" s="66"/>
       <c r="E102" s="66"/>
       <c r="F102" s="42"/>
       <c r="G102" s="43"/>
@@ -11775,7 +11791,7 @@
     <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="23"/>
       <c r="B107" s="65"/>
-      <c r="D107" s="66"/>
+      <c r="D107" s="70"/>
       <c r="E107" s="66"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
@@ -12047,7 +12063,7 @@
     <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="23"/>
       <c r="B111" s="65"/>
-      <c r="D111" s="70"/>
+      <c r="D111" s="66"/>
       <c r="E111" s="66"/>
       <c r="F111" s="42"/>
       <c r="G111" s="43"/>
@@ -12387,7 +12403,7 @@
     <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="23"/>
       <c r="B116" s="65"/>
-      <c r="D116" s="66"/>
+      <c r="D116" s="70"/>
       <c r="E116" s="66"/>
       <c r="F116" s="42"/>
       <c r="G116" s="43"/>
@@ -12659,7 +12675,7 @@
     <row r="120" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="23"/>
       <c r="B120" s="65"/>
-      <c r="D120" s="70"/>
+      <c r="D120" s="66"/>
       <c r="E120" s="66"/>
       <c r="F120" s="42"/>
       <c r="G120" s="43"/>
@@ -12999,7 +13015,7 @@
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23"/>
       <c r="B125" s="65"/>
-      <c r="D125" s="66"/>
+      <c r="D125" s="70"/>
       <c r="E125" s="66"/>
       <c r="F125" s="42"/>
       <c r="G125" s="43"/>
@@ -13271,7 +13287,7 @@
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23"/>
       <c r="B129" s="65"/>
-      <c r="D129" s="70"/>
+      <c r="D129" s="66"/>
       <c r="E129" s="66"/>
       <c r="F129" s="42"/>
       <c r="G129" s="43"/>
@@ -13608,18 +13624,77 @@
       <c r="BN133" s="46"/>
       <c r="BO133" s="46"/>
     </row>
+    <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="23"/>
+      <c r="B134" s="65"/>
+      <c r="D134" s="70"/>
+      <c r="E134" s="66"/>
+      <c r="F134" s="42"/>
+      <c r="G134" s="43"/>
+      <c r="H134" s="25"/>
+      <c r="I134" s="26"/>
+      <c r="J134" s="27"/>
+      <c r="K134" s="40"/>
+      <c r="L134" s="46"/>
+      <c r="M134" s="46"/>
+      <c r="N134" s="46"/>
+      <c r="O134" s="46"/>
+      <c r="P134" s="46"/>
+      <c r="Q134" s="46"/>
+      <c r="R134" s="46"/>
+      <c r="S134" s="46"/>
+      <c r="T134" s="46"/>
+      <c r="U134" s="46"/>
+      <c r="V134" s="46"/>
+      <c r="W134" s="46"/>
+      <c r="X134" s="46"/>
+      <c r="Y134" s="46"/>
+      <c r="Z134" s="46"/>
+      <c r="AA134" s="46"/>
+      <c r="AB134" s="46"/>
+      <c r="AC134" s="46"/>
+      <c r="AD134" s="46"/>
+      <c r="AE134" s="46"/>
+      <c r="AF134" s="46"/>
+      <c r="AG134" s="46"/>
+      <c r="AH134" s="46"/>
+      <c r="AI134" s="46"/>
+      <c r="AJ134" s="46"/>
+      <c r="AK134" s="46"/>
+      <c r="AL134" s="46"/>
+      <c r="AM134" s="46"/>
+      <c r="AN134" s="46"/>
+      <c r="AO134" s="46"/>
+      <c r="AP134" s="46"/>
+      <c r="AQ134" s="46"/>
+      <c r="AR134" s="46"/>
+      <c r="AS134" s="46"/>
+      <c r="AT134" s="46"/>
+      <c r="AU134" s="46"/>
+      <c r="AV134" s="46"/>
+      <c r="AW134" s="46"/>
+      <c r="AX134" s="46"/>
+      <c r="AY134" s="46"/>
+      <c r="AZ134" s="46"/>
+      <c r="BA134" s="46"/>
+      <c r="BB134" s="46"/>
+      <c r="BC134" s="46"/>
+      <c r="BD134" s="46"/>
+      <c r="BE134" s="46"/>
+      <c r="BF134" s="46"/>
+      <c r="BG134" s="46"/>
+      <c r="BH134" s="46"/>
+      <c r="BI134" s="46"/>
+      <c r="BJ134" s="46"/>
+      <c r="BK134" s="46"/>
+      <c r="BL134" s="46"/>
+      <c r="BM134" s="46"/>
+      <c r="BN134" s="46"/>
+      <c r="BO134" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -13630,9 +13705,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I93:I97">
+  <conditionalFormatting sqref="I8:I73 I94:I98">
     <cfRule type="dataBar" priority="181">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13651,7 +13735,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L93:BO93 L98:BO100 M101:BN106 BO104:BO106 L107:BO109 M110:BN115 BO113:BO115 L116:BO118 M119:BN124 BO122:BO124 L125:BO127 M128:BN133 BO131:BO133 M94:BN97 BO96:BO97">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L94:BO94 L99:BO101 M102:BN107 BO105:BO107 L108:BO110 M111:BN116 BO114:BO116 L117:BO119 M120:BN125 BO123:BO125 L126:BO128 M129:BN134 BO132:BO134 M95:BN98 BO97:BO98">
     <cfRule type="expression" dxfId="86" priority="227">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -13659,7 +13743,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L93:BO97">
+  <conditionalFormatting sqref="L6:BO62 L94:BO98">
     <cfRule type="expression" dxfId="84" priority="187">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -13669,7 +13753,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E134:E1048576 E93:E97">
+  <conditionalFormatting sqref="E1:E73 E135:E1048576 E94:E98">
     <cfRule type="cellIs" dxfId="82" priority="168" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13763,7 +13847,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I98:I106">
+  <conditionalFormatting sqref="I99:I107">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13777,12 +13861,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L98:BO106">
+  <conditionalFormatting sqref="L99:BO107">
     <cfRule type="expression" dxfId="60" priority="71">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E98:E106">
+  <conditionalFormatting sqref="E99:E107">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13805,7 +13889,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L101:BO106 L94:BO97">
+  <conditionalFormatting sqref="L102:BO107 L95:BO98">
     <cfRule type="expression" dxfId="52" priority="75">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13813,7 +13897,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I107:I115">
+  <conditionalFormatting sqref="I108:I116">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13827,12 +13911,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L107:BO115">
+  <conditionalFormatting sqref="L108:BO116">
     <cfRule type="expression" dxfId="50" priority="58">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E107:E115">
+  <conditionalFormatting sqref="E108:E116">
     <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13855,7 +13939,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L110:BO115">
+  <conditionalFormatting sqref="L111:BO116">
     <cfRule type="expression" dxfId="42" priority="62">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13863,7 +13947,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I116:I124">
+  <conditionalFormatting sqref="I117:I125">
     <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13877,12 +13961,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L116:BO124">
+  <conditionalFormatting sqref="L117:BO125">
     <cfRule type="expression" dxfId="40" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E116:E124">
+  <conditionalFormatting sqref="E117:E125">
     <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13905,7 +13989,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L119:BO124">
+  <conditionalFormatting sqref="L120:BO125">
     <cfRule type="expression" dxfId="32" priority="49">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13913,7 +13997,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I125:I133">
+  <conditionalFormatting sqref="I126:I134">
     <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13927,12 +14011,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO133">
+  <conditionalFormatting sqref="L126:BO134">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E125:E133">
+  <conditionalFormatting sqref="E126:E134">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13955,7 +14039,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L128:BO133">
+  <conditionalFormatting sqref="L129:BO134">
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14005,7 +14089,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO92">
+  <conditionalFormatting sqref="L87:BO93">
     <cfRule type="expression" dxfId="12" priority="10">
       <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
     </cfRule>
@@ -14013,7 +14097,7 @@
       <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I92">
+  <conditionalFormatting sqref="I87:I93">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14027,12 +14111,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO92">
+  <conditionalFormatting sqref="L87:BO93">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E92">
+  <conditionalFormatting sqref="E87:E93">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14111,7 +14195,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I93:I97</xm:sqref>
+          <xm:sqref>I8:I73 I94:I98</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14141,7 +14225,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I98:I106</xm:sqref>
+          <xm:sqref>I99:I107</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14156,7 +14240,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I107:I115</xm:sqref>
+          <xm:sqref>I108:I116</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14171,7 +14255,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I116:I124</xm:sqref>
+          <xm:sqref>I117:I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14186,7 +14270,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I125:I133</xm:sqref>
+          <xm:sqref>I126:I134</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -14216,7 +14300,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I87:I92</xm:sqref>
+          <xm:sqref>I87:I93</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added filtering for releases to only include DFM input variables (v0.13)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE7A265-6943-41BE-8B41-5E0CC4809AF2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3EF339-9269-4728-8DBB-47FDCD83685D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31470" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="119">
   <si>
     <t>WBS</t>
   </si>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t>Add Nowcast Releases to UI</t>
+  </si>
+  <si>
+    <t>Add Data Release Onhover to Create Line on Highcharts</t>
   </si>
 </sst>
 </file>
@@ -1710,13 +1713,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1726,10 +1722,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1738,6 +1730,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2951,11 +2954,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO134"/>
+  <dimension ref="A1:BO135"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
+      <selection pane="bottomLeft" activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2985,27 +2988,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3050,12 +3053,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3065,183 +3068,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8399,7 +8402,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A99" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A100" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10781,13 +10784,15 @@
         <v>8.6</v>
       </c>
       <c r="B93" s="65" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D93" s="66"/>
       <c r="E93" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F93" s="42"/>
+        <v>69</v>
+      </c>
+      <c r="F93" s="42">
+        <v>44325</v>
+      </c>
       <c r="G93" s="43"/>
       <c r="H93" s="25"/>
       <c r="I93" s="26"/>
@@ -10856,15 +10861,13 @@
         <v>8.7</v>
       </c>
       <c r="B94" s="65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D94" s="66"/>
       <c r="E94" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F94" s="42">
-        <v>44326</v>
-      </c>
+      <c r="F94" s="42"/>
       <c r="G94" s="43"/>
       <c r="H94" s="25"/>
       <c r="I94" s="26"/>
@@ -10933,14 +10936,14 @@
         <v>8.8</v>
       </c>
       <c r="B95" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D95" s="70"/>
+        <v>114</v>
+      </c>
+      <c r="D95" s="66"/>
       <c r="E95" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F95" s="42">
-        <v>44336</v>
+        <v>44326</v>
       </c>
       <c r="G95" s="43"/>
       <c r="H95" s="25"/>
@@ -11010,14 +11013,14 @@
         <v>8.9</v>
       </c>
       <c r="B96" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D96" s="70"/>
       <c r="E96" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F96" s="42">
-        <v>44338</v>
+        <v>44336</v>
       </c>
       <c r="G96" s="43"/>
       <c r="H96" s="25"/>
@@ -11087,14 +11090,14 @@
         <v>8.10</v>
       </c>
       <c r="B97" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D97" s="70"/>
       <c r="E97" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F97" s="42">
-        <v>44348</v>
+        <v>44338</v>
       </c>
       <c r="G97" s="43"/>
       <c r="H97" s="25"/>
@@ -11164,7 +11167,7 @@
         <v>8.11</v>
       </c>
       <c r="B98" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D98" s="70"/>
       <c r="E98" s="66" t="s">
@@ -11240,10 +11243,10 @@
         <f t="shared" si="9"/>
         <v>8.12</v>
       </c>
-      <c r="B99" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D99" s="66"/>
+      <c r="B99" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D99" s="70"/>
       <c r="E99" s="66" t="s">
         <v>67</v>
       </c>
@@ -11313,11 +11316,20 @@
       <c r="BO99" s="46"/>
     </row>
     <row r="100" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="23"/>
-      <c r="B100" s="65"/>
+      <c r="A100" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.13</v>
+      </c>
+      <c r="B100" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D100" s="66"/>
-      <c r="E100" s="66"/>
-      <c r="F100" s="42"/>
+      <c r="E100" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F100" s="42">
+        <v>44348</v>
+      </c>
       <c r="G100" s="43"/>
       <c r="H100" s="25"/>
       <c r="I100" s="26"/>
@@ -11519,7 +11531,7 @@
     <row r="103" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="23"/>
       <c r="B103" s="65"/>
-      <c r="D103" s="70"/>
+      <c r="D103" s="66"/>
       <c r="E103" s="66"/>
       <c r="F103" s="42"/>
       <c r="G103" s="43"/>
@@ -11859,7 +11871,7 @@
     <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="23"/>
       <c r="B108" s="65"/>
-      <c r="D108" s="66"/>
+      <c r="D108" s="70"/>
       <c r="E108" s="66"/>
       <c r="F108" s="42"/>
       <c r="G108" s="43"/>
@@ -12131,7 +12143,7 @@
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="23"/>
       <c r="B112" s="65"/>
-      <c r="D112" s="70"/>
+      <c r="D112" s="66"/>
       <c r="E112" s="66"/>
       <c r="F112" s="42"/>
       <c r="G112" s="43"/>
@@ -12471,7 +12483,7 @@
     <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="23"/>
       <c r="B117" s="65"/>
-      <c r="D117" s="66"/>
+      <c r="D117" s="70"/>
       <c r="E117" s="66"/>
       <c r="F117" s="42"/>
       <c r="G117" s="43"/>
@@ -12743,7 +12755,7 @@
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="23"/>
       <c r="B121" s="65"/>
-      <c r="D121" s="70"/>
+      <c r="D121" s="66"/>
       <c r="E121" s="66"/>
       <c r="F121" s="42"/>
       <c r="G121" s="43"/>
@@ -13083,7 +13095,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="66"/>
+      <c r="D126" s="70"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -13355,7 +13367,7 @@
     <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="23"/>
       <c r="B130" s="65"/>
-      <c r="D130" s="70"/>
+      <c r="D130" s="66"/>
       <c r="E130" s="66"/>
       <c r="F130" s="42"/>
       <c r="G130" s="43"/>
@@ -13692,9 +13704,86 @@
       <c r="BN134" s="46"/>
       <c r="BO134" s="46"/>
     </row>
+    <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="23"/>
+      <c r="B135" s="65"/>
+      <c r="D135" s="70"/>
+      <c r="E135" s="66"/>
+      <c r="F135" s="42"/>
+      <c r="G135" s="43"/>
+      <c r="H135" s="25"/>
+      <c r="I135" s="26"/>
+      <c r="J135" s="27"/>
+      <c r="K135" s="40"/>
+      <c r="L135" s="46"/>
+      <c r="M135" s="46"/>
+      <c r="N135" s="46"/>
+      <c r="O135" s="46"/>
+      <c r="P135" s="46"/>
+      <c r="Q135" s="46"/>
+      <c r="R135" s="46"/>
+      <c r="S135" s="46"/>
+      <c r="T135" s="46"/>
+      <c r="U135" s="46"/>
+      <c r="V135" s="46"/>
+      <c r="W135" s="46"/>
+      <c r="X135" s="46"/>
+      <c r="Y135" s="46"/>
+      <c r="Z135" s="46"/>
+      <c r="AA135" s="46"/>
+      <c r="AB135" s="46"/>
+      <c r="AC135" s="46"/>
+      <c r="AD135" s="46"/>
+      <c r="AE135" s="46"/>
+      <c r="AF135" s="46"/>
+      <c r="AG135" s="46"/>
+      <c r="AH135" s="46"/>
+      <c r="AI135" s="46"/>
+      <c r="AJ135" s="46"/>
+      <c r="AK135" s="46"/>
+      <c r="AL135" s="46"/>
+      <c r="AM135" s="46"/>
+      <c r="AN135" s="46"/>
+      <c r="AO135" s="46"/>
+      <c r="AP135" s="46"/>
+      <c r="AQ135" s="46"/>
+      <c r="AR135" s="46"/>
+      <c r="AS135" s="46"/>
+      <c r="AT135" s="46"/>
+      <c r="AU135" s="46"/>
+      <c r="AV135" s="46"/>
+      <c r="AW135" s="46"/>
+      <c r="AX135" s="46"/>
+      <c r="AY135" s="46"/>
+      <c r="AZ135" s="46"/>
+      <c r="BA135" s="46"/>
+      <c r="BB135" s="46"/>
+      <c r="BC135" s="46"/>
+      <c r="BD135" s="46"/>
+      <c r="BE135" s="46"/>
+      <c r="BF135" s="46"/>
+      <c r="BG135" s="46"/>
+      <c r="BH135" s="46"/>
+      <c r="BI135" s="46"/>
+      <c r="BJ135" s="46"/>
+      <c r="BK135" s="46"/>
+      <c r="BL135" s="46"/>
+      <c r="BM135" s="46"/>
+      <c r="BN135" s="46"/>
+      <c r="BO135" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -13705,18 +13794,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I94:I98">
+  <conditionalFormatting sqref="I8:I73 I95:I99">
     <cfRule type="dataBar" priority="181">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13735,7 +13815,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L94:BO94 L99:BO101 M102:BN107 BO105:BO107 L108:BO110 M111:BN116 BO114:BO116 L117:BO119 M120:BN125 BO123:BO125 L126:BO128 M129:BN134 BO132:BO134 M95:BN98 BO97:BO98">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO95 L100:BO102 M103:BN108 BO106:BO108 L109:BO111 M112:BN117 BO115:BO117 L118:BO120 M121:BN126 BO124:BO126 L127:BO129 M130:BN135 BO133:BO135 M96:BN99 BO98:BO99">
     <cfRule type="expression" dxfId="86" priority="227">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -13743,7 +13823,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L94:BO98">
+  <conditionalFormatting sqref="L6:BO62 L95:BO99">
     <cfRule type="expression" dxfId="84" priority="187">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -13753,7 +13833,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E135:E1048576 E94:E98">
+  <conditionalFormatting sqref="E1:E73 E136:E1048576 E95:E99">
     <cfRule type="cellIs" dxfId="82" priority="168" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13847,7 +13927,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I99:I107">
+  <conditionalFormatting sqref="I100:I108">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13861,12 +13941,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L99:BO107">
+  <conditionalFormatting sqref="L100:BO108">
     <cfRule type="expression" dxfId="60" priority="71">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E99:E107">
+  <conditionalFormatting sqref="E100:E108">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13889,7 +13969,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L102:BO107 L95:BO98">
+  <conditionalFormatting sqref="L103:BO108 L96:BO99">
     <cfRule type="expression" dxfId="52" priority="75">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13897,7 +13977,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I108:I116">
+  <conditionalFormatting sqref="I109:I117">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13911,12 +13991,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L108:BO116">
+  <conditionalFormatting sqref="L109:BO117">
     <cfRule type="expression" dxfId="50" priority="58">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E108:E116">
+  <conditionalFormatting sqref="E109:E117">
     <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13939,7 +14019,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L111:BO116">
+  <conditionalFormatting sqref="L112:BO117">
     <cfRule type="expression" dxfId="42" priority="62">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13947,7 +14027,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I117:I125">
+  <conditionalFormatting sqref="I118:I126">
     <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13961,12 +14041,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L117:BO125">
+  <conditionalFormatting sqref="L118:BO126">
     <cfRule type="expression" dxfId="40" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E117:E125">
+  <conditionalFormatting sqref="E118:E126">
     <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13989,7 +14069,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L120:BO125">
+  <conditionalFormatting sqref="L121:BO126">
     <cfRule type="expression" dxfId="32" priority="49">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13997,7 +14077,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I126:I134">
+  <conditionalFormatting sqref="I127:I135">
     <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14011,12 +14091,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L126:BO134">
+  <conditionalFormatting sqref="L127:BO135">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E126:E134">
+  <conditionalFormatting sqref="E127:E135">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14039,7 +14119,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L129:BO134">
+  <conditionalFormatting sqref="L130:BO135">
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14089,7 +14169,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO93">
+  <conditionalFormatting sqref="L87:BO94">
     <cfRule type="expression" dxfId="12" priority="10">
       <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
     </cfRule>
@@ -14097,7 +14177,7 @@
       <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I93">
+  <conditionalFormatting sqref="I87:I94">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14111,12 +14191,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO93">
+  <conditionalFormatting sqref="L87:BO94">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E93">
+  <conditionalFormatting sqref="E87:E94">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14195,7 +14275,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I94:I98</xm:sqref>
+          <xm:sqref>I8:I73 I95:I99</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14225,7 +14305,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I99:I107</xm:sqref>
+          <xm:sqref>I100:I108</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14240,7 +14320,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I108:I116</xm:sqref>
+          <xm:sqref>I109:I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14255,7 +14335,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I117:I125</xm:sqref>
+          <xm:sqref>I118:I126</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14270,7 +14350,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I126:I134</xm:sqref>
+          <xm:sqref>I127:I135</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -14300,7 +14380,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I87:I93</xm:sqref>
+          <xm:sqref>I87:I94</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Fixed bug in CME web scraping and major problem with Treasury forecasts caused by MAPE optimization of lambda parameter (v0.13)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CA62BE-6ACF-4DDF-80B0-A58FF1554547}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F25A848-8CF7-4F12-A48D-D2A7002C6A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
   <si>
     <t>WBS</t>
   </si>
@@ -785,6 +785,9 @@
   </si>
   <si>
     <t>Add Data Release Onhover to Create Line on Highcharts</t>
+  </si>
+  <si>
+    <t>Improve Inflation Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1713,6 +1716,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1722,6 +1732,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1730,17 +1744,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2954,11 +2957,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO135"/>
+  <dimension ref="A1:BO136"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F96" sqref="F96"/>
+      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2988,27 +2991,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3053,12 +3056,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3068,183 +3071,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8402,7 +8405,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A100" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A101" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10872,11 +10875,15 @@
         <v>67</v>
       </c>
       <c r="F94" s="42">
-        <v>44336</v>
-      </c>
-      <c r="G94" s="43"/>
+        <v>44341</v>
+      </c>
+      <c r="G94" s="43">
+        <v>44341</v>
+      </c>
       <c r="H94" s="25"/>
-      <c r="I94" s="26"/>
+      <c r="I94" s="26">
+        <v>1</v>
+      </c>
       <c r="J94" s="27"/>
       <c r="K94" s="40"/>
       <c r="L94" s="46"/>
@@ -10949,11 +10956,15 @@
         <v>67</v>
       </c>
       <c r="F95" s="42">
-        <v>44336</v>
-      </c>
-      <c r="G95" s="43"/>
+        <v>44341</v>
+      </c>
+      <c r="G95" s="43">
+        <v>44341</v>
+      </c>
       <c r="H95" s="25"/>
-      <c r="I95" s="26"/>
+      <c r="I95" s="26">
+        <v>1</v>
+      </c>
       <c r="J95" s="27"/>
       <c r="K95" s="40"/>
       <c r="L95" s="46"/>
@@ -11019,18 +11030,22 @@
         <v>8.9</v>
       </c>
       <c r="B96" s="65" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="D96" s="70"/>
       <c r="E96" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F96" s="42">
-        <v>44336</v>
-      </c>
-      <c r="G96" s="43"/>
+        <v>44341</v>
+      </c>
+      <c r="G96" s="43">
+        <v>44341</v>
+      </c>
       <c r="H96" s="25"/>
-      <c r="I96" s="26"/>
+      <c r="I96" s="26">
+        <v>1</v>
+      </c>
       <c r="J96" s="27"/>
       <c r="K96" s="40"/>
       <c r="L96" s="46"/>
@@ -11096,14 +11111,14 @@
         <v>8.10</v>
       </c>
       <c r="B97" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D97" s="70"/>
       <c r="E97" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F97" s="42">
-        <v>44338</v>
+        <v>44342</v>
       </c>
       <c r="G97" s="43"/>
       <c r="H97" s="25"/>
@@ -11173,14 +11188,14 @@
         <v>8.11</v>
       </c>
       <c r="B98" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D98" s="70"/>
       <c r="E98" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F98" s="42">
-        <v>44348</v>
+        <v>44343</v>
       </c>
       <c r="G98" s="43"/>
       <c r="H98" s="25"/>
@@ -11250,7 +11265,7 @@
         <v>8.12</v>
       </c>
       <c r="B99" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D99" s="70"/>
       <c r="E99" s="66" t="s">
@@ -11326,10 +11341,10 @@
         <f t="shared" si="9"/>
         <v>8.13</v>
       </c>
-      <c r="B100" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D100" s="66"/>
+      <c r="B100" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
         <v>67</v>
       </c>
@@ -11399,11 +11414,20 @@
       <c r="BO100" s="46"/>
     </row>
     <row r="101" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="23"/>
-      <c r="B101" s="65"/>
+      <c r="A101" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>8.14</v>
+      </c>
+      <c r="B101" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D101" s="66"/>
-      <c r="E101" s="66"/>
-      <c r="F101" s="42"/>
+      <c r="E101" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F101" s="42">
+        <v>44348</v>
+      </c>
       <c r="G101" s="43"/>
       <c r="H101" s="25"/>
       <c r="I101" s="26"/>
@@ -11605,7 +11629,7 @@
     <row r="104" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="23"/>
       <c r="B104" s="65"/>
-      <c r="D104" s="70"/>
+      <c r="D104" s="66"/>
       <c r="E104" s="66"/>
       <c r="F104" s="42"/>
       <c r="G104" s="43"/>
@@ -11945,7 +11969,7 @@
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="23"/>
       <c r="B109" s="65"/>
-      <c r="D109" s="66"/>
+      <c r="D109" s="70"/>
       <c r="E109" s="66"/>
       <c r="F109" s="42"/>
       <c r="G109" s="43"/>
@@ -12217,7 +12241,7 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23"/>
       <c r="B113" s="65"/>
-      <c r="D113" s="70"/>
+      <c r="D113" s="66"/>
       <c r="E113" s="66"/>
       <c r="F113" s="42"/>
       <c r="G113" s="43"/>
@@ -12557,7 +12581,7 @@
     <row r="118" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="23"/>
       <c r="B118" s="65"/>
-      <c r="D118" s="66"/>
+      <c r="D118" s="70"/>
       <c r="E118" s="66"/>
       <c r="F118" s="42"/>
       <c r="G118" s="43"/>
@@ -12829,7 +12853,7 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
       <c r="B122" s="65"/>
-      <c r="D122" s="70"/>
+      <c r="D122" s="66"/>
       <c r="E122" s="66"/>
       <c r="F122" s="42"/>
       <c r="G122" s="43"/>
@@ -13169,7 +13193,7 @@
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23"/>
       <c r="B127" s="65"/>
-      <c r="D127" s="66"/>
+      <c r="D127" s="70"/>
       <c r="E127" s="66"/>
       <c r="F127" s="42"/>
       <c r="G127" s="43"/>
@@ -13441,7 +13465,7 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
       <c r="B131" s="65"/>
-      <c r="D131" s="70"/>
+      <c r="D131" s="66"/>
       <c r="E131" s="66"/>
       <c r="F131" s="42"/>
       <c r="G131" s="43"/>
@@ -13778,18 +13802,77 @@
       <c r="BN135" s="46"/>
       <c r="BO135" s="46"/>
     </row>
+    <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="23"/>
+      <c r="B136" s="65"/>
+      <c r="D136" s="70"/>
+      <c r="E136" s="66"/>
+      <c r="F136" s="42"/>
+      <c r="G136" s="43"/>
+      <c r="H136" s="25"/>
+      <c r="I136" s="26"/>
+      <c r="J136" s="27"/>
+      <c r="K136" s="40"/>
+      <c r="L136" s="46"/>
+      <c r="M136" s="46"/>
+      <c r="N136" s="46"/>
+      <c r="O136" s="46"/>
+      <c r="P136" s="46"/>
+      <c r="Q136" s="46"/>
+      <c r="R136" s="46"/>
+      <c r="S136" s="46"/>
+      <c r="T136" s="46"/>
+      <c r="U136" s="46"/>
+      <c r="V136" s="46"/>
+      <c r="W136" s="46"/>
+      <c r="X136" s="46"/>
+      <c r="Y136" s="46"/>
+      <c r="Z136" s="46"/>
+      <c r="AA136" s="46"/>
+      <c r="AB136" s="46"/>
+      <c r="AC136" s="46"/>
+      <c r="AD136" s="46"/>
+      <c r="AE136" s="46"/>
+      <c r="AF136" s="46"/>
+      <c r="AG136" s="46"/>
+      <c r="AH136" s="46"/>
+      <c r="AI136" s="46"/>
+      <c r="AJ136" s="46"/>
+      <c r="AK136" s="46"/>
+      <c r="AL136" s="46"/>
+      <c r="AM136" s="46"/>
+      <c r="AN136" s="46"/>
+      <c r="AO136" s="46"/>
+      <c r="AP136" s="46"/>
+      <c r="AQ136" s="46"/>
+      <c r="AR136" s="46"/>
+      <c r="AS136" s="46"/>
+      <c r="AT136" s="46"/>
+      <c r="AU136" s="46"/>
+      <c r="AV136" s="46"/>
+      <c r="AW136" s="46"/>
+      <c r="AX136" s="46"/>
+      <c r="AY136" s="46"/>
+      <c r="AZ136" s="46"/>
+      <c r="BA136" s="46"/>
+      <c r="BB136" s="46"/>
+      <c r="BC136" s="46"/>
+      <c r="BD136" s="46"/>
+      <c r="BE136" s="46"/>
+      <c r="BF136" s="46"/>
+      <c r="BG136" s="46"/>
+      <c r="BH136" s="46"/>
+      <c r="BI136" s="46"/>
+      <c r="BJ136" s="46"/>
+      <c r="BK136" s="46"/>
+      <c r="BL136" s="46"/>
+      <c r="BM136" s="46"/>
+      <c r="BN136" s="46"/>
+      <c r="BO136" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -13800,9 +13883,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I99">
+  <conditionalFormatting sqref="I8:I73 I95:I100">
     <cfRule type="dataBar" priority="181">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13821,7 +13913,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO95 L100:BO102 M103:BN108 BO106:BO108 L109:BO111 M112:BN117 BO115:BO117 L118:BO120 M121:BN126 BO124:BO126 L127:BO129 M130:BN135 BO133:BO135 M96:BN99 BO98:BO99">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L101:BO103 M104:BN109 BO107:BO109 L110:BO112 M113:BN118 BO116:BO118 L119:BO121 M122:BN127 BO125:BO127 L128:BO130 M131:BN136 BO134:BO136 M97:BN100 BO99:BO100">
     <cfRule type="expression" dxfId="86" priority="227">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -13829,7 +13921,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO99">
+  <conditionalFormatting sqref="L6:BO62 L95:BO100">
     <cfRule type="expression" dxfId="84" priority="187">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -13839,7 +13931,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E136:E1048576 E95:E99">
+  <conditionalFormatting sqref="E1:E73 E137:E1048576 E95:E100">
     <cfRule type="cellIs" dxfId="82" priority="168" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13933,7 +14025,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I100:I108">
+  <conditionalFormatting sqref="I101:I109">
     <cfRule type="dataBar" priority="72">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13947,12 +14039,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L100:BO108">
+  <conditionalFormatting sqref="L101:BO109">
     <cfRule type="expression" dxfId="60" priority="71">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E100:E108">
+  <conditionalFormatting sqref="E101:E109">
     <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -13975,7 +14067,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L103:BO108 L96:BO99">
+  <conditionalFormatting sqref="L104:BO109 L97:BO100">
     <cfRule type="expression" dxfId="52" priority="75">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -13983,7 +14075,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I109:I117">
+  <conditionalFormatting sqref="I110:I118">
     <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13997,12 +14089,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L109:BO117">
+  <conditionalFormatting sqref="L110:BO118">
     <cfRule type="expression" dxfId="50" priority="58">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:E117">
+  <conditionalFormatting sqref="E110:E118">
     <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14025,7 +14117,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L112:BO117">
+  <conditionalFormatting sqref="L113:BO118">
     <cfRule type="expression" dxfId="42" priority="62">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14033,7 +14125,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I118:I126">
+  <conditionalFormatting sqref="I119:I127">
     <cfRule type="dataBar" priority="46">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14047,12 +14139,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L118:BO126">
+  <conditionalFormatting sqref="L119:BO127">
     <cfRule type="expression" dxfId="40" priority="45">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E118:E126">
+  <conditionalFormatting sqref="E119:E127">
     <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14075,7 +14167,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L121:BO126">
+  <conditionalFormatting sqref="L122:BO127">
     <cfRule type="expression" dxfId="32" priority="49">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14083,7 +14175,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I127:I135">
+  <conditionalFormatting sqref="I128:I136">
     <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14097,12 +14189,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L127:BO135">
+  <conditionalFormatting sqref="L128:BO136">
     <cfRule type="expression" dxfId="30" priority="32">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E127:E135">
+  <conditionalFormatting sqref="E128:E136">
     <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14125,7 +14217,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L130:BO135">
+  <conditionalFormatting sqref="L131:BO136">
     <cfRule type="expression" dxfId="22" priority="36">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14281,7 +14373,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I99</xm:sqref>
+          <xm:sqref>I8:I73 I95:I100</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14311,7 +14403,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I100:I108</xm:sqref>
+          <xm:sqref>I101:I109</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14326,7 +14418,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I109:I117</xm:sqref>
+          <xm:sqref>I110:I118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14341,7 +14433,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I118:I126</xm:sqref>
+          <xm:sqref>I119:I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14356,7 +14448,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I127:I135</xm:sqref>
+          <xm:sqref>I128:I136</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">

</xml_diff>

<commit_message>
Removed JOLTS new hires (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F25A848-8CF7-4F12-A48D-D2A7002C6A3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E796B6-BB0D-4C88-BE5D-A88DC96221D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="122">
   <si>
     <t>WBS</t>
   </si>
@@ -788,6 +788,12 @@
   </si>
   <si>
     <t>Improve Inflation Forecasts</t>
+  </si>
+  <si>
+    <t>Generate Full 5-Year Forecasts of All Key Variables</t>
+  </si>
+  <si>
+    <t>Structural Model Key Variables Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1716,13 +1722,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1732,10 +1731,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1744,6 +1739,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1792,7 +1798,82 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="98">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -2957,11 +3038,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO136"/>
+  <dimension ref="A1:BO138"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2991,27 +3072,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3056,12 +3137,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3071,183 +3152,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8405,7 +8486,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A101" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A103" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11105,97 +11186,99 @@
       <c r="BN96" s="46"/>
       <c r="BO96" s="46"/>
     </row>
-    <row r="97" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>8.10</v>
-      </c>
-      <c r="B97" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D97" s="70"/>
-      <c r="E97" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F97" s="42">
-        <v>44342</v>
-      </c>
-      <c r="G97" s="43"/>
-      <c r="H97" s="25"/>
-      <c r="I97" s="26"/>
-      <c r="J97" s="27"/>
-      <c r="K97" s="40"/>
-      <c r="L97" s="46"/>
-      <c r="M97" s="46"/>
-      <c r="N97" s="46"/>
-      <c r="O97" s="46"/>
-      <c r="P97" s="46"/>
-      <c r="Q97" s="46"/>
-      <c r="R97" s="46"/>
-      <c r="S97" s="46"/>
-      <c r="T97" s="46"/>
-      <c r="U97" s="46"/>
-      <c r="V97" s="46"/>
-      <c r="W97" s="46"/>
-      <c r="X97" s="46"/>
-      <c r="Y97" s="46"/>
-      <c r="Z97" s="46"/>
-      <c r="AA97" s="46"/>
-      <c r="AB97" s="46"/>
-      <c r="AC97" s="46"/>
-      <c r="AD97" s="46"/>
-      <c r="AE97" s="46"/>
-      <c r="AF97" s="46"/>
-      <c r="AG97" s="46"/>
-      <c r="AH97" s="46"/>
-      <c r="AI97" s="46"/>
-      <c r="AJ97" s="46"/>
-      <c r="AK97" s="46"/>
-      <c r="AL97" s="46"/>
-      <c r="AM97" s="46"/>
-      <c r="AN97" s="46"/>
-      <c r="AO97" s="46"/>
-      <c r="AP97" s="46"/>
-      <c r="AQ97" s="46"/>
-      <c r="AR97" s="46"/>
-      <c r="AS97" s="46"/>
-      <c r="AT97" s="46"/>
-      <c r="AU97" s="46"/>
-      <c r="AV97" s="46"/>
-      <c r="AW97" s="46"/>
-      <c r="AX97" s="46"/>
-      <c r="AY97" s="46"/>
-      <c r="AZ97" s="46"/>
-      <c r="BA97" s="46"/>
-      <c r="BB97" s="46"/>
-      <c r="BC97" s="46"/>
-      <c r="BD97" s="46"/>
-      <c r="BE97" s="46"/>
-      <c r="BF97" s="46"/>
-      <c r="BG97" s="46"/>
-      <c r="BH97" s="46"/>
-      <c r="BI97" s="46"/>
-      <c r="BJ97" s="46"/>
-      <c r="BK97" s="46"/>
-      <c r="BL97" s="46"/>
-      <c r="BM97" s="46"/>
-      <c r="BN97" s="46"/>
-      <c r="BO97" s="46"/>
+    <row r="97" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>9</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D97" s="19"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="44"/>
+      <c r="G97" s="44" t="str">
+        <f t="shared" ref="G97" si="16">IF(ISBLANK(F97)," - ",IF(H97=0,F97,F97+H97-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H97" s="20"/>
+      <c r="I97" s="21"/>
+      <c r="J97" s="22" t="str">
+        <f t="shared" ref="J97" si="17">IF(OR(G97=0,F97=0)," - ",NETWORKDAYS(F97,G97))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K97" s="41"/>
+      <c r="L97" s="48"/>
+      <c r="M97" s="48"/>
+      <c r="N97" s="48"/>
+      <c r="O97" s="48"/>
+      <c r="P97" s="48"/>
+      <c r="Q97" s="48"/>
+      <c r="R97" s="48"/>
+      <c r="S97" s="48"/>
+      <c r="T97" s="48"/>
+      <c r="U97" s="48"/>
+      <c r="V97" s="48"/>
+      <c r="W97" s="48"/>
+      <c r="X97" s="48"/>
+      <c r="Y97" s="48"/>
+      <c r="Z97" s="48"/>
+      <c r="AA97" s="48"/>
+      <c r="AB97" s="48"/>
+      <c r="AC97" s="48"/>
+      <c r="AD97" s="48"/>
+      <c r="AE97" s="48"/>
+      <c r="AF97" s="48"/>
+      <c r="AG97" s="48"/>
+      <c r="AH97" s="48"/>
+      <c r="AI97" s="48"/>
+      <c r="AJ97" s="48"/>
+      <c r="AK97" s="48"/>
+      <c r="AL97" s="48"/>
+      <c r="AM97" s="48"/>
+      <c r="AN97" s="48"/>
+      <c r="AO97" s="48"/>
+      <c r="AP97" s="48"/>
+      <c r="AQ97" s="48"/>
+      <c r="AR97" s="48"/>
+      <c r="AS97" s="48"/>
+      <c r="AT97" s="48"/>
+      <c r="AU97" s="48"/>
+      <c r="AV97" s="48"/>
+      <c r="AW97" s="48"/>
+      <c r="AX97" s="48"/>
+      <c r="AY97" s="48"/>
+      <c r="AZ97" s="48"/>
+      <c r="BA97" s="48"/>
+      <c r="BB97" s="48"/>
+      <c r="BC97" s="48"/>
+      <c r="BD97" s="48"/>
+      <c r="BE97" s="48"/>
+      <c r="BF97" s="48"/>
+      <c r="BG97" s="48"/>
+      <c r="BH97" s="48"/>
+      <c r="BI97" s="48"/>
+      <c r="BJ97" s="48"/>
+      <c r="BK97" s="48"/>
+      <c r="BL97" s="48"/>
+      <c r="BM97" s="48"/>
+      <c r="BN97" s="48"/>
+      <c r="BO97" s="48"/>
     </row>
     <row r="98" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>8.11</v>
+        <v>9.1</v>
       </c>
       <c r="B98" s="65" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="D98" s="70"/>
       <c r="E98" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F98" s="42">
-        <v>44343</v>
+        <v>44342</v>
       </c>
       <c r="G98" s="43"/>
       <c r="H98" s="25"/>
@@ -11262,17 +11345,17 @@
     <row r="99" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>8.12</v>
+        <v>9.2</v>
       </c>
       <c r="B99" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D99" s="70"/>
       <c r="E99" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F99" s="42">
-        <v>44348</v>
+        <v>44344</v>
       </c>
       <c r="G99" s="43"/>
       <c r="H99" s="25"/>
@@ -11339,17 +11422,17 @@
     <row r="100" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>8.13</v>
+        <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F100" s="42">
-        <v>44348</v>
+        <v>44343</v>
       </c>
       <c r="G100" s="43"/>
       <c r="H100" s="25"/>
@@ -11416,12 +11499,12 @@
     <row r="101" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>8.14</v>
-      </c>
-      <c r="B101" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D101" s="66"/>
+        <v>9.4</v>
+      </c>
+      <c r="B101" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
         <v>67</v>
       </c>
@@ -11491,11 +11574,20 @@
       <c r="BO101" s="46"/>
     </row>
     <row r="102" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="23"/>
-      <c r="B102" s="65"/>
-      <c r="D102" s="66"/>
-      <c r="E102" s="66"/>
-      <c r="F102" s="42"/>
+      <c r="A102" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>9.5</v>
+      </c>
+      <c r="B102" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D102" s="70"/>
+      <c r="E102" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F102" s="42">
+        <v>44348</v>
+      </c>
       <c r="G102" s="43"/>
       <c r="H102" s="25"/>
       <c r="I102" s="26"/>
@@ -11559,11 +11651,20 @@
       <c r="BO102" s="46"/>
     </row>
     <row r="103" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="23"/>
-      <c r="B103" s="65"/>
+      <c r="A103" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>9.6</v>
+      </c>
+      <c r="B103" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D103" s="66"/>
-      <c r="E103" s="66"/>
-      <c r="F103" s="42"/>
+      <c r="E103" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F103" s="42">
+        <v>44348</v>
+      </c>
       <c r="G103" s="43"/>
       <c r="H103" s="25"/>
       <c r="I103" s="26"/>
@@ -11697,7 +11798,7 @@
     <row r="105" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="23"/>
       <c r="B105" s="65"/>
-      <c r="D105" s="70"/>
+      <c r="D105" s="66"/>
       <c r="E105" s="66"/>
       <c r="F105" s="42"/>
       <c r="G105" s="43"/>
@@ -11765,7 +11866,7 @@
     <row r="106" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="23"/>
       <c r="B106" s="65"/>
-      <c r="D106" s="70"/>
+      <c r="D106" s="66"/>
       <c r="E106" s="66"/>
       <c r="F106" s="42"/>
       <c r="G106" s="43"/>
@@ -12037,7 +12138,7 @@
     <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="23"/>
       <c r="B110" s="65"/>
-      <c r="D110" s="66"/>
+      <c r="D110" s="70"/>
       <c r="E110" s="66"/>
       <c r="F110" s="42"/>
       <c r="G110" s="43"/>
@@ -12105,7 +12206,7 @@
     <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="23"/>
       <c r="B111" s="65"/>
-      <c r="D111" s="66"/>
+      <c r="D111" s="70"/>
       <c r="E111" s="66"/>
       <c r="F111" s="42"/>
       <c r="G111" s="43"/>
@@ -12309,7 +12410,7 @@
     <row r="114" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="23"/>
       <c r="B114" s="65"/>
-      <c r="D114" s="70"/>
+      <c r="D114" s="66"/>
       <c r="E114" s="66"/>
       <c r="F114" s="42"/>
       <c r="G114" s="43"/>
@@ -12377,7 +12478,7 @@
     <row r="115" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="23"/>
       <c r="B115" s="65"/>
-      <c r="D115" s="70"/>
+      <c r="D115" s="66"/>
       <c r="E115" s="66"/>
       <c r="F115" s="42"/>
       <c r="G115" s="43"/>
@@ -12649,7 +12750,7 @@
     <row r="119" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="23"/>
       <c r="B119" s="65"/>
-      <c r="D119" s="66"/>
+      <c r="D119" s="70"/>
       <c r="E119" s="66"/>
       <c r="F119" s="42"/>
       <c r="G119" s="43"/>
@@ -12717,7 +12818,7 @@
     <row r="120" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="23"/>
       <c r="B120" s="65"/>
-      <c r="D120" s="66"/>
+      <c r="D120" s="70"/>
       <c r="E120" s="66"/>
       <c r="F120" s="42"/>
       <c r="G120" s="43"/>
@@ -12921,7 +13022,7 @@
     <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="23"/>
       <c r="B123" s="65"/>
-      <c r="D123" s="70"/>
+      <c r="D123" s="66"/>
       <c r="E123" s="66"/>
       <c r="F123" s="42"/>
       <c r="G123" s="43"/>
@@ -12989,7 +13090,7 @@
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
       <c r="B124" s="65"/>
-      <c r="D124" s="70"/>
+      <c r="D124" s="66"/>
       <c r="E124" s="66"/>
       <c r="F124" s="42"/>
       <c r="G124" s="43"/>
@@ -13261,7 +13362,7 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23"/>
       <c r="B128" s="65"/>
-      <c r="D128" s="66"/>
+      <c r="D128" s="70"/>
       <c r="E128" s="66"/>
       <c r="F128" s="42"/>
       <c r="G128" s="43"/>
@@ -13329,7 +13430,7 @@
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23"/>
       <c r="B129" s="65"/>
-      <c r="D129" s="66"/>
+      <c r="D129" s="70"/>
       <c r="E129" s="66"/>
       <c r="F129" s="42"/>
       <c r="G129" s="43"/>
@@ -13533,7 +13634,7 @@
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23"/>
       <c r="B132" s="65"/>
-      <c r="D132" s="70"/>
+      <c r="D132" s="66"/>
       <c r="E132" s="66"/>
       <c r="F132" s="42"/>
       <c r="G132" s="43"/>
@@ -13601,7 +13702,7 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23"/>
       <c r="B133" s="65"/>
-      <c r="D133" s="70"/>
+      <c r="D133" s="66"/>
       <c r="E133" s="66"/>
       <c r="F133" s="42"/>
       <c r="G133" s="43"/>
@@ -13870,9 +13971,154 @@
       <c r="BN136" s="46"/>
       <c r="BO136" s="46"/>
     </row>
+    <row r="137" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="23"/>
+      <c r="B137" s="65"/>
+      <c r="D137" s="70"/>
+      <c r="E137" s="66"/>
+      <c r="F137" s="42"/>
+      <c r="G137" s="43"/>
+      <c r="H137" s="25"/>
+      <c r="I137" s="26"/>
+      <c r="J137" s="27"/>
+      <c r="K137" s="40"/>
+      <c r="L137" s="46"/>
+      <c r="M137" s="46"/>
+      <c r="N137" s="46"/>
+      <c r="O137" s="46"/>
+      <c r="P137" s="46"/>
+      <c r="Q137" s="46"/>
+      <c r="R137" s="46"/>
+      <c r="S137" s="46"/>
+      <c r="T137" s="46"/>
+      <c r="U137" s="46"/>
+      <c r="V137" s="46"/>
+      <c r="W137" s="46"/>
+      <c r="X137" s="46"/>
+      <c r="Y137" s="46"/>
+      <c r="Z137" s="46"/>
+      <c r="AA137" s="46"/>
+      <c r="AB137" s="46"/>
+      <c r="AC137" s="46"/>
+      <c r="AD137" s="46"/>
+      <c r="AE137" s="46"/>
+      <c r="AF137" s="46"/>
+      <c r="AG137" s="46"/>
+      <c r="AH137" s="46"/>
+      <c r="AI137" s="46"/>
+      <c r="AJ137" s="46"/>
+      <c r="AK137" s="46"/>
+      <c r="AL137" s="46"/>
+      <c r="AM137" s="46"/>
+      <c r="AN137" s="46"/>
+      <c r="AO137" s="46"/>
+      <c r="AP137" s="46"/>
+      <c r="AQ137" s="46"/>
+      <c r="AR137" s="46"/>
+      <c r="AS137" s="46"/>
+      <c r="AT137" s="46"/>
+      <c r="AU137" s="46"/>
+      <c r="AV137" s="46"/>
+      <c r="AW137" s="46"/>
+      <c r="AX137" s="46"/>
+      <c r="AY137" s="46"/>
+      <c r="AZ137" s="46"/>
+      <c r="BA137" s="46"/>
+      <c r="BB137" s="46"/>
+      <c r="BC137" s="46"/>
+      <c r="BD137" s="46"/>
+      <c r="BE137" s="46"/>
+      <c r="BF137" s="46"/>
+      <c r="BG137" s="46"/>
+      <c r="BH137" s="46"/>
+      <c r="BI137" s="46"/>
+      <c r="BJ137" s="46"/>
+      <c r="BK137" s="46"/>
+      <c r="BL137" s="46"/>
+      <c r="BM137" s="46"/>
+      <c r="BN137" s="46"/>
+      <c r="BO137" s="46"/>
+    </row>
+    <row r="138" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="23"/>
+      <c r="B138" s="65"/>
+      <c r="D138" s="70"/>
+      <c r="E138" s="66"/>
+      <c r="F138" s="42"/>
+      <c r="G138" s="43"/>
+      <c r="H138" s="25"/>
+      <c r="I138" s="26"/>
+      <c r="J138" s="27"/>
+      <c r="K138" s="40"/>
+      <c r="L138" s="46"/>
+      <c r="M138" s="46"/>
+      <c r="N138" s="46"/>
+      <c r="O138" s="46"/>
+      <c r="P138" s="46"/>
+      <c r="Q138" s="46"/>
+      <c r="R138" s="46"/>
+      <c r="S138" s="46"/>
+      <c r="T138" s="46"/>
+      <c r="U138" s="46"/>
+      <c r="V138" s="46"/>
+      <c r="W138" s="46"/>
+      <c r="X138" s="46"/>
+      <c r="Y138" s="46"/>
+      <c r="Z138" s="46"/>
+      <c r="AA138" s="46"/>
+      <c r="AB138" s="46"/>
+      <c r="AC138" s="46"/>
+      <c r="AD138" s="46"/>
+      <c r="AE138" s="46"/>
+      <c r="AF138" s="46"/>
+      <c r="AG138" s="46"/>
+      <c r="AH138" s="46"/>
+      <c r="AI138" s="46"/>
+      <c r="AJ138" s="46"/>
+      <c r="AK138" s="46"/>
+      <c r="AL138" s="46"/>
+      <c r="AM138" s="46"/>
+      <c r="AN138" s="46"/>
+      <c r="AO138" s="46"/>
+      <c r="AP138" s="46"/>
+      <c r="AQ138" s="46"/>
+      <c r="AR138" s="46"/>
+      <c r="AS138" s="46"/>
+      <c r="AT138" s="46"/>
+      <c r="AU138" s="46"/>
+      <c r="AV138" s="46"/>
+      <c r="AW138" s="46"/>
+      <c r="AX138" s="46"/>
+      <c r="AY138" s="46"/>
+      <c r="AZ138" s="46"/>
+      <c r="BA138" s="46"/>
+      <c r="BB138" s="46"/>
+      <c r="BC138" s="46"/>
+      <c r="BD138" s="46"/>
+      <c r="BE138" s="46"/>
+      <c r="BF138" s="46"/>
+      <c r="BG138" s="46"/>
+      <c r="BH138" s="46"/>
+      <c r="BI138" s="46"/>
+      <c r="BJ138" s="46"/>
+      <c r="BK138" s="46"/>
+      <c r="BL138" s="46"/>
+      <c r="BM138" s="46"/>
+      <c r="BN138" s="46"/>
+      <c r="BO138" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -13883,19 +14129,10 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I100">
-    <cfRule type="dataBar" priority="181">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I102">
+    <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13909,66 +14146,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="87" priority="224">
+    <cfRule type="expression" dxfId="97" priority="235">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L101:BO103 M104:BN109 BO107:BO109 L110:BO112 M113:BN118 BO116:BO118 L119:BO121 M122:BN127 BO125:BO127 L128:BO130 M131:BN136 BO134:BO136 M97:BN100 BO99:BO100">
-    <cfRule type="expression" dxfId="86" priority="227">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L103:BO105 M106:BN111 BO109:BO111 L112:BO114 M115:BN120 BO118:BO120 L121:BO123 M124:BN129 BO127:BO129 L130:BO132 M133:BN138 BO136:BO138 M98:BN102 BO101:BO102">
+    <cfRule type="expression" dxfId="96" priority="238">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="228">
+    <cfRule type="expression" dxfId="95" priority="239">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO100">
-    <cfRule type="expression" dxfId="84" priority="187">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO102">
+    <cfRule type="expression" dxfId="94" priority="198">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="83" priority="177">
+    <cfRule type="expression" dxfId="93" priority="188">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E137:E1048576 E95:E100">
-    <cfRule type="cellIs" dxfId="82" priority="168" operator="equal">
+  <conditionalFormatting sqref="E1:E73 E139:E1048576 E95:E96 E98:E102">
+    <cfRule type="cellIs" dxfId="92" priority="179" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="181" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="182" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="183" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="184" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="185" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="186" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="75" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="180" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="74" priority="233">
+    <cfRule type="expression" dxfId="84" priority="244">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="234">
+    <cfRule type="expression" dxfId="83" priority="245">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I84">
-    <cfRule type="dataBar" priority="163">
+    <cfRule type="dataBar" priority="174">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -13982,51 +14219,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="72" priority="164">
+    <cfRule type="expression" dxfId="82" priority="175">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="165">
+    <cfRule type="expression" dxfId="81" priority="176">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="70" priority="162">
+    <cfRule type="expression" dxfId="80" priority="173">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="69" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="166" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="167" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="168" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="169" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="170" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="171" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="172" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="62" priority="166">
+    <cfRule type="expression" dxfId="72" priority="177">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="167">
+    <cfRule type="expression" dxfId="71" priority="178">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I101:I109">
-    <cfRule type="dataBar" priority="72">
+  <conditionalFormatting sqref="I103:I111">
+    <cfRule type="dataBar" priority="83">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14039,44 +14276,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L101:BO109">
-    <cfRule type="expression" dxfId="60" priority="71">
+  <conditionalFormatting sqref="L103:BO111">
+    <cfRule type="expression" dxfId="70" priority="82">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E101:E109">
-    <cfRule type="cellIs" dxfId="59" priority="64" operator="equal">
+  <conditionalFormatting sqref="E103:E111">
+    <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="79" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="80" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="81" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L104:BO109 L97:BO100">
-    <cfRule type="expression" dxfId="52" priority="75">
+  <conditionalFormatting sqref="L106:BO111 L98:BO102">
+    <cfRule type="expression" dxfId="62" priority="86">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="76">
+    <cfRule type="expression" dxfId="61" priority="87">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I110:I118">
-    <cfRule type="dataBar" priority="59">
+  <conditionalFormatting sqref="I112:I120">
+    <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14089,44 +14326,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L110:BO118">
-    <cfRule type="expression" dxfId="50" priority="58">
+  <conditionalFormatting sqref="L112:BO120">
+    <cfRule type="expression" dxfId="60" priority="69">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E110:E118">
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
+  <conditionalFormatting sqref="E112:E120">
+    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="67" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="68" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L113:BO118">
-    <cfRule type="expression" dxfId="42" priority="62">
+  <conditionalFormatting sqref="L115:BO120">
+    <cfRule type="expression" dxfId="52" priority="73">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="63">
+    <cfRule type="expression" dxfId="51" priority="74">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I119:I127">
-    <cfRule type="dataBar" priority="46">
+  <conditionalFormatting sqref="I121:I129">
+    <cfRule type="dataBar" priority="57">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14139,44 +14376,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L119:BO127">
-    <cfRule type="expression" dxfId="40" priority="45">
+  <conditionalFormatting sqref="L121:BO129">
+    <cfRule type="expression" dxfId="50" priority="56">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E119:E127">
-    <cfRule type="cellIs" dxfId="39" priority="38" operator="equal">
+  <conditionalFormatting sqref="E121:E129">
+    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="52" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="53" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="54" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="55" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L122:BO127">
-    <cfRule type="expression" dxfId="32" priority="49">
+  <conditionalFormatting sqref="L124:BO129">
+    <cfRule type="expression" dxfId="42" priority="60">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="50">
+    <cfRule type="expression" dxfId="41" priority="61">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I128:I136">
-    <cfRule type="dataBar" priority="33">
+  <conditionalFormatting sqref="I130:I138">
+    <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14189,44 +14426,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L128:BO136">
-    <cfRule type="expression" dxfId="30" priority="32">
+  <conditionalFormatting sqref="L130:BO138">
+    <cfRule type="expression" dxfId="40" priority="43">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E128:E136">
-    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+  <conditionalFormatting sqref="E130:E138">
+    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L131:BO136">
-    <cfRule type="expression" dxfId="22" priority="36">
+  <conditionalFormatting sqref="L133:BO138">
+    <cfRule type="expression" dxfId="32" priority="47">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="37">
+    <cfRule type="expression" dxfId="31" priority="48">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85:I86">
-    <cfRule type="dataBar" priority="20">
+    <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14240,11 +14477,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:BO86">
+    <cfRule type="expression" dxfId="30" priority="30">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E86">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
+    <cfRule type="expression" dxfId="22" priority="21">
+      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87:I94">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E86">
+  <conditionalFormatting sqref="E87:E94">
     <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14267,15 +14554,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="12" priority="10">
-      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="11">
-      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I94">
+  <conditionalFormatting sqref="I97">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14284,17 +14571,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E94">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14373,7 +14660,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I100</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I102</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14403,7 +14690,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I101:I109</xm:sqref>
+          <xm:sqref>I103:I111</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14418,7 +14705,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I110:I118</xm:sqref>
+          <xm:sqref>I112:I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14433,7 +14720,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I119:I127</xm:sqref>
+          <xm:sqref>I121:I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14448,7 +14735,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I128:I136</xm:sqref>
+          <xm:sqref>I130:I138</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -14479,6 +14766,21 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>I87:I94</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{52A4FA6B-6481-4B97-9D81-1C74885277E0}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I97</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added better data import system (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E796B6-BB0D-4C88-BE5D-A88DC96221D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29F3A25-BE12-4668-8486-455239545772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="123">
   <si>
     <t>WBS</t>
   </si>
@@ -794,6 +794,9 @@
   </si>
   <si>
     <t>Structural Model Key Variables Forecasts</t>
+  </si>
+  <si>
+    <t>Revise Data Imports</t>
   </si>
 </sst>
 </file>
@@ -1722,6 +1725,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1731,6 +1741,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1739,17 +1753,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3038,11 +3041,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO138"/>
+  <dimension ref="A1:BO139"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
+      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3072,27 +3075,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3137,12 +3140,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3152,183 +3155,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8486,7 +8489,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A103" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A104" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11271,7 +11274,7 @@
         <v>9.1</v>
       </c>
       <c r="B98" s="65" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D98" s="70"/>
       <c r="E98" s="66" t="s">
@@ -11280,9 +11283,13 @@
       <c r="F98" s="42">
         <v>44342</v>
       </c>
-      <c r="G98" s="43"/>
+      <c r="G98" s="43">
+        <v>44346</v>
+      </c>
       <c r="H98" s="25"/>
-      <c r="I98" s="26"/>
+      <c r="I98" s="26">
+        <v>0.5</v>
+      </c>
       <c r="J98" s="27"/>
       <c r="K98" s="40"/>
       <c r="L98" s="46"/>
@@ -11348,15 +11355,13 @@
         <v>9.2</v>
       </c>
       <c r="B99" s="65" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D99" s="70"/>
       <c r="E99" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F99" s="42">
-        <v>44344</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F99" s="42"/>
       <c r="G99" s="43"/>
       <c r="H99" s="25"/>
       <c r="I99" s="26"/>
@@ -11425,14 +11430,14 @@
         <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F100" s="42">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="G100" s="43"/>
       <c r="H100" s="25"/>
@@ -11502,14 +11507,14 @@
         <v>9.4</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F101" s="42">
-        <v>44348</v>
+        <v>44343</v>
       </c>
       <c r="G101" s="43"/>
       <c r="H101" s="25"/>
@@ -11579,7 +11584,7 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
@@ -11655,10 +11660,10 @@
         <f t="shared" si="9"/>
         <v>9.6</v>
       </c>
-      <c r="B103" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D103" s="66"/>
+      <c r="B103" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D103" s="70"/>
       <c r="E103" s="66" t="s">
         <v>67</v>
       </c>
@@ -11728,11 +11733,20 @@
       <c r="BO103" s="46"/>
     </row>
     <row r="104" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="23"/>
-      <c r="B104" s="65"/>
+      <c r="A104" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>9.7</v>
+      </c>
+      <c r="B104" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D104" s="66"/>
-      <c r="E104" s="66"/>
-      <c r="F104" s="42"/>
+      <c r="E104" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F104" s="42">
+        <v>44348</v>
+      </c>
       <c r="G104" s="43"/>
       <c r="H104" s="25"/>
       <c r="I104" s="26"/>
@@ -11934,7 +11948,7 @@
     <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="23"/>
       <c r="B107" s="65"/>
-      <c r="D107" s="70"/>
+      <c r="D107" s="66"/>
       <c r="E107" s="66"/>
       <c r="F107" s="42"/>
       <c r="G107" s="43"/>
@@ -12274,7 +12288,7 @@
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="23"/>
       <c r="B112" s="65"/>
-      <c r="D112" s="66"/>
+      <c r="D112" s="70"/>
       <c r="E112" s="66"/>
       <c r="F112" s="42"/>
       <c r="G112" s="43"/>
@@ -12546,7 +12560,7 @@
     <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="23"/>
       <c r="B116" s="65"/>
-      <c r="D116" s="70"/>
+      <c r="D116" s="66"/>
       <c r="E116" s="66"/>
       <c r="F116" s="42"/>
       <c r="G116" s="43"/>
@@ -12886,7 +12900,7 @@
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="23"/>
       <c r="B121" s="65"/>
-      <c r="D121" s="66"/>
+      <c r="D121" s="70"/>
       <c r="E121" s="66"/>
       <c r="F121" s="42"/>
       <c r="G121" s="43"/>
@@ -13158,7 +13172,7 @@
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23"/>
       <c r="B125" s="65"/>
-      <c r="D125" s="70"/>
+      <c r="D125" s="66"/>
       <c r="E125" s="66"/>
       <c r="F125" s="42"/>
       <c r="G125" s="43"/>
@@ -13498,7 +13512,7 @@
     <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="23"/>
       <c r="B130" s="65"/>
-      <c r="D130" s="66"/>
+      <c r="D130" s="70"/>
       <c r="E130" s="66"/>
       <c r="F130" s="42"/>
       <c r="G130" s="43"/>
@@ -13770,7 +13784,7 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23"/>
       <c r="B134" s="65"/>
-      <c r="D134" s="70"/>
+      <c r="D134" s="66"/>
       <c r="E134" s="66"/>
       <c r="F134" s="42"/>
       <c r="G134" s="43"/>
@@ -14107,18 +14121,77 @@
       <c r="BN138" s="46"/>
       <c r="BO138" s="46"/>
     </row>
+    <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="23"/>
+      <c r="B139" s="65"/>
+      <c r="D139" s="70"/>
+      <c r="E139" s="66"/>
+      <c r="F139" s="42"/>
+      <c r="G139" s="43"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="26"/>
+      <c r="J139" s="27"/>
+      <c r="K139" s="40"/>
+      <c r="L139" s="46"/>
+      <c r="M139" s="46"/>
+      <c r="N139" s="46"/>
+      <c r="O139" s="46"/>
+      <c r="P139" s="46"/>
+      <c r="Q139" s="46"/>
+      <c r="R139" s="46"/>
+      <c r="S139" s="46"/>
+      <c r="T139" s="46"/>
+      <c r="U139" s="46"/>
+      <c r="V139" s="46"/>
+      <c r="W139" s="46"/>
+      <c r="X139" s="46"/>
+      <c r="Y139" s="46"/>
+      <c r="Z139" s="46"/>
+      <c r="AA139" s="46"/>
+      <c r="AB139" s="46"/>
+      <c r="AC139" s="46"/>
+      <c r="AD139" s="46"/>
+      <c r="AE139" s="46"/>
+      <c r="AF139" s="46"/>
+      <c r="AG139" s="46"/>
+      <c r="AH139" s="46"/>
+      <c r="AI139" s="46"/>
+      <c r="AJ139" s="46"/>
+      <c r="AK139" s="46"/>
+      <c r="AL139" s="46"/>
+      <c r="AM139" s="46"/>
+      <c r="AN139" s="46"/>
+      <c r="AO139" s="46"/>
+      <c r="AP139" s="46"/>
+      <c r="AQ139" s="46"/>
+      <c r="AR139" s="46"/>
+      <c r="AS139" s="46"/>
+      <c r="AT139" s="46"/>
+      <c r="AU139" s="46"/>
+      <c r="AV139" s="46"/>
+      <c r="AW139" s="46"/>
+      <c r="AX139" s="46"/>
+      <c r="AY139" s="46"/>
+      <c r="AZ139" s="46"/>
+      <c r="BA139" s="46"/>
+      <c r="BB139" s="46"/>
+      <c r="BC139" s="46"/>
+      <c r="BD139" s="46"/>
+      <c r="BE139" s="46"/>
+      <c r="BF139" s="46"/>
+      <c r="BG139" s="46"/>
+      <c r="BH139" s="46"/>
+      <c r="BI139" s="46"/>
+      <c r="BJ139" s="46"/>
+      <c r="BK139" s="46"/>
+      <c r="BL139" s="46"/>
+      <c r="BM139" s="46"/>
+      <c r="BN139" s="46"/>
+      <c r="BO139" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -14129,9 +14202,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I102">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103">
     <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14150,7 +14232,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L103:BO105 M106:BN111 BO109:BO111 L112:BO114 M115:BN120 BO118:BO120 L121:BO123 M124:BN129 BO127:BO129 L130:BO132 M133:BN138 BO136:BO138 M98:BN102 BO101:BO102">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L104:BO106 M107:BN112 BO110:BO112 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L131:BO133 M134:BN139 BO137:BO139 M98:BN103 BO102:BO103">
     <cfRule type="expression" dxfId="96" priority="238">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -14158,7 +14240,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO102">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103">
     <cfRule type="expression" dxfId="94" priority="198">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -14168,7 +14250,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E139:E1048576 E95:E96 E98:E102">
+  <conditionalFormatting sqref="E1:E73 E140:E1048576 E95:E96 E98:E103">
     <cfRule type="cellIs" dxfId="92" priority="179" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14262,7 +14344,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I103:I111">
+  <conditionalFormatting sqref="I104:I112">
     <cfRule type="dataBar" priority="83">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14276,12 +14358,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L103:BO111">
+  <conditionalFormatting sqref="L104:BO112">
     <cfRule type="expression" dxfId="70" priority="82">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E103:E111">
+  <conditionalFormatting sqref="E104:E112">
     <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14304,7 +14386,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L106:BO111 L98:BO102">
+  <conditionalFormatting sqref="L107:BO112 L98:BO103">
     <cfRule type="expression" dxfId="62" priority="86">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14312,7 +14394,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I112:I120">
+  <conditionalFormatting sqref="I113:I121">
     <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14326,12 +14408,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L112:BO120">
+  <conditionalFormatting sqref="L113:BO121">
     <cfRule type="expression" dxfId="60" priority="69">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E112:E120">
+  <conditionalFormatting sqref="E113:E121">
     <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14354,7 +14436,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L115:BO120">
+  <conditionalFormatting sqref="L116:BO121">
     <cfRule type="expression" dxfId="52" priority="73">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14362,7 +14444,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I121:I129">
+  <conditionalFormatting sqref="I122:I130">
     <cfRule type="dataBar" priority="57">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14376,12 +14458,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L121:BO129">
+  <conditionalFormatting sqref="L122:BO130">
     <cfRule type="expression" dxfId="50" priority="56">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E121:E129">
+  <conditionalFormatting sqref="E122:E130">
     <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14404,7 +14486,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L124:BO129">
+  <conditionalFormatting sqref="L125:BO130">
     <cfRule type="expression" dxfId="42" priority="60">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14412,7 +14494,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I130:I138">
+  <conditionalFormatting sqref="I131:I139">
     <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14426,12 +14508,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L130:BO138">
+  <conditionalFormatting sqref="L131:BO139">
     <cfRule type="expression" dxfId="40" priority="43">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E130:E138">
+  <conditionalFormatting sqref="E131:E139">
     <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14454,7 +14536,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L133:BO138">
+  <conditionalFormatting sqref="L134:BO139">
     <cfRule type="expression" dxfId="32" priority="47">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14660,7 +14742,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I98:I102</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I103</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14690,7 +14772,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I103:I111</xm:sqref>
+          <xm:sqref>I104:I112</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14705,7 +14787,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I112:I120</xm:sqref>
+          <xm:sqref>I113:I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14720,7 +14802,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I121:I129</xm:sqref>
+          <xm:sqref>I122:I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14735,7 +14817,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I130:I138</xm:sqref>
+          <xm:sqref>I131:I139</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">

</xml_diff>

<commit_message>
Added cleaner stationary transforms (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29F3A25-BE12-4668-8486-455239545772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9996C05-033E-4808-880F-E87591BCEC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
   <si>
     <t>WBS</t>
   </si>
@@ -797,6 +797,9 @@
   </si>
   <si>
     <t>Revise Data Imports</t>
+  </si>
+  <si>
+    <t>Revise Data Transforms</t>
   </si>
 </sst>
 </file>
@@ -1725,13 +1728,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1741,10 +1737,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1753,6 +1745,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3041,11 +3044,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO139"/>
+  <dimension ref="A1:BO140"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B99" sqref="B99"/>
+      <pane ySplit="7" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3075,27 +3078,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3140,12 +3143,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3155,183 +3158,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8489,7 +8492,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A104" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A105" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11288,7 +11291,7 @@
       </c>
       <c r="H98" s="25"/>
       <c r="I98" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J98" s="27"/>
       <c r="K98" s="40"/>
@@ -11355,16 +11358,22 @@
         <v>9.2</v>
       </c>
       <c r="B99" s="65" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D99" s="70"/>
       <c r="E99" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F99" s="42"/>
-      <c r="G99" s="43"/>
+      <c r="F99" s="42">
+        <v>44346</v>
+      </c>
+      <c r="G99" s="43">
+        <v>44347</v>
+      </c>
       <c r="H99" s="25"/>
-      <c r="I99" s="26"/>
+      <c r="I99" s="26">
+        <v>1</v>
+      </c>
       <c r="J99" s="27"/>
       <c r="K99" s="40"/>
       <c r="L99" s="46"/>
@@ -11430,15 +11439,13 @@
         <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F100" s="42">
-        <v>44344</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="F100" s="42"/>
       <c r="G100" s="43"/>
       <c r="H100" s="25"/>
       <c r="I100" s="26"/>
@@ -11507,14 +11514,14 @@
         <v>9.4</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F101" s="42">
-        <v>44343</v>
+        <v>44344</v>
       </c>
       <c r="G101" s="43"/>
       <c r="H101" s="25"/>
@@ -11584,14 +11591,14 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F102" s="42">
-        <v>44348</v>
+        <v>44343</v>
       </c>
       <c r="G102" s="43"/>
       <c r="H102" s="25"/>
@@ -11661,7 +11668,7 @@
         <v>9.6</v>
       </c>
       <c r="B103" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D103" s="70"/>
       <c r="E103" s="66" t="s">
@@ -11737,10 +11744,10 @@
         <f t="shared" si="9"/>
         <v>9.7</v>
       </c>
-      <c r="B104" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D104" s="66"/>
+      <c r="B104" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D104" s="70"/>
       <c r="E104" s="66" t="s">
         <v>67</v>
       </c>
@@ -11810,11 +11817,20 @@
       <c r="BO104" s="46"/>
     </row>
     <row r="105" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="23"/>
-      <c r="B105" s="65"/>
+      <c r="A105" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>9.8</v>
+      </c>
+      <c r="B105" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D105" s="66"/>
-      <c r="E105" s="66"/>
-      <c r="F105" s="42"/>
+      <c r="E105" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F105" s="42">
+        <v>44348</v>
+      </c>
       <c r="G105" s="43"/>
       <c r="H105" s="25"/>
       <c r="I105" s="26"/>
@@ -12016,7 +12032,7 @@
     <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="23"/>
       <c r="B108" s="65"/>
-      <c r="D108" s="70"/>
+      <c r="D108" s="66"/>
       <c r="E108" s="66"/>
       <c r="F108" s="42"/>
       <c r="G108" s="43"/>
@@ -12356,7 +12372,7 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23"/>
       <c r="B113" s="65"/>
-      <c r="D113" s="66"/>
+      <c r="D113" s="70"/>
       <c r="E113" s="66"/>
       <c r="F113" s="42"/>
       <c r="G113" s="43"/>
@@ -12628,7 +12644,7 @@
     <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="23"/>
       <c r="B117" s="65"/>
-      <c r="D117" s="70"/>
+      <c r="D117" s="66"/>
       <c r="E117" s="66"/>
       <c r="F117" s="42"/>
       <c r="G117" s="43"/>
@@ -12968,7 +12984,7 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
       <c r="B122" s="65"/>
-      <c r="D122" s="66"/>
+      <c r="D122" s="70"/>
       <c r="E122" s="66"/>
       <c r="F122" s="42"/>
       <c r="G122" s="43"/>
@@ -13240,7 +13256,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="70"/>
+      <c r="D126" s="66"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -13580,7 +13596,7 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
       <c r="B131" s="65"/>
-      <c r="D131" s="66"/>
+      <c r="D131" s="70"/>
       <c r="E131" s="66"/>
       <c r="F131" s="42"/>
       <c r="G131" s="43"/>
@@ -13852,7 +13868,7 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
       <c r="B135" s="65"/>
-      <c r="D135" s="70"/>
+      <c r="D135" s="66"/>
       <c r="E135" s="66"/>
       <c r="F135" s="42"/>
       <c r="G135" s="43"/>
@@ -14189,9 +14205,86 @@
       <c r="BN139" s="46"/>
       <c r="BO139" s="46"/>
     </row>
+    <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="23"/>
+      <c r="B140" s="65"/>
+      <c r="D140" s="70"/>
+      <c r="E140" s="66"/>
+      <c r="F140" s="42"/>
+      <c r="G140" s="43"/>
+      <c r="H140" s="25"/>
+      <c r="I140" s="26"/>
+      <c r="J140" s="27"/>
+      <c r="K140" s="40"/>
+      <c r="L140" s="46"/>
+      <c r="M140" s="46"/>
+      <c r="N140" s="46"/>
+      <c r="O140" s="46"/>
+      <c r="P140" s="46"/>
+      <c r="Q140" s="46"/>
+      <c r="R140" s="46"/>
+      <c r="S140" s="46"/>
+      <c r="T140" s="46"/>
+      <c r="U140" s="46"/>
+      <c r="V140" s="46"/>
+      <c r="W140" s="46"/>
+      <c r="X140" s="46"/>
+      <c r="Y140" s="46"/>
+      <c r="Z140" s="46"/>
+      <c r="AA140" s="46"/>
+      <c r="AB140" s="46"/>
+      <c r="AC140" s="46"/>
+      <c r="AD140" s="46"/>
+      <c r="AE140" s="46"/>
+      <c r="AF140" s="46"/>
+      <c r="AG140" s="46"/>
+      <c r="AH140" s="46"/>
+      <c r="AI140" s="46"/>
+      <c r="AJ140" s="46"/>
+      <c r="AK140" s="46"/>
+      <c r="AL140" s="46"/>
+      <c r="AM140" s="46"/>
+      <c r="AN140" s="46"/>
+      <c r="AO140" s="46"/>
+      <c r="AP140" s="46"/>
+      <c r="AQ140" s="46"/>
+      <c r="AR140" s="46"/>
+      <c r="AS140" s="46"/>
+      <c r="AT140" s="46"/>
+      <c r="AU140" s="46"/>
+      <c r="AV140" s="46"/>
+      <c r="AW140" s="46"/>
+      <c r="AX140" s="46"/>
+      <c r="AY140" s="46"/>
+      <c r="AZ140" s="46"/>
+      <c r="BA140" s="46"/>
+      <c r="BB140" s="46"/>
+      <c r="BC140" s="46"/>
+      <c r="BD140" s="46"/>
+      <c r="BE140" s="46"/>
+      <c r="BF140" s="46"/>
+      <c r="BG140" s="46"/>
+      <c r="BH140" s="46"/>
+      <c r="BI140" s="46"/>
+      <c r="BJ140" s="46"/>
+      <c r="BK140" s="46"/>
+      <c r="BL140" s="46"/>
+      <c r="BM140" s="46"/>
+      <c r="BN140" s="46"/>
+      <c r="BO140" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -14202,18 +14295,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I104">
     <cfRule type="dataBar" priority="192">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14232,7 +14316,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L104:BO106 M107:BN112 BO110:BO112 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L131:BO133 M134:BN139 BO137:BO139 M98:BN103 BO102:BO103">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L105:BO107 M108:BN113 BO111:BO113 L114:BO116 M117:BN122 BO120:BO122 L123:BO125 M126:BN131 BO129:BO131 L132:BO134 M135:BN140 BO138:BO140 M98:BN104 BO103:BO104">
     <cfRule type="expression" dxfId="96" priority="238">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -14240,7 +14324,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO104">
     <cfRule type="expression" dxfId="94" priority="198">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -14250,7 +14334,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E140:E1048576 E95:E96 E98:E103">
+  <conditionalFormatting sqref="E1:E73 E141:E1048576 E95:E96 E98:E104">
     <cfRule type="cellIs" dxfId="92" priority="179" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14344,7 +14428,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I104:I112">
+  <conditionalFormatting sqref="I105:I113">
     <cfRule type="dataBar" priority="83">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14358,12 +14442,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L104:BO112">
+  <conditionalFormatting sqref="L105:BO113">
     <cfRule type="expression" dxfId="70" priority="82">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E104:E112">
+  <conditionalFormatting sqref="E105:E113">
     <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14386,7 +14470,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L107:BO112 L98:BO103">
+  <conditionalFormatting sqref="L108:BO113 L98:BO104">
     <cfRule type="expression" dxfId="62" priority="86">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14394,7 +14478,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I113:I121">
+  <conditionalFormatting sqref="I114:I122">
     <cfRule type="dataBar" priority="70">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14408,12 +14492,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L113:BO121">
+  <conditionalFormatting sqref="L114:BO122">
     <cfRule type="expression" dxfId="60" priority="69">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113:E121">
+  <conditionalFormatting sqref="E114:E122">
     <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14436,7 +14520,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L116:BO121">
+  <conditionalFormatting sqref="L117:BO122">
     <cfRule type="expression" dxfId="52" priority="73">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14444,7 +14528,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122:I130">
+  <conditionalFormatting sqref="I123:I131">
     <cfRule type="dataBar" priority="57">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14458,12 +14542,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L122:BO130">
+  <conditionalFormatting sqref="L123:BO131">
     <cfRule type="expression" dxfId="50" priority="56">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122:E130">
+  <conditionalFormatting sqref="E123:E131">
     <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14486,7 +14570,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO130">
+  <conditionalFormatting sqref="L126:BO131">
     <cfRule type="expression" dxfId="42" priority="60">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14494,7 +14578,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I131:I139">
+  <conditionalFormatting sqref="I132:I140">
     <cfRule type="dataBar" priority="44">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14508,12 +14592,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L131:BO139">
+  <conditionalFormatting sqref="L132:BO140">
     <cfRule type="expression" dxfId="40" priority="43">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131:E139">
+  <conditionalFormatting sqref="E132:E140">
     <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14536,7 +14620,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L134:BO139">
+  <conditionalFormatting sqref="L135:BO140">
     <cfRule type="expression" dxfId="32" priority="47">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -14742,7 +14826,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I98:I103</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I104</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14772,7 +14856,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I104:I112</xm:sqref>
+          <xm:sqref>I105:I113</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14787,7 +14871,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I113:I121</xm:sqref>
+          <xm:sqref>I114:I122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14802,7 +14886,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I122:I130</xm:sqref>
+          <xm:sqref>I123:I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14817,7 +14901,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I131:I139</xm:sqref>
+          <xm:sqref>I132:I140</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">

</xml_diff>

<commit_message>
Added CME cookie bypass (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9996C05-033E-4808-880F-E87591BCEC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0EAF535-312E-437E-B257-0E29F3D9B9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2145" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="131">
   <si>
     <t>WBS</t>
   </si>
@@ -790,16 +790,37 @@
     <t>Improve Inflation Forecasts</t>
   </si>
   <si>
-    <t>Generate Full 5-Year Forecasts of All Key Variables</t>
-  </si>
-  <si>
-    <t>Structural Model Key Variables Forecasts</t>
-  </si>
-  <si>
     <t>Revise Data Imports</t>
   </si>
   <si>
     <t>Revise Data Transforms</t>
+  </si>
+  <si>
+    <t>Add Qualitative Forecast System</t>
+  </si>
+  <si>
+    <t>Add Structural Equations</t>
+  </si>
+  <si>
+    <t>Add Structural Estimation</t>
+  </si>
+  <si>
+    <t>Add Structural Forecasting</t>
+  </si>
+  <si>
+    <t>Add IRFs</t>
+  </si>
+  <si>
+    <t>Add Scenarios</t>
+  </si>
+  <si>
+    <t>Structural Model</t>
+  </si>
+  <si>
+    <t>UI Improvements</t>
+  </si>
+  <si>
+    <t>Add Baseline Qualitative-Adjustable Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1728,6 +1749,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1737,6 +1765,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1745,17 +1777,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1804,7 +1825,82 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="108">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3044,11 +3140,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO140"/>
+  <dimension ref="A1:BO147"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
+      <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O104" sqref="O104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3078,27 +3174,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3143,12 +3239,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3158,183 +3254,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8492,7 +8588,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A105" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A112" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11198,7 +11294,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="19"/>
@@ -11277,7 +11373,7 @@
         <v>9.1</v>
       </c>
       <c r="B98" s="65" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D98" s="70"/>
       <c r="E98" s="66" t="s">
@@ -11287,7 +11383,7 @@
         <v>44342</v>
       </c>
       <c r="G98" s="43">
-        <v>44346</v>
+        <v>44347</v>
       </c>
       <c r="H98" s="25"/>
       <c r="I98" s="26">
@@ -11358,7 +11454,7 @@
         <v>9.2</v>
       </c>
       <c r="B99" s="65" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D99" s="70"/>
       <c r="E99" s="66" t="s">
@@ -11439,13 +11535,15 @@
         <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F100" s="42"/>
+      <c r="F100" s="42">
+        <v>44348</v>
+      </c>
       <c r="G100" s="43"/>
       <c r="H100" s="25"/>
       <c r="I100" s="26"/>
@@ -11514,14 +11612,14 @@
         <v>9.4</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F101" s="42">
-        <v>44344</v>
+        <v>44349</v>
       </c>
       <c r="G101" s="43"/>
       <c r="H101" s="25"/>
@@ -11591,14 +11689,14 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>107</v>
+        <v>123</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F102" s="42">
-        <v>44343</v>
+        <v>44351</v>
       </c>
       <c r="G102" s="43"/>
       <c r="H102" s="25"/>
@@ -11668,14 +11766,14 @@
         <v>9.6</v>
       </c>
       <c r="B103" s="65" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D103" s="70"/>
       <c r="E103" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F103" s="42">
-        <v>44348</v>
+        <v>44351</v>
       </c>
       <c r="G103" s="43"/>
       <c r="H103" s="25"/>
@@ -11745,14 +11843,14 @@
         <v>9.7</v>
       </c>
       <c r="B104" s="65" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="D104" s="70"/>
       <c r="E104" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F104" s="42">
-        <v>44348</v>
+        <v>44351</v>
       </c>
       <c r="G104" s="43"/>
       <c r="H104" s="25"/>
@@ -11821,15 +11919,15 @@
         <f t="shared" si="9"/>
         <v>9.8</v>
       </c>
-      <c r="B105" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D105" s="66"/>
+      <c r="B105" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D105" s="70"/>
       <c r="E105" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F105" s="42">
-        <v>44348</v>
+        <v>44358</v>
       </c>
       <c r="G105" s="43"/>
       <c r="H105" s="25"/>
@@ -11894,11 +11992,20 @@
       <c r="BO105" s="46"/>
     </row>
     <row r="106" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="23"/>
-      <c r="B106" s="65"/>
-      <c r="D106" s="66"/>
-      <c r="E106" s="66"/>
-      <c r="F106" s="42"/>
+      <c r="A106" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>9.9</v>
+      </c>
+      <c r="B106" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D106" s="70"/>
+      <c r="E106" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F106" s="42">
+        <v>44358</v>
+      </c>
       <c r="G106" s="43"/>
       <c r="H106" s="25"/>
       <c r="I106" s="26"/>
@@ -11961,80 +12068,100 @@
       <c r="BN106" s="46"/>
       <c r="BO106" s="46"/>
     </row>
-    <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="23"/>
-      <c r="B107" s="65"/>
-      <c r="D107" s="66"/>
-      <c r="E107" s="66"/>
-      <c r="F107" s="42"/>
-      <c r="G107" s="43"/>
-      <c r="H107" s="25"/>
-      <c r="I107" s="26"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="40"/>
-      <c r="L107" s="46"/>
-      <c r="M107" s="46"/>
-      <c r="N107" s="46"/>
-      <c r="O107" s="46"/>
-      <c r="P107" s="46"/>
-      <c r="Q107" s="46"/>
-      <c r="R107" s="46"/>
-      <c r="S107" s="46"/>
-      <c r="T107" s="46"/>
-      <c r="U107" s="46"/>
-      <c r="V107" s="46"/>
-      <c r="W107" s="46"/>
-      <c r="X107" s="46"/>
-      <c r="Y107" s="46"/>
-      <c r="Z107" s="46"/>
-      <c r="AA107" s="46"/>
-      <c r="AB107" s="46"/>
-      <c r="AC107" s="46"/>
-      <c r="AD107" s="46"/>
-      <c r="AE107" s="46"/>
-      <c r="AF107" s="46"/>
-      <c r="AG107" s="46"/>
-      <c r="AH107" s="46"/>
-      <c r="AI107" s="46"/>
-      <c r="AJ107" s="46"/>
-      <c r="AK107" s="46"/>
-      <c r="AL107" s="46"/>
-      <c r="AM107" s="46"/>
-      <c r="AN107" s="46"/>
-      <c r="AO107" s="46"/>
-      <c r="AP107" s="46"/>
-      <c r="AQ107" s="46"/>
-      <c r="AR107" s="46"/>
-      <c r="AS107" s="46"/>
-      <c r="AT107" s="46"/>
-      <c r="AU107" s="46"/>
-      <c r="AV107" s="46"/>
-      <c r="AW107" s="46"/>
-      <c r="AX107" s="46"/>
-      <c r="AY107" s="46"/>
-      <c r="AZ107" s="46"/>
-      <c r="BA107" s="46"/>
-      <c r="BB107" s="46"/>
-      <c r="BC107" s="46"/>
-      <c r="BD107" s="46"/>
-      <c r="BE107" s="46"/>
-      <c r="BF107" s="46"/>
-      <c r="BG107" s="46"/>
-      <c r="BH107" s="46"/>
-      <c r="BI107" s="46"/>
-      <c r="BJ107" s="46"/>
-      <c r="BK107" s="46"/>
-      <c r="BL107" s="46"/>
-      <c r="BM107" s="46"/>
-      <c r="BN107" s="46"/>
-      <c r="BO107" s="46"/>
+    <row r="107" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>10</v>
+      </c>
+      <c r="B107" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="44" t="str">
+        <f t="shared" ref="G107" si="18">IF(ISBLANK(F107)," - ",IF(H107=0,F107,F107+H107-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H107" s="20"/>
+      <c r="I107" s="21"/>
+      <c r="J107" s="22" t="str">
+        <f t="shared" ref="J107" si="19">IF(OR(G107=0,F107=0)," - ",NETWORKDAYS(F107,G107))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K107" s="41"/>
+      <c r="L107" s="48"/>
+      <c r="M107" s="48"/>
+      <c r="N107" s="48"/>
+      <c r="O107" s="48"/>
+      <c r="P107" s="48"/>
+      <c r="Q107" s="48"/>
+      <c r="R107" s="48"/>
+      <c r="S107" s="48"/>
+      <c r="T107" s="48"/>
+      <c r="U107" s="48"/>
+      <c r="V107" s="48"/>
+      <c r="W107" s="48"/>
+      <c r="X107" s="48"/>
+      <c r="Y107" s="48"/>
+      <c r="Z107" s="48"/>
+      <c r="AA107" s="48"/>
+      <c r="AB107" s="48"/>
+      <c r="AC107" s="48"/>
+      <c r="AD107" s="48"/>
+      <c r="AE107" s="48"/>
+      <c r="AF107" s="48"/>
+      <c r="AG107" s="48"/>
+      <c r="AH107" s="48"/>
+      <c r="AI107" s="48"/>
+      <c r="AJ107" s="48"/>
+      <c r="AK107" s="48"/>
+      <c r="AL107" s="48"/>
+      <c r="AM107" s="48"/>
+      <c r="AN107" s="48"/>
+      <c r="AO107" s="48"/>
+      <c r="AP107" s="48"/>
+      <c r="AQ107" s="48"/>
+      <c r="AR107" s="48"/>
+      <c r="AS107" s="48"/>
+      <c r="AT107" s="48"/>
+      <c r="AU107" s="48"/>
+      <c r="AV107" s="48"/>
+      <c r="AW107" s="48"/>
+      <c r="AX107" s="48"/>
+      <c r="AY107" s="48"/>
+      <c r="AZ107" s="48"/>
+      <c r="BA107" s="48"/>
+      <c r="BB107" s="48"/>
+      <c r="BC107" s="48"/>
+      <c r="BD107" s="48"/>
+      <c r="BE107" s="48"/>
+      <c r="BF107" s="48"/>
+      <c r="BG107" s="48"/>
+      <c r="BH107" s="48"/>
+      <c r="BI107" s="48"/>
+      <c r="BJ107" s="48"/>
+      <c r="BK107" s="48"/>
+      <c r="BL107" s="48"/>
+      <c r="BM107" s="48"/>
+      <c r="BN107" s="48"/>
+      <c r="BO107" s="48"/>
     </row>
     <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="23"/>
-      <c r="B108" s="65"/>
-      <c r="D108" s="66"/>
-      <c r="E108" s="66"/>
-      <c r="F108" s="42"/>
+      <c r="A108" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.1</v>
+      </c>
+      <c r="B108" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D108" s="70"/>
+      <c r="E108" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="F108" s="42">
+        <v>44344</v>
+      </c>
       <c r="G108" s="43"/>
       <c r="H108" s="25"/>
       <c r="I108" s="26"/>
@@ -12098,11 +12225,20 @@
       <c r="BO108" s="46"/>
     </row>
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="23"/>
-      <c r="B109" s="65"/>
+      <c r="A109" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.2</v>
+      </c>
+      <c r="B109" s="65" t="s">
+        <v>107</v>
+      </c>
       <c r="D109" s="70"/>
-      <c r="E109" s="66"/>
-      <c r="F109" s="42"/>
+      <c r="E109" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="F109" s="42">
+        <v>44343</v>
+      </c>
       <c r="G109" s="43"/>
       <c r="H109" s="25"/>
       <c r="I109" s="26"/>
@@ -12166,11 +12302,20 @@
       <c r="BO109" s="46"/>
     </row>
     <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="23"/>
-      <c r="B110" s="65"/>
+      <c r="A110" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.3</v>
+      </c>
+      <c r="B110" s="65" t="s">
+        <v>108</v>
+      </c>
       <c r="D110" s="70"/>
-      <c r="E110" s="66"/>
-      <c r="F110" s="42"/>
+      <c r="E110" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F110" s="42">
+        <v>44348</v>
+      </c>
       <c r="G110" s="43"/>
       <c r="H110" s="25"/>
       <c r="I110" s="26"/>
@@ -12234,11 +12379,20 @@
       <c r="BO110" s="46"/>
     </row>
     <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="23"/>
-      <c r="B111" s="65"/>
+      <c r="A111" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.4</v>
+      </c>
+      <c r="B111" s="65" t="s">
+        <v>109</v>
+      </c>
       <c r="D111" s="70"/>
-      <c r="E111" s="66"/>
-      <c r="F111" s="42"/>
+      <c r="E111" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F111" s="42">
+        <v>44348</v>
+      </c>
       <c r="G111" s="43"/>
       <c r="H111" s="25"/>
       <c r="I111" s="26"/>
@@ -12302,11 +12456,20 @@
       <c r="BO111" s="46"/>
     </row>
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="23"/>
-      <c r="B112" s="65"/>
-      <c r="D112" s="70"/>
-      <c r="E112" s="66"/>
-      <c r="F112" s="42"/>
+      <c r="A112" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.5</v>
+      </c>
+      <c r="B112" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D112" s="66"/>
+      <c r="E112" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F112" s="42">
+        <v>44348</v>
+      </c>
       <c r="G112" s="43"/>
       <c r="H112" s="25"/>
       <c r="I112" s="26"/>
@@ -12372,7 +12535,7 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23"/>
       <c r="B113" s="65"/>
-      <c r="D113" s="70"/>
+      <c r="D113" s="66"/>
       <c r="E113" s="66"/>
       <c r="F113" s="42"/>
       <c r="G113" s="43"/>
@@ -12576,7 +12739,7 @@
     <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="23"/>
       <c r="B116" s="65"/>
-      <c r="D116" s="66"/>
+      <c r="D116" s="70"/>
       <c r="E116" s="66"/>
       <c r="F116" s="42"/>
       <c r="G116" s="43"/>
@@ -12644,7 +12807,7 @@
     <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="23"/>
       <c r="B117" s="65"/>
-      <c r="D117" s="66"/>
+      <c r="D117" s="70"/>
       <c r="E117" s="66"/>
       <c r="F117" s="42"/>
       <c r="G117" s="43"/>
@@ -12916,7 +13079,7 @@
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="23"/>
       <c r="B121" s="65"/>
-      <c r="D121" s="70"/>
+      <c r="D121" s="66"/>
       <c r="E121" s="66"/>
       <c r="F121" s="42"/>
       <c r="G121" s="43"/>
@@ -12984,7 +13147,7 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
       <c r="B122" s="65"/>
-      <c r="D122" s="70"/>
+      <c r="D122" s="66"/>
       <c r="E122" s="66"/>
       <c r="F122" s="42"/>
       <c r="G122" s="43"/>
@@ -13188,7 +13351,7 @@
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23"/>
       <c r="B125" s="65"/>
-      <c r="D125" s="66"/>
+      <c r="D125" s="70"/>
       <c r="E125" s="66"/>
       <c r="F125" s="42"/>
       <c r="G125" s="43"/>
@@ -13256,7 +13419,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="66"/>
+      <c r="D126" s="70"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -13528,7 +13691,7 @@
     <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="23"/>
       <c r="B130" s="65"/>
-      <c r="D130" s="70"/>
+      <c r="D130" s="66"/>
       <c r="E130" s="66"/>
       <c r="F130" s="42"/>
       <c r="G130" s="43"/>
@@ -13596,7 +13759,7 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
       <c r="B131" s="65"/>
-      <c r="D131" s="70"/>
+      <c r="D131" s="66"/>
       <c r="E131" s="66"/>
       <c r="F131" s="42"/>
       <c r="G131" s="43"/>
@@ -13800,7 +13963,7 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23"/>
       <c r="B134" s="65"/>
-      <c r="D134" s="66"/>
+      <c r="D134" s="70"/>
       <c r="E134" s="66"/>
       <c r="F134" s="42"/>
       <c r="G134" s="43"/>
@@ -13868,7 +14031,7 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
       <c r="B135" s="65"/>
-      <c r="D135" s="66"/>
+      <c r="D135" s="70"/>
       <c r="E135" s="66"/>
       <c r="F135" s="42"/>
       <c r="G135" s="43"/>
@@ -14140,7 +14303,7 @@
     <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="23"/>
       <c r="B139" s="65"/>
-      <c r="D139" s="70"/>
+      <c r="D139" s="66"/>
       <c r="E139" s="66"/>
       <c r="F139" s="42"/>
       <c r="G139" s="43"/>
@@ -14208,7 +14371,7 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23"/>
       <c r="B140" s="65"/>
-      <c r="D140" s="70"/>
+      <c r="D140" s="66"/>
       <c r="E140" s="66"/>
       <c r="F140" s="42"/>
       <c r="G140" s="43"/>
@@ -14273,18 +14436,485 @@
       <c r="BN140" s="46"/>
       <c r="BO140" s="46"/>
     </row>
+    <row r="141" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="23"/>
+      <c r="B141" s="65"/>
+      <c r="D141" s="66"/>
+      <c r="E141" s="66"/>
+      <c r="F141" s="42"/>
+      <c r="G141" s="43"/>
+      <c r="H141" s="25"/>
+      <c r="I141" s="26"/>
+      <c r="J141" s="27"/>
+      <c r="K141" s="40"/>
+      <c r="L141" s="46"/>
+      <c r="M141" s="46"/>
+      <c r="N141" s="46"/>
+      <c r="O141" s="46"/>
+      <c r="P141" s="46"/>
+      <c r="Q141" s="46"/>
+      <c r="R141" s="46"/>
+      <c r="S141" s="46"/>
+      <c r="T141" s="46"/>
+      <c r="U141" s="46"/>
+      <c r="V141" s="46"/>
+      <c r="W141" s="46"/>
+      <c r="X141" s="46"/>
+      <c r="Y141" s="46"/>
+      <c r="Z141" s="46"/>
+      <c r="AA141" s="46"/>
+      <c r="AB141" s="46"/>
+      <c r="AC141" s="46"/>
+      <c r="AD141" s="46"/>
+      <c r="AE141" s="46"/>
+      <c r="AF141" s="46"/>
+      <c r="AG141" s="46"/>
+      <c r="AH141" s="46"/>
+      <c r="AI141" s="46"/>
+      <c r="AJ141" s="46"/>
+      <c r="AK141" s="46"/>
+      <c r="AL141" s="46"/>
+      <c r="AM141" s="46"/>
+      <c r="AN141" s="46"/>
+      <c r="AO141" s="46"/>
+      <c r="AP141" s="46"/>
+      <c r="AQ141" s="46"/>
+      <c r="AR141" s="46"/>
+      <c r="AS141" s="46"/>
+      <c r="AT141" s="46"/>
+      <c r="AU141" s="46"/>
+      <c r="AV141" s="46"/>
+      <c r="AW141" s="46"/>
+      <c r="AX141" s="46"/>
+      <c r="AY141" s="46"/>
+      <c r="AZ141" s="46"/>
+      <c r="BA141" s="46"/>
+      <c r="BB141" s="46"/>
+      <c r="BC141" s="46"/>
+      <c r="BD141" s="46"/>
+      <c r="BE141" s="46"/>
+      <c r="BF141" s="46"/>
+      <c r="BG141" s="46"/>
+      <c r="BH141" s="46"/>
+      <c r="BI141" s="46"/>
+      <c r="BJ141" s="46"/>
+      <c r="BK141" s="46"/>
+      <c r="BL141" s="46"/>
+      <c r="BM141" s="46"/>
+      <c r="BN141" s="46"/>
+      <c r="BO141" s="46"/>
+    </row>
+    <row r="142" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="23"/>
+      <c r="B142" s="65"/>
+      <c r="D142" s="66"/>
+      <c r="E142" s="66"/>
+      <c r="F142" s="42"/>
+      <c r="G142" s="43"/>
+      <c r="H142" s="25"/>
+      <c r="I142" s="26"/>
+      <c r="J142" s="27"/>
+      <c r="K142" s="40"/>
+      <c r="L142" s="46"/>
+      <c r="M142" s="46"/>
+      <c r="N142" s="46"/>
+      <c r="O142" s="46"/>
+      <c r="P142" s="46"/>
+      <c r="Q142" s="46"/>
+      <c r="R142" s="46"/>
+      <c r="S142" s="46"/>
+      <c r="T142" s="46"/>
+      <c r="U142" s="46"/>
+      <c r="V142" s="46"/>
+      <c r="W142" s="46"/>
+      <c r="X142" s="46"/>
+      <c r="Y142" s="46"/>
+      <c r="Z142" s="46"/>
+      <c r="AA142" s="46"/>
+      <c r="AB142" s="46"/>
+      <c r="AC142" s="46"/>
+      <c r="AD142" s="46"/>
+      <c r="AE142" s="46"/>
+      <c r="AF142" s="46"/>
+      <c r="AG142" s="46"/>
+      <c r="AH142" s="46"/>
+      <c r="AI142" s="46"/>
+      <c r="AJ142" s="46"/>
+      <c r="AK142" s="46"/>
+      <c r="AL142" s="46"/>
+      <c r="AM142" s="46"/>
+      <c r="AN142" s="46"/>
+      <c r="AO142" s="46"/>
+      <c r="AP142" s="46"/>
+      <c r="AQ142" s="46"/>
+      <c r="AR142" s="46"/>
+      <c r="AS142" s="46"/>
+      <c r="AT142" s="46"/>
+      <c r="AU142" s="46"/>
+      <c r="AV142" s="46"/>
+      <c r="AW142" s="46"/>
+      <c r="AX142" s="46"/>
+      <c r="AY142" s="46"/>
+      <c r="AZ142" s="46"/>
+      <c r="BA142" s="46"/>
+      <c r="BB142" s="46"/>
+      <c r="BC142" s="46"/>
+      <c r="BD142" s="46"/>
+      <c r="BE142" s="46"/>
+      <c r="BF142" s="46"/>
+      <c r="BG142" s="46"/>
+      <c r="BH142" s="46"/>
+      <c r="BI142" s="46"/>
+      <c r="BJ142" s="46"/>
+      <c r="BK142" s="46"/>
+      <c r="BL142" s="46"/>
+      <c r="BM142" s="46"/>
+      <c r="BN142" s="46"/>
+      <c r="BO142" s="46"/>
+    </row>
+    <row r="143" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="23"/>
+      <c r="B143" s="65"/>
+      <c r="D143" s="70"/>
+      <c r="E143" s="66"/>
+      <c r="F143" s="42"/>
+      <c r="G143" s="43"/>
+      <c r="H143" s="25"/>
+      <c r="I143" s="26"/>
+      <c r="J143" s="27"/>
+      <c r="K143" s="40"/>
+      <c r="L143" s="46"/>
+      <c r="M143" s="46"/>
+      <c r="N143" s="46"/>
+      <c r="O143" s="46"/>
+      <c r="P143" s="46"/>
+      <c r="Q143" s="46"/>
+      <c r="R143" s="46"/>
+      <c r="S143" s="46"/>
+      <c r="T143" s="46"/>
+      <c r="U143" s="46"/>
+      <c r="V143" s="46"/>
+      <c r="W143" s="46"/>
+      <c r="X143" s="46"/>
+      <c r="Y143" s="46"/>
+      <c r="Z143" s="46"/>
+      <c r="AA143" s="46"/>
+      <c r="AB143" s="46"/>
+      <c r="AC143" s="46"/>
+      <c r="AD143" s="46"/>
+      <c r="AE143" s="46"/>
+      <c r="AF143" s="46"/>
+      <c r="AG143" s="46"/>
+      <c r="AH143" s="46"/>
+      <c r="AI143" s="46"/>
+      <c r="AJ143" s="46"/>
+      <c r="AK143" s="46"/>
+      <c r="AL143" s="46"/>
+      <c r="AM143" s="46"/>
+      <c r="AN143" s="46"/>
+      <c r="AO143" s="46"/>
+      <c r="AP143" s="46"/>
+      <c r="AQ143" s="46"/>
+      <c r="AR143" s="46"/>
+      <c r="AS143" s="46"/>
+      <c r="AT143" s="46"/>
+      <c r="AU143" s="46"/>
+      <c r="AV143" s="46"/>
+      <c r="AW143" s="46"/>
+      <c r="AX143" s="46"/>
+      <c r="AY143" s="46"/>
+      <c r="AZ143" s="46"/>
+      <c r="BA143" s="46"/>
+      <c r="BB143" s="46"/>
+      <c r="BC143" s="46"/>
+      <c r="BD143" s="46"/>
+      <c r="BE143" s="46"/>
+      <c r="BF143" s="46"/>
+      <c r="BG143" s="46"/>
+      <c r="BH143" s="46"/>
+      <c r="BI143" s="46"/>
+      <c r="BJ143" s="46"/>
+      <c r="BK143" s="46"/>
+      <c r="BL143" s="46"/>
+      <c r="BM143" s="46"/>
+      <c r="BN143" s="46"/>
+      <c r="BO143" s="46"/>
+    </row>
+    <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="23"/>
+      <c r="B144" s="65"/>
+      <c r="D144" s="70"/>
+      <c r="E144" s="66"/>
+      <c r="F144" s="42"/>
+      <c r="G144" s="43"/>
+      <c r="H144" s="25"/>
+      <c r="I144" s="26"/>
+      <c r="J144" s="27"/>
+      <c r="K144" s="40"/>
+      <c r="L144" s="46"/>
+      <c r="M144" s="46"/>
+      <c r="N144" s="46"/>
+      <c r="O144" s="46"/>
+      <c r="P144" s="46"/>
+      <c r="Q144" s="46"/>
+      <c r="R144" s="46"/>
+      <c r="S144" s="46"/>
+      <c r="T144" s="46"/>
+      <c r="U144" s="46"/>
+      <c r="V144" s="46"/>
+      <c r="W144" s="46"/>
+      <c r="X144" s="46"/>
+      <c r="Y144" s="46"/>
+      <c r="Z144" s="46"/>
+      <c r="AA144" s="46"/>
+      <c r="AB144" s="46"/>
+      <c r="AC144" s="46"/>
+      <c r="AD144" s="46"/>
+      <c r="AE144" s="46"/>
+      <c r="AF144" s="46"/>
+      <c r="AG144" s="46"/>
+      <c r="AH144" s="46"/>
+      <c r="AI144" s="46"/>
+      <c r="AJ144" s="46"/>
+      <c r="AK144" s="46"/>
+      <c r="AL144" s="46"/>
+      <c r="AM144" s="46"/>
+      <c r="AN144" s="46"/>
+      <c r="AO144" s="46"/>
+      <c r="AP144" s="46"/>
+      <c r="AQ144" s="46"/>
+      <c r="AR144" s="46"/>
+      <c r="AS144" s="46"/>
+      <c r="AT144" s="46"/>
+      <c r="AU144" s="46"/>
+      <c r="AV144" s="46"/>
+      <c r="AW144" s="46"/>
+      <c r="AX144" s="46"/>
+      <c r="AY144" s="46"/>
+      <c r="AZ144" s="46"/>
+      <c r="BA144" s="46"/>
+      <c r="BB144" s="46"/>
+      <c r="BC144" s="46"/>
+      <c r="BD144" s="46"/>
+      <c r="BE144" s="46"/>
+      <c r="BF144" s="46"/>
+      <c r="BG144" s="46"/>
+      <c r="BH144" s="46"/>
+      <c r="BI144" s="46"/>
+      <c r="BJ144" s="46"/>
+      <c r="BK144" s="46"/>
+      <c r="BL144" s="46"/>
+      <c r="BM144" s="46"/>
+      <c r="BN144" s="46"/>
+      <c r="BO144" s="46"/>
+    </row>
+    <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="23"/>
+      <c r="B145" s="65"/>
+      <c r="D145" s="70"/>
+      <c r="E145" s="66"/>
+      <c r="F145" s="42"/>
+      <c r="G145" s="43"/>
+      <c r="H145" s="25"/>
+      <c r="I145" s="26"/>
+      <c r="J145" s="27"/>
+      <c r="K145" s="40"/>
+      <c r="L145" s="46"/>
+      <c r="M145" s="46"/>
+      <c r="N145" s="46"/>
+      <c r="O145" s="46"/>
+      <c r="P145" s="46"/>
+      <c r="Q145" s="46"/>
+      <c r="R145" s="46"/>
+      <c r="S145" s="46"/>
+      <c r="T145" s="46"/>
+      <c r="U145" s="46"/>
+      <c r="V145" s="46"/>
+      <c r="W145" s="46"/>
+      <c r="X145" s="46"/>
+      <c r="Y145" s="46"/>
+      <c r="Z145" s="46"/>
+      <c r="AA145" s="46"/>
+      <c r="AB145" s="46"/>
+      <c r="AC145" s="46"/>
+      <c r="AD145" s="46"/>
+      <c r="AE145" s="46"/>
+      <c r="AF145" s="46"/>
+      <c r="AG145" s="46"/>
+      <c r="AH145" s="46"/>
+      <c r="AI145" s="46"/>
+      <c r="AJ145" s="46"/>
+      <c r="AK145" s="46"/>
+      <c r="AL145" s="46"/>
+      <c r="AM145" s="46"/>
+      <c r="AN145" s="46"/>
+      <c r="AO145" s="46"/>
+      <c r="AP145" s="46"/>
+      <c r="AQ145" s="46"/>
+      <c r="AR145" s="46"/>
+      <c r="AS145" s="46"/>
+      <c r="AT145" s="46"/>
+      <c r="AU145" s="46"/>
+      <c r="AV145" s="46"/>
+      <c r="AW145" s="46"/>
+      <c r="AX145" s="46"/>
+      <c r="AY145" s="46"/>
+      <c r="AZ145" s="46"/>
+      <c r="BA145" s="46"/>
+      <c r="BB145" s="46"/>
+      <c r="BC145" s="46"/>
+      <c r="BD145" s="46"/>
+      <c r="BE145" s="46"/>
+      <c r="BF145" s="46"/>
+      <c r="BG145" s="46"/>
+      <c r="BH145" s="46"/>
+      <c r="BI145" s="46"/>
+      <c r="BJ145" s="46"/>
+      <c r="BK145" s="46"/>
+      <c r="BL145" s="46"/>
+      <c r="BM145" s="46"/>
+      <c r="BN145" s="46"/>
+      <c r="BO145" s="46"/>
+    </row>
+    <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="23"/>
+      <c r="B146" s="65"/>
+      <c r="D146" s="70"/>
+      <c r="E146" s="66"/>
+      <c r="F146" s="42"/>
+      <c r="G146" s="43"/>
+      <c r="H146" s="25"/>
+      <c r="I146" s="26"/>
+      <c r="J146" s="27"/>
+      <c r="K146" s="40"/>
+      <c r="L146" s="46"/>
+      <c r="M146" s="46"/>
+      <c r="N146" s="46"/>
+      <c r="O146" s="46"/>
+      <c r="P146" s="46"/>
+      <c r="Q146" s="46"/>
+      <c r="R146" s="46"/>
+      <c r="S146" s="46"/>
+      <c r="T146" s="46"/>
+      <c r="U146" s="46"/>
+      <c r="V146" s="46"/>
+      <c r="W146" s="46"/>
+      <c r="X146" s="46"/>
+      <c r="Y146" s="46"/>
+      <c r="Z146" s="46"/>
+      <c r="AA146" s="46"/>
+      <c r="AB146" s="46"/>
+      <c r="AC146" s="46"/>
+      <c r="AD146" s="46"/>
+      <c r="AE146" s="46"/>
+      <c r="AF146" s="46"/>
+      <c r="AG146" s="46"/>
+      <c r="AH146" s="46"/>
+      <c r="AI146" s="46"/>
+      <c r="AJ146" s="46"/>
+      <c r="AK146" s="46"/>
+      <c r="AL146" s="46"/>
+      <c r="AM146" s="46"/>
+      <c r="AN146" s="46"/>
+      <c r="AO146" s="46"/>
+      <c r="AP146" s="46"/>
+      <c r="AQ146" s="46"/>
+      <c r="AR146" s="46"/>
+      <c r="AS146" s="46"/>
+      <c r="AT146" s="46"/>
+      <c r="AU146" s="46"/>
+      <c r="AV146" s="46"/>
+      <c r="AW146" s="46"/>
+      <c r="AX146" s="46"/>
+      <c r="AY146" s="46"/>
+      <c r="AZ146" s="46"/>
+      <c r="BA146" s="46"/>
+      <c r="BB146" s="46"/>
+      <c r="BC146" s="46"/>
+      <c r="BD146" s="46"/>
+      <c r="BE146" s="46"/>
+      <c r="BF146" s="46"/>
+      <c r="BG146" s="46"/>
+      <c r="BH146" s="46"/>
+      <c r="BI146" s="46"/>
+      <c r="BJ146" s="46"/>
+      <c r="BK146" s="46"/>
+      <c r="BL146" s="46"/>
+      <c r="BM146" s="46"/>
+      <c r="BN146" s="46"/>
+      <c r="BO146" s="46"/>
+    </row>
+    <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="23"/>
+      <c r="B147" s="65"/>
+      <c r="D147" s="70"/>
+      <c r="E147" s="66"/>
+      <c r="F147" s="42"/>
+      <c r="G147" s="43"/>
+      <c r="H147" s="25"/>
+      <c r="I147" s="26"/>
+      <c r="J147" s="27"/>
+      <c r="K147" s="40"/>
+      <c r="L147" s="46"/>
+      <c r="M147" s="46"/>
+      <c r="N147" s="46"/>
+      <c r="O147" s="46"/>
+      <c r="P147" s="46"/>
+      <c r="Q147" s="46"/>
+      <c r="R147" s="46"/>
+      <c r="S147" s="46"/>
+      <c r="T147" s="46"/>
+      <c r="U147" s="46"/>
+      <c r="V147" s="46"/>
+      <c r="W147" s="46"/>
+      <c r="X147" s="46"/>
+      <c r="Y147" s="46"/>
+      <c r="Z147" s="46"/>
+      <c r="AA147" s="46"/>
+      <c r="AB147" s="46"/>
+      <c r="AC147" s="46"/>
+      <c r="AD147" s="46"/>
+      <c r="AE147" s="46"/>
+      <c r="AF147" s="46"/>
+      <c r="AG147" s="46"/>
+      <c r="AH147" s="46"/>
+      <c r="AI147" s="46"/>
+      <c r="AJ147" s="46"/>
+      <c r="AK147" s="46"/>
+      <c r="AL147" s="46"/>
+      <c r="AM147" s="46"/>
+      <c r="AN147" s="46"/>
+      <c r="AO147" s="46"/>
+      <c r="AP147" s="46"/>
+      <c r="AQ147" s="46"/>
+      <c r="AR147" s="46"/>
+      <c r="AS147" s="46"/>
+      <c r="AT147" s="46"/>
+      <c r="AU147" s="46"/>
+      <c r="AV147" s="46"/>
+      <c r="AW147" s="46"/>
+      <c r="AX147" s="46"/>
+      <c r="AY147" s="46"/>
+      <c r="AZ147" s="46"/>
+      <c r="BA147" s="46"/>
+      <c r="BB147" s="46"/>
+      <c r="BC147" s="46"/>
+      <c r="BD147" s="46"/>
+      <c r="BE147" s="46"/>
+      <c r="BF147" s="46"/>
+      <c r="BG147" s="46"/>
+      <c r="BH147" s="46"/>
+      <c r="BI147" s="46"/>
+      <c r="BJ147" s="46"/>
+      <c r="BK147" s="46"/>
+      <c r="BL147" s="46"/>
+      <c r="BM147" s="46"/>
+      <c r="BN147" s="46"/>
+      <c r="BO147" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -14295,10 +14925,19 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I104">
-    <cfRule type="dataBar" priority="192">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I106 I108:I111">
+    <cfRule type="dataBar" priority="203">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14312,66 +14951,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="97" priority="235">
+    <cfRule type="expression" dxfId="107" priority="246">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L105:BO107 M108:BN113 BO111:BO113 L114:BO116 M117:BN122 BO120:BO122 L123:BO125 M126:BN131 BO129:BO131 L132:BO134 M135:BN140 BO138:BO140 M98:BN104 BO103:BO104">
-    <cfRule type="expression" dxfId="96" priority="238">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L112:BO114 M115:BN120 BO118:BO120 L121:BO123 M124:BN129 BO127:BO129 L130:BO132 M133:BN138 BO136:BO138 L139:BO141 M142:BN147 BO145:BO147 M98:BN106 BO110:BO111 M108:BN111">
+    <cfRule type="expression" dxfId="106" priority="249">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="95" priority="239">
+    <cfRule type="expression" dxfId="105" priority="250">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO104">
-    <cfRule type="expression" dxfId="94" priority="198">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO106 L108:BO111">
+    <cfRule type="expression" dxfId="104" priority="209">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="93" priority="188">
+    <cfRule type="expression" dxfId="103" priority="199">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E141:E1048576 E95:E96 E98:E104">
-    <cfRule type="cellIs" dxfId="92" priority="179" operator="equal">
+  <conditionalFormatting sqref="E1:E73 E148:E1048576 E95:E96 E98:E106 E108:E111">
+    <cfRule type="cellIs" dxfId="102" priority="190" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="192" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="193" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="194" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="195" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="196" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="197" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="85" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="191" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="84" priority="244">
+    <cfRule type="expression" dxfId="94" priority="255">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="83" priority="245">
+    <cfRule type="expression" dxfId="93" priority="256">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I84">
-    <cfRule type="dataBar" priority="174">
+    <cfRule type="dataBar" priority="185">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14385,51 +15024,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="82" priority="175">
+    <cfRule type="expression" dxfId="92" priority="186">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="176">
+    <cfRule type="expression" dxfId="91" priority="187">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="80" priority="173">
+    <cfRule type="expression" dxfId="90" priority="184">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="79" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="177" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="178" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="179" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="180" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="181" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="182" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="183" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="72" priority="177">
+    <cfRule type="expression" dxfId="82" priority="188">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="71" priority="178">
+    <cfRule type="expression" dxfId="81" priority="189">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I105:I113">
-    <cfRule type="dataBar" priority="83">
+  <conditionalFormatting sqref="I112:I120">
+    <cfRule type="dataBar" priority="94">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14442,44 +15081,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L105:BO113">
-    <cfRule type="expression" dxfId="70" priority="82">
+  <conditionalFormatting sqref="L112:BO120">
+    <cfRule type="expression" dxfId="80" priority="93">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E105:E113">
-    <cfRule type="cellIs" dxfId="69" priority="75" operator="equal">
+  <conditionalFormatting sqref="E112:E120">
+    <cfRule type="cellIs" dxfId="79" priority="86" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="87" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="88" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="89" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="90" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="91" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="92" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L108:BO113 L98:BO104">
-    <cfRule type="expression" dxfId="62" priority="86">
+  <conditionalFormatting sqref="L115:BO120 L98:BO106 L108:BO111">
+    <cfRule type="expression" dxfId="72" priority="97">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="87">
+    <cfRule type="expression" dxfId="71" priority="98">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I114:I122">
-    <cfRule type="dataBar" priority="70">
+  <conditionalFormatting sqref="I121:I129">
+    <cfRule type="dataBar" priority="81">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14492,44 +15131,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L114:BO122">
-    <cfRule type="expression" dxfId="60" priority="69">
+  <conditionalFormatting sqref="L121:BO129">
+    <cfRule type="expression" dxfId="70" priority="80">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E114:E122">
-    <cfRule type="cellIs" dxfId="59" priority="62" operator="equal">
+  <conditionalFormatting sqref="E121:E129">
+    <cfRule type="cellIs" dxfId="69" priority="73" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="74" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="75" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="76" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="77" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="78" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="79" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L117:BO122">
-    <cfRule type="expression" dxfId="52" priority="73">
+  <conditionalFormatting sqref="L124:BO129">
+    <cfRule type="expression" dxfId="62" priority="84">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="74">
+    <cfRule type="expression" dxfId="61" priority="85">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123:I131">
-    <cfRule type="dataBar" priority="57">
+  <conditionalFormatting sqref="I130:I138">
+    <cfRule type="dataBar" priority="68">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14542,44 +15181,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L123:BO131">
-    <cfRule type="expression" dxfId="50" priority="56">
+  <conditionalFormatting sqref="L130:BO138">
+    <cfRule type="expression" dxfId="60" priority="67">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E123:E131">
-    <cfRule type="cellIs" dxfId="49" priority="49" operator="equal">
+  <conditionalFormatting sqref="E130:E138">
+    <cfRule type="cellIs" dxfId="59" priority="60" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="61" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="62" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="64" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="65" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="66" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L126:BO131">
-    <cfRule type="expression" dxfId="42" priority="60">
+  <conditionalFormatting sqref="L133:BO138">
+    <cfRule type="expression" dxfId="52" priority="71">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="61">
+    <cfRule type="expression" dxfId="51" priority="72">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I132:I140">
-    <cfRule type="dataBar" priority="44">
+  <conditionalFormatting sqref="I139:I147">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14592,44 +15231,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L132:BO140">
-    <cfRule type="expression" dxfId="40" priority="43">
+  <conditionalFormatting sqref="L139:BO147">
+    <cfRule type="expression" dxfId="50" priority="54">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E132:E140">
-    <cfRule type="cellIs" dxfId="39" priority="36" operator="equal">
+  <conditionalFormatting sqref="E139:E147">
+    <cfRule type="cellIs" dxfId="49" priority="47" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="48" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="49" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="50" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L135:BO140">
-    <cfRule type="expression" dxfId="32" priority="47">
+  <conditionalFormatting sqref="L142:BO147">
+    <cfRule type="expression" dxfId="42" priority="58">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="48">
+    <cfRule type="expression" dxfId="41" priority="59">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85:I86">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -14643,11 +15282,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:BO86">
+    <cfRule type="expression" dxfId="40" priority="41">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E86">
+    <cfRule type="cellIs" dxfId="39" priority="34" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="35" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="36" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="37" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="35" priority="38" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="39" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="33" priority="40" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
+    <cfRule type="expression" dxfId="32" priority="32">
+      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87:I94">
+    <cfRule type="dataBar" priority="31">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
     <cfRule type="expression" dxfId="30" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E86">
+  <conditionalFormatting sqref="E87:E94">
     <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14670,15 +15359,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="22" priority="21">
-      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="21" priority="22">
-      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I94">
+  <conditionalFormatting sqref="I97">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14687,17 +15376,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E94">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14720,15 +15409,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO97">
+  <conditionalFormatting sqref="L107:BO107">
     <cfRule type="expression" dxfId="12" priority="10">
-      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
+      <formula>AND($F107&lt;=L$6,ROUNDDOWN(($G107-$F107+1)*$I107,0)+$F107-1&gt;=L$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="11">
-      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
+      <formula>AND(NOT(ISBLANK($F107)),$F107&lt;=L$6,$G107&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I97">
+  <conditionalFormatting sqref="I107">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14737,17 +15426,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
+          <x14:id>{9C28E6E5-6090-4FDF-A8AE-554DED5465F8}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO97">
+  <conditionalFormatting sqref="L107:BO107">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
+  <conditionalFormatting sqref="E107">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14826,7 +15515,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I98:I104</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I106 I108:I111</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -14856,7 +15545,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I105:I113</xm:sqref>
+          <xm:sqref>I112:I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -14871,7 +15560,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I114:I122</xm:sqref>
+          <xm:sqref>I121:I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -14886,7 +15575,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I123:I131</xm:sqref>
+          <xm:sqref>I130:I138</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -14901,7 +15590,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I132:I140</xm:sqref>
+          <xm:sqref>I139:I147</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -14947,6 +15636,21 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>I97</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9C28E6E5-6090-4FDF-A8AE-554DED5465F8}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I107</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added future implied forecasts note (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A64519-9D95-43FA-AA24-AC0C13E5D329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BD6B99-EBB7-4F85-AD73-7A820D8FB687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -796,9 +796,6 @@
     <t>Revise Data Transforms</t>
   </si>
   <si>
-    <t>Add Structural Equations</t>
-  </si>
-  <si>
     <t>Add Structural Estimation</t>
   </si>
   <si>
@@ -818,6 +815,9 @@
   </si>
   <si>
     <t>Add Baseline Qualitative-Adjustable Forecasts</t>
+  </si>
+  <si>
+    <t>Add Initial Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1746,6 +1746,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1755,6 +1762,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1763,17 +1774,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3127,7 +3127,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F110" sqref="F110"/>
+      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3157,27 +3157,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3222,12 +3222,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3237,183 +3237,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -11277,7 +11277,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="19"/>
@@ -11518,7 +11518,7 @@
         <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
@@ -11597,7 +11597,7 @@
         <v>9.4</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
@@ -11607,7 +11607,7 @@
         <v>44356</v>
       </c>
       <c r="G101" s="43">
-        <v>44359</v>
+        <v>44367</v>
       </c>
       <c r="H101" s="25"/>
       <c r="I101" s="26"/>
@@ -11676,14 +11676,14 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F102" s="42">
-        <v>44357</v>
+        <v>44365</v>
       </c>
       <c r="G102" s="43"/>
       <c r="H102" s="25"/>
@@ -11753,14 +11753,14 @@
         <v>9.6</v>
       </c>
       <c r="B103" s="65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D103" s="70"/>
       <c r="E103" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F103" s="42">
-        <v>44357</v>
+        <v>44365</v>
       </c>
       <c r="G103" s="43"/>
       <c r="H103" s="25"/>
@@ -11830,14 +11830,14 @@
         <v>9.7</v>
       </c>
       <c r="B104" s="65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D104" s="70"/>
       <c r="E104" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F104" s="42">
-        <v>44364</v>
+        <v>44372</v>
       </c>
       <c r="G104" s="43"/>
       <c r="H104" s="25"/>
@@ -11907,14 +11907,14 @@
         <v>9.8</v>
       </c>
       <c r="B105" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D105" s="70"/>
       <c r="E105" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F105" s="42">
-        <v>44364</v>
+        <v>44372</v>
       </c>
       <c r="G105" s="43"/>
       <c r="H105" s="25"/>
@@ -11984,7 +11984,7 @@
         <v>10</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D106" s="19"/>
       <c r="E106" s="19"/>
@@ -14825,15 +14825,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -14844,6 +14835,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I107:I110 I98:I105">

</xml_diff>

<commit_message>
Added separation of initial forecasts and external forecasts (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BD6B99-EBB7-4F85-AD73-7A820D8FB687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4DC23E-DB70-4DBB-BC4D-A7546D3AEFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
   <si>
     <t>WBS</t>
   </si>
@@ -817,7 +817,13 @@
     <t>Add Baseline Qualitative-Adjustable Forecasts</t>
   </si>
   <si>
-    <t>Add Initial Forecasts</t>
+    <t>Add Separation of Initial/External Forecasts</t>
+  </si>
+  <si>
+    <t>Add Initial Forecast Qual Derivaiton</t>
+  </si>
+  <si>
+    <t>Add Initial Forecast Calculated Vavriables</t>
   </si>
 </sst>
 </file>
@@ -1746,13 +1752,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1762,10 +1761,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1774,6 +1769,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3123,11 +3129,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO146"/>
+  <dimension ref="A1:BO148"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G101" sqref="G101"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3157,27 +3163,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3222,12 +3228,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3237,183 +3243,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 20</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 21</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 22</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 23</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 24</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44326</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44333</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44340</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44347</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44354</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44361</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44368</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44375</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8571,7 +8577,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A111" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A113" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11531,7 +11537,9 @@
         <v>44356</v>
       </c>
       <c r="H100" s="25"/>
-      <c r="I100" s="26"/>
+      <c r="I100" s="26">
+        <v>1</v>
+      </c>
       <c r="J100" s="27"/>
       <c r="K100" s="40"/>
       <c r="L100" s="46"/>
@@ -11607,10 +11615,12 @@
         <v>44356</v>
       </c>
       <c r="G101" s="43">
-        <v>44367</v>
+        <v>44365</v>
       </c>
       <c r="H101" s="25"/>
-      <c r="I101" s="26"/>
+      <c r="I101" s="26">
+        <v>1</v>
+      </c>
       <c r="J101" s="27"/>
       <c r="K101" s="40"/>
       <c r="L101" s="46"/>
@@ -11676,7 +11686,7 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
@@ -11753,7 +11763,7 @@
         <v>9.6</v>
       </c>
       <c r="B103" s="65" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D103" s="70"/>
       <c r="E103" s="66" t="s">
@@ -11830,14 +11840,14 @@
         <v>9.7</v>
       </c>
       <c r="B104" s="65" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D104" s="70"/>
       <c r="E104" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F104" s="42">
-        <v>44372</v>
+        <v>44365</v>
       </c>
       <c r="G104" s="43"/>
       <c r="H104" s="25"/>
@@ -11907,14 +11917,14 @@
         <v>9.8</v>
       </c>
       <c r="B105" s="65" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D105" s="70"/>
       <c r="E105" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F105" s="42">
-        <v>44372</v>
+        <v>44365</v>
       </c>
       <c r="G105" s="43"/>
       <c r="H105" s="25"/>
@@ -11978,99 +11988,97 @@
       <c r="BN105" s="46"/>
       <c r="BO105" s="46"/>
     </row>
-    <row r="106" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>10</v>
-      </c>
-      <c r="B106" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D106" s="19"/>
-      <c r="E106" s="19"/>
-      <c r="F106" s="44"/>
-      <c r="G106" s="44" t="str">
-        <f t="shared" ref="G106" si="18">IF(ISBLANK(F106)," - ",IF(H106=0,F106,F106+H106-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H106" s="20"/>
-      <c r="I106" s="21"/>
-      <c r="J106" s="22" t="str">
-        <f t="shared" ref="J106" si="19">IF(OR(G106=0,F106=0)," - ",NETWORKDAYS(F106,G106))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K106" s="41"/>
-      <c r="L106" s="48"/>
-      <c r="M106" s="48"/>
-      <c r="N106" s="48"/>
-      <c r="O106" s="48"/>
-      <c r="P106" s="48"/>
-      <c r="Q106" s="48"/>
-      <c r="R106" s="48"/>
-      <c r="S106" s="48"/>
-      <c r="T106" s="48"/>
-      <c r="U106" s="48"/>
-      <c r="V106" s="48"/>
-      <c r="W106" s="48"/>
-      <c r="X106" s="48"/>
-      <c r="Y106" s="48"/>
-      <c r="Z106" s="48"/>
-      <c r="AA106" s="48"/>
-      <c r="AB106" s="48"/>
-      <c r="AC106" s="48"/>
-      <c r="AD106" s="48"/>
-      <c r="AE106" s="48"/>
-      <c r="AF106" s="48"/>
-      <c r="AG106" s="48"/>
-      <c r="AH106" s="48"/>
-      <c r="AI106" s="48"/>
-      <c r="AJ106" s="48"/>
-      <c r="AK106" s="48"/>
-      <c r="AL106" s="48"/>
-      <c r="AM106" s="48"/>
-      <c r="AN106" s="48"/>
-      <c r="AO106" s="48"/>
-      <c r="AP106" s="48"/>
-      <c r="AQ106" s="48"/>
-      <c r="AR106" s="48"/>
-      <c r="AS106" s="48"/>
-      <c r="AT106" s="48"/>
-      <c r="AU106" s="48"/>
-      <c r="AV106" s="48"/>
-      <c r="AW106" s="48"/>
-      <c r="AX106" s="48"/>
-      <c r="AY106" s="48"/>
-      <c r="AZ106" s="48"/>
-      <c r="BA106" s="48"/>
-      <c r="BB106" s="48"/>
-      <c r="BC106" s="48"/>
-      <c r="BD106" s="48"/>
-      <c r="BE106" s="48"/>
-      <c r="BF106" s="48"/>
-      <c r="BG106" s="48"/>
-      <c r="BH106" s="48"/>
-      <c r="BI106" s="48"/>
-      <c r="BJ106" s="48"/>
-      <c r="BK106" s="48"/>
-      <c r="BL106" s="48"/>
-      <c r="BM106" s="48"/>
-      <c r="BN106" s="48"/>
-      <c r="BO106" s="48"/>
+    <row r="106" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>9.9</v>
+      </c>
+      <c r="B106" s="65" t="s">
+        <v>124</v>
+      </c>
+      <c r="D106" s="70"/>
+      <c r="E106" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F106" s="42">
+        <v>44372</v>
+      </c>
+      <c r="G106" s="43"/>
+      <c r="H106" s="25"/>
+      <c r="I106" s="26"/>
+      <c r="J106" s="27"/>
+      <c r="K106" s="40"/>
+      <c r="L106" s="46"/>
+      <c r="M106" s="46"/>
+      <c r="N106" s="46"/>
+      <c r="O106" s="46"/>
+      <c r="P106" s="46"/>
+      <c r="Q106" s="46"/>
+      <c r="R106" s="46"/>
+      <c r="S106" s="46"/>
+      <c r="T106" s="46"/>
+      <c r="U106" s="46"/>
+      <c r="V106" s="46"/>
+      <c r="W106" s="46"/>
+      <c r="X106" s="46"/>
+      <c r="Y106" s="46"/>
+      <c r="Z106" s="46"/>
+      <c r="AA106" s="46"/>
+      <c r="AB106" s="46"/>
+      <c r="AC106" s="46"/>
+      <c r="AD106" s="46"/>
+      <c r="AE106" s="46"/>
+      <c r="AF106" s="46"/>
+      <c r="AG106" s="46"/>
+      <c r="AH106" s="46"/>
+      <c r="AI106" s="46"/>
+      <c r="AJ106" s="46"/>
+      <c r="AK106" s="46"/>
+      <c r="AL106" s="46"/>
+      <c r="AM106" s="46"/>
+      <c r="AN106" s="46"/>
+      <c r="AO106" s="46"/>
+      <c r="AP106" s="46"/>
+      <c r="AQ106" s="46"/>
+      <c r="AR106" s="46"/>
+      <c r="AS106" s="46"/>
+      <c r="AT106" s="46"/>
+      <c r="AU106" s="46"/>
+      <c r="AV106" s="46"/>
+      <c r="AW106" s="46"/>
+      <c r="AX106" s="46"/>
+      <c r="AY106" s="46"/>
+      <c r="AZ106" s="46"/>
+      <c r="BA106" s="46"/>
+      <c r="BB106" s="46"/>
+      <c r="BC106" s="46"/>
+      <c r="BD106" s="46"/>
+      <c r="BE106" s="46"/>
+      <c r="BF106" s="46"/>
+      <c r="BG106" s="46"/>
+      <c r="BH106" s="46"/>
+      <c r="BI106" s="46"/>
+      <c r="BJ106" s="46"/>
+      <c r="BK106" s="46"/>
+      <c r="BL106" s="46"/>
+      <c r="BM106" s="46"/>
+      <c r="BN106" s="46"/>
+      <c r="BO106" s="46"/>
     </row>
     <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.1</v>
+        <v>9.10</v>
       </c>
       <c r="B107" s="65" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="D107" s="70"/>
       <c r="E107" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F107" s="42">
-        <v>44375</v>
+        <v>44372</v>
       </c>
       <c r="G107" s="43"/>
       <c r="H107" s="25"/>
@@ -12134,97 +12142,99 @@
       <c r="BN107" s="46"/>
       <c r="BO107" s="46"/>
     </row>
-    <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>10.2</v>
-      </c>
-      <c r="B108" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D108" s="70"/>
-      <c r="E108" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F108" s="42">
-        <v>44375</v>
-      </c>
-      <c r="G108" s="43"/>
-      <c r="H108" s="25"/>
-      <c r="I108" s="26"/>
-      <c r="J108" s="27"/>
-      <c r="K108" s="40"/>
-      <c r="L108" s="46"/>
-      <c r="M108" s="46"/>
-      <c r="N108" s="46"/>
-      <c r="O108" s="46"/>
-      <c r="P108" s="46"/>
-      <c r="Q108" s="46"/>
-      <c r="R108" s="46"/>
-      <c r="S108" s="46"/>
-      <c r="T108" s="46"/>
-      <c r="U108" s="46"/>
-      <c r="V108" s="46"/>
-      <c r="W108" s="46"/>
-      <c r="X108" s="46"/>
-      <c r="Y108" s="46"/>
-      <c r="Z108" s="46"/>
-      <c r="AA108" s="46"/>
-      <c r="AB108" s="46"/>
-      <c r="AC108" s="46"/>
-      <c r="AD108" s="46"/>
-      <c r="AE108" s="46"/>
-      <c r="AF108" s="46"/>
-      <c r="AG108" s="46"/>
-      <c r="AH108" s="46"/>
-      <c r="AI108" s="46"/>
-      <c r="AJ108" s="46"/>
-      <c r="AK108" s="46"/>
-      <c r="AL108" s="46"/>
-      <c r="AM108" s="46"/>
-      <c r="AN108" s="46"/>
-      <c r="AO108" s="46"/>
-      <c r="AP108" s="46"/>
-      <c r="AQ108" s="46"/>
-      <c r="AR108" s="46"/>
-      <c r="AS108" s="46"/>
-      <c r="AT108" s="46"/>
-      <c r="AU108" s="46"/>
-      <c r="AV108" s="46"/>
-      <c r="AW108" s="46"/>
-      <c r="AX108" s="46"/>
-      <c r="AY108" s="46"/>
-      <c r="AZ108" s="46"/>
-      <c r="BA108" s="46"/>
-      <c r="BB108" s="46"/>
-      <c r="BC108" s="46"/>
-      <c r="BD108" s="46"/>
-      <c r="BE108" s="46"/>
-      <c r="BF108" s="46"/>
-      <c r="BG108" s="46"/>
-      <c r="BH108" s="46"/>
-      <c r="BI108" s="46"/>
-      <c r="BJ108" s="46"/>
-      <c r="BK108" s="46"/>
-      <c r="BL108" s="46"/>
-      <c r="BM108" s="46"/>
-      <c r="BN108" s="46"/>
-      <c r="BO108" s="46"/>
+    <row r="108" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>10</v>
+      </c>
+      <c r="B108" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="44"/>
+      <c r="G108" s="44" t="str">
+        <f t="shared" ref="G108" si="18">IF(ISBLANK(F108)," - ",IF(H108=0,F108,F108+H108-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H108" s="20"/>
+      <c r="I108" s="21"/>
+      <c r="J108" s="22" t="str">
+        <f t="shared" ref="J108" si="19">IF(OR(G108=0,F108=0)," - ",NETWORKDAYS(F108,G108))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K108" s="41"/>
+      <c r="L108" s="48"/>
+      <c r="M108" s="48"/>
+      <c r="N108" s="48"/>
+      <c r="O108" s="48"/>
+      <c r="P108" s="48"/>
+      <c r="Q108" s="48"/>
+      <c r="R108" s="48"/>
+      <c r="S108" s="48"/>
+      <c r="T108" s="48"/>
+      <c r="U108" s="48"/>
+      <c r="V108" s="48"/>
+      <c r="W108" s="48"/>
+      <c r="X108" s="48"/>
+      <c r="Y108" s="48"/>
+      <c r="Z108" s="48"/>
+      <c r="AA108" s="48"/>
+      <c r="AB108" s="48"/>
+      <c r="AC108" s="48"/>
+      <c r="AD108" s="48"/>
+      <c r="AE108" s="48"/>
+      <c r="AF108" s="48"/>
+      <c r="AG108" s="48"/>
+      <c r="AH108" s="48"/>
+      <c r="AI108" s="48"/>
+      <c r="AJ108" s="48"/>
+      <c r="AK108" s="48"/>
+      <c r="AL108" s="48"/>
+      <c r="AM108" s="48"/>
+      <c r="AN108" s="48"/>
+      <c r="AO108" s="48"/>
+      <c r="AP108" s="48"/>
+      <c r="AQ108" s="48"/>
+      <c r="AR108" s="48"/>
+      <c r="AS108" s="48"/>
+      <c r="AT108" s="48"/>
+      <c r="AU108" s="48"/>
+      <c r="AV108" s="48"/>
+      <c r="AW108" s="48"/>
+      <c r="AX108" s="48"/>
+      <c r="AY108" s="48"/>
+      <c r="AZ108" s="48"/>
+      <c r="BA108" s="48"/>
+      <c r="BB108" s="48"/>
+      <c r="BC108" s="48"/>
+      <c r="BD108" s="48"/>
+      <c r="BE108" s="48"/>
+      <c r="BF108" s="48"/>
+      <c r="BG108" s="48"/>
+      <c r="BH108" s="48"/>
+      <c r="BI108" s="48"/>
+      <c r="BJ108" s="48"/>
+      <c r="BK108" s="48"/>
+      <c r="BL108" s="48"/>
+      <c r="BM108" s="48"/>
+      <c r="BN108" s="48"/>
+      <c r="BO108" s="48"/>
     </row>
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.3</v>
+        <v>10.1</v>
       </c>
       <c r="B109" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D109" s="70"/>
       <c r="E109" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F109" s="42">
-        <v>44378</v>
+        <v>44375</v>
       </c>
       <c r="G109" s="43"/>
       <c r="H109" s="25"/>
@@ -12291,17 +12301,17 @@
     <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.4</v>
+        <v>10.2</v>
       </c>
       <c r="B110" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D110" s="70"/>
       <c r="E110" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F110" s="42">
-        <v>44381</v>
+        <v>44375</v>
       </c>
       <c r="G110" s="43"/>
       <c r="H110" s="25"/>
@@ -12368,17 +12378,17 @@
     <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.5</v>
-      </c>
-      <c r="B111" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D111" s="66"/>
+        <v>10.3</v>
+      </c>
+      <c r="B111" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D111" s="70"/>
       <c r="E111" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F111" s="42">
-        <v>44531</v>
+        <v>44378</v>
       </c>
       <c r="G111" s="43"/>
       <c r="H111" s="25"/>
@@ -12443,11 +12453,20 @@
       <c r="BO111" s="46"/>
     </row>
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="23"/>
-      <c r="B112" s="65"/>
-      <c r="D112" s="66"/>
-      <c r="E112" s="66"/>
-      <c r="F112" s="42"/>
+      <c r="A112" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.4</v>
+      </c>
+      <c r="B112" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D112" s="70"/>
+      <c r="E112" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F112" s="42">
+        <v>44381</v>
+      </c>
       <c r="G112" s="43"/>
       <c r="H112" s="25"/>
       <c r="I112" s="26"/>
@@ -12511,11 +12530,20 @@
       <c r="BO112" s="46"/>
     </row>
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="23"/>
-      <c r="B113" s="65"/>
+      <c r="A113" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.5</v>
+      </c>
+      <c r="B113" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D113" s="66"/>
-      <c r="E113" s="66"/>
-      <c r="F113" s="42"/>
+      <c r="E113" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F113" s="42">
+        <v>44531</v>
+      </c>
       <c r="G113" s="43"/>
       <c r="H113" s="25"/>
       <c r="I113" s="26"/>
@@ -12649,7 +12677,7 @@
     <row r="115" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="23"/>
       <c r="B115" s="65"/>
-      <c r="D115" s="70"/>
+      <c r="D115" s="66"/>
       <c r="E115" s="66"/>
       <c r="F115" s="42"/>
       <c r="G115" s="43"/>
@@ -12717,7 +12745,7 @@
     <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="23"/>
       <c r="B116" s="65"/>
-      <c r="D116" s="70"/>
+      <c r="D116" s="66"/>
       <c r="E116" s="66"/>
       <c r="F116" s="42"/>
       <c r="G116" s="43"/>
@@ -12989,7 +13017,7 @@
     <row r="120" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="23"/>
       <c r="B120" s="65"/>
-      <c r="D120" s="66"/>
+      <c r="D120" s="70"/>
       <c r="E120" s="66"/>
       <c r="F120" s="42"/>
       <c r="G120" s="43"/>
@@ -13057,7 +13085,7 @@
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="23"/>
       <c r="B121" s="65"/>
-      <c r="D121" s="66"/>
+      <c r="D121" s="70"/>
       <c r="E121" s="66"/>
       <c r="F121" s="42"/>
       <c r="G121" s="43"/>
@@ -13261,7 +13289,7 @@
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
       <c r="B124" s="65"/>
-      <c r="D124" s="70"/>
+      <c r="D124" s="66"/>
       <c r="E124" s="66"/>
       <c r="F124" s="42"/>
       <c r="G124" s="43"/>
@@ -13329,7 +13357,7 @@
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23"/>
       <c r="B125" s="65"/>
-      <c r="D125" s="70"/>
+      <c r="D125" s="66"/>
       <c r="E125" s="66"/>
       <c r="F125" s="42"/>
       <c r="G125" s="43"/>
@@ -13601,7 +13629,7 @@
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23"/>
       <c r="B129" s="65"/>
-      <c r="D129" s="66"/>
+      <c r="D129" s="70"/>
       <c r="E129" s="66"/>
       <c r="F129" s="42"/>
       <c r="G129" s="43"/>
@@ -13669,7 +13697,7 @@
     <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="23"/>
       <c r="B130" s="65"/>
-      <c r="D130" s="66"/>
+      <c r="D130" s="70"/>
       <c r="E130" s="66"/>
       <c r="F130" s="42"/>
       <c r="G130" s="43"/>
@@ -13873,7 +13901,7 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23"/>
       <c r="B133" s="65"/>
-      <c r="D133" s="70"/>
+      <c r="D133" s="66"/>
       <c r="E133" s="66"/>
       <c r="F133" s="42"/>
       <c r="G133" s="43"/>
@@ -13941,7 +13969,7 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23"/>
       <c r="B134" s="65"/>
-      <c r="D134" s="70"/>
+      <c r="D134" s="66"/>
       <c r="E134" s="66"/>
       <c r="F134" s="42"/>
       <c r="G134" s="43"/>
@@ -14213,7 +14241,7 @@
     <row r="138" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="23"/>
       <c r="B138" s="65"/>
-      <c r="D138" s="66"/>
+      <c r="D138" s="70"/>
       <c r="E138" s="66"/>
       <c r="F138" s="42"/>
       <c r="G138" s="43"/>
@@ -14281,7 +14309,7 @@
     <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="23"/>
       <c r="B139" s="65"/>
-      <c r="D139" s="66"/>
+      <c r="D139" s="70"/>
       <c r="E139" s="66"/>
       <c r="F139" s="42"/>
       <c r="G139" s="43"/>
@@ -14485,7 +14513,7 @@
     <row r="142" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23"/>
       <c r="B142" s="65"/>
-      <c r="D142" s="70"/>
+      <c r="D142" s="66"/>
       <c r="E142" s="66"/>
       <c r="F142" s="42"/>
       <c r="G142" s="43"/>
@@ -14553,7 +14581,7 @@
     <row r="143" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23"/>
       <c r="B143" s="65"/>
-      <c r="D143" s="70"/>
+      <c r="D143" s="66"/>
       <c r="E143" s="66"/>
       <c r="F143" s="42"/>
       <c r="G143" s="43"/>
@@ -14822,9 +14850,154 @@
       <c r="BN146" s="46"/>
       <c r="BO146" s="46"/>
     </row>
+    <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="23"/>
+      <c r="B147" s="65"/>
+      <c r="D147" s="70"/>
+      <c r="E147" s="66"/>
+      <c r="F147" s="42"/>
+      <c r="G147" s="43"/>
+      <c r="H147" s="25"/>
+      <c r="I147" s="26"/>
+      <c r="J147" s="27"/>
+      <c r="K147" s="40"/>
+      <c r="L147" s="46"/>
+      <c r="M147" s="46"/>
+      <c r="N147" s="46"/>
+      <c r="O147" s="46"/>
+      <c r="P147" s="46"/>
+      <c r="Q147" s="46"/>
+      <c r="R147" s="46"/>
+      <c r="S147" s="46"/>
+      <c r="T147" s="46"/>
+      <c r="U147" s="46"/>
+      <c r="V147" s="46"/>
+      <c r="W147" s="46"/>
+      <c r="X147" s="46"/>
+      <c r="Y147" s="46"/>
+      <c r="Z147" s="46"/>
+      <c r="AA147" s="46"/>
+      <c r="AB147" s="46"/>
+      <c r="AC147" s="46"/>
+      <c r="AD147" s="46"/>
+      <c r="AE147" s="46"/>
+      <c r="AF147" s="46"/>
+      <c r="AG147" s="46"/>
+      <c r="AH147" s="46"/>
+      <c r="AI147" s="46"/>
+      <c r="AJ147" s="46"/>
+      <c r="AK147" s="46"/>
+      <c r="AL147" s="46"/>
+      <c r="AM147" s="46"/>
+      <c r="AN147" s="46"/>
+      <c r="AO147" s="46"/>
+      <c r="AP147" s="46"/>
+      <c r="AQ147" s="46"/>
+      <c r="AR147" s="46"/>
+      <c r="AS147" s="46"/>
+      <c r="AT147" s="46"/>
+      <c r="AU147" s="46"/>
+      <c r="AV147" s="46"/>
+      <c r="AW147" s="46"/>
+      <c r="AX147" s="46"/>
+      <c r="AY147" s="46"/>
+      <c r="AZ147" s="46"/>
+      <c r="BA147" s="46"/>
+      <c r="BB147" s="46"/>
+      <c r="BC147" s="46"/>
+      <c r="BD147" s="46"/>
+      <c r="BE147" s="46"/>
+      <c r="BF147" s="46"/>
+      <c r="BG147" s="46"/>
+      <c r="BH147" s="46"/>
+      <c r="BI147" s="46"/>
+      <c r="BJ147" s="46"/>
+      <c r="BK147" s="46"/>
+      <c r="BL147" s="46"/>
+      <c r="BM147" s="46"/>
+      <c r="BN147" s="46"/>
+      <c r="BO147" s="46"/>
+    </row>
+    <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="23"/>
+      <c r="B148" s="65"/>
+      <c r="D148" s="70"/>
+      <c r="E148" s="66"/>
+      <c r="F148" s="42"/>
+      <c r="G148" s="43"/>
+      <c r="H148" s="25"/>
+      <c r="I148" s="26"/>
+      <c r="J148" s="27"/>
+      <c r="K148" s="40"/>
+      <c r="L148" s="46"/>
+      <c r="M148" s="46"/>
+      <c r="N148" s="46"/>
+      <c r="O148" s="46"/>
+      <c r="P148" s="46"/>
+      <c r="Q148" s="46"/>
+      <c r="R148" s="46"/>
+      <c r="S148" s="46"/>
+      <c r="T148" s="46"/>
+      <c r="U148" s="46"/>
+      <c r="V148" s="46"/>
+      <c r="W148" s="46"/>
+      <c r="X148" s="46"/>
+      <c r="Y148" s="46"/>
+      <c r="Z148" s="46"/>
+      <c r="AA148" s="46"/>
+      <c r="AB148" s="46"/>
+      <c r="AC148" s="46"/>
+      <c r="AD148" s="46"/>
+      <c r="AE148" s="46"/>
+      <c r="AF148" s="46"/>
+      <c r="AG148" s="46"/>
+      <c r="AH148" s="46"/>
+      <c r="AI148" s="46"/>
+      <c r="AJ148" s="46"/>
+      <c r="AK148" s="46"/>
+      <c r="AL148" s="46"/>
+      <c r="AM148" s="46"/>
+      <c r="AN148" s="46"/>
+      <c r="AO148" s="46"/>
+      <c r="AP148" s="46"/>
+      <c r="AQ148" s="46"/>
+      <c r="AR148" s="46"/>
+      <c r="AS148" s="46"/>
+      <c r="AT148" s="46"/>
+      <c r="AU148" s="46"/>
+      <c r="AV148" s="46"/>
+      <c r="AW148" s="46"/>
+      <c r="AX148" s="46"/>
+      <c r="AY148" s="46"/>
+      <c r="AZ148" s="46"/>
+      <c r="BA148" s="46"/>
+      <c r="BB148" s="46"/>
+      <c r="BC148" s="46"/>
+      <c r="BD148" s="46"/>
+      <c r="BE148" s="46"/>
+      <c r="BF148" s="46"/>
+      <c r="BG148" s="46"/>
+      <c r="BH148" s="46"/>
+      <c r="BI148" s="46"/>
+      <c r="BJ148" s="46"/>
+      <c r="BK148" s="46"/>
+      <c r="BL148" s="46"/>
+      <c r="BM148" s="46"/>
+      <c r="BN148" s="46"/>
+      <c r="BO148" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -14835,18 +15008,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I107:I110 I98:I105">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I109:I112 I98:I107">
     <cfRule type="dataBar" priority="203">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14865,7 +15029,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L111:BO113 M114:BN119 BO117:BO119 L120:BO122 M123:BN128 BO126:BO128 L129:BO131 M132:BN137 BO135:BO137 L138:BO140 M141:BN146 BO144:BO146 M98:BN105 BO109:BO110 M107:BN110 L106:BO106">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L131:BO133 M134:BN139 BO137:BO139 L140:BO142 M143:BN148 BO146:BO148 M98:BN107 BO111:BO112 M109:BN112 L108:BO108">
     <cfRule type="expression" dxfId="104" priority="249">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -14873,7 +15037,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L107:BO110 L98:BO105">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L109:BO112 L98:BO107">
     <cfRule type="expression" dxfId="102" priority="209">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -14883,7 +15047,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E147:E1048576 E95:E96 E107:E110 E98:E105">
+  <conditionalFormatting sqref="E1:E73 E149:E1048576 E95:E96 E109:E112 E98:E107">
     <cfRule type="cellIs" dxfId="100" priority="190" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -14977,7 +15141,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I111:I119">
+  <conditionalFormatting sqref="I113:I121">
     <cfRule type="dataBar" priority="94">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -14991,12 +15155,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L111:BO119">
+  <conditionalFormatting sqref="L113:BO121">
     <cfRule type="expression" dxfId="78" priority="93">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E111:E119">
+  <conditionalFormatting sqref="E113:E121">
     <cfRule type="cellIs" dxfId="77" priority="86" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15019,7 +15183,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L114:BO119 L107:BO110 L98:BO105">
+  <conditionalFormatting sqref="L116:BO121 L109:BO112 L98:BO107">
     <cfRule type="expression" dxfId="70" priority="97">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15027,7 +15191,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I120:I128">
+  <conditionalFormatting sqref="I122:I130">
     <cfRule type="dataBar" priority="81">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15041,12 +15205,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L120:BO128">
+  <conditionalFormatting sqref="L122:BO130">
     <cfRule type="expression" dxfId="68" priority="80">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E120:E128">
+  <conditionalFormatting sqref="E122:E130">
     <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15069,7 +15233,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L123:BO128">
+  <conditionalFormatting sqref="L125:BO130">
     <cfRule type="expression" dxfId="60" priority="84">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15077,7 +15241,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I129:I137">
+  <conditionalFormatting sqref="I131:I139">
     <cfRule type="dataBar" priority="68">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15091,12 +15255,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L129:BO137">
+  <conditionalFormatting sqref="L131:BO139">
     <cfRule type="expression" dxfId="58" priority="67">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E129:E137">
+  <conditionalFormatting sqref="E131:E139">
     <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15119,7 +15283,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L132:BO137">
+  <conditionalFormatting sqref="L134:BO139">
     <cfRule type="expression" dxfId="50" priority="71">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15127,7 +15291,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I138:I146">
+  <conditionalFormatting sqref="I140:I148">
     <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15141,12 +15305,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L138:BO146">
+  <conditionalFormatting sqref="L140:BO148">
     <cfRule type="expression" dxfId="48" priority="54">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E138:E146">
+  <conditionalFormatting sqref="E140:E148">
     <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15169,7 +15333,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L141:BO146">
+  <conditionalFormatting sqref="L143:BO148">
     <cfRule type="expression" dxfId="40" priority="58">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15319,7 +15483,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I106">
+  <conditionalFormatting sqref="I108">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15333,12 +15497,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L106:BO106">
+  <conditionalFormatting sqref="L108:BO108">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
+  <conditionalFormatting sqref="E108">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15417,7 +15581,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I107:I110 I98:I105</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I109:I112 I98:I107</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -15447,7 +15611,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I111:I119</xm:sqref>
+          <xm:sqref>I113:I121</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -15462,7 +15626,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I120:I128</xm:sqref>
+          <xm:sqref>I122:I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -15477,7 +15641,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I129:I137</xm:sqref>
+          <xm:sqref>I131:I139</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -15492,7 +15656,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I138:I146</xm:sqref>
+          <xm:sqref>I140:I148</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -15552,7 +15716,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I106</xm:sqref>
+          <xm:sqref>I108</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Updated planner for structural equations (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4DC23E-DB70-4DBB-BC4D-A7546D3AEFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5849441E-2A0C-4698-901A-B9AFFAFA4F37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="134">
   <si>
     <t>WBS</t>
   </si>
@@ -802,12 +802,6 @@
     <t>Add Structural Forecasting</t>
   </si>
   <si>
-    <t>Add IRFs</t>
-  </si>
-  <si>
-    <t>Add Scenarios</t>
-  </si>
-  <si>
     <t>Structural Model</t>
   </si>
   <si>
@@ -824,6 +818,18 @@
   </si>
   <si>
     <t>Add Initial Forecast Calculated Vavriables</t>
+  </si>
+  <si>
+    <t>Add Scenario Calcs</t>
+  </si>
+  <si>
+    <t>External Forecast Improvements</t>
+  </si>
+  <si>
+    <t>Add More External Forecasts</t>
+  </si>
+  <si>
+    <t>Refactor External Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1752,6 +1758,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1761,6 +1774,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1769,17 +1786,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1828,7 +1834,82 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="106">
+  <dxfs count="116">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -2722,7 +2803,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="20"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="25"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3129,11 +3210,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO148"/>
+  <dimension ref="A1:BO150"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+      <pane ySplit="7" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G108" sqref="G108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3163,27 +3244,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3228,198 +3309,198 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 20</v>
-      </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+        <v>Week 25</v>
+      </c>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 21</v>
-      </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+        <v>Week 26</v>
+      </c>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 22</v>
-      </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+        <v>Week 27</v>
+      </c>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 23</v>
-      </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+        <v>Week 28</v>
+      </c>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 24</v>
-      </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+        <v>Week 29</v>
+      </c>
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 25</v>
-      </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+        <v>Week 30</v>
+      </c>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 26</v>
-      </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+        <v>Week 31</v>
+      </c>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 27</v>
-      </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+        <v>Week 32</v>
+      </c>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
-        <v>44326</v>
-      </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+        <v>44361</v>
+      </c>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
-        <v>44333</v>
-      </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+        <v>44368</v>
+      </c>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
-        <v>44340</v>
-      </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+        <v>44375</v>
+      </c>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
-        <v>44347</v>
-      </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+        <v>44382</v>
+      </c>
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
-        <v>44354</v>
-      </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+        <v>44389</v>
+      </c>
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
-        <v>44361</v>
-      </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+        <v>44396</v>
+      </c>
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
-        <v>44368</v>
-      </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+        <v>44403</v>
+      </c>
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
-        <v>44375</v>
-      </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+        <v>44410</v>
+      </c>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -3435,227 +3516,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44326</v>
+        <v>44361</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44327</v>
+        <v>44362</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44328</v>
+        <v>44363</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44329</v>
+        <v>44364</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44330</v>
+        <v>44365</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44331</v>
+        <v>44366</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44332</v>
+        <v>44367</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44333</v>
+        <v>44368</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44334</v>
+        <v>44369</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44335</v>
+        <v>44370</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44336</v>
+        <v>44371</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44337</v>
+        <v>44372</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44338</v>
+        <v>44373</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44339</v>
+        <v>44374</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44340</v>
+        <v>44375</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44341</v>
+        <v>44376</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44342</v>
+        <v>44377</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44343</v>
+        <v>44378</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44344</v>
+        <v>44379</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44345</v>
+        <v>44380</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44346</v>
+        <v>44381</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44347</v>
+        <v>44382</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44348</v>
+        <v>44383</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44349</v>
+        <v>44384</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44350</v>
+        <v>44385</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44351</v>
+        <v>44386</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44352</v>
+        <v>44387</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44353</v>
+        <v>44388</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44354</v>
+        <v>44389</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44355</v>
+        <v>44390</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44356</v>
+        <v>44391</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44357</v>
+        <v>44392</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44358</v>
+        <v>44393</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44359</v>
+        <v>44394</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44360</v>
+        <v>44395</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44361</v>
+        <v>44396</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44362</v>
+        <v>44397</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44363</v>
+        <v>44398</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44364</v>
+        <v>44399</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44365</v>
+        <v>44400</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44366</v>
+        <v>44401</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44367</v>
+        <v>44402</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44368</v>
+        <v>44403</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44369</v>
+        <v>44404</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44370</v>
+        <v>44405</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44371</v>
+        <v>44406</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44372</v>
+        <v>44407</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44373</v>
+        <v>44408</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44374</v>
+        <v>44409</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44375</v>
+        <v>44410</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44376</v>
+        <v>44411</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44377</v>
+        <v>44412</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44378</v>
+        <v>44413</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44379</v>
+        <v>44414</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44380</v>
+        <v>44415</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44381</v>
+        <v>44416</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8577,7 +8658,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A113" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A115" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11283,7 +11364,7 @@
         <v>9</v>
       </c>
       <c r="B97" s="17" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D97" s="19"/>
       <c r="E97" s="19"/>
@@ -11524,7 +11605,7 @@
         <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
@@ -11605,7 +11686,7 @@
         <v>9.4</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
@@ -11686,7 +11767,7 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
@@ -11695,9 +11776,13 @@
       <c r="F102" s="42">
         <v>44365</v>
       </c>
-      <c r="G102" s="43"/>
+      <c r="G102" s="43">
+        <v>44372</v>
+      </c>
       <c r="H102" s="25"/>
-      <c r="I102" s="26"/>
+      <c r="I102" s="26">
+        <v>1</v>
+      </c>
       <c r="J102" s="27"/>
       <c r="K102" s="40"/>
       <c r="L102" s="46"/>
@@ -11763,18 +11848,22 @@
         <v>9.6</v>
       </c>
       <c r="B103" s="65" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D103" s="70"/>
       <c r="E103" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F103" s="42">
-        <v>44365</v>
-      </c>
-      <c r="G103" s="43"/>
+        <v>44372</v>
+      </c>
+      <c r="G103" s="43">
+        <v>44379</v>
+      </c>
       <c r="H103" s="25"/>
-      <c r="I103" s="26"/>
+      <c r="I103" s="26">
+        <v>0</v>
+      </c>
       <c r="J103" s="27"/>
       <c r="K103" s="40"/>
       <c r="L103" s="46"/>
@@ -11847,11 +11936,15 @@
         <v>67</v>
       </c>
       <c r="F104" s="42">
-        <v>44365</v>
-      </c>
-      <c r="G104" s="43"/>
+        <v>44372</v>
+      </c>
+      <c r="G104" s="43">
+        <v>44374</v>
+      </c>
       <c r="H104" s="25"/>
-      <c r="I104" s="26"/>
+      <c r="I104" s="26">
+        <v>0</v>
+      </c>
       <c r="J104" s="27"/>
       <c r="K104" s="40"/>
       <c r="L104" s="46"/>
@@ -11924,11 +12017,15 @@
         <v>67</v>
       </c>
       <c r="F105" s="42">
-        <v>44365</v>
-      </c>
-      <c r="G105" s="43"/>
+        <v>44372</v>
+      </c>
+      <c r="G105" s="43">
+        <v>44374</v>
+      </c>
       <c r="H105" s="25"/>
-      <c r="I105" s="26"/>
+      <c r="I105" s="26">
+        <v>0</v>
+      </c>
       <c r="J105" s="27"/>
       <c r="K105" s="40"/>
       <c r="L105" s="46"/>
@@ -11994,20 +12091,24 @@
         <v>9.9</v>
       </c>
       <c r="B106" s="65" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="D106" s="70"/>
-      <c r="E106" s="66" t="s">
+      <c r="E106" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F106" s="42">
-        <v>44372</v>
-      </c>
-      <c r="G106" s="43"/>
-      <c r="H106" s="25"/>
-      <c r="I106" s="26"/>
-      <c r="J106" s="27"/>
-      <c r="K106" s="40"/>
+      <c r="F106" s="71">
+        <v>44375</v>
+      </c>
+      <c r="G106" s="72">
+        <v>44378</v>
+      </c>
+      <c r="H106" s="73"/>
+      <c r="I106" s="74">
+        <v>0</v>
+      </c>
+      <c r="J106" s="75"/>
+      <c r="K106" s="76"/>
       <c r="L106" s="46"/>
       <c r="M106" s="46"/>
       <c r="N106" s="46"/>
@@ -12065,182 +12166,182 @@
       <c r="BN106" s="46"/>
       <c r="BO106" s="46"/>
     </row>
-    <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>9.10</v>
-      </c>
-      <c r="B107" s="65" t="s">
-        <v>125</v>
-      </c>
-      <c r="D107" s="70"/>
-      <c r="E107" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F107" s="42">
-        <v>44372</v>
-      </c>
-      <c r="G107" s="43"/>
-      <c r="H107" s="25"/>
-      <c r="I107" s="26"/>
-      <c r="J107" s="27"/>
-      <c r="K107" s="40"/>
-      <c r="L107" s="46"/>
-      <c r="M107" s="46"/>
-      <c r="N107" s="46"/>
-      <c r="O107" s="46"/>
-      <c r="P107" s="46"/>
-      <c r="Q107" s="46"/>
-      <c r="R107" s="46"/>
-      <c r="S107" s="46"/>
-      <c r="T107" s="46"/>
-      <c r="U107" s="46"/>
-      <c r="V107" s="46"/>
-      <c r="W107" s="46"/>
-      <c r="X107" s="46"/>
-      <c r="Y107" s="46"/>
-      <c r="Z107" s="46"/>
-      <c r="AA107" s="46"/>
-      <c r="AB107" s="46"/>
-      <c r="AC107" s="46"/>
-      <c r="AD107" s="46"/>
-      <c r="AE107" s="46"/>
-      <c r="AF107" s="46"/>
-      <c r="AG107" s="46"/>
-      <c r="AH107" s="46"/>
-      <c r="AI107" s="46"/>
-      <c r="AJ107" s="46"/>
-      <c r="AK107" s="46"/>
-      <c r="AL107" s="46"/>
-      <c r="AM107" s="46"/>
-      <c r="AN107" s="46"/>
-      <c r="AO107" s="46"/>
-      <c r="AP107" s="46"/>
-      <c r="AQ107" s="46"/>
-      <c r="AR107" s="46"/>
-      <c r="AS107" s="46"/>
-      <c r="AT107" s="46"/>
-      <c r="AU107" s="46"/>
-      <c r="AV107" s="46"/>
-      <c r="AW107" s="46"/>
-      <c r="AX107" s="46"/>
-      <c r="AY107" s="46"/>
-      <c r="AZ107" s="46"/>
-      <c r="BA107" s="46"/>
-      <c r="BB107" s="46"/>
-      <c r="BC107" s="46"/>
-      <c r="BD107" s="46"/>
-      <c r="BE107" s="46"/>
-      <c r="BF107" s="46"/>
-      <c r="BG107" s="46"/>
-      <c r="BH107" s="46"/>
-      <c r="BI107" s="46"/>
-      <c r="BJ107" s="46"/>
-      <c r="BK107" s="46"/>
-      <c r="BL107" s="46"/>
-      <c r="BM107" s="46"/>
-      <c r="BN107" s="46"/>
-      <c r="BO107" s="46"/>
-    </row>
-    <row r="108" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="16" t="str">
+    <row r="107" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>10</v>
       </c>
-      <c r="B108" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="44"/>
-      <c r="G108" s="44" t="str">
-        <f t="shared" ref="G108" si="18">IF(ISBLANK(F108)," - ",IF(H108=0,F108,F108+H108-1))</f>
+      <c r="B107" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="44"/>
+      <c r="G107" s="44" t="str">
+        <f t="shared" ref="G107" si="18">IF(ISBLANK(F107)," - ",IF(H107=0,F107,F107+H107-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H108" s="20"/>
-      <c r="I108" s="21"/>
-      <c r="J108" s="22" t="str">
-        <f t="shared" ref="J108" si="19">IF(OR(G108=0,F108=0)," - ",NETWORKDAYS(F108,G108))</f>
+      <c r="H107" s="20"/>
+      <c r="I107" s="21"/>
+      <c r="J107" s="22" t="str">
+        <f t="shared" ref="J107" si="19">IF(OR(G107=0,F107=0)," - ",NETWORKDAYS(F107,G107))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K108" s="41"/>
-      <c r="L108" s="48"/>
-      <c r="M108" s="48"/>
-      <c r="N108" s="48"/>
-      <c r="O108" s="48"/>
-      <c r="P108" s="48"/>
-      <c r="Q108" s="48"/>
-      <c r="R108" s="48"/>
-      <c r="S108" s="48"/>
-      <c r="T108" s="48"/>
-      <c r="U108" s="48"/>
-      <c r="V108" s="48"/>
-      <c r="W108" s="48"/>
-      <c r="X108" s="48"/>
-      <c r="Y108" s="48"/>
-      <c r="Z108" s="48"/>
-      <c r="AA108" s="48"/>
-      <c r="AB108" s="48"/>
-      <c r="AC108" s="48"/>
-      <c r="AD108" s="48"/>
-      <c r="AE108" s="48"/>
-      <c r="AF108" s="48"/>
-      <c r="AG108" s="48"/>
-      <c r="AH108" s="48"/>
-      <c r="AI108" s="48"/>
-      <c r="AJ108" s="48"/>
-      <c r="AK108" s="48"/>
-      <c r="AL108" s="48"/>
-      <c r="AM108" s="48"/>
-      <c r="AN108" s="48"/>
-      <c r="AO108" s="48"/>
-      <c r="AP108" s="48"/>
-      <c r="AQ108" s="48"/>
-      <c r="AR108" s="48"/>
-      <c r="AS108" s="48"/>
-      <c r="AT108" s="48"/>
-      <c r="AU108" s="48"/>
-      <c r="AV108" s="48"/>
-      <c r="AW108" s="48"/>
-      <c r="AX108" s="48"/>
-      <c r="AY108" s="48"/>
-      <c r="AZ108" s="48"/>
-      <c r="BA108" s="48"/>
-      <c r="BB108" s="48"/>
-      <c r="BC108" s="48"/>
-      <c r="BD108" s="48"/>
-      <c r="BE108" s="48"/>
-      <c r="BF108" s="48"/>
-      <c r="BG108" s="48"/>
-      <c r="BH108" s="48"/>
-      <c r="BI108" s="48"/>
-      <c r="BJ108" s="48"/>
-      <c r="BK108" s="48"/>
-      <c r="BL108" s="48"/>
-      <c r="BM108" s="48"/>
-      <c r="BN108" s="48"/>
-      <c r="BO108" s="48"/>
+      <c r="K107" s="41"/>
+      <c r="L107" s="48"/>
+      <c r="M107" s="48"/>
+      <c r="N107" s="48"/>
+      <c r="O107" s="48"/>
+      <c r="P107" s="48"/>
+      <c r="Q107" s="48"/>
+      <c r="R107" s="48"/>
+      <c r="S107" s="48"/>
+      <c r="T107" s="48"/>
+      <c r="U107" s="48"/>
+      <c r="V107" s="48"/>
+      <c r="W107" s="48"/>
+      <c r="X107" s="48"/>
+      <c r="Y107" s="48"/>
+      <c r="Z107" s="48"/>
+      <c r="AA107" s="48"/>
+      <c r="AB107" s="48"/>
+      <c r="AC107" s="48"/>
+      <c r="AD107" s="48"/>
+      <c r="AE107" s="48"/>
+      <c r="AF107" s="48"/>
+      <c r="AG107" s="48"/>
+      <c r="AH107" s="48"/>
+      <c r="AI107" s="48"/>
+      <c r="AJ107" s="48"/>
+      <c r="AK107" s="48"/>
+      <c r="AL107" s="48"/>
+      <c r="AM107" s="48"/>
+      <c r="AN107" s="48"/>
+      <c r="AO107" s="48"/>
+      <c r="AP107" s="48"/>
+      <c r="AQ107" s="48"/>
+      <c r="AR107" s="48"/>
+      <c r="AS107" s="48"/>
+      <c r="AT107" s="48"/>
+      <c r="AU107" s="48"/>
+      <c r="AV107" s="48"/>
+      <c r="AW107" s="48"/>
+      <c r="AX107" s="48"/>
+      <c r="AY107" s="48"/>
+      <c r="AZ107" s="48"/>
+      <c r="BA107" s="48"/>
+      <c r="BB107" s="48"/>
+      <c r="BC107" s="48"/>
+      <c r="BD107" s="48"/>
+      <c r="BE107" s="48"/>
+      <c r="BF107" s="48"/>
+      <c r="BG107" s="48"/>
+      <c r="BH107" s="48"/>
+      <c r="BI107" s="48"/>
+      <c r="BJ107" s="48"/>
+      <c r="BK107" s="48"/>
+      <c r="BL107" s="48"/>
+      <c r="BM107" s="48"/>
+      <c r="BN107" s="48"/>
+      <c r="BO107" s="48"/>
+    </row>
+    <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.1</v>
+      </c>
+      <c r="B108" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D108" s="70"/>
+      <c r="E108" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F108" s="71">
+        <v>44379</v>
+      </c>
+      <c r="G108" s="72"/>
+      <c r="H108" s="73"/>
+      <c r="I108" s="74"/>
+      <c r="J108" s="75"/>
+      <c r="K108" s="76"/>
+      <c r="L108" s="46"/>
+      <c r="M108" s="46"/>
+      <c r="N108" s="46"/>
+      <c r="O108" s="46"/>
+      <c r="P108" s="46"/>
+      <c r="Q108" s="46"/>
+      <c r="R108" s="46"/>
+      <c r="S108" s="46"/>
+      <c r="T108" s="46"/>
+      <c r="U108" s="46"/>
+      <c r="V108" s="46"/>
+      <c r="W108" s="46"/>
+      <c r="X108" s="46"/>
+      <c r="Y108" s="46"/>
+      <c r="Z108" s="46"/>
+      <c r="AA108" s="46"/>
+      <c r="AB108" s="46"/>
+      <c r="AC108" s="46"/>
+      <c r="AD108" s="46"/>
+      <c r="AE108" s="46"/>
+      <c r="AF108" s="46"/>
+      <c r="AG108" s="46"/>
+      <c r="AH108" s="46"/>
+      <c r="AI108" s="46"/>
+      <c r="AJ108" s="46"/>
+      <c r="AK108" s="46"/>
+      <c r="AL108" s="46"/>
+      <c r="AM108" s="46"/>
+      <c r="AN108" s="46"/>
+      <c r="AO108" s="46"/>
+      <c r="AP108" s="46"/>
+      <c r="AQ108" s="46"/>
+      <c r="AR108" s="46"/>
+      <c r="AS108" s="46"/>
+      <c r="AT108" s="46"/>
+      <c r="AU108" s="46"/>
+      <c r="AV108" s="46"/>
+      <c r="AW108" s="46"/>
+      <c r="AX108" s="46"/>
+      <c r="AY108" s="46"/>
+      <c r="AZ108" s="46"/>
+      <c r="BA108" s="46"/>
+      <c r="BB108" s="46"/>
+      <c r="BC108" s="46"/>
+      <c r="BD108" s="46"/>
+      <c r="BE108" s="46"/>
+      <c r="BF108" s="46"/>
+      <c r="BG108" s="46"/>
+      <c r="BH108" s="46"/>
+      <c r="BI108" s="46"/>
+      <c r="BJ108" s="46"/>
+      <c r="BK108" s="46"/>
+      <c r="BL108" s="46"/>
+      <c r="BM108" s="46"/>
+      <c r="BN108" s="46"/>
+      <c r="BO108" s="46"/>
     </row>
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.1</v>
+        <v>10.2</v>
       </c>
       <c r="B109" s="65" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="D109" s="70"/>
-      <c r="E109" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F109" s="42">
-        <v>44375</v>
-      </c>
-      <c r="G109" s="43"/>
-      <c r="H109" s="25"/>
-      <c r="I109" s="26"/>
-      <c r="J109" s="27"/>
-      <c r="K109" s="40"/>
+      <c r="E109" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F109" s="71">
+        <v>44379</v>
+      </c>
+      <c r="G109" s="72"/>
+      <c r="H109" s="73"/>
+      <c r="I109" s="74"/>
+      <c r="J109" s="75"/>
+      <c r="K109" s="76"/>
       <c r="L109" s="46"/>
       <c r="M109" s="46"/>
       <c r="N109" s="46"/>
@@ -12298,97 +12399,99 @@
       <c r="BN109" s="46"/>
       <c r="BO109" s="46"/>
     </row>
-    <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>10.2</v>
-      </c>
-      <c r="B110" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D110" s="70"/>
-      <c r="E110" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F110" s="42">
-        <v>44375</v>
-      </c>
-      <c r="G110" s="43"/>
-      <c r="H110" s="25"/>
-      <c r="I110" s="26"/>
-      <c r="J110" s="27"/>
-      <c r="K110" s="40"/>
-      <c r="L110" s="46"/>
-      <c r="M110" s="46"/>
-      <c r="N110" s="46"/>
-      <c r="O110" s="46"/>
-      <c r="P110" s="46"/>
-      <c r="Q110" s="46"/>
-      <c r="R110" s="46"/>
-      <c r="S110" s="46"/>
-      <c r="T110" s="46"/>
-      <c r="U110" s="46"/>
-      <c r="V110" s="46"/>
-      <c r="W110" s="46"/>
-      <c r="X110" s="46"/>
-      <c r="Y110" s="46"/>
-      <c r="Z110" s="46"/>
-      <c r="AA110" s="46"/>
-      <c r="AB110" s="46"/>
-      <c r="AC110" s="46"/>
-      <c r="AD110" s="46"/>
-      <c r="AE110" s="46"/>
-      <c r="AF110" s="46"/>
-      <c r="AG110" s="46"/>
-      <c r="AH110" s="46"/>
-      <c r="AI110" s="46"/>
-      <c r="AJ110" s="46"/>
-      <c r="AK110" s="46"/>
-      <c r="AL110" s="46"/>
-      <c r="AM110" s="46"/>
-      <c r="AN110" s="46"/>
-      <c r="AO110" s="46"/>
-      <c r="AP110" s="46"/>
-      <c r="AQ110" s="46"/>
-      <c r="AR110" s="46"/>
-      <c r="AS110" s="46"/>
-      <c r="AT110" s="46"/>
-      <c r="AU110" s="46"/>
-      <c r="AV110" s="46"/>
-      <c r="AW110" s="46"/>
-      <c r="AX110" s="46"/>
-      <c r="AY110" s="46"/>
-      <c r="AZ110" s="46"/>
-      <c r="BA110" s="46"/>
-      <c r="BB110" s="46"/>
-      <c r="BC110" s="46"/>
-      <c r="BD110" s="46"/>
-      <c r="BE110" s="46"/>
-      <c r="BF110" s="46"/>
-      <c r="BG110" s="46"/>
-      <c r="BH110" s="46"/>
-      <c r="BI110" s="46"/>
-      <c r="BJ110" s="46"/>
-      <c r="BK110" s="46"/>
-      <c r="BL110" s="46"/>
-      <c r="BM110" s="46"/>
-      <c r="BN110" s="46"/>
-      <c r="BO110" s="46"/>
+    <row r="110" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>11</v>
+      </c>
+      <c r="B110" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="44"/>
+      <c r="G110" s="44" t="str">
+        <f t="shared" ref="G110" si="20">IF(ISBLANK(F110)," - ",IF(H110=0,F110,F110+H110-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H110" s="20"/>
+      <c r="I110" s="21"/>
+      <c r="J110" s="22" t="str">
+        <f t="shared" ref="J110" si="21">IF(OR(G110=0,F110=0)," - ",NETWORKDAYS(F110,G110))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K110" s="41"/>
+      <c r="L110" s="48"/>
+      <c r="M110" s="48"/>
+      <c r="N110" s="48"/>
+      <c r="O110" s="48"/>
+      <c r="P110" s="48"/>
+      <c r="Q110" s="48"/>
+      <c r="R110" s="48"/>
+      <c r="S110" s="48"/>
+      <c r="T110" s="48"/>
+      <c r="U110" s="48"/>
+      <c r="V110" s="48"/>
+      <c r="W110" s="48"/>
+      <c r="X110" s="48"/>
+      <c r="Y110" s="48"/>
+      <c r="Z110" s="48"/>
+      <c r="AA110" s="48"/>
+      <c r="AB110" s="48"/>
+      <c r="AC110" s="48"/>
+      <c r="AD110" s="48"/>
+      <c r="AE110" s="48"/>
+      <c r="AF110" s="48"/>
+      <c r="AG110" s="48"/>
+      <c r="AH110" s="48"/>
+      <c r="AI110" s="48"/>
+      <c r="AJ110" s="48"/>
+      <c r="AK110" s="48"/>
+      <c r="AL110" s="48"/>
+      <c r="AM110" s="48"/>
+      <c r="AN110" s="48"/>
+      <c r="AO110" s="48"/>
+      <c r="AP110" s="48"/>
+      <c r="AQ110" s="48"/>
+      <c r="AR110" s="48"/>
+      <c r="AS110" s="48"/>
+      <c r="AT110" s="48"/>
+      <c r="AU110" s="48"/>
+      <c r="AV110" s="48"/>
+      <c r="AW110" s="48"/>
+      <c r="AX110" s="48"/>
+      <c r="AY110" s="48"/>
+      <c r="AZ110" s="48"/>
+      <c r="BA110" s="48"/>
+      <c r="BB110" s="48"/>
+      <c r="BC110" s="48"/>
+      <c r="BD110" s="48"/>
+      <c r="BE110" s="48"/>
+      <c r="BF110" s="48"/>
+      <c r="BG110" s="48"/>
+      <c r="BH110" s="48"/>
+      <c r="BI110" s="48"/>
+      <c r="BJ110" s="48"/>
+      <c r="BK110" s="48"/>
+      <c r="BL110" s="48"/>
+      <c r="BM110" s="48"/>
+      <c r="BN110" s="48"/>
+      <c r="BO110" s="48"/>
     </row>
     <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.3</v>
+        <v>11.1</v>
       </c>
       <c r="B111" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D111" s="70"/>
       <c r="E111" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F111" s="42">
-        <v>44378</v>
+        <v>44379</v>
       </c>
       <c r="G111" s="43"/>
       <c r="H111" s="25"/>
@@ -12455,17 +12558,17 @@
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.4</v>
+        <v>11.2</v>
       </c>
       <c r="B112" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D112" s="70"/>
       <c r="E112" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F112" s="42">
-        <v>44381</v>
+        <v>44379</v>
       </c>
       <c r="G112" s="43"/>
       <c r="H112" s="25"/>
@@ -12532,17 +12635,17 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>10.5</v>
-      </c>
-      <c r="B113" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D113" s="66"/>
+        <v>11.3</v>
+      </c>
+      <c r="B113" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D113" s="70"/>
       <c r="E113" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F113" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G113" s="43"/>
       <c r="H113" s="25"/>
@@ -12607,11 +12710,20 @@
       <c r="BO113" s="46"/>
     </row>
     <row r="114" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="23"/>
-      <c r="B114" s="65"/>
-      <c r="D114" s="66"/>
-      <c r="E114" s="66"/>
-      <c r="F114" s="42"/>
+      <c r="A114" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.4</v>
+      </c>
+      <c r="B114" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D114" s="70"/>
+      <c r="E114" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F114" s="42">
+        <v>44379</v>
+      </c>
       <c r="G114" s="43"/>
       <c r="H114" s="25"/>
       <c r="I114" s="26"/>
@@ -12675,11 +12787,20 @@
       <c r="BO114" s="46"/>
     </row>
     <row r="115" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="23"/>
-      <c r="B115" s="65"/>
+      <c r="A115" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.5</v>
+      </c>
+      <c r="B115" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D115" s="66"/>
-      <c r="E115" s="66"/>
-      <c r="F115" s="42"/>
+      <c r="E115" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F115" s="42">
+        <v>44531</v>
+      </c>
       <c r="G115" s="43"/>
       <c r="H115" s="25"/>
       <c r="I115" s="26"/>
@@ -12813,7 +12934,7 @@
     <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="23"/>
       <c r="B117" s="65"/>
-      <c r="D117" s="70"/>
+      <c r="D117" s="66"/>
       <c r="E117" s="66"/>
       <c r="F117" s="42"/>
       <c r="G117" s="43"/>
@@ -12881,7 +13002,7 @@
     <row r="118" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="23"/>
       <c r="B118" s="65"/>
-      <c r="D118" s="70"/>
+      <c r="D118" s="66"/>
       <c r="E118" s="66"/>
       <c r="F118" s="42"/>
       <c r="G118" s="43"/>
@@ -13153,7 +13274,7 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23"/>
       <c r="B122" s="65"/>
-      <c r="D122" s="66"/>
+      <c r="D122" s="70"/>
       <c r="E122" s="66"/>
       <c r="F122" s="42"/>
       <c r="G122" s="43"/>
@@ -13221,7 +13342,7 @@
     <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="23"/>
       <c r="B123" s="65"/>
-      <c r="D123" s="66"/>
+      <c r="D123" s="70"/>
       <c r="E123" s="66"/>
       <c r="F123" s="42"/>
       <c r="G123" s="43"/>
@@ -13425,7 +13546,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="70"/>
+      <c r="D126" s="66"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -13493,7 +13614,7 @@
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23"/>
       <c r="B127" s="65"/>
-      <c r="D127" s="70"/>
+      <c r="D127" s="66"/>
       <c r="E127" s="66"/>
       <c r="F127" s="42"/>
       <c r="G127" s="43"/>
@@ -13765,7 +13886,7 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
       <c r="B131" s="65"/>
-      <c r="D131" s="66"/>
+      <c r="D131" s="70"/>
       <c r="E131" s="66"/>
       <c r="F131" s="42"/>
       <c r="G131" s="43"/>
@@ -13833,7 +13954,7 @@
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23"/>
       <c r="B132" s="65"/>
-      <c r="D132" s="66"/>
+      <c r="D132" s="70"/>
       <c r="E132" s="66"/>
       <c r="F132" s="42"/>
       <c r="G132" s="43"/>
@@ -14037,7 +14158,7 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
       <c r="B135" s="65"/>
-      <c r="D135" s="70"/>
+      <c r="D135" s="66"/>
       <c r="E135" s="66"/>
       <c r="F135" s="42"/>
       <c r="G135" s="43"/>
@@ -14105,7 +14226,7 @@
     <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="23"/>
       <c r="B136" s="65"/>
-      <c r="D136" s="70"/>
+      <c r="D136" s="66"/>
       <c r="E136" s="66"/>
       <c r="F136" s="42"/>
       <c r="G136" s="43"/>
@@ -14377,7 +14498,7 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23"/>
       <c r="B140" s="65"/>
-      <c r="D140" s="66"/>
+      <c r="D140" s="70"/>
       <c r="E140" s="66"/>
       <c r="F140" s="42"/>
       <c r="G140" s="43"/>
@@ -14445,7 +14566,7 @@
     <row r="141" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23"/>
       <c r="B141" s="65"/>
-      <c r="D141" s="66"/>
+      <c r="D141" s="70"/>
       <c r="E141" s="66"/>
       <c r="F141" s="42"/>
       <c r="G141" s="43"/>
@@ -14649,7 +14770,7 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23"/>
       <c r="B144" s="65"/>
-      <c r="D144" s="70"/>
+      <c r="D144" s="66"/>
       <c r="E144" s="66"/>
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
@@ -14717,7 +14838,7 @@
     <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23"/>
       <c r="B145" s="65"/>
-      <c r="D145" s="70"/>
+      <c r="D145" s="66"/>
       <c r="E145" s="66"/>
       <c r="F145" s="42"/>
       <c r="G145" s="43"/>
@@ -14986,18 +15107,145 @@
       <c r="BN148" s="46"/>
       <c r="BO148" s="46"/>
     </row>
+    <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="23"/>
+      <c r="B149" s="65"/>
+      <c r="D149" s="70"/>
+      <c r="E149" s="66"/>
+      <c r="F149" s="42"/>
+      <c r="G149" s="43"/>
+      <c r="H149" s="25"/>
+      <c r="I149" s="26"/>
+      <c r="J149" s="27"/>
+      <c r="K149" s="40"/>
+      <c r="L149" s="46"/>
+      <c r="M149" s="46"/>
+      <c r="N149" s="46"/>
+      <c r="O149" s="46"/>
+      <c r="P149" s="46"/>
+      <c r="Q149" s="46"/>
+      <c r="R149" s="46"/>
+      <c r="S149" s="46"/>
+      <c r="T149" s="46"/>
+      <c r="U149" s="46"/>
+      <c r="V149" s="46"/>
+      <c r="W149" s="46"/>
+      <c r="X149" s="46"/>
+      <c r="Y149" s="46"/>
+      <c r="Z149" s="46"/>
+      <c r="AA149" s="46"/>
+      <c r="AB149" s="46"/>
+      <c r="AC149" s="46"/>
+      <c r="AD149" s="46"/>
+      <c r="AE149" s="46"/>
+      <c r="AF149" s="46"/>
+      <c r="AG149" s="46"/>
+      <c r="AH149" s="46"/>
+      <c r="AI149" s="46"/>
+      <c r="AJ149" s="46"/>
+      <c r="AK149" s="46"/>
+      <c r="AL149" s="46"/>
+      <c r="AM149" s="46"/>
+      <c r="AN149" s="46"/>
+      <c r="AO149" s="46"/>
+      <c r="AP149" s="46"/>
+      <c r="AQ149" s="46"/>
+      <c r="AR149" s="46"/>
+      <c r="AS149" s="46"/>
+      <c r="AT149" s="46"/>
+      <c r="AU149" s="46"/>
+      <c r="AV149" s="46"/>
+      <c r="AW149" s="46"/>
+      <c r="AX149" s="46"/>
+      <c r="AY149" s="46"/>
+      <c r="AZ149" s="46"/>
+      <c r="BA149" s="46"/>
+      <c r="BB149" s="46"/>
+      <c r="BC149" s="46"/>
+      <c r="BD149" s="46"/>
+      <c r="BE149" s="46"/>
+      <c r="BF149" s="46"/>
+      <c r="BG149" s="46"/>
+      <c r="BH149" s="46"/>
+      <c r="BI149" s="46"/>
+      <c r="BJ149" s="46"/>
+      <c r="BK149" s="46"/>
+      <c r="BL149" s="46"/>
+      <c r="BM149" s="46"/>
+      <c r="BN149" s="46"/>
+      <c r="BO149" s="46"/>
+    </row>
+    <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="23"/>
+      <c r="B150" s="65"/>
+      <c r="D150" s="70"/>
+      <c r="E150" s="66"/>
+      <c r="F150" s="42"/>
+      <c r="G150" s="43"/>
+      <c r="H150" s="25"/>
+      <c r="I150" s="26"/>
+      <c r="J150" s="27"/>
+      <c r="K150" s="40"/>
+      <c r="L150" s="46"/>
+      <c r="M150" s="46"/>
+      <c r="N150" s="46"/>
+      <c r="O150" s="46"/>
+      <c r="P150" s="46"/>
+      <c r="Q150" s="46"/>
+      <c r="R150" s="46"/>
+      <c r="S150" s="46"/>
+      <c r="T150" s="46"/>
+      <c r="U150" s="46"/>
+      <c r="V150" s="46"/>
+      <c r="W150" s="46"/>
+      <c r="X150" s="46"/>
+      <c r="Y150" s="46"/>
+      <c r="Z150" s="46"/>
+      <c r="AA150" s="46"/>
+      <c r="AB150" s="46"/>
+      <c r="AC150" s="46"/>
+      <c r="AD150" s="46"/>
+      <c r="AE150" s="46"/>
+      <c r="AF150" s="46"/>
+      <c r="AG150" s="46"/>
+      <c r="AH150" s="46"/>
+      <c r="AI150" s="46"/>
+      <c r="AJ150" s="46"/>
+      <c r="AK150" s="46"/>
+      <c r="AL150" s="46"/>
+      <c r="AM150" s="46"/>
+      <c r="AN150" s="46"/>
+      <c r="AO150" s="46"/>
+      <c r="AP150" s="46"/>
+      <c r="AQ150" s="46"/>
+      <c r="AR150" s="46"/>
+      <c r="AS150" s="46"/>
+      <c r="AT150" s="46"/>
+      <c r="AU150" s="46"/>
+      <c r="AV150" s="46"/>
+      <c r="AW150" s="46"/>
+      <c r="AX150" s="46"/>
+      <c r="AY150" s="46"/>
+      <c r="AZ150" s="46"/>
+      <c r="BA150" s="46"/>
+      <c r="BB150" s="46"/>
+      <c r="BC150" s="46"/>
+      <c r="BD150" s="46"/>
+      <c r="BE150" s="46"/>
+      <c r="BF150" s="46"/>
+      <c r="BG150" s="46"/>
+      <c r="BH150" s="46"/>
+      <c r="BI150" s="46"/>
+      <c r="BJ150" s="46"/>
+      <c r="BK150" s="46"/>
+      <c r="BL150" s="46"/>
+      <c r="BM150" s="46"/>
+      <c r="BN150" s="46"/>
+      <c r="BO150" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -15008,10 +15256,19 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I109:I112 I98:I107">
-    <cfRule type="dataBar" priority="203">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I111:I114 I98:I106 I108:I109">
+    <cfRule type="dataBar" priority="214">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15025,66 +15282,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="105" priority="246">
+    <cfRule type="expression" dxfId="115" priority="257">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L113:BO115 M116:BN121 BO119:BO121 L122:BO124 M125:BN130 BO128:BO130 L131:BO133 M134:BN139 BO137:BO139 L140:BO142 M143:BN148 BO146:BO148 M98:BN107 BO111:BO112 M109:BN112 L108:BO108">
-    <cfRule type="expression" dxfId="104" priority="249">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 L115:BO117 M118:BN123 BO121:BO123 L124:BO126 M127:BN132 BO130:BO132 L133:BO135 M136:BN141 BO139:BO141 L142:BO144 M145:BN150 BO148:BO150 M98:BN106 BO113:BO114 M111:BN114 L110:BO110 M108:BN109">
+    <cfRule type="expression" dxfId="114" priority="260">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="250">
+    <cfRule type="expression" dxfId="113" priority="261">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L109:BO112 L98:BO107">
-    <cfRule type="expression" dxfId="102" priority="209">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L111:BO114 L98:BO106 L108:BO109">
+    <cfRule type="expression" dxfId="112" priority="220">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="101" priority="199">
+    <cfRule type="expression" dxfId="111" priority="210">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E149:E1048576 E95:E96 E109:E112 E98:E107">
-    <cfRule type="cellIs" dxfId="100" priority="190" operator="equal">
+  <conditionalFormatting sqref="E1:E73 E151:E1048576 E95:E96 E111:E114 E98:E106 E108:E109">
+    <cfRule type="cellIs" dxfId="110" priority="201" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="203" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="204" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="205" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="206" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="207" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="208" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="93" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="202" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="92" priority="255">
+    <cfRule type="expression" dxfId="102" priority="266">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="256">
+    <cfRule type="expression" dxfId="101" priority="267">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I84">
-    <cfRule type="dataBar" priority="185">
+    <cfRule type="dataBar" priority="196">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15098,51 +15355,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="90" priority="186">
+    <cfRule type="expression" dxfId="100" priority="197">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="187">
+    <cfRule type="expression" dxfId="99" priority="198">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="88" priority="184">
+    <cfRule type="expression" dxfId="98" priority="195">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="87" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="188" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="189" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="190" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="191" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="192" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="193" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="194" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="80" priority="188">
+    <cfRule type="expression" dxfId="90" priority="199">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="189">
+    <cfRule type="expression" dxfId="89" priority="200">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I113:I121">
-    <cfRule type="dataBar" priority="94">
+  <conditionalFormatting sqref="I115:I123">
+    <cfRule type="dataBar" priority="105">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15155,44 +15412,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L113:BO121">
-    <cfRule type="expression" dxfId="78" priority="93">
+  <conditionalFormatting sqref="L115:BO123">
+    <cfRule type="expression" dxfId="88" priority="104">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E113:E121">
-    <cfRule type="cellIs" dxfId="77" priority="86" operator="equal">
+  <conditionalFormatting sqref="E115:E123">
+    <cfRule type="cellIs" dxfId="87" priority="97" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="98" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="99" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="100" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="101" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="102" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="103" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L116:BO121 L109:BO112 L98:BO107">
-    <cfRule type="expression" dxfId="70" priority="97">
+  <conditionalFormatting sqref="L118:BO123 L111:BO114 L98:BO106 L108:BO109">
+    <cfRule type="expression" dxfId="80" priority="108">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="98">
+    <cfRule type="expression" dxfId="79" priority="109">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122:I130">
-    <cfRule type="dataBar" priority="81">
+  <conditionalFormatting sqref="I124:I132">
+    <cfRule type="dataBar" priority="92">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15205,44 +15462,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L122:BO130">
-    <cfRule type="expression" dxfId="68" priority="80">
+  <conditionalFormatting sqref="L124:BO132">
+    <cfRule type="expression" dxfId="78" priority="91">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122:E130">
-    <cfRule type="cellIs" dxfId="67" priority="73" operator="equal">
+  <conditionalFormatting sqref="E124:E132">
+    <cfRule type="cellIs" dxfId="77" priority="84" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="85" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="86" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="87" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="88" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="89" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="90" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO130">
-    <cfRule type="expression" dxfId="60" priority="84">
+  <conditionalFormatting sqref="L127:BO132">
+    <cfRule type="expression" dxfId="70" priority="95">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="85">
+    <cfRule type="expression" dxfId="69" priority="96">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I131:I139">
-    <cfRule type="dataBar" priority="68">
+  <conditionalFormatting sqref="I133:I141">
+    <cfRule type="dataBar" priority="79">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15255,44 +15512,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L131:BO139">
-    <cfRule type="expression" dxfId="58" priority="67">
+  <conditionalFormatting sqref="L133:BO141">
+    <cfRule type="expression" dxfId="68" priority="78">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131:E139">
-    <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
+  <conditionalFormatting sqref="E133:E141">
+    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="72" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="73" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="74" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="75" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="76" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="77" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L134:BO139">
-    <cfRule type="expression" dxfId="50" priority="71">
+  <conditionalFormatting sqref="L136:BO141">
+    <cfRule type="expression" dxfId="60" priority="82">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="72">
+    <cfRule type="expression" dxfId="59" priority="83">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I140:I148">
-    <cfRule type="dataBar" priority="55">
+  <conditionalFormatting sqref="I142:I150">
+    <cfRule type="dataBar" priority="66">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15305,44 +15562,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L140:BO148">
-    <cfRule type="expression" dxfId="48" priority="54">
+  <conditionalFormatting sqref="L142:BO150">
+    <cfRule type="expression" dxfId="58" priority="65">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E140:E148">
-    <cfRule type="cellIs" dxfId="47" priority="47" operator="equal">
+  <conditionalFormatting sqref="E142:E150">
+    <cfRule type="cellIs" dxfId="57" priority="58" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="59" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="60" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="61" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="62" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="63" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="64" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L143:BO148">
-    <cfRule type="expression" dxfId="40" priority="58">
+  <conditionalFormatting sqref="L145:BO150">
+    <cfRule type="expression" dxfId="50" priority="69">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="59">
+    <cfRule type="expression" dxfId="49" priority="70">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85:I86">
-    <cfRule type="dataBar" priority="42">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15356,11 +15613,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:BO86">
+    <cfRule type="expression" dxfId="48" priority="52">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E86">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="51" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
+    <cfRule type="expression" dxfId="40" priority="43">
+      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="44">
+      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87:I94">
+    <cfRule type="dataBar" priority="42">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
     <cfRule type="expression" dxfId="38" priority="41">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E86">
+  <conditionalFormatting sqref="E87:E94">
     <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15383,15 +15690,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="30" priority="32">
-      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="29" priority="33">
-      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I94">
+  <conditionalFormatting sqref="I97">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15400,17 +15707,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E94">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15433,58 +15740,8 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO97">
-    <cfRule type="expression" dxfId="20" priority="21">
-      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="22">
-      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I97">
+  <conditionalFormatting sqref="I110">
     <cfRule type="dataBar" priority="20">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO97">
-    <cfRule type="expression" dxfId="18" priority="19">
-      <formula>L$6=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
-      <formula>"LINUX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
-      <formula>"PHP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
-      <formula>"CSS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
-      <formula>"HTML"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
-      <formula>"R"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
-      <formula>"SQL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
-      <formula>"JS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I108">
-    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -15497,12 +15754,62 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L108:BO108">
+  <conditionalFormatting sqref="L110:BO110">
+    <cfRule type="expression" dxfId="20" priority="19">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E110">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L107:BO107">
+    <cfRule type="expression" dxfId="12" priority="10">
+      <formula>AND($F107&lt;=L$6,ROUNDDOWN(($G107-$F107+1)*$I107,0)+$F107-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="11">
+      <formula>AND(NOT(ISBLANK($F107)),$F107&lt;=L$6,$G107&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I107">
+    <cfRule type="dataBar" priority="9">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{377308A7-991B-4596-8880-3ACC1EA2DAB7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L107:BO107">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E108">
+  <conditionalFormatting sqref="E107">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15581,7 +15888,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I109:I112 I98:I107</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I111:I114 I98:I106 I108:I109</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -15611,7 +15918,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I113:I121</xm:sqref>
+          <xm:sqref>I115:I123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -15626,7 +15933,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I122:I130</xm:sqref>
+          <xm:sqref>I124:I132</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -15641,7 +15948,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I131:I139</xm:sqref>
+          <xm:sqref>I133:I141</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -15656,7 +15963,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I140:I148</xm:sqref>
+          <xm:sqref>I142:I150</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -15716,7 +16023,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I108</xm:sqref>
+          <xm:sqref>I110</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I107</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Added updated docs (v0.14)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4083E787-973A-4A77-A4AA-7669CD331D1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94038AE5-9F26-428F-9D64-318989FC8F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="140">
   <si>
     <t>WBS</t>
   </si>
@@ -802,9 +802,6 @@
     <t>Add Structural Forecasting</t>
   </si>
   <si>
-    <t>Structural Model</t>
-  </si>
-  <si>
     <t>UI Improvements</t>
   </si>
   <si>
@@ -829,10 +826,28 @@
     <t>Refactor External Forecasts</t>
   </si>
   <si>
-    <t>Structural Model Prep</t>
+    <t>Add Other Initial Forecasts</t>
   </si>
   <si>
-    <t>Add Other Initial Forecasts</t>
+    <t>Structural Model Dev</t>
+  </si>
+  <si>
+    <t>Model Rewrite</t>
+  </si>
+  <si>
+    <t>Add Nowcast to New Flow</t>
+  </si>
+  <si>
+    <t>Add Alt Initial Forecasts</t>
+  </si>
+  <si>
+    <t>Rework Webpage Nav</t>
+  </si>
+  <si>
+    <t>Add New Forecasts to Site</t>
+  </si>
+  <si>
+    <t>Add Scenario Calculations</t>
   </si>
 </sst>
 </file>
@@ -1761,6 +1776,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1770,6 +1792,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1778,17 +1804,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3274,11 +3289,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO151"/>
+  <dimension ref="A1:BO157"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
+      <pane ySplit="7" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3308,27 +3323,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3373,12 +3388,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3388,183 +3403,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8722,7 +8737,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A116" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A122" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -11669,7 +11684,7 @@
         <v>9.3</v>
       </c>
       <c r="B100" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D100" s="70"/>
       <c r="E100" s="66" t="s">
@@ -11750,7 +11765,7 @@
         <v>9.4</v>
       </c>
       <c r="B101" s="65" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D101" s="70"/>
       <c r="E101" s="66" t="s">
@@ -11831,7 +11846,7 @@
         <v>9.5</v>
       </c>
       <c r="B102" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D102" s="70"/>
       <c r="E102" s="66" t="s">
@@ -11912,7 +11927,7 @@
         <v>9.6</v>
       </c>
       <c r="B103" s="65" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D103" s="70"/>
       <c r="E103" s="70" t="s">
@@ -11993,7 +12008,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D104" s="19"/>
       <c r="E104" s="19"/>
@@ -12086,7 +12101,7 @@
       </c>
       <c r="H105" s="25"/>
       <c r="I105" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J105" s="27"/>
       <c r="K105" s="40"/>
@@ -12167,7 +12182,7 @@
       </c>
       <c r="H106" s="25"/>
       <c r="I106" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J106" s="27"/>
       <c r="K106" s="40"/>
@@ -12229,27 +12244,22 @@
       <c r="BO106" s="46"/>
     </row>
     <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>10.3</v>
-      </c>
+      <c r="A107" s="23"/>
       <c r="B107" s="65" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="D107" s="70"/>
-      <c r="E107" s="70" t="s">
+      <c r="E107" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F107" s="71">
-        <v>44379</v>
+        <v>44382</v>
       </c>
       <c r="G107" s="72">
-        <v>44382</v>
+        <v>44385</v>
       </c>
       <c r="H107" s="73"/>
-      <c r="I107" s="74">
-        <v>0</v>
-      </c>
+      <c r="I107" s="74"/>
       <c r="J107" s="75"/>
       <c r="K107" s="76"/>
       <c r="L107" s="46"/>
@@ -12309,100 +12319,88 @@
       <c r="BN107" s="46"/>
       <c r="BO107" s="46"/>
     </row>
-    <row r="108" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>11</v>
-      </c>
-      <c r="B108" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="D108" s="19"/>
-      <c r="E108" s="19"/>
-      <c r="F108" s="44"/>
-      <c r="G108" s="44" t="str">
-        <f t="shared" ref="G108" si="20">IF(ISBLANK(F108)," - ",IF(H108=0,F108,F108+H108-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H108" s="20"/>
-      <c r="I108" s="21"/>
-      <c r="J108" s="22" t="str">
-        <f t="shared" ref="J108" si="21">IF(OR(G108=0,F108=0)," - ",NETWORKDAYS(F108,G108))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K108" s="41"/>
-      <c r="L108" s="48"/>
-      <c r="M108" s="48"/>
-      <c r="N108" s="48"/>
-      <c r="O108" s="48"/>
-      <c r="P108" s="48"/>
-      <c r="Q108" s="48"/>
-      <c r="R108" s="48"/>
-      <c r="S108" s="48"/>
-      <c r="T108" s="48"/>
-      <c r="U108" s="48"/>
-      <c r="V108" s="48"/>
-      <c r="W108" s="48"/>
-      <c r="X108" s="48"/>
-      <c r="Y108" s="48"/>
-      <c r="Z108" s="48"/>
-      <c r="AA108" s="48"/>
-      <c r="AB108" s="48"/>
-      <c r="AC108" s="48"/>
-      <c r="AD108" s="48"/>
-      <c r="AE108" s="48"/>
-      <c r="AF108" s="48"/>
-      <c r="AG108" s="48"/>
-      <c r="AH108" s="48"/>
-      <c r="AI108" s="48"/>
-      <c r="AJ108" s="48"/>
-      <c r="AK108" s="48"/>
-      <c r="AL108" s="48"/>
-      <c r="AM108" s="48"/>
-      <c r="AN108" s="48"/>
-      <c r="AO108" s="48"/>
-      <c r="AP108" s="48"/>
-      <c r="AQ108" s="48"/>
-      <c r="AR108" s="48"/>
-      <c r="AS108" s="48"/>
-      <c r="AT108" s="48"/>
-      <c r="AU108" s="48"/>
-      <c r="AV108" s="48"/>
-      <c r="AW108" s="48"/>
-      <c r="AX108" s="48"/>
-      <c r="AY108" s="48"/>
-      <c r="AZ108" s="48"/>
-      <c r="BA108" s="48"/>
-      <c r="BB108" s="48"/>
-      <c r="BC108" s="48"/>
-      <c r="BD108" s="48"/>
-      <c r="BE108" s="48"/>
-      <c r="BF108" s="48"/>
-      <c r="BG108" s="48"/>
-      <c r="BH108" s="48"/>
-      <c r="BI108" s="48"/>
-      <c r="BJ108" s="48"/>
-      <c r="BK108" s="48"/>
-      <c r="BL108" s="48"/>
-      <c r="BM108" s="48"/>
-      <c r="BN108" s="48"/>
-      <c r="BO108" s="48"/>
+    <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="23"/>
+      <c r="B108" s="65" t="s">
+        <v>136</v>
+      </c>
+      <c r="D108" s="70"/>
+      <c r="E108" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F108" s="71"/>
+      <c r="G108" s="72"/>
+      <c r="H108" s="73"/>
+      <c r="I108" s="74"/>
+      <c r="J108" s="75"/>
+      <c r="K108" s="76"/>
+      <c r="L108" s="46"/>
+      <c r="M108" s="46"/>
+      <c r="N108" s="46"/>
+      <c r="O108" s="46"/>
+      <c r="P108" s="46"/>
+      <c r="Q108" s="46"/>
+      <c r="R108" s="46"/>
+      <c r="S108" s="46"/>
+      <c r="T108" s="46"/>
+      <c r="U108" s="46"/>
+      <c r="V108" s="46"/>
+      <c r="W108" s="46"/>
+      <c r="X108" s="46"/>
+      <c r="Y108" s="46"/>
+      <c r="Z108" s="46"/>
+      <c r="AA108" s="46"/>
+      <c r="AB108" s="46"/>
+      <c r="AC108" s="46"/>
+      <c r="AD108" s="46"/>
+      <c r="AE108" s="46"/>
+      <c r="AF108" s="46"/>
+      <c r="AG108" s="46"/>
+      <c r="AH108" s="46"/>
+      <c r="AI108" s="46"/>
+      <c r="AJ108" s="46"/>
+      <c r="AK108" s="46"/>
+      <c r="AL108" s="46"/>
+      <c r="AM108" s="46"/>
+      <c r="AN108" s="46"/>
+      <c r="AO108" s="46"/>
+      <c r="AP108" s="46"/>
+      <c r="AQ108" s="46"/>
+      <c r="AR108" s="46"/>
+      <c r="AS108" s="46"/>
+      <c r="AT108" s="46"/>
+      <c r="AU108" s="46"/>
+      <c r="AV108" s="46"/>
+      <c r="AW108" s="46"/>
+      <c r="AX108" s="46"/>
+      <c r="AY108" s="46"/>
+      <c r="AZ108" s="46"/>
+      <c r="BA108" s="46"/>
+      <c r="BB108" s="46"/>
+      <c r="BC108" s="46"/>
+      <c r="BD108" s="46"/>
+      <c r="BE108" s="46"/>
+      <c r="BF108" s="46"/>
+      <c r="BG108" s="46"/>
+      <c r="BH108" s="46"/>
+      <c r="BI108" s="46"/>
+      <c r="BJ108" s="46"/>
+      <c r="BK108" s="46"/>
+      <c r="BL108" s="46"/>
+      <c r="BM108" s="46"/>
+      <c r="BN108" s="46"/>
+      <c r="BO108" s="46"/>
     </row>
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>11.1</v>
-      </c>
+      <c r="A109" s="23"/>
       <c r="B109" s="65" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="D109" s="70"/>
       <c r="E109" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F109" s="71">
-        <v>44379</v>
-      </c>
+      <c r="F109" s="71"/>
       <c r="G109" s="72"/>
       <c r="H109" s="73"/>
       <c r="I109" s="74"/>
@@ -12466,20 +12464,13 @@
       <c r="BO109" s="46"/>
     </row>
     <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>11.2</v>
-      </c>
+      <c r="A110" s="23"/>
       <c r="B110" s="65" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D110" s="70"/>
-      <c r="E110" s="70" t="s">
-        <v>67</v>
-      </c>
-      <c r="F110" s="71">
-        <v>44379</v>
-      </c>
+      <c r="E110" s="66"/>
+      <c r="F110" s="71"/>
       <c r="G110" s="72"/>
       <c r="H110" s="73"/>
       <c r="I110" s="74"/>
@@ -12542,105 +12533,91 @@
       <c r="BN110" s="46"/>
       <c r="BO110" s="46"/>
     </row>
-    <row r="111" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>12</v>
-      </c>
-      <c r="B111" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D111" s="19"/>
-      <c r="E111" s="19"/>
-      <c r="F111" s="44"/>
-      <c r="G111" s="44" t="str">
-        <f t="shared" ref="G111" si="22">IF(ISBLANK(F111)," - ",IF(H111=0,F111,F111+H111-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H111" s="20"/>
-      <c r="I111" s="21"/>
-      <c r="J111" s="22" t="str">
-        <f t="shared" ref="J111" si="23">IF(OR(G111=0,F111=0)," - ",NETWORKDAYS(F111,G111))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K111" s="41"/>
-      <c r="L111" s="48"/>
-      <c r="M111" s="48"/>
-      <c r="N111" s="48"/>
-      <c r="O111" s="48"/>
-      <c r="P111" s="48"/>
-      <c r="Q111" s="48"/>
-      <c r="R111" s="48"/>
-      <c r="S111" s="48"/>
-      <c r="T111" s="48"/>
-      <c r="U111" s="48"/>
-      <c r="V111" s="48"/>
-      <c r="W111" s="48"/>
-      <c r="X111" s="48"/>
-      <c r="Y111" s="48"/>
-      <c r="Z111" s="48"/>
-      <c r="AA111" s="48"/>
-      <c r="AB111" s="48"/>
-      <c r="AC111" s="48"/>
-      <c r="AD111" s="48"/>
-      <c r="AE111" s="48"/>
-      <c r="AF111" s="48"/>
-      <c r="AG111" s="48"/>
-      <c r="AH111" s="48"/>
-      <c r="AI111" s="48"/>
-      <c r="AJ111" s="48"/>
-      <c r="AK111" s="48"/>
-      <c r="AL111" s="48"/>
-      <c r="AM111" s="48"/>
-      <c r="AN111" s="48"/>
-      <c r="AO111" s="48"/>
-      <c r="AP111" s="48"/>
-      <c r="AQ111" s="48"/>
-      <c r="AR111" s="48"/>
-      <c r="AS111" s="48"/>
-      <c r="AT111" s="48"/>
-      <c r="AU111" s="48"/>
-      <c r="AV111" s="48"/>
-      <c r="AW111" s="48"/>
-      <c r="AX111" s="48"/>
-      <c r="AY111" s="48"/>
-      <c r="AZ111" s="48"/>
-      <c r="BA111" s="48"/>
-      <c r="BB111" s="48"/>
-      <c r="BC111" s="48"/>
-      <c r="BD111" s="48"/>
-      <c r="BE111" s="48"/>
-      <c r="BF111" s="48"/>
-      <c r="BG111" s="48"/>
-      <c r="BH111" s="48"/>
-      <c r="BI111" s="48"/>
-      <c r="BJ111" s="48"/>
-      <c r="BK111" s="48"/>
-      <c r="BL111" s="48"/>
-      <c r="BM111" s="48"/>
-      <c r="BN111" s="48"/>
-      <c r="BO111" s="48"/>
+    <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="23"/>
+      <c r="B111" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="D111" s="70"/>
+      <c r="E111" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="F111" s="71"/>
+      <c r="G111" s="72"/>
+      <c r="H111" s="73"/>
+      <c r="I111" s="74"/>
+      <c r="J111" s="75"/>
+      <c r="K111" s="76"/>
+      <c r="L111" s="46"/>
+      <c r="M111" s="46"/>
+      <c r="N111" s="46"/>
+      <c r="O111" s="46"/>
+      <c r="P111" s="46"/>
+      <c r="Q111" s="46"/>
+      <c r="R111" s="46"/>
+      <c r="S111" s="46"/>
+      <c r="T111" s="46"/>
+      <c r="U111" s="46"/>
+      <c r="V111" s="46"/>
+      <c r="W111" s="46"/>
+      <c r="X111" s="46"/>
+      <c r="Y111" s="46"/>
+      <c r="Z111" s="46"/>
+      <c r="AA111" s="46"/>
+      <c r="AB111" s="46"/>
+      <c r="AC111" s="46"/>
+      <c r="AD111" s="46"/>
+      <c r="AE111" s="46"/>
+      <c r="AF111" s="46"/>
+      <c r="AG111" s="46"/>
+      <c r="AH111" s="46"/>
+      <c r="AI111" s="46"/>
+      <c r="AJ111" s="46"/>
+      <c r="AK111" s="46"/>
+      <c r="AL111" s="46"/>
+      <c r="AM111" s="46"/>
+      <c r="AN111" s="46"/>
+      <c r="AO111" s="46"/>
+      <c r="AP111" s="46"/>
+      <c r="AQ111" s="46"/>
+      <c r="AR111" s="46"/>
+      <c r="AS111" s="46"/>
+      <c r="AT111" s="46"/>
+      <c r="AU111" s="46"/>
+      <c r="AV111" s="46"/>
+      <c r="AW111" s="46"/>
+      <c r="AX111" s="46"/>
+      <c r="AY111" s="46"/>
+      <c r="AZ111" s="46"/>
+      <c r="BA111" s="46"/>
+      <c r="BB111" s="46"/>
+      <c r="BC111" s="46"/>
+      <c r="BD111" s="46"/>
+      <c r="BE111" s="46"/>
+      <c r="BF111" s="46"/>
+      <c r="BG111" s="46"/>
+      <c r="BH111" s="46"/>
+      <c r="BI111" s="46"/>
+      <c r="BJ111" s="46"/>
+      <c r="BK111" s="46"/>
+      <c r="BL111" s="46"/>
+      <c r="BM111" s="46"/>
+      <c r="BN111" s="46"/>
+      <c r="BO111" s="46"/>
     </row>
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>12.1</v>
-      </c>
-      <c r="B112" s="65" t="s">
-        <v>105</v>
-      </c>
+      <c r="A112" s="23"/>
+      <c r="B112" s="65"/>
       <c r="D112" s="70"/>
       <c r="E112" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F112" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G112" s="43"/>
-      <c r="H112" s="25"/>
-      <c r="I112" s="26"/>
-      <c r="J112" s="27"/>
-      <c r="K112" s="40"/>
+        <v>67</v>
+      </c>
+      <c r="F112" s="71"/>
+      <c r="G112" s="72"/>
+      <c r="H112" s="73"/>
+      <c r="I112" s="74"/>
+      <c r="J112" s="75"/>
+      <c r="K112" s="76"/>
       <c r="L112" s="46"/>
       <c r="M112" s="46"/>
       <c r="N112" s="46"/>
@@ -12701,23 +12678,27 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
+        <v>0.1</v>
       </c>
       <c r="B113" s="65" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="D113" s="70"/>
       <c r="E113" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F113" s="42">
+        <v>67</v>
+      </c>
+      <c r="F113" s="71">
         <v>44379</v>
       </c>
-      <c r="G113" s="43"/>
-      <c r="H113" s="25"/>
-      <c r="I113" s="26"/>
-      <c r="J113" s="27"/>
-      <c r="K113" s="40"/>
+      <c r="G113" s="72">
+        <v>44382</v>
+      </c>
+      <c r="H113" s="73"/>
+      <c r="I113" s="74">
+        <v>0</v>
+      </c>
+      <c r="J113" s="75"/>
+      <c r="K113" s="76"/>
       <c r="L113" s="46"/>
       <c r="M113" s="46"/>
       <c r="N113" s="46"/>
@@ -12775,103 +12756,105 @@
       <c r="BN113" s="46"/>
       <c r="BO113" s="46"/>
     </row>
-    <row r="114" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>12.3</v>
-      </c>
-      <c r="B114" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="D114" s="70"/>
-      <c r="E114" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F114" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G114" s="43"/>
-      <c r="H114" s="25"/>
-      <c r="I114" s="26"/>
-      <c r="J114" s="27"/>
-      <c r="K114" s="40"/>
-      <c r="L114" s="46"/>
-      <c r="M114" s="46"/>
-      <c r="N114" s="46"/>
-      <c r="O114" s="46"/>
-      <c r="P114" s="46"/>
-      <c r="Q114" s="46"/>
-      <c r="R114" s="46"/>
-      <c r="S114" s="46"/>
-      <c r="T114" s="46"/>
-      <c r="U114" s="46"/>
-      <c r="V114" s="46"/>
-      <c r="W114" s="46"/>
-      <c r="X114" s="46"/>
-      <c r="Y114" s="46"/>
-      <c r="Z114" s="46"/>
-      <c r="AA114" s="46"/>
-      <c r="AB114" s="46"/>
-      <c r="AC114" s="46"/>
-      <c r="AD114" s="46"/>
-      <c r="AE114" s="46"/>
-      <c r="AF114" s="46"/>
-      <c r="AG114" s="46"/>
-      <c r="AH114" s="46"/>
-      <c r="AI114" s="46"/>
-      <c r="AJ114" s="46"/>
-      <c r="AK114" s="46"/>
-      <c r="AL114" s="46"/>
-      <c r="AM114" s="46"/>
-      <c r="AN114" s="46"/>
-      <c r="AO114" s="46"/>
-      <c r="AP114" s="46"/>
-      <c r="AQ114" s="46"/>
-      <c r="AR114" s="46"/>
-      <c r="AS114" s="46"/>
-      <c r="AT114" s="46"/>
-      <c r="AU114" s="46"/>
-      <c r="AV114" s="46"/>
-      <c r="AW114" s="46"/>
-      <c r="AX114" s="46"/>
-      <c r="AY114" s="46"/>
-      <c r="AZ114" s="46"/>
-      <c r="BA114" s="46"/>
-      <c r="BB114" s="46"/>
-      <c r="BC114" s="46"/>
-      <c r="BD114" s="46"/>
-      <c r="BE114" s="46"/>
-      <c r="BF114" s="46"/>
-      <c r="BG114" s="46"/>
-      <c r="BH114" s="46"/>
-      <c r="BI114" s="46"/>
-      <c r="BJ114" s="46"/>
-      <c r="BK114" s="46"/>
-      <c r="BL114" s="46"/>
-      <c r="BM114" s="46"/>
-      <c r="BN114" s="46"/>
-      <c r="BO114" s="46"/>
+    <row r="114" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B114" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="44"/>
+      <c r="G114" s="44" t="str">
+        <f t="shared" ref="G114" si="20">IF(ISBLANK(F114)," - ",IF(H114=0,F114,F114+H114-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H114" s="20"/>
+      <c r="I114" s="21"/>
+      <c r="J114" s="22" t="str">
+        <f t="shared" ref="J114" si="21">IF(OR(G114=0,F114=0)," - ",NETWORKDAYS(F114,G114))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K114" s="41"/>
+      <c r="L114" s="48"/>
+      <c r="M114" s="48"/>
+      <c r="N114" s="48"/>
+      <c r="O114" s="48"/>
+      <c r="P114" s="48"/>
+      <c r="Q114" s="48"/>
+      <c r="R114" s="48"/>
+      <c r="S114" s="48"/>
+      <c r="T114" s="48"/>
+      <c r="U114" s="48"/>
+      <c r="V114" s="48"/>
+      <c r="W114" s="48"/>
+      <c r="X114" s="48"/>
+      <c r="Y114" s="48"/>
+      <c r="Z114" s="48"/>
+      <c r="AA114" s="48"/>
+      <c r="AB114" s="48"/>
+      <c r="AC114" s="48"/>
+      <c r="AD114" s="48"/>
+      <c r="AE114" s="48"/>
+      <c r="AF114" s="48"/>
+      <c r="AG114" s="48"/>
+      <c r="AH114" s="48"/>
+      <c r="AI114" s="48"/>
+      <c r="AJ114" s="48"/>
+      <c r="AK114" s="48"/>
+      <c r="AL114" s="48"/>
+      <c r="AM114" s="48"/>
+      <c r="AN114" s="48"/>
+      <c r="AO114" s="48"/>
+      <c r="AP114" s="48"/>
+      <c r="AQ114" s="48"/>
+      <c r="AR114" s="48"/>
+      <c r="AS114" s="48"/>
+      <c r="AT114" s="48"/>
+      <c r="AU114" s="48"/>
+      <c r="AV114" s="48"/>
+      <c r="AW114" s="48"/>
+      <c r="AX114" s="48"/>
+      <c r="AY114" s="48"/>
+      <c r="AZ114" s="48"/>
+      <c r="BA114" s="48"/>
+      <c r="BB114" s="48"/>
+      <c r="BC114" s="48"/>
+      <c r="BD114" s="48"/>
+      <c r="BE114" s="48"/>
+      <c r="BF114" s="48"/>
+      <c r="BG114" s="48"/>
+      <c r="BH114" s="48"/>
+      <c r="BI114" s="48"/>
+      <c r="BJ114" s="48"/>
+      <c r="BK114" s="48"/>
+      <c r="BL114" s="48"/>
+      <c r="BM114" s="48"/>
+      <c r="BN114" s="48"/>
+      <c r="BO114" s="48"/>
     </row>
     <row r="115" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.4</v>
+        <v>1.1</v>
       </c>
       <c r="B115" s="65" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="D115" s="70"/>
       <c r="E115" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F115" s="42">
+      <c r="F115" s="71">
         <v>44379</v>
       </c>
-      <c r="G115" s="43"/>
-      <c r="H115" s="25"/>
-      <c r="I115" s="26"/>
-      <c r="J115" s="27"/>
-      <c r="K115" s="40"/>
+      <c r="G115" s="72"/>
+      <c r="H115" s="73"/>
+      <c r="I115" s="74"/>
+      <c r="J115" s="75"/>
+      <c r="K115" s="76"/>
       <c r="L115" s="46"/>
       <c r="M115" s="46"/>
       <c r="N115" s="46"/>
@@ -12932,23 +12915,23 @@
     <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.5</v>
-      </c>
-      <c r="B116" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D116" s="66"/>
-      <c r="E116" s="66" t="s">
+        <v>1.2</v>
+      </c>
+      <c r="B116" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="D116" s="70"/>
+      <c r="E116" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="F116" s="42">
-        <v>44531</v>
-      </c>
-      <c r="G116" s="43"/>
-      <c r="H116" s="25"/>
-      <c r="I116" s="26"/>
-      <c r="J116" s="27"/>
-      <c r="K116" s="40"/>
+      <c r="F116" s="71">
+        <v>44379</v>
+      </c>
+      <c r="G116" s="72"/>
+      <c r="H116" s="73"/>
+      <c r="I116" s="74"/>
+      <c r="J116" s="75"/>
+      <c r="K116" s="76"/>
       <c r="L116" s="46"/>
       <c r="M116" s="46"/>
       <c r="N116" s="46"/>
@@ -13006,80 +12989,100 @@
       <c r="BN116" s="46"/>
       <c r="BO116" s="46"/>
     </row>
-    <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="23"/>
-      <c r="B117" s="65"/>
-      <c r="D117" s="66"/>
-      <c r="E117" s="66"/>
-      <c r="F117" s="42"/>
-      <c r="G117" s="43"/>
-      <c r="H117" s="25"/>
-      <c r="I117" s="26"/>
-      <c r="J117" s="27"/>
-      <c r="K117" s="40"/>
-      <c r="L117" s="46"/>
-      <c r="M117" s="46"/>
-      <c r="N117" s="46"/>
-      <c r="O117" s="46"/>
-      <c r="P117" s="46"/>
-      <c r="Q117" s="46"/>
-      <c r="R117" s="46"/>
-      <c r="S117" s="46"/>
-      <c r="T117" s="46"/>
-      <c r="U117" s="46"/>
-      <c r="V117" s="46"/>
-      <c r="W117" s="46"/>
-      <c r="X117" s="46"/>
-      <c r="Y117" s="46"/>
-      <c r="Z117" s="46"/>
-      <c r="AA117" s="46"/>
-      <c r="AB117" s="46"/>
-      <c r="AC117" s="46"/>
-      <c r="AD117" s="46"/>
-      <c r="AE117" s="46"/>
-      <c r="AF117" s="46"/>
-      <c r="AG117" s="46"/>
-      <c r="AH117" s="46"/>
-      <c r="AI117" s="46"/>
-      <c r="AJ117" s="46"/>
-      <c r="AK117" s="46"/>
-      <c r="AL117" s="46"/>
-      <c r="AM117" s="46"/>
-      <c r="AN117" s="46"/>
-      <c r="AO117" s="46"/>
-      <c r="AP117" s="46"/>
-      <c r="AQ117" s="46"/>
-      <c r="AR117" s="46"/>
-      <c r="AS117" s="46"/>
-      <c r="AT117" s="46"/>
-      <c r="AU117" s="46"/>
-      <c r="AV117" s="46"/>
-      <c r="AW117" s="46"/>
-      <c r="AX117" s="46"/>
-      <c r="AY117" s="46"/>
-      <c r="AZ117" s="46"/>
-      <c r="BA117" s="46"/>
-      <c r="BB117" s="46"/>
-      <c r="BC117" s="46"/>
-      <c r="BD117" s="46"/>
-      <c r="BE117" s="46"/>
-      <c r="BF117" s="46"/>
-      <c r="BG117" s="46"/>
-      <c r="BH117" s="46"/>
-      <c r="BI117" s="46"/>
-      <c r="BJ117" s="46"/>
-      <c r="BK117" s="46"/>
-      <c r="BL117" s="46"/>
-      <c r="BM117" s="46"/>
-      <c r="BN117" s="46"/>
-      <c r="BO117" s="46"/>
+    <row r="117" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>2</v>
+      </c>
+      <c r="B117" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="44" t="str">
+        <f t="shared" ref="G117" si="22">IF(ISBLANK(F117)," - ",IF(H117=0,F117,F117+H117-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H117" s="20"/>
+      <c r="I117" s="21"/>
+      <c r="J117" s="22" t="str">
+        <f t="shared" ref="J117" si="23">IF(OR(G117=0,F117=0)," - ",NETWORKDAYS(F117,G117))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K117" s="41"/>
+      <c r="L117" s="48"/>
+      <c r="M117" s="48"/>
+      <c r="N117" s="48"/>
+      <c r="O117" s="48"/>
+      <c r="P117" s="48"/>
+      <c r="Q117" s="48"/>
+      <c r="R117" s="48"/>
+      <c r="S117" s="48"/>
+      <c r="T117" s="48"/>
+      <c r="U117" s="48"/>
+      <c r="V117" s="48"/>
+      <c r="W117" s="48"/>
+      <c r="X117" s="48"/>
+      <c r="Y117" s="48"/>
+      <c r="Z117" s="48"/>
+      <c r="AA117" s="48"/>
+      <c r="AB117" s="48"/>
+      <c r="AC117" s="48"/>
+      <c r="AD117" s="48"/>
+      <c r="AE117" s="48"/>
+      <c r="AF117" s="48"/>
+      <c r="AG117" s="48"/>
+      <c r="AH117" s="48"/>
+      <c r="AI117" s="48"/>
+      <c r="AJ117" s="48"/>
+      <c r="AK117" s="48"/>
+      <c r="AL117" s="48"/>
+      <c r="AM117" s="48"/>
+      <c r="AN117" s="48"/>
+      <c r="AO117" s="48"/>
+      <c r="AP117" s="48"/>
+      <c r="AQ117" s="48"/>
+      <c r="AR117" s="48"/>
+      <c r="AS117" s="48"/>
+      <c r="AT117" s="48"/>
+      <c r="AU117" s="48"/>
+      <c r="AV117" s="48"/>
+      <c r="AW117" s="48"/>
+      <c r="AX117" s="48"/>
+      <c r="AY117" s="48"/>
+      <c r="AZ117" s="48"/>
+      <c r="BA117" s="48"/>
+      <c r="BB117" s="48"/>
+      <c r="BC117" s="48"/>
+      <c r="BD117" s="48"/>
+      <c r="BE117" s="48"/>
+      <c r="BF117" s="48"/>
+      <c r="BG117" s="48"/>
+      <c r="BH117" s="48"/>
+      <c r="BI117" s="48"/>
+      <c r="BJ117" s="48"/>
+      <c r="BK117" s="48"/>
+      <c r="BL117" s="48"/>
+      <c r="BM117" s="48"/>
+      <c r="BN117" s="48"/>
+      <c r="BO117" s="48"/>
     </row>
     <row r="118" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="23"/>
-      <c r="B118" s="65"/>
-      <c r="D118" s="66"/>
-      <c r="E118" s="66"/>
-      <c r="F118" s="42"/>
+      <c r="A118" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>2.1</v>
+      </c>
+      <c r="B118" s="65" t="s">
+        <v>105</v>
+      </c>
+      <c r="D118" s="70"/>
+      <c r="E118" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="F118" s="42">
+        <v>44379</v>
+      </c>
       <c r="G118" s="43"/>
       <c r="H118" s="25"/>
       <c r="I118" s="26"/>
@@ -13143,11 +13146,20 @@
       <c r="BO118" s="46"/>
     </row>
     <row r="119" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="23"/>
-      <c r="B119" s="65"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="42"/>
+      <c r="A119" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>2.2</v>
+      </c>
+      <c r="B119" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="D119" s="70"/>
+      <c r="E119" s="66" t="s">
+        <v>70</v>
+      </c>
+      <c r="F119" s="42">
+        <v>44379</v>
+      </c>
       <c r="G119" s="43"/>
       <c r="H119" s="25"/>
       <c r="I119" s="26"/>
@@ -13211,11 +13223,20 @@
       <c r="BO119" s="46"/>
     </row>
     <row r="120" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="23"/>
-      <c r="B120" s="65"/>
+      <c r="A120" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>2.3</v>
+      </c>
+      <c r="B120" s="65" t="s">
+        <v>108</v>
+      </c>
       <c r="D120" s="70"/>
-      <c r="E120" s="66"/>
-      <c r="F120" s="42"/>
+      <c r="E120" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F120" s="42">
+        <v>44379</v>
+      </c>
       <c r="G120" s="43"/>
       <c r="H120" s="25"/>
       <c r="I120" s="26"/>
@@ -13279,11 +13300,20 @@
       <c r="BO120" s="46"/>
     </row>
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="23"/>
-      <c r="B121" s="65"/>
+      <c r="A121" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>2.4</v>
+      </c>
+      <c r="B121" s="65" t="s">
+        <v>109</v>
+      </c>
       <c r="D121" s="70"/>
-      <c r="E121" s="66"/>
-      <c r="F121" s="42"/>
+      <c r="E121" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F121" s="42">
+        <v>44379</v>
+      </c>
       <c r="G121" s="43"/>
       <c r="H121" s="25"/>
       <c r="I121" s="26"/>
@@ -13347,11 +13377,20 @@
       <c r="BO121" s="46"/>
     </row>
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="23"/>
-      <c r="B122" s="65"/>
-      <c r="D122" s="70"/>
-      <c r="E122" s="66"/>
-      <c r="F122" s="42"/>
+      <c r="A122" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>2.5</v>
+      </c>
+      <c r="B122" s="77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D122" s="66"/>
+      <c r="E122" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F122" s="42">
+        <v>44531</v>
+      </c>
       <c r="G122" s="43"/>
       <c r="H122" s="25"/>
       <c r="I122" s="26"/>
@@ -13417,7 +13456,7 @@
     <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="23"/>
       <c r="B123" s="65"/>
-      <c r="D123" s="70"/>
+      <c r="D123" s="66"/>
       <c r="E123" s="66"/>
       <c r="F123" s="42"/>
       <c r="G123" s="43"/>
@@ -13485,7 +13524,7 @@
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23"/>
       <c r="B124" s="65"/>
-      <c r="D124" s="70"/>
+      <c r="D124" s="66"/>
       <c r="E124" s="66"/>
       <c r="F124" s="42"/>
       <c r="G124" s="43"/>
@@ -13621,7 +13660,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="66"/>
+      <c r="D126" s="70"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -13689,7 +13728,7 @@
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23"/>
       <c r="B127" s="65"/>
-      <c r="D127" s="66"/>
+      <c r="D127" s="70"/>
       <c r="E127" s="66"/>
       <c r="F127" s="42"/>
       <c r="G127" s="43"/>
@@ -13757,7 +13796,7 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23"/>
       <c r="B128" s="65"/>
-      <c r="D128" s="66"/>
+      <c r="D128" s="70"/>
       <c r="E128" s="66"/>
       <c r="F128" s="42"/>
       <c r="G128" s="43"/>
@@ -13961,7 +14000,7 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
       <c r="B131" s="65"/>
-      <c r="D131" s="70"/>
+      <c r="D131" s="66"/>
       <c r="E131" s="66"/>
       <c r="F131" s="42"/>
       <c r="G131" s="43"/>
@@ -14029,7 +14068,7 @@
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23"/>
       <c r="B132" s="65"/>
-      <c r="D132" s="70"/>
+      <c r="D132" s="66"/>
       <c r="E132" s="66"/>
       <c r="F132" s="42"/>
       <c r="G132" s="43"/>
@@ -14097,7 +14136,7 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23"/>
       <c r="B133" s="65"/>
-      <c r="D133" s="70"/>
+      <c r="D133" s="66"/>
       <c r="E133" s="66"/>
       <c r="F133" s="42"/>
       <c r="G133" s="43"/>
@@ -14233,7 +14272,7 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
       <c r="B135" s="65"/>
-      <c r="D135" s="66"/>
+      <c r="D135" s="70"/>
       <c r="E135" s="66"/>
       <c r="F135" s="42"/>
       <c r="G135" s="43"/>
@@ -14301,7 +14340,7 @@
     <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="23"/>
       <c r="B136" s="65"/>
-      <c r="D136" s="66"/>
+      <c r="D136" s="70"/>
       <c r="E136" s="66"/>
       <c r="F136" s="42"/>
       <c r="G136" s="43"/>
@@ -14369,7 +14408,7 @@
     <row r="137" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="23"/>
       <c r="B137" s="65"/>
-      <c r="D137" s="66"/>
+      <c r="D137" s="70"/>
       <c r="E137" s="66"/>
       <c r="F137" s="42"/>
       <c r="G137" s="43"/>
@@ -14573,7 +14612,7 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23"/>
       <c r="B140" s="65"/>
-      <c r="D140" s="70"/>
+      <c r="D140" s="66"/>
       <c r="E140" s="66"/>
       <c r="F140" s="42"/>
       <c r="G140" s="43"/>
@@ -14641,7 +14680,7 @@
     <row r="141" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23"/>
       <c r="B141" s="65"/>
-      <c r="D141" s="70"/>
+      <c r="D141" s="66"/>
       <c r="E141" s="66"/>
       <c r="F141" s="42"/>
       <c r="G141" s="43"/>
@@ -14709,7 +14748,7 @@
     <row r="142" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23"/>
       <c r="B142" s="65"/>
-      <c r="D142" s="70"/>
+      <c r="D142" s="66"/>
       <c r="E142" s="66"/>
       <c r="F142" s="42"/>
       <c r="G142" s="43"/>
@@ -14845,7 +14884,7 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23"/>
       <c r="B144" s="65"/>
-      <c r="D144" s="66"/>
+      <c r="D144" s="70"/>
       <c r="E144" s="66"/>
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
@@ -14913,7 +14952,7 @@
     <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23"/>
       <c r="B145" s="65"/>
-      <c r="D145" s="66"/>
+      <c r="D145" s="70"/>
       <c r="E145" s="66"/>
       <c r="F145" s="42"/>
       <c r="G145" s="43"/>
@@ -14981,7 +15020,7 @@
     <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23"/>
       <c r="B146" s="65"/>
-      <c r="D146" s="66"/>
+      <c r="D146" s="70"/>
       <c r="E146" s="66"/>
       <c r="F146" s="42"/>
       <c r="G146" s="43"/>
@@ -15185,7 +15224,7 @@
     <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="23"/>
       <c r="B149" s="65"/>
-      <c r="D149" s="70"/>
+      <c r="D149" s="66"/>
       <c r="E149" s="66"/>
       <c r="F149" s="42"/>
       <c r="G149" s="43"/>
@@ -15253,7 +15292,7 @@
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23"/>
       <c r="B150" s="65"/>
-      <c r="D150" s="70"/>
+      <c r="D150" s="66"/>
       <c r="E150" s="66"/>
       <c r="F150" s="42"/>
       <c r="G150" s="43"/>
@@ -15321,7 +15360,7 @@
     <row r="151" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="23"/>
       <c r="B151" s="65"/>
-      <c r="D151" s="70"/>
+      <c r="D151" s="66"/>
       <c r="E151" s="66"/>
       <c r="F151" s="42"/>
       <c r="G151" s="43"/>
@@ -15386,18 +15425,417 @@
       <c r="BN151" s="46"/>
       <c r="BO151" s="46"/>
     </row>
+    <row r="152" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="23"/>
+      <c r="B152" s="65"/>
+      <c r="D152" s="66"/>
+      <c r="E152" s="66"/>
+      <c r="F152" s="42"/>
+      <c r="G152" s="43"/>
+      <c r="H152" s="25"/>
+      <c r="I152" s="26"/>
+      <c r="J152" s="27"/>
+      <c r="K152" s="40"/>
+      <c r="L152" s="46"/>
+      <c r="M152" s="46"/>
+      <c r="N152" s="46"/>
+      <c r="O152" s="46"/>
+      <c r="P152" s="46"/>
+      <c r="Q152" s="46"/>
+      <c r="R152" s="46"/>
+      <c r="S152" s="46"/>
+      <c r="T152" s="46"/>
+      <c r="U152" s="46"/>
+      <c r="V152" s="46"/>
+      <c r="W152" s="46"/>
+      <c r="X152" s="46"/>
+      <c r="Y152" s="46"/>
+      <c r="Z152" s="46"/>
+      <c r="AA152" s="46"/>
+      <c r="AB152" s="46"/>
+      <c r="AC152" s="46"/>
+      <c r="AD152" s="46"/>
+      <c r="AE152" s="46"/>
+      <c r="AF152" s="46"/>
+      <c r="AG152" s="46"/>
+      <c r="AH152" s="46"/>
+      <c r="AI152" s="46"/>
+      <c r="AJ152" s="46"/>
+      <c r="AK152" s="46"/>
+      <c r="AL152" s="46"/>
+      <c r="AM152" s="46"/>
+      <c r="AN152" s="46"/>
+      <c r="AO152" s="46"/>
+      <c r="AP152" s="46"/>
+      <c r="AQ152" s="46"/>
+      <c r="AR152" s="46"/>
+      <c r="AS152" s="46"/>
+      <c r="AT152" s="46"/>
+      <c r="AU152" s="46"/>
+      <c r="AV152" s="46"/>
+      <c r="AW152" s="46"/>
+      <c r="AX152" s="46"/>
+      <c r="AY152" s="46"/>
+      <c r="AZ152" s="46"/>
+      <c r="BA152" s="46"/>
+      <c r="BB152" s="46"/>
+      <c r="BC152" s="46"/>
+      <c r="BD152" s="46"/>
+      <c r="BE152" s="46"/>
+      <c r="BF152" s="46"/>
+      <c r="BG152" s="46"/>
+      <c r="BH152" s="46"/>
+      <c r="BI152" s="46"/>
+      <c r="BJ152" s="46"/>
+      <c r="BK152" s="46"/>
+      <c r="BL152" s="46"/>
+      <c r="BM152" s="46"/>
+      <c r="BN152" s="46"/>
+      <c r="BO152" s="46"/>
+    </row>
+    <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="23"/>
+      <c r="B153" s="65"/>
+      <c r="D153" s="70"/>
+      <c r="E153" s="66"/>
+      <c r="F153" s="42"/>
+      <c r="G153" s="43"/>
+      <c r="H153" s="25"/>
+      <c r="I153" s="26"/>
+      <c r="J153" s="27"/>
+      <c r="K153" s="40"/>
+      <c r="L153" s="46"/>
+      <c r="M153" s="46"/>
+      <c r="N153" s="46"/>
+      <c r="O153" s="46"/>
+      <c r="P153" s="46"/>
+      <c r="Q153" s="46"/>
+      <c r="R153" s="46"/>
+      <c r="S153" s="46"/>
+      <c r="T153" s="46"/>
+      <c r="U153" s="46"/>
+      <c r="V153" s="46"/>
+      <c r="W153" s="46"/>
+      <c r="X153" s="46"/>
+      <c r="Y153" s="46"/>
+      <c r="Z153" s="46"/>
+      <c r="AA153" s="46"/>
+      <c r="AB153" s="46"/>
+      <c r="AC153" s="46"/>
+      <c r="AD153" s="46"/>
+      <c r="AE153" s="46"/>
+      <c r="AF153" s="46"/>
+      <c r="AG153" s="46"/>
+      <c r="AH153" s="46"/>
+      <c r="AI153" s="46"/>
+      <c r="AJ153" s="46"/>
+      <c r="AK153" s="46"/>
+      <c r="AL153" s="46"/>
+      <c r="AM153" s="46"/>
+      <c r="AN153" s="46"/>
+      <c r="AO153" s="46"/>
+      <c r="AP153" s="46"/>
+      <c r="AQ153" s="46"/>
+      <c r="AR153" s="46"/>
+      <c r="AS153" s="46"/>
+      <c r="AT153" s="46"/>
+      <c r="AU153" s="46"/>
+      <c r="AV153" s="46"/>
+      <c r="AW153" s="46"/>
+      <c r="AX153" s="46"/>
+      <c r="AY153" s="46"/>
+      <c r="AZ153" s="46"/>
+      <c r="BA153" s="46"/>
+      <c r="BB153" s="46"/>
+      <c r="BC153" s="46"/>
+      <c r="BD153" s="46"/>
+      <c r="BE153" s="46"/>
+      <c r="BF153" s="46"/>
+      <c r="BG153" s="46"/>
+      <c r="BH153" s="46"/>
+      <c r="BI153" s="46"/>
+      <c r="BJ153" s="46"/>
+      <c r="BK153" s="46"/>
+      <c r="BL153" s="46"/>
+      <c r="BM153" s="46"/>
+      <c r="BN153" s="46"/>
+      <c r="BO153" s="46"/>
+    </row>
+    <row r="154" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="23"/>
+      <c r="B154" s="65"/>
+      <c r="D154" s="70"/>
+      <c r="E154" s="66"/>
+      <c r="F154" s="42"/>
+      <c r="G154" s="43"/>
+      <c r="H154" s="25"/>
+      <c r="I154" s="26"/>
+      <c r="J154" s="27"/>
+      <c r="K154" s="40"/>
+      <c r="L154" s="46"/>
+      <c r="M154" s="46"/>
+      <c r="N154" s="46"/>
+      <c r="O154" s="46"/>
+      <c r="P154" s="46"/>
+      <c r="Q154" s="46"/>
+      <c r="R154" s="46"/>
+      <c r="S154" s="46"/>
+      <c r="T154" s="46"/>
+      <c r="U154" s="46"/>
+      <c r="V154" s="46"/>
+      <c r="W154" s="46"/>
+      <c r="X154" s="46"/>
+      <c r="Y154" s="46"/>
+      <c r="Z154" s="46"/>
+      <c r="AA154" s="46"/>
+      <c r="AB154" s="46"/>
+      <c r="AC154" s="46"/>
+      <c r="AD154" s="46"/>
+      <c r="AE154" s="46"/>
+      <c r="AF154" s="46"/>
+      <c r="AG154" s="46"/>
+      <c r="AH154" s="46"/>
+      <c r="AI154" s="46"/>
+      <c r="AJ154" s="46"/>
+      <c r="AK154" s="46"/>
+      <c r="AL154" s="46"/>
+      <c r="AM154" s="46"/>
+      <c r="AN154" s="46"/>
+      <c r="AO154" s="46"/>
+      <c r="AP154" s="46"/>
+      <c r="AQ154" s="46"/>
+      <c r="AR154" s="46"/>
+      <c r="AS154" s="46"/>
+      <c r="AT154" s="46"/>
+      <c r="AU154" s="46"/>
+      <c r="AV154" s="46"/>
+      <c r="AW154" s="46"/>
+      <c r="AX154" s="46"/>
+      <c r="AY154" s="46"/>
+      <c r="AZ154" s="46"/>
+      <c r="BA154" s="46"/>
+      <c r="BB154" s="46"/>
+      <c r="BC154" s="46"/>
+      <c r="BD154" s="46"/>
+      <c r="BE154" s="46"/>
+      <c r="BF154" s="46"/>
+      <c r="BG154" s="46"/>
+      <c r="BH154" s="46"/>
+      <c r="BI154" s="46"/>
+      <c r="BJ154" s="46"/>
+      <c r="BK154" s="46"/>
+      <c r="BL154" s="46"/>
+      <c r="BM154" s="46"/>
+      <c r="BN154" s="46"/>
+      <c r="BO154" s="46"/>
+    </row>
+    <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="23"/>
+      <c r="B155" s="65"/>
+      <c r="D155" s="70"/>
+      <c r="E155" s="66"/>
+      <c r="F155" s="42"/>
+      <c r="G155" s="43"/>
+      <c r="H155" s="25"/>
+      <c r="I155" s="26"/>
+      <c r="J155" s="27"/>
+      <c r="K155" s="40"/>
+      <c r="L155" s="46"/>
+      <c r="M155" s="46"/>
+      <c r="N155" s="46"/>
+      <c r="O155" s="46"/>
+      <c r="P155" s="46"/>
+      <c r="Q155" s="46"/>
+      <c r="R155" s="46"/>
+      <c r="S155" s="46"/>
+      <c r="T155" s="46"/>
+      <c r="U155" s="46"/>
+      <c r="V155" s="46"/>
+      <c r="W155" s="46"/>
+      <c r="X155" s="46"/>
+      <c r="Y155" s="46"/>
+      <c r="Z155" s="46"/>
+      <c r="AA155" s="46"/>
+      <c r="AB155" s="46"/>
+      <c r="AC155" s="46"/>
+      <c r="AD155" s="46"/>
+      <c r="AE155" s="46"/>
+      <c r="AF155" s="46"/>
+      <c r="AG155" s="46"/>
+      <c r="AH155" s="46"/>
+      <c r="AI155" s="46"/>
+      <c r="AJ155" s="46"/>
+      <c r="AK155" s="46"/>
+      <c r="AL155" s="46"/>
+      <c r="AM155" s="46"/>
+      <c r="AN155" s="46"/>
+      <c r="AO155" s="46"/>
+      <c r="AP155" s="46"/>
+      <c r="AQ155" s="46"/>
+      <c r="AR155" s="46"/>
+      <c r="AS155" s="46"/>
+      <c r="AT155" s="46"/>
+      <c r="AU155" s="46"/>
+      <c r="AV155" s="46"/>
+      <c r="AW155" s="46"/>
+      <c r="AX155" s="46"/>
+      <c r="AY155" s="46"/>
+      <c r="AZ155" s="46"/>
+      <c r="BA155" s="46"/>
+      <c r="BB155" s="46"/>
+      <c r="BC155" s="46"/>
+      <c r="BD155" s="46"/>
+      <c r="BE155" s="46"/>
+      <c r="BF155" s="46"/>
+      <c r="BG155" s="46"/>
+      <c r="BH155" s="46"/>
+      <c r="BI155" s="46"/>
+      <c r="BJ155" s="46"/>
+      <c r="BK155" s="46"/>
+      <c r="BL155" s="46"/>
+      <c r="BM155" s="46"/>
+      <c r="BN155" s="46"/>
+      <c r="BO155" s="46"/>
+    </row>
+    <row r="156" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="23"/>
+      <c r="B156" s="65"/>
+      <c r="D156" s="70"/>
+      <c r="E156" s="66"/>
+      <c r="F156" s="42"/>
+      <c r="G156" s="43"/>
+      <c r="H156" s="25"/>
+      <c r="I156" s="26"/>
+      <c r="J156" s="27"/>
+      <c r="K156" s="40"/>
+      <c r="L156" s="46"/>
+      <c r="M156" s="46"/>
+      <c r="N156" s="46"/>
+      <c r="O156" s="46"/>
+      <c r="P156" s="46"/>
+      <c r="Q156" s="46"/>
+      <c r="R156" s="46"/>
+      <c r="S156" s="46"/>
+      <c r="T156" s="46"/>
+      <c r="U156" s="46"/>
+      <c r="V156" s="46"/>
+      <c r="W156" s="46"/>
+      <c r="X156" s="46"/>
+      <c r="Y156" s="46"/>
+      <c r="Z156" s="46"/>
+      <c r="AA156" s="46"/>
+      <c r="AB156" s="46"/>
+      <c r="AC156" s="46"/>
+      <c r="AD156" s="46"/>
+      <c r="AE156" s="46"/>
+      <c r="AF156" s="46"/>
+      <c r="AG156" s="46"/>
+      <c r="AH156" s="46"/>
+      <c r="AI156" s="46"/>
+      <c r="AJ156" s="46"/>
+      <c r="AK156" s="46"/>
+      <c r="AL156" s="46"/>
+      <c r="AM156" s="46"/>
+      <c r="AN156" s="46"/>
+      <c r="AO156" s="46"/>
+      <c r="AP156" s="46"/>
+      <c r="AQ156" s="46"/>
+      <c r="AR156" s="46"/>
+      <c r="AS156" s="46"/>
+      <c r="AT156" s="46"/>
+      <c r="AU156" s="46"/>
+      <c r="AV156" s="46"/>
+      <c r="AW156" s="46"/>
+      <c r="AX156" s="46"/>
+      <c r="AY156" s="46"/>
+      <c r="AZ156" s="46"/>
+      <c r="BA156" s="46"/>
+      <c r="BB156" s="46"/>
+      <c r="BC156" s="46"/>
+      <c r="BD156" s="46"/>
+      <c r="BE156" s="46"/>
+      <c r="BF156" s="46"/>
+      <c r="BG156" s="46"/>
+      <c r="BH156" s="46"/>
+      <c r="BI156" s="46"/>
+      <c r="BJ156" s="46"/>
+      <c r="BK156" s="46"/>
+      <c r="BL156" s="46"/>
+      <c r="BM156" s="46"/>
+      <c r="BN156" s="46"/>
+      <c r="BO156" s="46"/>
+    </row>
+    <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="23"/>
+      <c r="B157" s="65"/>
+      <c r="D157" s="70"/>
+      <c r="E157" s="66"/>
+      <c r="F157" s="42"/>
+      <c r="G157" s="43"/>
+      <c r="H157" s="25"/>
+      <c r="I157" s="26"/>
+      <c r="J157" s="27"/>
+      <c r="K157" s="40"/>
+      <c r="L157" s="46"/>
+      <c r="M157" s="46"/>
+      <c r="N157" s="46"/>
+      <c r="O157" s="46"/>
+      <c r="P157" s="46"/>
+      <c r="Q157" s="46"/>
+      <c r="R157" s="46"/>
+      <c r="S157" s="46"/>
+      <c r="T157" s="46"/>
+      <c r="U157" s="46"/>
+      <c r="V157" s="46"/>
+      <c r="W157" s="46"/>
+      <c r="X157" s="46"/>
+      <c r="Y157" s="46"/>
+      <c r="Z157" s="46"/>
+      <c r="AA157" s="46"/>
+      <c r="AB157" s="46"/>
+      <c r="AC157" s="46"/>
+      <c r="AD157" s="46"/>
+      <c r="AE157" s="46"/>
+      <c r="AF157" s="46"/>
+      <c r="AG157" s="46"/>
+      <c r="AH157" s="46"/>
+      <c r="AI157" s="46"/>
+      <c r="AJ157" s="46"/>
+      <c r="AK157" s="46"/>
+      <c r="AL157" s="46"/>
+      <c r="AM157" s="46"/>
+      <c r="AN157" s="46"/>
+      <c r="AO157" s="46"/>
+      <c r="AP157" s="46"/>
+      <c r="AQ157" s="46"/>
+      <c r="AR157" s="46"/>
+      <c r="AS157" s="46"/>
+      <c r="AT157" s="46"/>
+      <c r="AU157" s="46"/>
+      <c r="AV157" s="46"/>
+      <c r="AW157" s="46"/>
+      <c r="AX157" s="46"/>
+      <c r="AY157" s="46"/>
+      <c r="AZ157" s="46"/>
+      <c r="BA157" s="46"/>
+      <c r="BB157" s="46"/>
+      <c r="BC157" s="46"/>
+      <c r="BD157" s="46"/>
+      <c r="BE157" s="46"/>
+      <c r="BF157" s="46"/>
+      <c r="BG157" s="46"/>
+      <c r="BH157" s="46"/>
+      <c r="BI157" s="46"/>
+      <c r="BJ157" s="46"/>
+      <c r="BK157" s="46"/>
+      <c r="BL157" s="46"/>
+      <c r="BM157" s="46"/>
+      <c r="BN157" s="46"/>
+      <c r="BO157" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -15408,9 +15846,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I112:I115 I98:I103 I109:I110 I105:I107">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I118:I121 I98:I103 I115:I116 I105:I113">
     <cfRule type="dataBar" priority="225">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15429,7 +15876,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 L116:BO118 M119:BN124 BO122:BO124 L125:BO127 M128:BN133 BO131:BO133 L134:BO136 M137:BN142 BO140:BO142 L143:BO145 M146:BN151 BO149:BO151 BO114:BO115 M112:BN115 L111:BO111 M109:BN110 M105:BN107 L108:BO108">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 L122:BO124 M125:BN130 BO128:BO130 L131:BO133 M134:BN139 BO137:BO139 L140:BO142 M143:BN148 BO146:BO148 L149:BO151 M152:BN157 BO155:BO157 BO120:BO121 M118:BN121 L117:BO117 M115:BN116 M105:BN113 L114:BO114">
     <cfRule type="expression" dxfId="122" priority="271">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -15437,7 +15884,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L112:BO115 L98:BO103 L109:BO110 L105:BO107">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L118:BO121 L98:BO103 L115:BO116 L105:BO113">
     <cfRule type="expression" dxfId="120" priority="231">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -15447,7 +15894,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E152:E1048576 E95:E96 E112:E115 E98:E103 E109:E110 E105:E107">
+  <conditionalFormatting sqref="E1:E73 E158:E1048576 E95:E96 E118:E121 E98:E103 E115:E116 E105:E113">
     <cfRule type="cellIs" dxfId="118" priority="212" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15541,7 +15988,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I116:I124">
+  <conditionalFormatting sqref="I122:I130">
     <cfRule type="dataBar" priority="116">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15555,12 +16002,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L116:BO124">
+  <conditionalFormatting sqref="L122:BO130">
     <cfRule type="expression" dxfId="96" priority="115">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E116:E124">
+  <conditionalFormatting sqref="E122:E130">
     <cfRule type="cellIs" dxfId="95" priority="108" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15583,7 +16030,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L119:BO124 L112:BO115 L98:BO103 L109:BO110 L105:BO107">
+  <conditionalFormatting sqref="L125:BO130 L118:BO121 L98:BO103 L115:BO116 L105:BO113">
     <cfRule type="expression" dxfId="88" priority="119">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15591,7 +16038,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I125:I133">
+  <conditionalFormatting sqref="I131:I139">
     <cfRule type="dataBar" priority="103">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15605,12 +16052,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO133">
+  <conditionalFormatting sqref="L131:BO139">
     <cfRule type="expression" dxfId="86" priority="102">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E125:E133">
+  <conditionalFormatting sqref="E131:E139">
     <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15633,7 +16080,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L128:BO133">
+  <conditionalFormatting sqref="L134:BO139">
     <cfRule type="expression" dxfId="78" priority="106">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15641,7 +16088,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I134:I142">
+  <conditionalFormatting sqref="I140:I148">
     <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15655,12 +16102,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L134:BO142">
+  <conditionalFormatting sqref="L140:BO148">
     <cfRule type="expression" dxfId="76" priority="89">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E134:E142">
+  <conditionalFormatting sqref="E140:E148">
     <cfRule type="cellIs" dxfId="75" priority="82" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15683,7 +16130,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L137:BO142">
+  <conditionalFormatting sqref="L143:BO148">
     <cfRule type="expression" dxfId="68" priority="93">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15691,7 +16138,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I143:I151">
+  <conditionalFormatting sqref="I149:I157">
     <cfRule type="dataBar" priority="77">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15705,12 +16152,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L143:BO151">
+  <conditionalFormatting sqref="L149:BO157">
     <cfRule type="expression" dxfId="66" priority="76">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143:E151">
+  <conditionalFormatting sqref="E149:E157">
     <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15733,7 +16180,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L146:BO151">
+  <conditionalFormatting sqref="L152:BO157">
     <cfRule type="expression" dxfId="58" priority="80">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -15883,7 +16330,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I111">
+  <conditionalFormatting sqref="I117">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15897,12 +16344,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L111:BO111">
+  <conditionalFormatting sqref="L117:BO117">
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E111">
+  <conditionalFormatting sqref="E117">
     <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15925,7 +16372,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I108">
+  <conditionalFormatting sqref="I114">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15939,12 +16386,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L108:BO108">
+  <conditionalFormatting sqref="L114:BO114">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E108">
+  <conditionalFormatting sqref="E114">
     <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16073,7 +16520,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I112:I115 I98:I103 I109:I110 I105:I107</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I118:I121 I98:I103 I115:I116 I105:I113</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -16103,7 +16550,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I116:I124</xm:sqref>
+          <xm:sqref>I122:I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -16118,7 +16565,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I125:I133</xm:sqref>
+          <xm:sqref>I131:I139</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -16133,7 +16580,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I134:I142</xm:sqref>
+          <xm:sqref>I140:I148</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -16148,7 +16595,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I143:I151</xm:sqref>
+          <xm:sqref>I149:I157</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -16208,7 +16655,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I111</xm:sqref>
+          <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
@@ -16223,7 +16670,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I108</xm:sqref>
+          <xm:sqref>I114</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Matched stationary forms for nowcast inputs to previous params tab (v0.15)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94038AE5-9F26-428F-9D64-318989FC8F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1C3FCE-E772-4F58-86BF-24ED78E2E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="141">
   <si>
     <t>WBS</t>
   </si>
@@ -848,6 +848,9 @@
   </si>
   <si>
     <t>Add Scenario Calculations</t>
+  </si>
+  <si>
+    <t>Update Docs</t>
   </si>
 </sst>
 </file>
@@ -1776,13 +1779,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1792,10 +1788,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1804,6 +1796,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3293,7 +3296,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
+      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3323,27 +3326,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3388,12 +3391,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3403,183 +3406,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -12607,7 +12610,9 @@
     </row>
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="23"/>
-      <c r="B112" s="65"/>
+      <c r="B112" s="65" t="s">
+        <v>140</v>
+      </c>
       <c r="D112" s="70"/>
       <c r="E112" s="66" t="s">
         <v>67</v>
@@ -15836,6 +15841,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -15846,15 +15860,6 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I118:I121 I98:I103 I115:I116 I105:I113">

</xml_diff>

<commit_message>
Reworked model flow (v0.15)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1C3FCE-E772-4F58-86BF-24ED78E2E3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E88B4F-EAEB-4078-B516-1C425DF4B90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="142">
   <si>
     <t>WBS</t>
   </si>
@@ -851,6 +851,9 @@
   </si>
   <si>
     <t>Update Docs</t>
+  </si>
+  <si>
+    <t>Update Model Flow</t>
   </si>
 </sst>
 </file>
@@ -1779,6 +1782,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1788,6 +1798,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1796,17 +1810,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3292,11 +3295,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO157"/>
+  <dimension ref="A1:BO158"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E110" sqref="E110"/>
+      <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V117" sqref="V117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3326,27 +3329,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3391,12 +3394,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3406,183 +3409,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8740,7 +8743,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A122" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A123" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -12247,22 +12250,27 @@
       <c r="BO106" s="46"/>
     </row>
     <row r="107" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="23"/>
+      <c r="A107" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.3</v>
+      </c>
       <c r="B107" s="65" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="D107" s="70"/>
       <c r="E107" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F107" s="71">
-        <v>44382</v>
-      </c>
-      <c r="G107" s="72">
-        <v>44385</v>
+      <c r="F107" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G107" s="43">
+        <v>44383</v>
       </c>
       <c r="H107" s="73"/>
-      <c r="I107" s="74"/>
+      <c r="I107" s="26">
+        <v>1</v>
+      </c>
       <c r="J107" s="75"/>
       <c r="K107" s="76"/>
       <c r="L107" s="46"/>
@@ -12323,18 +12331,27 @@
       <c r="BO107" s="46"/>
     </row>
     <row r="108" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="23"/>
+      <c r="A108" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.4</v>
+      </c>
       <c r="B108" s="65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D108" s="70"/>
       <c r="E108" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F108" s="71"/>
-      <c r="G108" s="72"/>
+      <c r="F108" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G108" s="43">
+        <v>44385</v>
+      </c>
       <c r="H108" s="73"/>
-      <c r="I108" s="74"/>
+      <c r="I108" s="26">
+        <v>1</v>
+      </c>
       <c r="J108" s="75"/>
       <c r="K108" s="76"/>
       <c r="L108" s="46"/>
@@ -12395,18 +12412,23 @@
       <c r="BO108" s="46"/>
     </row>
     <row r="109" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="23"/>
+      <c r="A109" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.5</v>
+      </c>
       <c r="B109" s="65" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D109" s="70"/>
       <c r="E109" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F109" s="71"/>
-      <c r="G109" s="72"/>
+      <c r="F109" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G109" s="43"/>
       <c r="H109" s="73"/>
-      <c r="I109" s="74"/>
+      <c r="I109" s="26"/>
       <c r="J109" s="75"/>
       <c r="K109" s="76"/>
       <c r="L109" s="46"/>
@@ -12467,16 +12489,23 @@
       <c r="BO109" s="46"/>
     </row>
     <row r="110" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="23"/>
+      <c r="A110" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.6</v>
+      </c>
       <c r="B110" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D110" s="70"/>
-      <c r="E110" s="66"/>
-      <c r="F110" s="71"/>
-      <c r="G110" s="72"/>
+      <c r="E110" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F110" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G110" s="43"/>
       <c r="H110" s="73"/>
-      <c r="I110" s="74"/>
+      <c r="I110" s="26"/>
       <c r="J110" s="75"/>
       <c r="K110" s="76"/>
       <c r="L110" s="46"/>
@@ -12537,18 +12566,23 @@
       <c r="BO110" s="46"/>
     </row>
     <row r="111" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="23"/>
+      <c r="A111" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.7</v>
+      </c>
       <c r="B111" s="65" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D111" s="70"/>
       <c r="E111" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F111" s="71"/>
-      <c r="G111" s="72"/>
+        <v>67</v>
+      </c>
+      <c r="F111" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G111" s="43"/>
       <c r="H111" s="73"/>
-      <c r="I111" s="74"/>
+      <c r="I111" s="26"/>
       <c r="J111" s="75"/>
       <c r="K111" s="76"/>
       <c r="L111" s="46"/>
@@ -12609,18 +12643,23 @@
       <c r="BO111" s="46"/>
     </row>
     <row r="112" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="23"/>
+      <c r="A112" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.8</v>
+      </c>
       <c r="B112" s="65" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D112" s="70"/>
       <c r="E112" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F112" s="71"/>
-      <c r="G112" s="72"/>
+        <v>70</v>
+      </c>
+      <c r="F112" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G112" s="43"/>
       <c r="H112" s="73"/>
-      <c r="I112" s="74"/>
+      <c r="I112" s="26"/>
       <c r="J112" s="75"/>
       <c r="K112" s="76"/>
       <c r="L112" s="46"/>
@@ -12683,25 +12722,21 @@
     <row r="113" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.1</v>
+        <v>10.9</v>
       </c>
       <c r="B113" s="65" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="D113" s="70"/>
       <c r="E113" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F113" s="71">
-        <v>44379</v>
-      </c>
-      <c r="G113" s="72">
-        <v>44382</v>
-      </c>
+      <c r="F113" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G113" s="43"/>
       <c r="H113" s="73"/>
-      <c r="I113" s="74">
-        <v>0</v>
-      </c>
+      <c r="I113" s="26"/>
       <c r="J113" s="75"/>
       <c r="K113" s="76"/>
       <c r="L113" s="46"/>
@@ -12761,180 +12796,180 @@
       <c r="BN113" s="46"/>
       <c r="BO113" s="46"/>
     </row>
-    <row r="114" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="16" t="str">
+    <row r="114" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.10</v>
+      </c>
+      <c r="B114" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D114" s="70"/>
+      <c r="E114" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F114" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G114" s="43"/>
+      <c r="H114" s="73"/>
+      <c r="I114" s="26"/>
+      <c r="J114" s="75"/>
+      <c r="K114" s="76"/>
+      <c r="L114" s="46"/>
+      <c r="M114" s="46"/>
+      <c r="N114" s="46"/>
+      <c r="O114" s="46"/>
+      <c r="P114" s="46"/>
+      <c r="Q114" s="46"/>
+      <c r="R114" s="46"/>
+      <c r="S114" s="46"/>
+      <c r="T114" s="46"/>
+      <c r="U114" s="46"/>
+      <c r="V114" s="46"/>
+      <c r="W114" s="46"/>
+      <c r="X114" s="46"/>
+      <c r="Y114" s="46"/>
+      <c r="Z114" s="46"/>
+      <c r="AA114" s="46"/>
+      <c r="AB114" s="46"/>
+      <c r="AC114" s="46"/>
+      <c r="AD114" s="46"/>
+      <c r="AE114" s="46"/>
+      <c r="AF114" s="46"/>
+      <c r="AG114" s="46"/>
+      <c r="AH114" s="46"/>
+      <c r="AI114" s="46"/>
+      <c r="AJ114" s="46"/>
+      <c r="AK114" s="46"/>
+      <c r="AL114" s="46"/>
+      <c r="AM114" s="46"/>
+      <c r="AN114" s="46"/>
+      <c r="AO114" s="46"/>
+      <c r="AP114" s="46"/>
+      <c r="AQ114" s="46"/>
+      <c r="AR114" s="46"/>
+      <c r="AS114" s="46"/>
+      <c r="AT114" s="46"/>
+      <c r="AU114" s="46"/>
+      <c r="AV114" s="46"/>
+      <c r="AW114" s="46"/>
+      <c r="AX114" s="46"/>
+      <c r="AY114" s="46"/>
+      <c r="AZ114" s="46"/>
+      <c r="BA114" s="46"/>
+      <c r="BB114" s="46"/>
+      <c r="BC114" s="46"/>
+      <c r="BD114" s="46"/>
+      <c r="BE114" s="46"/>
+      <c r="BF114" s="46"/>
+      <c r="BG114" s="46"/>
+      <c r="BH114" s="46"/>
+      <c r="BI114" s="46"/>
+      <c r="BJ114" s="46"/>
+      <c r="BK114" s="46"/>
+      <c r="BL114" s="46"/>
+      <c r="BM114" s="46"/>
+      <c r="BN114" s="46"/>
+      <c r="BO114" s="46"/>
+    </row>
+    <row r="115" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B114" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B115" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D114" s="19"/>
-      <c r="E114" s="19"/>
-      <c r="F114" s="44"/>
-      <c r="G114" s="44" t="str">
-        <f t="shared" ref="G114" si="20">IF(ISBLANK(F114)," - ",IF(H114=0,F114,F114+H114-1))</f>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="44"/>
+      <c r="G115" s="44" t="str">
+        <f t="shared" ref="G115" si="20">IF(ISBLANK(F115)," - ",IF(H115=0,F115,F115+H115-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H114" s="20"/>
-      <c r="I114" s="21"/>
-      <c r="J114" s="22" t="str">
-        <f t="shared" ref="J114" si="21">IF(OR(G114=0,F114=0)," - ",NETWORKDAYS(F114,G114))</f>
+      <c r="H115" s="20"/>
+      <c r="I115" s="21"/>
+      <c r="J115" s="22" t="str">
+        <f t="shared" ref="J115" si="21">IF(OR(G115=0,F115=0)," - ",NETWORKDAYS(F115,G115))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K114" s="41"/>
-      <c r="L114" s="48"/>
-      <c r="M114" s="48"/>
-      <c r="N114" s="48"/>
-      <c r="O114" s="48"/>
-      <c r="P114" s="48"/>
-      <c r="Q114" s="48"/>
-      <c r="R114" s="48"/>
-      <c r="S114" s="48"/>
-      <c r="T114" s="48"/>
-      <c r="U114" s="48"/>
-      <c r="V114" s="48"/>
-      <c r="W114" s="48"/>
-      <c r="X114" s="48"/>
-      <c r="Y114" s="48"/>
-      <c r="Z114" s="48"/>
-      <c r="AA114" s="48"/>
-      <c r="AB114" s="48"/>
-      <c r="AC114" s="48"/>
-      <c r="AD114" s="48"/>
-      <c r="AE114" s="48"/>
-      <c r="AF114" s="48"/>
-      <c r="AG114" s="48"/>
-      <c r="AH114" s="48"/>
-      <c r="AI114" s="48"/>
-      <c r="AJ114" s="48"/>
-      <c r="AK114" s="48"/>
-      <c r="AL114" s="48"/>
-      <c r="AM114" s="48"/>
-      <c r="AN114" s="48"/>
-      <c r="AO114" s="48"/>
-      <c r="AP114" s="48"/>
-      <c r="AQ114" s="48"/>
-      <c r="AR114" s="48"/>
-      <c r="AS114" s="48"/>
-      <c r="AT114" s="48"/>
-      <c r="AU114" s="48"/>
-      <c r="AV114" s="48"/>
-      <c r="AW114" s="48"/>
-      <c r="AX114" s="48"/>
-      <c r="AY114" s="48"/>
-      <c r="AZ114" s="48"/>
-      <c r="BA114" s="48"/>
-      <c r="BB114" s="48"/>
-      <c r="BC114" s="48"/>
-      <c r="BD114" s="48"/>
-      <c r="BE114" s="48"/>
-      <c r="BF114" s="48"/>
-      <c r="BG114" s="48"/>
-      <c r="BH114" s="48"/>
-      <c r="BI114" s="48"/>
-      <c r="BJ114" s="48"/>
-      <c r="BK114" s="48"/>
-      <c r="BL114" s="48"/>
-      <c r="BM114" s="48"/>
-      <c r="BN114" s="48"/>
-      <c r="BO114" s="48"/>
-    </row>
-    <row r="115" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>1.1</v>
-      </c>
-      <c r="B115" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="D115" s="70"/>
-      <c r="E115" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F115" s="71">
-        <v>44379</v>
-      </c>
-      <c r="G115" s="72"/>
-      <c r="H115" s="73"/>
-      <c r="I115" s="74"/>
-      <c r="J115" s="75"/>
-      <c r="K115" s="76"/>
-      <c r="L115" s="46"/>
-      <c r="M115" s="46"/>
-      <c r="N115" s="46"/>
-      <c r="O115" s="46"/>
-      <c r="P115" s="46"/>
-      <c r="Q115" s="46"/>
-      <c r="R115" s="46"/>
-      <c r="S115" s="46"/>
-      <c r="T115" s="46"/>
-      <c r="U115" s="46"/>
-      <c r="V115" s="46"/>
-      <c r="W115" s="46"/>
-      <c r="X115" s="46"/>
-      <c r="Y115" s="46"/>
-      <c r="Z115" s="46"/>
-      <c r="AA115" s="46"/>
-      <c r="AB115" s="46"/>
-      <c r="AC115" s="46"/>
-      <c r="AD115" s="46"/>
-      <c r="AE115" s="46"/>
-      <c r="AF115" s="46"/>
-      <c r="AG115" s="46"/>
-      <c r="AH115" s="46"/>
-      <c r="AI115" s="46"/>
-      <c r="AJ115" s="46"/>
-      <c r="AK115" s="46"/>
-      <c r="AL115" s="46"/>
-      <c r="AM115" s="46"/>
-      <c r="AN115" s="46"/>
-      <c r="AO115" s="46"/>
-      <c r="AP115" s="46"/>
-      <c r="AQ115" s="46"/>
-      <c r="AR115" s="46"/>
-      <c r="AS115" s="46"/>
-      <c r="AT115" s="46"/>
-      <c r="AU115" s="46"/>
-      <c r="AV115" s="46"/>
-      <c r="AW115" s="46"/>
-      <c r="AX115" s="46"/>
-      <c r="AY115" s="46"/>
-      <c r="AZ115" s="46"/>
-      <c r="BA115" s="46"/>
-      <c r="BB115" s="46"/>
-      <c r="BC115" s="46"/>
-      <c r="BD115" s="46"/>
-      <c r="BE115" s="46"/>
-      <c r="BF115" s="46"/>
-      <c r="BG115" s="46"/>
-      <c r="BH115" s="46"/>
-      <c r="BI115" s="46"/>
-      <c r="BJ115" s="46"/>
-      <c r="BK115" s="46"/>
-      <c r="BL115" s="46"/>
-      <c r="BM115" s="46"/>
-      <c r="BN115" s="46"/>
-      <c r="BO115" s="46"/>
+      <c r="K115" s="41"/>
+      <c r="L115" s="48"/>
+      <c r="M115" s="48"/>
+      <c r="N115" s="48"/>
+      <c r="O115" s="48"/>
+      <c r="P115" s="48"/>
+      <c r="Q115" s="48"/>
+      <c r="R115" s="48"/>
+      <c r="S115" s="48"/>
+      <c r="T115" s="48"/>
+      <c r="U115" s="48"/>
+      <c r="V115" s="48"/>
+      <c r="W115" s="48"/>
+      <c r="X115" s="48"/>
+      <c r="Y115" s="48"/>
+      <c r="Z115" s="48"/>
+      <c r="AA115" s="48"/>
+      <c r="AB115" s="48"/>
+      <c r="AC115" s="48"/>
+      <c r="AD115" s="48"/>
+      <c r="AE115" s="48"/>
+      <c r="AF115" s="48"/>
+      <c r="AG115" s="48"/>
+      <c r="AH115" s="48"/>
+      <c r="AI115" s="48"/>
+      <c r="AJ115" s="48"/>
+      <c r="AK115" s="48"/>
+      <c r="AL115" s="48"/>
+      <c r="AM115" s="48"/>
+      <c r="AN115" s="48"/>
+      <c r="AO115" s="48"/>
+      <c r="AP115" s="48"/>
+      <c r="AQ115" s="48"/>
+      <c r="AR115" s="48"/>
+      <c r="AS115" s="48"/>
+      <c r="AT115" s="48"/>
+      <c r="AU115" s="48"/>
+      <c r="AV115" s="48"/>
+      <c r="AW115" s="48"/>
+      <c r="AX115" s="48"/>
+      <c r="AY115" s="48"/>
+      <c r="AZ115" s="48"/>
+      <c r="BA115" s="48"/>
+      <c r="BB115" s="48"/>
+      <c r="BC115" s="48"/>
+      <c r="BD115" s="48"/>
+      <c r="BE115" s="48"/>
+      <c r="BF115" s="48"/>
+      <c r="BG115" s="48"/>
+      <c r="BH115" s="48"/>
+      <c r="BI115" s="48"/>
+      <c r="BJ115" s="48"/>
+      <c r="BK115" s="48"/>
+      <c r="BL115" s="48"/>
+      <c r="BM115" s="48"/>
+      <c r="BN115" s="48"/>
+      <c r="BO115" s="48"/>
     </row>
     <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>1.2</v>
+        <v>11.1</v>
       </c>
       <c r="B116" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D116" s="70"/>
-      <c r="E116" s="70" t="s">
+      <c r="E116" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F116" s="71">
-        <v>44379</v>
-      </c>
-      <c r="G116" s="72"/>
+      <c r="F116" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G116" s="43"/>
       <c r="H116" s="73"/>
-      <c r="I116" s="74"/>
+      <c r="I116" s="26"/>
       <c r="J116" s="75"/>
       <c r="K116" s="76"/>
       <c r="L116" s="46"/>
@@ -12994,173 +13029,173 @@
       <c r="BN116" s="46"/>
       <c r="BO116" s="46"/>
     </row>
-    <row r="117" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="16" t="str">
+    <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.2</v>
+      </c>
+      <c r="B117" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="D117" s="70"/>
+      <c r="E117" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F117" s="42">
+        <v>44383</v>
+      </c>
+      <c r="G117" s="43"/>
+      <c r="H117" s="73"/>
+      <c r="I117" s="74"/>
+      <c r="J117" s="75"/>
+      <c r="K117" s="76"/>
+      <c r="L117" s="46"/>
+      <c r="M117" s="46"/>
+      <c r="N117" s="46"/>
+      <c r="O117" s="46"/>
+      <c r="P117" s="46"/>
+      <c r="Q117" s="46"/>
+      <c r="R117" s="46"/>
+      <c r="S117" s="46"/>
+      <c r="T117" s="46"/>
+      <c r="U117" s="46"/>
+      <c r="V117" s="46"/>
+      <c r="W117" s="46"/>
+      <c r="X117" s="46"/>
+      <c r="Y117" s="46"/>
+      <c r="Z117" s="46"/>
+      <c r="AA117" s="46"/>
+      <c r="AB117" s="46"/>
+      <c r="AC117" s="46"/>
+      <c r="AD117" s="46"/>
+      <c r="AE117" s="46"/>
+      <c r="AF117" s="46"/>
+      <c r="AG117" s="46"/>
+      <c r="AH117" s="46"/>
+      <c r="AI117" s="46"/>
+      <c r="AJ117" s="46"/>
+      <c r="AK117" s="46"/>
+      <c r="AL117" s="46"/>
+      <c r="AM117" s="46"/>
+      <c r="AN117" s="46"/>
+      <c r="AO117" s="46"/>
+      <c r="AP117" s="46"/>
+      <c r="AQ117" s="46"/>
+      <c r="AR117" s="46"/>
+      <c r="AS117" s="46"/>
+      <c r="AT117" s="46"/>
+      <c r="AU117" s="46"/>
+      <c r="AV117" s="46"/>
+      <c r="AW117" s="46"/>
+      <c r="AX117" s="46"/>
+      <c r="AY117" s="46"/>
+      <c r="AZ117" s="46"/>
+      <c r="BA117" s="46"/>
+      <c r="BB117" s="46"/>
+      <c r="BC117" s="46"/>
+      <c r="BD117" s="46"/>
+      <c r="BE117" s="46"/>
+      <c r="BF117" s="46"/>
+      <c r="BG117" s="46"/>
+      <c r="BH117" s="46"/>
+      <c r="BI117" s="46"/>
+      <c r="BJ117" s="46"/>
+      <c r="BK117" s="46"/>
+      <c r="BL117" s="46"/>
+      <c r="BM117" s="46"/>
+      <c r="BN117" s="46"/>
+      <c r="BO117" s="46"/>
+    </row>
+    <row r="118" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>2</v>
-      </c>
-      <c r="B117" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B118" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D117" s="19"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="44"/>
-      <c r="G117" s="44" t="str">
-        <f t="shared" ref="G117" si="22">IF(ISBLANK(F117)," - ",IF(H117=0,F117,F117+H117-1))</f>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="44"/>
+      <c r="G118" s="44" t="str">
+        <f t="shared" ref="G118" si="22">IF(ISBLANK(F118)," - ",IF(H118=0,F118,F118+H118-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H117" s="20"/>
-      <c r="I117" s="21"/>
-      <c r="J117" s="22" t="str">
-        <f t="shared" ref="J117" si="23">IF(OR(G117=0,F117=0)," - ",NETWORKDAYS(F117,G117))</f>
+      <c r="H118" s="20"/>
+      <c r="I118" s="21"/>
+      <c r="J118" s="22" t="str">
+        <f t="shared" ref="J118" si="23">IF(OR(G118=0,F118=0)," - ",NETWORKDAYS(F118,G118))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K117" s="41"/>
-      <c r="L117" s="48"/>
-      <c r="M117" s="48"/>
-      <c r="N117" s="48"/>
-      <c r="O117" s="48"/>
-      <c r="P117" s="48"/>
-      <c r="Q117" s="48"/>
-      <c r="R117" s="48"/>
-      <c r="S117" s="48"/>
-      <c r="T117" s="48"/>
-      <c r="U117" s="48"/>
-      <c r="V117" s="48"/>
-      <c r="W117" s="48"/>
-      <c r="X117" s="48"/>
-      <c r="Y117" s="48"/>
-      <c r="Z117" s="48"/>
-      <c r="AA117" s="48"/>
-      <c r="AB117" s="48"/>
-      <c r="AC117" s="48"/>
-      <c r="AD117" s="48"/>
-      <c r="AE117" s="48"/>
-      <c r="AF117" s="48"/>
-      <c r="AG117" s="48"/>
-      <c r="AH117" s="48"/>
-      <c r="AI117" s="48"/>
-      <c r="AJ117" s="48"/>
-      <c r="AK117" s="48"/>
-      <c r="AL117" s="48"/>
-      <c r="AM117" s="48"/>
-      <c r="AN117" s="48"/>
-      <c r="AO117" s="48"/>
-      <c r="AP117" s="48"/>
-      <c r="AQ117" s="48"/>
-      <c r="AR117" s="48"/>
-      <c r="AS117" s="48"/>
-      <c r="AT117" s="48"/>
-      <c r="AU117" s="48"/>
-      <c r="AV117" s="48"/>
-      <c r="AW117" s="48"/>
-      <c r="AX117" s="48"/>
-      <c r="AY117" s="48"/>
-      <c r="AZ117" s="48"/>
-      <c r="BA117" s="48"/>
-      <c r="BB117" s="48"/>
-      <c r="BC117" s="48"/>
-      <c r="BD117" s="48"/>
-      <c r="BE117" s="48"/>
-      <c r="BF117" s="48"/>
-      <c r="BG117" s="48"/>
-      <c r="BH117" s="48"/>
-      <c r="BI117" s="48"/>
-      <c r="BJ117" s="48"/>
-      <c r="BK117" s="48"/>
-      <c r="BL117" s="48"/>
-      <c r="BM117" s="48"/>
-      <c r="BN117" s="48"/>
-      <c r="BO117" s="48"/>
-    </row>
-    <row r="118" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>2.1</v>
-      </c>
-      <c r="B118" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D118" s="70"/>
-      <c r="E118" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F118" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G118" s="43"/>
-      <c r="H118" s="25"/>
-      <c r="I118" s="26"/>
-      <c r="J118" s="27"/>
-      <c r="K118" s="40"/>
-      <c r="L118" s="46"/>
-      <c r="M118" s="46"/>
-      <c r="N118" s="46"/>
-      <c r="O118" s="46"/>
-      <c r="P118" s="46"/>
-      <c r="Q118" s="46"/>
-      <c r="R118" s="46"/>
-      <c r="S118" s="46"/>
-      <c r="T118" s="46"/>
-      <c r="U118" s="46"/>
-      <c r="V118" s="46"/>
-      <c r="W118" s="46"/>
-      <c r="X118" s="46"/>
-      <c r="Y118" s="46"/>
-      <c r="Z118" s="46"/>
-      <c r="AA118" s="46"/>
-      <c r="AB118" s="46"/>
-      <c r="AC118" s="46"/>
-      <c r="AD118" s="46"/>
-      <c r="AE118" s="46"/>
-      <c r="AF118" s="46"/>
-      <c r="AG118" s="46"/>
-      <c r="AH118" s="46"/>
-      <c r="AI118" s="46"/>
-      <c r="AJ118" s="46"/>
-      <c r="AK118" s="46"/>
-      <c r="AL118" s="46"/>
-      <c r="AM118" s="46"/>
-      <c r="AN118" s="46"/>
-      <c r="AO118" s="46"/>
-      <c r="AP118" s="46"/>
-      <c r="AQ118" s="46"/>
-      <c r="AR118" s="46"/>
-      <c r="AS118" s="46"/>
-      <c r="AT118" s="46"/>
-      <c r="AU118" s="46"/>
-      <c r="AV118" s="46"/>
-      <c r="AW118" s="46"/>
-      <c r="AX118" s="46"/>
-      <c r="AY118" s="46"/>
-      <c r="AZ118" s="46"/>
-      <c r="BA118" s="46"/>
-      <c r="BB118" s="46"/>
-      <c r="BC118" s="46"/>
-      <c r="BD118" s="46"/>
-      <c r="BE118" s="46"/>
-      <c r="BF118" s="46"/>
-      <c r="BG118" s="46"/>
-      <c r="BH118" s="46"/>
-      <c r="BI118" s="46"/>
-      <c r="BJ118" s="46"/>
-      <c r="BK118" s="46"/>
-      <c r="BL118" s="46"/>
-      <c r="BM118" s="46"/>
-      <c r="BN118" s="46"/>
-      <c r="BO118" s="46"/>
+      <c r="K118" s="41"/>
+      <c r="L118" s="48"/>
+      <c r="M118" s="48"/>
+      <c r="N118" s="48"/>
+      <c r="O118" s="48"/>
+      <c r="P118" s="48"/>
+      <c r="Q118" s="48"/>
+      <c r="R118" s="48"/>
+      <c r="S118" s="48"/>
+      <c r="T118" s="48"/>
+      <c r="U118" s="48"/>
+      <c r="V118" s="48"/>
+      <c r="W118" s="48"/>
+      <c r="X118" s="48"/>
+      <c r="Y118" s="48"/>
+      <c r="Z118" s="48"/>
+      <c r="AA118" s="48"/>
+      <c r="AB118" s="48"/>
+      <c r="AC118" s="48"/>
+      <c r="AD118" s="48"/>
+      <c r="AE118" s="48"/>
+      <c r="AF118" s="48"/>
+      <c r="AG118" s="48"/>
+      <c r="AH118" s="48"/>
+      <c r="AI118" s="48"/>
+      <c r="AJ118" s="48"/>
+      <c r="AK118" s="48"/>
+      <c r="AL118" s="48"/>
+      <c r="AM118" s="48"/>
+      <c r="AN118" s="48"/>
+      <c r="AO118" s="48"/>
+      <c r="AP118" s="48"/>
+      <c r="AQ118" s="48"/>
+      <c r="AR118" s="48"/>
+      <c r="AS118" s="48"/>
+      <c r="AT118" s="48"/>
+      <c r="AU118" s="48"/>
+      <c r="AV118" s="48"/>
+      <c r="AW118" s="48"/>
+      <c r="AX118" s="48"/>
+      <c r="AY118" s="48"/>
+      <c r="AZ118" s="48"/>
+      <c r="BA118" s="48"/>
+      <c r="BB118" s="48"/>
+      <c r="BC118" s="48"/>
+      <c r="BD118" s="48"/>
+      <c r="BE118" s="48"/>
+      <c r="BF118" s="48"/>
+      <c r="BG118" s="48"/>
+      <c r="BH118" s="48"/>
+      <c r="BI118" s="48"/>
+      <c r="BJ118" s="48"/>
+      <c r="BK118" s="48"/>
+      <c r="BL118" s="48"/>
+      <c r="BM118" s="48"/>
+      <c r="BN118" s="48"/>
+      <c r="BO118" s="48"/>
     </row>
     <row r="119" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>2.2</v>
+        <v>12.1</v>
       </c>
       <c r="B119" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D119" s="70"/>
       <c r="E119" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F119" s="42">
         <v>44379</v>
@@ -13230,14 +13265,14 @@
     <row r="120" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>2.3</v>
+        <v>12.2</v>
       </c>
       <c r="B120" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D120" s="70"/>
       <c r="E120" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F120" s="42">
         <v>44379</v>
@@ -13307,10 +13342,10 @@
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>2.4</v>
+        <v>12.3</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D121" s="70"/>
       <c r="E121" s="66" t="s">
@@ -13384,17 +13419,17 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>2.5</v>
-      </c>
-      <c r="B122" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D122" s="66"/>
+        <v>12.4</v>
+      </c>
+      <c r="B122" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D122" s="70"/>
       <c r="E122" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F122" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G122" s="43"/>
       <c r="H122" s="25"/>
@@ -13459,11 +13494,20 @@
       <c r="BO122" s="46"/>
     </row>
     <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="23"/>
-      <c r="B123" s="65"/>
+      <c r="A123" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.5</v>
+      </c>
+      <c r="B123" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D123" s="66"/>
-      <c r="E123" s="66"/>
-      <c r="F123" s="42"/>
+      <c r="E123" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F123" s="42">
+        <v>44531</v>
+      </c>
       <c r="G123" s="43"/>
       <c r="H123" s="25"/>
       <c r="I123" s="26"/>
@@ -13665,7 +13709,7 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23"/>
       <c r="B126" s="65"/>
-      <c r="D126" s="70"/>
+      <c r="D126" s="66"/>
       <c r="E126" s="66"/>
       <c r="F126" s="42"/>
       <c r="G126" s="43"/>
@@ -14005,7 +14049,7 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23"/>
       <c r="B131" s="65"/>
-      <c r="D131" s="66"/>
+      <c r="D131" s="70"/>
       <c r="E131" s="66"/>
       <c r="F131" s="42"/>
       <c r="G131" s="43"/>
@@ -14277,7 +14321,7 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
       <c r="B135" s="65"/>
-      <c r="D135" s="70"/>
+      <c r="D135" s="66"/>
       <c r="E135" s="66"/>
       <c r="F135" s="42"/>
       <c r="G135" s="43"/>
@@ -14617,7 +14661,7 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23"/>
       <c r="B140" s="65"/>
-      <c r="D140" s="66"/>
+      <c r="D140" s="70"/>
       <c r="E140" s="66"/>
       <c r="F140" s="42"/>
       <c r="G140" s="43"/>
@@ -14889,7 +14933,7 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23"/>
       <c r="B144" s="65"/>
-      <c r="D144" s="70"/>
+      <c r="D144" s="66"/>
       <c r="E144" s="66"/>
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
@@ -15229,7 +15273,7 @@
     <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="23"/>
       <c r="B149" s="65"/>
-      <c r="D149" s="66"/>
+      <c r="D149" s="70"/>
       <c r="E149" s="66"/>
       <c r="F149" s="42"/>
       <c r="G149" s="43"/>
@@ -15501,7 +15545,7 @@
     <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="23"/>
       <c r="B153" s="65"/>
-      <c r="D153" s="70"/>
+      <c r="D153" s="66"/>
       <c r="E153" s="66"/>
       <c r="F153" s="42"/>
       <c r="G153" s="43"/>
@@ -15838,18 +15882,77 @@
       <c r="BN157" s="46"/>
       <c r="BO157" s="46"/>
     </row>
+    <row r="158" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="23"/>
+      <c r="B158" s="65"/>
+      <c r="D158" s="70"/>
+      <c r="E158" s="66"/>
+      <c r="F158" s="42"/>
+      <c r="G158" s="43"/>
+      <c r="H158" s="25"/>
+      <c r="I158" s="26"/>
+      <c r="J158" s="27"/>
+      <c r="K158" s="40"/>
+      <c r="L158" s="46"/>
+      <c r="M158" s="46"/>
+      <c r="N158" s="46"/>
+      <c r="O158" s="46"/>
+      <c r="P158" s="46"/>
+      <c r="Q158" s="46"/>
+      <c r="R158" s="46"/>
+      <c r="S158" s="46"/>
+      <c r="T158" s="46"/>
+      <c r="U158" s="46"/>
+      <c r="V158" s="46"/>
+      <c r="W158" s="46"/>
+      <c r="X158" s="46"/>
+      <c r="Y158" s="46"/>
+      <c r="Z158" s="46"/>
+      <c r="AA158" s="46"/>
+      <c r="AB158" s="46"/>
+      <c r="AC158" s="46"/>
+      <c r="AD158" s="46"/>
+      <c r="AE158" s="46"/>
+      <c r="AF158" s="46"/>
+      <c r="AG158" s="46"/>
+      <c r="AH158" s="46"/>
+      <c r="AI158" s="46"/>
+      <c r="AJ158" s="46"/>
+      <c r="AK158" s="46"/>
+      <c r="AL158" s="46"/>
+      <c r="AM158" s="46"/>
+      <c r="AN158" s="46"/>
+      <c r="AO158" s="46"/>
+      <c r="AP158" s="46"/>
+      <c r="AQ158" s="46"/>
+      <c r="AR158" s="46"/>
+      <c r="AS158" s="46"/>
+      <c r="AT158" s="46"/>
+      <c r="AU158" s="46"/>
+      <c r="AV158" s="46"/>
+      <c r="AW158" s="46"/>
+      <c r="AX158" s="46"/>
+      <c r="AY158" s="46"/>
+      <c r="AZ158" s="46"/>
+      <c r="BA158" s="46"/>
+      <c r="BB158" s="46"/>
+      <c r="BC158" s="46"/>
+      <c r="BD158" s="46"/>
+      <c r="BE158" s="46"/>
+      <c r="BF158" s="46"/>
+      <c r="BG158" s="46"/>
+      <c r="BH158" s="46"/>
+      <c r="BI158" s="46"/>
+      <c r="BJ158" s="46"/>
+      <c r="BK158" s="46"/>
+      <c r="BL158" s="46"/>
+      <c r="BM158" s="46"/>
+      <c r="BN158" s="46"/>
+      <c r="BO158" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -15860,9 +15963,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I118:I121 I98:I103 I115:I116 I105:I113">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I119:I122 I98:I103 I105:I114 I116:I117">
     <cfRule type="dataBar" priority="225">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -15881,7 +15993,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 L122:BO124 M125:BN130 BO128:BO130 L131:BO133 M134:BN139 BO137:BO139 L140:BO142 M143:BN148 BO146:BO148 L149:BO151 M152:BN157 BO155:BO157 BO120:BO121 M118:BN121 L117:BO117 M115:BN116 M105:BN113 L114:BO114">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 L123:BO125 M126:BN131 BO129:BO131 L132:BO134 M135:BN140 BO138:BO140 L141:BO143 M144:BN149 BO147:BO149 L150:BO152 M153:BN158 BO156:BO158 BO121:BO122 M119:BN122 L118:BO118 M116:BN117 M105:BN114 L115:BO115">
     <cfRule type="expression" dxfId="122" priority="271">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -15889,7 +16001,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L118:BO121 L98:BO103 L115:BO116 L105:BO113">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L119:BO122 L98:BO103 L116:BO117 L105:BO114">
     <cfRule type="expression" dxfId="120" priority="231">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -15899,7 +16011,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E158:E1048576 E95:E96 E118:E121 E98:E103 E115:E116 E105:E113">
+  <conditionalFormatting sqref="E1:E73 E159:E1048576 E95:E96 E119:E122 E98:E103 E116:E117 E105:E114">
     <cfRule type="cellIs" dxfId="118" priority="212" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -15993,7 +16105,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122:I130">
+  <conditionalFormatting sqref="I123:I131">
     <cfRule type="dataBar" priority="116">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16007,12 +16119,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L122:BO130">
+  <conditionalFormatting sqref="L123:BO131">
     <cfRule type="expression" dxfId="96" priority="115">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122:E130">
+  <conditionalFormatting sqref="E123:E131">
     <cfRule type="cellIs" dxfId="95" priority="108" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16035,7 +16147,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO130 L118:BO121 L98:BO103 L115:BO116 L105:BO113">
+  <conditionalFormatting sqref="L126:BO131 L119:BO122 L98:BO103 L116:BO117 L105:BO114">
     <cfRule type="expression" dxfId="88" priority="119">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16043,7 +16155,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I131:I139">
+  <conditionalFormatting sqref="I132:I140">
     <cfRule type="dataBar" priority="103">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16057,12 +16169,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L131:BO139">
+  <conditionalFormatting sqref="L132:BO140">
     <cfRule type="expression" dxfId="86" priority="102">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131:E139">
+  <conditionalFormatting sqref="E132:E140">
     <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16085,7 +16197,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L134:BO139">
+  <conditionalFormatting sqref="L135:BO140">
     <cfRule type="expression" dxfId="78" priority="106">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16093,7 +16205,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I140:I148">
+  <conditionalFormatting sqref="I141:I149">
     <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16107,12 +16219,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L140:BO148">
+  <conditionalFormatting sqref="L141:BO149">
     <cfRule type="expression" dxfId="76" priority="89">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E140:E148">
+  <conditionalFormatting sqref="E141:E149">
     <cfRule type="cellIs" dxfId="75" priority="82" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16135,7 +16247,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L143:BO148">
+  <conditionalFormatting sqref="L144:BO149">
     <cfRule type="expression" dxfId="68" priority="93">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16143,7 +16255,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I149:I157">
+  <conditionalFormatting sqref="I150:I158">
     <cfRule type="dataBar" priority="77">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16157,12 +16269,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L149:BO157">
+  <conditionalFormatting sqref="L150:BO158">
     <cfRule type="expression" dxfId="66" priority="76">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149:E157">
+  <conditionalFormatting sqref="E150:E158">
     <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16185,7 +16297,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L152:BO157">
+  <conditionalFormatting sqref="L153:BO158">
     <cfRule type="expression" dxfId="58" priority="80">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16335,7 +16447,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I117">
+  <conditionalFormatting sqref="I118">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16349,12 +16461,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L117:BO117">
+  <conditionalFormatting sqref="L118:BO118">
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E117">
+  <conditionalFormatting sqref="E118">
     <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16377,7 +16489,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I114">
+  <conditionalFormatting sqref="I115">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16391,12 +16503,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L114:BO114">
+  <conditionalFormatting sqref="L115:BO115">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E114">
+  <conditionalFormatting sqref="E115">
     <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16525,7 +16637,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I118:I121 I98:I103 I115:I116 I105:I113</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I119:I122 I98:I103 I105:I114 I116:I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -16555,7 +16667,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I122:I130</xm:sqref>
+          <xm:sqref>I123:I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -16570,7 +16682,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I131:I139</xm:sqref>
+          <xm:sqref>I132:I140</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -16585,7 +16697,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I140:I148</xm:sqref>
+          <xm:sqref>I141:I149</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -16600,7 +16712,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I149:I157</xm:sqref>
+          <xm:sqref>I150:I158</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -16660,7 +16772,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I117</xm:sqref>
+          <xm:sqref>I118</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
@@ -16675,7 +16787,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I114</xm:sqref>
+          <xm:sqref>I115</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
More nowcast refactoring (v0.15)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C732A35-DCE1-4F12-A36E-6A09DCFC9148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A537C50-0FFC-4602-9822-53950C36ECCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1788,6 +1788,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1797,6 +1804,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1805,17 +1816,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3305,7 +3305,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I114" sqref="I114"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3335,27 +3335,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3400,12 +3400,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3415,183 +3415,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -12433,7 +12433,7 @@
         <v>44383</v>
       </c>
       <c r="G109" s="43">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="H109" s="73"/>
       <c r="I109" s="26">
@@ -12511,10 +12511,10 @@
         <v>67</v>
       </c>
       <c r="F110" s="42">
-        <v>44389</v>
+        <v>44390</v>
       </c>
       <c r="G110" s="43">
-        <v>44389</v>
+        <v>44392</v>
       </c>
       <c r="H110" s="73"/>
       <c r="I110" s="26"/>
@@ -12590,7 +12590,7 @@
         <v>67</v>
       </c>
       <c r="F111" s="42">
-        <v>44389</v>
+        <v>44392</v>
       </c>
       <c r="G111" s="43"/>
       <c r="H111" s="73"/>
@@ -16042,15 +16042,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16061,6 +16052,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I120:I123 I98:I103 I105:I115 I117:I118">

</xml_diff>

<commit_message>
Refactoring nowcast - mostly matching previous version (v0.15)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A537C50-0FFC-4602-9822-53950C36ECCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA75CA4-E9C2-4875-A9BE-30D939A1F7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1788,13 +1788,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1804,10 +1797,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1816,6 +1805,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3305,7 +3305,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+      <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3335,27 +3335,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3400,12 +3400,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3415,183 +3415,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -12437,7 +12437,7 @@
       </c>
       <c r="H109" s="73"/>
       <c r="I109" s="26">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="J109" s="75"/>
       <c r="K109" s="76"/>
@@ -16042,6 +16042,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16052,15 +16061,6 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I120:I123 I98:I103 I105:I115 I117:I118">

</xml_diff>

<commit_message>
Added stationary transform to nowcast output (v0.15)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA75CA4-E9C2-4875-A9BE-30D939A1F7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AB15B6-877F-4B61-80D6-5FBD3E6A51F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1788,6 +1788,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1797,6 +1804,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1805,17 +1816,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3305,7 +3305,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I110" sqref="I110"/>
+      <selection pane="bottomLeft" activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3335,27 +3335,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3400,12 +3400,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3415,183 +3415,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -12437,7 +12437,7 @@
       </c>
       <c r="H109" s="73"/>
       <c r="I109" s="26">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="J109" s="75"/>
       <c r="K109" s="76"/>
@@ -12514,7 +12514,7 @@
         <v>44390</v>
       </c>
       <c r="G110" s="43">
-        <v>44392</v>
+        <v>44398</v>
       </c>
       <c r="H110" s="73"/>
       <c r="I110" s="26"/>
@@ -12590,7 +12590,7 @@
         <v>67</v>
       </c>
       <c r="F111" s="42">
-        <v>44392</v>
+        <v>44398</v>
       </c>
       <c r="G111" s="43"/>
       <c r="H111" s="73"/>
@@ -12667,7 +12667,7 @@
         <v>67</v>
       </c>
       <c r="F112" s="42">
-        <v>44392</v>
+        <v>44398</v>
       </c>
       <c r="G112" s="43"/>
       <c r="H112" s="73"/>
@@ -12744,7 +12744,7 @@
         <v>70</v>
       </c>
       <c r="F113" s="42">
-        <v>44392</v>
+        <v>44398</v>
       </c>
       <c r="G113" s="43"/>
       <c r="H113" s="73"/>
@@ -12821,7 +12821,7 @@
         <v>67</v>
       </c>
       <c r="F114" s="42">
-        <v>44392</v>
+        <v>44398</v>
       </c>
       <c r="G114" s="43"/>
       <c r="H114" s="73"/>
@@ -12898,7 +12898,7 @@
         <v>67</v>
       </c>
       <c r="F115" s="42">
-        <v>44392</v>
+        <v>44398</v>
       </c>
       <c r="G115" s="43"/>
       <c r="H115" s="73"/>
@@ -16042,15 +16042,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16061,6 +16052,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I120:I123 I98:I103 I105:I115 I117:I118">

</xml_diff>

<commit_message>
Added DNS curve rebuilding (v0.15)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AB15B6-877F-4B61-80D6-5FBD3E6A51F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE5E23A2-E689-469B-BC8F-40BB141231E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="145">
   <si>
     <t>WBS</t>
   </si>
@@ -860,6 +860,9 @@
   </si>
   <si>
     <t>XLSX</t>
+  </si>
+  <si>
+    <t>Add Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1788,13 +1791,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1804,10 +1800,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1816,6 +1808,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3301,11 +3304,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO159"/>
+  <dimension ref="A1:BO160"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F118" sqref="F118"/>
+      <selection pane="bottomLeft" activeCell="N118" sqref="N118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3335,27 +3338,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3400,12 +3403,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3415,183 +3418,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8749,7 +8752,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A124" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A125" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -12962,172 +12965,172 @@
       <c r="BN115" s="46"/>
       <c r="BO115" s="46"/>
     </row>
-    <row r="116" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="16" t="str">
+    <row r="116" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>10.12</v>
+      </c>
+      <c r="B116" s="65" t="s">
+        <v>144</v>
+      </c>
+      <c r="D116" s="70"/>
+      <c r="E116" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F116" s="71">
+        <v>44397</v>
+      </c>
+      <c r="G116" s="72"/>
+      <c r="H116" s="73"/>
+      <c r="I116" s="74"/>
+      <c r="J116" s="75"/>
+      <c r="K116" s="76"/>
+      <c r="L116" s="46"/>
+      <c r="M116" s="46"/>
+      <c r="N116" s="46"/>
+      <c r="O116" s="46"/>
+      <c r="P116" s="46"/>
+      <c r="Q116" s="46"/>
+      <c r="R116" s="46"/>
+      <c r="S116" s="46"/>
+      <c r="T116" s="46"/>
+      <c r="U116" s="46"/>
+      <c r="V116" s="46"/>
+      <c r="W116" s="46"/>
+      <c r="X116" s="46"/>
+      <c r="Y116" s="46"/>
+      <c r="Z116" s="46"/>
+      <c r="AA116" s="46"/>
+      <c r="AB116" s="46"/>
+      <c r="AC116" s="46"/>
+      <c r="AD116" s="46"/>
+      <c r="AE116" s="46"/>
+      <c r="AF116" s="46"/>
+      <c r="AG116" s="46"/>
+      <c r="AH116" s="46"/>
+      <c r="AI116" s="46"/>
+      <c r="AJ116" s="46"/>
+      <c r="AK116" s="46"/>
+      <c r="AL116" s="46"/>
+      <c r="AM116" s="46"/>
+      <c r="AN116" s="46"/>
+      <c r="AO116" s="46"/>
+      <c r="AP116" s="46"/>
+      <c r="AQ116" s="46"/>
+      <c r="AR116" s="46"/>
+      <c r="AS116" s="46"/>
+      <c r="AT116" s="46"/>
+      <c r="AU116" s="46"/>
+      <c r="AV116" s="46"/>
+      <c r="AW116" s="46"/>
+      <c r="AX116" s="46"/>
+      <c r="AY116" s="46"/>
+      <c r="AZ116" s="46"/>
+      <c r="BA116" s="46"/>
+      <c r="BB116" s="46"/>
+      <c r="BC116" s="46"/>
+      <c r="BD116" s="46"/>
+      <c r="BE116" s="46"/>
+      <c r="BF116" s="46"/>
+      <c r="BG116" s="46"/>
+      <c r="BH116" s="46"/>
+      <c r="BI116" s="46"/>
+      <c r="BJ116" s="46"/>
+      <c r="BK116" s="46"/>
+      <c r="BL116" s="46"/>
+      <c r="BM116" s="46"/>
+      <c r="BN116" s="46"/>
+      <c r="BO116" s="46"/>
+    </row>
+    <row r="117" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>11</v>
       </c>
-      <c r="B116" s="17" t="s">
+      <c r="B117" s="17" t="s">
         <v>129</v>
       </c>
-      <c r="D116" s="19"/>
-      <c r="E116" s="19"/>
-      <c r="F116" s="44"/>
-      <c r="G116" s="44" t="str">
-        <f t="shared" ref="G116" si="20">IF(ISBLANK(F116)," - ",IF(H116=0,F116,F116+H116-1))</f>
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="44"/>
+      <c r="G117" s="44" t="str">
+        <f t="shared" ref="G117" si="20">IF(ISBLANK(F117)," - ",IF(H117=0,F117,F117+H117-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H116" s="20"/>
-      <c r="I116" s="21"/>
-      <c r="J116" s="22" t="str">
-        <f t="shared" ref="J116" si="21">IF(OR(G116=0,F116=0)," - ",NETWORKDAYS(F116,G116))</f>
+      <c r="H117" s="20"/>
+      <c r="I117" s="21"/>
+      <c r="J117" s="22" t="str">
+        <f t="shared" ref="J117" si="21">IF(OR(G117=0,F117=0)," - ",NETWORKDAYS(F117,G117))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K116" s="41"/>
-      <c r="L116" s="48"/>
-      <c r="M116" s="48"/>
-      <c r="N116" s="48"/>
-      <c r="O116" s="48"/>
-      <c r="P116" s="48"/>
-      <c r="Q116" s="48"/>
-      <c r="R116" s="48"/>
-      <c r="S116" s="48"/>
-      <c r="T116" s="48"/>
-      <c r="U116" s="48"/>
-      <c r="V116" s="48"/>
-      <c r="W116" s="48"/>
-      <c r="X116" s="48"/>
-      <c r="Y116" s="48"/>
-      <c r="Z116" s="48"/>
-      <c r="AA116" s="48"/>
-      <c r="AB116" s="48"/>
-      <c r="AC116" s="48"/>
-      <c r="AD116" s="48"/>
-      <c r="AE116" s="48"/>
-      <c r="AF116" s="48"/>
-      <c r="AG116" s="48"/>
-      <c r="AH116" s="48"/>
-      <c r="AI116" s="48"/>
-      <c r="AJ116" s="48"/>
-      <c r="AK116" s="48"/>
-      <c r="AL116" s="48"/>
-      <c r="AM116" s="48"/>
-      <c r="AN116" s="48"/>
-      <c r="AO116" s="48"/>
-      <c r="AP116" s="48"/>
-      <c r="AQ116" s="48"/>
-      <c r="AR116" s="48"/>
-      <c r="AS116" s="48"/>
-      <c r="AT116" s="48"/>
-      <c r="AU116" s="48"/>
-      <c r="AV116" s="48"/>
-      <c r="AW116" s="48"/>
-      <c r="AX116" s="48"/>
-      <c r="AY116" s="48"/>
-      <c r="AZ116" s="48"/>
-      <c r="BA116" s="48"/>
-      <c r="BB116" s="48"/>
-      <c r="BC116" s="48"/>
-      <c r="BD116" s="48"/>
-      <c r="BE116" s="48"/>
-      <c r="BF116" s="48"/>
-      <c r="BG116" s="48"/>
-      <c r="BH116" s="48"/>
-      <c r="BI116" s="48"/>
-      <c r="BJ116" s="48"/>
-      <c r="BK116" s="48"/>
-      <c r="BL116" s="48"/>
-      <c r="BM116" s="48"/>
-      <c r="BN116" s="48"/>
-      <c r="BO116" s="48"/>
-    </row>
-    <row r="117" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>11.1</v>
-      </c>
-      <c r="B117" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="D117" s="70"/>
-      <c r="E117" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F117" s="42">
-        <v>44392</v>
-      </c>
-      <c r="G117" s="43"/>
-      <c r="H117" s="73"/>
-      <c r="I117" s="26"/>
-      <c r="J117" s="75"/>
-      <c r="K117" s="76"/>
-      <c r="L117" s="46"/>
-      <c r="M117" s="46"/>
-      <c r="N117" s="46"/>
-      <c r="O117" s="46"/>
-      <c r="P117" s="46"/>
-      <c r="Q117" s="46"/>
-      <c r="R117" s="46"/>
-      <c r="S117" s="46"/>
-      <c r="T117" s="46"/>
-      <c r="U117" s="46"/>
-      <c r="V117" s="46"/>
-      <c r="W117" s="46"/>
-      <c r="X117" s="46"/>
-      <c r="Y117" s="46"/>
-      <c r="Z117" s="46"/>
-      <c r="AA117" s="46"/>
-      <c r="AB117" s="46"/>
-      <c r="AC117" s="46"/>
-      <c r="AD117" s="46"/>
-      <c r="AE117" s="46"/>
-      <c r="AF117" s="46"/>
-      <c r="AG117" s="46"/>
-      <c r="AH117" s="46"/>
-      <c r="AI117" s="46"/>
-      <c r="AJ117" s="46"/>
-      <c r="AK117" s="46"/>
-      <c r="AL117" s="46"/>
-      <c r="AM117" s="46"/>
-      <c r="AN117" s="46"/>
-      <c r="AO117" s="46"/>
-      <c r="AP117" s="46"/>
-      <c r="AQ117" s="46"/>
-      <c r="AR117" s="46"/>
-      <c r="AS117" s="46"/>
-      <c r="AT117" s="46"/>
-      <c r="AU117" s="46"/>
-      <c r="AV117" s="46"/>
-      <c r="AW117" s="46"/>
-      <c r="AX117" s="46"/>
-      <c r="AY117" s="46"/>
-      <c r="AZ117" s="46"/>
-      <c r="BA117" s="46"/>
-      <c r="BB117" s="46"/>
-      <c r="BC117" s="46"/>
-      <c r="BD117" s="46"/>
-      <c r="BE117" s="46"/>
-      <c r="BF117" s="46"/>
-      <c r="BG117" s="46"/>
-      <c r="BH117" s="46"/>
-      <c r="BI117" s="46"/>
-      <c r="BJ117" s="46"/>
-      <c r="BK117" s="46"/>
-      <c r="BL117" s="46"/>
-      <c r="BM117" s="46"/>
-      <c r="BN117" s="46"/>
-      <c r="BO117" s="46"/>
+      <c r="K117" s="41"/>
+      <c r="L117" s="48"/>
+      <c r="M117" s="48"/>
+      <c r="N117" s="48"/>
+      <c r="O117" s="48"/>
+      <c r="P117" s="48"/>
+      <c r="Q117" s="48"/>
+      <c r="R117" s="48"/>
+      <c r="S117" s="48"/>
+      <c r="T117" s="48"/>
+      <c r="U117" s="48"/>
+      <c r="V117" s="48"/>
+      <c r="W117" s="48"/>
+      <c r="X117" s="48"/>
+      <c r="Y117" s="48"/>
+      <c r="Z117" s="48"/>
+      <c r="AA117" s="48"/>
+      <c r="AB117" s="48"/>
+      <c r="AC117" s="48"/>
+      <c r="AD117" s="48"/>
+      <c r="AE117" s="48"/>
+      <c r="AF117" s="48"/>
+      <c r="AG117" s="48"/>
+      <c r="AH117" s="48"/>
+      <c r="AI117" s="48"/>
+      <c r="AJ117" s="48"/>
+      <c r="AK117" s="48"/>
+      <c r="AL117" s="48"/>
+      <c r="AM117" s="48"/>
+      <c r="AN117" s="48"/>
+      <c r="AO117" s="48"/>
+      <c r="AP117" s="48"/>
+      <c r="AQ117" s="48"/>
+      <c r="AR117" s="48"/>
+      <c r="AS117" s="48"/>
+      <c r="AT117" s="48"/>
+      <c r="AU117" s="48"/>
+      <c r="AV117" s="48"/>
+      <c r="AW117" s="48"/>
+      <c r="AX117" s="48"/>
+      <c r="AY117" s="48"/>
+      <c r="AZ117" s="48"/>
+      <c r="BA117" s="48"/>
+      <c r="BB117" s="48"/>
+      <c r="BC117" s="48"/>
+      <c r="BD117" s="48"/>
+      <c r="BE117" s="48"/>
+      <c r="BF117" s="48"/>
+      <c r="BG117" s="48"/>
+      <c r="BH117" s="48"/>
+      <c r="BI117" s="48"/>
+      <c r="BJ117" s="48"/>
+      <c r="BK117" s="48"/>
+      <c r="BL117" s="48"/>
+      <c r="BM117" s="48"/>
+      <c r="BN117" s="48"/>
+      <c r="BO117" s="48"/>
     </row>
     <row r="118" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>11.2</v>
+        <v>11.1</v>
       </c>
       <c r="B118" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D118" s="70"/>
-      <c r="E118" s="70" t="s">
+      <c r="E118" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F118" s="42">
@@ -13135,7 +13138,7 @@
       </c>
       <c r="G118" s="43"/>
       <c r="H118" s="73"/>
-      <c r="I118" s="74"/>
+      <c r="I118" s="26"/>
       <c r="J118" s="75"/>
       <c r="K118" s="76"/>
       <c r="L118" s="46"/>
@@ -13195,173 +13198,173 @@
       <c r="BN118" s="46"/>
       <c r="BO118" s="46"/>
     </row>
-    <row r="119" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="16" t="str">
+    <row r="119" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.2</v>
+      </c>
+      <c r="B119" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="D119" s="70"/>
+      <c r="E119" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F119" s="42">
+        <v>44392</v>
+      </c>
+      <c r="G119" s="43"/>
+      <c r="H119" s="73"/>
+      <c r="I119" s="74"/>
+      <c r="J119" s="75"/>
+      <c r="K119" s="76"/>
+      <c r="L119" s="46"/>
+      <c r="M119" s="46"/>
+      <c r="N119" s="46"/>
+      <c r="O119" s="46"/>
+      <c r="P119" s="46"/>
+      <c r="Q119" s="46"/>
+      <c r="R119" s="46"/>
+      <c r="S119" s="46"/>
+      <c r="T119" s="46"/>
+      <c r="U119" s="46"/>
+      <c r="V119" s="46"/>
+      <c r="W119" s="46"/>
+      <c r="X119" s="46"/>
+      <c r="Y119" s="46"/>
+      <c r="Z119" s="46"/>
+      <c r="AA119" s="46"/>
+      <c r="AB119" s="46"/>
+      <c r="AC119" s="46"/>
+      <c r="AD119" s="46"/>
+      <c r="AE119" s="46"/>
+      <c r="AF119" s="46"/>
+      <c r="AG119" s="46"/>
+      <c r="AH119" s="46"/>
+      <c r="AI119" s="46"/>
+      <c r="AJ119" s="46"/>
+      <c r="AK119" s="46"/>
+      <c r="AL119" s="46"/>
+      <c r="AM119" s="46"/>
+      <c r="AN119" s="46"/>
+      <c r="AO119" s="46"/>
+      <c r="AP119" s="46"/>
+      <c r="AQ119" s="46"/>
+      <c r="AR119" s="46"/>
+      <c r="AS119" s="46"/>
+      <c r="AT119" s="46"/>
+      <c r="AU119" s="46"/>
+      <c r="AV119" s="46"/>
+      <c r="AW119" s="46"/>
+      <c r="AX119" s="46"/>
+      <c r="AY119" s="46"/>
+      <c r="AZ119" s="46"/>
+      <c r="BA119" s="46"/>
+      <c r="BB119" s="46"/>
+      <c r="BC119" s="46"/>
+      <c r="BD119" s="46"/>
+      <c r="BE119" s="46"/>
+      <c r="BF119" s="46"/>
+      <c r="BG119" s="46"/>
+      <c r="BH119" s="46"/>
+      <c r="BI119" s="46"/>
+      <c r="BJ119" s="46"/>
+      <c r="BK119" s="46"/>
+      <c r="BL119" s="46"/>
+      <c r="BM119" s="46"/>
+      <c r="BN119" s="46"/>
+      <c r="BO119" s="46"/>
+    </row>
+    <row r="120" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B119" s="17" t="s">
+      <c r="B120" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="D119" s="19"/>
-      <c r="E119" s="19"/>
-      <c r="F119" s="44"/>
-      <c r="G119" s="44" t="str">
-        <f t="shared" ref="G119" si="22">IF(ISBLANK(F119)," - ",IF(H119=0,F119,F119+H119-1))</f>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="44"/>
+      <c r="G120" s="44" t="str">
+        <f t="shared" ref="G120" si="22">IF(ISBLANK(F120)," - ",IF(H120=0,F120,F120+H120-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H119" s="20"/>
-      <c r="I119" s="21"/>
-      <c r="J119" s="22" t="str">
-        <f t="shared" ref="J119" si="23">IF(OR(G119=0,F119=0)," - ",NETWORKDAYS(F119,G119))</f>
+      <c r="H120" s="20"/>
+      <c r="I120" s="21"/>
+      <c r="J120" s="22" t="str">
+        <f t="shared" ref="J120" si="23">IF(OR(G120=0,F120=0)," - ",NETWORKDAYS(F120,G120))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K119" s="41"/>
-      <c r="L119" s="48"/>
-      <c r="M119" s="48"/>
-      <c r="N119" s="48"/>
-      <c r="O119" s="48"/>
-      <c r="P119" s="48"/>
-      <c r="Q119" s="48"/>
-      <c r="R119" s="48"/>
-      <c r="S119" s="48"/>
-      <c r="T119" s="48"/>
-      <c r="U119" s="48"/>
-      <c r="V119" s="48"/>
-      <c r="W119" s="48"/>
-      <c r="X119" s="48"/>
-      <c r="Y119" s="48"/>
-      <c r="Z119" s="48"/>
-      <c r="AA119" s="48"/>
-      <c r="AB119" s="48"/>
-      <c r="AC119" s="48"/>
-      <c r="AD119" s="48"/>
-      <c r="AE119" s="48"/>
-      <c r="AF119" s="48"/>
-      <c r="AG119" s="48"/>
-      <c r="AH119" s="48"/>
-      <c r="AI119" s="48"/>
-      <c r="AJ119" s="48"/>
-      <c r="AK119" s="48"/>
-      <c r="AL119" s="48"/>
-      <c r="AM119" s="48"/>
-      <c r="AN119" s="48"/>
-      <c r="AO119" s="48"/>
-      <c r="AP119" s="48"/>
-      <c r="AQ119" s="48"/>
-      <c r="AR119" s="48"/>
-      <c r="AS119" s="48"/>
-      <c r="AT119" s="48"/>
-      <c r="AU119" s="48"/>
-      <c r="AV119" s="48"/>
-      <c r="AW119" s="48"/>
-      <c r="AX119" s="48"/>
-      <c r="AY119" s="48"/>
-      <c r="AZ119" s="48"/>
-      <c r="BA119" s="48"/>
-      <c r="BB119" s="48"/>
-      <c r="BC119" s="48"/>
-      <c r="BD119" s="48"/>
-      <c r="BE119" s="48"/>
-      <c r="BF119" s="48"/>
-      <c r="BG119" s="48"/>
-      <c r="BH119" s="48"/>
-      <c r="BI119" s="48"/>
-      <c r="BJ119" s="48"/>
-      <c r="BK119" s="48"/>
-      <c r="BL119" s="48"/>
-      <c r="BM119" s="48"/>
-      <c r="BN119" s="48"/>
-      <c r="BO119" s="48"/>
-    </row>
-    <row r="120" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>12.1</v>
-      </c>
-      <c r="B120" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D120" s="70"/>
-      <c r="E120" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F120" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G120" s="43"/>
-      <c r="H120" s="25"/>
-      <c r="I120" s="26"/>
-      <c r="J120" s="27"/>
-      <c r="K120" s="40"/>
-      <c r="L120" s="46"/>
-      <c r="M120" s="46"/>
-      <c r="N120" s="46"/>
-      <c r="O120" s="46"/>
-      <c r="P120" s="46"/>
-      <c r="Q120" s="46"/>
-      <c r="R120" s="46"/>
-      <c r="S120" s="46"/>
-      <c r="T120" s="46"/>
-      <c r="U120" s="46"/>
-      <c r="V120" s="46"/>
-      <c r="W120" s="46"/>
-      <c r="X120" s="46"/>
-      <c r="Y120" s="46"/>
-      <c r="Z120" s="46"/>
-      <c r="AA120" s="46"/>
-      <c r="AB120" s="46"/>
-      <c r="AC120" s="46"/>
-      <c r="AD120" s="46"/>
-      <c r="AE120" s="46"/>
-      <c r="AF120" s="46"/>
-      <c r="AG120" s="46"/>
-      <c r="AH120" s="46"/>
-      <c r="AI120" s="46"/>
-      <c r="AJ120" s="46"/>
-      <c r="AK120" s="46"/>
-      <c r="AL120" s="46"/>
-      <c r="AM120" s="46"/>
-      <c r="AN120" s="46"/>
-      <c r="AO120" s="46"/>
-      <c r="AP120" s="46"/>
-      <c r="AQ120" s="46"/>
-      <c r="AR120" s="46"/>
-      <c r="AS120" s="46"/>
-      <c r="AT120" s="46"/>
-      <c r="AU120" s="46"/>
-      <c r="AV120" s="46"/>
-      <c r="AW120" s="46"/>
-      <c r="AX120" s="46"/>
-      <c r="AY120" s="46"/>
-      <c r="AZ120" s="46"/>
-      <c r="BA120" s="46"/>
-      <c r="BB120" s="46"/>
-      <c r="BC120" s="46"/>
-      <c r="BD120" s="46"/>
-      <c r="BE120" s="46"/>
-      <c r="BF120" s="46"/>
-      <c r="BG120" s="46"/>
-      <c r="BH120" s="46"/>
-      <c r="BI120" s="46"/>
-      <c r="BJ120" s="46"/>
-      <c r="BK120" s="46"/>
-      <c r="BL120" s="46"/>
-      <c r="BM120" s="46"/>
-      <c r="BN120" s="46"/>
-      <c r="BO120" s="46"/>
+      <c r="K120" s="41"/>
+      <c r="L120" s="48"/>
+      <c r="M120" s="48"/>
+      <c r="N120" s="48"/>
+      <c r="O120" s="48"/>
+      <c r="P120" s="48"/>
+      <c r="Q120" s="48"/>
+      <c r="R120" s="48"/>
+      <c r="S120" s="48"/>
+      <c r="T120" s="48"/>
+      <c r="U120" s="48"/>
+      <c r="V120" s="48"/>
+      <c r="W120" s="48"/>
+      <c r="X120" s="48"/>
+      <c r="Y120" s="48"/>
+      <c r="Z120" s="48"/>
+      <c r="AA120" s="48"/>
+      <c r="AB120" s="48"/>
+      <c r="AC120" s="48"/>
+      <c r="AD120" s="48"/>
+      <c r="AE120" s="48"/>
+      <c r="AF120" s="48"/>
+      <c r="AG120" s="48"/>
+      <c r="AH120" s="48"/>
+      <c r="AI120" s="48"/>
+      <c r="AJ120" s="48"/>
+      <c r="AK120" s="48"/>
+      <c r="AL120" s="48"/>
+      <c r="AM120" s="48"/>
+      <c r="AN120" s="48"/>
+      <c r="AO120" s="48"/>
+      <c r="AP120" s="48"/>
+      <c r="AQ120" s="48"/>
+      <c r="AR120" s="48"/>
+      <c r="AS120" s="48"/>
+      <c r="AT120" s="48"/>
+      <c r="AU120" s="48"/>
+      <c r="AV120" s="48"/>
+      <c r="AW120" s="48"/>
+      <c r="AX120" s="48"/>
+      <c r="AY120" s="48"/>
+      <c r="AZ120" s="48"/>
+      <c r="BA120" s="48"/>
+      <c r="BB120" s="48"/>
+      <c r="BC120" s="48"/>
+      <c r="BD120" s="48"/>
+      <c r="BE120" s="48"/>
+      <c r="BF120" s="48"/>
+      <c r="BG120" s="48"/>
+      <c r="BH120" s="48"/>
+      <c r="BI120" s="48"/>
+      <c r="BJ120" s="48"/>
+      <c r="BK120" s="48"/>
+      <c r="BL120" s="48"/>
+      <c r="BM120" s="48"/>
+      <c r="BN120" s="48"/>
+      <c r="BO120" s="48"/>
     </row>
     <row r="121" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D121" s="70"/>
       <c r="E121" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F121" s="42">
         <v>44379</v>
@@ -13431,14 +13434,14 @@
     <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="B122" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D122" s="70"/>
       <c r="E122" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F122" s="42">
         <v>44379</v>
@@ -13508,10 +13511,10 @@
     <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.4</v>
+        <v>12.3</v>
       </c>
       <c r="B123" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D123" s="70"/>
       <c r="E123" s="66" t="s">
@@ -13585,17 +13588,17 @@
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.5</v>
-      </c>
-      <c r="B124" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D124" s="66"/>
+        <v>12.4</v>
+      </c>
+      <c r="B124" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D124" s="70"/>
       <c r="E124" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F124" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G124" s="43"/>
       <c r="H124" s="25"/>
@@ -13660,11 +13663,20 @@
       <c r="BO124" s="46"/>
     </row>
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="23"/>
-      <c r="B125" s="65"/>
+      <c r="A125" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.5</v>
+      </c>
+      <c r="B125" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D125" s="66"/>
-      <c r="E125" s="66"/>
-      <c r="F125" s="42"/>
+      <c r="E125" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F125" s="42">
+        <v>44531</v>
+      </c>
       <c r="G125" s="43"/>
       <c r="H125" s="25"/>
       <c r="I125" s="26"/>
@@ -13866,7 +13878,7 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23"/>
       <c r="B128" s="65"/>
-      <c r="D128" s="70"/>
+      <c r="D128" s="66"/>
       <c r="E128" s="66"/>
       <c r="F128" s="42"/>
       <c r="G128" s="43"/>
@@ -14206,7 +14218,7 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23"/>
       <c r="B133" s="65"/>
-      <c r="D133" s="66"/>
+      <c r="D133" s="70"/>
       <c r="E133" s="66"/>
       <c r="F133" s="42"/>
       <c r="G133" s="43"/>
@@ -14478,7 +14490,7 @@
     <row r="137" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="23"/>
       <c r="B137" s="65"/>
-      <c r="D137" s="70"/>
+      <c r="D137" s="66"/>
       <c r="E137" s="66"/>
       <c r="F137" s="42"/>
       <c r="G137" s="43"/>
@@ -14818,7 +14830,7 @@
     <row r="142" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23"/>
       <c r="B142" s="65"/>
-      <c r="D142" s="66"/>
+      <c r="D142" s="70"/>
       <c r="E142" s="66"/>
       <c r="F142" s="42"/>
       <c r="G142" s="43"/>
@@ -15090,7 +15102,7 @@
     <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23"/>
       <c r="B146" s="65"/>
-      <c r="D146" s="70"/>
+      <c r="D146" s="66"/>
       <c r="E146" s="66"/>
       <c r="F146" s="42"/>
       <c r="G146" s="43"/>
@@ -15430,7 +15442,7 @@
     <row r="151" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="23"/>
       <c r="B151" s="65"/>
-      <c r="D151" s="66"/>
+      <c r="D151" s="70"/>
       <c r="E151" s="66"/>
       <c r="F151" s="42"/>
       <c r="G151" s="43"/>
@@ -15702,7 +15714,7 @@
     <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="23"/>
       <c r="B155" s="65"/>
-      <c r="D155" s="70"/>
+      <c r="D155" s="66"/>
       <c r="E155" s="66"/>
       <c r="F155" s="42"/>
       <c r="G155" s="43"/>
@@ -16039,9 +16051,86 @@
       <c r="BN159" s="46"/>
       <c r="BO159" s="46"/>
     </row>
+    <row r="160" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="23"/>
+      <c r="B160" s="65"/>
+      <c r="D160" s="70"/>
+      <c r="E160" s="66"/>
+      <c r="F160" s="42"/>
+      <c r="G160" s="43"/>
+      <c r="H160" s="25"/>
+      <c r="I160" s="26"/>
+      <c r="J160" s="27"/>
+      <c r="K160" s="40"/>
+      <c r="L160" s="46"/>
+      <c r="M160" s="46"/>
+      <c r="N160" s="46"/>
+      <c r="O160" s="46"/>
+      <c r="P160" s="46"/>
+      <c r="Q160" s="46"/>
+      <c r="R160" s="46"/>
+      <c r="S160" s="46"/>
+      <c r="T160" s="46"/>
+      <c r="U160" s="46"/>
+      <c r="V160" s="46"/>
+      <c r="W160" s="46"/>
+      <c r="X160" s="46"/>
+      <c r="Y160" s="46"/>
+      <c r="Z160" s="46"/>
+      <c r="AA160" s="46"/>
+      <c r="AB160" s="46"/>
+      <c r="AC160" s="46"/>
+      <c r="AD160" s="46"/>
+      <c r="AE160" s="46"/>
+      <c r="AF160" s="46"/>
+      <c r="AG160" s="46"/>
+      <c r="AH160" s="46"/>
+      <c r="AI160" s="46"/>
+      <c r="AJ160" s="46"/>
+      <c r="AK160" s="46"/>
+      <c r="AL160" s="46"/>
+      <c r="AM160" s="46"/>
+      <c r="AN160" s="46"/>
+      <c r="AO160" s="46"/>
+      <c r="AP160" s="46"/>
+      <c r="AQ160" s="46"/>
+      <c r="AR160" s="46"/>
+      <c r="AS160" s="46"/>
+      <c r="AT160" s="46"/>
+      <c r="AU160" s="46"/>
+      <c r="AV160" s="46"/>
+      <c r="AW160" s="46"/>
+      <c r="AX160" s="46"/>
+      <c r="AY160" s="46"/>
+      <c r="AZ160" s="46"/>
+      <c r="BA160" s="46"/>
+      <c r="BB160" s="46"/>
+      <c r="BC160" s="46"/>
+      <c r="BD160" s="46"/>
+      <c r="BE160" s="46"/>
+      <c r="BF160" s="46"/>
+      <c r="BG160" s="46"/>
+      <c r="BH160" s="46"/>
+      <c r="BI160" s="46"/>
+      <c r="BJ160" s="46"/>
+      <c r="BK160" s="46"/>
+      <c r="BL160" s="46"/>
+      <c r="BM160" s="46"/>
+      <c r="BN160" s="46"/>
+      <c r="BO160" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16052,18 +16141,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I120:I123 I98:I103 I105:I115 I117:I118">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I121:I124 I98:I103 I105:I116 I118:I119">
     <cfRule type="dataBar" priority="225">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16082,7 +16162,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 L124:BO126 M127:BN132 BO130:BO132 L133:BO135 M136:BN141 BO139:BO141 L142:BO144 M145:BN150 BO148:BO150 L151:BO153 M154:BN159 BO157:BO159 BO122:BO123 M120:BN123 L119:BO119 M117:BN118 M105:BN115 L116:BO116">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 L125:BO127 M128:BN133 BO131:BO133 L134:BO136 M137:BN142 BO140:BO142 L143:BO145 M146:BN151 BO149:BO151 L152:BO154 M155:BN160 BO158:BO160 BO123:BO124 M121:BN124 L120:BO120 M118:BN119 M105:BN116 L117:BO117">
     <cfRule type="expression" dxfId="122" priority="271">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -16090,7 +16170,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L120:BO123 L98:BO103 L117:BO118 L105:BO115">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L121:BO124 L98:BO103 L118:BO119 L105:BO116">
     <cfRule type="expression" dxfId="120" priority="231">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -16100,7 +16180,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E160:E1048576 E95:E96 E120:E123 E98:E103 E117:E118 E105:E115">
+  <conditionalFormatting sqref="E1:E73 E161:E1048576 E95:E96 E121:E124 E98:E103 E118:E119 E105:E116">
     <cfRule type="cellIs" dxfId="118" priority="212" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16194,7 +16274,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I124:I132">
+  <conditionalFormatting sqref="I125:I133">
     <cfRule type="dataBar" priority="116">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16208,12 +16288,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L124:BO132">
+  <conditionalFormatting sqref="L125:BO133">
     <cfRule type="expression" dxfId="96" priority="115">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E124:E132">
+  <conditionalFormatting sqref="E125:E133">
     <cfRule type="cellIs" dxfId="95" priority="108" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16236,7 +16316,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L127:BO132 L120:BO123 L98:BO103 L117:BO118 L105:BO115">
+  <conditionalFormatting sqref="L128:BO133 L121:BO124 L98:BO103 L118:BO119 L105:BO116">
     <cfRule type="expression" dxfId="88" priority="119">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16244,7 +16324,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I133:I141">
+  <conditionalFormatting sqref="I134:I142">
     <cfRule type="dataBar" priority="103">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16258,12 +16338,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L133:BO141">
+  <conditionalFormatting sqref="L134:BO142">
     <cfRule type="expression" dxfId="86" priority="102">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E133:E141">
+  <conditionalFormatting sqref="E134:E142">
     <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16286,7 +16366,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L136:BO141">
+  <conditionalFormatting sqref="L137:BO142">
     <cfRule type="expression" dxfId="78" priority="106">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16294,7 +16374,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I142:I150">
+  <conditionalFormatting sqref="I143:I151">
     <cfRule type="dataBar" priority="90">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16308,12 +16388,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L142:BO150">
+  <conditionalFormatting sqref="L143:BO151">
     <cfRule type="expression" dxfId="76" priority="89">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E142:E150">
+  <conditionalFormatting sqref="E143:E151">
     <cfRule type="cellIs" dxfId="75" priority="82" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16336,7 +16416,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L145:BO150">
+  <conditionalFormatting sqref="L146:BO151">
     <cfRule type="expression" dxfId="68" priority="93">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16344,7 +16424,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I151:I159">
+  <conditionalFormatting sqref="I152:I160">
     <cfRule type="dataBar" priority="77">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16358,12 +16438,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L151:BO159">
+  <conditionalFormatting sqref="L152:BO160">
     <cfRule type="expression" dxfId="66" priority="76">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E151:E159">
+  <conditionalFormatting sqref="E152:E160">
     <cfRule type="cellIs" dxfId="65" priority="69" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16386,7 +16466,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L154:BO159">
+  <conditionalFormatting sqref="L155:BO160">
     <cfRule type="expression" dxfId="58" priority="80">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16536,7 +16616,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I119">
+  <conditionalFormatting sqref="I120">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16550,12 +16630,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L119:BO119">
+  <conditionalFormatting sqref="L120:BO120">
     <cfRule type="expression" dxfId="28" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E119">
+  <conditionalFormatting sqref="E120">
     <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16578,7 +16658,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I116">
+  <conditionalFormatting sqref="I117">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16592,12 +16672,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L116:BO116">
+  <conditionalFormatting sqref="L117:BO117">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E116">
+  <conditionalFormatting sqref="E117">
     <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16726,7 +16806,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I120:I123 I98:I103 I105:I115 I117:I118</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I121:I124 I98:I103 I105:I116 I118:I119</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -16756,7 +16836,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I124:I132</xm:sqref>
+          <xm:sqref>I125:I133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -16771,7 +16851,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I133:I141</xm:sqref>
+          <xm:sqref>I134:I142</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -16786,7 +16866,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I142:I150</xm:sqref>
+          <xm:sqref>I143:I151</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -16801,7 +16881,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I151:I159</xm:sqref>
+          <xm:sqref>I152:I160</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -16861,7 +16941,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I119</xm:sqref>
+          <xm:sqref>I120</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
@@ -16876,7 +16956,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I116</xm:sqref>
+          <xm:sqref>I117</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Finished model stacking (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CF5E5E-B4F0-4328-8EE0-A5CB888A749A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAD157B-346D-4634-80D8-6C827AFDEA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="151">
   <si>
     <t>WBS</t>
   </si>
@@ -878,6 +878,9 @@
   </si>
   <si>
     <t>Add Forecasts to SQL</t>
+  </si>
+  <si>
+    <t>Nowcast Model Stacking - Reduce Variance</t>
   </si>
 </sst>
 </file>
@@ -1806,13 +1809,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1822,10 +1818,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1834,6 +1826,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3394,11 +3397,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO165"/>
+  <dimension ref="A1:BO166"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
+      <selection pane="bottomLeft" activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3428,27 +3431,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3493,12 +3496,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3508,183 +3511,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 25</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 26</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44361</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44368</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44375</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44382</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44389</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44396</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44403</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44410</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8842,7 +8845,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A130" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A131" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -12919,21 +12922,21 @@
         <v>11.3</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D114" s="70"/>
       <c r="E114" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F114" s="42">
-        <v>44407</v>
+        <v>44406</v>
       </c>
       <c r="G114" s="43">
         <v>44407</v>
       </c>
       <c r="H114" s="73"/>
       <c r="I114" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J114" s="75"/>
       <c r="K114" s="76"/>
@@ -13000,17 +13003,17 @@
         <v>11.4</v>
       </c>
       <c r="B115" s="65" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D115" s="70"/>
       <c r="E115" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F115" s="42">
         <v>44407</v>
       </c>
       <c r="G115" s="43">
-        <v>44407</v>
+        <v>44408</v>
       </c>
       <c r="H115" s="73"/>
       <c r="I115" s="26">
@@ -13081,11 +13084,11 @@
         <v>11.5</v>
       </c>
       <c r="B116" s="65" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="D116" s="70"/>
       <c r="E116" s="66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F116" s="42">
         <v>44408</v>
@@ -13094,7 +13097,9 @@
         <v>44409</v>
       </c>
       <c r="H116" s="73"/>
-      <c r="I116" s="26"/>
+      <c r="I116" s="26">
+        <v>0</v>
+      </c>
       <c r="J116" s="75"/>
       <c r="K116" s="76"/>
       <c r="L116" s="46"/>
@@ -13160,11 +13165,11 @@
         <v>11.6</v>
       </c>
       <c r="B117" s="65" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D117" s="70"/>
       <c r="E117" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F117" s="42">
         <v>44408</v>
@@ -13239,22 +13244,20 @@
         <v>11.7</v>
       </c>
       <c r="B118" s="65" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D118" s="70"/>
       <c r="E118" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F118" s="42">
-        <v>44409</v>
+        <v>44408</v>
       </c>
       <c r="G118" s="43">
         <v>44409</v>
       </c>
       <c r="H118" s="73"/>
-      <c r="I118" s="26">
-        <v>0.3</v>
-      </c>
+      <c r="I118" s="26"/>
       <c r="J118" s="75"/>
       <c r="K118" s="76"/>
       <c r="L118" s="46"/>
@@ -13320,20 +13323,22 @@
         <v>11.8</v>
       </c>
       <c r="B119" s="65" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D119" s="70"/>
       <c r="E119" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F119" s="42">
-        <v>44410</v>
+        <v>44409</v>
       </c>
       <c r="G119" s="43">
-        <v>44414</v>
+        <v>44409</v>
       </c>
       <c r="H119" s="73"/>
-      <c r="I119" s="26"/>
+      <c r="I119" s="26">
+        <v>0.3</v>
+      </c>
       <c r="J119" s="75"/>
       <c r="K119" s="76"/>
       <c r="L119" s="46"/>
@@ -13399,7 +13404,7 @@
         <v>11.9</v>
       </c>
       <c r="B120" s="65" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D120" s="70"/>
       <c r="E120" s="66" t="s">
@@ -13478,20 +13483,20 @@
         <v>11.10</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D121" s="70"/>
-      <c r="E121" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F121" s="71">
+      <c r="E121" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F121" s="42">
         <v>44410</v>
       </c>
-      <c r="G121" s="72">
+      <c r="G121" s="43">
         <v>44414</v>
       </c>
       <c r="H121" s="73"/>
-      <c r="I121" s="74"/>
+      <c r="I121" s="26"/>
       <c r="J121" s="75"/>
       <c r="K121" s="76"/>
       <c r="L121" s="46"/>
@@ -13551,172 +13556,174 @@
       <c r="BN121" s="46"/>
       <c r="BO121" s="46"/>
     </row>
-    <row r="122" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="16" t="str">
+    <row r="122" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.11</v>
+      </c>
+      <c r="B122" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="D122" s="70"/>
+      <c r="E122" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F122" s="71">
+        <v>44410</v>
+      </c>
+      <c r="G122" s="72">
+        <v>44414</v>
+      </c>
+      <c r="H122" s="73"/>
+      <c r="I122" s="74"/>
+      <c r="J122" s="75"/>
+      <c r="K122" s="76"/>
+      <c r="L122" s="46"/>
+      <c r="M122" s="46"/>
+      <c r="N122" s="46"/>
+      <c r="O122" s="46"/>
+      <c r="P122" s="46"/>
+      <c r="Q122" s="46"/>
+      <c r="R122" s="46"/>
+      <c r="S122" s="46"/>
+      <c r="T122" s="46"/>
+      <c r="U122" s="46"/>
+      <c r="V122" s="46"/>
+      <c r="W122" s="46"/>
+      <c r="X122" s="46"/>
+      <c r="Y122" s="46"/>
+      <c r="Z122" s="46"/>
+      <c r="AA122" s="46"/>
+      <c r="AB122" s="46"/>
+      <c r="AC122" s="46"/>
+      <c r="AD122" s="46"/>
+      <c r="AE122" s="46"/>
+      <c r="AF122" s="46"/>
+      <c r="AG122" s="46"/>
+      <c r="AH122" s="46"/>
+      <c r="AI122" s="46"/>
+      <c r="AJ122" s="46"/>
+      <c r="AK122" s="46"/>
+      <c r="AL122" s="46"/>
+      <c r="AM122" s="46"/>
+      <c r="AN122" s="46"/>
+      <c r="AO122" s="46"/>
+      <c r="AP122" s="46"/>
+      <c r="AQ122" s="46"/>
+      <c r="AR122" s="46"/>
+      <c r="AS122" s="46"/>
+      <c r="AT122" s="46"/>
+      <c r="AU122" s="46"/>
+      <c r="AV122" s="46"/>
+      <c r="AW122" s="46"/>
+      <c r="AX122" s="46"/>
+      <c r="AY122" s="46"/>
+      <c r="AZ122" s="46"/>
+      <c r="BA122" s="46"/>
+      <c r="BB122" s="46"/>
+      <c r="BC122" s="46"/>
+      <c r="BD122" s="46"/>
+      <c r="BE122" s="46"/>
+      <c r="BF122" s="46"/>
+      <c r="BG122" s="46"/>
+      <c r="BH122" s="46"/>
+      <c r="BI122" s="46"/>
+      <c r="BJ122" s="46"/>
+      <c r="BK122" s="46"/>
+      <c r="BL122" s="46"/>
+      <c r="BM122" s="46"/>
+      <c r="BN122" s="46"/>
+      <c r="BO122" s="46"/>
+    </row>
+    <row r="123" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B122" s="17" t="s">
+      <c r="B123" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D122" s="19"/>
-      <c r="E122" s="19"/>
-      <c r="F122" s="44"/>
-      <c r="G122" s="44" t="str">
-        <f t="shared" ref="G122" si="22">IF(ISBLANK(F122)," - ",IF(H122=0,F122,F122+H122-1))</f>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="44"/>
+      <c r="G123" s="44" t="str">
+        <f t="shared" ref="G123" si="22">IF(ISBLANK(F123)," - ",IF(H123=0,F123,F123+H123-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H122" s="20"/>
-      <c r="I122" s="21"/>
-      <c r="J122" s="22" t="str">
-        <f t="shared" ref="J122" si="23">IF(OR(G122=0,F122=0)," - ",NETWORKDAYS(F122,G122))</f>
+      <c r="H123" s="20"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="22" t="str">
+        <f t="shared" ref="J123" si="23">IF(OR(G123=0,F123=0)," - ",NETWORKDAYS(F123,G123))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K122" s="41"/>
-      <c r="L122" s="48"/>
-      <c r="M122" s="48"/>
-      <c r="N122" s="48"/>
-      <c r="O122" s="48"/>
-      <c r="P122" s="48"/>
-      <c r="Q122" s="48"/>
-      <c r="R122" s="48"/>
-      <c r="S122" s="48"/>
-      <c r="T122" s="48"/>
-      <c r="U122" s="48"/>
-      <c r="V122" s="48"/>
-      <c r="W122" s="48"/>
-      <c r="X122" s="48"/>
-      <c r="Y122" s="48"/>
-      <c r="Z122" s="48"/>
-      <c r="AA122" s="48"/>
-      <c r="AB122" s="48"/>
-      <c r="AC122" s="48"/>
-      <c r="AD122" s="48"/>
-      <c r="AE122" s="48"/>
-      <c r="AF122" s="48"/>
-      <c r="AG122" s="48"/>
-      <c r="AH122" s="48"/>
-      <c r="AI122" s="48"/>
-      <c r="AJ122" s="48"/>
-      <c r="AK122" s="48"/>
-      <c r="AL122" s="48"/>
-      <c r="AM122" s="48"/>
-      <c r="AN122" s="48"/>
-      <c r="AO122" s="48"/>
-      <c r="AP122" s="48"/>
-      <c r="AQ122" s="48"/>
-      <c r="AR122" s="48"/>
-      <c r="AS122" s="48"/>
-      <c r="AT122" s="48"/>
-      <c r="AU122" s="48"/>
-      <c r="AV122" s="48"/>
-      <c r="AW122" s="48"/>
-      <c r="AX122" s="48"/>
-      <c r="AY122" s="48"/>
-      <c r="AZ122" s="48"/>
-      <c r="BA122" s="48"/>
-      <c r="BB122" s="48"/>
-      <c r="BC122" s="48"/>
-      <c r="BD122" s="48"/>
-      <c r="BE122" s="48"/>
-      <c r="BF122" s="48"/>
-      <c r="BG122" s="48"/>
-      <c r="BH122" s="48"/>
-      <c r="BI122" s="48"/>
-      <c r="BJ122" s="48"/>
-      <c r="BK122" s="48"/>
-      <c r="BL122" s="48"/>
-      <c r="BM122" s="48"/>
-      <c r="BN122" s="48"/>
-      <c r="BO122" s="48"/>
-    </row>
-    <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>12.1</v>
-      </c>
-      <c r="B123" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="D123" s="70"/>
-      <c r="E123" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F123" s="42">
-        <v>44392</v>
-      </c>
-      <c r="G123" s="43"/>
-      <c r="H123" s="73"/>
-      <c r="I123" s="26"/>
-      <c r="J123" s="75"/>
-      <c r="K123" s="76"/>
-      <c r="L123" s="46"/>
-      <c r="M123" s="46"/>
-      <c r="N123" s="46"/>
-      <c r="O123" s="46"/>
-      <c r="P123" s="46"/>
-      <c r="Q123" s="46"/>
-      <c r="R123" s="46"/>
-      <c r="S123" s="46"/>
-      <c r="T123" s="46"/>
-      <c r="U123" s="46"/>
-      <c r="V123" s="46"/>
-      <c r="W123" s="46"/>
-      <c r="X123" s="46"/>
-      <c r="Y123" s="46"/>
-      <c r="Z123" s="46"/>
-      <c r="AA123" s="46"/>
-      <c r="AB123" s="46"/>
-      <c r="AC123" s="46"/>
-      <c r="AD123" s="46"/>
-      <c r="AE123" s="46"/>
-      <c r="AF123" s="46"/>
-      <c r="AG123" s="46"/>
-      <c r="AH123" s="46"/>
-      <c r="AI123" s="46"/>
-      <c r="AJ123" s="46"/>
-      <c r="AK123" s="46"/>
-      <c r="AL123" s="46"/>
-      <c r="AM123" s="46"/>
-      <c r="AN123" s="46"/>
-      <c r="AO123" s="46"/>
-      <c r="AP123" s="46"/>
-      <c r="AQ123" s="46"/>
-      <c r="AR123" s="46"/>
-      <c r="AS123" s="46"/>
-      <c r="AT123" s="46"/>
-      <c r="AU123" s="46"/>
-      <c r="AV123" s="46"/>
-      <c r="AW123" s="46"/>
-      <c r="AX123" s="46"/>
-      <c r="AY123" s="46"/>
-      <c r="AZ123" s="46"/>
-      <c r="BA123" s="46"/>
-      <c r="BB123" s="46"/>
-      <c r="BC123" s="46"/>
-      <c r="BD123" s="46"/>
-      <c r="BE123" s="46"/>
-      <c r="BF123" s="46"/>
-      <c r="BG123" s="46"/>
-      <c r="BH123" s="46"/>
-      <c r="BI123" s="46"/>
-      <c r="BJ123" s="46"/>
-      <c r="BK123" s="46"/>
-      <c r="BL123" s="46"/>
-      <c r="BM123" s="46"/>
-      <c r="BN123" s="46"/>
-      <c r="BO123" s="46"/>
+      <c r="K123" s="41"/>
+      <c r="L123" s="48"/>
+      <c r="M123" s="48"/>
+      <c r="N123" s="48"/>
+      <c r="O123" s="48"/>
+      <c r="P123" s="48"/>
+      <c r="Q123" s="48"/>
+      <c r="R123" s="48"/>
+      <c r="S123" s="48"/>
+      <c r="T123" s="48"/>
+      <c r="U123" s="48"/>
+      <c r="V123" s="48"/>
+      <c r="W123" s="48"/>
+      <c r="X123" s="48"/>
+      <c r="Y123" s="48"/>
+      <c r="Z123" s="48"/>
+      <c r="AA123" s="48"/>
+      <c r="AB123" s="48"/>
+      <c r="AC123" s="48"/>
+      <c r="AD123" s="48"/>
+      <c r="AE123" s="48"/>
+      <c r="AF123" s="48"/>
+      <c r="AG123" s="48"/>
+      <c r="AH123" s="48"/>
+      <c r="AI123" s="48"/>
+      <c r="AJ123" s="48"/>
+      <c r="AK123" s="48"/>
+      <c r="AL123" s="48"/>
+      <c r="AM123" s="48"/>
+      <c r="AN123" s="48"/>
+      <c r="AO123" s="48"/>
+      <c r="AP123" s="48"/>
+      <c r="AQ123" s="48"/>
+      <c r="AR123" s="48"/>
+      <c r="AS123" s="48"/>
+      <c r="AT123" s="48"/>
+      <c r="AU123" s="48"/>
+      <c r="AV123" s="48"/>
+      <c r="AW123" s="48"/>
+      <c r="AX123" s="48"/>
+      <c r="AY123" s="48"/>
+      <c r="AZ123" s="48"/>
+      <c r="BA123" s="48"/>
+      <c r="BB123" s="48"/>
+      <c r="BC123" s="48"/>
+      <c r="BD123" s="48"/>
+      <c r="BE123" s="48"/>
+      <c r="BF123" s="48"/>
+      <c r="BG123" s="48"/>
+      <c r="BH123" s="48"/>
+      <c r="BI123" s="48"/>
+      <c r="BJ123" s="48"/>
+      <c r="BK123" s="48"/>
+      <c r="BL123" s="48"/>
+      <c r="BM123" s="48"/>
+      <c r="BN123" s="48"/>
+      <c r="BO123" s="48"/>
     </row>
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="B124" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D124" s="70"/>
-      <c r="E124" s="70" t="s">
+      <c r="E124" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F124" s="42">
@@ -13724,7 +13731,7 @@
       </c>
       <c r="G124" s="43"/>
       <c r="H124" s="73"/>
-      <c r="I124" s="74"/>
+      <c r="I124" s="26"/>
       <c r="J124" s="75"/>
       <c r="K124" s="76"/>
       <c r="L124" s="46"/>
@@ -13784,173 +13791,173 @@
       <c r="BN124" s="46"/>
       <c r="BO124" s="46"/>
     </row>
-    <row r="125" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="16" t="str">
+    <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.2</v>
+      </c>
+      <c r="B125" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D125" s="70"/>
+      <c r="E125" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F125" s="42">
+        <v>44392</v>
+      </c>
+      <c r="G125" s="43"/>
+      <c r="H125" s="73"/>
+      <c r="I125" s="74"/>
+      <c r="J125" s="75"/>
+      <c r="K125" s="76"/>
+      <c r="L125" s="46"/>
+      <c r="M125" s="46"/>
+      <c r="N125" s="46"/>
+      <c r="O125" s="46"/>
+      <c r="P125" s="46"/>
+      <c r="Q125" s="46"/>
+      <c r="R125" s="46"/>
+      <c r="S125" s="46"/>
+      <c r="T125" s="46"/>
+      <c r="U125" s="46"/>
+      <c r="V125" s="46"/>
+      <c r="W125" s="46"/>
+      <c r="X125" s="46"/>
+      <c r="Y125" s="46"/>
+      <c r="Z125" s="46"/>
+      <c r="AA125" s="46"/>
+      <c r="AB125" s="46"/>
+      <c r="AC125" s="46"/>
+      <c r="AD125" s="46"/>
+      <c r="AE125" s="46"/>
+      <c r="AF125" s="46"/>
+      <c r="AG125" s="46"/>
+      <c r="AH125" s="46"/>
+      <c r="AI125" s="46"/>
+      <c r="AJ125" s="46"/>
+      <c r="AK125" s="46"/>
+      <c r="AL125" s="46"/>
+      <c r="AM125" s="46"/>
+      <c r="AN125" s="46"/>
+      <c r="AO125" s="46"/>
+      <c r="AP125" s="46"/>
+      <c r="AQ125" s="46"/>
+      <c r="AR125" s="46"/>
+      <c r="AS125" s="46"/>
+      <c r="AT125" s="46"/>
+      <c r="AU125" s="46"/>
+      <c r="AV125" s="46"/>
+      <c r="AW125" s="46"/>
+      <c r="AX125" s="46"/>
+      <c r="AY125" s="46"/>
+      <c r="AZ125" s="46"/>
+      <c r="BA125" s="46"/>
+      <c r="BB125" s="46"/>
+      <c r="BC125" s="46"/>
+      <c r="BD125" s="46"/>
+      <c r="BE125" s="46"/>
+      <c r="BF125" s="46"/>
+      <c r="BG125" s="46"/>
+      <c r="BH125" s="46"/>
+      <c r="BI125" s="46"/>
+      <c r="BJ125" s="46"/>
+      <c r="BK125" s="46"/>
+      <c r="BL125" s="46"/>
+      <c r="BM125" s="46"/>
+      <c r="BN125" s="46"/>
+      <c r="BO125" s="46"/>
+    </row>
+    <row r="126" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>13</v>
       </c>
-      <c r="B125" s="17" t="s">
+      <c r="B126" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D125" s="19"/>
-      <c r="E125" s="19"/>
-      <c r="F125" s="44"/>
-      <c r="G125" s="44" t="str">
-        <f t="shared" ref="G125" si="24">IF(ISBLANK(F125)," - ",IF(H125=0,F125,F125+H125-1))</f>
+      <c r="D126" s="19"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="44"/>
+      <c r="G126" s="44" t="str">
+        <f t="shared" ref="G126" si="24">IF(ISBLANK(F126)," - ",IF(H126=0,F126,F126+H126-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H125" s="20"/>
-      <c r="I125" s="21"/>
-      <c r="J125" s="22" t="str">
-        <f t="shared" ref="J125" si="25">IF(OR(G125=0,F125=0)," - ",NETWORKDAYS(F125,G125))</f>
+      <c r="H126" s="20"/>
+      <c r="I126" s="21"/>
+      <c r="J126" s="22" t="str">
+        <f t="shared" ref="J126" si="25">IF(OR(G126=0,F126=0)," - ",NETWORKDAYS(F126,G126))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K125" s="41"/>
-      <c r="L125" s="48"/>
-      <c r="M125" s="48"/>
-      <c r="N125" s="48"/>
-      <c r="O125" s="48"/>
-      <c r="P125" s="48"/>
-      <c r="Q125" s="48"/>
-      <c r="R125" s="48"/>
-      <c r="S125" s="48"/>
-      <c r="T125" s="48"/>
-      <c r="U125" s="48"/>
-      <c r="V125" s="48"/>
-      <c r="W125" s="48"/>
-      <c r="X125" s="48"/>
-      <c r="Y125" s="48"/>
-      <c r="Z125" s="48"/>
-      <c r="AA125" s="48"/>
-      <c r="AB125" s="48"/>
-      <c r="AC125" s="48"/>
-      <c r="AD125" s="48"/>
-      <c r="AE125" s="48"/>
-      <c r="AF125" s="48"/>
-      <c r="AG125" s="48"/>
-      <c r="AH125" s="48"/>
-      <c r="AI125" s="48"/>
-      <c r="AJ125" s="48"/>
-      <c r="AK125" s="48"/>
-      <c r="AL125" s="48"/>
-      <c r="AM125" s="48"/>
-      <c r="AN125" s="48"/>
-      <c r="AO125" s="48"/>
-      <c r="AP125" s="48"/>
-      <c r="AQ125" s="48"/>
-      <c r="AR125" s="48"/>
-      <c r="AS125" s="48"/>
-      <c r="AT125" s="48"/>
-      <c r="AU125" s="48"/>
-      <c r="AV125" s="48"/>
-      <c r="AW125" s="48"/>
-      <c r="AX125" s="48"/>
-      <c r="AY125" s="48"/>
-      <c r="AZ125" s="48"/>
-      <c r="BA125" s="48"/>
-      <c r="BB125" s="48"/>
-      <c r="BC125" s="48"/>
-      <c r="BD125" s="48"/>
-      <c r="BE125" s="48"/>
-      <c r="BF125" s="48"/>
-      <c r="BG125" s="48"/>
-      <c r="BH125" s="48"/>
-      <c r="BI125" s="48"/>
-      <c r="BJ125" s="48"/>
-      <c r="BK125" s="48"/>
-      <c r="BL125" s="48"/>
-      <c r="BM125" s="48"/>
-      <c r="BN125" s="48"/>
-      <c r="BO125" s="48"/>
-    </row>
-    <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.1</v>
-      </c>
-      <c r="B126" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D126" s="70"/>
-      <c r="E126" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F126" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G126" s="43"/>
-      <c r="H126" s="25"/>
-      <c r="I126" s="26"/>
-      <c r="J126" s="27"/>
-      <c r="K126" s="40"/>
-      <c r="L126" s="46"/>
-      <c r="M126" s="46"/>
-      <c r="N126" s="46"/>
-      <c r="O126" s="46"/>
-      <c r="P126" s="46"/>
-      <c r="Q126" s="46"/>
-      <c r="R126" s="46"/>
-      <c r="S126" s="46"/>
-      <c r="T126" s="46"/>
-      <c r="U126" s="46"/>
-      <c r="V126" s="46"/>
-      <c r="W126" s="46"/>
-      <c r="X126" s="46"/>
-      <c r="Y126" s="46"/>
-      <c r="Z126" s="46"/>
-      <c r="AA126" s="46"/>
-      <c r="AB126" s="46"/>
-      <c r="AC126" s="46"/>
-      <c r="AD126" s="46"/>
-      <c r="AE126" s="46"/>
-      <c r="AF126" s="46"/>
-      <c r="AG126" s="46"/>
-      <c r="AH126" s="46"/>
-      <c r="AI126" s="46"/>
-      <c r="AJ126" s="46"/>
-      <c r="AK126" s="46"/>
-      <c r="AL126" s="46"/>
-      <c r="AM126" s="46"/>
-      <c r="AN126" s="46"/>
-      <c r="AO126" s="46"/>
-      <c r="AP126" s="46"/>
-      <c r="AQ126" s="46"/>
-      <c r="AR126" s="46"/>
-      <c r="AS126" s="46"/>
-      <c r="AT126" s="46"/>
-      <c r="AU126" s="46"/>
-      <c r="AV126" s="46"/>
-      <c r="AW126" s="46"/>
-      <c r="AX126" s="46"/>
-      <c r="AY126" s="46"/>
-      <c r="AZ126" s="46"/>
-      <c r="BA126" s="46"/>
-      <c r="BB126" s="46"/>
-      <c r="BC126" s="46"/>
-      <c r="BD126" s="46"/>
-      <c r="BE126" s="46"/>
-      <c r="BF126" s="46"/>
-      <c r="BG126" s="46"/>
-      <c r="BH126" s="46"/>
-      <c r="BI126" s="46"/>
-      <c r="BJ126" s="46"/>
-      <c r="BK126" s="46"/>
-      <c r="BL126" s="46"/>
-      <c r="BM126" s="46"/>
-      <c r="BN126" s="46"/>
-      <c r="BO126" s="46"/>
+      <c r="K126" s="41"/>
+      <c r="L126" s="48"/>
+      <c r="M126" s="48"/>
+      <c r="N126" s="48"/>
+      <c r="O126" s="48"/>
+      <c r="P126" s="48"/>
+      <c r="Q126" s="48"/>
+      <c r="R126" s="48"/>
+      <c r="S126" s="48"/>
+      <c r="T126" s="48"/>
+      <c r="U126" s="48"/>
+      <c r="V126" s="48"/>
+      <c r="W126" s="48"/>
+      <c r="X126" s="48"/>
+      <c r="Y126" s="48"/>
+      <c r="Z126" s="48"/>
+      <c r="AA126" s="48"/>
+      <c r="AB126" s="48"/>
+      <c r="AC126" s="48"/>
+      <c r="AD126" s="48"/>
+      <c r="AE126" s="48"/>
+      <c r="AF126" s="48"/>
+      <c r="AG126" s="48"/>
+      <c r="AH126" s="48"/>
+      <c r="AI126" s="48"/>
+      <c r="AJ126" s="48"/>
+      <c r="AK126" s="48"/>
+      <c r="AL126" s="48"/>
+      <c r="AM126" s="48"/>
+      <c r="AN126" s="48"/>
+      <c r="AO126" s="48"/>
+      <c r="AP126" s="48"/>
+      <c r="AQ126" s="48"/>
+      <c r="AR126" s="48"/>
+      <c r="AS126" s="48"/>
+      <c r="AT126" s="48"/>
+      <c r="AU126" s="48"/>
+      <c r="AV126" s="48"/>
+      <c r="AW126" s="48"/>
+      <c r="AX126" s="48"/>
+      <c r="AY126" s="48"/>
+      <c r="AZ126" s="48"/>
+      <c r="BA126" s="48"/>
+      <c r="BB126" s="48"/>
+      <c r="BC126" s="48"/>
+      <c r="BD126" s="48"/>
+      <c r="BE126" s="48"/>
+      <c r="BF126" s="48"/>
+      <c r="BG126" s="48"/>
+      <c r="BH126" s="48"/>
+      <c r="BI126" s="48"/>
+      <c r="BJ126" s="48"/>
+      <c r="BK126" s="48"/>
+      <c r="BL126" s="48"/>
+      <c r="BM126" s="48"/>
+      <c r="BN126" s="48"/>
+      <c r="BO126" s="48"/>
     </row>
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="B127" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D127" s="70"/>
       <c r="E127" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F127" s="42">
         <v>44379</v>
@@ -14020,14 +14027,14 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="B128" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D128" s="70"/>
       <c r="E128" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F128" s="42">
         <v>44379</v>
@@ -14097,10 +14104,10 @@
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D129" s="70"/>
       <c r="E129" s="66" t="s">
@@ -14174,17 +14181,17 @@
     <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B130" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D130" s="66"/>
+        <v>13.4</v>
+      </c>
+      <c r="B130" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D130" s="70"/>
       <c r="E130" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F130" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G130" s="43"/>
       <c r="H130" s="25"/>
@@ -14249,11 +14256,20 @@
       <c r="BO130" s="46"/>
     </row>
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="23"/>
-      <c r="B131" s="65"/>
+      <c r="A131" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B131" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D131" s="66"/>
-      <c r="E131" s="66"/>
-      <c r="F131" s="42"/>
+      <c r="E131" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F131" s="42">
+        <v>44531</v>
+      </c>
       <c r="G131" s="43"/>
       <c r="H131" s="25"/>
       <c r="I131" s="26"/>
@@ -14455,7 +14471,7 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23"/>
       <c r="B134" s="65"/>
-      <c r="D134" s="70"/>
+      <c r="D134" s="66"/>
       <c r="E134" s="66"/>
       <c r="F134" s="42"/>
       <c r="G134" s="43"/>
@@ -14795,7 +14811,7 @@
     <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="23"/>
       <c r="B139" s="65"/>
-      <c r="D139" s="66"/>
+      <c r="D139" s="70"/>
       <c r="E139" s="66"/>
       <c r="F139" s="42"/>
       <c r="G139" s="43"/>
@@ -15067,7 +15083,7 @@
     <row r="143" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23"/>
       <c r="B143" s="65"/>
-      <c r="D143" s="70"/>
+      <c r="D143" s="66"/>
       <c r="E143" s="66"/>
       <c r="F143" s="42"/>
       <c r="G143" s="43"/>
@@ -15407,7 +15423,7 @@
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="23"/>
       <c r="B148" s="65"/>
-      <c r="D148" s="66"/>
+      <c r="D148" s="70"/>
       <c r="E148" s="66"/>
       <c r="F148" s="42"/>
       <c r="G148" s="43"/>
@@ -15679,7 +15695,7 @@
     <row r="152" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="23"/>
       <c r="B152" s="65"/>
-      <c r="D152" s="70"/>
+      <c r="D152" s="66"/>
       <c r="E152" s="66"/>
       <c r="F152" s="42"/>
       <c r="G152" s="43"/>
@@ -16019,7 +16035,7 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23"/>
       <c r="B157" s="65"/>
-      <c r="D157" s="66"/>
+      <c r="D157" s="70"/>
       <c r="E157" s="66"/>
       <c r="F157" s="42"/>
       <c r="G157" s="43"/>
@@ -16291,7 +16307,7 @@
     <row r="161" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="23"/>
       <c r="B161" s="65"/>
-      <c r="D161" s="70"/>
+      <c r="D161" s="66"/>
       <c r="E161" s="66"/>
       <c r="F161" s="42"/>
       <c r="G161" s="43"/>
@@ -16628,9 +16644,86 @@
       <c r="BN165" s="46"/>
       <c r="BO165" s="46"/>
     </row>
+    <row r="166" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="23"/>
+      <c r="B166" s="65"/>
+      <c r="D166" s="70"/>
+      <c r="E166" s="66"/>
+      <c r="F166" s="42"/>
+      <c r="G166" s="43"/>
+      <c r="H166" s="25"/>
+      <c r="I166" s="26"/>
+      <c r="J166" s="27"/>
+      <c r="K166" s="40"/>
+      <c r="L166" s="46"/>
+      <c r="M166" s="46"/>
+      <c r="N166" s="46"/>
+      <c r="O166" s="46"/>
+      <c r="P166" s="46"/>
+      <c r="Q166" s="46"/>
+      <c r="R166" s="46"/>
+      <c r="S166" s="46"/>
+      <c r="T166" s="46"/>
+      <c r="U166" s="46"/>
+      <c r="V166" s="46"/>
+      <c r="W166" s="46"/>
+      <c r="X166" s="46"/>
+      <c r="Y166" s="46"/>
+      <c r="Z166" s="46"/>
+      <c r="AA166" s="46"/>
+      <c r="AB166" s="46"/>
+      <c r="AC166" s="46"/>
+      <c r="AD166" s="46"/>
+      <c r="AE166" s="46"/>
+      <c r="AF166" s="46"/>
+      <c r="AG166" s="46"/>
+      <c r="AH166" s="46"/>
+      <c r="AI166" s="46"/>
+      <c r="AJ166" s="46"/>
+      <c r="AK166" s="46"/>
+      <c r="AL166" s="46"/>
+      <c r="AM166" s="46"/>
+      <c r="AN166" s="46"/>
+      <c r="AO166" s="46"/>
+      <c r="AP166" s="46"/>
+      <c r="AQ166" s="46"/>
+      <c r="AR166" s="46"/>
+      <c r="AS166" s="46"/>
+      <c r="AT166" s="46"/>
+      <c r="AU166" s="46"/>
+      <c r="AV166" s="46"/>
+      <c r="AW166" s="46"/>
+      <c r="AX166" s="46"/>
+      <c r="AY166" s="46"/>
+      <c r="AZ166" s="46"/>
+      <c r="BA166" s="46"/>
+      <c r="BB166" s="46"/>
+      <c r="BC166" s="46"/>
+      <c r="BD166" s="46"/>
+      <c r="BE166" s="46"/>
+      <c r="BF166" s="46"/>
+      <c r="BG166" s="46"/>
+      <c r="BH166" s="46"/>
+      <c r="BI166" s="46"/>
+      <c r="BJ166" s="46"/>
+      <c r="BK166" s="46"/>
+      <c r="BL166" s="46"/>
+      <c r="BM166" s="46"/>
+      <c r="BN166" s="46"/>
+      <c r="BO166" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16641,18 +16734,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I126:I129 I98:I103 I105:I110 I123:I124 I112:I121">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I127:I130 I98:I103 I105:I110 I124:I125 I112:I122">
     <cfRule type="dataBar" priority="236">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16671,7 +16755,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 L130:BO132 M133:BN138 BO136:BO138 L139:BO141 M142:BN147 BO145:BO147 L148:BO150 M151:BN156 BO154:BO156 L157:BO159 M160:BN165 BO163:BO165 BO128:BO129 M126:BN129 L125:BO125 M123:BN124 L122:BO122 M112:BN121">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 L131:BO133 M134:BN139 BO137:BO139 L140:BO142 M143:BN148 BO146:BO148 L149:BO151 M152:BN157 BO155:BO157 L158:BO160 M161:BN166 BO164:BO166 BO129:BO130 M127:BN130 L126:BO126 M124:BN125 L123:BO123 M112:BN122">
     <cfRule type="expression" dxfId="132" priority="282">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -16679,7 +16763,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L126:BO129 L98:BO103 L123:BO124 L105:BO110 L112:BO121">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L127:BO130 L98:BO103 L124:BO125 L105:BO110 L112:BO122">
     <cfRule type="expression" dxfId="130" priority="242">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -16689,7 +16773,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E166:E1048576 E95:E96 E126:E129 E98:E103 E123:E124 E105:E110 E112:E121">
+  <conditionalFormatting sqref="E1:E73 E167:E1048576 E95:E96 E127:E130 E98:E103 E124:E125 E105:E110 E112:E122">
     <cfRule type="cellIs" dxfId="128" priority="223" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16783,7 +16867,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I130:I138">
+  <conditionalFormatting sqref="I131:I139">
     <cfRule type="dataBar" priority="127">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16797,12 +16881,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L130:BO138">
+  <conditionalFormatting sqref="L131:BO139">
     <cfRule type="expression" dxfId="106" priority="126">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E130:E138">
+  <conditionalFormatting sqref="E131:E139">
     <cfRule type="cellIs" dxfId="105" priority="119" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16825,7 +16909,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L133:BO138 L126:BO129 L98:BO103 L123:BO124 L105:BO110 L112:BO121">
+  <conditionalFormatting sqref="L134:BO139 L127:BO130 L98:BO103 L124:BO125 L105:BO110 L112:BO122">
     <cfRule type="expression" dxfId="98" priority="130">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16833,7 +16917,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I139:I147">
+  <conditionalFormatting sqref="I140:I148">
     <cfRule type="dataBar" priority="114">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16847,12 +16931,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L139:BO147">
+  <conditionalFormatting sqref="L140:BO148">
     <cfRule type="expression" dxfId="96" priority="113">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E139:E147">
+  <conditionalFormatting sqref="E140:E148">
     <cfRule type="cellIs" dxfId="95" priority="106" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16875,7 +16959,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L142:BO147">
+  <conditionalFormatting sqref="L143:BO148">
     <cfRule type="expression" dxfId="88" priority="117">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16883,7 +16967,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I148:I156">
+  <conditionalFormatting sqref="I149:I157">
     <cfRule type="dataBar" priority="101">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16897,12 +16981,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L148:BO156">
+  <conditionalFormatting sqref="L149:BO157">
     <cfRule type="expression" dxfId="86" priority="100">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E148:E156">
+  <conditionalFormatting sqref="E149:E157">
     <cfRule type="cellIs" dxfId="85" priority="93" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16925,7 +17009,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L151:BO156">
+  <conditionalFormatting sqref="L152:BO157">
     <cfRule type="expression" dxfId="78" priority="104">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16933,7 +17017,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I157:I165">
+  <conditionalFormatting sqref="I158:I166">
     <cfRule type="dataBar" priority="88">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16947,12 +17031,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L157:BO165">
+  <conditionalFormatting sqref="L158:BO166">
     <cfRule type="expression" dxfId="76" priority="87">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E157:E165">
+  <conditionalFormatting sqref="E158:E166">
     <cfRule type="cellIs" dxfId="75" priority="80" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16975,7 +17059,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L160:BO165">
+  <conditionalFormatting sqref="L161:BO166">
     <cfRule type="expression" dxfId="68" priority="91">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17125,7 +17209,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I125">
+  <conditionalFormatting sqref="I126">
     <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17139,12 +17223,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L125:BO125">
+  <conditionalFormatting sqref="L126:BO126">
     <cfRule type="expression" dxfId="38" priority="41">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E125">
+  <conditionalFormatting sqref="E126">
     <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17167,7 +17251,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122">
+  <conditionalFormatting sqref="I123">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17181,12 +17265,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L122:BO122">
+  <conditionalFormatting sqref="L123:BO123">
     <cfRule type="expression" dxfId="30" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E122">
+  <conditionalFormatting sqref="E123">
     <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17365,7 +17449,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I126:I129 I98:I103 I105:I110 I123:I124 I112:I121</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I127:I130 I98:I103 I105:I110 I124:I125 I112:I122</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17395,7 +17479,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I130:I138</xm:sqref>
+          <xm:sqref>I131:I139</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -17410,7 +17494,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I139:I147</xm:sqref>
+          <xm:sqref>I140:I148</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -17425,7 +17509,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I148:I156</xm:sqref>
+          <xm:sqref>I149:I157</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -17440,7 +17524,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I157:I165</xm:sqref>
+          <xm:sqref>I158:I166</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -17500,7 +17584,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I125</xm:sqref>
+          <xm:sqref>I126</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
@@ -17515,7 +17599,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I122</xm:sqref>
+          <xm:sqref>I123</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Added monthly interpolation of quarterly CSM covariates (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECAD157B-346D-4634-80D8-6C827AFDEA4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C03590A-A77F-4177-8311-F0B619E9BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -1809,6 +1809,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1818,6 +1825,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1826,17 +1837,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -2990,7 +2990,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="25"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="27"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3401,7 +3401,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F117" sqref="F117"/>
+      <selection pane="bottomLeft" activeCell="F123" sqref="F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3431,27 +3431,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3496,198 +3496,198 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 25</v>
-      </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+        <v>Week 27</v>
+      </c>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 26</v>
-      </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+        <v>Week 28</v>
+      </c>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 27</v>
-      </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+        <v>Week 29</v>
+      </c>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 28</v>
-      </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+        <v>Week 30</v>
+      </c>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 29</v>
-      </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+        <v>Week 31</v>
+      </c>
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 30</v>
-      </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+        <v>Week 32</v>
+      </c>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 31</v>
-      </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+        <v>Week 33</v>
+      </c>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 32</v>
-      </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+        <v>Week 34</v>
+      </c>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
-        <v>44361</v>
-      </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+        <v>44375</v>
+      </c>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
-        <v>44368</v>
-      </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+        <v>44382</v>
+      </c>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
-        <v>44375</v>
-      </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+        <v>44389</v>
+      </c>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
-        <v>44382</v>
-      </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+        <v>44396</v>
+      </c>
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
-        <v>44389</v>
-      </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+        <v>44403</v>
+      </c>
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
-        <v>44396</v>
-      </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+        <v>44410</v>
+      </c>
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
-        <v>44403</v>
-      </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+        <v>44417</v>
+      </c>
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
-        <v>44410</v>
-      </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+        <v>44424</v>
+      </c>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -3703,227 +3703,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44361</v>
+        <v>44375</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44362</v>
+        <v>44376</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44363</v>
+        <v>44377</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44364</v>
+        <v>44378</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44365</v>
+        <v>44379</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44366</v>
+        <v>44380</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44367</v>
+        <v>44381</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44368</v>
+        <v>44382</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44369</v>
+        <v>44383</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44370</v>
+        <v>44384</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44371</v>
+        <v>44385</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44372</v>
+        <v>44386</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44373</v>
+        <v>44387</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44374</v>
+        <v>44388</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44375</v>
+        <v>44389</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44376</v>
+        <v>44390</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44377</v>
+        <v>44391</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44378</v>
+        <v>44392</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44379</v>
+        <v>44393</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44380</v>
+        <v>44394</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44381</v>
+        <v>44395</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44382</v>
+        <v>44396</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44383</v>
+        <v>44397</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44384</v>
+        <v>44398</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44385</v>
+        <v>44399</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44386</v>
+        <v>44400</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44387</v>
+        <v>44401</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44388</v>
+        <v>44402</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44389</v>
+        <v>44403</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44390</v>
+        <v>44404</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44391</v>
+        <v>44405</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44392</v>
+        <v>44406</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44393</v>
+        <v>44407</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44394</v>
+        <v>44408</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44395</v>
+        <v>44409</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44396</v>
+        <v>44410</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44397</v>
+        <v>44411</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44398</v>
+        <v>44412</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44399</v>
+        <v>44413</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44400</v>
+        <v>44414</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44401</v>
+        <v>44415</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44402</v>
+        <v>44416</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44403</v>
+        <v>44417</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44404</v>
+        <v>44418</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44405</v>
+        <v>44419</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44406</v>
+        <v>44420</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44407</v>
+        <v>44421</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44408</v>
+        <v>44422</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44409</v>
+        <v>44423</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44410</v>
+        <v>44424</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44411</v>
+        <v>44425</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44412</v>
+        <v>44426</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44413</v>
+        <v>44427</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44414</v>
+        <v>44428</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44415</v>
+        <v>44429</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44416</v>
+        <v>44430</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -12851,11 +12851,11 @@
         <v>44405</v>
       </c>
       <c r="G113" s="43">
-        <v>44407</v>
+        <v>44409</v>
       </c>
       <c r="H113" s="73"/>
       <c r="I113" s="26">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J113" s="75"/>
       <c r="K113" s="76"/>
@@ -12932,7 +12932,7 @@
         <v>44406</v>
       </c>
       <c r="G114" s="43">
-        <v>44407</v>
+        <v>44409</v>
       </c>
       <c r="H114" s="73"/>
       <c r="I114" s="26">
@@ -13010,10 +13010,10 @@
         <v>67</v>
       </c>
       <c r="F115" s="42">
-        <v>44407</v>
+        <v>44410</v>
       </c>
       <c r="G115" s="43">
-        <v>44408</v>
+        <v>44411</v>
       </c>
       <c r="H115" s="73"/>
       <c r="I115" s="26">
@@ -13091,10 +13091,10 @@
         <v>68</v>
       </c>
       <c r="F116" s="42">
-        <v>44408</v>
+        <v>44410</v>
       </c>
       <c r="G116" s="43">
-        <v>44409</v>
+        <v>44411</v>
       </c>
       <c r="H116" s="73"/>
       <c r="I116" s="26">
@@ -13172,10 +13172,10 @@
         <v>67</v>
       </c>
       <c r="F117" s="42">
-        <v>44408</v>
+        <v>44410</v>
       </c>
       <c r="G117" s="43">
-        <v>44409</v>
+        <v>44412</v>
       </c>
       <c r="H117" s="73"/>
       <c r="I117" s="26"/>
@@ -13251,10 +13251,10 @@
         <v>70</v>
       </c>
       <c r="F118" s="42">
-        <v>44408</v>
+        <v>44410</v>
       </c>
       <c r="G118" s="43">
-        <v>44409</v>
+        <v>44412</v>
       </c>
       <c r="H118" s="73"/>
       <c r="I118" s="26"/>
@@ -13330,10 +13330,10 @@
         <v>67</v>
       </c>
       <c r="F119" s="42">
-        <v>44409</v>
+        <v>44413</v>
       </c>
       <c r="G119" s="43">
-        <v>44409</v>
+        <v>44412</v>
       </c>
       <c r="H119" s="73"/>
       <c r="I119" s="26">
@@ -13411,7 +13411,7 @@
         <v>67</v>
       </c>
       <c r="F120" s="42">
-        <v>44410</v>
+        <v>44413</v>
       </c>
       <c r="G120" s="43">
         <v>44414</v>
@@ -13490,7 +13490,7 @@
         <v>67</v>
       </c>
       <c r="F121" s="42">
-        <v>44410</v>
+        <v>44413</v>
       </c>
       <c r="G121" s="43">
         <v>44414</v>
@@ -13569,7 +13569,7 @@
         <v>70</v>
       </c>
       <c r="F122" s="71">
-        <v>44410</v>
+        <v>44413</v>
       </c>
       <c r="G122" s="72">
         <v>44414</v>
@@ -16715,15 +16715,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16734,6 +16725,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I127:I130 I98:I103 I105:I110 I124:I125 I112:I122">

</xml_diff>

<commit_message>
Removed some junk files and updated PM (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C03590A-A77F-4177-8311-F0B619E9BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9660502-D6C0-4F72-AF6B-0467C2981624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="154">
   <si>
     <t>WBS</t>
   </si>
@@ -881,6 +881,15 @@
   </si>
   <si>
     <t>Nowcast Model Stacking - Reduce Variance</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>CSM Transformations</t>
+  </si>
+  <si>
+    <t>CSM Equation Fixing</t>
   </si>
 </sst>
 </file>
@@ -1809,13 +1818,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1825,10 +1827,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1837,6 +1835,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3397,11 +3406,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO166"/>
+  <dimension ref="A1:BO168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F123" sqref="F123"/>
+      <selection pane="bottomLeft" activeCell="I117" sqref="I117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3431,27 +3440,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3496,12 +3505,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3511,183 +3520,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 27</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 28</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 29</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 30</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 31</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 32</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 33</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 34</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44375</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44382</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44389</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44396</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44403</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44410</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44417</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44424</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8845,7 +8854,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A131" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A133" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -13003,7 +13012,7 @@
         <v>11.4</v>
       </c>
       <c r="B115" s="65" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D115" s="70"/>
       <c r="E115" s="66" t="s">
@@ -13013,11 +13022,11 @@
         <v>44410</v>
       </c>
       <c r="G115" s="43">
-        <v>44411</v>
+        <v>44419</v>
       </c>
       <c r="H115" s="73"/>
       <c r="I115" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J115" s="75"/>
       <c r="K115" s="76"/>
@@ -13084,22 +13093,20 @@
         <v>11.5</v>
       </c>
       <c r="B116" s="65" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D116" s="70"/>
       <c r="E116" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F116" s="42">
-        <v>44410</v>
+        <v>44419</v>
       </c>
       <c r="G116" s="43">
-        <v>44411</v>
+        <v>44420</v>
       </c>
       <c r="H116" s="73"/>
-      <c r="I116" s="26">
-        <v>0</v>
-      </c>
+      <c r="I116" s="26"/>
       <c r="J116" s="75"/>
       <c r="K116" s="76"/>
       <c r="L116" s="46"/>
@@ -13165,20 +13172,22 @@
         <v>11.6</v>
       </c>
       <c r="B117" s="65" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D117" s="70"/>
       <c r="E117" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F117" s="42">
-        <v>44410</v>
+        <v>44420</v>
       </c>
       <c r="G117" s="43">
-        <v>44412</v>
+        <v>44423</v>
       </c>
       <c r="H117" s="73"/>
-      <c r="I117" s="26"/>
+      <c r="I117" s="26" t="s">
+        <v>151</v>
+      </c>
       <c r="J117" s="75"/>
       <c r="K117" s="76"/>
       <c r="L117" s="46"/>
@@ -13244,20 +13253,22 @@
         <v>11.7</v>
       </c>
       <c r="B118" s="65" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="D118" s="70"/>
       <c r="E118" s="66" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F118" s="42">
-        <v>44410</v>
+        <v>44420</v>
       </c>
       <c r="G118" s="43">
-        <v>44412</v>
+        <v>44423</v>
       </c>
       <c r="H118" s="73"/>
-      <c r="I118" s="26"/>
+      <c r="I118" s="26">
+        <v>0</v>
+      </c>
       <c r="J118" s="75"/>
       <c r="K118" s="76"/>
       <c r="L118" s="46"/>
@@ -13323,22 +13334,20 @@
         <v>11.8</v>
       </c>
       <c r="B119" s="65" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="D119" s="70"/>
       <c r="E119" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F119" s="42">
-        <v>44413</v>
+        <v>44423</v>
       </c>
       <c r="G119" s="43">
-        <v>44412</v>
+        <v>44428</v>
       </c>
       <c r="H119" s="73"/>
-      <c r="I119" s="26">
-        <v>0.3</v>
-      </c>
+      <c r="I119" s="26"/>
       <c r="J119" s="75"/>
       <c r="K119" s="76"/>
       <c r="L119" s="46"/>
@@ -13404,17 +13413,17 @@
         <v>11.9</v>
       </c>
       <c r="B120" s="65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D120" s="70"/>
       <c r="E120" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F120" s="42">
-        <v>44413</v>
+        <v>44428</v>
       </c>
       <c r="G120" s="43">
-        <v>44414</v>
+        <v>44433</v>
       </c>
       <c r="H120" s="73"/>
       <c r="I120" s="26"/>
@@ -13483,20 +13492,22 @@
         <v>11.10</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D121" s="70"/>
       <c r="E121" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F121" s="42">
-        <v>44413</v>
+        <v>44428</v>
       </c>
       <c r="G121" s="43">
-        <v>44414</v>
+        <v>44433</v>
       </c>
       <c r="H121" s="73"/>
-      <c r="I121" s="26"/>
+      <c r="I121" s="26">
+        <v>0.3</v>
+      </c>
       <c r="J121" s="75"/>
       <c r="K121" s="76"/>
       <c r="L121" s="46"/>
@@ -13562,20 +13573,20 @@
         <v>11.11</v>
       </c>
       <c r="B122" s="65" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D122" s="70"/>
-      <c r="E122" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F122" s="71">
-        <v>44413</v>
-      </c>
-      <c r="G122" s="72">
-        <v>44414</v>
+      <c r="E122" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F122" s="42">
+        <v>44428</v>
+      </c>
+      <c r="G122" s="43">
+        <v>44433</v>
       </c>
       <c r="H122" s="73"/>
-      <c r="I122" s="74"/>
+      <c r="I122" s="26"/>
       <c r="J122" s="75"/>
       <c r="K122" s="76"/>
       <c r="L122" s="46"/>
@@ -13635,103 +13646,105 @@
       <c r="BN122" s="46"/>
       <c r="BO122" s="46"/>
     </row>
-    <row r="123" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>12</v>
-      </c>
-      <c r="B123" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="D123" s="19"/>
-      <c r="E123" s="19"/>
-      <c r="F123" s="44"/>
-      <c r="G123" s="44" t="str">
-        <f t="shared" ref="G123" si="22">IF(ISBLANK(F123)," - ",IF(H123=0,F123,F123+H123-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H123" s="20"/>
-      <c r="I123" s="21"/>
-      <c r="J123" s="22" t="str">
-        <f t="shared" ref="J123" si="23">IF(OR(G123=0,F123=0)," - ",NETWORKDAYS(F123,G123))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K123" s="41"/>
-      <c r="L123" s="48"/>
-      <c r="M123" s="48"/>
-      <c r="N123" s="48"/>
-      <c r="O123" s="48"/>
-      <c r="P123" s="48"/>
-      <c r="Q123" s="48"/>
-      <c r="R123" s="48"/>
-      <c r="S123" s="48"/>
-      <c r="T123" s="48"/>
-      <c r="U123" s="48"/>
-      <c r="V123" s="48"/>
-      <c r="W123" s="48"/>
-      <c r="X123" s="48"/>
-      <c r="Y123" s="48"/>
-      <c r="Z123" s="48"/>
-      <c r="AA123" s="48"/>
-      <c r="AB123" s="48"/>
-      <c r="AC123" s="48"/>
-      <c r="AD123" s="48"/>
-      <c r="AE123" s="48"/>
-      <c r="AF123" s="48"/>
-      <c r="AG123" s="48"/>
-      <c r="AH123" s="48"/>
-      <c r="AI123" s="48"/>
-      <c r="AJ123" s="48"/>
-      <c r="AK123" s="48"/>
-      <c r="AL123" s="48"/>
-      <c r="AM123" s="48"/>
-      <c r="AN123" s="48"/>
-      <c r="AO123" s="48"/>
-      <c r="AP123" s="48"/>
-      <c r="AQ123" s="48"/>
-      <c r="AR123" s="48"/>
-      <c r="AS123" s="48"/>
-      <c r="AT123" s="48"/>
-      <c r="AU123" s="48"/>
-      <c r="AV123" s="48"/>
-      <c r="AW123" s="48"/>
-      <c r="AX123" s="48"/>
-      <c r="AY123" s="48"/>
-      <c r="AZ123" s="48"/>
-      <c r="BA123" s="48"/>
-      <c r="BB123" s="48"/>
-      <c r="BC123" s="48"/>
-      <c r="BD123" s="48"/>
-      <c r="BE123" s="48"/>
-      <c r="BF123" s="48"/>
-      <c r="BG123" s="48"/>
-      <c r="BH123" s="48"/>
-      <c r="BI123" s="48"/>
-      <c r="BJ123" s="48"/>
-      <c r="BK123" s="48"/>
-      <c r="BL123" s="48"/>
-      <c r="BM123" s="48"/>
-      <c r="BN123" s="48"/>
-      <c r="BO123" s="48"/>
+    <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.12</v>
+      </c>
+      <c r="B123" s="65" t="s">
+        <v>146</v>
+      </c>
+      <c r="D123" s="70"/>
+      <c r="E123" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F123" s="42">
+        <v>44428</v>
+      </c>
+      <c r="G123" s="43">
+        <v>44433</v>
+      </c>
+      <c r="H123" s="73"/>
+      <c r="I123" s="26"/>
+      <c r="J123" s="75"/>
+      <c r="K123" s="76"/>
+      <c r="L123" s="46"/>
+      <c r="M123" s="46"/>
+      <c r="N123" s="46"/>
+      <c r="O123" s="46"/>
+      <c r="P123" s="46"/>
+      <c r="Q123" s="46"/>
+      <c r="R123" s="46"/>
+      <c r="S123" s="46"/>
+      <c r="T123" s="46"/>
+      <c r="U123" s="46"/>
+      <c r="V123" s="46"/>
+      <c r="W123" s="46"/>
+      <c r="X123" s="46"/>
+      <c r="Y123" s="46"/>
+      <c r="Z123" s="46"/>
+      <c r="AA123" s="46"/>
+      <c r="AB123" s="46"/>
+      <c r="AC123" s="46"/>
+      <c r="AD123" s="46"/>
+      <c r="AE123" s="46"/>
+      <c r="AF123" s="46"/>
+      <c r="AG123" s="46"/>
+      <c r="AH123" s="46"/>
+      <c r="AI123" s="46"/>
+      <c r="AJ123" s="46"/>
+      <c r="AK123" s="46"/>
+      <c r="AL123" s="46"/>
+      <c r="AM123" s="46"/>
+      <c r="AN123" s="46"/>
+      <c r="AO123" s="46"/>
+      <c r="AP123" s="46"/>
+      <c r="AQ123" s="46"/>
+      <c r="AR123" s="46"/>
+      <c r="AS123" s="46"/>
+      <c r="AT123" s="46"/>
+      <c r="AU123" s="46"/>
+      <c r="AV123" s="46"/>
+      <c r="AW123" s="46"/>
+      <c r="AX123" s="46"/>
+      <c r="AY123" s="46"/>
+      <c r="AZ123" s="46"/>
+      <c r="BA123" s="46"/>
+      <c r="BB123" s="46"/>
+      <c r="BC123" s="46"/>
+      <c r="BD123" s="46"/>
+      <c r="BE123" s="46"/>
+      <c r="BF123" s="46"/>
+      <c r="BG123" s="46"/>
+      <c r="BH123" s="46"/>
+      <c r="BI123" s="46"/>
+      <c r="BJ123" s="46"/>
+      <c r="BK123" s="46"/>
+      <c r="BL123" s="46"/>
+      <c r="BM123" s="46"/>
+      <c r="BN123" s="46"/>
+      <c r="BO123" s="46"/>
     </row>
     <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.1</v>
+        <v>11.13</v>
       </c>
       <c r="B124" s="65" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="D124" s="70"/>
-      <c r="E124" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F124" s="42">
-        <v>44392</v>
-      </c>
-      <c r="G124" s="43"/>
+      <c r="E124" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F124" s="71">
+        <v>44428</v>
+      </c>
+      <c r="G124" s="72">
+        <v>44433</v>
+      </c>
       <c r="H124" s="73"/>
-      <c r="I124" s="26"/>
+      <c r="I124" s="74"/>
       <c r="J124" s="75"/>
       <c r="K124" s="76"/>
       <c r="L124" s="46"/>
@@ -13791,182 +13804,182 @@
       <c r="BN124" s="46"/>
       <c r="BO124" s="46"/>
     </row>
-    <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125" s="23" t="str">
+    <row r="125" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>12</v>
+      </c>
+      <c r="B125" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="D125" s="19"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="44"/>
+      <c r="G125" s="44" t="str">
+        <f t="shared" ref="G125" si="22">IF(ISBLANK(F125)," - ",IF(H125=0,F125,F125+H125-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H125" s="20"/>
+      <c r="I125" s="21"/>
+      <c r="J125" s="22" t="str">
+        <f t="shared" ref="J125" si="23">IF(OR(G125=0,F125=0)," - ",NETWORKDAYS(F125,G125))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K125" s="41"/>
+      <c r="L125" s="48"/>
+      <c r="M125" s="48"/>
+      <c r="N125" s="48"/>
+      <c r="O125" s="48"/>
+      <c r="P125" s="48"/>
+      <c r="Q125" s="48"/>
+      <c r="R125" s="48"/>
+      <c r="S125" s="48"/>
+      <c r="T125" s="48"/>
+      <c r="U125" s="48"/>
+      <c r="V125" s="48"/>
+      <c r="W125" s="48"/>
+      <c r="X125" s="48"/>
+      <c r="Y125" s="48"/>
+      <c r="Z125" s="48"/>
+      <c r="AA125" s="48"/>
+      <c r="AB125" s="48"/>
+      <c r="AC125" s="48"/>
+      <c r="AD125" s="48"/>
+      <c r="AE125" s="48"/>
+      <c r="AF125" s="48"/>
+      <c r="AG125" s="48"/>
+      <c r="AH125" s="48"/>
+      <c r="AI125" s="48"/>
+      <c r="AJ125" s="48"/>
+      <c r="AK125" s="48"/>
+      <c r="AL125" s="48"/>
+      <c r="AM125" s="48"/>
+      <c r="AN125" s="48"/>
+      <c r="AO125" s="48"/>
+      <c r="AP125" s="48"/>
+      <c r="AQ125" s="48"/>
+      <c r="AR125" s="48"/>
+      <c r="AS125" s="48"/>
+      <c r="AT125" s="48"/>
+      <c r="AU125" s="48"/>
+      <c r="AV125" s="48"/>
+      <c r="AW125" s="48"/>
+      <c r="AX125" s="48"/>
+      <c r="AY125" s="48"/>
+      <c r="AZ125" s="48"/>
+      <c r="BA125" s="48"/>
+      <c r="BB125" s="48"/>
+      <c r="BC125" s="48"/>
+      <c r="BD125" s="48"/>
+      <c r="BE125" s="48"/>
+      <c r="BF125" s="48"/>
+      <c r="BG125" s="48"/>
+      <c r="BH125" s="48"/>
+      <c r="BI125" s="48"/>
+      <c r="BJ125" s="48"/>
+      <c r="BK125" s="48"/>
+      <c r="BL125" s="48"/>
+      <c r="BM125" s="48"/>
+      <c r="BN125" s="48"/>
+      <c r="BO125" s="48"/>
+    </row>
+    <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
-      </c>
-      <c r="B125" s="65" t="s">
-        <v>128</v>
-      </c>
-      <c r="D125" s="70"/>
-      <c r="E125" s="70" t="s">
+        <v>12.1</v>
+      </c>
+      <c r="B126" s="65" t="s">
+        <v>127</v>
+      </c>
+      <c r="D126" s="70"/>
+      <c r="E126" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F125" s="42">
+      <c r="F126" s="42">
         <v>44392</v>
       </c>
-      <c r="G125" s="43"/>
-      <c r="H125" s="73"/>
-      <c r="I125" s="74"/>
-      <c r="J125" s="75"/>
-      <c r="K125" s="76"/>
-      <c r="L125" s="46"/>
-      <c r="M125" s="46"/>
-      <c r="N125" s="46"/>
-      <c r="O125" s="46"/>
-      <c r="P125" s="46"/>
-      <c r="Q125" s="46"/>
-      <c r="R125" s="46"/>
-      <c r="S125" s="46"/>
-      <c r="T125" s="46"/>
-      <c r="U125" s="46"/>
-      <c r="V125" s="46"/>
-      <c r="W125" s="46"/>
-      <c r="X125" s="46"/>
-      <c r="Y125" s="46"/>
-      <c r="Z125" s="46"/>
-      <c r="AA125" s="46"/>
-      <c r="AB125" s="46"/>
-      <c r="AC125" s="46"/>
-      <c r="AD125" s="46"/>
-      <c r="AE125" s="46"/>
-      <c r="AF125" s="46"/>
-      <c r="AG125" s="46"/>
-      <c r="AH125" s="46"/>
-      <c r="AI125" s="46"/>
-      <c r="AJ125" s="46"/>
-      <c r="AK125" s="46"/>
-      <c r="AL125" s="46"/>
-      <c r="AM125" s="46"/>
-      <c r="AN125" s="46"/>
-      <c r="AO125" s="46"/>
-      <c r="AP125" s="46"/>
-      <c r="AQ125" s="46"/>
-      <c r="AR125" s="46"/>
-      <c r="AS125" s="46"/>
-      <c r="AT125" s="46"/>
-      <c r="AU125" s="46"/>
-      <c r="AV125" s="46"/>
-      <c r="AW125" s="46"/>
-      <c r="AX125" s="46"/>
-      <c r="AY125" s="46"/>
-      <c r="AZ125" s="46"/>
-      <c r="BA125" s="46"/>
-      <c r="BB125" s="46"/>
-      <c r="BC125" s="46"/>
-      <c r="BD125" s="46"/>
-      <c r="BE125" s="46"/>
-      <c r="BF125" s="46"/>
-      <c r="BG125" s="46"/>
-      <c r="BH125" s="46"/>
-      <c r="BI125" s="46"/>
-      <c r="BJ125" s="46"/>
-      <c r="BK125" s="46"/>
-      <c r="BL125" s="46"/>
-      <c r="BM125" s="46"/>
-      <c r="BN125" s="46"/>
-      <c r="BO125" s="46"/>
-    </row>
-    <row r="126" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>13</v>
-      </c>
-      <c r="B126" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D126" s="19"/>
-      <c r="E126" s="19"/>
-      <c r="F126" s="44"/>
-      <c r="G126" s="44" t="str">
-        <f t="shared" ref="G126" si="24">IF(ISBLANK(F126)," - ",IF(H126=0,F126,F126+H126-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H126" s="20"/>
-      <c r="I126" s="21"/>
-      <c r="J126" s="22" t="str">
-        <f t="shared" ref="J126" si="25">IF(OR(G126=0,F126=0)," - ",NETWORKDAYS(F126,G126))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K126" s="41"/>
-      <c r="L126" s="48"/>
-      <c r="M126" s="48"/>
-      <c r="N126" s="48"/>
-      <c r="O126" s="48"/>
-      <c r="P126" s="48"/>
-      <c r="Q126" s="48"/>
-      <c r="R126" s="48"/>
-      <c r="S126" s="48"/>
-      <c r="T126" s="48"/>
-      <c r="U126" s="48"/>
-      <c r="V126" s="48"/>
-      <c r="W126" s="48"/>
-      <c r="X126" s="48"/>
-      <c r="Y126" s="48"/>
-      <c r="Z126" s="48"/>
-      <c r="AA126" s="48"/>
-      <c r="AB126" s="48"/>
-      <c r="AC126" s="48"/>
-      <c r="AD126" s="48"/>
-      <c r="AE126" s="48"/>
-      <c r="AF126" s="48"/>
-      <c r="AG126" s="48"/>
-      <c r="AH126" s="48"/>
-      <c r="AI126" s="48"/>
-      <c r="AJ126" s="48"/>
-      <c r="AK126" s="48"/>
-      <c r="AL126" s="48"/>
-      <c r="AM126" s="48"/>
-      <c r="AN126" s="48"/>
-      <c r="AO126" s="48"/>
-      <c r="AP126" s="48"/>
-      <c r="AQ126" s="48"/>
-      <c r="AR126" s="48"/>
-      <c r="AS126" s="48"/>
-      <c r="AT126" s="48"/>
-      <c r="AU126" s="48"/>
-      <c r="AV126" s="48"/>
-      <c r="AW126" s="48"/>
-      <c r="AX126" s="48"/>
-      <c r="AY126" s="48"/>
-      <c r="AZ126" s="48"/>
-      <c r="BA126" s="48"/>
-      <c r="BB126" s="48"/>
-      <c r="BC126" s="48"/>
-      <c r="BD126" s="48"/>
-      <c r="BE126" s="48"/>
-      <c r="BF126" s="48"/>
-      <c r="BG126" s="48"/>
-      <c r="BH126" s="48"/>
-      <c r="BI126" s="48"/>
-      <c r="BJ126" s="48"/>
-      <c r="BK126" s="48"/>
-      <c r="BL126" s="48"/>
-      <c r="BM126" s="48"/>
-      <c r="BN126" s="48"/>
-      <c r="BO126" s="48"/>
+      <c r="G126" s="43"/>
+      <c r="H126" s="73"/>
+      <c r="I126" s="26"/>
+      <c r="J126" s="75"/>
+      <c r="K126" s="76"/>
+      <c r="L126" s="46"/>
+      <c r="M126" s="46"/>
+      <c r="N126" s="46"/>
+      <c r="O126" s="46"/>
+      <c r="P126" s="46"/>
+      <c r="Q126" s="46"/>
+      <c r="R126" s="46"/>
+      <c r="S126" s="46"/>
+      <c r="T126" s="46"/>
+      <c r="U126" s="46"/>
+      <c r="V126" s="46"/>
+      <c r="W126" s="46"/>
+      <c r="X126" s="46"/>
+      <c r="Y126" s="46"/>
+      <c r="Z126" s="46"/>
+      <c r="AA126" s="46"/>
+      <c r="AB126" s="46"/>
+      <c r="AC126" s="46"/>
+      <c r="AD126" s="46"/>
+      <c r="AE126" s="46"/>
+      <c r="AF126" s="46"/>
+      <c r="AG126" s="46"/>
+      <c r="AH126" s="46"/>
+      <c r="AI126" s="46"/>
+      <c r="AJ126" s="46"/>
+      <c r="AK126" s="46"/>
+      <c r="AL126" s="46"/>
+      <c r="AM126" s="46"/>
+      <c r="AN126" s="46"/>
+      <c r="AO126" s="46"/>
+      <c r="AP126" s="46"/>
+      <c r="AQ126" s="46"/>
+      <c r="AR126" s="46"/>
+      <c r="AS126" s="46"/>
+      <c r="AT126" s="46"/>
+      <c r="AU126" s="46"/>
+      <c r="AV126" s="46"/>
+      <c r="AW126" s="46"/>
+      <c r="AX126" s="46"/>
+      <c r="AY126" s="46"/>
+      <c r="AZ126" s="46"/>
+      <c r="BA126" s="46"/>
+      <c r="BB126" s="46"/>
+      <c r="BC126" s="46"/>
+      <c r="BD126" s="46"/>
+      <c r="BE126" s="46"/>
+      <c r="BF126" s="46"/>
+      <c r="BG126" s="46"/>
+      <c r="BH126" s="46"/>
+      <c r="BI126" s="46"/>
+      <c r="BJ126" s="46"/>
+      <c r="BK126" s="46"/>
+      <c r="BL126" s="46"/>
+      <c r="BM126" s="46"/>
+      <c r="BN126" s="46"/>
+      <c r="BO126" s="46"/>
     </row>
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.1</v>
+        <v>12.2</v>
       </c>
       <c r="B127" s="65" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="D127" s="70"/>
-      <c r="E127" s="66" t="s">
-        <v>69</v>
+      <c r="E127" s="70" t="s">
+        <v>67</v>
       </c>
       <c r="F127" s="42">
-        <v>44379</v>
+        <v>44392</v>
       </c>
       <c r="G127" s="43"/>
-      <c r="H127" s="25"/>
-      <c r="I127" s="26"/>
-      <c r="J127" s="27"/>
-      <c r="K127" s="40"/>
+      <c r="H127" s="73"/>
+      <c r="I127" s="74"/>
+      <c r="J127" s="75"/>
+      <c r="K127" s="76"/>
       <c r="L127" s="46"/>
       <c r="M127" s="46"/>
       <c r="N127" s="46"/>
@@ -14024,94 +14037,96 @@
       <c r="BN127" s="46"/>
       <c r="BO127" s="46"/>
     </row>
-    <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.2</v>
-      </c>
-      <c r="B128" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D128" s="70"/>
-      <c r="E128" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F128" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G128" s="43"/>
-      <c r="H128" s="25"/>
-      <c r="I128" s="26"/>
-      <c r="J128" s="27"/>
-      <c r="K128" s="40"/>
-      <c r="L128" s="46"/>
-      <c r="M128" s="46"/>
-      <c r="N128" s="46"/>
-      <c r="O128" s="46"/>
-      <c r="P128" s="46"/>
-      <c r="Q128" s="46"/>
-      <c r="R128" s="46"/>
-      <c r="S128" s="46"/>
-      <c r="T128" s="46"/>
-      <c r="U128" s="46"/>
-      <c r="V128" s="46"/>
-      <c r="W128" s="46"/>
-      <c r="X128" s="46"/>
-      <c r="Y128" s="46"/>
-      <c r="Z128" s="46"/>
-      <c r="AA128" s="46"/>
-      <c r="AB128" s="46"/>
-      <c r="AC128" s="46"/>
-      <c r="AD128" s="46"/>
-      <c r="AE128" s="46"/>
-      <c r="AF128" s="46"/>
-      <c r="AG128" s="46"/>
-      <c r="AH128" s="46"/>
-      <c r="AI128" s="46"/>
-      <c r="AJ128" s="46"/>
-      <c r="AK128" s="46"/>
-      <c r="AL128" s="46"/>
-      <c r="AM128" s="46"/>
-      <c r="AN128" s="46"/>
-      <c r="AO128" s="46"/>
-      <c r="AP128" s="46"/>
-      <c r="AQ128" s="46"/>
-      <c r="AR128" s="46"/>
-      <c r="AS128" s="46"/>
-      <c r="AT128" s="46"/>
-      <c r="AU128" s="46"/>
-      <c r="AV128" s="46"/>
-      <c r="AW128" s="46"/>
-      <c r="AX128" s="46"/>
-      <c r="AY128" s="46"/>
-      <c r="AZ128" s="46"/>
-      <c r="BA128" s="46"/>
-      <c r="BB128" s="46"/>
-      <c r="BC128" s="46"/>
-      <c r="BD128" s="46"/>
-      <c r="BE128" s="46"/>
-      <c r="BF128" s="46"/>
-      <c r="BG128" s="46"/>
-      <c r="BH128" s="46"/>
-      <c r="BI128" s="46"/>
-      <c r="BJ128" s="46"/>
-      <c r="BK128" s="46"/>
-      <c r="BL128" s="46"/>
-      <c r="BM128" s="46"/>
-      <c r="BN128" s="46"/>
-      <c r="BO128" s="46"/>
+    <row r="128" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>13</v>
+      </c>
+      <c r="B128" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="44"/>
+      <c r="G128" s="44" t="str">
+        <f t="shared" ref="G128" si="24">IF(ISBLANK(F128)," - ",IF(H128=0,F128,F128+H128-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H128" s="20"/>
+      <c r="I128" s="21"/>
+      <c r="J128" s="22" t="str">
+        <f t="shared" ref="J128" si="25">IF(OR(G128=0,F128=0)," - ",NETWORKDAYS(F128,G128))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K128" s="41"/>
+      <c r="L128" s="48"/>
+      <c r="M128" s="48"/>
+      <c r="N128" s="48"/>
+      <c r="O128" s="48"/>
+      <c r="P128" s="48"/>
+      <c r="Q128" s="48"/>
+      <c r="R128" s="48"/>
+      <c r="S128" s="48"/>
+      <c r="T128" s="48"/>
+      <c r="U128" s="48"/>
+      <c r="V128" s="48"/>
+      <c r="W128" s="48"/>
+      <c r="X128" s="48"/>
+      <c r="Y128" s="48"/>
+      <c r="Z128" s="48"/>
+      <c r="AA128" s="48"/>
+      <c r="AB128" s="48"/>
+      <c r="AC128" s="48"/>
+      <c r="AD128" s="48"/>
+      <c r="AE128" s="48"/>
+      <c r="AF128" s="48"/>
+      <c r="AG128" s="48"/>
+      <c r="AH128" s="48"/>
+      <c r="AI128" s="48"/>
+      <c r="AJ128" s="48"/>
+      <c r="AK128" s="48"/>
+      <c r="AL128" s="48"/>
+      <c r="AM128" s="48"/>
+      <c r="AN128" s="48"/>
+      <c r="AO128" s="48"/>
+      <c r="AP128" s="48"/>
+      <c r="AQ128" s="48"/>
+      <c r="AR128" s="48"/>
+      <c r="AS128" s="48"/>
+      <c r="AT128" s="48"/>
+      <c r="AU128" s="48"/>
+      <c r="AV128" s="48"/>
+      <c r="AW128" s="48"/>
+      <c r="AX128" s="48"/>
+      <c r="AY128" s="48"/>
+      <c r="AZ128" s="48"/>
+      <c r="BA128" s="48"/>
+      <c r="BB128" s="48"/>
+      <c r="BC128" s="48"/>
+      <c r="BD128" s="48"/>
+      <c r="BE128" s="48"/>
+      <c r="BF128" s="48"/>
+      <c r="BG128" s="48"/>
+      <c r="BH128" s="48"/>
+      <c r="BI128" s="48"/>
+      <c r="BJ128" s="48"/>
+      <c r="BK128" s="48"/>
+      <c r="BL128" s="48"/>
+      <c r="BM128" s="48"/>
+      <c r="BN128" s="48"/>
+      <c r="BO128" s="48"/>
     </row>
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.1</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D129" s="70"/>
       <c r="E129" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F129" s="42">
         <v>44379</v>
@@ -14181,14 +14196,14 @@
     <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.2</v>
       </c>
       <c r="B130" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D130" s="70"/>
       <c r="E130" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F130" s="42">
         <v>44379</v>
@@ -14258,17 +14273,17 @@
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B131" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D131" s="66"/>
+        <v>13.3</v>
+      </c>
+      <c r="B131" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D131" s="70"/>
       <c r="E131" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F131" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G131" s="43"/>
       <c r="H131" s="25"/>
@@ -14333,11 +14348,20 @@
       <c r="BO131" s="46"/>
     </row>
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A132" s="23"/>
-      <c r="B132" s="65"/>
-      <c r="D132" s="66"/>
-      <c r="E132" s="66"/>
-      <c r="F132" s="42"/>
+      <c r="A132" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.4</v>
+      </c>
+      <c r="B132" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D132" s="70"/>
+      <c r="E132" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F132" s="42">
+        <v>44379</v>
+      </c>
       <c r="G132" s="43"/>
       <c r="H132" s="25"/>
       <c r="I132" s="26"/>
@@ -14401,11 +14425,20 @@
       <c r="BO132" s="46"/>
     </row>
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="23"/>
-      <c r="B133" s="65"/>
+      <c r="A133" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B133" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D133" s="66"/>
-      <c r="E133" s="66"/>
-      <c r="F133" s="42"/>
+      <c r="E133" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F133" s="42">
+        <v>44531</v>
+      </c>
       <c r="G133" s="43"/>
       <c r="H133" s="25"/>
       <c r="I133" s="26"/>
@@ -14539,7 +14572,7 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23"/>
       <c r="B135" s="65"/>
-      <c r="D135" s="70"/>
+      <c r="D135" s="66"/>
       <c r="E135" s="66"/>
       <c r="F135" s="42"/>
       <c r="G135" s="43"/>
@@ -14607,7 +14640,7 @@
     <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="23"/>
       <c r="B136" s="65"/>
-      <c r="D136" s="70"/>
+      <c r="D136" s="66"/>
       <c r="E136" s="66"/>
       <c r="F136" s="42"/>
       <c r="G136" s="43"/>
@@ -14879,7 +14912,7 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23"/>
       <c r="B140" s="65"/>
-      <c r="D140" s="66"/>
+      <c r="D140" s="70"/>
       <c r="E140" s="66"/>
       <c r="F140" s="42"/>
       <c r="G140" s="43"/>
@@ -14947,7 +14980,7 @@
     <row r="141" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23"/>
       <c r="B141" s="65"/>
-      <c r="D141" s="66"/>
+      <c r="D141" s="70"/>
       <c r="E141" s="66"/>
       <c r="F141" s="42"/>
       <c r="G141" s="43"/>
@@ -15151,7 +15184,7 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23"/>
       <c r="B144" s="65"/>
-      <c r="D144" s="70"/>
+      <c r="D144" s="66"/>
       <c r="E144" s="66"/>
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
@@ -15219,7 +15252,7 @@
     <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23"/>
       <c r="B145" s="65"/>
-      <c r="D145" s="70"/>
+      <c r="D145" s="66"/>
       <c r="E145" s="66"/>
       <c r="F145" s="42"/>
       <c r="G145" s="43"/>
@@ -15491,7 +15524,7 @@
     <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="23"/>
       <c r="B149" s="65"/>
-      <c r="D149" s="66"/>
+      <c r="D149" s="70"/>
       <c r="E149" s="66"/>
       <c r="F149" s="42"/>
       <c r="G149" s="43"/>
@@ -15559,7 +15592,7 @@
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23"/>
       <c r="B150" s="65"/>
-      <c r="D150" s="66"/>
+      <c r="D150" s="70"/>
       <c r="E150" s="66"/>
       <c r="F150" s="42"/>
       <c r="G150" s="43"/>
@@ -15763,7 +15796,7 @@
     <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="23"/>
       <c r="B153" s="65"/>
-      <c r="D153" s="70"/>
+      <c r="D153" s="66"/>
       <c r="E153" s="66"/>
       <c r="F153" s="42"/>
       <c r="G153" s="43"/>
@@ -15831,7 +15864,7 @@
     <row r="154" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="23"/>
       <c r="B154" s="65"/>
-      <c r="D154" s="70"/>
+      <c r="D154" s="66"/>
       <c r="E154" s="66"/>
       <c r="F154" s="42"/>
       <c r="G154" s="43"/>
@@ -16103,7 +16136,7 @@
     <row r="158" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="23"/>
       <c r="B158" s="65"/>
-      <c r="D158" s="66"/>
+      <c r="D158" s="70"/>
       <c r="E158" s="66"/>
       <c r="F158" s="42"/>
       <c r="G158" s="43"/>
@@ -16171,7 +16204,7 @@
     <row r="159" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="23"/>
       <c r="B159" s="65"/>
-      <c r="D159" s="66"/>
+      <c r="D159" s="70"/>
       <c r="E159" s="66"/>
       <c r="F159" s="42"/>
       <c r="G159" s="43"/>
@@ -16375,7 +16408,7 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23"/>
       <c r="B162" s="65"/>
-      <c r="D162" s="70"/>
+      <c r="D162" s="66"/>
       <c r="E162" s="66"/>
       <c r="F162" s="42"/>
       <c r="G162" s="43"/>
@@ -16443,7 +16476,7 @@
     <row r="163" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="23"/>
       <c r="B163" s="65"/>
-      <c r="D163" s="70"/>
+      <c r="D163" s="66"/>
       <c r="E163" s="66"/>
       <c r="F163" s="42"/>
       <c r="G163" s="43"/>
@@ -16712,9 +16745,154 @@
       <c r="BN166" s="46"/>
       <c r="BO166" s="46"/>
     </row>
+    <row r="167" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="23"/>
+      <c r="B167" s="65"/>
+      <c r="D167" s="70"/>
+      <c r="E167" s="66"/>
+      <c r="F167" s="42"/>
+      <c r="G167" s="43"/>
+      <c r="H167" s="25"/>
+      <c r="I167" s="26"/>
+      <c r="J167" s="27"/>
+      <c r="K167" s="40"/>
+      <c r="L167" s="46"/>
+      <c r="M167" s="46"/>
+      <c r="N167" s="46"/>
+      <c r="O167" s="46"/>
+      <c r="P167" s="46"/>
+      <c r="Q167" s="46"/>
+      <c r="R167" s="46"/>
+      <c r="S167" s="46"/>
+      <c r="T167" s="46"/>
+      <c r="U167" s="46"/>
+      <c r="V167" s="46"/>
+      <c r="W167" s="46"/>
+      <c r="X167" s="46"/>
+      <c r="Y167" s="46"/>
+      <c r="Z167" s="46"/>
+      <c r="AA167" s="46"/>
+      <c r="AB167" s="46"/>
+      <c r="AC167" s="46"/>
+      <c r="AD167" s="46"/>
+      <c r="AE167" s="46"/>
+      <c r="AF167" s="46"/>
+      <c r="AG167" s="46"/>
+      <c r="AH167" s="46"/>
+      <c r="AI167" s="46"/>
+      <c r="AJ167" s="46"/>
+      <c r="AK167" s="46"/>
+      <c r="AL167" s="46"/>
+      <c r="AM167" s="46"/>
+      <c r="AN167" s="46"/>
+      <c r="AO167" s="46"/>
+      <c r="AP167" s="46"/>
+      <c r="AQ167" s="46"/>
+      <c r="AR167" s="46"/>
+      <c r="AS167" s="46"/>
+      <c r="AT167" s="46"/>
+      <c r="AU167" s="46"/>
+      <c r="AV167" s="46"/>
+      <c r="AW167" s="46"/>
+      <c r="AX167" s="46"/>
+      <c r="AY167" s="46"/>
+      <c r="AZ167" s="46"/>
+      <c r="BA167" s="46"/>
+      <c r="BB167" s="46"/>
+      <c r="BC167" s="46"/>
+      <c r="BD167" s="46"/>
+      <c r="BE167" s="46"/>
+      <c r="BF167" s="46"/>
+      <c r="BG167" s="46"/>
+      <c r="BH167" s="46"/>
+      <c r="BI167" s="46"/>
+      <c r="BJ167" s="46"/>
+      <c r="BK167" s="46"/>
+      <c r="BL167" s="46"/>
+      <c r="BM167" s="46"/>
+      <c r="BN167" s="46"/>
+      <c r="BO167" s="46"/>
+    </row>
+    <row r="168" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="23"/>
+      <c r="B168" s="65"/>
+      <c r="D168" s="70"/>
+      <c r="E168" s="66"/>
+      <c r="F168" s="42"/>
+      <c r="G168" s="43"/>
+      <c r="H168" s="25"/>
+      <c r="I168" s="26"/>
+      <c r="J168" s="27"/>
+      <c r="K168" s="40"/>
+      <c r="L168" s="46"/>
+      <c r="M168" s="46"/>
+      <c r="N168" s="46"/>
+      <c r="O168" s="46"/>
+      <c r="P168" s="46"/>
+      <c r="Q168" s="46"/>
+      <c r="R168" s="46"/>
+      <c r="S168" s="46"/>
+      <c r="T168" s="46"/>
+      <c r="U168" s="46"/>
+      <c r="V168" s="46"/>
+      <c r="W168" s="46"/>
+      <c r="X168" s="46"/>
+      <c r="Y168" s="46"/>
+      <c r="Z168" s="46"/>
+      <c r="AA168" s="46"/>
+      <c r="AB168" s="46"/>
+      <c r="AC168" s="46"/>
+      <c r="AD168" s="46"/>
+      <c r="AE168" s="46"/>
+      <c r="AF168" s="46"/>
+      <c r="AG168" s="46"/>
+      <c r="AH168" s="46"/>
+      <c r="AI168" s="46"/>
+      <c r="AJ168" s="46"/>
+      <c r="AK168" s="46"/>
+      <c r="AL168" s="46"/>
+      <c r="AM168" s="46"/>
+      <c r="AN168" s="46"/>
+      <c r="AO168" s="46"/>
+      <c r="AP168" s="46"/>
+      <c r="AQ168" s="46"/>
+      <c r="AR168" s="46"/>
+      <c r="AS168" s="46"/>
+      <c r="AT168" s="46"/>
+      <c r="AU168" s="46"/>
+      <c r="AV168" s="46"/>
+      <c r="AW168" s="46"/>
+      <c r="AX168" s="46"/>
+      <c r="AY168" s="46"/>
+      <c r="AZ168" s="46"/>
+      <c r="BA168" s="46"/>
+      <c r="BB168" s="46"/>
+      <c r="BC168" s="46"/>
+      <c r="BD168" s="46"/>
+      <c r="BE168" s="46"/>
+      <c r="BF168" s="46"/>
+      <c r="BG168" s="46"/>
+      <c r="BH168" s="46"/>
+      <c r="BI168" s="46"/>
+      <c r="BJ168" s="46"/>
+      <c r="BK168" s="46"/>
+      <c r="BL168" s="46"/>
+      <c r="BM168" s="46"/>
+      <c r="BN168" s="46"/>
+      <c r="BO168" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -16725,18 +16903,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I127:I130 I98:I103 I105:I110 I124:I125 I112:I122">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I129:I132 I98:I103 I105:I110 I126:I127 I112:I124">
     <cfRule type="dataBar" priority="236">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16755,7 +16924,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 L131:BO133 M134:BN139 BO137:BO139 L140:BO142 M143:BN148 BO146:BO148 L149:BO151 M152:BN157 BO155:BO157 L158:BO160 M161:BN166 BO164:BO166 BO129:BO130 M127:BN130 L126:BO126 M124:BN125 L123:BO123 M112:BN122">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 L133:BO135 M136:BN141 BO139:BO141 L142:BO144 M145:BN150 BO148:BO150 L151:BO153 M154:BN159 BO157:BO159 L160:BO162 M163:BN168 BO166:BO168 BO131:BO132 M129:BN132 L128:BO128 M126:BN127 L125:BO125 M112:BN124">
     <cfRule type="expression" dxfId="132" priority="282">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -16763,7 +16932,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L127:BO130 L98:BO103 L124:BO125 L105:BO110 L112:BO122">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L129:BO132 L98:BO103 L126:BO127 L105:BO110 L112:BO124">
     <cfRule type="expression" dxfId="130" priority="242">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -16773,7 +16942,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E167:E1048576 E95:E96 E127:E130 E98:E103 E124:E125 E105:E110 E112:E122">
+  <conditionalFormatting sqref="E1:E73 E169:E1048576 E95:E96 E129:E132 E98:E103 E126:E127 E105:E110 E112:E124">
     <cfRule type="cellIs" dxfId="128" priority="223" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16867,7 +17036,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I131:I139">
+  <conditionalFormatting sqref="I133:I141">
     <cfRule type="dataBar" priority="127">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16881,12 +17050,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L131:BO139">
+  <conditionalFormatting sqref="L133:BO141">
     <cfRule type="expression" dxfId="106" priority="126">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131:E139">
+  <conditionalFormatting sqref="E133:E141">
     <cfRule type="cellIs" dxfId="105" priority="119" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16909,7 +17078,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L134:BO139 L127:BO130 L98:BO103 L124:BO125 L105:BO110 L112:BO122">
+  <conditionalFormatting sqref="L136:BO141 L129:BO132 L98:BO103 L126:BO127 L105:BO110 L112:BO124">
     <cfRule type="expression" dxfId="98" priority="130">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16917,7 +17086,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I140:I148">
+  <conditionalFormatting sqref="I142:I150">
     <cfRule type="dataBar" priority="114">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16931,12 +17100,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L140:BO148">
+  <conditionalFormatting sqref="L142:BO150">
     <cfRule type="expression" dxfId="96" priority="113">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E140:E148">
+  <conditionalFormatting sqref="E142:E150">
     <cfRule type="cellIs" dxfId="95" priority="106" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -16959,7 +17128,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L143:BO148">
+  <conditionalFormatting sqref="L145:BO150">
     <cfRule type="expression" dxfId="88" priority="117">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -16967,7 +17136,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I149:I157">
+  <conditionalFormatting sqref="I151:I159">
     <cfRule type="dataBar" priority="101">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -16981,12 +17150,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L149:BO157">
+  <conditionalFormatting sqref="L151:BO159">
     <cfRule type="expression" dxfId="86" priority="100">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E149:E157">
+  <conditionalFormatting sqref="E151:E159">
     <cfRule type="cellIs" dxfId="85" priority="93" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17009,7 +17178,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L152:BO157">
+  <conditionalFormatting sqref="L154:BO159">
     <cfRule type="expression" dxfId="78" priority="104">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17017,7 +17186,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I158:I166">
+  <conditionalFormatting sqref="I160:I168">
     <cfRule type="dataBar" priority="88">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17031,12 +17200,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L158:BO166">
+  <conditionalFormatting sqref="L160:BO168">
     <cfRule type="expression" dxfId="76" priority="87">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E158:E166">
+  <conditionalFormatting sqref="E160:E168">
     <cfRule type="cellIs" dxfId="75" priority="80" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17059,7 +17228,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L161:BO166">
+  <conditionalFormatting sqref="L163:BO168">
     <cfRule type="expression" dxfId="68" priority="91">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17209,7 +17378,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I126">
+  <conditionalFormatting sqref="I128">
     <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17223,12 +17392,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L126:BO126">
+  <conditionalFormatting sqref="L128:BO128">
     <cfRule type="expression" dxfId="38" priority="41">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E126">
+  <conditionalFormatting sqref="E128">
     <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17251,7 +17420,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123">
+  <conditionalFormatting sqref="I125">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17265,12 +17434,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L123:BO123">
+  <conditionalFormatting sqref="L125:BO125">
     <cfRule type="expression" dxfId="30" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E123">
+  <conditionalFormatting sqref="E125">
     <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17449,7 +17618,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I127:I130 I98:I103 I105:I110 I124:I125 I112:I122</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I129:I132 I98:I103 I105:I110 I126:I127 I112:I124</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17479,7 +17648,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I131:I139</xm:sqref>
+          <xm:sqref>I133:I141</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -17494,7 +17663,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I140:I148</xm:sqref>
+          <xm:sqref>I142:I150</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -17509,7 +17678,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I149:I157</xm:sqref>
+          <xm:sqref>I151:I159</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -17524,7 +17693,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I158:I166</xm:sqref>
+          <xm:sqref>I160:I168</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -17584,7 +17753,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I126</xm:sqref>
+          <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
@@ -17599,7 +17768,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I123</xm:sqref>
+          <xm:sqref>I125</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Misc cleanup and bugfixes (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC368AF-1F87-4FE3-9F85-86BE3B594428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F1978EA-CF28-488F-971E-2D406AFBEDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="156">
   <si>
     <t>WBS</t>
   </si>
@@ -893,6 +893,9 @@
   </si>
   <si>
     <t>CSM Equation Fixing (Moving Averages Bug)</t>
+  </si>
+  <si>
+    <t>Add Proper Forecast Type Checks</t>
   </si>
 </sst>
 </file>
@@ -1821,6 +1824,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1830,6 +1840,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1838,17 +1852,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3002,7 +3005,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="32"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="34"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3409,11 +3412,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO170"/>
+  <dimension ref="A1:BO171"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="T110" sqref="T110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3443,27 +3446,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3508,198 +3511,198 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 32</v>
-      </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+        <v>Week 34</v>
+      </c>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 33</v>
-      </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+        <v>Week 35</v>
+      </c>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 34</v>
-      </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+        <v>Week 36</v>
+      </c>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 35</v>
-      </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+        <v>Week 37</v>
+      </c>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 36</v>
-      </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+        <v>Week 38</v>
+      </c>
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 37</v>
-      </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+        <v>Week 39</v>
+      </c>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 38</v>
-      </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+        <v>Week 40</v>
+      </c>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 39</v>
-      </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+        <v>Week 41</v>
+      </c>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
-        <v>44410</v>
-      </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+        <v>44424</v>
+      </c>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
-        <v>44417</v>
-      </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+        <v>44431</v>
+      </c>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
-        <v>44424</v>
-      </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+        <v>44438</v>
+      </c>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
-        <v>44431</v>
-      </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+        <v>44445</v>
+      </c>
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
-        <v>44438</v>
-      </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+        <v>44452</v>
+      </c>
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
-        <v>44445</v>
-      </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+        <v>44459</v>
+      </c>
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
-        <v>44452</v>
-      </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+        <v>44466</v>
+      </c>
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
-        <v>44459</v>
-      </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+        <v>44473</v>
+      </c>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -3715,227 +3718,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44410</v>
+        <v>44424</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44411</v>
+        <v>44425</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44412</v>
+        <v>44426</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44413</v>
+        <v>44427</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44414</v>
+        <v>44428</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44415</v>
+        <v>44429</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44416</v>
+        <v>44430</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44417</v>
+        <v>44431</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44418</v>
+        <v>44432</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44419</v>
+        <v>44433</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44420</v>
+        <v>44434</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44421</v>
+        <v>44435</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44422</v>
+        <v>44436</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44423</v>
+        <v>44437</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44424</v>
+        <v>44438</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44425</v>
+        <v>44439</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44426</v>
+        <v>44440</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44427</v>
+        <v>44441</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44428</v>
+        <v>44442</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44429</v>
+        <v>44443</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44430</v>
+        <v>44444</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44431</v>
+        <v>44445</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44432</v>
+        <v>44446</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44433</v>
+        <v>44447</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44434</v>
+        <v>44448</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44435</v>
+        <v>44449</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44436</v>
+        <v>44450</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44437</v>
+        <v>44451</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44438</v>
+        <v>44452</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44439</v>
+        <v>44453</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44440</v>
+        <v>44454</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44441</v>
+        <v>44455</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44442</v>
+        <v>44456</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44443</v>
+        <v>44457</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44444</v>
+        <v>44458</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44445</v>
+        <v>44459</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44446</v>
+        <v>44460</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44447</v>
+        <v>44461</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44448</v>
+        <v>44462</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44449</v>
+        <v>44463</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44450</v>
+        <v>44464</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44451</v>
+        <v>44465</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44452</v>
+        <v>44466</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44453</v>
+        <v>44467</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44454</v>
+        <v>44468</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44455</v>
+        <v>44469</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44456</v>
+        <v>44470</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44457</v>
+        <v>44471</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44458</v>
+        <v>44472</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44459</v>
+        <v>44473</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44460</v>
+        <v>44474</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44461</v>
+        <v>44475</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44462</v>
+        <v>44476</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44463</v>
+        <v>44477</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44464</v>
+        <v>44478</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44465</v>
+        <v>44479</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8857,7 +8860,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A135" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A136" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -13258,21 +13261,21 @@
         <v>11.7</v>
       </c>
       <c r="B118" s="65" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D118" s="70"/>
       <c r="E118" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F118" s="42">
-        <v>44428</v>
+        <v>44429</v>
       </c>
       <c r="G118" s="43">
-        <v>44428</v>
+        <v>44430</v>
       </c>
       <c r="H118" s="73"/>
       <c r="I118" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J118" s="75"/>
       <c r="K118" s="76"/>
@@ -13339,21 +13342,21 @@
         <v>11.8</v>
       </c>
       <c r="B119" s="65" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D119" s="70"/>
       <c r="E119" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F119" s="42">
-        <v>44430</v>
+        <v>44429</v>
       </c>
       <c r="G119" s="43">
-        <v>44429</v>
+        <v>44433</v>
       </c>
       <c r="H119" s="73"/>
       <c r="I119" s="26">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="J119" s="75"/>
       <c r="K119" s="76"/>
@@ -13420,17 +13423,17 @@
         <v>11.9</v>
       </c>
       <c r="B120" s="65" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D120" s="70"/>
       <c r="E120" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F120" s="42">
-        <v>44430</v>
+        <v>44433</v>
       </c>
       <c r="G120" s="43">
-        <v>44430</v>
+        <v>44440</v>
       </c>
       <c r="H120" s="73"/>
       <c r="I120" s="26">
@@ -13501,20 +13504,22 @@
         <v>11.10</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="D121" s="70"/>
       <c r="E121" s="66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F121" s="42">
-        <v>44430</v>
+        <v>44433</v>
       </c>
       <c r="G121" s="43">
         <v>44440</v>
       </c>
       <c r="H121" s="73"/>
-      <c r="I121" s="26"/>
+      <c r="I121" s="26">
+        <v>0</v>
+      </c>
       <c r="J121" s="75"/>
       <c r="K121" s="76"/>
       <c r="L121" s="46"/>
@@ -13580,17 +13585,17 @@
         <v>11.11</v>
       </c>
       <c r="B122" s="65" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D122" s="70"/>
       <c r="E122" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F122" s="42">
-        <v>44430</v>
+        <v>44438</v>
       </c>
       <c r="G122" s="43">
-        <v>44433</v>
+        <v>44444</v>
       </c>
       <c r="H122" s="73"/>
       <c r="I122" s="26"/>
@@ -13659,22 +13664,20 @@
         <v>11.12</v>
       </c>
       <c r="B123" s="65" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D123" s="70"/>
       <c r="E123" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F123" s="42">
-        <v>44430</v>
+        <v>44449</v>
       </c>
       <c r="G123" s="43">
-        <v>44433</v>
+        <v>44454</v>
       </c>
       <c r="H123" s="73"/>
-      <c r="I123" s="26">
-        <v>0.3</v>
-      </c>
+      <c r="I123" s="26"/>
       <c r="J123" s="75"/>
       <c r="K123" s="76"/>
       <c r="L123" s="46"/>
@@ -13740,20 +13743,22 @@
         <v>11.13</v>
       </c>
       <c r="B124" s="65" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D124" s="70"/>
       <c r="E124" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F124" s="42">
-        <v>44430</v>
+        <v>44449</v>
       </c>
       <c r="G124" s="43">
-        <v>44433</v>
+        <v>44454</v>
       </c>
       <c r="H124" s="73"/>
-      <c r="I124" s="26"/>
+      <c r="I124" s="26">
+        <v>0.3</v>
+      </c>
       <c r="J124" s="75"/>
       <c r="K124" s="76"/>
       <c r="L124" s="46"/>
@@ -13819,17 +13824,17 @@
         <v>11.14</v>
       </c>
       <c r="B125" s="65" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="D125" s="70"/>
       <c r="E125" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F125" s="42">
-        <v>44430</v>
+        <v>44449</v>
       </c>
       <c r="G125" s="43">
-        <v>44433</v>
+        <v>44454</v>
       </c>
       <c r="H125" s="73"/>
       <c r="I125" s="26"/>
@@ -13898,20 +13903,20 @@
         <v>11.15</v>
       </c>
       <c r="B126" s="65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D126" s="70"/>
-      <c r="E126" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F126" s="71">
-        <v>44433</v>
-      </c>
-      <c r="G126" s="72">
-        <v>44433</v>
+      <c r="E126" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F126" s="42">
+        <v>44449</v>
+      </c>
+      <c r="G126" s="43">
+        <v>44454</v>
       </c>
       <c r="H126" s="73"/>
-      <c r="I126" s="74"/>
+      <c r="I126" s="26"/>
       <c r="J126" s="75"/>
       <c r="K126" s="76"/>
       <c r="L126" s="46"/>
@@ -13971,172 +13976,174 @@
       <c r="BN126" s="46"/>
       <c r="BO126" s="46"/>
     </row>
-    <row r="127" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A127" s="16" t="str">
+    <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.16</v>
+      </c>
+      <c r="B127" s="65" t="s">
+        <v>147</v>
+      </c>
+      <c r="D127" s="70"/>
+      <c r="E127" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F127" s="71">
+        <v>44449</v>
+      </c>
+      <c r="G127" s="72">
+        <v>44454</v>
+      </c>
+      <c r="H127" s="73"/>
+      <c r="I127" s="74"/>
+      <c r="J127" s="75"/>
+      <c r="K127" s="76"/>
+      <c r="L127" s="46"/>
+      <c r="M127" s="46"/>
+      <c r="N127" s="46"/>
+      <c r="O127" s="46"/>
+      <c r="P127" s="46"/>
+      <c r="Q127" s="46"/>
+      <c r="R127" s="46"/>
+      <c r="S127" s="46"/>
+      <c r="T127" s="46"/>
+      <c r="U127" s="46"/>
+      <c r="V127" s="46"/>
+      <c r="W127" s="46"/>
+      <c r="X127" s="46"/>
+      <c r="Y127" s="46"/>
+      <c r="Z127" s="46"/>
+      <c r="AA127" s="46"/>
+      <c r="AB127" s="46"/>
+      <c r="AC127" s="46"/>
+      <c r="AD127" s="46"/>
+      <c r="AE127" s="46"/>
+      <c r="AF127" s="46"/>
+      <c r="AG127" s="46"/>
+      <c r="AH127" s="46"/>
+      <c r="AI127" s="46"/>
+      <c r="AJ127" s="46"/>
+      <c r="AK127" s="46"/>
+      <c r="AL127" s="46"/>
+      <c r="AM127" s="46"/>
+      <c r="AN127" s="46"/>
+      <c r="AO127" s="46"/>
+      <c r="AP127" s="46"/>
+      <c r="AQ127" s="46"/>
+      <c r="AR127" s="46"/>
+      <c r="AS127" s="46"/>
+      <c r="AT127" s="46"/>
+      <c r="AU127" s="46"/>
+      <c r="AV127" s="46"/>
+      <c r="AW127" s="46"/>
+      <c r="AX127" s="46"/>
+      <c r="AY127" s="46"/>
+      <c r="AZ127" s="46"/>
+      <c r="BA127" s="46"/>
+      <c r="BB127" s="46"/>
+      <c r="BC127" s="46"/>
+      <c r="BD127" s="46"/>
+      <c r="BE127" s="46"/>
+      <c r="BF127" s="46"/>
+      <c r="BG127" s="46"/>
+      <c r="BH127" s="46"/>
+      <c r="BI127" s="46"/>
+      <c r="BJ127" s="46"/>
+      <c r="BK127" s="46"/>
+      <c r="BL127" s="46"/>
+      <c r="BM127" s="46"/>
+      <c r="BN127" s="46"/>
+      <c r="BO127" s="46"/>
+    </row>
+    <row r="128" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B127" s="17" t="s">
+      <c r="B128" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="D127" s="19"/>
-      <c r="E127" s="19"/>
-      <c r="F127" s="44"/>
-      <c r="G127" s="44" t="str">
-        <f t="shared" ref="G127" si="22">IF(ISBLANK(F127)," - ",IF(H127=0,F127,F127+H127-1))</f>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="44"/>
+      <c r="G128" s="44" t="str">
+        <f t="shared" ref="G128" si="22">IF(ISBLANK(F128)," - ",IF(H128=0,F128,F128+H128-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H127" s="20"/>
-      <c r="I127" s="21"/>
-      <c r="J127" s="22" t="str">
-        <f t="shared" ref="J127" si="23">IF(OR(G127=0,F127=0)," - ",NETWORKDAYS(F127,G127))</f>
+      <c r="H128" s="20"/>
+      <c r="I128" s="21"/>
+      <c r="J128" s="22" t="str">
+        <f t="shared" ref="J128" si="23">IF(OR(G128=0,F128=0)," - ",NETWORKDAYS(F128,G128))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K127" s="41"/>
-      <c r="L127" s="48"/>
-      <c r="M127" s="48"/>
-      <c r="N127" s="48"/>
-      <c r="O127" s="48"/>
-      <c r="P127" s="48"/>
-      <c r="Q127" s="48"/>
-      <c r="R127" s="48"/>
-      <c r="S127" s="48"/>
-      <c r="T127" s="48"/>
-      <c r="U127" s="48"/>
-      <c r="V127" s="48"/>
-      <c r="W127" s="48"/>
-      <c r="X127" s="48"/>
-      <c r="Y127" s="48"/>
-      <c r="Z127" s="48"/>
-      <c r="AA127" s="48"/>
-      <c r="AB127" s="48"/>
-      <c r="AC127" s="48"/>
-      <c r="AD127" s="48"/>
-      <c r="AE127" s="48"/>
-      <c r="AF127" s="48"/>
-      <c r="AG127" s="48"/>
-      <c r="AH127" s="48"/>
-      <c r="AI127" s="48"/>
-      <c r="AJ127" s="48"/>
-      <c r="AK127" s="48"/>
-      <c r="AL127" s="48"/>
-      <c r="AM127" s="48"/>
-      <c r="AN127" s="48"/>
-      <c r="AO127" s="48"/>
-      <c r="AP127" s="48"/>
-      <c r="AQ127" s="48"/>
-      <c r="AR127" s="48"/>
-      <c r="AS127" s="48"/>
-      <c r="AT127" s="48"/>
-      <c r="AU127" s="48"/>
-      <c r="AV127" s="48"/>
-      <c r="AW127" s="48"/>
-      <c r="AX127" s="48"/>
-      <c r="AY127" s="48"/>
-      <c r="AZ127" s="48"/>
-      <c r="BA127" s="48"/>
-      <c r="BB127" s="48"/>
-      <c r="BC127" s="48"/>
-      <c r="BD127" s="48"/>
-      <c r="BE127" s="48"/>
-      <c r="BF127" s="48"/>
-      <c r="BG127" s="48"/>
-      <c r="BH127" s="48"/>
-      <c r="BI127" s="48"/>
-      <c r="BJ127" s="48"/>
-      <c r="BK127" s="48"/>
-      <c r="BL127" s="48"/>
-      <c r="BM127" s="48"/>
-      <c r="BN127" s="48"/>
-      <c r="BO127" s="48"/>
-    </row>
-    <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A128" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>12.1</v>
-      </c>
-      <c r="B128" s="65" t="s">
-        <v>127</v>
-      </c>
-      <c r="D128" s="70"/>
-      <c r="E128" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F128" s="42">
-        <v>44392</v>
-      </c>
-      <c r="G128" s="43"/>
-      <c r="H128" s="73"/>
-      <c r="I128" s="26"/>
-      <c r="J128" s="75"/>
-      <c r="K128" s="76"/>
-      <c r="L128" s="46"/>
-      <c r="M128" s="46"/>
-      <c r="N128" s="46"/>
-      <c r="O128" s="46"/>
-      <c r="P128" s="46"/>
-      <c r="Q128" s="46"/>
-      <c r="R128" s="46"/>
-      <c r="S128" s="46"/>
-      <c r="T128" s="46"/>
-      <c r="U128" s="46"/>
-      <c r="V128" s="46"/>
-      <c r="W128" s="46"/>
-      <c r="X128" s="46"/>
-      <c r="Y128" s="46"/>
-      <c r="Z128" s="46"/>
-      <c r="AA128" s="46"/>
-      <c r="AB128" s="46"/>
-      <c r="AC128" s="46"/>
-      <c r="AD128" s="46"/>
-      <c r="AE128" s="46"/>
-      <c r="AF128" s="46"/>
-      <c r="AG128" s="46"/>
-      <c r="AH128" s="46"/>
-      <c r="AI128" s="46"/>
-      <c r="AJ128" s="46"/>
-      <c r="AK128" s="46"/>
-      <c r="AL128" s="46"/>
-      <c r="AM128" s="46"/>
-      <c r="AN128" s="46"/>
-      <c r="AO128" s="46"/>
-      <c r="AP128" s="46"/>
-      <c r="AQ128" s="46"/>
-      <c r="AR128" s="46"/>
-      <c r="AS128" s="46"/>
-      <c r="AT128" s="46"/>
-      <c r="AU128" s="46"/>
-      <c r="AV128" s="46"/>
-      <c r="AW128" s="46"/>
-      <c r="AX128" s="46"/>
-      <c r="AY128" s="46"/>
-      <c r="AZ128" s="46"/>
-      <c r="BA128" s="46"/>
-      <c r="BB128" s="46"/>
-      <c r="BC128" s="46"/>
-      <c r="BD128" s="46"/>
-      <c r="BE128" s="46"/>
-      <c r="BF128" s="46"/>
-      <c r="BG128" s="46"/>
-      <c r="BH128" s="46"/>
-      <c r="BI128" s="46"/>
-      <c r="BJ128" s="46"/>
-      <c r="BK128" s="46"/>
-      <c r="BL128" s="46"/>
-      <c r="BM128" s="46"/>
-      <c r="BN128" s="46"/>
-      <c r="BO128" s="46"/>
+      <c r="K128" s="41"/>
+      <c r="L128" s="48"/>
+      <c r="M128" s="48"/>
+      <c r="N128" s="48"/>
+      <c r="O128" s="48"/>
+      <c r="P128" s="48"/>
+      <c r="Q128" s="48"/>
+      <c r="R128" s="48"/>
+      <c r="S128" s="48"/>
+      <c r="T128" s="48"/>
+      <c r="U128" s="48"/>
+      <c r="V128" s="48"/>
+      <c r="W128" s="48"/>
+      <c r="X128" s="48"/>
+      <c r="Y128" s="48"/>
+      <c r="Z128" s="48"/>
+      <c r="AA128" s="48"/>
+      <c r="AB128" s="48"/>
+      <c r="AC128" s="48"/>
+      <c r="AD128" s="48"/>
+      <c r="AE128" s="48"/>
+      <c r="AF128" s="48"/>
+      <c r="AG128" s="48"/>
+      <c r="AH128" s="48"/>
+      <c r="AI128" s="48"/>
+      <c r="AJ128" s="48"/>
+      <c r="AK128" s="48"/>
+      <c r="AL128" s="48"/>
+      <c r="AM128" s="48"/>
+      <c r="AN128" s="48"/>
+      <c r="AO128" s="48"/>
+      <c r="AP128" s="48"/>
+      <c r="AQ128" s="48"/>
+      <c r="AR128" s="48"/>
+      <c r="AS128" s="48"/>
+      <c r="AT128" s="48"/>
+      <c r="AU128" s="48"/>
+      <c r="AV128" s="48"/>
+      <c r="AW128" s="48"/>
+      <c r="AX128" s="48"/>
+      <c r="AY128" s="48"/>
+      <c r="AZ128" s="48"/>
+      <c r="BA128" s="48"/>
+      <c r="BB128" s="48"/>
+      <c r="BC128" s="48"/>
+      <c r="BD128" s="48"/>
+      <c r="BE128" s="48"/>
+      <c r="BF128" s="48"/>
+      <c r="BG128" s="48"/>
+      <c r="BH128" s="48"/>
+      <c r="BI128" s="48"/>
+      <c r="BJ128" s="48"/>
+      <c r="BK128" s="48"/>
+      <c r="BL128" s="48"/>
+      <c r="BM128" s="48"/>
+      <c r="BN128" s="48"/>
+      <c r="BO128" s="48"/>
     </row>
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D129" s="70"/>
-      <c r="E129" s="70" t="s">
+      <c r="E129" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F129" s="42">
@@ -14144,7 +14151,7 @@
       </c>
       <c r="G129" s="43"/>
       <c r="H129" s="73"/>
-      <c r="I129" s="74"/>
+      <c r="I129" s="26"/>
       <c r="J129" s="75"/>
       <c r="K129" s="76"/>
       <c r="L129" s="46"/>
@@ -14204,173 +14211,173 @@
       <c r="BN129" s="46"/>
       <c r="BO129" s="46"/>
     </row>
-    <row r="130" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="16" t="str">
+    <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.2</v>
+      </c>
+      <c r="B130" s="65" t="s">
+        <v>128</v>
+      </c>
+      <c r="D130" s="70"/>
+      <c r="E130" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F130" s="42">
+        <v>44392</v>
+      </c>
+      <c r="G130" s="43"/>
+      <c r="H130" s="73"/>
+      <c r="I130" s="74"/>
+      <c r="J130" s="75"/>
+      <c r="K130" s="76"/>
+      <c r="L130" s="46"/>
+      <c r="M130" s="46"/>
+      <c r="N130" s="46"/>
+      <c r="O130" s="46"/>
+      <c r="P130" s="46"/>
+      <c r="Q130" s="46"/>
+      <c r="R130" s="46"/>
+      <c r="S130" s="46"/>
+      <c r="T130" s="46"/>
+      <c r="U130" s="46"/>
+      <c r="V130" s="46"/>
+      <c r="W130" s="46"/>
+      <c r="X130" s="46"/>
+      <c r="Y130" s="46"/>
+      <c r="Z130" s="46"/>
+      <c r="AA130" s="46"/>
+      <c r="AB130" s="46"/>
+      <c r="AC130" s="46"/>
+      <c r="AD130" s="46"/>
+      <c r="AE130" s="46"/>
+      <c r="AF130" s="46"/>
+      <c r="AG130" s="46"/>
+      <c r="AH130" s="46"/>
+      <c r="AI130" s="46"/>
+      <c r="AJ130" s="46"/>
+      <c r="AK130" s="46"/>
+      <c r="AL130" s="46"/>
+      <c r="AM130" s="46"/>
+      <c r="AN130" s="46"/>
+      <c r="AO130" s="46"/>
+      <c r="AP130" s="46"/>
+      <c r="AQ130" s="46"/>
+      <c r="AR130" s="46"/>
+      <c r="AS130" s="46"/>
+      <c r="AT130" s="46"/>
+      <c r="AU130" s="46"/>
+      <c r="AV130" s="46"/>
+      <c r="AW130" s="46"/>
+      <c r="AX130" s="46"/>
+      <c r="AY130" s="46"/>
+      <c r="AZ130" s="46"/>
+      <c r="BA130" s="46"/>
+      <c r="BB130" s="46"/>
+      <c r="BC130" s="46"/>
+      <c r="BD130" s="46"/>
+      <c r="BE130" s="46"/>
+      <c r="BF130" s="46"/>
+      <c r="BG130" s="46"/>
+      <c r="BH130" s="46"/>
+      <c r="BI130" s="46"/>
+      <c r="BJ130" s="46"/>
+      <c r="BK130" s="46"/>
+      <c r="BL130" s="46"/>
+      <c r="BM130" s="46"/>
+      <c r="BN130" s="46"/>
+      <c r="BO130" s="46"/>
+    </row>
+    <row r="131" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>13</v>
       </c>
-      <c r="B130" s="17" t="s">
+      <c r="B131" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="44"/>
-      <c r="G130" s="44" t="str">
-        <f t="shared" ref="G130" si="24">IF(ISBLANK(F130)," - ",IF(H130=0,F130,F130+H130-1))</f>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="44"/>
+      <c r="G131" s="44" t="str">
+        <f t="shared" ref="G131" si="24">IF(ISBLANK(F131)," - ",IF(H131=0,F131,F131+H131-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H130" s="20"/>
-      <c r="I130" s="21"/>
-      <c r="J130" s="22" t="str">
-        <f t="shared" ref="J130" si="25">IF(OR(G130=0,F130=0)," - ",NETWORKDAYS(F130,G130))</f>
+      <c r="H131" s="20"/>
+      <c r="I131" s="21"/>
+      <c r="J131" s="22" t="str">
+        <f t="shared" ref="J131" si="25">IF(OR(G131=0,F131=0)," - ",NETWORKDAYS(F131,G131))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K130" s="41"/>
-      <c r="L130" s="48"/>
-      <c r="M130" s="48"/>
-      <c r="N130" s="48"/>
-      <c r="O130" s="48"/>
-      <c r="P130" s="48"/>
-      <c r="Q130" s="48"/>
-      <c r="R130" s="48"/>
-      <c r="S130" s="48"/>
-      <c r="T130" s="48"/>
-      <c r="U130" s="48"/>
-      <c r="V130" s="48"/>
-      <c r="W130" s="48"/>
-      <c r="X130" s="48"/>
-      <c r="Y130" s="48"/>
-      <c r="Z130" s="48"/>
-      <c r="AA130" s="48"/>
-      <c r="AB130" s="48"/>
-      <c r="AC130" s="48"/>
-      <c r="AD130" s="48"/>
-      <c r="AE130" s="48"/>
-      <c r="AF130" s="48"/>
-      <c r="AG130" s="48"/>
-      <c r="AH130" s="48"/>
-      <c r="AI130" s="48"/>
-      <c r="AJ130" s="48"/>
-      <c r="AK130" s="48"/>
-      <c r="AL130" s="48"/>
-      <c r="AM130" s="48"/>
-      <c r="AN130" s="48"/>
-      <c r="AO130" s="48"/>
-      <c r="AP130" s="48"/>
-      <c r="AQ130" s="48"/>
-      <c r="AR130" s="48"/>
-      <c r="AS130" s="48"/>
-      <c r="AT130" s="48"/>
-      <c r="AU130" s="48"/>
-      <c r="AV130" s="48"/>
-      <c r="AW130" s="48"/>
-      <c r="AX130" s="48"/>
-      <c r="AY130" s="48"/>
-      <c r="AZ130" s="48"/>
-      <c r="BA130" s="48"/>
-      <c r="BB130" s="48"/>
-      <c r="BC130" s="48"/>
-      <c r="BD130" s="48"/>
-      <c r="BE130" s="48"/>
-      <c r="BF130" s="48"/>
-      <c r="BG130" s="48"/>
-      <c r="BH130" s="48"/>
-      <c r="BI130" s="48"/>
-      <c r="BJ130" s="48"/>
-      <c r="BK130" s="48"/>
-      <c r="BL130" s="48"/>
-      <c r="BM130" s="48"/>
-      <c r="BN130" s="48"/>
-      <c r="BO130" s="48"/>
-    </row>
-    <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.1</v>
-      </c>
-      <c r="B131" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D131" s="70"/>
-      <c r="E131" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F131" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G131" s="43"/>
-      <c r="H131" s="25"/>
-      <c r="I131" s="26"/>
-      <c r="J131" s="27"/>
-      <c r="K131" s="40"/>
-      <c r="L131" s="46"/>
-      <c r="M131" s="46"/>
-      <c r="N131" s="46"/>
-      <c r="O131" s="46"/>
-      <c r="P131" s="46"/>
-      <c r="Q131" s="46"/>
-      <c r="R131" s="46"/>
-      <c r="S131" s="46"/>
-      <c r="T131" s="46"/>
-      <c r="U131" s="46"/>
-      <c r="V131" s="46"/>
-      <c r="W131" s="46"/>
-      <c r="X131" s="46"/>
-      <c r="Y131" s="46"/>
-      <c r="Z131" s="46"/>
-      <c r="AA131" s="46"/>
-      <c r="AB131" s="46"/>
-      <c r="AC131" s="46"/>
-      <c r="AD131" s="46"/>
-      <c r="AE131" s="46"/>
-      <c r="AF131" s="46"/>
-      <c r="AG131" s="46"/>
-      <c r="AH131" s="46"/>
-      <c r="AI131" s="46"/>
-      <c r="AJ131" s="46"/>
-      <c r="AK131" s="46"/>
-      <c r="AL131" s="46"/>
-      <c r="AM131" s="46"/>
-      <c r="AN131" s="46"/>
-      <c r="AO131" s="46"/>
-      <c r="AP131" s="46"/>
-      <c r="AQ131" s="46"/>
-      <c r="AR131" s="46"/>
-      <c r="AS131" s="46"/>
-      <c r="AT131" s="46"/>
-      <c r="AU131" s="46"/>
-      <c r="AV131" s="46"/>
-      <c r="AW131" s="46"/>
-      <c r="AX131" s="46"/>
-      <c r="AY131" s="46"/>
-      <c r="AZ131" s="46"/>
-      <c r="BA131" s="46"/>
-      <c r="BB131" s="46"/>
-      <c r="BC131" s="46"/>
-      <c r="BD131" s="46"/>
-      <c r="BE131" s="46"/>
-      <c r="BF131" s="46"/>
-      <c r="BG131" s="46"/>
-      <c r="BH131" s="46"/>
-      <c r="BI131" s="46"/>
-      <c r="BJ131" s="46"/>
-      <c r="BK131" s="46"/>
-      <c r="BL131" s="46"/>
-      <c r="BM131" s="46"/>
-      <c r="BN131" s="46"/>
-      <c r="BO131" s="46"/>
+      <c r="K131" s="41"/>
+      <c r="L131" s="48"/>
+      <c r="M131" s="48"/>
+      <c r="N131" s="48"/>
+      <c r="O131" s="48"/>
+      <c r="P131" s="48"/>
+      <c r="Q131" s="48"/>
+      <c r="R131" s="48"/>
+      <c r="S131" s="48"/>
+      <c r="T131" s="48"/>
+      <c r="U131" s="48"/>
+      <c r="V131" s="48"/>
+      <c r="W131" s="48"/>
+      <c r="X131" s="48"/>
+      <c r="Y131" s="48"/>
+      <c r="Z131" s="48"/>
+      <c r="AA131" s="48"/>
+      <c r="AB131" s="48"/>
+      <c r="AC131" s="48"/>
+      <c r="AD131" s="48"/>
+      <c r="AE131" s="48"/>
+      <c r="AF131" s="48"/>
+      <c r="AG131" s="48"/>
+      <c r="AH131" s="48"/>
+      <c r="AI131" s="48"/>
+      <c r="AJ131" s="48"/>
+      <c r="AK131" s="48"/>
+      <c r="AL131" s="48"/>
+      <c r="AM131" s="48"/>
+      <c r="AN131" s="48"/>
+      <c r="AO131" s="48"/>
+      <c r="AP131" s="48"/>
+      <c r="AQ131" s="48"/>
+      <c r="AR131" s="48"/>
+      <c r="AS131" s="48"/>
+      <c r="AT131" s="48"/>
+      <c r="AU131" s="48"/>
+      <c r="AV131" s="48"/>
+      <c r="AW131" s="48"/>
+      <c r="AX131" s="48"/>
+      <c r="AY131" s="48"/>
+      <c r="AZ131" s="48"/>
+      <c r="BA131" s="48"/>
+      <c r="BB131" s="48"/>
+      <c r="BC131" s="48"/>
+      <c r="BD131" s="48"/>
+      <c r="BE131" s="48"/>
+      <c r="BF131" s="48"/>
+      <c r="BG131" s="48"/>
+      <c r="BH131" s="48"/>
+      <c r="BI131" s="48"/>
+      <c r="BJ131" s="48"/>
+      <c r="BK131" s="48"/>
+      <c r="BL131" s="48"/>
+      <c r="BM131" s="48"/>
+      <c r="BN131" s="48"/>
+      <c r="BO131" s="48"/>
     </row>
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D132" s="70"/>
       <c r="E132" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F132" s="42">
         <v>44379</v>
@@ -14440,14 +14447,14 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F133" s="42">
         <v>44379</v>
@@ -14517,10 +14524,10 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
@@ -14594,17 +14601,17 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B135" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D135" s="66"/>
+        <v>13.4</v>
+      </c>
+      <c r="B135" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F135" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G135" s="43"/>
       <c r="H135" s="25"/>
@@ -14669,11 +14676,20 @@
       <c r="BO135" s="46"/>
     </row>
     <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="23"/>
-      <c r="B136" s="65"/>
+      <c r="A136" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B136" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D136" s="66"/>
-      <c r="E136" s="66"/>
-      <c r="F136" s="42"/>
+      <c r="E136" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F136" s="42">
+        <v>44531</v>
+      </c>
       <c r="G136" s="43"/>
       <c r="H136" s="25"/>
       <c r="I136" s="26"/>
@@ -14875,7 +14891,7 @@
     <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="23"/>
       <c r="B139" s="65"/>
-      <c r="D139" s="70"/>
+      <c r="D139" s="66"/>
       <c r="E139" s="66"/>
       <c r="F139" s="42"/>
       <c r="G139" s="43"/>
@@ -15215,7 +15231,7 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23"/>
       <c r="B144" s="65"/>
-      <c r="D144" s="66"/>
+      <c r="D144" s="70"/>
       <c r="E144" s="66"/>
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
@@ -15487,7 +15503,7 @@
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="23"/>
       <c r="B148" s="65"/>
-      <c r="D148" s="70"/>
+      <c r="D148" s="66"/>
       <c r="E148" s="66"/>
       <c r="F148" s="42"/>
       <c r="G148" s="43"/>
@@ -15827,7 +15843,7 @@
     <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="23"/>
       <c r="B153" s="65"/>
-      <c r="D153" s="66"/>
+      <c r="D153" s="70"/>
       <c r="E153" s="66"/>
       <c r="F153" s="42"/>
       <c r="G153" s="43"/>
@@ -16099,7 +16115,7 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23"/>
       <c r="B157" s="65"/>
-      <c r="D157" s="70"/>
+      <c r="D157" s="66"/>
       <c r="E157" s="66"/>
       <c r="F157" s="42"/>
       <c r="G157" s="43"/>
@@ -16439,7 +16455,7 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23"/>
       <c r="B162" s="65"/>
-      <c r="D162" s="66"/>
+      <c r="D162" s="70"/>
       <c r="E162" s="66"/>
       <c r="F162" s="42"/>
       <c r="G162" s="43"/>
@@ -16711,7 +16727,7 @@
     <row r="166" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23"/>
       <c r="B166" s="65"/>
-      <c r="D166" s="70"/>
+      <c r="D166" s="66"/>
       <c r="E166" s="66"/>
       <c r="F166" s="42"/>
       <c r="G166" s="43"/>
@@ -17048,18 +17064,77 @@
       <c r="BN170" s="46"/>
       <c r="BO170" s="46"/>
     </row>
+    <row r="171" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="23"/>
+      <c r="B171" s="65"/>
+      <c r="D171" s="70"/>
+      <c r="E171" s="66"/>
+      <c r="F171" s="42"/>
+      <c r="G171" s="43"/>
+      <c r="H171" s="25"/>
+      <c r="I171" s="26"/>
+      <c r="J171" s="27"/>
+      <c r="K171" s="40"/>
+      <c r="L171" s="46"/>
+      <c r="M171" s="46"/>
+      <c r="N171" s="46"/>
+      <c r="O171" s="46"/>
+      <c r="P171" s="46"/>
+      <c r="Q171" s="46"/>
+      <c r="R171" s="46"/>
+      <c r="S171" s="46"/>
+      <c r="T171" s="46"/>
+      <c r="U171" s="46"/>
+      <c r="V171" s="46"/>
+      <c r="W171" s="46"/>
+      <c r="X171" s="46"/>
+      <c r="Y171" s="46"/>
+      <c r="Z171" s="46"/>
+      <c r="AA171" s="46"/>
+      <c r="AB171" s="46"/>
+      <c r="AC171" s="46"/>
+      <c r="AD171" s="46"/>
+      <c r="AE171" s="46"/>
+      <c r="AF171" s="46"/>
+      <c r="AG171" s="46"/>
+      <c r="AH171" s="46"/>
+      <c r="AI171" s="46"/>
+      <c r="AJ171" s="46"/>
+      <c r="AK171" s="46"/>
+      <c r="AL171" s="46"/>
+      <c r="AM171" s="46"/>
+      <c r="AN171" s="46"/>
+      <c r="AO171" s="46"/>
+      <c r="AP171" s="46"/>
+      <c r="AQ171" s="46"/>
+      <c r="AR171" s="46"/>
+      <c r="AS171" s="46"/>
+      <c r="AT171" s="46"/>
+      <c r="AU171" s="46"/>
+      <c r="AV171" s="46"/>
+      <c r="AW171" s="46"/>
+      <c r="AX171" s="46"/>
+      <c r="AY171" s="46"/>
+      <c r="AZ171" s="46"/>
+      <c r="BA171" s="46"/>
+      <c r="BB171" s="46"/>
+      <c r="BC171" s="46"/>
+      <c r="BD171" s="46"/>
+      <c r="BE171" s="46"/>
+      <c r="BF171" s="46"/>
+      <c r="BG171" s="46"/>
+      <c r="BH171" s="46"/>
+      <c r="BI171" s="46"/>
+      <c r="BJ171" s="46"/>
+      <c r="BK171" s="46"/>
+      <c r="BL171" s="46"/>
+      <c r="BM171" s="46"/>
+      <c r="BN171" s="46"/>
+      <c r="BO171" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17070,9 +17145,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I128:I129 I112:I126">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I132:I135 I98:I103 I105:I110 I129:I130 I112:I127">
     <cfRule type="dataBar" priority="236">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17091,7 +17175,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 L135:BO137 M138:BN143 BO141:BO143 L144:BO146 M147:BN152 BO150:BO152 L153:BO155 M156:BN161 BO159:BO161 L162:BO164 M165:BN170 BO168:BO170 BO133:BO134 M131:BN134 L130:BO130 M128:BN129 L127:BO127 M112:BN126">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 L136:BO138 M139:BN144 BO142:BO144 L145:BO147 M148:BN153 BO151:BO153 L154:BO156 M157:BN162 BO160:BO162 L163:BO165 M166:BN171 BO169:BO171 BO134:BO135 M132:BN135 L131:BO131 M129:BN130 L128:BO128 M112:BN127">
     <cfRule type="expression" dxfId="132" priority="282">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -17099,7 +17183,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L131:BO134 L98:BO103 L128:BO129 L105:BO110 L112:BO126">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L132:BO135 L98:BO103 L129:BO130 L105:BO110 L112:BO127">
     <cfRule type="expression" dxfId="130" priority="242">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -17109,7 +17193,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E171:E1048576 E95:E96 E131:E134 E98:E103 E128:E129 E105:E110 E112:E126">
+  <conditionalFormatting sqref="E1:E73 E172:E1048576 E95:E96 E132:E135 E98:E103 E129:E130 E105:E110 E112:E127">
     <cfRule type="cellIs" dxfId="128" priority="223" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17203,7 +17287,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I135:I143">
+  <conditionalFormatting sqref="I136:I144">
     <cfRule type="dataBar" priority="127">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17217,12 +17301,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L135:BO143">
+  <conditionalFormatting sqref="L136:BO144">
     <cfRule type="expression" dxfId="106" priority="126">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E135:E143">
+  <conditionalFormatting sqref="E136:E144">
     <cfRule type="cellIs" dxfId="105" priority="119" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17245,7 +17329,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L138:BO143 L131:BO134 L98:BO103 L128:BO129 L105:BO110 L112:BO126">
+  <conditionalFormatting sqref="L139:BO144 L132:BO135 L98:BO103 L129:BO130 L105:BO110 L112:BO127">
     <cfRule type="expression" dxfId="98" priority="130">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17253,7 +17337,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I144:I152">
+  <conditionalFormatting sqref="I145:I153">
     <cfRule type="dataBar" priority="114">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17267,12 +17351,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L144:BO152">
+  <conditionalFormatting sqref="L145:BO153">
     <cfRule type="expression" dxfId="96" priority="113">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E144:E152">
+  <conditionalFormatting sqref="E145:E153">
     <cfRule type="cellIs" dxfId="95" priority="106" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17295,7 +17379,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L147:BO152">
+  <conditionalFormatting sqref="L148:BO153">
     <cfRule type="expression" dxfId="88" priority="117">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17303,7 +17387,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I153:I161">
+  <conditionalFormatting sqref="I154:I162">
     <cfRule type="dataBar" priority="101">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17317,12 +17401,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L153:BO161">
+  <conditionalFormatting sqref="L154:BO162">
     <cfRule type="expression" dxfId="86" priority="100">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E153:E161">
+  <conditionalFormatting sqref="E154:E162">
     <cfRule type="cellIs" dxfId="85" priority="93" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17345,7 +17429,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L156:BO161">
+  <conditionalFormatting sqref="L157:BO162">
     <cfRule type="expression" dxfId="78" priority="104">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17353,7 +17437,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I162:I170">
+  <conditionalFormatting sqref="I163:I171">
     <cfRule type="dataBar" priority="88">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17367,12 +17451,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L162:BO170">
+  <conditionalFormatting sqref="L163:BO171">
     <cfRule type="expression" dxfId="76" priority="87">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E162:E170">
+  <conditionalFormatting sqref="E163:E171">
     <cfRule type="cellIs" dxfId="75" priority="80" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17395,7 +17479,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L165:BO170">
+  <conditionalFormatting sqref="L166:BO171">
     <cfRule type="expression" dxfId="68" priority="91">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17545,7 +17629,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I130">
+  <conditionalFormatting sqref="I131">
     <cfRule type="dataBar" priority="42">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17559,12 +17643,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L130:BO130">
+  <conditionalFormatting sqref="L131:BO131">
     <cfRule type="expression" dxfId="38" priority="41">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E130">
+  <conditionalFormatting sqref="E131">
     <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17587,7 +17671,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I127">
+  <conditionalFormatting sqref="I128">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17601,12 +17685,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L127:BO127">
+  <conditionalFormatting sqref="L128:BO128">
     <cfRule type="expression" dxfId="30" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E127">
+  <conditionalFormatting sqref="E128">
     <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17785,7 +17869,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I128:I129 I112:I126</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I132:I135 I98:I103 I105:I110 I129:I130 I112:I127</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17815,7 +17899,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I135:I143</xm:sqref>
+          <xm:sqref>I136:I144</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -17830,7 +17914,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I144:I152</xm:sqref>
+          <xm:sqref>I145:I153</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -17845,7 +17929,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I153:I161</xm:sqref>
+          <xm:sqref>I154:I162</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -17860,7 +17944,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I162:I170</xm:sqref>
+          <xm:sqref>I163:I171</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -17920,7 +18004,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I130</xm:sqref>
+          <xm:sqref>I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{377308A7-991B-4596-8880-3ACC1EA2DAB7}">
@@ -17935,7 +18019,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I127</xm:sqref>
+          <xm:sqref>I128</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Added downside scenario and fixes to code to allow for multiple scenarios (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF8BD8A-12EE-448C-B170-DF2EEA6AA01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE63E4C-E8FE-4430-9314-897E78DE6B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="155">
   <si>
     <t>WBS</t>
   </si>
@@ -890,6 +890,9 @@
   </si>
   <si>
     <t>Website Improvements (v0.17)</t>
+  </si>
+  <si>
+    <t>Add Additional Scenarios</t>
   </si>
 </sst>
 </file>
@@ -1818,6 +1821,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1827,6 +1837,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1835,17 +1849,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3420,11 +3423,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO169"/>
+  <dimension ref="A1:BO170"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I125" sqref="I125"/>
+      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3454,27 +3457,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3519,12 +3522,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3534,183 +3537,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44431</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44438</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44445</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44452</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44459</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44466</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44473</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44480</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8868,7 +8871,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A134" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A135" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -13364,7 +13367,7 @@
       </c>
       <c r="H119" s="73"/>
       <c r="I119" s="26">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="J119" s="75"/>
       <c r="K119" s="76"/>
@@ -13431,7 +13434,7 @@
         <v>11.9</v>
       </c>
       <c r="B120" s="65" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="D120" s="70"/>
       <c r="E120" s="66" t="s">
@@ -13445,7 +13448,7 @@
       </c>
       <c r="H120" s="73"/>
       <c r="I120" s="26">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="J120" s="75"/>
       <c r="K120" s="76"/>
@@ -13512,21 +13515,21 @@
         <v>11.10</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D121" s="70"/>
       <c r="E121" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F121" s="42">
-        <v>44437</v>
+        <v>44436</v>
       </c>
       <c r="G121" s="43">
         <v>44438</v>
       </c>
       <c r="H121" s="73"/>
       <c r="I121" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J121" s="75"/>
       <c r="K121" s="76"/>
@@ -13593,17 +13596,17 @@
         <v>11.11</v>
       </c>
       <c r="B122" s="65" t="s">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="D122" s="70"/>
       <c r="E122" s="66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F122" s="42">
+        <v>44437</v>
+      </c>
+      <c r="G122" s="43">
         <v>44438</v>
-      </c>
-      <c r="G122" s="43">
-        <v>44442</v>
       </c>
       <c r="H122" s="73"/>
       <c r="I122" s="26">
@@ -13668,175 +13671,177 @@
       <c r="BN122" s="46"/>
       <c r="BO122" s="46"/>
     </row>
-    <row r="123" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="16" t="str">
+    <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>11.12</v>
+      </c>
+      <c r="B123" s="65" t="s">
+        <v>131</v>
+      </c>
+      <c r="D123" s="70"/>
+      <c r="E123" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F123" s="42">
+        <v>44438</v>
+      </c>
+      <c r="G123" s="43">
+        <v>44442</v>
+      </c>
+      <c r="H123" s="73"/>
+      <c r="I123" s="26">
+        <v>0</v>
+      </c>
+      <c r="J123" s="75"/>
+      <c r="K123" s="76"/>
+      <c r="L123" s="46"/>
+      <c r="M123" s="46"/>
+      <c r="N123" s="46"/>
+      <c r="O123" s="46"/>
+      <c r="P123" s="46"/>
+      <c r="Q123" s="46"/>
+      <c r="R123" s="46"/>
+      <c r="S123" s="46"/>
+      <c r="T123" s="46"/>
+      <c r="U123" s="46"/>
+      <c r="V123" s="46"/>
+      <c r="W123" s="46"/>
+      <c r="X123" s="46"/>
+      <c r="Y123" s="46"/>
+      <c r="Z123" s="46"/>
+      <c r="AA123" s="46"/>
+      <c r="AB123" s="46"/>
+      <c r="AC123" s="46"/>
+      <c r="AD123" s="46"/>
+      <c r="AE123" s="46"/>
+      <c r="AF123" s="46"/>
+      <c r="AG123" s="46"/>
+      <c r="AH123" s="46"/>
+      <c r="AI123" s="46"/>
+      <c r="AJ123" s="46"/>
+      <c r="AK123" s="46"/>
+      <c r="AL123" s="46"/>
+      <c r="AM123" s="46"/>
+      <c r="AN123" s="46"/>
+      <c r="AO123" s="46"/>
+      <c r="AP123" s="46"/>
+      <c r="AQ123" s="46"/>
+      <c r="AR123" s="46"/>
+      <c r="AS123" s="46"/>
+      <c r="AT123" s="46"/>
+      <c r="AU123" s="46"/>
+      <c r="AV123" s="46"/>
+      <c r="AW123" s="46"/>
+      <c r="AX123" s="46"/>
+      <c r="AY123" s="46"/>
+      <c r="AZ123" s="46"/>
+      <c r="BA123" s="46"/>
+      <c r="BB123" s="46"/>
+      <c r="BC123" s="46"/>
+      <c r="BD123" s="46"/>
+      <c r="BE123" s="46"/>
+      <c r="BF123" s="46"/>
+      <c r="BG123" s="46"/>
+      <c r="BH123" s="46"/>
+      <c r="BI123" s="46"/>
+      <c r="BJ123" s="46"/>
+      <c r="BK123" s="46"/>
+      <c r="BL123" s="46"/>
+      <c r="BM123" s="46"/>
+      <c r="BN123" s="46"/>
+      <c r="BO123" s="46"/>
+    </row>
+    <row r="124" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B123" s="17" t="s">
+      <c r="B124" s="17" t="s">
         <v>153</v>
       </c>
-      <c r="D123" s="19"/>
-      <c r="E123" s="19"/>
-      <c r="F123" s="44"/>
-      <c r="G123" s="44" t="str">
-        <f t="shared" ref="G123" si="22">IF(ISBLANK(F123)," - ",IF(H123=0,F123,F123+H123-1))</f>
+      <c r="D124" s="19"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="44"/>
+      <c r="G124" s="44" t="str">
+        <f t="shared" ref="G124" si="22">IF(ISBLANK(F124)," - ",IF(H124=0,F124,F124+H124-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H123" s="20"/>
-      <c r="I123" s="21"/>
-      <c r="J123" s="22" t="str">
-        <f t="shared" ref="J123" si="23">IF(OR(G123=0,F123=0)," - ",NETWORKDAYS(F123,G123))</f>
+      <c r="H124" s="20"/>
+      <c r="I124" s="21"/>
+      <c r="J124" s="22" t="str">
+        <f t="shared" ref="J124" si="23">IF(OR(G124=0,F124=0)," - ",NETWORKDAYS(F124,G124))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K123" s="41"/>
-      <c r="L123" s="48"/>
-      <c r="M123" s="48"/>
-      <c r="N123" s="48"/>
-      <c r="O123" s="48"/>
-      <c r="P123" s="48"/>
-      <c r="Q123" s="48"/>
-      <c r="R123" s="48"/>
-      <c r="S123" s="48"/>
-      <c r="T123" s="48"/>
-      <c r="U123" s="48"/>
-      <c r="V123" s="48"/>
-      <c r="W123" s="48"/>
-      <c r="X123" s="48"/>
-      <c r="Y123" s="48"/>
-      <c r="Z123" s="48"/>
-      <c r="AA123" s="48"/>
-      <c r="AB123" s="48"/>
-      <c r="AC123" s="48"/>
-      <c r="AD123" s="48"/>
-      <c r="AE123" s="48"/>
-      <c r="AF123" s="48"/>
-      <c r="AG123" s="48"/>
-      <c r="AH123" s="48"/>
-      <c r="AI123" s="48"/>
-      <c r="AJ123" s="48"/>
-      <c r="AK123" s="48"/>
-      <c r="AL123" s="48"/>
-      <c r="AM123" s="48"/>
-      <c r="AN123" s="48"/>
-      <c r="AO123" s="48"/>
-      <c r="AP123" s="48"/>
-      <c r="AQ123" s="48"/>
-      <c r="AR123" s="48"/>
-      <c r="AS123" s="48"/>
-      <c r="AT123" s="48"/>
-      <c r="AU123" s="48"/>
-      <c r="AV123" s="48"/>
-      <c r="AW123" s="48"/>
-      <c r="AX123" s="48"/>
-      <c r="AY123" s="48"/>
-      <c r="AZ123" s="48"/>
-      <c r="BA123" s="48"/>
-      <c r="BB123" s="48"/>
-      <c r="BC123" s="48"/>
-      <c r="BD123" s="48"/>
-      <c r="BE123" s="48"/>
-      <c r="BF123" s="48"/>
-      <c r="BG123" s="48"/>
-      <c r="BH123" s="48"/>
-      <c r="BI123" s="48"/>
-      <c r="BJ123" s="48"/>
-      <c r="BK123" s="48"/>
-      <c r="BL123" s="48"/>
-      <c r="BM123" s="48"/>
-      <c r="BN123" s="48"/>
-      <c r="BO123" s="48"/>
-    </row>
-    <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>12.1</v>
-      </c>
-      <c r="B124" s="65" t="s">
-        <v>130</v>
-      </c>
-      <c r="D124" s="70"/>
-      <c r="E124" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F124" s="42">
-        <v>44449</v>
-      </c>
-      <c r="G124" s="43">
-        <v>44454</v>
-      </c>
-      <c r="H124" s="73"/>
-      <c r="I124" s="26"/>
-      <c r="J124" s="75"/>
-      <c r="K124" s="76"/>
-      <c r="L124" s="46"/>
-      <c r="M124" s="46"/>
-      <c r="N124" s="46"/>
-      <c r="O124" s="46"/>
-      <c r="P124" s="46"/>
-      <c r="Q124" s="46"/>
-      <c r="R124" s="46"/>
-      <c r="S124" s="46"/>
-      <c r="T124" s="46"/>
-      <c r="U124" s="46"/>
-      <c r="V124" s="46"/>
-      <c r="W124" s="46"/>
-      <c r="X124" s="46"/>
-      <c r="Y124" s="46"/>
-      <c r="Z124" s="46"/>
-      <c r="AA124" s="46"/>
-      <c r="AB124" s="46"/>
-      <c r="AC124" s="46"/>
-      <c r="AD124" s="46"/>
-      <c r="AE124" s="46"/>
-      <c r="AF124" s="46"/>
-      <c r="AG124" s="46"/>
-      <c r="AH124" s="46"/>
-      <c r="AI124" s="46"/>
-      <c r="AJ124" s="46"/>
-      <c r="AK124" s="46"/>
-      <c r="AL124" s="46"/>
-      <c r="AM124" s="46"/>
-      <c r="AN124" s="46"/>
-      <c r="AO124" s="46"/>
-      <c r="AP124" s="46"/>
-      <c r="AQ124" s="46"/>
-      <c r="AR124" s="46"/>
-      <c r="AS124" s="46"/>
-      <c r="AT124" s="46"/>
-      <c r="AU124" s="46"/>
-      <c r="AV124" s="46"/>
-      <c r="AW124" s="46"/>
-      <c r="AX124" s="46"/>
-      <c r="AY124" s="46"/>
-      <c r="AZ124" s="46"/>
-      <c r="BA124" s="46"/>
-      <c r="BB124" s="46"/>
-      <c r="BC124" s="46"/>
-      <c r="BD124" s="46"/>
-      <c r="BE124" s="46"/>
-      <c r="BF124" s="46"/>
-      <c r="BG124" s="46"/>
-      <c r="BH124" s="46"/>
-      <c r="BI124" s="46"/>
-      <c r="BJ124" s="46"/>
-      <c r="BK124" s="46"/>
-      <c r="BL124" s="46"/>
-      <c r="BM124" s="46"/>
-      <c r="BN124" s="46"/>
-      <c r="BO124" s="46"/>
+      <c r="K124" s="41"/>
+      <c r="L124" s="48"/>
+      <c r="M124" s="48"/>
+      <c r="N124" s="48"/>
+      <c r="O124" s="48"/>
+      <c r="P124" s="48"/>
+      <c r="Q124" s="48"/>
+      <c r="R124" s="48"/>
+      <c r="S124" s="48"/>
+      <c r="T124" s="48"/>
+      <c r="U124" s="48"/>
+      <c r="V124" s="48"/>
+      <c r="W124" s="48"/>
+      <c r="X124" s="48"/>
+      <c r="Y124" s="48"/>
+      <c r="Z124" s="48"/>
+      <c r="AA124" s="48"/>
+      <c r="AB124" s="48"/>
+      <c r="AC124" s="48"/>
+      <c r="AD124" s="48"/>
+      <c r="AE124" s="48"/>
+      <c r="AF124" s="48"/>
+      <c r="AG124" s="48"/>
+      <c r="AH124" s="48"/>
+      <c r="AI124" s="48"/>
+      <c r="AJ124" s="48"/>
+      <c r="AK124" s="48"/>
+      <c r="AL124" s="48"/>
+      <c r="AM124" s="48"/>
+      <c r="AN124" s="48"/>
+      <c r="AO124" s="48"/>
+      <c r="AP124" s="48"/>
+      <c r="AQ124" s="48"/>
+      <c r="AR124" s="48"/>
+      <c r="AS124" s="48"/>
+      <c r="AT124" s="48"/>
+      <c r="AU124" s="48"/>
+      <c r="AV124" s="48"/>
+      <c r="AW124" s="48"/>
+      <c r="AX124" s="48"/>
+      <c r="AY124" s="48"/>
+      <c r="AZ124" s="48"/>
+      <c r="BA124" s="48"/>
+      <c r="BB124" s="48"/>
+      <c r="BC124" s="48"/>
+      <c r="BD124" s="48"/>
+      <c r="BE124" s="48"/>
+      <c r="BF124" s="48"/>
+      <c r="BG124" s="48"/>
+      <c r="BH124" s="48"/>
+      <c r="BI124" s="48"/>
+      <c r="BJ124" s="48"/>
+      <c r="BK124" s="48"/>
+      <c r="BL124" s="48"/>
+      <c r="BM124" s="48"/>
+      <c r="BN124" s="48"/>
+      <c r="BO124" s="48"/>
     </row>
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
+        <v>12.1</v>
       </c>
       <c r="B125" s="65" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="D125" s="70"/>
       <c r="E125" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F125" s="42">
         <v>44449</v>
@@ -13845,9 +13850,7 @@
         <v>44454</v>
       </c>
       <c r="H125" s="73"/>
-      <c r="I125" s="26">
-        <v>0.3</v>
-      </c>
+      <c r="I125" s="26"/>
       <c r="J125" s="75"/>
       <c r="K125" s="76"/>
       <c r="L125" s="46"/>
@@ -13910,10 +13913,10 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.3</v>
+        <v>12.2</v>
       </c>
       <c r="B126" s="65" t="s">
-        <v>132</v>
+        <v>144</v>
       </c>
       <c r="D126" s="70"/>
       <c r="E126" s="66" t="s">
@@ -13926,7 +13929,9 @@
         <v>44454</v>
       </c>
       <c r="H126" s="73"/>
-      <c r="I126" s="26"/>
+      <c r="I126" s="26">
+        <v>0.3</v>
+      </c>
       <c r="J126" s="75"/>
       <c r="K126" s="76"/>
       <c r="L126" s="46"/>
@@ -13989,10 +13994,10 @@
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.4</v>
+        <v>12.3</v>
       </c>
       <c r="B127" s="65" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="D127" s="70"/>
       <c r="E127" s="66" t="s">
@@ -14068,23 +14073,23 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.5</v>
+        <v>12.4</v>
       </c>
       <c r="B128" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D128" s="70"/>
-      <c r="E128" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F128" s="71">
+      <c r="E128" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F128" s="42">
         <v>44449</v>
       </c>
-      <c r="G128" s="72">
+      <c r="G128" s="43">
         <v>44454</v>
       </c>
       <c r="H128" s="73"/>
-      <c r="I128" s="74"/>
+      <c r="I128" s="26"/>
       <c r="J128" s="75"/>
       <c r="K128" s="76"/>
       <c r="L128" s="46"/>
@@ -14144,173 +14149,175 @@
       <c r="BN128" s="46"/>
       <c r="BO128" s="46"/>
     </row>
-    <row r="129" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A129" s="16" t="str">
+    <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.5</v>
+      </c>
+      <c r="B129" s="65" t="s">
+        <v>143</v>
+      </c>
+      <c r="D129" s="70"/>
+      <c r="E129" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F129" s="71">
+        <v>44449</v>
+      </c>
+      <c r="G129" s="72">
+        <v>44454</v>
+      </c>
+      <c r="H129" s="73"/>
+      <c r="I129" s="74"/>
+      <c r="J129" s="75"/>
+      <c r="K129" s="76"/>
+      <c r="L129" s="46"/>
+      <c r="M129" s="46"/>
+      <c r="N129" s="46"/>
+      <c r="O129" s="46"/>
+      <c r="P129" s="46"/>
+      <c r="Q129" s="46"/>
+      <c r="R129" s="46"/>
+      <c r="S129" s="46"/>
+      <c r="T129" s="46"/>
+      <c r="U129" s="46"/>
+      <c r="V129" s="46"/>
+      <c r="W129" s="46"/>
+      <c r="X129" s="46"/>
+      <c r="Y129" s="46"/>
+      <c r="Z129" s="46"/>
+      <c r="AA129" s="46"/>
+      <c r="AB129" s="46"/>
+      <c r="AC129" s="46"/>
+      <c r="AD129" s="46"/>
+      <c r="AE129" s="46"/>
+      <c r="AF129" s="46"/>
+      <c r="AG129" s="46"/>
+      <c r="AH129" s="46"/>
+      <c r="AI129" s="46"/>
+      <c r="AJ129" s="46"/>
+      <c r="AK129" s="46"/>
+      <c r="AL129" s="46"/>
+      <c r="AM129" s="46"/>
+      <c r="AN129" s="46"/>
+      <c r="AO129" s="46"/>
+      <c r="AP129" s="46"/>
+      <c r="AQ129" s="46"/>
+      <c r="AR129" s="46"/>
+      <c r="AS129" s="46"/>
+      <c r="AT129" s="46"/>
+      <c r="AU129" s="46"/>
+      <c r="AV129" s="46"/>
+      <c r="AW129" s="46"/>
+      <c r="AX129" s="46"/>
+      <c r="AY129" s="46"/>
+      <c r="AZ129" s="46"/>
+      <c r="BA129" s="46"/>
+      <c r="BB129" s="46"/>
+      <c r="BC129" s="46"/>
+      <c r="BD129" s="46"/>
+      <c r="BE129" s="46"/>
+      <c r="BF129" s="46"/>
+      <c r="BG129" s="46"/>
+      <c r="BH129" s="46"/>
+      <c r="BI129" s="46"/>
+      <c r="BJ129" s="46"/>
+      <c r="BK129" s="46"/>
+      <c r="BL129" s="46"/>
+      <c r="BM129" s="46"/>
+      <c r="BN129" s="46"/>
+      <c r="BO129" s="46"/>
+    </row>
+    <row r="130" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>13</v>
       </c>
-      <c r="B129" s="17" t="s">
+      <c r="B130" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D129" s="19"/>
-      <c r="E129" s="19"/>
-      <c r="F129" s="44"/>
-      <c r="G129" s="44" t="str">
-        <f t="shared" ref="G129" si="24">IF(ISBLANK(F129)," - ",IF(H129=0,F129,F129+H129-1))</f>
+      <c r="D130" s="19"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="44"/>
+      <c r="G130" s="44" t="str">
+        <f t="shared" ref="G130" si="24">IF(ISBLANK(F130)," - ",IF(H130=0,F130,F130+H130-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H129" s="20"/>
-      <c r="I129" s="21"/>
-      <c r="J129" s="22" t="str">
-        <f t="shared" ref="J129" si="25">IF(OR(G129=0,F129=0)," - ",NETWORKDAYS(F129,G129))</f>
+      <c r="H130" s="20"/>
+      <c r="I130" s="21"/>
+      <c r="J130" s="22" t="str">
+        <f t="shared" ref="J130" si="25">IF(OR(G130=0,F130=0)," - ",NETWORKDAYS(F130,G130))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K129" s="41"/>
-      <c r="L129" s="48"/>
-      <c r="M129" s="48"/>
-      <c r="N129" s="48"/>
-      <c r="O129" s="48"/>
-      <c r="P129" s="48"/>
-      <c r="Q129" s="48"/>
-      <c r="R129" s="48"/>
-      <c r="S129" s="48"/>
-      <c r="T129" s="48"/>
-      <c r="U129" s="48"/>
-      <c r="V129" s="48"/>
-      <c r="W129" s="48"/>
-      <c r="X129" s="48"/>
-      <c r="Y129" s="48"/>
-      <c r="Z129" s="48"/>
-      <c r="AA129" s="48"/>
-      <c r="AB129" s="48"/>
-      <c r="AC129" s="48"/>
-      <c r="AD129" s="48"/>
-      <c r="AE129" s="48"/>
-      <c r="AF129" s="48"/>
-      <c r="AG129" s="48"/>
-      <c r="AH129" s="48"/>
-      <c r="AI129" s="48"/>
-      <c r="AJ129" s="48"/>
-      <c r="AK129" s="48"/>
-      <c r="AL129" s="48"/>
-      <c r="AM129" s="48"/>
-      <c r="AN129" s="48"/>
-      <c r="AO129" s="48"/>
-      <c r="AP129" s="48"/>
-      <c r="AQ129" s="48"/>
-      <c r="AR129" s="48"/>
-      <c r="AS129" s="48"/>
-      <c r="AT129" s="48"/>
-      <c r="AU129" s="48"/>
-      <c r="AV129" s="48"/>
-      <c r="AW129" s="48"/>
-      <c r="AX129" s="48"/>
-      <c r="AY129" s="48"/>
-      <c r="AZ129" s="48"/>
-      <c r="BA129" s="48"/>
-      <c r="BB129" s="48"/>
-      <c r="BC129" s="48"/>
-      <c r="BD129" s="48"/>
-      <c r="BE129" s="48"/>
-      <c r="BF129" s="48"/>
-      <c r="BG129" s="48"/>
-      <c r="BH129" s="48"/>
-      <c r="BI129" s="48"/>
-      <c r="BJ129" s="48"/>
-      <c r="BK129" s="48"/>
-      <c r="BL129" s="48"/>
-      <c r="BM129" s="48"/>
-      <c r="BN129" s="48"/>
-      <c r="BO129" s="48"/>
-    </row>
-    <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.1</v>
-      </c>
-      <c r="B130" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D130" s="70"/>
-      <c r="E130" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F130" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G130" s="43"/>
-      <c r="H130" s="25"/>
-      <c r="I130" s="26"/>
-      <c r="J130" s="27"/>
-      <c r="K130" s="40"/>
-      <c r="L130" s="46"/>
-      <c r="M130" s="46"/>
-      <c r="N130" s="46"/>
-      <c r="O130" s="46"/>
-      <c r="P130" s="46"/>
-      <c r="Q130" s="46"/>
-      <c r="R130" s="46"/>
-      <c r="S130" s="46"/>
-      <c r="T130" s="46"/>
-      <c r="U130" s="46"/>
-      <c r="V130" s="46"/>
-      <c r="W130" s="46"/>
-      <c r="X130" s="46"/>
-      <c r="Y130" s="46"/>
-      <c r="Z130" s="46"/>
-      <c r="AA130" s="46"/>
-      <c r="AB130" s="46"/>
-      <c r="AC130" s="46"/>
-      <c r="AD130" s="46"/>
-      <c r="AE130" s="46"/>
-      <c r="AF130" s="46"/>
-      <c r="AG130" s="46"/>
-      <c r="AH130" s="46"/>
-      <c r="AI130" s="46"/>
-      <c r="AJ130" s="46"/>
-      <c r="AK130" s="46"/>
-      <c r="AL130" s="46"/>
-      <c r="AM130" s="46"/>
-      <c r="AN130" s="46"/>
-      <c r="AO130" s="46"/>
-      <c r="AP130" s="46"/>
-      <c r="AQ130" s="46"/>
-      <c r="AR130" s="46"/>
-      <c r="AS130" s="46"/>
-      <c r="AT130" s="46"/>
-      <c r="AU130" s="46"/>
-      <c r="AV130" s="46"/>
-      <c r="AW130" s="46"/>
-      <c r="AX130" s="46"/>
-      <c r="AY130" s="46"/>
-      <c r="AZ130" s="46"/>
-      <c r="BA130" s="46"/>
-      <c r="BB130" s="46"/>
-      <c r="BC130" s="46"/>
-      <c r="BD130" s="46"/>
-      <c r="BE130" s="46"/>
-      <c r="BF130" s="46"/>
-      <c r="BG130" s="46"/>
-      <c r="BH130" s="46"/>
-      <c r="BI130" s="46"/>
-      <c r="BJ130" s="46"/>
-      <c r="BK130" s="46"/>
-      <c r="BL130" s="46"/>
-      <c r="BM130" s="46"/>
-      <c r="BN130" s="46"/>
-      <c r="BO130" s="46"/>
+      <c r="K130" s="41"/>
+      <c r="L130" s="48"/>
+      <c r="M130" s="48"/>
+      <c r="N130" s="48"/>
+      <c r="O130" s="48"/>
+      <c r="P130" s="48"/>
+      <c r="Q130" s="48"/>
+      <c r="R130" s="48"/>
+      <c r="S130" s="48"/>
+      <c r="T130" s="48"/>
+      <c r="U130" s="48"/>
+      <c r="V130" s="48"/>
+      <c r="W130" s="48"/>
+      <c r="X130" s="48"/>
+      <c r="Y130" s="48"/>
+      <c r="Z130" s="48"/>
+      <c r="AA130" s="48"/>
+      <c r="AB130" s="48"/>
+      <c r="AC130" s="48"/>
+      <c r="AD130" s="48"/>
+      <c r="AE130" s="48"/>
+      <c r="AF130" s="48"/>
+      <c r="AG130" s="48"/>
+      <c r="AH130" s="48"/>
+      <c r="AI130" s="48"/>
+      <c r="AJ130" s="48"/>
+      <c r="AK130" s="48"/>
+      <c r="AL130" s="48"/>
+      <c r="AM130" s="48"/>
+      <c r="AN130" s="48"/>
+      <c r="AO130" s="48"/>
+      <c r="AP130" s="48"/>
+      <c r="AQ130" s="48"/>
+      <c r="AR130" s="48"/>
+      <c r="AS130" s="48"/>
+      <c r="AT130" s="48"/>
+      <c r="AU130" s="48"/>
+      <c r="AV130" s="48"/>
+      <c r="AW130" s="48"/>
+      <c r="AX130" s="48"/>
+      <c r="AY130" s="48"/>
+      <c r="AZ130" s="48"/>
+      <c r="BA130" s="48"/>
+      <c r="BB130" s="48"/>
+      <c r="BC130" s="48"/>
+      <c r="BD130" s="48"/>
+      <c r="BE130" s="48"/>
+      <c r="BF130" s="48"/>
+      <c r="BG130" s="48"/>
+      <c r="BH130" s="48"/>
+      <c r="BI130" s="48"/>
+      <c r="BJ130" s="48"/>
+      <c r="BK130" s="48"/>
+      <c r="BL130" s="48"/>
+      <c r="BM130" s="48"/>
+      <c r="BN130" s="48"/>
+      <c r="BO130" s="48"/>
     </row>
     <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="B131" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D131" s="70"/>
       <c r="E131" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F131" s="42">
         <v>44379</v>
@@ -14380,14 +14387,14 @@
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D132" s="70"/>
       <c r="E132" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F132" s="42">
         <v>44379</v>
@@ -14457,10 +14464,10 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
@@ -14534,17 +14541,17 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B134" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D134" s="66"/>
+        <v>13.4</v>
+      </c>
+      <c r="B134" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F134" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G134" s="43"/>
       <c r="H134" s="25"/>
@@ -14609,11 +14616,20 @@
       <c r="BO134" s="46"/>
     </row>
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="23"/>
-      <c r="B135" s="65"/>
+      <c r="A135" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B135" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D135" s="66"/>
-      <c r="E135" s="66"/>
-      <c r="F135" s="42"/>
+      <c r="E135" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F135" s="42">
+        <v>44531</v>
+      </c>
       <c r="G135" s="43"/>
       <c r="H135" s="25"/>
       <c r="I135" s="26"/>
@@ -14815,7 +14831,7 @@
     <row r="138" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="23"/>
       <c r="B138" s="65"/>
-      <c r="D138" s="70"/>
+      <c r="D138" s="66"/>
       <c r="E138" s="66"/>
       <c r="F138" s="42"/>
       <c r="G138" s="43"/>
@@ -15155,7 +15171,7 @@
     <row r="143" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23"/>
       <c r="B143" s="65"/>
-      <c r="D143" s="66"/>
+      <c r="D143" s="70"/>
       <c r="E143" s="66"/>
       <c r="F143" s="42"/>
       <c r="G143" s="43"/>
@@ -15427,7 +15443,7 @@
     <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="23"/>
       <c r="B147" s="65"/>
-      <c r="D147" s="70"/>
+      <c r="D147" s="66"/>
       <c r="E147" s="66"/>
       <c r="F147" s="42"/>
       <c r="G147" s="43"/>
@@ -15767,7 +15783,7 @@
     <row r="152" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="23"/>
       <c r="B152" s="65"/>
-      <c r="D152" s="66"/>
+      <c r="D152" s="70"/>
       <c r="E152" s="66"/>
       <c r="F152" s="42"/>
       <c r="G152" s="43"/>
@@ -16039,7 +16055,7 @@
     <row r="156" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="23"/>
       <c r="B156" s="65"/>
-      <c r="D156" s="70"/>
+      <c r="D156" s="66"/>
       <c r="E156" s="66"/>
       <c r="F156" s="42"/>
       <c r="G156" s="43"/>
@@ -16379,7 +16395,7 @@
     <row r="161" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="23"/>
       <c r="B161" s="65"/>
-      <c r="D161" s="66"/>
+      <c r="D161" s="70"/>
       <c r="E161" s="66"/>
       <c r="F161" s="42"/>
       <c r="G161" s="43"/>
@@ -16651,7 +16667,7 @@
     <row r="165" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="23"/>
       <c r="B165" s="65"/>
-      <c r="D165" s="70"/>
+      <c r="D165" s="66"/>
       <c r="E165" s="66"/>
       <c r="F165" s="42"/>
       <c r="G165" s="43"/>
@@ -16988,18 +17004,77 @@
       <c r="BN169" s="46"/>
       <c r="BO169" s="46"/>
     </row>
+    <row r="170" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="23"/>
+      <c r="B170" s="65"/>
+      <c r="D170" s="70"/>
+      <c r="E170" s="66"/>
+      <c r="F170" s="42"/>
+      <c r="G170" s="43"/>
+      <c r="H170" s="25"/>
+      <c r="I170" s="26"/>
+      <c r="J170" s="27"/>
+      <c r="K170" s="40"/>
+      <c r="L170" s="46"/>
+      <c r="M170" s="46"/>
+      <c r="N170" s="46"/>
+      <c r="O170" s="46"/>
+      <c r="P170" s="46"/>
+      <c r="Q170" s="46"/>
+      <c r="R170" s="46"/>
+      <c r="S170" s="46"/>
+      <c r="T170" s="46"/>
+      <c r="U170" s="46"/>
+      <c r="V170" s="46"/>
+      <c r="W170" s="46"/>
+      <c r="X170" s="46"/>
+      <c r="Y170" s="46"/>
+      <c r="Z170" s="46"/>
+      <c r="AA170" s="46"/>
+      <c r="AB170" s="46"/>
+      <c r="AC170" s="46"/>
+      <c r="AD170" s="46"/>
+      <c r="AE170" s="46"/>
+      <c r="AF170" s="46"/>
+      <c r="AG170" s="46"/>
+      <c r="AH170" s="46"/>
+      <c r="AI170" s="46"/>
+      <c r="AJ170" s="46"/>
+      <c r="AK170" s="46"/>
+      <c r="AL170" s="46"/>
+      <c r="AM170" s="46"/>
+      <c r="AN170" s="46"/>
+      <c r="AO170" s="46"/>
+      <c r="AP170" s="46"/>
+      <c r="AQ170" s="46"/>
+      <c r="AR170" s="46"/>
+      <c r="AS170" s="46"/>
+      <c r="AT170" s="46"/>
+      <c r="AU170" s="46"/>
+      <c r="AV170" s="46"/>
+      <c r="AW170" s="46"/>
+      <c r="AX170" s="46"/>
+      <c r="AY170" s="46"/>
+      <c r="AZ170" s="46"/>
+      <c r="BA170" s="46"/>
+      <c r="BB170" s="46"/>
+      <c r="BC170" s="46"/>
+      <c r="BD170" s="46"/>
+      <c r="BE170" s="46"/>
+      <c r="BF170" s="46"/>
+      <c r="BG170" s="46"/>
+      <c r="BH170" s="46"/>
+      <c r="BI170" s="46"/>
+      <c r="BJ170" s="46"/>
+      <c r="BK170" s="46"/>
+      <c r="BL170" s="46"/>
+      <c r="BM170" s="46"/>
+      <c r="BN170" s="46"/>
+      <c r="BO170" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17010,9 +17085,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I130:I133 I98:I103 I105:I110 I112:I122 I124:I128">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I123 I125:I129">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17031,7 +17115,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN128 L134:BO136 M137:BN142 BO140:BO142 L143:BO145 M146:BN151 BO149:BO151 L152:BO154 M155:BN160 BO158:BO160 L161:BO163 M164:BN169 BO167:BO169 BO132:BO133 M130:BN133 L129:BO129">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN123 M125:BN129 L135:BO137 M138:BN143 BO141:BO143 L144:BO146 M147:BN152 BO150:BO152 L153:BO155 M156:BN161 BO159:BO161 L162:BO164 M165:BN170 BO168:BO170 BO133:BO134 M131:BN134 L130:BO130">
     <cfRule type="expression" dxfId="134" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -17039,7 +17123,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L130:BO133 L98:BO103 L105:BO110 L112:BO122 L124:BO128">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L131:BO134 L98:BO103 L105:BO110 L112:BO123 L125:BO129">
     <cfRule type="expression" dxfId="132" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -17049,7 +17133,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E170:E1048576 E95:E96 E130:E133 E98:E103 E105:E110 E112:E122 E124:E128">
+  <conditionalFormatting sqref="E1:E73 E171:E1048576 E95:E96 E131:E134 E98:E103 E105:E110 E112:E123 E125:E129">
     <cfRule type="cellIs" dxfId="130" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17143,7 +17227,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I134:I142">
+  <conditionalFormatting sqref="I135:I143">
     <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17157,12 +17241,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L134:BO142">
+  <conditionalFormatting sqref="L135:BO143">
     <cfRule type="expression" dxfId="108" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E134:E142">
+  <conditionalFormatting sqref="E135:E143">
     <cfRule type="cellIs" dxfId="107" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17185,7 +17269,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L137:BO142 L130:BO133 L98:BO103 L105:BO110 L112:BO122 L124:BO128">
+  <conditionalFormatting sqref="L138:BO143 L131:BO134 L98:BO103 L105:BO110 L112:BO123 L125:BO129">
     <cfRule type="expression" dxfId="100" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17193,7 +17277,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I143:I151">
+  <conditionalFormatting sqref="I144:I152">
     <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17207,12 +17291,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L143:BO151">
+  <conditionalFormatting sqref="L144:BO152">
     <cfRule type="expression" dxfId="98" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E143:E151">
+  <conditionalFormatting sqref="E144:E152">
     <cfRule type="cellIs" dxfId="97" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17235,7 +17319,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L146:BO151">
+  <conditionalFormatting sqref="L147:BO152">
     <cfRule type="expression" dxfId="90" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17243,7 +17327,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I152:I160">
+  <conditionalFormatting sqref="I153:I161">
     <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17257,12 +17341,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L152:BO160">
+  <conditionalFormatting sqref="L153:BO161">
     <cfRule type="expression" dxfId="88" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E152:E160">
+  <conditionalFormatting sqref="E153:E161">
     <cfRule type="cellIs" dxfId="87" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17285,7 +17369,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L155:BO160">
+  <conditionalFormatting sqref="L156:BO161">
     <cfRule type="expression" dxfId="80" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17293,7 +17377,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I161:I169">
+  <conditionalFormatting sqref="I162:I170">
     <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17307,12 +17391,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L161:BO169">
+  <conditionalFormatting sqref="L162:BO170">
     <cfRule type="expression" dxfId="78" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E161:E169">
+  <conditionalFormatting sqref="E162:E170">
     <cfRule type="cellIs" dxfId="77" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17335,7 +17419,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L164:BO169">
+  <conditionalFormatting sqref="L165:BO170">
     <cfRule type="expression" dxfId="70" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17485,7 +17569,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I129">
+  <conditionalFormatting sqref="I130">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17499,12 +17583,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L129:BO129">
+  <conditionalFormatting sqref="L130:BO130">
     <cfRule type="expression" dxfId="40" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E129">
+  <conditionalFormatting sqref="E130">
     <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17627,15 +17711,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L123:BO123">
+  <conditionalFormatting sqref="L124:BO124">
     <cfRule type="expression" dxfId="12" priority="10">
-      <formula>AND($F123&lt;=L$6,ROUNDDOWN(($G123-$F123+1)*$I123,0)+$F123-1&gt;=L$6)</formula>
+      <formula>AND($F124&lt;=L$6,ROUNDDOWN(($G124-$F124+1)*$I124,0)+$F124-1&gt;=L$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="11" priority="11">
-      <formula>AND(NOT(ISBLANK($F123)),$F123&lt;=L$6,$G123&gt;=L$6)</formula>
+      <formula>AND(NOT(ISBLANK($F124)),$F124&lt;=L$6,$G124&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123">
+  <conditionalFormatting sqref="I124">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17649,12 +17733,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L123:BO123">
+  <conditionalFormatting sqref="L124:BO124">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E123">
+  <conditionalFormatting sqref="E124">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17733,7 +17817,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I130:I133 I98:I103 I105:I110 I112:I122 I124:I128</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I123 I125:I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17763,7 +17847,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I134:I142</xm:sqref>
+          <xm:sqref>I135:I143</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -17778,7 +17862,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I143:I151</xm:sqref>
+          <xm:sqref>I144:I152</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -17793,7 +17877,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I152:I160</xm:sqref>
+          <xm:sqref>I153:I161</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -17808,7 +17892,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I161:I169</xm:sqref>
+          <xm:sqref>I162:I170</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -17868,7 +17952,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I129</xm:sqref>
+          <xm:sqref>I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">
@@ -17913,7 +17997,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I123</xm:sqref>
+          <xm:sqref>I124</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Updated downside sofr/ffr calcs (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE63E4C-E8FE-4430-9314-897E78DE6B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04863B1-FC09-4D26-B1B8-F0D513652831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1821,13 +1821,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1837,10 +1830,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1849,6 +1838,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3426,8 +3426,8 @@
   <dimension ref="A1:BO170"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3457,27 +3457,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3522,12 +3522,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3537,183 +3537,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44431</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44438</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44445</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44452</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44459</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44466</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44473</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44480</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -13448,7 +13448,7 @@
       </c>
       <c r="H120" s="73"/>
       <c r="I120" s="26">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="J120" s="75"/>
       <c r="K120" s="76"/>
@@ -17075,6 +17075,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17085,15 +17094,6 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I123 I125:I129">

</xml_diff>

<commit_message>
Finalized README and inputs for v0.16 (v0.16)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04863B1-FC09-4D26-B1B8-F0D513652831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4722B2E-5CF1-4651-BC64-28319E10026E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,9 +823,6 @@
     <t>Rework Webpage Nav</t>
   </si>
   <si>
-    <t>Add New Forecasts to Site</t>
-  </si>
-  <si>
     <t>Update Docs</t>
   </si>
   <si>
@@ -893,6 +890,9 @@
   </si>
   <si>
     <t>Add Additional Scenarios</t>
+  </si>
+  <si>
+    <t>Add New Forecasts from SQL</t>
   </si>
 </sst>
 </file>
@@ -1821,6 +1821,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1830,6 +1837,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1838,17 +1849,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1897,7 +1897,7 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="136">
+  <dxfs count="134">
     <dxf>
       <border>
         <left style="thin">
@@ -1984,20 +1984,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -3426,8 +3412,8 @@
   <dimension ref="A1:BO170"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G120" sqref="G120"/>
+      <pane ySplit="7" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T120" sqref="T120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3457,27 +3443,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3522,12 +3508,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3537,183 +3523,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44431</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44438</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44445</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44452</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44459</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44466</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44473</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44480</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -12142,7 +12128,7 @@
         <v>10</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D104" s="19"/>
       <c r="E104" s="19"/>
@@ -12221,7 +12207,7 @@
         <v>10.1</v>
       </c>
       <c r="B105" s="65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D105" s="70"/>
       <c r="E105" s="66" t="s">
@@ -12302,7 +12288,7 @@
         <v>10.2</v>
       </c>
       <c r="B106" s="65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D106" s="70"/>
       <c r="E106" s="66" t="s">
@@ -12383,7 +12369,7 @@
         <v>10.3</v>
       </c>
       <c r="B107" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D107" s="70"/>
       <c r="E107" s="66" t="s">
@@ -12464,11 +12450,11 @@
         <v>10.4</v>
       </c>
       <c r="B108" s="65" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D108" s="70"/>
       <c r="E108" s="66" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F108" s="42">
         <v>44383</v>
@@ -12707,7 +12693,7 @@
         <v>11</v>
       </c>
       <c r="B111" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D111" s="19"/>
       <c r="E111" s="19"/>
@@ -12786,7 +12772,7 @@
         <v>11.1</v>
       </c>
       <c r="B112" s="65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D112" s="70"/>
       <c r="E112" s="66" t="s">
@@ -12867,7 +12853,7 @@
         <v>11.2</v>
       </c>
       <c r="B113" s="65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D113" s="70"/>
       <c r="E113" s="66" t="s">
@@ -12948,7 +12934,7 @@
         <v>11.3</v>
       </c>
       <c r="B114" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D114" s="70"/>
       <c r="E114" s="66" t="s">
@@ -13029,7 +13015,7 @@
         <v>11.4</v>
       </c>
       <c r="B115" s="65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D115" s="70"/>
       <c r="E115" s="66" t="s">
@@ -13110,7 +13096,7 @@
         <v>11.5</v>
       </c>
       <c r="B116" s="65" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D116" s="70"/>
       <c r="E116" s="66" t="s">
@@ -13191,7 +13177,7 @@
         <v>11.6</v>
       </c>
       <c r="B117" s="65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D117" s="70"/>
       <c r="E117" s="66" t="s">
@@ -13272,7 +13258,7 @@
         <v>11.7</v>
       </c>
       <c r="B118" s="65" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D118" s="70"/>
       <c r="E118" s="66" t="s">
@@ -13353,7 +13339,7 @@
         <v>11.8</v>
       </c>
       <c r="B119" s="65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D119" s="70"/>
       <c r="E119" s="66" t="s">
@@ -13434,7 +13420,7 @@
         <v>11.9</v>
       </c>
       <c r="B120" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D120" s="70"/>
       <c r="E120" s="66" t="s">
@@ -13515,7 +13501,7 @@
         <v>11.10</v>
       </c>
       <c r="B121" s="65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D121" s="70"/>
       <c r="E121" s="66" t="s">
@@ -13596,7 +13582,7 @@
         <v>11.11</v>
       </c>
       <c r="B122" s="65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D122" s="70"/>
       <c r="E122" s="66" t="s">
@@ -13606,11 +13592,11 @@
         <v>44437</v>
       </c>
       <c r="G122" s="43">
-        <v>44438</v>
+        <v>44442</v>
       </c>
       <c r="H122" s="73"/>
       <c r="I122" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J122" s="75"/>
       <c r="K122" s="76"/>
@@ -13671,170 +13657,170 @@
       <c r="BN122" s="46"/>
       <c r="BO122" s="46"/>
     </row>
-    <row r="123" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>11.12</v>
-      </c>
-      <c r="B123" s="65" t="s">
-        <v>131</v>
-      </c>
-      <c r="D123" s="70"/>
-      <c r="E123" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F123" s="42">
-        <v>44438</v>
-      </c>
-      <c r="G123" s="43">
-        <v>44442</v>
-      </c>
-      <c r="H123" s="73"/>
-      <c r="I123" s="26">
-        <v>0</v>
-      </c>
-      <c r="J123" s="75"/>
-      <c r="K123" s="76"/>
-      <c r="L123" s="46"/>
-      <c r="M123" s="46"/>
-      <c r="N123" s="46"/>
-      <c r="O123" s="46"/>
-      <c r="P123" s="46"/>
-      <c r="Q123" s="46"/>
-      <c r="R123" s="46"/>
-      <c r="S123" s="46"/>
-      <c r="T123" s="46"/>
-      <c r="U123" s="46"/>
-      <c r="V123" s="46"/>
-      <c r="W123" s="46"/>
-      <c r="X123" s="46"/>
-      <c r="Y123" s="46"/>
-      <c r="Z123" s="46"/>
-      <c r="AA123" s="46"/>
-      <c r="AB123" s="46"/>
-      <c r="AC123" s="46"/>
-      <c r="AD123" s="46"/>
-      <c r="AE123" s="46"/>
-      <c r="AF123" s="46"/>
-      <c r="AG123" s="46"/>
-      <c r="AH123" s="46"/>
-      <c r="AI123" s="46"/>
-      <c r="AJ123" s="46"/>
-      <c r="AK123" s="46"/>
-      <c r="AL123" s="46"/>
-      <c r="AM123" s="46"/>
-      <c r="AN123" s="46"/>
-      <c r="AO123" s="46"/>
-      <c r="AP123" s="46"/>
-      <c r="AQ123" s="46"/>
-      <c r="AR123" s="46"/>
-      <c r="AS123" s="46"/>
-      <c r="AT123" s="46"/>
-      <c r="AU123" s="46"/>
-      <c r="AV123" s="46"/>
-      <c r="AW123" s="46"/>
-      <c r="AX123" s="46"/>
-      <c r="AY123" s="46"/>
-      <c r="AZ123" s="46"/>
-      <c r="BA123" s="46"/>
-      <c r="BB123" s="46"/>
-      <c r="BC123" s="46"/>
-      <c r="BD123" s="46"/>
-      <c r="BE123" s="46"/>
-      <c r="BF123" s="46"/>
-      <c r="BG123" s="46"/>
-      <c r="BH123" s="46"/>
-      <c r="BI123" s="46"/>
-      <c r="BJ123" s="46"/>
-      <c r="BK123" s="46"/>
-      <c r="BL123" s="46"/>
-      <c r="BM123" s="46"/>
-      <c r="BN123" s="46"/>
-      <c r="BO123" s="46"/>
-    </row>
-    <row r="124" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124" s="16" t="str">
+    <row r="123" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B124" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="D124" s="19"/>
-      <c r="E124" s="19"/>
-      <c r="F124" s="44"/>
-      <c r="G124" s="44" t="str">
-        <f t="shared" ref="G124" si="22">IF(ISBLANK(F124)," - ",IF(H124=0,F124,F124+H124-1))</f>
+      <c r="B123" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="44"/>
+      <c r="G123" s="44" t="str">
+        <f t="shared" ref="G123" si="22">IF(ISBLANK(F123)," - ",IF(H123=0,F123,F123+H123-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H124" s="20"/>
-      <c r="I124" s="21"/>
-      <c r="J124" s="22" t="str">
-        <f t="shared" ref="J124" si="23">IF(OR(G124=0,F124=0)," - ",NETWORKDAYS(F124,G124))</f>
+      <c r="H123" s="20"/>
+      <c r="I123" s="21"/>
+      <c r="J123" s="22" t="str">
+        <f t="shared" ref="J123" si="23">IF(OR(G123=0,F123=0)," - ",NETWORKDAYS(F123,G123))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K124" s="41"/>
-      <c r="L124" s="48"/>
-      <c r="M124" s="48"/>
-      <c r="N124" s="48"/>
-      <c r="O124" s="48"/>
-      <c r="P124" s="48"/>
-      <c r="Q124" s="48"/>
-      <c r="R124" s="48"/>
-      <c r="S124" s="48"/>
-      <c r="T124" s="48"/>
-      <c r="U124" s="48"/>
-      <c r="V124" s="48"/>
-      <c r="W124" s="48"/>
-      <c r="X124" s="48"/>
-      <c r="Y124" s="48"/>
-      <c r="Z124" s="48"/>
-      <c r="AA124" s="48"/>
-      <c r="AB124" s="48"/>
-      <c r="AC124" s="48"/>
-      <c r="AD124" s="48"/>
-      <c r="AE124" s="48"/>
-      <c r="AF124" s="48"/>
-      <c r="AG124" s="48"/>
-      <c r="AH124" s="48"/>
-      <c r="AI124" s="48"/>
-      <c r="AJ124" s="48"/>
-      <c r="AK124" s="48"/>
-      <c r="AL124" s="48"/>
-      <c r="AM124" s="48"/>
-      <c r="AN124" s="48"/>
-      <c r="AO124" s="48"/>
-      <c r="AP124" s="48"/>
-      <c r="AQ124" s="48"/>
-      <c r="AR124" s="48"/>
-      <c r="AS124" s="48"/>
-      <c r="AT124" s="48"/>
-      <c r="AU124" s="48"/>
-      <c r="AV124" s="48"/>
-      <c r="AW124" s="48"/>
-      <c r="AX124" s="48"/>
-      <c r="AY124" s="48"/>
-      <c r="AZ124" s="48"/>
-      <c r="BA124" s="48"/>
-      <c r="BB124" s="48"/>
-      <c r="BC124" s="48"/>
-      <c r="BD124" s="48"/>
-      <c r="BE124" s="48"/>
-      <c r="BF124" s="48"/>
-      <c r="BG124" s="48"/>
-      <c r="BH124" s="48"/>
-      <c r="BI124" s="48"/>
-      <c r="BJ124" s="48"/>
-      <c r="BK124" s="48"/>
-      <c r="BL124" s="48"/>
-      <c r="BM124" s="48"/>
-      <c r="BN124" s="48"/>
-      <c r="BO124" s="48"/>
+      <c r="K123" s="41"/>
+      <c r="L123" s="48"/>
+      <c r="M123" s="48"/>
+      <c r="N123" s="48"/>
+      <c r="O123" s="48"/>
+      <c r="P123" s="48"/>
+      <c r="Q123" s="48"/>
+      <c r="R123" s="48"/>
+      <c r="S123" s="48"/>
+      <c r="T123" s="48"/>
+      <c r="U123" s="48"/>
+      <c r="V123" s="48"/>
+      <c r="W123" s="48"/>
+      <c r="X123" s="48"/>
+      <c r="Y123" s="48"/>
+      <c r="Z123" s="48"/>
+      <c r="AA123" s="48"/>
+      <c r="AB123" s="48"/>
+      <c r="AC123" s="48"/>
+      <c r="AD123" s="48"/>
+      <c r="AE123" s="48"/>
+      <c r="AF123" s="48"/>
+      <c r="AG123" s="48"/>
+      <c r="AH123" s="48"/>
+      <c r="AI123" s="48"/>
+      <c r="AJ123" s="48"/>
+      <c r="AK123" s="48"/>
+      <c r="AL123" s="48"/>
+      <c r="AM123" s="48"/>
+      <c r="AN123" s="48"/>
+      <c r="AO123" s="48"/>
+      <c r="AP123" s="48"/>
+      <c r="AQ123" s="48"/>
+      <c r="AR123" s="48"/>
+      <c r="AS123" s="48"/>
+      <c r="AT123" s="48"/>
+      <c r="AU123" s="48"/>
+      <c r="AV123" s="48"/>
+      <c r="AW123" s="48"/>
+      <c r="AX123" s="48"/>
+      <c r="AY123" s="48"/>
+      <c r="AZ123" s="48"/>
+      <c r="BA123" s="48"/>
+      <c r="BB123" s="48"/>
+      <c r="BC123" s="48"/>
+      <c r="BD123" s="48"/>
+      <c r="BE123" s="48"/>
+      <c r="BF123" s="48"/>
+      <c r="BG123" s="48"/>
+      <c r="BH123" s="48"/>
+      <c r="BI123" s="48"/>
+      <c r="BJ123" s="48"/>
+      <c r="BK123" s="48"/>
+      <c r="BL123" s="48"/>
+      <c r="BM123" s="48"/>
+      <c r="BN123" s="48"/>
+      <c r="BO123" s="48"/>
+    </row>
+    <row r="124" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.1</v>
+      </c>
+      <c r="B124" s="65" t="s">
+        <v>154</v>
+      </c>
+      <c r="D124" s="70"/>
+      <c r="E124" s="66" t="s">
+        <v>69</v>
+      </c>
+      <c r="F124" s="42">
+        <v>44443</v>
+      </c>
+      <c r="G124" s="43">
+        <v>44446</v>
+      </c>
+      <c r="H124" s="73"/>
+      <c r="I124" s="26">
+        <v>0</v>
+      </c>
+      <c r="J124" s="75"/>
+      <c r="K124" s="76"/>
+      <c r="L124" s="46"/>
+      <c r="M124" s="46"/>
+      <c r="N124" s="46"/>
+      <c r="O124" s="46"/>
+      <c r="P124" s="46"/>
+      <c r="Q124" s="46"/>
+      <c r="R124" s="46"/>
+      <c r="S124" s="46"/>
+      <c r="T124" s="46"/>
+      <c r="U124" s="46"/>
+      <c r="V124" s="46"/>
+      <c r="W124" s="46"/>
+      <c r="X124" s="46"/>
+      <c r="Y124" s="46"/>
+      <c r="Z124" s="46"/>
+      <c r="AA124" s="46"/>
+      <c r="AB124" s="46"/>
+      <c r="AC124" s="46"/>
+      <c r="AD124" s="46"/>
+      <c r="AE124" s="46"/>
+      <c r="AF124" s="46"/>
+      <c r="AG124" s="46"/>
+      <c r="AH124" s="46"/>
+      <c r="AI124" s="46"/>
+      <c r="AJ124" s="46"/>
+      <c r="AK124" s="46"/>
+      <c r="AL124" s="46"/>
+      <c r="AM124" s="46"/>
+      <c r="AN124" s="46"/>
+      <c r="AO124" s="46"/>
+      <c r="AP124" s="46"/>
+      <c r="AQ124" s="46"/>
+      <c r="AR124" s="46"/>
+      <c r="AS124" s="46"/>
+      <c r="AT124" s="46"/>
+      <c r="AU124" s="46"/>
+      <c r="AV124" s="46"/>
+      <c r="AW124" s="46"/>
+      <c r="AX124" s="46"/>
+      <c r="AY124" s="46"/>
+      <c r="AZ124" s="46"/>
+      <c r="BA124" s="46"/>
+      <c r="BB124" s="46"/>
+      <c r="BC124" s="46"/>
+      <c r="BD124" s="46"/>
+      <c r="BE124" s="46"/>
+      <c r="BF124" s="46"/>
+      <c r="BG124" s="46"/>
+      <c r="BH124" s="46"/>
+      <c r="BI124" s="46"/>
+      <c r="BJ124" s="46"/>
+      <c r="BK124" s="46"/>
+      <c r="BL124" s="46"/>
+      <c r="BM124" s="46"/>
+      <c r="BN124" s="46"/>
+      <c r="BO124" s="46"/>
     </row>
     <row r="125" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.1</v>
+        <v>12.2</v>
       </c>
       <c r="B125" s="65" t="s">
         <v>130</v>
@@ -13844,13 +13830,15 @@
         <v>70</v>
       </c>
       <c r="F125" s="42">
+        <v>44445</v>
+      </c>
+      <c r="G125" s="43">
         <v>44449</v>
       </c>
-      <c r="G125" s="43">
-        <v>44454</v>
-      </c>
       <c r="H125" s="73"/>
-      <c r="I125" s="26"/>
+      <c r="I125" s="26">
+        <v>0</v>
+      </c>
       <c r="J125" s="75"/>
       <c r="K125" s="76"/>
       <c r="L125" s="46"/>
@@ -13913,10 +13901,10 @@
     <row r="126" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.2</v>
+        <v>12.3</v>
       </c>
       <c r="B126" s="65" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D126" s="70"/>
       <c r="E126" s="66" t="s">
@@ -13994,10 +13982,10 @@
     <row r="127" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.3</v>
+        <v>12.4</v>
       </c>
       <c r="B127" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D127" s="70"/>
       <c r="E127" s="66" t="s">
@@ -14073,10 +14061,10 @@
     <row r="128" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.4</v>
+        <v>12.5</v>
       </c>
       <c r="B128" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D128" s="70"/>
       <c r="E128" s="66" t="s">
@@ -14152,10 +14140,10 @@
     <row r="129" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>12.5</v>
+        <v>12.6</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D129" s="70"/>
       <c r="E129" s="70" t="s">
@@ -17075,15 +17063,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17094,9 +17073,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I123 I125:I129">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I122 I124:I129">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17111,61 +17099,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="135" priority="290">
+    <cfRule type="expression" dxfId="133" priority="290">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN123 M125:BN129 L135:BO137 M138:BN143 BO141:BO143 L144:BO146 M147:BN152 BO150:BO152 L153:BO155 M156:BN161 BO159:BO161 L162:BO164 M165:BN170 BO168:BO170 BO133:BO134 M131:BN134 L130:BO130">
-    <cfRule type="expression" dxfId="134" priority="293">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN129 L135:BO137 M138:BN143 BO141:BO143 L144:BO146 M147:BN152 BO150:BO152 L153:BO155 M156:BN161 BO159:BO161 L162:BO164 M165:BN170 BO168:BO170 BO133:BO134 M131:BN134 L130:BO130 L123:BO123">
+    <cfRule type="expression" dxfId="132" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="294">
+    <cfRule type="expression" dxfId="131" priority="294">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L131:BO134 L98:BO103 L105:BO110 L112:BO123 L125:BO129">
-    <cfRule type="expression" dxfId="132" priority="253">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L131:BO134 L98:BO103 L105:BO110 L112:BO122 L124:BO129">
+    <cfRule type="expression" dxfId="130" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="131" priority="243">
+    <cfRule type="expression" dxfId="129" priority="243">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E171:E1048576 E95:E96 E131:E134 E98:E103 E105:E110 E112:E123 E125:E129">
-    <cfRule type="cellIs" dxfId="130" priority="234" operator="equal">
+  <conditionalFormatting sqref="E1:E73 E171:E1048576 E95:E96 E131:E134 E98:E103 E105:E110 E112:E122 E124:E129">
+    <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="236" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="237" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="238" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="239" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="240" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="241" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="123" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="235" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="122" priority="299">
+    <cfRule type="expression" dxfId="120" priority="299">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="300">
+    <cfRule type="expression" dxfId="119" priority="300">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17184,46 +17172,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="120" priority="230">
+    <cfRule type="expression" dxfId="118" priority="230">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="231">
+    <cfRule type="expression" dxfId="117" priority="231">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="118" priority="228">
+    <cfRule type="expression" dxfId="116" priority="228">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="117" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="221" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="222" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="223" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="224" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="225" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="226" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="227" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="110" priority="232">
+    <cfRule type="expression" dxfId="108" priority="232">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="233">
+    <cfRule type="expression" dxfId="107" priority="233">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17242,38 +17230,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L135:BO143">
-    <cfRule type="expression" dxfId="108" priority="137">
+    <cfRule type="expression" dxfId="106" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E135:E143">
-    <cfRule type="cellIs" dxfId="107" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="131" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="132" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="133" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="134" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="135" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="136" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L138:BO143 L131:BO134 L98:BO103 L105:BO110 L112:BO123 L125:BO129">
-    <cfRule type="expression" dxfId="100" priority="141">
+  <conditionalFormatting sqref="L138:BO143 L131:BO134 L98:BO103 L105:BO110 L112:BO122 L124:BO129">
+    <cfRule type="expression" dxfId="98" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="142">
+    <cfRule type="expression" dxfId="97" priority="142">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17292,38 +17280,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L144:BO152">
-    <cfRule type="expression" dxfId="98" priority="124">
+    <cfRule type="expression" dxfId="96" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E144:E152">
-    <cfRule type="cellIs" dxfId="97" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="118" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="119" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="120" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="121" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="122" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="123" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L147:BO152">
-    <cfRule type="expression" dxfId="90" priority="128">
+    <cfRule type="expression" dxfId="88" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="129">
+    <cfRule type="expression" dxfId="87" priority="129">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17342,38 +17330,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L153:BO161">
-    <cfRule type="expression" dxfId="88" priority="111">
+    <cfRule type="expression" dxfId="86" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E153:E161">
-    <cfRule type="cellIs" dxfId="87" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="105" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="106" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="107" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="108" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="109" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="110" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L156:BO161">
-    <cfRule type="expression" dxfId="80" priority="115">
+    <cfRule type="expression" dxfId="78" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="116">
+    <cfRule type="expression" dxfId="77" priority="116">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17392,38 +17380,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L162:BO170">
-    <cfRule type="expression" dxfId="78" priority="98">
+    <cfRule type="expression" dxfId="76" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E162:E170">
-    <cfRule type="cellIs" dxfId="77" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="92" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="93" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="94" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="95" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="96" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="97" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L165:BO170">
-    <cfRule type="expression" dxfId="70" priority="102">
+    <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="103">
+    <cfRule type="expression" dxfId="67" priority="103">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17442,38 +17430,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:BO86">
-    <cfRule type="expression" dxfId="68" priority="85">
+    <cfRule type="expression" dxfId="66" priority="85">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:E86">
-    <cfRule type="cellIs" dxfId="67" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="78" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="79" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="80" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="81" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="82" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="83" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="84" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L87:BO94">
-    <cfRule type="expression" dxfId="60" priority="76">
+    <cfRule type="expression" dxfId="58" priority="76">
       <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="77">
+    <cfRule type="expression" dxfId="57" priority="77">
       <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17492,38 +17480,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L87:BO94">
-    <cfRule type="expression" dxfId="58" priority="74">
+    <cfRule type="expression" dxfId="56" priority="74">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E87:E94">
-    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="67" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="68" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="69" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="70" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="71" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="72" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="73" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L97:BO97">
-    <cfRule type="expression" dxfId="50" priority="65">
+    <cfRule type="expression" dxfId="48" priority="65">
       <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="66">
+    <cfRule type="expression" dxfId="47" priority="66">
       <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17542,30 +17530,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L97:BO97">
-    <cfRule type="expression" dxfId="48" priority="63">
+    <cfRule type="expression" dxfId="46" priority="63">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="56" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="57" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="58" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="59" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="60" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="61" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="62" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17584,38 +17572,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L130:BO130">
-    <cfRule type="expression" dxfId="40" priority="52">
+    <cfRule type="expression" dxfId="38" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E130">
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="46" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="47" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="48" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="49" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="50" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="51" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L104:BO104">
-    <cfRule type="expression" dxfId="32" priority="32">
+    <cfRule type="expression" dxfId="30" priority="32">
       <formula>AND($F104&lt;=L$6,ROUNDDOWN(($G104-$F104+1)*$I104,0)+$F104-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="33">
+    <cfRule type="expression" dxfId="29" priority="33">
       <formula>AND(NOT(ISBLANK($F104)),$F104&lt;=L$6,$G104&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17634,38 +17622,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L104:BO104">
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="28" priority="30">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E104">
-    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L111:BO111">
-    <cfRule type="expression" dxfId="22" priority="21">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>AND($F111&lt;=L$6,ROUNDDOWN(($G111-$F111+1)*$I111,0)+$F111-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="22">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>AND(NOT(ISBLANK($F111)),$F111&lt;=L$6,$G111&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17684,42 +17672,34 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L111:BO111">
-    <cfRule type="expression" dxfId="20" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E111">
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="13" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="16" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L124:BO124">
-    <cfRule type="expression" dxfId="12" priority="10">
-      <formula>AND($F124&lt;=L$6,ROUNDDOWN(($G124-$F124+1)*$I124,0)+$F124-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>AND(NOT(ISBLANK($F124)),$F124&lt;=L$6,$G124&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I124">
+  <conditionalFormatting sqref="I123">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17733,12 +17713,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L124:BO124">
+  <conditionalFormatting sqref="L123:BO123">
     <cfRule type="expression" dxfId="10" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E124">
+  <conditionalFormatting sqref="E123">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17817,7 +17797,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I123 I125:I129</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I122 I124:I129</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17997,7 +17977,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I124</xm:sqref>
+          <xm:sqref>I123</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Initial adding of Windows automation of new model scripts (v0.17)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4722B2E-5CF1-4651-BC64-28319E10026E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D60E27-F256-4ACC-91E7-03A31CC48183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="156">
   <si>
     <t>WBS</t>
   </si>
@@ -893,6 +893,9 @@
   </si>
   <si>
     <t>Add New Forecasts from SQL</t>
+  </si>
+  <si>
+    <t>Add Automation</t>
   </si>
 </sst>
 </file>
@@ -1821,13 +1824,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1837,10 +1833,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1849,6 +1841,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3409,11 +3412,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO170"/>
+  <dimension ref="A1:BO171"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T120" sqref="T120"/>
+      <selection pane="bottomLeft" activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3443,27 +3446,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3508,12 +3511,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3523,183 +3526,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44431</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44438</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44445</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44452</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44459</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44466</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44473</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44480</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8857,7 +8860,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A135" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A136" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -13823,14 +13826,14 @@
         <v>12.2</v>
       </c>
       <c r="B125" s="65" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D125" s="70"/>
       <c r="E125" s="66" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F125" s="42">
-        <v>44445</v>
+        <v>44443</v>
       </c>
       <c r="G125" s="43">
         <v>44449</v>
@@ -13904,21 +13907,21 @@
         <v>12.3</v>
       </c>
       <c r="B126" s="65" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="D126" s="70"/>
       <c r="E126" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F126" s="42">
+        <v>44445</v>
+      </c>
+      <c r="G126" s="43">
         <v>44449</v>
-      </c>
-      <c r="G126" s="43">
-        <v>44454</v>
       </c>
       <c r="H126" s="73"/>
       <c r="I126" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="J126" s="75"/>
       <c r="K126" s="76"/>
@@ -13985,7 +13988,7 @@
         <v>12.4</v>
       </c>
       <c r="B127" s="65" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
       <c r="D127" s="70"/>
       <c r="E127" s="66" t="s">
@@ -13998,7 +14001,9 @@
         <v>44454</v>
       </c>
       <c r="H127" s="73"/>
-      <c r="I127" s="26"/>
+      <c r="I127" s="26">
+        <v>0.3</v>
+      </c>
       <c r="J127" s="75"/>
       <c r="K127" s="76"/>
       <c r="L127" s="46"/>
@@ -14064,7 +14069,7 @@
         <v>12.5</v>
       </c>
       <c r="B128" s="65" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D128" s="70"/>
       <c r="E128" s="66" t="s">
@@ -14143,20 +14148,20 @@
         <v>12.6</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D129" s="70"/>
-      <c r="E129" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F129" s="71">
+      <c r="E129" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F129" s="42">
         <v>44449</v>
       </c>
-      <c r="G129" s="72">
+      <c r="G129" s="43">
         <v>44454</v>
       </c>
       <c r="H129" s="73"/>
-      <c r="I129" s="74"/>
+      <c r="I129" s="26"/>
       <c r="J129" s="75"/>
       <c r="K129" s="76"/>
       <c r="L129" s="46"/>
@@ -14216,173 +14221,175 @@
       <c r="BN129" s="46"/>
       <c r="BO129" s="46"/>
     </row>
-    <row r="130" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A130" s="16" t="str">
+    <row r="130" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.7</v>
+      </c>
+      <c r="B130" s="65" t="s">
+        <v>142</v>
+      </c>
+      <c r="D130" s="70"/>
+      <c r="E130" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F130" s="71">
+        <v>44449</v>
+      </c>
+      <c r="G130" s="72">
+        <v>44454</v>
+      </c>
+      <c r="H130" s="73"/>
+      <c r="I130" s="74"/>
+      <c r="J130" s="75"/>
+      <c r="K130" s="76"/>
+      <c r="L130" s="46"/>
+      <c r="M130" s="46"/>
+      <c r="N130" s="46"/>
+      <c r="O130" s="46"/>
+      <c r="P130" s="46"/>
+      <c r="Q130" s="46"/>
+      <c r="R130" s="46"/>
+      <c r="S130" s="46"/>
+      <c r="T130" s="46"/>
+      <c r="U130" s="46"/>
+      <c r="V130" s="46"/>
+      <c r="W130" s="46"/>
+      <c r="X130" s="46"/>
+      <c r="Y130" s="46"/>
+      <c r="Z130" s="46"/>
+      <c r="AA130" s="46"/>
+      <c r="AB130" s="46"/>
+      <c r="AC130" s="46"/>
+      <c r="AD130" s="46"/>
+      <c r="AE130" s="46"/>
+      <c r="AF130" s="46"/>
+      <c r="AG130" s="46"/>
+      <c r="AH130" s="46"/>
+      <c r="AI130" s="46"/>
+      <c r="AJ130" s="46"/>
+      <c r="AK130" s="46"/>
+      <c r="AL130" s="46"/>
+      <c r="AM130" s="46"/>
+      <c r="AN130" s="46"/>
+      <c r="AO130" s="46"/>
+      <c r="AP130" s="46"/>
+      <c r="AQ130" s="46"/>
+      <c r="AR130" s="46"/>
+      <c r="AS130" s="46"/>
+      <c r="AT130" s="46"/>
+      <c r="AU130" s="46"/>
+      <c r="AV130" s="46"/>
+      <c r="AW130" s="46"/>
+      <c r="AX130" s="46"/>
+      <c r="AY130" s="46"/>
+      <c r="AZ130" s="46"/>
+      <c r="BA130" s="46"/>
+      <c r="BB130" s="46"/>
+      <c r="BC130" s="46"/>
+      <c r="BD130" s="46"/>
+      <c r="BE130" s="46"/>
+      <c r="BF130" s="46"/>
+      <c r="BG130" s="46"/>
+      <c r="BH130" s="46"/>
+      <c r="BI130" s="46"/>
+      <c r="BJ130" s="46"/>
+      <c r="BK130" s="46"/>
+      <c r="BL130" s="46"/>
+      <c r="BM130" s="46"/>
+      <c r="BN130" s="46"/>
+      <c r="BO130" s="46"/>
+    </row>
+    <row r="131" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="16" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>13</v>
       </c>
-      <c r="B130" s="17" t="s">
+      <c r="B131" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="D130" s="19"/>
-      <c r="E130" s="19"/>
-      <c r="F130" s="44"/>
-      <c r="G130" s="44" t="str">
-        <f t="shared" ref="G130" si="24">IF(ISBLANK(F130)," - ",IF(H130=0,F130,F130+H130-1))</f>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="44"/>
+      <c r="G131" s="44" t="str">
+        <f t="shared" ref="G131" si="24">IF(ISBLANK(F131)," - ",IF(H131=0,F131,F131+H131-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="H130" s="20"/>
-      <c r="I130" s="21"/>
-      <c r="J130" s="22" t="str">
-        <f t="shared" ref="J130" si="25">IF(OR(G130=0,F130=0)," - ",NETWORKDAYS(F130,G130))</f>
+      <c r="H131" s="20"/>
+      <c r="I131" s="21"/>
+      <c r="J131" s="22" t="str">
+        <f t="shared" ref="J131" si="25">IF(OR(G131=0,F131=0)," - ",NETWORKDAYS(F131,G131))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="K130" s="41"/>
-      <c r="L130" s="48"/>
-      <c r="M130" s="48"/>
-      <c r="N130" s="48"/>
-      <c r="O130" s="48"/>
-      <c r="P130" s="48"/>
-      <c r="Q130" s="48"/>
-      <c r="R130" s="48"/>
-      <c r="S130" s="48"/>
-      <c r="T130" s="48"/>
-      <c r="U130" s="48"/>
-      <c r="V130" s="48"/>
-      <c r="W130" s="48"/>
-      <c r="X130" s="48"/>
-      <c r="Y130" s="48"/>
-      <c r="Z130" s="48"/>
-      <c r="AA130" s="48"/>
-      <c r="AB130" s="48"/>
-      <c r="AC130" s="48"/>
-      <c r="AD130" s="48"/>
-      <c r="AE130" s="48"/>
-      <c r="AF130" s="48"/>
-      <c r="AG130" s="48"/>
-      <c r="AH130" s="48"/>
-      <c r="AI130" s="48"/>
-      <c r="AJ130" s="48"/>
-      <c r="AK130" s="48"/>
-      <c r="AL130" s="48"/>
-      <c r="AM130" s="48"/>
-      <c r="AN130" s="48"/>
-      <c r="AO130" s="48"/>
-      <c r="AP130" s="48"/>
-      <c r="AQ130" s="48"/>
-      <c r="AR130" s="48"/>
-      <c r="AS130" s="48"/>
-      <c r="AT130" s="48"/>
-      <c r="AU130" s="48"/>
-      <c r="AV130" s="48"/>
-      <c r="AW130" s="48"/>
-      <c r="AX130" s="48"/>
-      <c r="AY130" s="48"/>
-      <c r="AZ130" s="48"/>
-      <c r="BA130" s="48"/>
-      <c r="BB130" s="48"/>
-      <c r="BC130" s="48"/>
-      <c r="BD130" s="48"/>
-      <c r="BE130" s="48"/>
-      <c r="BF130" s="48"/>
-      <c r="BG130" s="48"/>
-      <c r="BH130" s="48"/>
-      <c r="BI130" s="48"/>
-      <c r="BJ130" s="48"/>
-      <c r="BK130" s="48"/>
-      <c r="BL130" s="48"/>
-      <c r="BM130" s="48"/>
-      <c r="BN130" s="48"/>
-      <c r="BO130" s="48"/>
-    </row>
-    <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.1</v>
-      </c>
-      <c r="B131" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="D131" s="70"/>
-      <c r="E131" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F131" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G131" s="43"/>
-      <c r="H131" s="25"/>
-      <c r="I131" s="26"/>
-      <c r="J131" s="27"/>
-      <c r="K131" s="40"/>
-      <c r="L131" s="46"/>
-      <c r="M131" s="46"/>
-      <c r="N131" s="46"/>
-      <c r="O131" s="46"/>
-      <c r="P131" s="46"/>
-      <c r="Q131" s="46"/>
-      <c r="R131" s="46"/>
-      <c r="S131" s="46"/>
-      <c r="T131" s="46"/>
-      <c r="U131" s="46"/>
-      <c r="V131" s="46"/>
-      <c r="W131" s="46"/>
-      <c r="X131" s="46"/>
-      <c r="Y131" s="46"/>
-      <c r="Z131" s="46"/>
-      <c r="AA131" s="46"/>
-      <c r="AB131" s="46"/>
-      <c r="AC131" s="46"/>
-      <c r="AD131" s="46"/>
-      <c r="AE131" s="46"/>
-      <c r="AF131" s="46"/>
-      <c r="AG131" s="46"/>
-      <c r="AH131" s="46"/>
-      <c r="AI131" s="46"/>
-      <c r="AJ131" s="46"/>
-      <c r="AK131" s="46"/>
-      <c r="AL131" s="46"/>
-      <c r="AM131" s="46"/>
-      <c r="AN131" s="46"/>
-      <c r="AO131" s="46"/>
-      <c r="AP131" s="46"/>
-      <c r="AQ131" s="46"/>
-      <c r="AR131" s="46"/>
-      <c r="AS131" s="46"/>
-      <c r="AT131" s="46"/>
-      <c r="AU131" s="46"/>
-      <c r="AV131" s="46"/>
-      <c r="AW131" s="46"/>
-      <c r="AX131" s="46"/>
-      <c r="AY131" s="46"/>
-      <c r="AZ131" s="46"/>
-      <c r="BA131" s="46"/>
-      <c r="BB131" s="46"/>
-      <c r="BC131" s="46"/>
-      <c r="BD131" s="46"/>
-      <c r="BE131" s="46"/>
-      <c r="BF131" s="46"/>
-      <c r="BG131" s="46"/>
-      <c r="BH131" s="46"/>
-      <c r="BI131" s="46"/>
-      <c r="BJ131" s="46"/>
-      <c r="BK131" s="46"/>
-      <c r="BL131" s="46"/>
-      <c r="BM131" s="46"/>
-      <c r="BN131" s="46"/>
-      <c r="BO131" s="46"/>
+      <c r="K131" s="41"/>
+      <c r="L131" s="48"/>
+      <c r="M131" s="48"/>
+      <c r="N131" s="48"/>
+      <c r="O131" s="48"/>
+      <c r="P131" s="48"/>
+      <c r="Q131" s="48"/>
+      <c r="R131" s="48"/>
+      <c r="S131" s="48"/>
+      <c r="T131" s="48"/>
+      <c r="U131" s="48"/>
+      <c r="V131" s="48"/>
+      <c r="W131" s="48"/>
+      <c r="X131" s="48"/>
+      <c r="Y131" s="48"/>
+      <c r="Z131" s="48"/>
+      <c r="AA131" s="48"/>
+      <c r="AB131" s="48"/>
+      <c r="AC131" s="48"/>
+      <c r="AD131" s="48"/>
+      <c r="AE131" s="48"/>
+      <c r="AF131" s="48"/>
+      <c r="AG131" s="48"/>
+      <c r="AH131" s="48"/>
+      <c r="AI131" s="48"/>
+      <c r="AJ131" s="48"/>
+      <c r="AK131" s="48"/>
+      <c r="AL131" s="48"/>
+      <c r="AM131" s="48"/>
+      <c r="AN131" s="48"/>
+      <c r="AO131" s="48"/>
+      <c r="AP131" s="48"/>
+      <c r="AQ131" s="48"/>
+      <c r="AR131" s="48"/>
+      <c r="AS131" s="48"/>
+      <c r="AT131" s="48"/>
+      <c r="AU131" s="48"/>
+      <c r="AV131" s="48"/>
+      <c r="AW131" s="48"/>
+      <c r="AX131" s="48"/>
+      <c r="AY131" s="48"/>
+      <c r="AZ131" s="48"/>
+      <c r="BA131" s="48"/>
+      <c r="BB131" s="48"/>
+      <c r="BC131" s="48"/>
+      <c r="BD131" s="48"/>
+      <c r="BE131" s="48"/>
+      <c r="BF131" s="48"/>
+      <c r="BG131" s="48"/>
+      <c r="BH131" s="48"/>
+      <c r="BI131" s="48"/>
+      <c r="BJ131" s="48"/>
+      <c r="BK131" s="48"/>
+      <c r="BL131" s="48"/>
+      <c r="BM131" s="48"/>
+      <c r="BN131" s="48"/>
+      <c r="BO131" s="48"/>
     </row>
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.2</v>
+        <v>13.1</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D132" s="70"/>
       <c r="E132" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F132" s="42">
         <v>44379</v>
@@ -14452,14 +14459,14 @@
     <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.2</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F133" s="42">
         <v>44379</v>
@@ -14529,10 +14536,10 @@
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.3</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
@@ -14606,17 +14613,17 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B135" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D135" s="66"/>
+        <v>13.4</v>
+      </c>
+      <c r="B135" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F135" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G135" s="43"/>
       <c r="H135" s="25"/>
@@ -14681,11 +14688,20 @@
       <c r="BO135" s="46"/>
     </row>
     <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="23"/>
-      <c r="B136" s="65"/>
+      <c r="A136" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B136" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D136" s="66"/>
-      <c r="E136" s="66"/>
-      <c r="F136" s="42"/>
+      <c r="E136" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F136" s="42">
+        <v>44531</v>
+      </c>
       <c r="G136" s="43"/>
       <c r="H136" s="25"/>
       <c r="I136" s="26"/>
@@ -14887,7 +14903,7 @@
     <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="23"/>
       <c r="B139" s="65"/>
-      <c r="D139" s="70"/>
+      <c r="D139" s="66"/>
       <c r="E139" s="66"/>
       <c r="F139" s="42"/>
       <c r="G139" s="43"/>
@@ -15227,7 +15243,7 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23"/>
       <c r="B144" s="65"/>
-      <c r="D144" s="66"/>
+      <c r="D144" s="70"/>
       <c r="E144" s="66"/>
       <c r="F144" s="42"/>
       <c r="G144" s="43"/>
@@ -15499,7 +15515,7 @@
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="23"/>
       <c r="B148" s="65"/>
-      <c r="D148" s="70"/>
+      <c r="D148" s="66"/>
       <c r="E148" s="66"/>
       <c r="F148" s="42"/>
       <c r="G148" s="43"/>
@@ -15839,7 +15855,7 @@
     <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="23"/>
       <c r="B153" s="65"/>
-      <c r="D153" s="66"/>
+      <c r="D153" s="70"/>
       <c r="E153" s="66"/>
       <c r="F153" s="42"/>
       <c r="G153" s="43"/>
@@ -16111,7 +16127,7 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23"/>
       <c r="B157" s="65"/>
-      <c r="D157" s="70"/>
+      <c r="D157" s="66"/>
       <c r="E157" s="66"/>
       <c r="F157" s="42"/>
       <c r="G157" s="43"/>
@@ -16451,7 +16467,7 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23"/>
       <c r="B162" s="65"/>
-      <c r="D162" s="66"/>
+      <c r="D162" s="70"/>
       <c r="E162" s="66"/>
       <c r="F162" s="42"/>
       <c r="G162" s="43"/>
@@ -16723,7 +16739,7 @@
     <row r="166" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23"/>
       <c r="B166" s="65"/>
-      <c r="D166" s="70"/>
+      <c r="D166" s="66"/>
       <c r="E166" s="66"/>
       <c r="F166" s="42"/>
       <c r="G166" s="43"/>
@@ -17060,9 +17076,86 @@
       <c r="BN170" s="46"/>
       <c r="BO170" s="46"/>
     </row>
+    <row r="171" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="23"/>
+      <c r="B171" s="65"/>
+      <c r="D171" s="70"/>
+      <c r="E171" s="66"/>
+      <c r="F171" s="42"/>
+      <c r="G171" s="43"/>
+      <c r="H171" s="25"/>
+      <c r="I171" s="26"/>
+      <c r="J171" s="27"/>
+      <c r="K171" s="40"/>
+      <c r="L171" s="46"/>
+      <c r="M171" s="46"/>
+      <c r="N171" s="46"/>
+      <c r="O171" s="46"/>
+      <c r="P171" s="46"/>
+      <c r="Q171" s="46"/>
+      <c r="R171" s="46"/>
+      <c r="S171" s="46"/>
+      <c r="T171" s="46"/>
+      <c r="U171" s="46"/>
+      <c r="V171" s="46"/>
+      <c r="W171" s="46"/>
+      <c r="X171" s="46"/>
+      <c r="Y171" s="46"/>
+      <c r="Z171" s="46"/>
+      <c r="AA171" s="46"/>
+      <c r="AB171" s="46"/>
+      <c r="AC171" s="46"/>
+      <c r="AD171" s="46"/>
+      <c r="AE171" s="46"/>
+      <c r="AF171" s="46"/>
+      <c r="AG171" s="46"/>
+      <c r="AH171" s="46"/>
+      <c r="AI171" s="46"/>
+      <c r="AJ171" s="46"/>
+      <c r="AK171" s="46"/>
+      <c r="AL171" s="46"/>
+      <c r="AM171" s="46"/>
+      <c r="AN171" s="46"/>
+      <c r="AO171" s="46"/>
+      <c r="AP171" s="46"/>
+      <c r="AQ171" s="46"/>
+      <c r="AR171" s="46"/>
+      <c r="AS171" s="46"/>
+      <c r="AT171" s="46"/>
+      <c r="AU171" s="46"/>
+      <c r="AV171" s="46"/>
+      <c r="AW171" s="46"/>
+      <c r="AX171" s="46"/>
+      <c r="AY171" s="46"/>
+      <c r="AZ171" s="46"/>
+      <c r="BA171" s="46"/>
+      <c r="BB171" s="46"/>
+      <c r="BC171" s="46"/>
+      <c r="BD171" s="46"/>
+      <c r="BE171" s="46"/>
+      <c r="BF171" s="46"/>
+      <c r="BG171" s="46"/>
+      <c r="BH171" s="46"/>
+      <c r="BI171" s="46"/>
+      <c r="BJ171" s="46"/>
+      <c r="BK171" s="46"/>
+      <c r="BL171" s="46"/>
+      <c r="BM171" s="46"/>
+      <c r="BN171" s="46"/>
+      <c r="BO171" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17073,18 +17166,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I122 I124:I129">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I132:I135 I98:I103 I105:I110 I112:I122 I124:I130">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17103,7 +17187,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN129 L135:BO137 M138:BN143 BO141:BO143 L144:BO146 M147:BN152 BO150:BO152 L153:BO155 M156:BN161 BO159:BO161 L162:BO164 M165:BN170 BO168:BO170 BO133:BO134 M131:BN134 L130:BO130 L123:BO123">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN130 L136:BO138 M139:BN144 BO142:BO144 L145:BO147 M148:BN153 BO151:BO153 L154:BO156 M157:BN162 BO160:BO162 L163:BO165 M166:BN171 BO169:BO171 BO134:BO135 M132:BN135 L131:BO131 L123:BO123">
     <cfRule type="expression" dxfId="132" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -17111,7 +17195,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L131:BO134 L98:BO103 L105:BO110 L112:BO122 L124:BO129">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L132:BO135 L98:BO103 L105:BO110 L112:BO122 L124:BO130">
     <cfRule type="expression" dxfId="130" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -17121,7 +17205,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E171:E1048576 E95:E96 E131:E134 E98:E103 E105:E110 E112:E122 E124:E129">
+  <conditionalFormatting sqref="E1:E73 E172:E1048576 E95:E96 E132:E135 E98:E103 E105:E110 E112:E122 E124:E130">
     <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17215,7 +17299,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I135:I143">
+  <conditionalFormatting sqref="I136:I144">
     <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17229,12 +17313,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L135:BO143">
+  <conditionalFormatting sqref="L136:BO144">
     <cfRule type="expression" dxfId="106" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E135:E143">
+  <conditionalFormatting sqref="E136:E144">
     <cfRule type="cellIs" dxfId="105" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17257,7 +17341,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L138:BO143 L131:BO134 L98:BO103 L105:BO110 L112:BO122 L124:BO129">
+  <conditionalFormatting sqref="L139:BO144 L132:BO135 L98:BO103 L105:BO110 L112:BO122 L124:BO130">
     <cfRule type="expression" dxfId="98" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17265,7 +17349,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I144:I152">
+  <conditionalFormatting sqref="I145:I153">
     <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17279,12 +17363,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L144:BO152">
+  <conditionalFormatting sqref="L145:BO153">
     <cfRule type="expression" dxfId="96" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E144:E152">
+  <conditionalFormatting sqref="E145:E153">
     <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17307,7 +17391,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L147:BO152">
+  <conditionalFormatting sqref="L148:BO153">
     <cfRule type="expression" dxfId="88" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17315,7 +17399,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I153:I161">
+  <conditionalFormatting sqref="I154:I162">
     <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17329,12 +17413,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L153:BO161">
+  <conditionalFormatting sqref="L154:BO162">
     <cfRule type="expression" dxfId="86" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E153:E161">
+  <conditionalFormatting sqref="E154:E162">
     <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17357,7 +17441,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L156:BO161">
+  <conditionalFormatting sqref="L157:BO162">
     <cfRule type="expression" dxfId="78" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17365,7 +17449,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I162:I170">
+  <conditionalFormatting sqref="I163:I171">
     <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17379,12 +17463,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L162:BO170">
+  <conditionalFormatting sqref="L163:BO171">
     <cfRule type="expression" dxfId="76" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E162:E170">
+  <conditionalFormatting sqref="E163:E171">
     <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17407,7 +17491,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L165:BO170">
+  <conditionalFormatting sqref="L166:BO171">
     <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17557,7 +17641,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I130">
+  <conditionalFormatting sqref="I131">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17571,12 +17655,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L130:BO130">
+  <conditionalFormatting sqref="L131:BO131">
     <cfRule type="expression" dxfId="38" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E130">
+  <conditionalFormatting sqref="E131">
     <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17797,7 +17881,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I131:I134 I98:I103 I105:I110 I112:I122 I124:I129</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I132:I135 I98:I103 I105:I110 I112:I122 I124:I130</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17827,7 +17911,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I135:I143</xm:sqref>
+          <xm:sqref>I136:I144</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -17842,7 +17926,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I144:I152</xm:sqref>
+          <xm:sqref>I145:I153</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -17857,7 +17941,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I153:I161</xm:sqref>
+          <xm:sqref>I154:I162</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -17872,7 +17956,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I162:I170</xm:sqref>
+          <xm:sqref>I163:I171</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -17932,7 +18016,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I130</xm:sqref>
+          <xm:sqref>I131</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Added code to break down SQL inserts into chunks due to memory issues (v0.17)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D60E27-F256-4ACC-91E7-03A31CC48183}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF654AD-F674-4DD5-B5FE-01EA33EF5FFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="158">
   <si>
     <t>WBS</t>
   </si>
@@ -892,10 +892,16 @@
     <t>Add Additional Scenarios</t>
   </si>
   <si>
-    <t>Add New Forecasts from SQL</t>
+    <t>Add Automation</t>
   </si>
   <si>
-    <t>Add Automation</t>
+    <t>Add New Economic Scenarios Page</t>
+  </si>
+  <si>
+    <t>Add New Variable-by-Variable Page</t>
+  </si>
+  <si>
+    <t>Add PHP Scenarios Pull</t>
   </si>
 </sst>
 </file>
@@ -1824,6 +1830,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1833,6 +1846,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1841,17 +1858,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3412,11 +3418,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO171"/>
+  <dimension ref="A1:BO173"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G126" sqref="G126"/>
+      <selection pane="bottomLeft" activeCell="I125" sqref="I125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3446,27 +3452,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3511,12 +3517,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3526,183 +3532,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 35</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 36</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 37</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 38</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 39</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 40</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44431</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44438</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44445</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44452</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44459</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44466</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44473</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44480</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8860,7 +8866,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A136" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A138" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -13749,7 +13755,7 @@
       </c>
       <c r="D124" s="70"/>
       <c r="E124" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F124" s="42">
         <v>44443</v>
@@ -13759,7 +13765,7 @@
       </c>
       <c r="H124" s="73"/>
       <c r="I124" s="26">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J124" s="75"/>
       <c r="K124" s="76"/>
@@ -13826,21 +13832,21 @@
         <v>12.2</v>
       </c>
       <c r="B125" s="65" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D125" s="70"/>
       <c r="E125" s="66" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F125" s="42">
         <v>44443</v>
       </c>
       <c r="G125" s="43">
-        <v>44449</v>
+        <v>44444</v>
       </c>
       <c r="H125" s="73"/>
       <c r="I125" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J125" s="75"/>
       <c r="K125" s="76"/>
@@ -13907,21 +13913,21 @@
         <v>12.3</v>
       </c>
       <c r="B126" s="65" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D126" s="70"/>
       <c r="E126" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F126" s="42">
-        <v>44445</v>
+        <v>44443</v>
       </c>
       <c r="G126" s="43">
         <v>44449</v>
       </c>
       <c r="H126" s="73"/>
       <c r="I126" s="26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J126" s="75"/>
       <c r="K126" s="76"/>
@@ -13988,21 +13994,21 @@
         <v>12.4</v>
       </c>
       <c r="B127" s="65" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="D127" s="70"/>
       <c r="E127" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F127" s="42">
         <v>44449</v>
       </c>
       <c r="G127" s="43">
-        <v>44454</v>
+        <v>44449</v>
       </c>
       <c r="H127" s="73"/>
       <c r="I127" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="J127" s="75"/>
       <c r="K127" s="76"/>
@@ -14069,20 +14075,22 @@
         <v>12.5</v>
       </c>
       <c r="B128" s="65" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D128" s="70"/>
       <c r="E128" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F128" s="42">
+        <v>44459</v>
+      </c>
+      <c r="G128" s="43">
         <v>44449</v>
       </c>
-      <c r="G128" s="43">
-        <v>44454</v>
-      </c>
       <c r="H128" s="73"/>
-      <c r="I128" s="26"/>
+      <c r="I128" s="26">
+        <v>0</v>
+      </c>
       <c r="J128" s="75"/>
       <c r="K128" s="76"/>
       <c r="L128" s="46"/>
@@ -14148,20 +14156,22 @@
         <v>12.6</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D129" s="70"/>
       <c r="E129" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F129" s="42">
-        <v>44449</v>
+        <v>44459</v>
       </c>
       <c r="G129" s="43">
-        <v>44454</v>
+        <v>44469</v>
       </c>
       <c r="H129" s="73"/>
-      <c r="I129" s="26"/>
+      <c r="I129" s="26">
+        <v>0.3</v>
+      </c>
       <c r="J129" s="75"/>
       <c r="K129" s="76"/>
       <c r="L129" s="46"/>
@@ -14227,20 +14237,22 @@
         <v>12.7</v>
       </c>
       <c r="B130" s="65" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="D130" s="70"/>
-      <c r="E130" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F130" s="71">
-        <v>44449</v>
-      </c>
-      <c r="G130" s="72">
-        <v>44454</v>
+      <c r="E130" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F130" s="42">
+        <v>44459</v>
+      </c>
+      <c r="G130" s="43">
+        <v>44469</v>
       </c>
       <c r="H130" s="73"/>
-      <c r="I130" s="74"/>
+      <c r="I130" s="26">
+        <v>0</v>
+      </c>
       <c r="J130" s="75"/>
       <c r="K130" s="76"/>
       <c r="L130" s="46"/>
@@ -14300,105 +14312,111 @@
       <c r="BN130" s="46"/>
       <c r="BO130" s="46"/>
     </row>
-    <row r="131" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>13</v>
-      </c>
-      <c r="B131" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D131" s="19"/>
-      <c r="E131" s="19"/>
-      <c r="F131" s="44"/>
-      <c r="G131" s="44" t="str">
-        <f t="shared" ref="G131" si="24">IF(ISBLANK(F131)," - ",IF(H131=0,F131,F131+H131-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H131" s="20"/>
-      <c r="I131" s="21"/>
-      <c r="J131" s="22" t="str">
-        <f t="shared" ref="J131" si="25">IF(OR(G131=0,F131=0)," - ",NETWORKDAYS(F131,G131))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K131" s="41"/>
-      <c r="L131" s="48"/>
-      <c r="M131" s="48"/>
-      <c r="N131" s="48"/>
-      <c r="O131" s="48"/>
-      <c r="P131" s="48"/>
-      <c r="Q131" s="48"/>
-      <c r="R131" s="48"/>
-      <c r="S131" s="48"/>
-      <c r="T131" s="48"/>
-      <c r="U131" s="48"/>
-      <c r="V131" s="48"/>
-      <c r="W131" s="48"/>
-      <c r="X131" s="48"/>
-      <c r="Y131" s="48"/>
-      <c r="Z131" s="48"/>
-      <c r="AA131" s="48"/>
-      <c r="AB131" s="48"/>
-      <c r="AC131" s="48"/>
-      <c r="AD131" s="48"/>
-      <c r="AE131" s="48"/>
-      <c r="AF131" s="48"/>
-      <c r="AG131" s="48"/>
-      <c r="AH131" s="48"/>
-      <c r="AI131" s="48"/>
-      <c r="AJ131" s="48"/>
-      <c r="AK131" s="48"/>
-      <c r="AL131" s="48"/>
-      <c r="AM131" s="48"/>
-      <c r="AN131" s="48"/>
-      <c r="AO131" s="48"/>
-      <c r="AP131" s="48"/>
-      <c r="AQ131" s="48"/>
-      <c r="AR131" s="48"/>
-      <c r="AS131" s="48"/>
-      <c r="AT131" s="48"/>
-      <c r="AU131" s="48"/>
-      <c r="AV131" s="48"/>
-      <c r="AW131" s="48"/>
-      <c r="AX131" s="48"/>
-      <c r="AY131" s="48"/>
-      <c r="AZ131" s="48"/>
-      <c r="BA131" s="48"/>
-      <c r="BB131" s="48"/>
-      <c r="BC131" s="48"/>
-      <c r="BD131" s="48"/>
-      <c r="BE131" s="48"/>
-      <c r="BF131" s="48"/>
-      <c r="BG131" s="48"/>
-      <c r="BH131" s="48"/>
-      <c r="BI131" s="48"/>
-      <c r="BJ131" s="48"/>
-      <c r="BK131" s="48"/>
-      <c r="BL131" s="48"/>
-      <c r="BM131" s="48"/>
-      <c r="BN131" s="48"/>
-      <c r="BO131" s="48"/>
+    <row r="131" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.8</v>
+      </c>
+      <c r="B131" s="65" t="s">
+        <v>141</v>
+      </c>
+      <c r="D131" s="70"/>
+      <c r="E131" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F131" s="42">
+        <v>44459</v>
+      </c>
+      <c r="G131" s="43">
+        <v>44469</v>
+      </c>
+      <c r="H131" s="73"/>
+      <c r="I131" s="26">
+        <v>0</v>
+      </c>
+      <c r="J131" s="75"/>
+      <c r="K131" s="76"/>
+      <c r="L131" s="46"/>
+      <c r="M131" s="46"/>
+      <c r="N131" s="46"/>
+      <c r="O131" s="46"/>
+      <c r="P131" s="46"/>
+      <c r="Q131" s="46"/>
+      <c r="R131" s="46"/>
+      <c r="S131" s="46"/>
+      <c r="T131" s="46"/>
+      <c r="U131" s="46"/>
+      <c r="V131" s="46"/>
+      <c r="W131" s="46"/>
+      <c r="X131" s="46"/>
+      <c r="Y131" s="46"/>
+      <c r="Z131" s="46"/>
+      <c r="AA131" s="46"/>
+      <c r="AB131" s="46"/>
+      <c r="AC131" s="46"/>
+      <c r="AD131" s="46"/>
+      <c r="AE131" s="46"/>
+      <c r="AF131" s="46"/>
+      <c r="AG131" s="46"/>
+      <c r="AH131" s="46"/>
+      <c r="AI131" s="46"/>
+      <c r="AJ131" s="46"/>
+      <c r="AK131" s="46"/>
+      <c r="AL131" s="46"/>
+      <c r="AM131" s="46"/>
+      <c r="AN131" s="46"/>
+      <c r="AO131" s="46"/>
+      <c r="AP131" s="46"/>
+      <c r="AQ131" s="46"/>
+      <c r="AR131" s="46"/>
+      <c r="AS131" s="46"/>
+      <c r="AT131" s="46"/>
+      <c r="AU131" s="46"/>
+      <c r="AV131" s="46"/>
+      <c r="AW131" s="46"/>
+      <c r="AX131" s="46"/>
+      <c r="AY131" s="46"/>
+      <c r="AZ131" s="46"/>
+      <c r="BA131" s="46"/>
+      <c r="BB131" s="46"/>
+      <c r="BC131" s="46"/>
+      <c r="BD131" s="46"/>
+      <c r="BE131" s="46"/>
+      <c r="BF131" s="46"/>
+      <c r="BG131" s="46"/>
+      <c r="BH131" s="46"/>
+      <c r="BI131" s="46"/>
+      <c r="BJ131" s="46"/>
+      <c r="BK131" s="46"/>
+      <c r="BL131" s="46"/>
+      <c r="BM131" s="46"/>
+      <c r="BN131" s="46"/>
+      <c r="BO131" s="46"/>
     </row>
     <row r="132" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.1</v>
+        <v>12.9</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>105</v>
+        <v>142</v>
       </c>
       <c r="D132" s="70"/>
-      <c r="E132" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F132" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G132" s="43"/>
-      <c r="H132" s="25"/>
-      <c r="I132" s="26"/>
-      <c r="J132" s="27"/>
-      <c r="K132" s="40"/>
+      <c r="E132" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F132" s="71">
+        <v>44459</v>
+      </c>
+      <c r="G132" s="72">
+        <v>44469</v>
+      </c>
+      <c r="H132" s="73"/>
+      <c r="I132" s="74">
+        <v>0</v>
+      </c>
+      <c r="J132" s="75"/>
+      <c r="K132" s="76"/>
       <c r="L132" s="46"/>
       <c r="M132" s="46"/>
       <c r="N132" s="46"/>
@@ -14456,94 +14474,96 @@
       <c r="BN132" s="46"/>
       <c r="BO132" s="46"/>
     </row>
-    <row r="133" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A133" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.2</v>
-      </c>
-      <c r="B133" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D133" s="70"/>
-      <c r="E133" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F133" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G133" s="43"/>
-      <c r="H133" s="25"/>
-      <c r="I133" s="26"/>
-      <c r="J133" s="27"/>
-      <c r="K133" s="40"/>
-      <c r="L133" s="46"/>
-      <c r="M133" s="46"/>
-      <c r="N133" s="46"/>
-      <c r="O133" s="46"/>
-      <c r="P133" s="46"/>
-      <c r="Q133" s="46"/>
-      <c r="R133" s="46"/>
-      <c r="S133" s="46"/>
-      <c r="T133" s="46"/>
-      <c r="U133" s="46"/>
-      <c r="V133" s="46"/>
-      <c r="W133" s="46"/>
-      <c r="X133" s="46"/>
-      <c r="Y133" s="46"/>
-      <c r="Z133" s="46"/>
-      <c r="AA133" s="46"/>
-      <c r="AB133" s="46"/>
-      <c r="AC133" s="46"/>
-      <c r="AD133" s="46"/>
-      <c r="AE133" s="46"/>
-      <c r="AF133" s="46"/>
-      <c r="AG133" s="46"/>
-      <c r="AH133" s="46"/>
-      <c r="AI133" s="46"/>
-      <c r="AJ133" s="46"/>
-      <c r="AK133" s="46"/>
-      <c r="AL133" s="46"/>
-      <c r="AM133" s="46"/>
-      <c r="AN133" s="46"/>
-      <c r="AO133" s="46"/>
-      <c r="AP133" s="46"/>
-      <c r="AQ133" s="46"/>
-      <c r="AR133" s="46"/>
-      <c r="AS133" s="46"/>
-      <c r="AT133" s="46"/>
-      <c r="AU133" s="46"/>
-      <c r="AV133" s="46"/>
-      <c r="AW133" s="46"/>
-      <c r="AX133" s="46"/>
-      <c r="AY133" s="46"/>
-      <c r="AZ133" s="46"/>
-      <c r="BA133" s="46"/>
-      <c r="BB133" s="46"/>
-      <c r="BC133" s="46"/>
-      <c r="BD133" s="46"/>
-      <c r="BE133" s="46"/>
-      <c r="BF133" s="46"/>
-      <c r="BG133" s="46"/>
-      <c r="BH133" s="46"/>
-      <c r="BI133" s="46"/>
-      <c r="BJ133" s="46"/>
-      <c r="BK133" s="46"/>
-      <c r="BL133" s="46"/>
-      <c r="BM133" s="46"/>
-      <c r="BN133" s="46"/>
-      <c r="BO133" s="46"/>
+    <row r="133" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>13</v>
+      </c>
+      <c r="B133" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D133" s="19"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="44"/>
+      <c r="G133" s="44" t="str">
+        <f t="shared" ref="G133" si="24">IF(ISBLANK(F133)," - ",IF(H133=0,F133,F133+H133-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H133" s="20"/>
+      <c r="I133" s="21"/>
+      <c r="J133" s="22" t="str">
+        <f t="shared" ref="J133" si="25">IF(OR(G133=0,F133=0)," - ",NETWORKDAYS(F133,G133))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K133" s="41"/>
+      <c r="L133" s="48"/>
+      <c r="M133" s="48"/>
+      <c r="N133" s="48"/>
+      <c r="O133" s="48"/>
+      <c r="P133" s="48"/>
+      <c r="Q133" s="48"/>
+      <c r="R133" s="48"/>
+      <c r="S133" s="48"/>
+      <c r="T133" s="48"/>
+      <c r="U133" s="48"/>
+      <c r="V133" s="48"/>
+      <c r="W133" s="48"/>
+      <c r="X133" s="48"/>
+      <c r="Y133" s="48"/>
+      <c r="Z133" s="48"/>
+      <c r="AA133" s="48"/>
+      <c r="AB133" s="48"/>
+      <c r="AC133" s="48"/>
+      <c r="AD133" s="48"/>
+      <c r="AE133" s="48"/>
+      <c r="AF133" s="48"/>
+      <c r="AG133" s="48"/>
+      <c r="AH133" s="48"/>
+      <c r="AI133" s="48"/>
+      <c r="AJ133" s="48"/>
+      <c r="AK133" s="48"/>
+      <c r="AL133" s="48"/>
+      <c r="AM133" s="48"/>
+      <c r="AN133" s="48"/>
+      <c r="AO133" s="48"/>
+      <c r="AP133" s="48"/>
+      <c r="AQ133" s="48"/>
+      <c r="AR133" s="48"/>
+      <c r="AS133" s="48"/>
+      <c r="AT133" s="48"/>
+      <c r="AU133" s="48"/>
+      <c r="AV133" s="48"/>
+      <c r="AW133" s="48"/>
+      <c r="AX133" s="48"/>
+      <c r="AY133" s="48"/>
+      <c r="AZ133" s="48"/>
+      <c r="BA133" s="48"/>
+      <c r="BB133" s="48"/>
+      <c r="BC133" s="48"/>
+      <c r="BD133" s="48"/>
+      <c r="BE133" s="48"/>
+      <c r="BF133" s="48"/>
+      <c r="BG133" s="48"/>
+      <c r="BH133" s="48"/>
+      <c r="BI133" s="48"/>
+      <c r="BJ133" s="48"/>
+      <c r="BK133" s="48"/>
+      <c r="BL133" s="48"/>
+      <c r="BM133" s="48"/>
+      <c r="BN133" s="48"/>
+      <c r="BO133" s="48"/>
     </row>
     <row r="134" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.1</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F134" s="42">
         <v>44379</v>
@@ -14613,14 +14633,14 @@
     <row r="135" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.2</v>
       </c>
       <c r="B135" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F135" s="42">
         <v>44379</v>
@@ -14690,17 +14710,17 @@
     <row r="136" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B136" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D136" s="66"/>
+        <v>13.3</v>
+      </c>
+      <c r="B136" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D136" s="70"/>
       <c r="E136" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F136" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G136" s="43"/>
       <c r="H136" s="25"/>
@@ -14765,11 +14785,20 @@
       <c r="BO136" s="46"/>
     </row>
     <row r="137" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="23"/>
-      <c r="B137" s="65"/>
-      <c r="D137" s="66"/>
-      <c r="E137" s="66"/>
-      <c r="F137" s="42"/>
+      <c r="A137" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.4</v>
+      </c>
+      <c r="B137" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D137" s="70"/>
+      <c r="E137" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F137" s="42">
+        <v>44379</v>
+      </c>
       <c r="G137" s="43"/>
       <c r="H137" s="25"/>
       <c r="I137" s="26"/>
@@ -14833,11 +14862,20 @@
       <c r="BO137" s="46"/>
     </row>
     <row r="138" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="23"/>
-      <c r="B138" s="65"/>
+      <c r="A138" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B138" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D138" s="66"/>
-      <c r="E138" s="66"/>
-      <c r="F138" s="42"/>
+      <c r="E138" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F138" s="42">
+        <v>44531</v>
+      </c>
       <c r="G138" s="43"/>
       <c r="H138" s="25"/>
       <c r="I138" s="26"/>
@@ -14971,7 +15009,7 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23"/>
       <c r="B140" s="65"/>
-      <c r="D140" s="70"/>
+      <c r="D140" s="66"/>
       <c r="E140" s="66"/>
       <c r="F140" s="42"/>
       <c r="G140" s="43"/>
@@ -15039,7 +15077,7 @@
     <row r="141" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23"/>
       <c r="B141" s="65"/>
-      <c r="D141" s="70"/>
+      <c r="D141" s="66"/>
       <c r="E141" s="66"/>
       <c r="F141" s="42"/>
       <c r="G141" s="43"/>
@@ -15311,7 +15349,7 @@
     <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23"/>
       <c r="B145" s="65"/>
-      <c r="D145" s="66"/>
+      <c r="D145" s="70"/>
       <c r="E145" s="66"/>
       <c r="F145" s="42"/>
       <c r="G145" s="43"/>
@@ -15379,7 +15417,7 @@
     <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23"/>
       <c r="B146" s="65"/>
-      <c r="D146" s="66"/>
+      <c r="D146" s="70"/>
       <c r="E146" s="66"/>
       <c r="F146" s="42"/>
       <c r="G146" s="43"/>
@@ -15583,7 +15621,7 @@
     <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="23"/>
       <c r="B149" s="65"/>
-      <c r="D149" s="70"/>
+      <c r="D149" s="66"/>
       <c r="E149" s="66"/>
       <c r="F149" s="42"/>
       <c r="G149" s="43"/>
@@ -15651,7 +15689,7 @@
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23"/>
       <c r="B150" s="65"/>
-      <c r="D150" s="70"/>
+      <c r="D150" s="66"/>
       <c r="E150" s="66"/>
       <c r="F150" s="42"/>
       <c r="G150" s="43"/>
@@ -15923,7 +15961,7 @@
     <row r="154" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="23"/>
       <c r="B154" s="65"/>
-      <c r="D154" s="66"/>
+      <c r="D154" s="70"/>
       <c r="E154" s="66"/>
       <c r="F154" s="42"/>
       <c r="G154" s="43"/>
@@ -15991,7 +16029,7 @@
     <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="23"/>
       <c r="B155" s="65"/>
-      <c r="D155" s="66"/>
+      <c r="D155" s="70"/>
       <c r="E155" s="66"/>
       <c r="F155" s="42"/>
       <c r="G155" s="43"/>
@@ -16195,7 +16233,7 @@
     <row r="158" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="23"/>
       <c r="B158" s="65"/>
-      <c r="D158" s="70"/>
+      <c r="D158" s="66"/>
       <c r="E158" s="66"/>
       <c r="F158" s="42"/>
       <c r="G158" s="43"/>
@@ -16263,7 +16301,7 @@
     <row r="159" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="23"/>
       <c r="B159" s="65"/>
-      <c r="D159" s="70"/>
+      <c r="D159" s="66"/>
       <c r="E159" s="66"/>
       <c r="F159" s="42"/>
       <c r="G159" s="43"/>
@@ -16535,7 +16573,7 @@
     <row r="163" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="23"/>
       <c r="B163" s="65"/>
-      <c r="D163" s="66"/>
+      <c r="D163" s="70"/>
       <c r="E163" s="66"/>
       <c r="F163" s="42"/>
       <c r="G163" s="43"/>
@@ -16603,7 +16641,7 @@
     <row r="164" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="23"/>
       <c r="B164" s="65"/>
-      <c r="D164" s="66"/>
+      <c r="D164" s="70"/>
       <c r="E164" s="66"/>
       <c r="F164" s="42"/>
       <c r="G164" s="43"/>
@@ -16807,7 +16845,7 @@
     <row r="167" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="23"/>
       <c r="B167" s="65"/>
-      <c r="D167" s="70"/>
+      <c r="D167" s="66"/>
       <c r="E167" s="66"/>
       <c r="F167" s="42"/>
       <c r="G167" s="43"/>
@@ -16875,7 +16913,7 @@
     <row r="168" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="23"/>
       <c r="B168" s="65"/>
-      <c r="D168" s="70"/>
+      <c r="D168" s="66"/>
       <c r="E168" s="66"/>
       <c r="F168" s="42"/>
       <c r="G168" s="43"/>
@@ -17144,18 +17182,145 @@
       <c r="BN171" s="46"/>
       <c r="BO171" s="46"/>
     </row>
+    <row r="172" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="23"/>
+      <c r="B172" s="65"/>
+      <c r="D172" s="70"/>
+      <c r="E172" s="66"/>
+      <c r="F172" s="42"/>
+      <c r="G172" s="43"/>
+      <c r="H172" s="25"/>
+      <c r="I172" s="26"/>
+      <c r="J172" s="27"/>
+      <c r="K172" s="40"/>
+      <c r="L172" s="46"/>
+      <c r="M172" s="46"/>
+      <c r="N172" s="46"/>
+      <c r="O172" s="46"/>
+      <c r="P172" s="46"/>
+      <c r="Q172" s="46"/>
+      <c r="R172" s="46"/>
+      <c r="S172" s="46"/>
+      <c r="T172" s="46"/>
+      <c r="U172" s="46"/>
+      <c r="V172" s="46"/>
+      <c r="W172" s="46"/>
+      <c r="X172" s="46"/>
+      <c r="Y172" s="46"/>
+      <c r="Z172" s="46"/>
+      <c r="AA172" s="46"/>
+      <c r="AB172" s="46"/>
+      <c r="AC172" s="46"/>
+      <c r="AD172" s="46"/>
+      <c r="AE172" s="46"/>
+      <c r="AF172" s="46"/>
+      <c r="AG172" s="46"/>
+      <c r="AH172" s="46"/>
+      <c r="AI172" s="46"/>
+      <c r="AJ172" s="46"/>
+      <c r="AK172" s="46"/>
+      <c r="AL172" s="46"/>
+      <c r="AM172" s="46"/>
+      <c r="AN172" s="46"/>
+      <c r="AO172" s="46"/>
+      <c r="AP172" s="46"/>
+      <c r="AQ172" s="46"/>
+      <c r="AR172" s="46"/>
+      <c r="AS172" s="46"/>
+      <c r="AT172" s="46"/>
+      <c r="AU172" s="46"/>
+      <c r="AV172" s="46"/>
+      <c r="AW172" s="46"/>
+      <c r="AX172" s="46"/>
+      <c r="AY172" s="46"/>
+      <c r="AZ172" s="46"/>
+      <c r="BA172" s="46"/>
+      <c r="BB172" s="46"/>
+      <c r="BC172" s="46"/>
+      <c r="BD172" s="46"/>
+      <c r="BE172" s="46"/>
+      <c r="BF172" s="46"/>
+      <c r="BG172" s="46"/>
+      <c r="BH172" s="46"/>
+      <c r="BI172" s="46"/>
+      <c r="BJ172" s="46"/>
+      <c r="BK172" s="46"/>
+      <c r="BL172" s="46"/>
+      <c r="BM172" s="46"/>
+      <c r="BN172" s="46"/>
+      <c r="BO172" s="46"/>
+    </row>
+    <row r="173" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="23"/>
+      <c r="B173" s="65"/>
+      <c r="D173" s="70"/>
+      <c r="E173" s="66"/>
+      <c r="F173" s="42"/>
+      <c r="G173" s="43"/>
+      <c r="H173" s="25"/>
+      <c r="I173" s="26"/>
+      <c r="J173" s="27"/>
+      <c r="K173" s="40"/>
+      <c r="L173" s="46"/>
+      <c r="M173" s="46"/>
+      <c r="N173" s="46"/>
+      <c r="O173" s="46"/>
+      <c r="P173" s="46"/>
+      <c r="Q173" s="46"/>
+      <c r="R173" s="46"/>
+      <c r="S173" s="46"/>
+      <c r="T173" s="46"/>
+      <c r="U173" s="46"/>
+      <c r="V173" s="46"/>
+      <c r="W173" s="46"/>
+      <c r="X173" s="46"/>
+      <c r="Y173" s="46"/>
+      <c r="Z173" s="46"/>
+      <c r="AA173" s="46"/>
+      <c r="AB173" s="46"/>
+      <c r="AC173" s="46"/>
+      <c r="AD173" s="46"/>
+      <c r="AE173" s="46"/>
+      <c r="AF173" s="46"/>
+      <c r="AG173" s="46"/>
+      <c r="AH173" s="46"/>
+      <c r="AI173" s="46"/>
+      <c r="AJ173" s="46"/>
+      <c r="AK173" s="46"/>
+      <c r="AL173" s="46"/>
+      <c r="AM173" s="46"/>
+      <c r="AN173" s="46"/>
+      <c r="AO173" s="46"/>
+      <c r="AP173" s="46"/>
+      <c r="AQ173" s="46"/>
+      <c r="AR173" s="46"/>
+      <c r="AS173" s="46"/>
+      <c r="AT173" s="46"/>
+      <c r="AU173" s="46"/>
+      <c r="AV173" s="46"/>
+      <c r="AW173" s="46"/>
+      <c r="AX173" s="46"/>
+      <c r="AY173" s="46"/>
+      <c r="AZ173" s="46"/>
+      <c r="BA173" s="46"/>
+      <c r="BB173" s="46"/>
+      <c r="BC173" s="46"/>
+      <c r="BD173" s="46"/>
+      <c r="BE173" s="46"/>
+      <c r="BF173" s="46"/>
+      <c r="BG173" s="46"/>
+      <c r="BH173" s="46"/>
+      <c r="BI173" s="46"/>
+      <c r="BJ173" s="46"/>
+      <c r="BK173" s="46"/>
+      <c r="BL173" s="46"/>
+      <c r="BM173" s="46"/>
+      <c r="BN173" s="46"/>
+      <c r="BO173" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17166,9 +17331,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I132:I135 I98:I103 I105:I110 I112:I122 I124:I130">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I134:I137 I98:I103 I105:I110 I112:I122 I124:I132">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17187,7 +17361,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN130 L136:BO138 M139:BN144 BO142:BO144 L145:BO147 M148:BN153 BO151:BO153 L154:BO156 M157:BN162 BO160:BO162 L163:BO165 M166:BN171 BO169:BO171 BO134:BO135 M132:BN135 L131:BO131 L123:BO123">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN132 L138:BO140 M141:BN146 BO144:BO146 L147:BO149 M150:BN155 BO153:BO155 L156:BO158 M159:BN164 BO162:BO164 L165:BO167 M168:BN173 BO171:BO173 BO136:BO137 M134:BN137 L133:BO133 L123:BO123">
     <cfRule type="expression" dxfId="132" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -17195,7 +17369,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L132:BO135 L98:BO103 L105:BO110 L112:BO122 L124:BO130">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L134:BO137 L98:BO103 L105:BO110 L112:BO122 L124:BO132">
     <cfRule type="expression" dxfId="130" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -17205,7 +17379,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E172:E1048576 E95:E96 E132:E135 E98:E103 E105:E110 E112:E122 E124:E130">
+  <conditionalFormatting sqref="E1:E73 E174:E1048576 E95:E96 E134:E137 E98:E103 E105:E110 E112:E122 E124:E132">
     <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17299,7 +17473,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I136:I144">
+  <conditionalFormatting sqref="I138:I146">
     <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17313,12 +17487,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L136:BO144">
+  <conditionalFormatting sqref="L138:BO146">
     <cfRule type="expression" dxfId="106" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E136:E144">
+  <conditionalFormatting sqref="E138:E146">
     <cfRule type="cellIs" dxfId="105" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17341,7 +17515,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L139:BO144 L132:BO135 L98:BO103 L105:BO110 L112:BO122 L124:BO130">
+  <conditionalFormatting sqref="L141:BO146 L134:BO137 L98:BO103 L105:BO110 L112:BO122 L124:BO132">
     <cfRule type="expression" dxfId="98" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17349,7 +17523,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I145:I153">
+  <conditionalFormatting sqref="I147:I155">
     <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17363,12 +17537,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L145:BO153">
+  <conditionalFormatting sqref="L147:BO155">
     <cfRule type="expression" dxfId="96" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E145:E153">
+  <conditionalFormatting sqref="E147:E155">
     <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17391,7 +17565,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L148:BO153">
+  <conditionalFormatting sqref="L150:BO155">
     <cfRule type="expression" dxfId="88" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17399,7 +17573,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I154:I162">
+  <conditionalFormatting sqref="I156:I164">
     <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17413,12 +17587,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L154:BO162">
+  <conditionalFormatting sqref="L156:BO164">
     <cfRule type="expression" dxfId="86" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E154:E162">
+  <conditionalFormatting sqref="E156:E164">
     <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17441,7 +17615,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L157:BO162">
+  <conditionalFormatting sqref="L159:BO164">
     <cfRule type="expression" dxfId="78" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17449,7 +17623,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I163:I171">
+  <conditionalFormatting sqref="I165:I173">
     <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17463,12 +17637,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L163:BO171">
+  <conditionalFormatting sqref="L165:BO173">
     <cfRule type="expression" dxfId="76" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E163:E171">
+  <conditionalFormatting sqref="E165:E173">
     <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17491,7 +17665,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L166:BO171">
+  <conditionalFormatting sqref="L168:BO173">
     <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -17641,7 +17815,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I131">
+  <conditionalFormatting sqref="I133">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -17655,12 +17829,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L131:BO131">
+  <conditionalFormatting sqref="L133:BO133">
     <cfRule type="expression" dxfId="38" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E131">
+  <conditionalFormatting sqref="E133">
     <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -17881,7 +18055,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I132:I135 I98:I103 I105:I110 I112:I122 I124:I130</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I134:I137 I98:I103 I105:I110 I112:I122 I124:I132</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -17911,7 +18085,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I136:I144</xm:sqref>
+          <xm:sqref>I138:I146</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -17926,7 +18100,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I145:I153</xm:sqref>
+          <xm:sqref>I147:I155</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -17941,7 +18115,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I154:I162</xm:sqref>
+          <xm:sqref>I156:I164</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -17956,7 +18130,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I163:I171</xm:sqref>
+          <xm:sqref>I165:I173</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -18016,7 +18190,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I131</xm:sqref>
+          <xm:sqref>I133</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Added CBO import (v0.17)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDD78D8-8072-4C74-B2B2-5450552F5451}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7976D6-651B-4218-AA88-FC055F198889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1857,13 +1857,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1873,10 +1866,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1885,6 +1874,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3449,7 +3449,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B136" sqref="B136"/>
+      <selection pane="bottomLeft" activeCell="I131" sqref="I131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3479,27 +3479,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3544,12 +3544,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3559,183 +3559,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 41</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 42</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 43</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 44</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 45</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 46</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 47</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 48</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44473</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44480</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44487</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44494</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44501</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44508</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44515</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44522</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -14116,7 +14116,7 @@
       </c>
       <c r="H128" s="73"/>
       <c r="I128" s="26">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="J128" s="75"/>
       <c r="K128" s="76"/>
@@ -14197,7 +14197,7 @@
       </c>
       <c r="H129" s="73"/>
       <c r="I129" s="26">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="J129" s="75"/>
       <c r="K129" s="76"/>
@@ -14278,7 +14278,7 @@
       </c>
       <c r="H130" s="73"/>
       <c r="I130" s="26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J130" s="75"/>
       <c r="K130" s="76"/>
@@ -18077,6 +18077,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -18087,15 +18096,6 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I143:I146 I98:I103 I105:I110 I112:I122 I124:I141">

</xml_diff>

<commit_message>
Updated PM and README (V0.17)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B7976D6-651B-4218-AA88-FC055F198889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB4B56-8918-44B2-B220-57D20D87EC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
   <si>
     <t>WBS</t>
   </si>
@@ -929,6 +929,15 @@
   </si>
   <si>
     <t>Split External Forecasts Import - Create Own Database</t>
+  </si>
+  <si>
+    <t>Refactor Model Pulls to use Repo DB</t>
+  </si>
+  <si>
+    <t>SQL to Pull from Correct Vintage</t>
+  </si>
+  <si>
+    <t>Website Color &amp; Redesign</t>
   </si>
 </sst>
 </file>
@@ -1857,6 +1866,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1866,6 +1882,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1874,17 +1894,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3038,7 +3047,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="41"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="43"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3445,11 +3454,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO182"/>
+  <dimension ref="A1:BO185"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I131" sqref="I131"/>
+      <pane ySplit="7" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M140" sqref="M140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3479,27 +3488,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3544,198 +3553,198 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 41</v>
-      </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+        <v>Week 43</v>
+      </c>
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 42</v>
-      </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+        <v>Week 44</v>
+      </c>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 43</v>
-      </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+        <v>Week 45</v>
+      </c>
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 44</v>
-      </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+        <v>Week 46</v>
+      </c>
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 45</v>
-      </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+        <v>Week 47</v>
+      </c>
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 46</v>
-      </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+        <v>Week 48</v>
+      </c>
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 47</v>
-      </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+        <v>Week 49</v>
+      </c>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 48</v>
-      </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+        <v>Week 50</v>
+      </c>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
-        <v>44473</v>
-      </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+        <v>44487</v>
+      </c>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
-        <v>44480</v>
-      </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+        <v>44494</v>
+      </c>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
-        <v>44487</v>
-      </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+        <v>44501</v>
+      </c>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
-        <v>44494</v>
-      </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+        <v>44508</v>
+      </c>
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
-        <v>44501</v>
-      </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+        <v>44515</v>
+      </c>
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
-        <v>44508</v>
-      </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+        <v>44522</v>
+      </c>
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
-        <v>44515</v>
-      </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+        <v>44529</v>
+      </c>
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
-        <v>44522</v>
-      </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+        <v>44536</v>
+      </c>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -3751,227 +3760,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44473</v>
+        <v>44487</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44474</v>
+        <v>44488</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44475</v>
+        <v>44489</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44476</v>
+        <v>44490</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44477</v>
+        <v>44491</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44478</v>
+        <v>44492</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44479</v>
+        <v>44493</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44480</v>
+        <v>44494</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44481</v>
+        <v>44495</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44482</v>
+        <v>44496</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44483</v>
+        <v>44497</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44484</v>
+        <v>44498</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44485</v>
+        <v>44499</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44486</v>
+        <v>44500</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44487</v>
+        <v>44501</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44488</v>
+        <v>44502</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44489</v>
+        <v>44503</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44490</v>
+        <v>44504</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44491</v>
+        <v>44505</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44492</v>
+        <v>44506</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44493</v>
+        <v>44507</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44494</v>
+        <v>44508</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44495</v>
+        <v>44509</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44496</v>
+        <v>44510</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44497</v>
+        <v>44511</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44498</v>
+        <v>44512</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44499</v>
+        <v>44513</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44500</v>
+        <v>44514</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44501</v>
+        <v>44515</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44502</v>
+        <v>44516</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44503</v>
+        <v>44517</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44504</v>
+        <v>44518</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44505</v>
+        <v>44519</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44506</v>
+        <v>44520</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44507</v>
+        <v>44521</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44508</v>
+        <v>44522</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44509</v>
+        <v>44523</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44510</v>
+        <v>44524</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44511</v>
+        <v>44525</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44512</v>
+        <v>44526</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44513</v>
+        <v>44527</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44514</v>
+        <v>44528</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44515</v>
+        <v>44529</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44516</v>
+        <v>44530</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44517</v>
+        <v>44531</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44518</v>
+        <v>44532</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44519</v>
+        <v>44533</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44520</v>
+        <v>44534</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44521</v>
+        <v>44535</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44522</v>
+        <v>44536</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44523</v>
+        <v>44537</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44524</v>
+        <v>44538</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44525</v>
+        <v>44539</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44526</v>
+        <v>44540</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44527</v>
+        <v>44541</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44528</v>
+        <v>44542</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8893,7 +8902,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A147" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A150" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -14112,11 +14121,11 @@
         <v>44475</v>
       </c>
       <c r="G128" s="43">
-        <v>44477</v>
+        <v>44487</v>
       </c>
       <c r="H128" s="73"/>
       <c r="I128" s="26">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="J128" s="75"/>
       <c r="K128" s="76"/>
@@ -14190,14 +14199,14 @@
         <v>67</v>
       </c>
       <c r="F129" s="42">
-        <v>44476</v>
+        <v>44479</v>
       </c>
       <c r="G129" s="43">
-        <v>44479</v>
+        <v>44487</v>
       </c>
       <c r="H129" s="73"/>
       <c r="I129" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J129" s="75"/>
       <c r="K129" s="76"/>
@@ -14274,11 +14283,11 @@
         <v>44476</v>
       </c>
       <c r="G130" s="43">
-        <v>44479</v>
+        <v>44488</v>
       </c>
       <c r="H130" s="73"/>
       <c r="I130" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J130" s="75"/>
       <c r="K130" s="76"/>
@@ -14345,17 +14354,17 @@
         <v>12.8</v>
       </c>
       <c r="B131" s="65" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="D131" s="70"/>
       <c r="E131" s="66" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F131" s="42">
-        <v>44478</v>
+        <v>44489</v>
       </c>
       <c r="G131" s="43">
-        <v>44484</v>
+        <v>44492</v>
       </c>
       <c r="H131" s="73"/>
       <c r="I131" s="26">
@@ -14426,17 +14435,17 @@
         <v>12.9</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
       <c r="D132" s="70"/>
       <c r="E132" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F132" s="42">
-        <v>44478</v>
+        <v>44489</v>
       </c>
       <c r="G132" s="43">
-        <v>44484</v>
+        <v>44492</v>
       </c>
       <c r="H132" s="73"/>
       <c r="I132" s="26">
@@ -14507,17 +14516,17 @@
         <v>12.10</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F133" s="42">
-        <v>44478</v>
+        <v>44492</v>
       </c>
       <c r="G133" s="43">
-        <v>44484</v>
+        <v>44493</v>
       </c>
       <c r="H133" s="73"/>
       <c r="I133" s="26">
@@ -14588,17 +14597,17 @@
         <v>12.11</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
         <v>69</v>
       </c>
       <c r="F134" s="42">
-        <v>44478</v>
+        <v>44494</v>
       </c>
       <c r="G134" s="43">
-        <v>44484</v>
+        <v>44499</v>
       </c>
       <c r="H134" s="73"/>
       <c r="I134" s="26">
@@ -14669,17 +14678,17 @@
         <v>12.12</v>
       </c>
       <c r="B135" s="65" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F135" s="42">
-        <v>44484</v>
+        <v>44494</v>
       </c>
       <c r="G135" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H135" s="73"/>
       <c r="I135" s="26">
@@ -14750,21 +14759,21 @@
         <v>12.13</v>
       </c>
       <c r="B136" s="65" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
       <c r="D136" s="70"/>
       <c r="E136" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F136" s="42">
-        <v>44484</v>
+        <v>44494</v>
       </c>
       <c r="G136" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H136" s="73"/>
       <c r="I136" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="J136" s="75"/>
       <c r="K136" s="76"/>
@@ -14831,17 +14840,17 @@
         <v>12.14</v>
       </c>
       <c r="B137" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D137" s="70"/>
       <c r="E137" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F137" s="42">
-        <v>44484</v>
+        <v>44494</v>
       </c>
       <c r="G137" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H137" s="73"/>
       <c r="I137" s="26">
@@ -14912,17 +14921,17 @@
         <v>12.15</v>
       </c>
       <c r="B138" s="65" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
       <c r="D138" s="70"/>
       <c r="E138" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F138" s="42">
-        <v>44484</v>
+        <v>44494</v>
       </c>
       <c r="G138" s="43">
-        <v>44510</v>
+        <v>44501</v>
       </c>
       <c r="H138" s="73"/>
       <c r="I138" s="26">
@@ -14993,21 +15002,21 @@
         <v>12.16</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D139" s="70"/>
-      <c r="E139" s="70" t="s">
+      <c r="E139" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F139" s="71">
-        <v>44489</v>
-      </c>
-      <c r="G139" s="72">
-        <v>44510</v>
+      <c r="F139" s="42">
+        <v>44494</v>
+      </c>
+      <c r="G139" s="43">
+        <v>44501</v>
       </c>
       <c r="H139" s="73"/>
-      <c r="I139" s="74">
-        <v>0</v>
+      <c r="I139" s="26">
+        <v>0.3</v>
       </c>
       <c r="J139" s="75"/>
       <c r="K139" s="76"/>
@@ -15074,20 +15083,20 @@
         <v>12.17</v>
       </c>
       <c r="B140" s="65" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="D140" s="70"/>
-      <c r="E140" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F140" s="71">
-        <v>44489</v>
-      </c>
-      <c r="G140" s="72">
-        <v>44510</v>
+      <c r="E140" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F140" s="42">
+        <v>44494</v>
+      </c>
+      <c r="G140" s="43">
+        <v>44501</v>
       </c>
       <c r="H140" s="73"/>
-      <c r="I140" s="74">
+      <c r="I140" s="26">
         <v>0</v>
       </c>
       <c r="J140" s="75"/>
@@ -15155,20 +15164,20 @@
         <v>12.18</v>
       </c>
       <c r="B141" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D141" s="70"/>
-      <c r="E141" s="70" t="s">
-        <v>71</v>
-      </c>
-      <c r="F141" s="71">
-        <v>44489</v>
-      </c>
-      <c r="G141" s="72">
-        <v>44520</v>
+      <c r="E141" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F141" s="42">
+        <v>44494</v>
+      </c>
+      <c r="G141" s="43">
+        <v>44510</v>
       </c>
       <c r="H141" s="73"/>
-      <c r="I141" s="74">
+      <c r="I141" s="26">
         <v>0</v>
       </c>
       <c r="J141" s="75"/>
@@ -15230,105 +15239,111 @@
       <c r="BN141" s="46"/>
       <c r="BO141" s="46"/>
     </row>
-    <row r="142" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>13</v>
-      </c>
-      <c r="B142" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D142" s="19"/>
-      <c r="E142" s="19"/>
-      <c r="F142" s="44"/>
-      <c r="G142" s="44" t="str">
-        <f t="shared" ref="G142" si="24">IF(ISBLANK(F142)," - ",IF(H142=0,F142,F142+H142-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H142" s="20"/>
-      <c r="I142" s="21"/>
-      <c r="J142" s="22" t="str">
-        <f t="shared" ref="J142" si="25">IF(OR(G142=0,F142=0)," - ",NETWORKDAYS(F142,G142))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K142" s="41"/>
-      <c r="L142" s="48"/>
-      <c r="M142" s="48"/>
-      <c r="N142" s="48"/>
-      <c r="O142" s="48"/>
-      <c r="P142" s="48"/>
-      <c r="Q142" s="48"/>
-      <c r="R142" s="48"/>
-      <c r="S142" s="48"/>
-      <c r="T142" s="48"/>
-      <c r="U142" s="48"/>
-      <c r="V142" s="48"/>
-      <c r="W142" s="48"/>
-      <c r="X142" s="48"/>
-      <c r="Y142" s="48"/>
-      <c r="Z142" s="48"/>
-      <c r="AA142" s="48"/>
-      <c r="AB142" s="48"/>
-      <c r="AC142" s="48"/>
-      <c r="AD142" s="48"/>
-      <c r="AE142" s="48"/>
-      <c r="AF142" s="48"/>
-      <c r="AG142" s="48"/>
-      <c r="AH142" s="48"/>
-      <c r="AI142" s="48"/>
-      <c r="AJ142" s="48"/>
-      <c r="AK142" s="48"/>
-      <c r="AL142" s="48"/>
-      <c r="AM142" s="48"/>
-      <c r="AN142" s="48"/>
-      <c r="AO142" s="48"/>
-      <c r="AP142" s="48"/>
-      <c r="AQ142" s="48"/>
-      <c r="AR142" s="48"/>
-      <c r="AS142" s="48"/>
-      <c r="AT142" s="48"/>
-      <c r="AU142" s="48"/>
-      <c r="AV142" s="48"/>
-      <c r="AW142" s="48"/>
-      <c r="AX142" s="48"/>
-      <c r="AY142" s="48"/>
-      <c r="AZ142" s="48"/>
-      <c r="BA142" s="48"/>
-      <c r="BB142" s="48"/>
-      <c r="BC142" s="48"/>
-      <c r="BD142" s="48"/>
-      <c r="BE142" s="48"/>
-      <c r="BF142" s="48"/>
-      <c r="BG142" s="48"/>
-      <c r="BH142" s="48"/>
-      <c r="BI142" s="48"/>
-      <c r="BJ142" s="48"/>
-      <c r="BK142" s="48"/>
-      <c r="BL142" s="48"/>
-      <c r="BM142" s="48"/>
-      <c r="BN142" s="48"/>
-      <c r="BO142" s="48"/>
+    <row r="142" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.19</v>
+      </c>
+      <c r="B142" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="D142" s="70"/>
+      <c r="E142" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="F142" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G142" s="72">
+        <v>44510</v>
+      </c>
+      <c r="H142" s="73"/>
+      <c r="I142" s="74">
+        <v>0</v>
+      </c>
+      <c r="J142" s="75"/>
+      <c r="K142" s="76"/>
+      <c r="L142" s="46"/>
+      <c r="M142" s="46"/>
+      <c r="N142" s="46"/>
+      <c r="O142" s="46"/>
+      <c r="P142" s="46"/>
+      <c r="Q142" s="46"/>
+      <c r="R142" s="46"/>
+      <c r="S142" s="46"/>
+      <c r="T142" s="46"/>
+      <c r="U142" s="46"/>
+      <c r="V142" s="46"/>
+      <c r="W142" s="46"/>
+      <c r="X142" s="46"/>
+      <c r="Y142" s="46"/>
+      <c r="Z142" s="46"/>
+      <c r="AA142" s="46"/>
+      <c r="AB142" s="46"/>
+      <c r="AC142" s="46"/>
+      <c r="AD142" s="46"/>
+      <c r="AE142" s="46"/>
+      <c r="AF142" s="46"/>
+      <c r="AG142" s="46"/>
+      <c r="AH142" s="46"/>
+      <c r="AI142" s="46"/>
+      <c r="AJ142" s="46"/>
+      <c r="AK142" s="46"/>
+      <c r="AL142" s="46"/>
+      <c r="AM142" s="46"/>
+      <c r="AN142" s="46"/>
+      <c r="AO142" s="46"/>
+      <c r="AP142" s="46"/>
+      <c r="AQ142" s="46"/>
+      <c r="AR142" s="46"/>
+      <c r="AS142" s="46"/>
+      <c r="AT142" s="46"/>
+      <c r="AU142" s="46"/>
+      <c r="AV142" s="46"/>
+      <c r="AW142" s="46"/>
+      <c r="AX142" s="46"/>
+      <c r="AY142" s="46"/>
+      <c r="AZ142" s="46"/>
+      <c r="BA142" s="46"/>
+      <c r="BB142" s="46"/>
+      <c r="BC142" s="46"/>
+      <c r="BD142" s="46"/>
+      <c r="BE142" s="46"/>
+      <c r="BF142" s="46"/>
+      <c r="BG142" s="46"/>
+      <c r="BH142" s="46"/>
+      <c r="BI142" s="46"/>
+      <c r="BJ142" s="46"/>
+      <c r="BK142" s="46"/>
+      <c r="BL142" s="46"/>
+      <c r="BM142" s="46"/>
+      <c r="BN142" s="46"/>
+      <c r="BO142" s="46"/>
     </row>
     <row r="143" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.1</v>
+        <v>12.20</v>
       </c>
       <c r="B143" s="65" t="s">
-        <v>105</v>
+        <v>140</v>
       </c>
       <c r="D143" s="70"/>
-      <c r="E143" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F143" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G143" s="43"/>
-      <c r="H143" s="25"/>
-      <c r="I143" s="26"/>
-      <c r="J143" s="27"/>
-      <c r="K143" s="40"/>
+      <c r="E143" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F143" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G143" s="72">
+        <v>44510</v>
+      </c>
+      <c r="H143" s="73"/>
+      <c r="I143" s="74">
+        <v>0</v>
+      </c>
+      <c r="J143" s="75"/>
+      <c r="K143" s="76"/>
       <c r="L143" s="46"/>
       <c r="M143" s="46"/>
       <c r="N143" s="46"/>
@@ -15389,23 +15404,27 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.2</v>
+        <v>12.21</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="D144" s="70"/>
-      <c r="E144" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F144" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G144" s="43"/>
-      <c r="H144" s="25"/>
-      <c r="I144" s="26"/>
-      <c r="J144" s="27"/>
-      <c r="K144" s="40"/>
+      <c r="E144" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F144" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G144" s="72">
+        <v>44520</v>
+      </c>
+      <c r="H144" s="73"/>
+      <c r="I144" s="74">
+        <v>0</v>
+      </c>
+      <c r="J144" s="75"/>
+      <c r="K144" s="76"/>
       <c r="L144" s="46"/>
       <c r="M144" s="46"/>
       <c r="N144" s="46"/>
@@ -15463,94 +15482,96 @@
       <c r="BN144" s="46"/>
       <c r="BO144" s="46"/>
     </row>
-    <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.3</v>
-      </c>
-      <c r="B145" s="65" t="s">
-        <v>108</v>
-      </c>
-      <c r="D145" s="70"/>
-      <c r="E145" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="F145" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G145" s="43"/>
-      <c r="H145" s="25"/>
-      <c r="I145" s="26"/>
-      <c r="J145" s="27"/>
-      <c r="K145" s="40"/>
-      <c r="L145" s="46"/>
-      <c r="M145" s="46"/>
-      <c r="N145" s="46"/>
-      <c r="O145" s="46"/>
-      <c r="P145" s="46"/>
-      <c r="Q145" s="46"/>
-      <c r="R145" s="46"/>
-      <c r="S145" s="46"/>
-      <c r="T145" s="46"/>
-      <c r="U145" s="46"/>
-      <c r="V145" s="46"/>
-      <c r="W145" s="46"/>
-      <c r="X145" s="46"/>
-      <c r="Y145" s="46"/>
-      <c r="Z145" s="46"/>
-      <c r="AA145" s="46"/>
-      <c r="AB145" s="46"/>
-      <c r="AC145" s="46"/>
-      <c r="AD145" s="46"/>
-      <c r="AE145" s="46"/>
-      <c r="AF145" s="46"/>
-      <c r="AG145" s="46"/>
-      <c r="AH145" s="46"/>
-      <c r="AI145" s="46"/>
-      <c r="AJ145" s="46"/>
-      <c r="AK145" s="46"/>
-      <c r="AL145" s="46"/>
-      <c r="AM145" s="46"/>
-      <c r="AN145" s="46"/>
-      <c r="AO145" s="46"/>
-      <c r="AP145" s="46"/>
-      <c r="AQ145" s="46"/>
-      <c r="AR145" s="46"/>
-      <c r="AS145" s="46"/>
-      <c r="AT145" s="46"/>
-      <c r="AU145" s="46"/>
-      <c r="AV145" s="46"/>
-      <c r="AW145" s="46"/>
-      <c r="AX145" s="46"/>
-      <c r="AY145" s="46"/>
-      <c r="AZ145" s="46"/>
-      <c r="BA145" s="46"/>
-      <c r="BB145" s="46"/>
-      <c r="BC145" s="46"/>
-      <c r="BD145" s="46"/>
-      <c r="BE145" s="46"/>
-      <c r="BF145" s="46"/>
-      <c r="BG145" s="46"/>
-      <c r="BH145" s="46"/>
-      <c r="BI145" s="46"/>
-      <c r="BJ145" s="46"/>
-      <c r="BK145" s="46"/>
-      <c r="BL145" s="46"/>
-      <c r="BM145" s="46"/>
-      <c r="BN145" s="46"/>
-      <c r="BO145" s="46"/>
+    <row r="145" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>13</v>
+      </c>
+      <c r="B145" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D145" s="19"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="44"/>
+      <c r="G145" s="44" t="str">
+        <f t="shared" ref="G145" si="24">IF(ISBLANK(F145)," - ",IF(H145=0,F145,F145+H145-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H145" s="20"/>
+      <c r="I145" s="21"/>
+      <c r="J145" s="22" t="str">
+        <f t="shared" ref="J145" si="25">IF(OR(G145=0,F145=0)," - ",NETWORKDAYS(F145,G145))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K145" s="41"/>
+      <c r="L145" s="48"/>
+      <c r="M145" s="48"/>
+      <c r="N145" s="48"/>
+      <c r="O145" s="48"/>
+      <c r="P145" s="48"/>
+      <c r="Q145" s="48"/>
+      <c r="R145" s="48"/>
+      <c r="S145" s="48"/>
+      <c r="T145" s="48"/>
+      <c r="U145" s="48"/>
+      <c r="V145" s="48"/>
+      <c r="W145" s="48"/>
+      <c r="X145" s="48"/>
+      <c r="Y145" s="48"/>
+      <c r="Z145" s="48"/>
+      <c r="AA145" s="48"/>
+      <c r="AB145" s="48"/>
+      <c r="AC145" s="48"/>
+      <c r="AD145" s="48"/>
+      <c r="AE145" s="48"/>
+      <c r="AF145" s="48"/>
+      <c r="AG145" s="48"/>
+      <c r="AH145" s="48"/>
+      <c r="AI145" s="48"/>
+      <c r="AJ145" s="48"/>
+      <c r="AK145" s="48"/>
+      <c r="AL145" s="48"/>
+      <c r="AM145" s="48"/>
+      <c r="AN145" s="48"/>
+      <c r="AO145" s="48"/>
+      <c r="AP145" s="48"/>
+      <c r="AQ145" s="48"/>
+      <c r="AR145" s="48"/>
+      <c r="AS145" s="48"/>
+      <c r="AT145" s="48"/>
+      <c r="AU145" s="48"/>
+      <c r="AV145" s="48"/>
+      <c r="AW145" s="48"/>
+      <c r="AX145" s="48"/>
+      <c r="AY145" s="48"/>
+      <c r="AZ145" s="48"/>
+      <c r="BA145" s="48"/>
+      <c r="BB145" s="48"/>
+      <c r="BC145" s="48"/>
+      <c r="BD145" s="48"/>
+      <c r="BE145" s="48"/>
+      <c r="BF145" s="48"/>
+      <c r="BG145" s="48"/>
+      <c r="BH145" s="48"/>
+      <c r="BI145" s="48"/>
+      <c r="BJ145" s="48"/>
+      <c r="BK145" s="48"/>
+      <c r="BL145" s="48"/>
+      <c r="BM145" s="48"/>
+      <c r="BN145" s="48"/>
+      <c r="BO145" s="48"/>
     </row>
     <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.1</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D146" s="70"/>
       <c r="E146" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F146" s="42">
         <v>44379</v>
@@ -15620,17 +15641,17 @@
     <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B147" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D147" s="66"/>
+        <v>13.2</v>
+      </c>
+      <c r="B147" s="65" t="s">
+        <v>107</v>
+      </c>
+      <c r="D147" s="70"/>
       <c r="E147" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F147" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G147" s="43"/>
       <c r="H147" s="25"/>
@@ -15695,11 +15716,20 @@
       <c r="BO147" s="46"/>
     </row>
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="23"/>
-      <c r="B148" s="65"/>
-      <c r="D148" s="66"/>
-      <c r="E148" s="66"/>
-      <c r="F148" s="42"/>
+      <c r="A148" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.3</v>
+      </c>
+      <c r="B148" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D148" s="70"/>
+      <c r="E148" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F148" s="42">
+        <v>44379</v>
+      </c>
       <c r="G148" s="43"/>
       <c r="H148" s="25"/>
       <c r="I148" s="26"/>
@@ -15763,11 +15793,20 @@
       <c r="BO148" s="46"/>
     </row>
     <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="23"/>
-      <c r="B149" s="65"/>
-      <c r="D149" s="66"/>
-      <c r="E149" s="66"/>
-      <c r="F149" s="42"/>
+      <c r="A149" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.4</v>
+      </c>
+      <c r="B149" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D149" s="70"/>
+      <c r="E149" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F149" s="42">
+        <v>44379</v>
+      </c>
       <c r="G149" s="43"/>
       <c r="H149" s="25"/>
       <c r="I149" s="26"/>
@@ -15831,11 +15870,20 @@
       <c r="BO149" s="46"/>
     </row>
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="23"/>
-      <c r="B150" s="65"/>
+      <c r="A150" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B150" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D150" s="66"/>
-      <c r="E150" s="66"/>
-      <c r="F150" s="42"/>
+      <c r="E150" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F150" s="42">
+        <v>44531</v>
+      </c>
       <c r="G150" s="43"/>
       <c r="H150" s="25"/>
       <c r="I150" s="26"/>
@@ -15901,7 +15949,7 @@
     <row r="151" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="23"/>
       <c r="B151" s="65"/>
-      <c r="D151" s="70"/>
+      <c r="D151" s="66"/>
       <c r="E151" s="66"/>
       <c r="F151" s="42"/>
       <c r="G151" s="43"/>
@@ -15969,7 +16017,7 @@
     <row r="152" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="23"/>
       <c r="B152" s="65"/>
-      <c r="D152" s="70"/>
+      <c r="D152" s="66"/>
       <c r="E152" s="66"/>
       <c r="F152" s="42"/>
       <c r="G152" s="43"/>
@@ -16037,7 +16085,7 @@
     <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="23"/>
       <c r="B153" s="65"/>
-      <c r="D153" s="70"/>
+      <c r="D153" s="66"/>
       <c r="E153" s="66"/>
       <c r="F153" s="42"/>
       <c r="G153" s="43"/>
@@ -16241,7 +16289,7 @@
     <row r="156" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="23"/>
       <c r="B156" s="65"/>
-      <c r="D156" s="66"/>
+      <c r="D156" s="70"/>
       <c r="E156" s="66"/>
       <c r="F156" s="42"/>
       <c r="G156" s="43"/>
@@ -16309,7 +16357,7 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23"/>
       <c r="B157" s="65"/>
-      <c r="D157" s="66"/>
+      <c r="D157" s="70"/>
       <c r="E157" s="66"/>
       <c r="F157" s="42"/>
       <c r="G157" s="43"/>
@@ -16377,7 +16425,7 @@
     <row r="158" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="23"/>
       <c r="B158" s="65"/>
-      <c r="D158" s="66"/>
+      <c r="D158" s="70"/>
       <c r="E158" s="66"/>
       <c r="F158" s="42"/>
       <c r="G158" s="43"/>
@@ -16513,7 +16561,7 @@
     <row r="160" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="23"/>
       <c r="B160" s="65"/>
-      <c r="D160" s="70"/>
+      <c r="D160" s="66"/>
       <c r="E160" s="66"/>
       <c r="F160" s="42"/>
       <c r="G160" s="43"/>
@@ -16581,7 +16629,7 @@
     <row r="161" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="23"/>
       <c r="B161" s="65"/>
-      <c r="D161" s="70"/>
+      <c r="D161" s="66"/>
       <c r="E161" s="66"/>
       <c r="F161" s="42"/>
       <c r="G161" s="43"/>
@@ -16649,7 +16697,7 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23"/>
       <c r="B162" s="65"/>
-      <c r="D162" s="70"/>
+      <c r="D162" s="66"/>
       <c r="E162" s="66"/>
       <c r="F162" s="42"/>
       <c r="G162" s="43"/>
@@ -16853,7 +16901,7 @@
     <row r="165" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="23"/>
       <c r="B165" s="65"/>
-      <c r="D165" s="66"/>
+      <c r="D165" s="70"/>
       <c r="E165" s="66"/>
       <c r="F165" s="42"/>
       <c r="G165" s="43"/>
@@ -16921,7 +16969,7 @@
     <row r="166" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23"/>
       <c r="B166" s="65"/>
-      <c r="D166" s="66"/>
+      <c r="D166" s="70"/>
       <c r="E166" s="66"/>
       <c r="F166" s="42"/>
       <c r="G166" s="43"/>
@@ -16989,7 +17037,7 @@
     <row r="167" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="23"/>
       <c r="B167" s="65"/>
-      <c r="D167" s="66"/>
+      <c r="D167" s="70"/>
       <c r="E167" s="66"/>
       <c r="F167" s="42"/>
       <c r="G167" s="43"/>
@@ -17125,7 +17173,7 @@
     <row r="169" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="23"/>
       <c r="B169" s="65"/>
-      <c r="D169" s="70"/>
+      <c r="D169" s="66"/>
       <c r="E169" s="66"/>
       <c r="F169" s="42"/>
       <c r="G169" s="43"/>
@@ -17193,7 +17241,7 @@
     <row r="170" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="23"/>
       <c r="B170" s="65"/>
-      <c r="D170" s="70"/>
+      <c r="D170" s="66"/>
       <c r="E170" s="66"/>
       <c r="F170" s="42"/>
       <c r="G170" s="43"/>
@@ -17261,7 +17309,7 @@
     <row r="171" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="23"/>
       <c r="B171" s="65"/>
-      <c r="D171" s="70"/>
+      <c r="D171" s="66"/>
       <c r="E171" s="66"/>
       <c r="F171" s="42"/>
       <c r="G171" s="43"/>
@@ -17465,7 +17513,7 @@
     <row r="174" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="23"/>
       <c r="B174" s="65"/>
-      <c r="D174" s="66"/>
+      <c r="D174" s="70"/>
       <c r="E174" s="66"/>
       <c r="F174" s="42"/>
       <c r="G174" s="43"/>
@@ -17533,7 +17581,7 @@
     <row r="175" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="23"/>
       <c r="B175" s="65"/>
-      <c r="D175" s="66"/>
+      <c r="D175" s="70"/>
       <c r="E175" s="66"/>
       <c r="F175" s="42"/>
       <c r="G175" s="43"/>
@@ -17601,7 +17649,7 @@
     <row r="176" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="23"/>
       <c r="B176" s="65"/>
-      <c r="D176" s="66"/>
+      <c r="D176" s="70"/>
       <c r="E176" s="66"/>
       <c r="F176" s="42"/>
       <c r="G176" s="43"/>
@@ -17737,7 +17785,7 @@
     <row r="178" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="23"/>
       <c r="B178" s="65"/>
-      <c r="D178" s="70"/>
+      <c r="D178" s="66"/>
       <c r="E178" s="66"/>
       <c r="F178" s="42"/>
       <c r="G178" s="43"/>
@@ -17805,7 +17853,7 @@
     <row r="179" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="23"/>
       <c r="B179" s="65"/>
-      <c r="D179" s="70"/>
+      <c r="D179" s="66"/>
       <c r="E179" s="66"/>
       <c r="F179" s="42"/>
       <c r="G179" s="43"/>
@@ -17873,7 +17921,7 @@
     <row r="180" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="23"/>
       <c r="B180" s="65"/>
-      <c r="D180" s="70"/>
+      <c r="D180" s="66"/>
       <c r="E180" s="66"/>
       <c r="F180" s="42"/>
       <c r="G180" s="43"/>
@@ -18074,18 +18122,213 @@
       <c r="BN182" s="46"/>
       <c r="BO182" s="46"/>
     </row>
+    <row r="183" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="23"/>
+      <c r="B183" s="65"/>
+      <c r="D183" s="70"/>
+      <c r="E183" s="66"/>
+      <c r="F183" s="42"/>
+      <c r="G183" s="43"/>
+      <c r="H183" s="25"/>
+      <c r="I183" s="26"/>
+      <c r="J183" s="27"/>
+      <c r="K183" s="40"/>
+      <c r="L183" s="46"/>
+      <c r="M183" s="46"/>
+      <c r="N183" s="46"/>
+      <c r="O183" s="46"/>
+      <c r="P183" s="46"/>
+      <c r="Q183" s="46"/>
+      <c r="R183" s="46"/>
+      <c r="S183" s="46"/>
+      <c r="T183" s="46"/>
+      <c r="U183" s="46"/>
+      <c r="V183" s="46"/>
+      <c r="W183" s="46"/>
+      <c r="X183" s="46"/>
+      <c r="Y183" s="46"/>
+      <c r="Z183" s="46"/>
+      <c r="AA183" s="46"/>
+      <c r="AB183" s="46"/>
+      <c r="AC183" s="46"/>
+      <c r="AD183" s="46"/>
+      <c r="AE183" s="46"/>
+      <c r="AF183" s="46"/>
+      <c r="AG183" s="46"/>
+      <c r="AH183" s="46"/>
+      <c r="AI183" s="46"/>
+      <c r="AJ183" s="46"/>
+      <c r="AK183" s="46"/>
+      <c r="AL183" s="46"/>
+      <c r="AM183" s="46"/>
+      <c r="AN183" s="46"/>
+      <c r="AO183" s="46"/>
+      <c r="AP183" s="46"/>
+      <c r="AQ183" s="46"/>
+      <c r="AR183" s="46"/>
+      <c r="AS183" s="46"/>
+      <c r="AT183" s="46"/>
+      <c r="AU183" s="46"/>
+      <c r="AV183" s="46"/>
+      <c r="AW183" s="46"/>
+      <c r="AX183" s="46"/>
+      <c r="AY183" s="46"/>
+      <c r="AZ183" s="46"/>
+      <c r="BA183" s="46"/>
+      <c r="BB183" s="46"/>
+      <c r="BC183" s="46"/>
+      <c r="BD183" s="46"/>
+      <c r="BE183" s="46"/>
+      <c r="BF183" s="46"/>
+      <c r="BG183" s="46"/>
+      <c r="BH183" s="46"/>
+      <c r="BI183" s="46"/>
+      <c r="BJ183" s="46"/>
+      <c r="BK183" s="46"/>
+      <c r="BL183" s="46"/>
+      <c r="BM183" s="46"/>
+      <c r="BN183" s="46"/>
+      <c r="BO183" s="46"/>
+    </row>
+    <row r="184" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="23"/>
+      <c r="B184" s="65"/>
+      <c r="D184" s="70"/>
+      <c r="E184" s="66"/>
+      <c r="F184" s="42"/>
+      <c r="G184" s="43"/>
+      <c r="H184" s="25"/>
+      <c r="I184" s="26"/>
+      <c r="J184" s="27"/>
+      <c r="K184" s="40"/>
+      <c r="L184" s="46"/>
+      <c r="M184" s="46"/>
+      <c r="N184" s="46"/>
+      <c r="O184" s="46"/>
+      <c r="P184" s="46"/>
+      <c r="Q184" s="46"/>
+      <c r="R184" s="46"/>
+      <c r="S184" s="46"/>
+      <c r="T184" s="46"/>
+      <c r="U184" s="46"/>
+      <c r="V184" s="46"/>
+      <c r="W184" s="46"/>
+      <c r="X184" s="46"/>
+      <c r="Y184" s="46"/>
+      <c r="Z184" s="46"/>
+      <c r="AA184" s="46"/>
+      <c r="AB184" s="46"/>
+      <c r="AC184" s="46"/>
+      <c r="AD184" s="46"/>
+      <c r="AE184" s="46"/>
+      <c r="AF184" s="46"/>
+      <c r="AG184" s="46"/>
+      <c r="AH184" s="46"/>
+      <c r="AI184" s="46"/>
+      <c r="AJ184" s="46"/>
+      <c r="AK184" s="46"/>
+      <c r="AL184" s="46"/>
+      <c r="AM184" s="46"/>
+      <c r="AN184" s="46"/>
+      <c r="AO184" s="46"/>
+      <c r="AP184" s="46"/>
+      <c r="AQ184" s="46"/>
+      <c r="AR184" s="46"/>
+      <c r="AS184" s="46"/>
+      <c r="AT184" s="46"/>
+      <c r="AU184" s="46"/>
+      <c r="AV184" s="46"/>
+      <c r="AW184" s="46"/>
+      <c r="AX184" s="46"/>
+      <c r="AY184" s="46"/>
+      <c r="AZ184" s="46"/>
+      <c r="BA184" s="46"/>
+      <c r="BB184" s="46"/>
+      <c r="BC184" s="46"/>
+      <c r="BD184" s="46"/>
+      <c r="BE184" s="46"/>
+      <c r="BF184" s="46"/>
+      <c r="BG184" s="46"/>
+      <c r="BH184" s="46"/>
+      <c r="BI184" s="46"/>
+      <c r="BJ184" s="46"/>
+      <c r="BK184" s="46"/>
+      <c r="BL184" s="46"/>
+      <c r="BM184" s="46"/>
+      <c r="BN184" s="46"/>
+      <c r="BO184" s="46"/>
+    </row>
+    <row r="185" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="23"/>
+      <c r="B185" s="65"/>
+      <c r="D185" s="70"/>
+      <c r="E185" s="66"/>
+      <c r="F185" s="42"/>
+      <c r="G185" s="43"/>
+      <c r="H185" s="25"/>
+      <c r="I185" s="26"/>
+      <c r="J185" s="27"/>
+      <c r="K185" s="40"/>
+      <c r="L185" s="46"/>
+      <c r="M185" s="46"/>
+      <c r="N185" s="46"/>
+      <c r="O185" s="46"/>
+      <c r="P185" s="46"/>
+      <c r="Q185" s="46"/>
+      <c r="R185" s="46"/>
+      <c r="S185" s="46"/>
+      <c r="T185" s="46"/>
+      <c r="U185" s="46"/>
+      <c r="V185" s="46"/>
+      <c r="W185" s="46"/>
+      <c r="X185" s="46"/>
+      <c r="Y185" s="46"/>
+      <c r="Z185" s="46"/>
+      <c r="AA185" s="46"/>
+      <c r="AB185" s="46"/>
+      <c r="AC185" s="46"/>
+      <c r="AD185" s="46"/>
+      <c r="AE185" s="46"/>
+      <c r="AF185" s="46"/>
+      <c r="AG185" s="46"/>
+      <c r="AH185" s="46"/>
+      <c r="AI185" s="46"/>
+      <c r="AJ185" s="46"/>
+      <c r="AK185" s="46"/>
+      <c r="AL185" s="46"/>
+      <c r="AM185" s="46"/>
+      <c r="AN185" s="46"/>
+      <c r="AO185" s="46"/>
+      <c r="AP185" s="46"/>
+      <c r="AQ185" s="46"/>
+      <c r="AR185" s="46"/>
+      <c r="AS185" s="46"/>
+      <c r="AT185" s="46"/>
+      <c r="AU185" s="46"/>
+      <c r="AV185" s="46"/>
+      <c r="AW185" s="46"/>
+      <c r="AX185" s="46"/>
+      <c r="AY185" s="46"/>
+      <c r="AZ185" s="46"/>
+      <c r="BA185" s="46"/>
+      <c r="BB185" s="46"/>
+      <c r="BC185" s="46"/>
+      <c r="BD185" s="46"/>
+      <c r="BE185" s="46"/>
+      <c r="BF185" s="46"/>
+      <c r="BG185" s="46"/>
+      <c r="BH185" s="46"/>
+      <c r="BI185" s="46"/>
+      <c r="BJ185" s="46"/>
+      <c r="BK185" s="46"/>
+      <c r="BL185" s="46"/>
+      <c r="BM185" s="46"/>
+      <c r="BN185" s="46"/>
+      <c r="BO185" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -18096,9 +18339,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I143:I146 I98:I103 I105:I110 I112:I122 I124:I141">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I146:I149 I98:I103 I105:I110 I112:I122 I124:I144">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18117,7 +18369,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN141 L147:BO149 M150:BN155 BO153:BO155 L156:BO158 M159:BN164 BO162:BO164 L165:BO167 M168:BN173 BO171:BO173 L174:BO176 M177:BN182 BO180:BO182 BO145:BO146 M143:BN146 L142:BO142 L123:BO123">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN144 L150:BO152 M153:BN158 BO156:BO158 L159:BO161 M162:BN167 BO165:BO167 L168:BO170 M171:BN176 BO174:BO176 L177:BO179 M180:BN185 BO183:BO185 BO148:BO149 M146:BN149 L145:BO145 L123:BO123">
     <cfRule type="expression" dxfId="132" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -18125,7 +18377,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L143:BO146 L98:BO103 L105:BO110 L112:BO122 L124:BO141">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L146:BO149 L98:BO103 L105:BO110 L112:BO122 L124:BO144">
     <cfRule type="expression" dxfId="130" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -18135,7 +18387,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E183:E1048576 E95:E96 E143:E146 E98:E103 E105:E110 E112:E122 E124:E141">
+  <conditionalFormatting sqref="E1:E73 E186:E1048576 E95:E96 E146:E149 E98:E103 E105:E110 E112:E122 E124:E144">
     <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18229,7 +18481,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I147:I155">
+  <conditionalFormatting sqref="I150:I158">
     <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18243,12 +18495,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L147:BO155">
+  <conditionalFormatting sqref="L150:BO158">
     <cfRule type="expression" dxfId="106" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E147:E155">
+  <conditionalFormatting sqref="E150:E158">
     <cfRule type="cellIs" dxfId="105" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18271,7 +18523,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L150:BO155 L143:BO146 L98:BO103 L105:BO110 L112:BO122 L124:BO141">
+  <conditionalFormatting sqref="L153:BO158 L146:BO149 L98:BO103 L105:BO110 L112:BO122 L124:BO144">
     <cfRule type="expression" dxfId="98" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18279,7 +18531,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I156:I164">
+  <conditionalFormatting sqref="I159:I167">
     <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18293,12 +18545,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L156:BO164">
+  <conditionalFormatting sqref="L159:BO167">
     <cfRule type="expression" dxfId="96" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E156:E164">
+  <conditionalFormatting sqref="E159:E167">
     <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18321,7 +18573,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L159:BO164">
+  <conditionalFormatting sqref="L162:BO167">
     <cfRule type="expression" dxfId="88" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18329,7 +18581,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I165:I173">
+  <conditionalFormatting sqref="I168:I176">
     <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18343,12 +18595,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L165:BO173">
+  <conditionalFormatting sqref="L168:BO176">
     <cfRule type="expression" dxfId="86" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E165:E173">
+  <conditionalFormatting sqref="E168:E176">
     <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18371,7 +18623,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L168:BO173">
+  <conditionalFormatting sqref="L171:BO176">
     <cfRule type="expression" dxfId="78" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18379,7 +18631,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I174:I182">
+  <conditionalFormatting sqref="I177:I185">
     <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18393,12 +18645,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L174:BO182">
+  <conditionalFormatting sqref="L177:BO185">
     <cfRule type="expression" dxfId="76" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E174:E182">
+  <conditionalFormatting sqref="E177:E185">
     <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18421,7 +18673,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L177:BO182">
+  <conditionalFormatting sqref="L180:BO185">
     <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18571,7 +18823,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I142">
+  <conditionalFormatting sqref="I145">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18585,12 +18837,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L142:BO142">
+  <conditionalFormatting sqref="L145:BO145">
     <cfRule type="expression" dxfId="38" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E142">
+  <conditionalFormatting sqref="E145">
     <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18811,7 +19063,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I143:I146 I98:I103 I105:I110 I112:I122 I124:I141</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I146:I149 I98:I103 I105:I110 I112:I122 I124:I144</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -18841,7 +19093,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I147:I155</xm:sqref>
+          <xm:sqref>I150:I158</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -18856,7 +19108,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I156:I164</xm:sqref>
+          <xm:sqref>I159:I167</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -18871,7 +19123,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I165:I173</xm:sqref>
+          <xm:sqref>I168:I176</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -18886,7 +19138,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I174:I182</xm:sqref>
+          <xm:sqref>I177:I185</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -18946,7 +19198,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I142</xm:sqref>
+          <xm:sqref>I145</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Added pulling of vintage dates from new ext_tsvalues table (v0.17)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB4B56-8918-44B2-B220-57D20D87EC3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105D2D4-ABF8-4966-8076-5EBA6CEC8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="173">
   <si>
     <t>WBS</t>
   </si>
@@ -938,6 +938,15 @@
   </si>
   <si>
     <t>Website Color &amp; Redesign</t>
+  </si>
+  <si>
+    <t>Bash</t>
+  </si>
+  <si>
+    <t>Move Task Scheduler to Cron Job on Prod VPS</t>
+  </si>
+  <si>
+    <t>R to Enter Data On Vintage Change</t>
   </si>
 </sst>
 </file>
@@ -1866,13 +1875,6 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1882,10 +1884,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1894,6 +1892,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3454,11 +3463,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO185"/>
+  <dimension ref="A1:BO187"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M140" sqref="M140"/>
+      <pane ySplit="7" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3488,27 +3497,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="78"/>
-      <c r="M1" s="78"/>
-      <c r="N1" s="78"/>
-      <c r="O1" s="78"/>
-      <c r="P1" s="78"/>
-      <c r="Q1" s="78"/>
-      <c r="R1" s="78"/>
-      <c r="S1" s="78"/>
-      <c r="T1" s="78"/>
-      <c r="U1" s="78"/>
-      <c r="V1" s="78"/>
-      <c r="W1" s="78"/>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="78"/>
-      <c r="AC1" s="78"/>
-      <c r="AD1" s="78"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="78"/>
+      <c r="L1" s="84"/>
+      <c r="M1" s="84"/>
+      <c r="N1" s="84"/>
+      <c r="O1" s="84"/>
+      <c r="P1" s="84"/>
+      <c r="Q1" s="84"/>
+      <c r="R1" s="84"/>
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="84"/>
+      <c r="AA1" s="84"/>
+      <c r="AB1" s="84"/>
+      <c r="AC1" s="84"/>
+      <c r="AD1" s="84"/>
+      <c r="AE1" s="84"/>
+      <c r="AF1" s="84"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3553,12 +3562,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="83">
+      <c r="C4" s="86">
         <v>44192</v>
       </c>
-      <c r="D4" s="83"/>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3568,183 +3577,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="80" t="str">
+      <c r="L4" s="78" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 43</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81"/>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="82"/>
-      <c r="S4" s="80" t="str">
+      <c r="M4" s="79"/>
+      <c r="N4" s="79"/>
+      <c r="O4" s="79"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="79"/>
+      <c r="R4" s="80"/>
+      <c r="S4" s="78" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 44</v>
       </c>
-      <c r="T4" s="81"/>
-      <c r="U4" s="81"/>
-      <c r="V4" s="81"/>
-      <c r="W4" s="81"/>
-      <c r="X4" s="81"/>
-      <c r="Y4" s="82"/>
-      <c r="Z4" s="80" t="str">
+      <c r="T4" s="79"/>
+      <c r="U4" s="79"/>
+      <c r="V4" s="79"/>
+      <c r="W4" s="79"/>
+      <c r="X4" s="79"/>
+      <c r="Y4" s="80"/>
+      <c r="Z4" s="78" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 45</v>
       </c>
-      <c r="AA4" s="81"/>
-      <c r="AB4" s="81"/>
-      <c r="AC4" s="81"/>
-      <c r="AD4" s="81"/>
-      <c r="AE4" s="81"/>
-      <c r="AF4" s="82"/>
-      <c r="AG4" s="80" t="str">
+      <c r="AA4" s="79"/>
+      <c r="AB4" s="79"/>
+      <c r="AC4" s="79"/>
+      <c r="AD4" s="79"/>
+      <c r="AE4" s="79"/>
+      <c r="AF4" s="80"/>
+      <c r="AG4" s="78" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 46</v>
       </c>
-      <c r="AH4" s="81"/>
-      <c r="AI4" s="81"/>
-      <c r="AJ4" s="81"/>
-      <c r="AK4" s="81"/>
-      <c r="AL4" s="81"/>
-      <c r="AM4" s="82"/>
-      <c r="AN4" s="80" t="str">
+      <c r="AH4" s="79"/>
+      <c r="AI4" s="79"/>
+      <c r="AJ4" s="79"/>
+      <c r="AK4" s="79"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="80"/>
+      <c r="AN4" s="78" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 47</v>
       </c>
-      <c r="AO4" s="81"/>
-      <c r="AP4" s="81"/>
-      <c r="AQ4" s="81"/>
-      <c r="AR4" s="81"/>
-      <c r="AS4" s="81"/>
-      <c r="AT4" s="82"/>
-      <c r="AU4" s="80" t="str">
+      <c r="AO4" s="79"/>
+      <c r="AP4" s="79"/>
+      <c r="AQ4" s="79"/>
+      <c r="AR4" s="79"/>
+      <c r="AS4" s="79"/>
+      <c r="AT4" s="80"/>
+      <c r="AU4" s="78" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 48</v>
       </c>
-      <c r="AV4" s="81"/>
-      <c r="AW4" s="81"/>
-      <c r="AX4" s="81"/>
-      <c r="AY4" s="81"/>
-      <c r="AZ4" s="81"/>
-      <c r="BA4" s="82"/>
-      <c r="BB4" s="80" t="str">
+      <c r="AV4" s="79"/>
+      <c r="AW4" s="79"/>
+      <c r="AX4" s="79"/>
+      <c r="AY4" s="79"/>
+      <c r="AZ4" s="79"/>
+      <c r="BA4" s="80"/>
+      <c r="BB4" s="78" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 49</v>
       </c>
-      <c r="BC4" s="81"/>
-      <c r="BD4" s="81"/>
-      <c r="BE4" s="81"/>
-      <c r="BF4" s="81"/>
-      <c r="BG4" s="81"/>
-      <c r="BH4" s="82"/>
-      <c r="BI4" s="80" t="str">
+      <c r="BC4" s="79"/>
+      <c r="BD4" s="79"/>
+      <c r="BE4" s="79"/>
+      <c r="BF4" s="79"/>
+      <c r="BG4" s="79"/>
+      <c r="BH4" s="80"/>
+      <c r="BI4" s="78" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 50</v>
       </c>
-      <c r="BJ4" s="81"/>
-      <c r="BK4" s="81"/>
-      <c r="BL4" s="81"/>
-      <c r="BM4" s="81"/>
-      <c r="BN4" s="81"/>
-      <c r="BO4" s="82"/>
+      <c r="BJ4" s="79"/>
+      <c r="BK4" s="79"/>
+      <c r="BL4" s="79"/>
+      <c r="BM4" s="79"/>
+      <c r="BN4" s="79"/>
+      <c r="BO4" s="80"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="85" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="84">
+      <c r="L5" s="81">
         <f>L6</f>
         <v>44487</v>
       </c>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="86"/>
-      <c r="S5" s="84">
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="83"/>
+      <c r="S5" s="81">
         <f>S6</f>
         <v>44494</v>
       </c>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="86"/>
-      <c r="Z5" s="84">
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="82"/>
+      <c r="X5" s="82"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="81">
         <f>Z6</f>
         <v>44501</v>
       </c>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85"/>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="86"/>
-      <c r="AG5" s="84">
+      <c r="AA5" s="82"/>
+      <c r="AB5" s="82"/>
+      <c r="AC5" s="82"/>
+      <c r="AD5" s="82"/>
+      <c r="AE5" s="82"/>
+      <c r="AF5" s="83"/>
+      <c r="AG5" s="81">
         <f>AG6</f>
         <v>44508</v>
       </c>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="85"/>
-      <c r="AJ5" s="85"/>
-      <c r="AK5" s="85"/>
-      <c r="AL5" s="85"/>
-      <c r="AM5" s="86"/>
-      <c r="AN5" s="84">
+      <c r="AH5" s="82"/>
+      <c r="AI5" s="82"/>
+      <c r="AJ5" s="82"/>
+      <c r="AK5" s="82"/>
+      <c r="AL5" s="82"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="81">
         <f>AN6</f>
         <v>44515</v>
       </c>
-      <c r="AO5" s="85"/>
-      <c r="AP5" s="85"/>
-      <c r="AQ5" s="85"/>
-      <c r="AR5" s="85"/>
-      <c r="AS5" s="85"/>
-      <c r="AT5" s="86"/>
-      <c r="AU5" s="84">
+      <c r="AO5" s="82"/>
+      <c r="AP5" s="82"/>
+      <c r="AQ5" s="82"/>
+      <c r="AR5" s="82"/>
+      <c r="AS5" s="82"/>
+      <c r="AT5" s="83"/>
+      <c r="AU5" s="81">
         <f>AU6</f>
         <v>44522</v>
       </c>
-      <c r="AV5" s="85"/>
-      <c r="AW5" s="85"/>
-      <c r="AX5" s="85"/>
-      <c r="AY5" s="85"/>
-      <c r="AZ5" s="85"/>
-      <c r="BA5" s="86"/>
-      <c r="BB5" s="84">
+      <c r="AV5" s="82"/>
+      <c r="AW5" s="82"/>
+      <c r="AX5" s="82"/>
+      <c r="AY5" s="82"/>
+      <c r="AZ5" s="82"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="81">
         <f>BB6</f>
         <v>44529</v>
       </c>
-      <c r="BC5" s="85"/>
-      <c r="BD5" s="85"/>
-      <c r="BE5" s="85"/>
-      <c r="BF5" s="85"/>
-      <c r="BG5" s="85"/>
-      <c r="BH5" s="86"/>
-      <c r="BI5" s="84">
+      <c r="BC5" s="82"/>
+      <c r="BD5" s="82"/>
+      <c r="BE5" s="82"/>
+      <c r="BF5" s="82"/>
+      <c r="BG5" s="82"/>
+      <c r="BH5" s="83"/>
+      <c r="BI5" s="81">
         <f>BI6</f>
         <v>44536</v>
       </c>
-      <c r="BJ5" s="85"/>
-      <c r="BK5" s="85"/>
-      <c r="BL5" s="85"/>
-      <c r="BM5" s="85"/>
-      <c r="BN5" s="85"/>
-      <c r="BO5" s="86"/>
+      <c r="BJ5" s="82"/>
+      <c r="BK5" s="82"/>
+      <c r="BL5" s="82"/>
+      <c r="BM5" s="82"/>
+      <c r="BN5" s="82"/>
+      <c r="BO5" s="83"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8902,7 +8911,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A150" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A152" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -14354,21 +14363,21 @@
         <v>12.8</v>
       </c>
       <c r="B131" s="65" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D131" s="70"/>
       <c r="E131" s="66" t="s">
-        <v>68</v>
+        <v>170</v>
       </c>
       <c r="F131" s="42">
         <v>44489</v>
       </c>
       <c r="G131" s="43">
-        <v>44492</v>
+        <v>44490</v>
       </c>
       <c r="H131" s="73"/>
       <c r="I131" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J131" s="75"/>
       <c r="K131" s="76"/>
@@ -14435,17 +14444,17 @@
         <v>12.9</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="D132" s="70"/>
       <c r="E132" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F132" s="42">
-        <v>44489</v>
+        <v>44490</v>
       </c>
       <c r="G132" s="43">
-        <v>44492</v>
+        <v>44491</v>
       </c>
       <c r="H132" s="73"/>
       <c r="I132" s="26">
@@ -14516,17 +14525,17 @@
         <v>12.10</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F133" s="42">
+        <v>44490</v>
+      </c>
+      <c r="G133" s="43">
         <v>44492</v>
-      </c>
-      <c r="G133" s="43">
-        <v>44493</v>
       </c>
       <c r="H133" s="73"/>
       <c r="I133" s="26">
@@ -14597,17 +14606,17 @@
         <v>12.11</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F134" s="42">
-        <v>44494</v>
+        <v>44491</v>
       </c>
       <c r="G134" s="43">
-        <v>44499</v>
+        <v>44493</v>
       </c>
       <c r="H134" s="73"/>
       <c r="I134" s="26">
@@ -14678,14 +14687,14 @@
         <v>12.12</v>
       </c>
       <c r="B135" s="65" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F135" s="42">
-        <v>44494</v>
+        <v>44493</v>
       </c>
       <c r="G135" s="43">
         <v>44499</v>
@@ -14759,7 +14768,7 @@
         <v>12.13</v>
       </c>
       <c r="B136" s="65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D136" s="70"/>
       <c r="E136" s="66" t="s">
@@ -14840,7 +14849,7 @@
         <v>12.14</v>
       </c>
       <c r="B137" s="65" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D137" s="70"/>
       <c r="E137" s="66" t="s">
@@ -14921,17 +14930,17 @@
         <v>12.15</v>
       </c>
       <c r="B138" s="65" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="D138" s="70"/>
       <c r="E138" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F138" s="42">
         <v>44494</v>
       </c>
       <c r="G138" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H138" s="73"/>
       <c r="I138" s="26">
@@ -15002,21 +15011,21 @@
         <v>12.16</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D139" s="70"/>
       <c r="E139" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F139" s="42">
         <v>44494</v>
       </c>
       <c r="G139" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H139" s="73"/>
       <c r="I139" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="J139" s="75"/>
       <c r="K139" s="76"/>
@@ -15083,11 +15092,11 @@
         <v>12.17</v>
       </c>
       <c r="B140" s="65" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="D140" s="70"/>
       <c r="E140" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F140" s="42">
         <v>44494</v>
@@ -15164,7 +15173,7 @@
         <v>12.18</v>
       </c>
       <c r="B141" s="65" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D141" s="70"/>
       <c r="E141" s="66" t="s">
@@ -15174,11 +15183,11 @@
         <v>44494</v>
       </c>
       <c r="G141" s="43">
-        <v>44510</v>
+        <v>44501</v>
       </c>
       <c r="H141" s="73"/>
       <c r="I141" s="26">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="J141" s="75"/>
       <c r="K141" s="76"/>
@@ -15245,20 +15254,20 @@
         <v>12.19</v>
       </c>
       <c r="B142" s="65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D142" s="70"/>
-      <c r="E142" s="70" t="s">
+      <c r="E142" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F142" s="71">
+      <c r="F142" s="42">
         <v>44494</v>
       </c>
-      <c r="G142" s="72">
-        <v>44510</v>
+      <c r="G142" s="43">
+        <v>44501</v>
       </c>
       <c r="H142" s="73"/>
-      <c r="I142" s="74">
+      <c r="I142" s="26">
         <v>0</v>
       </c>
       <c r="J142" s="75"/>
@@ -15326,20 +15335,20 @@
         <v>12.20</v>
       </c>
       <c r="B143" s="65" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D143" s="70"/>
-      <c r="E143" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F143" s="71">
+      <c r="E143" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F143" s="42">
         <v>44494</v>
       </c>
-      <c r="G143" s="72">
+      <c r="G143" s="43">
         <v>44510</v>
       </c>
       <c r="H143" s="73"/>
-      <c r="I143" s="74">
+      <c r="I143" s="26">
         <v>0</v>
       </c>
       <c r="J143" s="75"/>
@@ -15407,17 +15416,17 @@
         <v>12.21</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D144" s="70"/>
       <c r="E144" s="70" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F144" s="71">
         <v>44494</v>
       </c>
       <c r="G144" s="72">
-        <v>44520</v>
+        <v>44510</v>
       </c>
       <c r="H144" s="73"/>
       <c r="I144" s="74">
@@ -15482,105 +15491,111 @@
       <c r="BN144" s="46"/>
       <c r="BO144" s="46"/>
     </row>
-    <row r="145" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>13</v>
-      </c>
-      <c r="B145" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D145" s="19"/>
-      <c r="E145" s="19"/>
-      <c r="F145" s="44"/>
-      <c r="G145" s="44" t="str">
-        <f t="shared" ref="G145" si="24">IF(ISBLANK(F145)," - ",IF(H145=0,F145,F145+H145-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H145" s="20"/>
-      <c r="I145" s="21"/>
-      <c r="J145" s="22" t="str">
-        <f t="shared" ref="J145" si="25">IF(OR(G145=0,F145=0)," - ",NETWORKDAYS(F145,G145))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K145" s="41"/>
-      <c r="L145" s="48"/>
-      <c r="M145" s="48"/>
-      <c r="N145" s="48"/>
-      <c r="O145" s="48"/>
-      <c r="P145" s="48"/>
-      <c r="Q145" s="48"/>
-      <c r="R145" s="48"/>
-      <c r="S145" s="48"/>
-      <c r="T145" s="48"/>
-      <c r="U145" s="48"/>
-      <c r="V145" s="48"/>
-      <c r="W145" s="48"/>
-      <c r="X145" s="48"/>
-      <c r="Y145" s="48"/>
-      <c r="Z145" s="48"/>
-      <c r="AA145" s="48"/>
-      <c r="AB145" s="48"/>
-      <c r="AC145" s="48"/>
-      <c r="AD145" s="48"/>
-      <c r="AE145" s="48"/>
-      <c r="AF145" s="48"/>
-      <c r="AG145" s="48"/>
-      <c r="AH145" s="48"/>
-      <c r="AI145" s="48"/>
-      <c r="AJ145" s="48"/>
-      <c r="AK145" s="48"/>
-      <c r="AL145" s="48"/>
-      <c r="AM145" s="48"/>
-      <c r="AN145" s="48"/>
-      <c r="AO145" s="48"/>
-      <c r="AP145" s="48"/>
-      <c r="AQ145" s="48"/>
-      <c r="AR145" s="48"/>
-      <c r="AS145" s="48"/>
-      <c r="AT145" s="48"/>
-      <c r="AU145" s="48"/>
-      <c r="AV145" s="48"/>
-      <c r="AW145" s="48"/>
-      <c r="AX145" s="48"/>
-      <c r="AY145" s="48"/>
-      <c r="AZ145" s="48"/>
-      <c r="BA145" s="48"/>
-      <c r="BB145" s="48"/>
-      <c r="BC145" s="48"/>
-      <c r="BD145" s="48"/>
-      <c r="BE145" s="48"/>
-      <c r="BF145" s="48"/>
-      <c r="BG145" s="48"/>
-      <c r="BH145" s="48"/>
-      <c r="BI145" s="48"/>
-      <c r="BJ145" s="48"/>
-      <c r="BK145" s="48"/>
-      <c r="BL145" s="48"/>
-      <c r="BM145" s="48"/>
-      <c r="BN145" s="48"/>
-      <c r="BO145" s="48"/>
+    <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.22</v>
+      </c>
+      <c r="B145" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="D145" s="70"/>
+      <c r="E145" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F145" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G145" s="72">
+        <v>44510</v>
+      </c>
+      <c r="H145" s="73"/>
+      <c r="I145" s="74">
+        <v>0</v>
+      </c>
+      <c r="J145" s="75"/>
+      <c r="K145" s="76"/>
+      <c r="L145" s="46"/>
+      <c r="M145" s="46"/>
+      <c r="N145" s="46"/>
+      <c r="O145" s="46"/>
+      <c r="P145" s="46"/>
+      <c r="Q145" s="46"/>
+      <c r="R145" s="46"/>
+      <c r="S145" s="46"/>
+      <c r="T145" s="46"/>
+      <c r="U145" s="46"/>
+      <c r="V145" s="46"/>
+      <c r="W145" s="46"/>
+      <c r="X145" s="46"/>
+      <c r="Y145" s="46"/>
+      <c r="Z145" s="46"/>
+      <c r="AA145" s="46"/>
+      <c r="AB145" s="46"/>
+      <c r="AC145" s="46"/>
+      <c r="AD145" s="46"/>
+      <c r="AE145" s="46"/>
+      <c r="AF145" s="46"/>
+      <c r="AG145" s="46"/>
+      <c r="AH145" s="46"/>
+      <c r="AI145" s="46"/>
+      <c r="AJ145" s="46"/>
+      <c r="AK145" s="46"/>
+      <c r="AL145" s="46"/>
+      <c r="AM145" s="46"/>
+      <c r="AN145" s="46"/>
+      <c r="AO145" s="46"/>
+      <c r="AP145" s="46"/>
+      <c r="AQ145" s="46"/>
+      <c r="AR145" s="46"/>
+      <c r="AS145" s="46"/>
+      <c r="AT145" s="46"/>
+      <c r="AU145" s="46"/>
+      <c r="AV145" s="46"/>
+      <c r="AW145" s="46"/>
+      <c r="AX145" s="46"/>
+      <c r="AY145" s="46"/>
+      <c r="AZ145" s="46"/>
+      <c r="BA145" s="46"/>
+      <c r="BB145" s="46"/>
+      <c r="BC145" s="46"/>
+      <c r="BD145" s="46"/>
+      <c r="BE145" s="46"/>
+      <c r="BF145" s="46"/>
+      <c r="BG145" s="46"/>
+      <c r="BH145" s="46"/>
+      <c r="BI145" s="46"/>
+      <c r="BJ145" s="46"/>
+      <c r="BK145" s="46"/>
+      <c r="BL145" s="46"/>
+      <c r="BM145" s="46"/>
+      <c r="BN145" s="46"/>
+      <c r="BO145" s="46"/>
     </row>
     <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.1</v>
+        <v>12.23</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="D146" s="70"/>
-      <c r="E146" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F146" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G146" s="43"/>
-      <c r="H146" s="25"/>
-      <c r="I146" s="26"/>
-      <c r="J146" s="27"/>
-      <c r="K146" s="40"/>
+      <c r="E146" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F146" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G146" s="72">
+        <v>44520</v>
+      </c>
+      <c r="H146" s="73"/>
+      <c r="I146" s="74">
+        <v>0</v>
+      </c>
+      <c r="J146" s="75"/>
+      <c r="K146" s="76"/>
       <c r="L146" s="46"/>
       <c r="M146" s="46"/>
       <c r="N146" s="46"/>
@@ -15638,94 +15653,96 @@
       <c r="BN146" s="46"/>
       <c r="BO146" s="46"/>
     </row>
-    <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.2</v>
-      </c>
-      <c r="B147" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D147" s="70"/>
-      <c r="E147" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F147" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G147" s="43"/>
-      <c r="H147" s="25"/>
-      <c r="I147" s="26"/>
-      <c r="J147" s="27"/>
-      <c r="K147" s="40"/>
-      <c r="L147" s="46"/>
-      <c r="M147" s="46"/>
-      <c r="N147" s="46"/>
-      <c r="O147" s="46"/>
-      <c r="P147" s="46"/>
-      <c r="Q147" s="46"/>
-      <c r="R147" s="46"/>
-      <c r="S147" s="46"/>
-      <c r="T147" s="46"/>
-      <c r="U147" s="46"/>
-      <c r="V147" s="46"/>
-      <c r="W147" s="46"/>
-      <c r="X147" s="46"/>
-      <c r="Y147" s="46"/>
-      <c r="Z147" s="46"/>
-      <c r="AA147" s="46"/>
-      <c r="AB147" s="46"/>
-      <c r="AC147" s="46"/>
-      <c r="AD147" s="46"/>
-      <c r="AE147" s="46"/>
-      <c r="AF147" s="46"/>
-      <c r="AG147" s="46"/>
-      <c r="AH147" s="46"/>
-      <c r="AI147" s="46"/>
-      <c r="AJ147" s="46"/>
-      <c r="AK147" s="46"/>
-      <c r="AL147" s="46"/>
-      <c r="AM147" s="46"/>
-      <c r="AN147" s="46"/>
-      <c r="AO147" s="46"/>
-      <c r="AP147" s="46"/>
-      <c r="AQ147" s="46"/>
-      <c r="AR147" s="46"/>
-      <c r="AS147" s="46"/>
-      <c r="AT147" s="46"/>
-      <c r="AU147" s="46"/>
-      <c r="AV147" s="46"/>
-      <c r="AW147" s="46"/>
-      <c r="AX147" s="46"/>
-      <c r="AY147" s="46"/>
-      <c r="AZ147" s="46"/>
-      <c r="BA147" s="46"/>
-      <c r="BB147" s="46"/>
-      <c r="BC147" s="46"/>
-      <c r="BD147" s="46"/>
-      <c r="BE147" s="46"/>
-      <c r="BF147" s="46"/>
-      <c r="BG147" s="46"/>
-      <c r="BH147" s="46"/>
-      <c r="BI147" s="46"/>
-      <c r="BJ147" s="46"/>
-      <c r="BK147" s="46"/>
-      <c r="BL147" s="46"/>
-      <c r="BM147" s="46"/>
-      <c r="BN147" s="46"/>
-      <c r="BO147" s="46"/>
+    <row r="147" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>13</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D147" s="19"/>
+      <c r="E147" s="19"/>
+      <c r="F147" s="44"/>
+      <c r="G147" s="44" t="str">
+        <f t="shared" ref="G147" si="24">IF(ISBLANK(F147)," - ",IF(H147=0,F147,F147+H147-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H147" s="20"/>
+      <c r="I147" s="21"/>
+      <c r="J147" s="22" t="str">
+        <f t="shared" ref="J147" si="25">IF(OR(G147=0,F147=0)," - ",NETWORKDAYS(F147,G147))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K147" s="41"/>
+      <c r="L147" s="48"/>
+      <c r="M147" s="48"/>
+      <c r="N147" s="48"/>
+      <c r="O147" s="48"/>
+      <c r="P147" s="48"/>
+      <c r="Q147" s="48"/>
+      <c r="R147" s="48"/>
+      <c r="S147" s="48"/>
+      <c r="T147" s="48"/>
+      <c r="U147" s="48"/>
+      <c r="V147" s="48"/>
+      <c r="W147" s="48"/>
+      <c r="X147" s="48"/>
+      <c r="Y147" s="48"/>
+      <c r="Z147" s="48"/>
+      <c r="AA147" s="48"/>
+      <c r="AB147" s="48"/>
+      <c r="AC147" s="48"/>
+      <c r="AD147" s="48"/>
+      <c r="AE147" s="48"/>
+      <c r="AF147" s="48"/>
+      <c r="AG147" s="48"/>
+      <c r="AH147" s="48"/>
+      <c r="AI147" s="48"/>
+      <c r="AJ147" s="48"/>
+      <c r="AK147" s="48"/>
+      <c r="AL147" s="48"/>
+      <c r="AM147" s="48"/>
+      <c r="AN147" s="48"/>
+      <c r="AO147" s="48"/>
+      <c r="AP147" s="48"/>
+      <c r="AQ147" s="48"/>
+      <c r="AR147" s="48"/>
+      <c r="AS147" s="48"/>
+      <c r="AT147" s="48"/>
+      <c r="AU147" s="48"/>
+      <c r="AV147" s="48"/>
+      <c r="AW147" s="48"/>
+      <c r="AX147" s="48"/>
+      <c r="AY147" s="48"/>
+      <c r="AZ147" s="48"/>
+      <c r="BA147" s="48"/>
+      <c r="BB147" s="48"/>
+      <c r="BC147" s="48"/>
+      <c r="BD147" s="48"/>
+      <c r="BE147" s="48"/>
+      <c r="BF147" s="48"/>
+      <c r="BG147" s="48"/>
+      <c r="BH147" s="48"/>
+      <c r="BI147" s="48"/>
+      <c r="BJ147" s="48"/>
+      <c r="BK147" s="48"/>
+      <c r="BL147" s="48"/>
+      <c r="BM147" s="48"/>
+      <c r="BN147" s="48"/>
+      <c r="BO147" s="48"/>
     </row>
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.1</v>
       </c>
       <c r="B148" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D148" s="70"/>
       <c r="E148" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F148" s="42">
         <v>44379</v>
@@ -15795,14 +15812,14 @@
     <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.2</v>
       </c>
       <c r="B149" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D149" s="70"/>
       <c r="E149" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F149" s="42">
         <v>44379</v>
@@ -15872,17 +15889,17 @@
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B150" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D150" s="66"/>
+        <v>13.3</v>
+      </c>
+      <c r="B150" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D150" s="70"/>
       <c r="E150" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F150" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G150" s="43"/>
       <c r="H150" s="25"/>
@@ -15947,11 +15964,20 @@
       <c r="BO150" s="46"/>
     </row>
     <row r="151" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="23"/>
-      <c r="B151" s="65"/>
-      <c r="D151" s="66"/>
-      <c r="E151" s="66"/>
-      <c r="F151" s="42"/>
+      <c r="A151" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.4</v>
+      </c>
+      <c r="B151" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D151" s="70"/>
+      <c r="E151" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F151" s="42">
+        <v>44379</v>
+      </c>
       <c r="G151" s="43"/>
       <c r="H151" s="25"/>
       <c r="I151" s="26"/>
@@ -16015,11 +16041,20 @@
       <c r="BO151" s="46"/>
     </row>
     <row r="152" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A152" s="23"/>
-      <c r="B152" s="65"/>
+      <c r="A152" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B152" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D152" s="66"/>
-      <c r="E152" s="66"/>
-      <c r="F152" s="42"/>
+      <c r="E152" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F152" s="42">
+        <v>44531</v>
+      </c>
       <c r="G152" s="43"/>
       <c r="H152" s="25"/>
       <c r="I152" s="26"/>
@@ -16153,7 +16188,7 @@
     <row r="154" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="23"/>
       <c r="B154" s="65"/>
-      <c r="D154" s="70"/>
+      <c r="D154" s="66"/>
       <c r="E154" s="66"/>
       <c r="F154" s="42"/>
       <c r="G154" s="43"/>
@@ -16221,7 +16256,7 @@
     <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="23"/>
       <c r="B155" s="65"/>
-      <c r="D155" s="70"/>
+      <c r="D155" s="66"/>
       <c r="E155" s="66"/>
       <c r="F155" s="42"/>
       <c r="G155" s="43"/>
@@ -16493,7 +16528,7 @@
     <row r="159" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="23"/>
       <c r="B159" s="65"/>
-      <c r="D159" s="66"/>
+      <c r="D159" s="70"/>
       <c r="E159" s="66"/>
       <c r="F159" s="42"/>
       <c r="G159" s="43"/>
@@ -16561,7 +16596,7 @@
     <row r="160" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="23"/>
       <c r="B160" s="65"/>
-      <c r="D160" s="66"/>
+      <c r="D160" s="70"/>
       <c r="E160" s="66"/>
       <c r="F160" s="42"/>
       <c r="G160" s="43"/>
@@ -16765,7 +16800,7 @@
     <row r="163" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="23"/>
       <c r="B163" s="65"/>
-      <c r="D163" s="70"/>
+      <c r="D163" s="66"/>
       <c r="E163" s="66"/>
       <c r="F163" s="42"/>
       <c r="G163" s="43"/>
@@ -16833,7 +16868,7 @@
     <row r="164" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="23"/>
       <c r="B164" s="65"/>
-      <c r="D164" s="70"/>
+      <c r="D164" s="66"/>
       <c r="E164" s="66"/>
       <c r="F164" s="42"/>
       <c r="G164" s="43"/>
@@ -17105,7 +17140,7 @@
     <row r="168" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="23"/>
       <c r="B168" s="65"/>
-      <c r="D168" s="66"/>
+      <c r="D168" s="70"/>
       <c r="E168" s="66"/>
       <c r="F168" s="42"/>
       <c r="G168" s="43"/>
@@ -17173,7 +17208,7 @@
     <row r="169" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="23"/>
       <c r="B169" s="65"/>
-      <c r="D169" s="66"/>
+      <c r="D169" s="70"/>
       <c r="E169" s="66"/>
       <c r="F169" s="42"/>
       <c r="G169" s="43"/>
@@ -17377,7 +17412,7 @@
     <row r="172" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="23"/>
       <c r="B172" s="65"/>
-      <c r="D172" s="70"/>
+      <c r="D172" s="66"/>
       <c r="E172" s="66"/>
       <c r="F172" s="42"/>
       <c r="G172" s="43"/>
@@ -17445,7 +17480,7 @@
     <row r="173" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="23"/>
       <c r="B173" s="65"/>
-      <c r="D173" s="70"/>
+      <c r="D173" s="66"/>
       <c r="E173" s="66"/>
       <c r="F173" s="42"/>
       <c r="G173" s="43"/>
@@ -17717,7 +17752,7 @@
     <row r="177" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="23"/>
       <c r="B177" s="65"/>
-      <c r="D177" s="66"/>
+      <c r="D177" s="70"/>
       <c r="E177" s="66"/>
       <c r="F177" s="42"/>
       <c r="G177" s="43"/>
@@ -17785,7 +17820,7 @@
     <row r="178" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="23"/>
       <c r="B178" s="65"/>
-      <c r="D178" s="66"/>
+      <c r="D178" s="70"/>
       <c r="E178" s="66"/>
       <c r="F178" s="42"/>
       <c r="G178" s="43"/>
@@ -17989,7 +18024,7 @@
     <row r="181" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A181" s="23"/>
       <c r="B181" s="65"/>
-      <c r="D181" s="70"/>
+      <c r="D181" s="66"/>
       <c r="E181" s="66"/>
       <c r="F181" s="42"/>
       <c r="G181" s="43"/>
@@ -18057,7 +18092,7 @@
     <row r="182" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A182" s="23"/>
       <c r="B182" s="65"/>
-      <c r="D182" s="70"/>
+      <c r="D182" s="66"/>
       <c r="E182" s="66"/>
       <c r="F182" s="42"/>
       <c r="G182" s="43"/>
@@ -18326,9 +18361,154 @@
       <c r="BN185" s="46"/>
       <c r="BO185" s="46"/>
     </row>
+    <row r="186" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="23"/>
+      <c r="B186" s="65"/>
+      <c r="D186" s="70"/>
+      <c r="E186" s="66"/>
+      <c r="F186" s="42"/>
+      <c r="G186" s="43"/>
+      <c r="H186" s="25"/>
+      <c r="I186" s="26"/>
+      <c r="J186" s="27"/>
+      <c r="K186" s="40"/>
+      <c r="L186" s="46"/>
+      <c r="M186" s="46"/>
+      <c r="N186" s="46"/>
+      <c r="O186" s="46"/>
+      <c r="P186" s="46"/>
+      <c r="Q186" s="46"/>
+      <c r="R186" s="46"/>
+      <c r="S186" s="46"/>
+      <c r="T186" s="46"/>
+      <c r="U186" s="46"/>
+      <c r="V186" s="46"/>
+      <c r="W186" s="46"/>
+      <c r="X186" s="46"/>
+      <c r="Y186" s="46"/>
+      <c r="Z186" s="46"/>
+      <c r="AA186" s="46"/>
+      <c r="AB186" s="46"/>
+      <c r="AC186" s="46"/>
+      <c r="AD186" s="46"/>
+      <c r="AE186" s="46"/>
+      <c r="AF186" s="46"/>
+      <c r="AG186" s="46"/>
+      <c r="AH186" s="46"/>
+      <c r="AI186" s="46"/>
+      <c r="AJ186" s="46"/>
+      <c r="AK186" s="46"/>
+      <c r="AL186" s="46"/>
+      <c r="AM186" s="46"/>
+      <c r="AN186" s="46"/>
+      <c r="AO186" s="46"/>
+      <c r="AP186" s="46"/>
+      <c r="AQ186" s="46"/>
+      <c r="AR186" s="46"/>
+      <c r="AS186" s="46"/>
+      <c r="AT186" s="46"/>
+      <c r="AU186" s="46"/>
+      <c r="AV186" s="46"/>
+      <c r="AW186" s="46"/>
+      <c r="AX186" s="46"/>
+      <c r="AY186" s="46"/>
+      <c r="AZ186" s="46"/>
+      <c r="BA186" s="46"/>
+      <c r="BB186" s="46"/>
+      <c r="BC186" s="46"/>
+      <c r="BD186" s="46"/>
+      <c r="BE186" s="46"/>
+      <c r="BF186" s="46"/>
+      <c r="BG186" s="46"/>
+      <c r="BH186" s="46"/>
+      <c r="BI186" s="46"/>
+      <c r="BJ186" s="46"/>
+      <c r="BK186" s="46"/>
+      <c r="BL186" s="46"/>
+      <c r="BM186" s="46"/>
+      <c r="BN186" s="46"/>
+      <c r="BO186" s="46"/>
+    </row>
+    <row r="187" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="23"/>
+      <c r="B187" s="65"/>
+      <c r="D187" s="70"/>
+      <c r="E187" s="66"/>
+      <c r="F187" s="42"/>
+      <c r="G187" s="43"/>
+      <c r="H187" s="25"/>
+      <c r="I187" s="26"/>
+      <c r="J187" s="27"/>
+      <c r="K187" s="40"/>
+      <c r="L187" s="46"/>
+      <c r="M187" s="46"/>
+      <c r="N187" s="46"/>
+      <c r="O187" s="46"/>
+      <c r="P187" s="46"/>
+      <c r="Q187" s="46"/>
+      <c r="R187" s="46"/>
+      <c r="S187" s="46"/>
+      <c r="T187" s="46"/>
+      <c r="U187" s="46"/>
+      <c r="V187" s="46"/>
+      <c r="W187" s="46"/>
+      <c r="X187" s="46"/>
+      <c r="Y187" s="46"/>
+      <c r="Z187" s="46"/>
+      <c r="AA187" s="46"/>
+      <c r="AB187" s="46"/>
+      <c r="AC187" s="46"/>
+      <c r="AD187" s="46"/>
+      <c r="AE187" s="46"/>
+      <c r="AF187" s="46"/>
+      <c r="AG187" s="46"/>
+      <c r="AH187" s="46"/>
+      <c r="AI187" s="46"/>
+      <c r="AJ187" s="46"/>
+      <c r="AK187" s="46"/>
+      <c r="AL187" s="46"/>
+      <c r="AM187" s="46"/>
+      <c r="AN187" s="46"/>
+      <c r="AO187" s="46"/>
+      <c r="AP187" s="46"/>
+      <c r="AQ187" s="46"/>
+      <c r="AR187" s="46"/>
+      <c r="AS187" s="46"/>
+      <c r="AT187" s="46"/>
+      <c r="AU187" s="46"/>
+      <c r="AV187" s="46"/>
+      <c r="AW187" s="46"/>
+      <c r="AX187" s="46"/>
+      <c r="AY187" s="46"/>
+      <c r="AZ187" s="46"/>
+      <c r="BA187" s="46"/>
+      <c r="BB187" s="46"/>
+      <c r="BC187" s="46"/>
+      <c r="BD187" s="46"/>
+      <c r="BE187" s="46"/>
+      <c r="BF187" s="46"/>
+      <c r="BG187" s="46"/>
+      <c r="BH187" s="46"/>
+      <c r="BI187" s="46"/>
+      <c r="BJ187" s="46"/>
+      <c r="BK187" s="46"/>
+      <c r="BL187" s="46"/>
+      <c r="BM187" s="46"/>
+      <c r="BN187" s="46"/>
+      <c r="BO187" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -18339,18 +18519,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I146:I149 I98:I103 I105:I110 I112:I122 I124:I144">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I148:I151 I98:I103 I105:I110 I112:I122 I124:I146">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18369,7 +18540,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN144 L150:BO152 M153:BN158 BO156:BO158 L159:BO161 M162:BN167 BO165:BO167 L168:BO170 M171:BN176 BO174:BO176 L177:BO179 M180:BN185 BO183:BO185 BO148:BO149 M146:BN149 L145:BO145 L123:BO123">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN146 L152:BO154 M155:BN160 BO158:BO160 L161:BO163 M164:BN169 BO167:BO169 L170:BO172 M173:BN178 BO176:BO178 L179:BO181 M182:BN187 BO185:BO187 BO150:BO151 M148:BN151 L147:BO147 L123:BO123">
     <cfRule type="expression" dxfId="132" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -18377,7 +18548,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L146:BO149 L98:BO103 L105:BO110 L112:BO122 L124:BO144">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L148:BO151 L98:BO103 L105:BO110 L112:BO122 L124:BO146">
     <cfRule type="expression" dxfId="130" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -18387,7 +18558,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E186:E1048576 E95:E96 E146:E149 E98:E103 E105:E110 E112:E122 E124:E144">
+  <conditionalFormatting sqref="E1:E73 E188:E1048576 E95:E96 E148:E151 E98:E103 E105:E110 E112:E122 E124:E146">
     <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18481,7 +18652,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I150:I158">
+  <conditionalFormatting sqref="I152:I160">
     <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18495,12 +18666,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L150:BO158">
+  <conditionalFormatting sqref="L152:BO160">
     <cfRule type="expression" dxfId="106" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E150:E158">
+  <conditionalFormatting sqref="E152:E160">
     <cfRule type="cellIs" dxfId="105" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18523,7 +18694,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L153:BO158 L146:BO149 L98:BO103 L105:BO110 L112:BO122 L124:BO144">
+  <conditionalFormatting sqref="L155:BO160 L148:BO151 L98:BO103 L105:BO110 L112:BO122 L124:BO146">
     <cfRule type="expression" dxfId="98" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18531,7 +18702,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I159:I167">
+  <conditionalFormatting sqref="I161:I169">
     <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18545,12 +18716,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L159:BO167">
+  <conditionalFormatting sqref="L161:BO169">
     <cfRule type="expression" dxfId="96" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E159:E167">
+  <conditionalFormatting sqref="E161:E169">
     <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18573,7 +18744,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L162:BO167">
+  <conditionalFormatting sqref="L164:BO169">
     <cfRule type="expression" dxfId="88" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18581,7 +18752,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I168:I176">
+  <conditionalFormatting sqref="I170:I178">
     <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18595,12 +18766,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L168:BO176">
+  <conditionalFormatting sqref="L170:BO178">
     <cfRule type="expression" dxfId="86" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E168:E176">
+  <conditionalFormatting sqref="E170:E178">
     <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18623,7 +18794,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L171:BO176">
+  <conditionalFormatting sqref="L173:BO178">
     <cfRule type="expression" dxfId="78" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18631,7 +18802,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I177:I185">
+  <conditionalFormatting sqref="I179:I187">
     <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18645,12 +18816,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L177:BO185">
+  <conditionalFormatting sqref="L179:BO187">
     <cfRule type="expression" dxfId="76" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E177:E185">
+  <conditionalFormatting sqref="E179:E187">
     <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18673,7 +18844,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L180:BO185">
+  <conditionalFormatting sqref="L182:BO187">
     <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18823,7 +18994,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I145">
+  <conditionalFormatting sqref="I147">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18837,12 +19008,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L145:BO145">
+  <conditionalFormatting sqref="L147:BO147">
     <cfRule type="expression" dxfId="38" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E145">
+  <conditionalFormatting sqref="E147">
     <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19063,7 +19234,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I146:I149 I98:I103 I105:I110 I112:I122 I124:I144</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I148:I151 I98:I103 I105:I110 I112:I122 I124:I146</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -19093,7 +19264,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I150:I158</xm:sqref>
+          <xm:sqref>I152:I160</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -19108,7 +19279,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I159:I167</xm:sqref>
+          <xm:sqref>I161:I169</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -19123,7 +19294,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I168:I176</xm:sqref>
+          <xm:sqref>I170:I178</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -19138,7 +19309,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I177:I185</xm:sqref>
+          <xm:sqref>I179:I187</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -19198,7 +19369,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I145</xm:sqref>
+          <xm:sqref>I147</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Removed unnecessary external forecasts pull in m1 since moved to pull-external-forecasts.r (v0.17)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B105D2D4-ABF8-4966-8076-5EBA6CEC8676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A28D7E-6655-4B1D-A4E4-8458B23E6B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="175">
   <si>
     <t>WBS</t>
   </si>
@@ -922,9 +922,6 @@
     <t>Model Data Resiliency Upgrades</t>
   </si>
   <si>
-    <t>Model Productionalization &amp; Website Upgrade (v0.17)</t>
-  </si>
-  <si>
     <t>Split Data Import</t>
   </si>
   <si>
@@ -946,7 +943,16 @@
     <t>Move Task Scheduler to Cron Job on Prod VPS</t>
   </si>
   <si>
-    <t>R to Enter Data On Vintage Change</t>
+    <t>Model Prod, Vintage Analysis, Website Overhaul (v0.17)</t>
+  </si>
+  <si>
+    <t>Pull Historical Vintages</t>
+  </si>
+  <si>
+    <t>Add Vintage Backtesting</t>
+  </si>
+  <si>
+    <t>Add Optimal Model Stacking</t>
   </si>
 </sst>
 </file>
@@ -1875,6 +1881,13 @@
     <xf numFmtId="0" fontId="44" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1884,6 +1897,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1892,17 +1909,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3463,11 +3469,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO187"/>
+  <dimension ref="A1:BO189"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F134" sqref="F134"/>
+      <pane ySplit="7" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3497,27 +3503,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="84"/>
-      <c r="O1" s="84"/>
-      <c r="P1" s="84"/>
-      <c r="Q1" s="84"/>
-      <c r="R1" s="84"/>
-      <c r="S1" s="84"/>
-      <c r="T1" s="84"/>
-      <c r="U1" s="84"/>
-      <c r="V1" s="84"/>
-      <c r="W1" s="84"/>
-      <c r="X1" s="84"/>
-      <c r="Y1" s="84"/>
-      <c r="Z1" s="84"/>
-      <c r="AA1" s="84"/>
-      <c r="AB1" s="84"/>
-      <c r="AC1" s="84"/>
-      <c r="AD1" s="84"/>
-      <c r="AE1" s="84"/>
-      <c r="AF1" s="84"/>
+      <c r="L1" s="78"/>
+      <c r="M1" s="78"/>
+      <c r="N1" s="78"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
+      <c r="W1" s="78"/>
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="78"/>
+      <c r="AC1" s="78"/>
+      <c r="AD1" s="78"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="78"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3562,12 +3568,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="86">
+      <c r="C4" s="83">
         <v>44192</v>
       </c>
-      <c r="D4" s="86"/>
-      <c r="E4" s="86"/>
-      <c r="F4" s="86"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3577,183 +3583,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="78" t="str">
+      <c r="L4" s="80" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 43</v>
       </c>
-      <c r="M4" s="79"/>
-      <c r="N4" s="79"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="79"/>
-      <c r="Q4" s="79"/>
-      <c r="R4" s="80"/>
-      <c r="S4" s="78" t="str">
+      <c r="M4" s="81"/>
+      <c r="N4" s="81"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="80" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 44</v>
       </c>
-      <c r="T4" s="79"/>
-      <c r="U4" s="79"/>
-      <c r="V4" s="79"/>
-      <c r="W4" s="79"/>
-      <c r="X4" s="79"/>
-      <c r="Y4" s="80"/>
-      <c r="Z4" s="78" t="str">
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="81"/>
+      <c r="W4" s="81"/>
+      <c r="X4" s="81"/>
+      <c r="Y4" s="82"/>
+      <c r="Z4" s="80" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 45</v>
       </c>
-      <c r="AA4" s="79"/>
-      <c r="AB4" s="79"/>
-      <c r="AC4" s="79"/>
-      <c r="AD4" s="79"/>
-      <c r="AE4" s="79"/>
-      <c r="AF4" s="80"/>
-      <c r="AG4" s="78" t="str">
+      <c r="AA4" s="81"/>
+      <c r="AB4" s="81"/>
+      <c r="AC4" s="81"/>
+      <c r="AD4" s="81"/>
+      <c r="AE4" s="81"/>
+      <c r="AF4" s="82"/>
+      <c r="AG4" s="80" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 46</v>
       </c>
-      <c r="AH4" s="79"/>
-      <c r="AI4" s="79"/>
-      <c r="AJ4" s="79"/>
-      <c r="AK4" s="79"/>
-      <c r="AL4" s="79"/>
-      <c r="AM4" s="80"/>
-      <c r="AN4" s="78" t="str">
+      <c r="AH4" s="81"/>
+      <c r="AI4" s="81"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="81"/>
+      <c r="AL4" s="81"/>
+      <c r="AM4" s="82"/>
+      <c r="AN4" s="80" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 47</v>
       </c>
-      <c r="AO4" s="79"/>
-      <c r="AP4" s="79"/>
-      <c r="AQ4" s="79"/>
-      <c r="AR4" s="79"/>
-      <c r="AS4" s="79"/>
-      <c r="AT4" s="80"/>
-      <c r="AU4" s="78" t="str">
+      <c r="AO4" s="81"/>
+      <c r="AP4" s="81"/>
+      <c r="AQ4" s="81"/>
+      <c r="AR4" s="81"/>
+      <c r="AS4" s="81"/>
+      <c r="AT4" s="82"/>
+      <c r="AU4" s="80" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 48</v>
       </c>
-      <c r="AV4" s="79"/>
-      <c r="AW4" s="79"/>
-      <c r="AX4" s="79"/>
-      <c r="AY4" s="79"/>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="80"/>
-      <c r="BB4" s="78" t="str">
+      <c r="AV4" s="81"/>
+      <c r="AW4" s="81"/>
+      <c r="AX4" s="81"/>
+      <c r="AY4" s="81"/>
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="82"/>
+      <c r="BB4" s="80" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 49</v>
       </c>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="79"/>
-      <c r="BH4" s="80"/>
-      <c r="BI4" s="78" t="str">
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="81"/>
+      <c r="BH4" s="82"/>
+      <c r="BI4" s="80" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 50</v>
       </c>
-      <c r="BJ4" s="79"/>
-      <c r="BK4" s="79"/>
-      <c r="BL4" s="79"/>
-      <c r="BM4" s="79"/>
-      <c r="BN4" s="79"/>
-      <c r="BO4" s="80"/>
+      <c r="BJ4" s="81"/>
+      <c r="BK4" s="81"/>
+      <c r="BL4" s="81"/>
+      <c r="BM4" s="81"/>
+      <c r="BN4" s="81"/>
+      <c r="BO4" s="82"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="85" t="s">
+      <c r="C5" s="79" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="85"/>
-      <c r="E5" s="85"/>
-      <c r="F5" s="85"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="81">
+      <c r="L5" s="84">
         <f>L6</f>
         <v>44487</v>
       </c>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
-      <c r="P5" s="82"/>
-      <c r="Q5" s="82"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="81">
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="86"/>
+      <c r="S5" s="84">
         <f>S6</f>
         <v>44494</v>
       </c>
-      <c r="T5" s="82"/>
-      <c r="U5" s="82"/>
-      <c r="V5" s="82"/>
-      <c r="W5" s="82"/>
-      <c r="X5" s="82"/>
-      <c r="Y5" s="83"/>
-      <c r="Z5" s="81">
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="86"/>
+      <c r="Z5" s="84">
         <f>Z6</f>
         <v>44501</v>
       </c>
-      <c r="AA5" s="82"/>
-      <c r="AB5" s="82"/>
-      <c r="AC5" s="82"/>
-      <c r="AD5" s="82"/>
-      <c r="AE5" s="82"/>
-      <c r="AF5" s="83"/>
-      <c r="AG5" s="81">
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85"/>
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="86"/>
+      <c r="AG5" s="84">
         <f>AG6</f>
         <v>44508</v>
       </c>
-      <c r="AH5" s="82"/>
-      <c r="AI5" s="82"/>
-      <c r="AJ5" s="82"/>
-      <c r="AK5" s="82"/>
-      <c r="AL5" s="82"/>
-      <c r="AM5" s="83"/>
-      <c r="AN5" s="81">
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="85"/>
+      <c r="AJ5" s="85"/>
+      <c r="AK5" s="85"/>
+      <c r="AL5" s="85"/>
+      <c r="AM5" s="86"/>
+      <c r="AN5" s="84">
         <f>AN6</f>
         <v>44515</v>
       </c>
-      <c r="AO5" s="82"/>
-      <c r="AP5" s="82"/>
-      <c r="AQ5" s="82"/>
-      <c r="AR5" s="82"/>
-      <c r="AS5" s="82"/>
-      <c r="AT5" s="83"/>
-      <c r="AU5" s="81">
+      <c r="AO5" s="85"/>
+      <c r="AP5" s="85"/>
+      <c r="AQ5" s="85"/>
+      <c r="AR5" s="85"/>
+      <c r="AS5" s="85"/>
+      <c r="AT5" s="86"/>
+      <c r="AU5" s="84">
         <f>AU6</f>
         <v>44522</v>
       </c>
-      <c r="AV5" s="82"/>
-      <c r="AW5" s="82"/>
-      <c r="AX5" s="82"/>
-      <c r="AY5" s="82"/>
-      <c r="AZ5" s="82"/>
-      <c r="BA5" s="83"/>
-      <c r="BB5" s="81">
+      <c r="AV5" s="85"/>
+      <c r="AW5" s="85"/>
+      <c r="AX5" s="85"/>
+      <c r="AY5" s="85"/>
+      <c r="AZ5" s="85"/>
+      <c r="BA5" s="86"/>
+      <c r="BB5" s="84">
         <f>BB6</f>
         <v>44529</v>
       </c>
-      <c r="BC5" s="82"/>
-      <c r="BD5" s="82"/>
-      <c r="BE5" s="82"/>
-      <c r="BF5" s="82"/>
-      <c r="BG5" s="82"/>
-      <c r="BH5" s="83"/>
-      <c r="BI5" s="81">
+      <c r="BC5" s="85"/>
+      <c r="BD5" s="85"/>
+      <c r="BE5" s="85"/>
+      <c r="BF5" s="85"/>
+      <c r="BG5" s="85"/>
+      <c r="BH5" s="86"/>
+      <c r="BI5" s="84">
         <f>BI6</f>
         <v>44536</v>
       </c>
-      <c r="BJ5" s="82"/>
-      <c r="BK5" s="82"/>
-      <c r="BL5" s="82"/>
-      <c r="BM5" s="82"/>
-      <c r="BN5" s="82"/>
-      <c r="BO5" s="83"/>
+      <c r="BJ5" s="85"/>
+      <c r="BK5" s="85"/>
+      <c r="BL5" s="85"/>
+      <c r="BM5" s="85"/>
+      <c r="BN5" s="85"/>
+      <c r="BO5" s="86"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8911,7 +8917,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A152" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A154" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -13717,7 +13723,7 @@
         <v>12</v>
       </c>
       <c r="B123" s="17" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="D123" s="19"/>
       <c r="E123" s="19"/>
@@ -14201,7 +14207,7 @@
         <v>12.6</v>
       </c>
       <c r="B129" s="65" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D129" s="70"/>
       <c r="E129" s="66" t="s">
@@ -14282,7 +14288,7 @@
         <v>12.7</v>
       </c>
       <c r="B130" s="65" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D130" s="70"/>
       <c r="E130" s="66" t="s">
@@ -14363,11 +14369,11 @@
         <v>12.8</v>
       </c>
       <c r="B131" s="65" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D131" s="70"/>
       <c r="E131" s="66" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F131" s="42">
         <v>44489</v>
@@ -14444,7 +14450,7 @@
         <v>12.9</v>
       </c>
       <c r="B132" s="65" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D132" s="70"/>
       <c r="E132" s="66" t="s">
@@ -14525,17 +14531,17 @@
         <v>12.10</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F133" s="42">
         <v>44490</v>
       </c>
       <c r="G133" s="43">
-        <v>44492</v>
+        <v>44491</v>
       </c>
       <c r="H133" s="73"/>
       <c r="I133" s="26">
@@ -14610,13 +14616,13 @@
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F134" s="42">
-        <v>44491</v>
+        <v>44490</v>
       </c>
       <c r="G134" s="43">
-        <v>44493</v>
+        <v>44492</v>
       </c>
       <c r="H134" s="73"/>
       <c r="I134" s="26">
@@ -14687,17 +14693,17 @@
         <v>12.12</v>
       </c>
       <c r="B135" s="65" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F135" s="42">
+        <v>44491</v>
+      </c>
+      <c r="G135" s="43">
         <v>44493</v>
-      </c>
-      <c r="G135" s="43">
-        <v>44499</v>
       </c>
       <c r="H135" s="73"/>
       <c r="I135" s="26">
@@ -14768,17 +14774,17 @@
         <v>12.13</v>
       </c>
       <c r="B136" s="65" t="s">
-        <v>155</v>
+        <v>174</v>
       </c>
       <c r="D136" s="70"/>
       <c r="E136" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F136" s="42">
-        <v>44494</v>
+        <v>44491</v>
       </c>
       <c r="G136" s="43">
-        <v>44499</v>
+        <v>44493</v>
       </c>
       <c r="H136" s="73"/>
       <c r="I136" s="26">
@@ -14849,14 +14855,14 @@
         <v>12.14</v>
       </c>
       <c r="B137" s="65" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="D137" s="70"/>
       <c r="E137" s="66" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F137" s="42">
-        <v>44494</v>
+        <v>44493</v>
       </c>
       <c r="G137" s="43">
         <v>44499</v>
@@ -14930,7 +14936,7 @@
         <v>12.15</v>
       </c>
       <c r="B138" s="65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D138" s="70"/>
       <c r="E138" s="66" t="s">
@@ -15011,7 +15017,7 @@
         <v>12.16</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D139" s="70"/>
       <c r="E139" s="66" t="s">
@@ -15092,17 +15098,17 @@
         <v>12.17</v>
       </c>
       <c r="B140" s="65" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
       <c r="D140" s="70"/>
       <c r="E140" s="66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F140" s="42">
         <v>44494</v>
       </c>
       <c r="G140" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H140" s="73"/>
       <c r="I140" s="26">
@@ -15173,21 +15179,21 @@
         <v>12.18</v>
       </c>
       <c r="B141" s="65" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D141" s="70"/>
       <c r="E141" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F141" s="42">
         <v>44494</v>
       </c>
       <c r="G141" s="43">
-        <v>44501</v>
+        <v>44499</v>
       </c>
       <c r="H141" s="73"/>
       <c r="I141" s="26">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="J141" s="75"/>
       <c r="K141" s="76"/>
@@ -15254,11 +15260,11 @@
         <v>12.19</v>
       </c>
       <c r="B142" s="65" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="D142" s="70"/>
       <c r="E142" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F142" s="42">
         <v>44494</v>
@@ -15335,7 +15341,7 @@
         <v>12.20</v>
       </c>
       <c r="B143" s="65" t="s">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="D143" s="70"/>
       <c r="E143" s="66" t="s">
@@ -15345,11 +15351,11 @@
         <v>44494</v>
       </c>
       <c r="G143" s="43">
-        <v>44510</v>
+        <v>44501</v>
       </c>
       <c r="H143" s="73"/>
       <c r="I143" s="26">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="J143" s="75"/>
       <c r="K143" s="76"/>
@@ -15416,20 +15422,20 @@
         <v>12.21</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D144" s="70"/>
-      <c r="E144" s="70" t="s">
+      <c r="E144" s="66" t="s">
         <v>67</v>
       </c>
-      <c r="F144" s="71">
+      <c r="F144" s="42">
         <v>44494</v>
       </c>
-      <c r="G144" s="72">
-        <v>44510</v>
+      <c r="G144" s="43">
+        <v>44501</v>
       </c>
       <c r="H144" s="73"/>
-      <c r="I144" s="74">
+      <c r="I144" s="26">
         <v>0</v>
       </c>
       <c r="J144" s="75"/>
@@ -15497,20 +15503,20 @@
         <v>12.22</v>
       </c>
       <c r="B145" s="65" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="D145" s="70"/>
-      <c r="E145" s="70" t="s">
-        <v>70</v>
-      </c>
-      <c r="F145" s="71">
+      <c r="E145" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F145" s="42">
         <v>44494</v>
       </c>
-      <c r="G145" s="72">
+      <c r="G145" s="43">
         <v>44510</v>
       </c>
       <c r="H145" s="73"/>
-      <c r="I145" s="74">
+      <c r="I145" s="26">
         <v>0</v>
       </c>
       <c r="J145" s="75"/>
@@ -15578,17 +15584,17 @@
         <v>12.23</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D146" s="70"/>
       <c r="E146" s="70" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F146" s="71">
         <v>44494</v>
       </c>
       <c r="G146" s="72">
-        <v>44520</v>
+        <v>44510</v>
       </c>
       <c r="H146" s="73"/>
       <c r="I146" s="74">
@@ -15653,105 +15659,111 @@
       <c r="BN146" s="46"/>
       <c r="BO146" s="46"/>
     </row>
-    <row r="147" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A147" s="16" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>13</v>
-      </c>
-      <c r="B147" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="D147" s="19"/>
-      <c r="E147" s="19"/>
-      <c r="F147" s="44"/>
-      <c r="G147" s="44" t="str">
-        <f t="shared" ref="G147" si="24">IF(ISBLANK(F147)," - ",IF(H147=0,F147,F147+H147-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="H147" s="20"/>
-      <c r="I147" s="21"/>
-      <c r="J147" s="22" t="str">
-        <f t="shared" ref="J147" si="25">IF(OR(G147=0,F147=0)," - ",NETWORKDAYS(F147,G147))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="K147" s="41"/>
-      <c r="L147" s="48"/>
-      <c r="M147" s="48"/>
-      <c r="N147" s="48"/>
-      <c r="O147" s="48"/>
-      <c r="P147" s="48"/>
-      <c r="Q147" s="48"/>
-      <c r="R147" s="48"/>
-      <c r="S147" s="48"/>
-      <c r="T147" s="48"/>
-      <c r="U147" s="48"/>
-      <c r="V147" s="48"/>
-      <c r="W147" s="48"/>
-      <c r="X147" s="48"/>
-      <c r="Y147" s="48"/>
-      <c r="Z147" s="48"/>
-      <c r="AA147" s="48"/>
-      <c r="AB147" s="48"/>
-      <c r="AC147" s="48"/>
-      <c r="AD147" s="48"/>
-      <c r="AE147" s="48"/>
-      <c r="AF147" s="48"/>
-      <c r="AG147" s="48"/>
-      <c r="AH147" s="48"/>
-      <c r="AI147" s="48"/>
-      <c r="AJ147" s="48"/>
-      <c r="AK147" s="48"/>
-      <c r="AL147" s="48"/>
-      <c r="AM147" s="48"/>
-      <c r="AN147" s="48"/>
-      <c r="AO147" s="48"/>
-      <c r="AP147" s="48"/>
-      <c r="AQ147" s="48"/>
-      <c r="AR147" s="48"/>
-      <c r="AS147" s="48"/>
-      <c r="AT147" s="48"/>
-      <c r="AU147" s="48"/>
-      <c r="AV147" s="48"/>
-      <c r="AW147" s="48"/>
-      <c r="AX147" s="48"/>
-      <c r="AY147" s="48"/>
-      <c r="AZ147" s="48"/>
-      <c r="BA147" s="48"/>
-      <c r="BB147" s="48"/>
-      <c r="BC147" s="48"/>
-      <c r="BD147" s="48"/>
-      <c r="BE147" s="48"/>
-      <c r="BF147" s="48"/>
-      <c r="BG147" s="48"/>
-      <c r="BH147" s="48"/>
-      <c r="BI147" s="48"/>
-      <c r="BJ147" s="48"/>
-      <c r="BK147" s="48"/>
-      <c r="BL147" s="48"/>
-      <c r="BM147" s="48"/>
-      <c r="BN147" s="48"/>
-      <c r="BO147" s="48"/>
+    <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>12.24</v>
+      </c>
+      <c r="B147" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="D147" s="70"/>
+      <c r="E147" s="70" t="s">
+        <v>70</v>
+      </c>
+      <c r="F147" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G147" s="72">
+        <v>44510</v>
+      </c>
+      <c r="H147" s="73"/>
+      <c r="I147" s="74">
+        <v>0</v>
+      </c>
+      <c r="J147" s="75"/>
+      <c r="K147" s="76"/>
+      <c r="L147" s="46"/>
+      <c r="M147" s="46"/>
+      <c r="N147" s="46"/>
+      <c r="O147" s="46"/>
+      <c r="P147" s="46"/>
+      <c r="Q147" s="46"/>
+      <c r="R147" s="46"/>
+      <c r="S147" s="46"/>
+      <c r="T147" s="46"/>
+      <c r="U147" s="46"/>
+      <c r="V147" s="46"/>
+      <c r="W147" s="46"/>
+      <c r="X147" s="46"/>
+      <c r="Y147" s="46"/>
+      <c r="Z147" s="46"/>
+      <c r="AA147" s="46"/>
+      <c r="AB147" s="46"/>
+      <c r="AC147" s="46"/>
+      <c r="AD147" s="46"/>
+      <c r="AE147" s="46"/>
+      <c r="AF147" s="46"/>
+      <c r="AG147" s="46"/>
+      <c r="AH147" s="46"/>
+      <c r="AI147" s="46"/>
+      <c r="AJ147" s="46"/>
+      <c r="AK147" s="46"/>
+      <c r="AL147" s="46"/>
+      <c r="AM147" s="46"/>
+      <c r="AN147" s="46"/>
+      <c r="AO147" s="46"/>
+      <c r="AP147" s="46"/>
+      <c r="AQ147" s="46"/>
+      <c r="AR147" s="46"/>
+      <c r="AS147" s="46"/>
+      <c r="AT147" s="46"/>
+      <c r="AU147" s="46"/>
+      <c r="AV147" s="46"/>
+      <c r="AW147" s="46"/>
+      <c r="AX147" s="46"/>
+      <c r="AY147" s="46"/>
+      <c r="AZ147" s="46"/>
+      <c r="BA147" s="46"/>
+      <c r="BB147" s="46"/>
+      <c r="BC147" s="46"/>
+      <c r="BD147" s="46"/>
+      <c r="BE147" s="46"/>
+      <c r="BF147" s="46"/>
+      <c r="BG147" s="46"/>
+      <c r="BH147" s="46"/>
+      <c r="BI147" s="46"/>
+      <c r="BJ147" s="46"/>
+      <c r="BK147" s="46"/>
+      <c r="BL147" s="46"/>
+      <c r="BM147" s="46"/>
+      <c r="BN147" s="46"/>
+      <c r="BO147" s="46"/>
     </row>
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.1</v>
+        <v>12.25</v>
       </c>
       <c r="B148" s="65" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="D148" s="70"/>
-      <c r="E148" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="F148" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G148" s="43"/>
-      <c r="H148" s="25"/>
-      <c r="I148" s="26"/>
-      <c r="J148" s="27"/>
-      <c r="K148" s="40"/>
+      <c r="E148" s="70" t="s">
+        <v>71</v>
+      </c>
+      <c r="F148" s="71">
+        <v>44494</v>
+      </c>
+      <c r="G148" s="72">
+        <v>44520</v>
+      </c>
+      <c r="H148" s="73"/>
+      <c r="I148" s="74">
+        <v>0</v>
+      </c>
+      <c r="J148" s="75"/>
+      <c r="K148" s="76"/>
       <c r="L148" s="46"/>
       <c r="M148" s="46"/>
       <c r="N148" s="46"/>
@@ -15809,94 +15821,96 @@
       <c r="BN148" s="46"/>
       <c r="BO148" s="46"/>
     </row>
-    <row r="149" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A149" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.2</v>
-      </c>
-      <c r="B149" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="D149" s="70"/>
-      <c r="E149" s="66" t="s">
-        <v>70</v>
-      </c>
-      <c r="F149" s="42">
-        <v>44379</v>
-      </c>
-      <c r="G149" s="43"/>
-      <c r="H149" s="25"/>
-      <c r="I149" s="26"/>
-      <c r="J149" s="27"/>
-      <c r="K149" s="40"/>
-      <c r="L149" s="46"/>
-      <c r="M149" s="46"/>
-      <c r="N149" s="46"/>
-      <c r="O149" s="46"/>
-      <c r="P149" s="46"/>
-      <c r="Q149" s="46"/>
-      <c r="R149" s="46"/>
-      <c r="S149" s="46"/>
-      <c r="T149" s="46"/>
-      <c r="U149" s="46"/>
-      <c r="V149" s="46"/>
-      <c r="W149" s="46"/>
-      <c r="X149" s="46"/>
-      <c r="Y149" s="46"/>
-      <c r="Z149" s="46"/>
-      <c r="AA149" s="46"/>
-      <c r="AB149" s="46"/>
-      <c r="AC149" s="46"/>
-      <c r="AD149" s="46"/>
-      <c r="AE149" s="46"/>
-      <c r="AF149" s="46"/>
-      <c r="AG149" s="46"/>
-      <c r="AH149" s="46"/>
-      <c r="AI149" s="46"/>
-      <c r="AJ149" s="46"/>
-      <c r="AK149" s="46"/>
-      <c r="AL149" s="46"/>
-      <c r="AM149" s="46"/>
-      <c r="AN149" s="46"/>
-      <c r="AO149" s="46"/>
-      <c r="AP149" s="46"/>
-      <c r="AQ149" s="46"/>
-      <c r="AR149" s="46"/>
-      <c r="AS149" s="46"/>
-      <c r="AT149" s="46"/>
-      <c r="AU149" s="46"/>
-      <c r="AV149" s="46"/>
-      <c r="AW149" s="46"/>
-      <c r="AX149" s="46"/>
-      <c r="AY149" s="46"/>
-      <c r="AZ149" s="46"/>
-      <c r="BA149" s="46"/>
-      <c r="BB149" s="46"/>
-      <c r="BC149" s="46"/>
-      <c r="BD149" s="46"/>
-      <c r="BE149" s="46"/>
-      <c r="BF149" s="46"/>
-      <c r="BG149" s="46"/>
-      <c r="BH149" s="46"/>
-      <c r="BI149" s="46"/>
-      <c r="BJ149" s="46"/>
-      <c r="BK149" s="46"/>
-      <c r="BL149" s="46"/>
-      <c r="BM149" s="46"/>
-      <c r="BN149" s="46"/>
-      <c r="BO149" s="46"/>
+    <row r="149" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>13</v>
+      </c>
+      <c r="B149" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D149" s="19"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="44"/>
+      <c r="G149" s="44" t="str">
+        <f t="shared" ref="G149" si="24">IF(ISBLANK(F149)," - ",IF(H149=0,F149,F149+H149-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H149" s="20"/>
+      <c r="I149" s="21"/>
+      <c r="J149" s="22" t="str">
+        <f t="shared" ref="J149" si="25">IF(OR(G149=0,F149=0)," - ",NETWORKDAYS(F149,G149))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K149" s="41"/>
+      <c r="L149" s="48"/>
+      <c r="M149" s="48"/>
+      <c r="N149" s="48"/>
+      <c r="O149" s="48"/>
+      <c r="P149" s="48"/>
+      <c r="Q149" s="48"/>
+      <c r="R149" s="48"/>
+      <c r="S149" s="48"/>
+      <c r="T149" s="48"/>
+      <c r="U149" s="48"/>
+      <c r="V149" s="48"/>
+      <c r="W149" s="48"/>
+      <c r="X149" s="48"/>
+      <c r="Y149" s="48"/>
+      <c r="Z149" s="48"/>
+      <c r="AA149" s="48"/>
+      <c r="AB149" s="48"/>
+      <c r="AC149" s="48"/>
+      <c r="AD149" s="48"/>
+      <c r="AE149" s="48"/>
+      <c r="AF149" s="48"/>
+      <c r="AG149" s="48"/>
+      <c r="AH149" s="48"/>
+      <c r="AI149" s="48"/>
+      <c r="AJ149" s="48"/>
+      <c r="AK149" s="48"/>
+      <c r="AL149" s="48"/>
+      <c r="AM149" s="48"/>
+      <c r="AN149" s="48"/>
+      <c r="AO149" s="48"/>
+      <c r="AP149" s="48"/>
+      <c r="AQ149" s="48"/>
+      <c r="AR149" s="48"/>
+      <c r="AS149" s="48"/>
+      <c r="AT149" s="48"/>
+      <c r="AU149" s="48"/>
+      <c r="AV149" s="48"/>
+      <c r="AW149" s="48"/>
+      <c r="AX149" s="48"/>
+      <c r="AY149" s="48"/>
+      <c r="AZ149" s="48"/>
+      <c r="BA149" s="48"/>
+      <c r="BB149" s="48"/>
+      <c r="BC149" s="48"/>
+      <c r="BD149" s="48"/>
+      <c r="BE149" s="48"/>
+      <c r="BF149" s="48"/>
+      <c r="BG149" s="48"/>
+      <c r="BH149" s="48"/>
+      <c r="BI149" s="48"/>
+      <c r="BJ149" s="48"/>
+      <c r="BK149" s="48"/>
+      <c r="BL149" s="48"/>
+      <c r="BM149" s="48"/>
+      <c r="BN149" s="48"/>
+      <c r="BO149" s="48"/>
     </row>
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.3</v>
+        <v>13.1</v>
       </c>
       <c r="B150" s="65" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D150" s="70"/>
       <c r="E150" s="66" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F150" s="42">
         <v>44379</v>
@@ -15966,14 +15980,14 @@
     <row r="151" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.4</v>
+        <v>13.2</v>
       </c>
       <c r="B151" s="65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D151" s="70"/>
       <c r="E151" s="66" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F151" s="42">
         <v>44379</v>
@@ -16043,17 +16057,17 @@
     <row r="152" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B152" s="77" t="s">
-        <v>110</v>
-      </c>
-      <c r="D152" s="66"/>
+        <v>13.3</v>
+      </c>
+      <c r="B152" s="65" t="s">
+        <v>108</v>
+      </c>
+      <c r="D152" s="70"/>
       <c r="E152" s="66" t="s">
         <v>67</v>
       </c>
       <c r="F152" s="42">
-        <v>44531</v>
+        <v>44379</v>
       </c>
       <c r="G152" s="43"/>
       <c r="H152" s="25"/>
@@ -16118,11 +16132,20 @@
       <c r="BO152" s="46"/>
     </row>
     <row r="153" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="23"/>
-      <c r="B153" s="65"/>
-      <c r="D153" s="66"/>
-      <c r="E153" s="66"/>
-      <c r="F153" s="42"/>
+      <c r="A153" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.4</v>
+      </c>
+      <c r="B153" s="65" t="s">
+        <v>109</v>
+      </c>
+      <c r="D153" s="70"/>
+      <c r="E153" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F153" s="42">
+        <v>44379</v>
+      </c>
       <c r="G153" s="43"/>
       <c r="H153" s="25"/>
       <c r="I153" s="26"/>
@@ -16186,11 +16209,20 @@
       <c r="BO153" s="46"/>
     </row>
     <row r="154" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="23"/>
-      <c r="B154" s="65"/>
+      <c r="A154" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>13.5</v>
+      </c>
+      <c r="B154" s="77" t="s">
+        <v>110</v>
+      </c>
       <c r="D154" s="66"/>
-      <c r="E154" s="66"/>
-      <c r="F154" s="42"/>
+      <c r="E154" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="F154" s="42">
+        <v>44531</v>
+      </c>
       <c r="G154" s="43"/>
       <c r="H154" s="25"/>
       <c r="I154" s="26"/>
@@ -16324,7 +16356,7 @@
     <row r="156" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="23"/>
       <c r="B156" s="65"/>
-      <c r="D156" s="70"/>
+      <c r="D156" s="66"/>
       <c r="E156" s="66"/>
       <c r="F156" s="42"/>
       <c r="G156" s="43"/>
@@ -16392,7 +16424,7 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23"/>
       <c r="B157" s="65"/>
-      <c r="D157" s="70"/>
+      <c r="D157" s="66"/>
       <c r="E157" s="66"/>
       <c r="F157" s="42"/>
       <c r="G157" s="43"/>
@@ -16664,7 +16696,7 @@
     <row r="161" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="23"/>
       <c r="B161" s="65"/>
-      <c r="D161" s="66"/>
+      <c r="D161" s="70"/>
       <c r="E161" s="66"/>
       <c r="F161" s="42"/>
       <c r="G161" s="43"/>
@@ -16732,7 +16764,7 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23"/>
       <c r="B162" s="65"/>
-      <c r="D162" s="66"/>
+      <c r="D162" s="70"/>
       <c r="E162" s="66"/>
       <c r="F162" s="42"/>
       <c r="G162" s="43"/>
@@ -16936,7 +16968,7 @@
     <row r="165" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="23"/>
       <c r="B165" s="65"/>
-      <c r="D165" s="70"/>
+      <c r="D165" s="66"/>
       <c r="E165" s="66"/>
       <c r="F165" s="42"/>
       <c r="G165" s="43"/>
@@ -17004,7 +17036,7 @@
     <row r="166" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23"/>
       <c r="B166" s="65"/>
-      <c r="D166" s="70"/>
+      <c r="D166" s="66"/>
       <c r="E166" s="66"/>
       <c r="F166" s="42"/>
       <c r="G166" s="43"/>
@@ -17276,7 +17308,7 @@
     <row r="170" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="23"/>
       <c r="B170" s="65"/>
-      <c r="D170" s="66"/>
+      <c r="D170" s="70"/>
       <c r="E170" s="66"/>
       <c r="F170" s="42"/>
       <c r="G170" s="43"/>
@@ -17344,7 +17376,7 @@
     <row r="171" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="23"/>
       <c r="B171" s="65"/>
-      <c r="D171" s="66"/>
+      <c r="D171" s="70"/>
       <c r="E171" s="66"/>
       <c r="F171" s="42"/>
       <c r="G171" s="43"/>
@@ -17548,7 +17580,7 @@
     <row r="174" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="23"/>
       <c r="B174" s="65"/>
-      <c r="D174" s="70"/>
+      <c r="D174" s="66"/>
       <c r="E174" s="66"/>
       <c r="F174" s="42"/>
       <c r="G174" s="43"/>
@@ -17616,7 +17648,7 @@
     <row r="175" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="23"/>
       <c r="B175" s="65"/>
-      <c r="D175" s="70"/>
+      <c r="D175" s="66"/>
       <c r="E175" s="66"/>
       <c r="F175" s="42"/>
       <c r="G175" s="43"/>
@@ -17888,7 +17920,7 @@
     <row r="179" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="23"/>
       <c r="B179" s="65"/>
-      <c r="D179" s="66"/>
+      <c r="D179" s="70"/>
       <c r="E179" s="66"/>
       <c r="F179" s="42"/>
       <c r="G179" s="43"/>
@@ -17956,7 +17988,7 @@
     <row r="180" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="23"/>
       <c r="B180" s="65"/>
-      <c r="D180" s="66"/>
+      <c r="D180" s="70"/>
       <c r="E180" s="66"/>
       <c r="F180" s="42"/>
       <c r="G180" s="43"/>
@@ -18160,7 +18192,7 @@
     <row r="183" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="23"/>
       <c r="B183" s="65"/>
-      <c r="D183" s="70"/>
+      <c r="D183" s="66"/>
       <c r="E183" s="66"/>
       <c r="F183" s="42"/>
       <c r="G183" s="43"/>
@@ -18228,7 +18260,7 @@
     <row r="184" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="23"/>
       <c r="B184" s="65"/>
-      <c r="D184" s="70"/>
+      <c r="D184" s="66"/>
       <c r="E184" s="66"/>
       <c r="F184" s="42"/>
       <c r="G184" s="43"/>
@@ -18497,18 +18529,145 @@
       <c r="BN187" s="46"/>
       <c r="BO187" s="46"/>
     </row>
+    <row r="188" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="23"/>
+      <c r="B188" s="65"/>
+      <c r="D188" s="70"/>
+      <c r="E188" s="66"/>
+      <c r="F188" s="42"/>
+      <c r="G188" s="43"/>
+      <c r="H188" s="25"/>
+      <c r="I188" s="26"/>
+      <c r="J188" s="27"/>
+      <c r="K188" s="40"/>
+      <c r="L188" s="46"/>
+      <c r="M188" s="46"/>
+      <c r="N188" s="46"/>
+      <c r="O188" s="46"/>
+      <c r="P188" s="46"/>
+      <c r="Q188" s="46"/>
+      <c r="R188" s="46"/>
+      <c r="S188" s="46"/>
+      <c r="T188" s="46"/>
+      <c r="U188" s="46"/>
+      <c r="V188" s="46"/>
+      <c r="W188" s="46"/>
+      <c r="X188" s="46"/>
+      <c r="Y188" s="46"/>
+      <c r="Z188" s="46"/>
+      <c r="AA188" s="46"/>
+      <c r="AB188" s="46"/>
+      <c r="AC188" s="46"/>
+      <c r="AD188" s="46"/>
+      <c r="AE188" s="46"/>
+      <c r="AF188" s="46"/>
+      <c r="AG188" s="46"/>
+      <c r="AH188" s="46"/>
+      <c r="AI188" s="46"/>
+      <c r="AJ188" s="46"/>
+      <c r="AK188" s="46"/>
+      <c r="AL188" s="46"/>
+      <c r="AM188" s="46"/>
+      <c r="AN188" s="46"/>
+      <c r="AO188" s="46"/>
+      <c r="AP188" s="46"/>
+      <c r="AQ188" s="46"/>
+      <c r="AR188" s="46"/>
+      <c r="AS188" s="46"/>
+      <c r="AT188" s="46"/>
+      <c r="AU188" s="46"/>
+      <c r="AV188" s="46"/>
+      <c r="AW188" s="46"/>
+      <c r="AX188" s="46"/>
+      <c r="AY188" s="46"/>
+      <c r="AZ188" s="46"/>
+      <c r="BA188" s="46"/>
+      <c r="BB188" s="46"/>
+      <c r="BC188" s="46"/>
+      <c r="BD188" s="46"/>
+      <c r="BE188" s="46"/>
+      <c r="BF188" s="46"/>
+      <c r="BG188" s="46"/>
+      <c r="BH188" s="46"/>
+      <c r="BI188" s="46"/>
+      <c r="BJ188" s="46"/>
+      <c r="BK188" s="46"/>
+      <c r="BL188" s="46"/>
+      <c r="BM188" s="46"/>
+      <c r="BN188" s="46"/>
+      <c r="BO188" s="46"/>
+    </row>
+    <row r="189" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="23"/>
+      <c r="B189" s="65"/>
+      <c r="D189" s="70"/>
+      <c r="E189" s="66"/>
+      <c r="F189" s="42"/>
+      <c r="G189" s="43"/>
+      <c r="H189" s="25"/>
+      <c r="I189" s="26"/>
+      <c r="J189" s="27"/>
+      <c r="K189" s="40"/>
+      <c r="L189" s="46"/>
+      <c r="M189" s="46"/>
+      <c r="N189" s="46"/>
+      <c r="O189" s="46"/>
+      <c r="P189" s="46"/>
+      <c r="Q189" s="46"/>
+      <c r="R189" s="46"/>
+      <c r="S189" s="46"/>
+      <c r="T189" s="46"/>
+      <c r="U189" s="46"/>
+      <c r="V189" s="46"/>
+      <c r="W189" s="46"/>
+      <c r="X189" s="46"/>
+      <c r="Y189" s="46"/>
+      <c r="Z189" s="46"/>
+      <c r="AA189" s="46"/>
+      <c r="AB189" s="46"/>
+      <c r="AC189" s="46"/>
+      <c r="AD189" s="46"/>
+      <c r="AE189" s="46"/>
+      <c r="AF189" s="46"/>
+      <c r="AG189" s="46"/>
+      <c r="AH189" s="46"/>
+      <c r="AI189" s="46"/>
+      <c r="AJ189" s="46"/>
+      <c r="AK189" s="46"/>
+      <c r="AL189" s="46"/>
+      <c r="AM189" s="46"/>
+      <c r="AN189" s="46"/>
+      <c r="AO189" s="46"/>
+      <c r="AP189" s="46"/>
+      <c r="AQ189" s="46"/>
+      <c r="AR189" s="46"/>
+      <c r="AS189" s="46"/>
+      <c r="AT189" s="46"/>
+      <c r="AU189" s="46"/>
+      <c r="AV189" s="46"/>
+      <c r="AW189" s="46"/>
+      <c r="AX189" s="46"/>
+      <c r="AY189" s="46"/>
+      <c r="AZ189" s="46"/>
+      <c r="BA189" s="46"/>
+      <c r="BB189" s="46"/>
+      <c r="BC189" s="46"/>
+      <c r="BD189" s="46"/>
+      <c r="BE189" s="46"/>
+      <c r="BF189" s="46"/>
+      <c r="BG189" s="46"/>
+      <c r="BH189" s="46"/>
+      <c r="BI189" s="46"/>
+      <c r="BJ189" s="46"/>
+      <c r="BK189" s="46"/>
+      <c r="BL189" s="46"/>
+      <c r="BM189" s="46"/>
+      <c r="BN189" s="46"/>
+      <c r="BO189" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -18519,9 +18678,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I148:I151 I98:I103 I105:I110 I112:I122 I124:I146">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I150:I153 I98:I103 I105:I110 I112:I122 I124:I148">
     <cfRule type="dataBar" priority="247">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18540,7 +18708,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 M124:BN146 L152:BO154 M155:BN160 BO158:BO160 L161:BO163 M164:BN169 BO167:BO169 L170:BO172 M173:BN178 BO176:BO178 L179:BO181 M182:BN187 BO185:BO187 BO150:BO151 M148:BN151 L147:BO147 L123:BO123">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN148 L154:BO156 M157:BN162 BO160:BO162 L163:BO165 M166:BN171 BO169:BO171 L172:BO174 M175:BN180 BO178:BO180 L181:BO183 M184:BN189 BO187:BO189 BO152:BO153 M150:BN153 L149:BO149">
     <cfRule type="expression" dxfId="132" priority="293">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -18548,7 +18716,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L148:BO151 L98:BO103 L105:BO110 L112:BO122 L124:BO146">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L150:BO153 L98:BO103 L105:BO110 L112:BO122 L124:BO148">
     <cfRule type="expression" dxfId="130" priority="253">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -18558,7 +18726,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E188:E1048576 E95:E96 E148:E151 E98:E103 E105:E110 E112:E122 E124:E146">
+  <conditionalFormatting sqref="E1:E73 E190:E1048576 E95:E96 E150:E153 E98:E103 E105:E110 E112:E122 E124:E148">
     <cfRule type="cellIs" dxfId="128" priority="234" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18652,7 +18820,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I152:I160">
+  <conditionalFormatting sqref="I154:I162">
     <cfRule type="dataBar" priority="138">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18666,12 +18834,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L152:BO160">
+  <conditionalFormatting sqref="L154:BO162">
     <cfRule type="expression" dxfId="106" priority="137">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E152:E160">
+  <conditionalFormatting sqref="E154:E162">
     <cfRule type="cellIs" dxfId="105" priority="130" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18694,7 +18862,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L155:BO160 L148:BO151 L98:BO103 L105:BO110 L112:BO122 L124:BO146">
+  <conditionalFormatting sqref="L157:BO162 L150:BO153 L98:BO103 L105:BO110 L112:BO122 L124:BO148">
     <cfRule type="expression" dxfId="98" priority="141">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18702,7 +18870,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I161:I169">
+  <conditionalFormatting sqref="I163:I171">
     <cfRule type="dataBar" priority="125">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18716,12 +18884,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L161:BO169">
+  <conditionalFormatting sqref="L163:BO171">
     <cfRule type="expression" dxfId="96" priority="124">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E161:E169">
+  <conditionalFormatting sqref="E163:E171">
     <cfRule type="cellIs" dxfId="95" priority="117" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18744,7 +18912,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L164:BO169">
+  <conditionalFormatting sqref="L166:BO171">
     <cfRule type="expression" dxfId="88" priority="128">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18752,7 +18920,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I170:I178">
+  <conditionalFormatting sqref="I172:I180">
     <cfRule type="dataBar" priority="112">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18766,12 +18934,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L170:BO178">
+  <conditionalFormatting sqref="L172:BO180">
     <cfRule type="expression" dxfId="86" priority="111">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E170:E178">
+  <conditionalFormatting sqref="E172:E180">
     <cfRule type="cellIs" dxfId="85" priority="104" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18794,7 +18962,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L173:BO178">
+  <conditionalFormatting sqref="L175:BO180">
     <cfRule type="expression" dxfId="78" priority="115">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18802,7 +18970,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I179:I187">
+  <conditionalFormatting sqref="I181:I189">
     <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18816,12 +18984,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L179:BO187">
+  <conditionalFormatting sqref="L181:BO189">
     <cfRule type="expression" dxfId="76" priority="98">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E179:E187">
+  <conditionalFormatting sqref="E181:E189">
     <cfRule type="cellIs" dxfId="75" priority="91" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18844,7 +19012,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L182:BO187">
+  <conditionalFormatting sqref="L184:BO189">
     <cfRule type="expression" dxfId="68" priority="102">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -18994,7 +19162,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I147">
+  <conditionalFormatting sqref="I149">
     <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19008,12 +19176,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L147:BO147">
+  <conditionalFormatting sqref="L149:BO149">
     <cfRule type="expression" dxfId="38" priority="52">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E147">
+  <conditionalFormatting sqref="E149">
     <cfRule type="cellIs" dxfId="37" priority="45" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19234,7 +19402,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I148:I151 I98:I103 I105:I110 I112:I122 I124:I146</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I150:I153 I98:I103 I105:I110 I112:I122 I124:I148</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -19264,7 +19432,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I152:I160</xm:sqref>
+          <xm:sqref>I154:I162</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BE7EDBFF-F2C7-44BF-B90F-771A4AD5A3F0}">
@@ -19279,7 +19447,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I161:I169</xm:sqref>
+          <xm:sqref>I163:I171</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -19294,7 +19462,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I170:I178</xm:sqref>
+          <xm:sqref>I172:I180</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -19309,7 +19477,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I179:I187</xm:sqref>
+          <xm:sqref>I181:I189</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -19369,7 +19537,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I147</xm:sqref>
+          <xm:sqref>I149</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A4E2E746-60FD-494C-9AA4-8453C3BBE609}">

</xml_diff>

<commit_message>
Added test topological map (v0.18)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C82261-6D32-4FDD-9F18-43507B2F9E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B0B003-0709-4608-9029-687F05633816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1847,6 +1847,13 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1856,6 +1863,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1864,17 +1875,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3391,8 +3391,8 @@
   <dimension ref="A1:BO181"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I144" sqref="I144"/>
+      <pane ySplit="7" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3422,27 +3422,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3487,12 +3487,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="82">
         <v>44192</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3502,183 +3502,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="77" t="str">
+      <c r="L4" s="79" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 49</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="77" t="str">
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="79" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 50</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="77" t="str">
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="79" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 51</v>
       </c>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="78"/>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="77" t="str">
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="80"/>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="79" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 52</v>
       </c>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="78"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="77" t="str">
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="79" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="77" t="str">
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="80"/>
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="81"/>
+      <c r="AU4" s="79" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="78"/>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="77" t="str">
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="79" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="78"/>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="77" t="str">
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="80"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="79" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="78"/>
-      <c r="BM4" s="78"/>
-      <c r="BN4" s="78"/>
-      <c r="BO4" s="79"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="80"/>
+      <c r="BM4" s="80"/>
+      <c r="BN4" s="80"/>
+      <c r="BO4" s="81"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="80">
+      <c r="L5" s="83">
         <f>L6</f>
         <v>44529</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="80">
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="83">
         <f>S6</f>
         <v>44536</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="80">
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="83">
         <f>Z6</f>
         <v>44543</v>
       </c>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="82"/>
-      <c r="AG5" s="80">
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="84"/>
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="84"/>
+      <c r="AE5" s="84"/>
+      <c r="AF5" s="85"/>
+      <c r="AG5" s="83">
         <f>AG6</f>
         <v>44550</v>
       </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="82"/>
-      <c r="AN5" s="80">
+      <c r="AH5" s="84"/>
+      <c r="AI5" s="84"/>
+      <c r="AJ5" s="84"/>
+      <c r="AK5" s="84"/>
+      <c r="AL5" s="84"/>
+      <c r="AM5" s="85"/>
+      <c r="AN5" s="83">
         <f>AN6</f>
         <v>44557</v>
       </c>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AT5" s="82"/>
-      <c r="AU5" s="80">
+      <c r="AO5" s="84"/>
+      <c r="AP5" s="84"/>
+      <c r="AQ5" s="84"/>
+      <c r="AR5" s="84"/>
+      <c r="AS5" s="84"/>
+      <c r="AT5" s="85"/>
+      <c r="AU5" s="83">
         <f>AU6</f>
         <v>44564</v>
       </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="82"/>
-      <c r="BB5" s="80">
+      <c r="AV5" s="84"/>
+      <c r="AW5" s="84"/>
+      <c r="AX5" s="84"/>
+      <c r="AY5" s="84"/>
+      <c r="AZ5" s="84"/>
+      <c r="BA5" s="85"/>
+      <c r="BB5" s="83">
         <f>BB6</f>
         <v>44571</v>
       </c>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BH5" s="82"/>
-      <c r="BI5" s="80">
+      <c r="BC5" s="84"/>
+      <c r="BD5" s="84"/>
+      <c r="BE5" s="84"/>
+      <c r="BF5" s="84"/>
+      <c r="BG5" s="84"/>
+      <c r="BH5" s="85"/>
+      <c r="BI5" s="83">
         <f>BI6</f>
         <v>44578</v>
       </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="82"/>
+      <c r="BJ5" s="84"/>
+      <c r="BK5" s="84"/>
+      <c r="BL5" s="84"/>
+      <c r="BM5" s="84"/>
+      <c r="BN5" s="84"/>
+      <c r="BO5" s="85"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -14620,11 +14620,11 @@
         <v>44529</v>
       </c>
       <c r="G135" s="43">
-        <v>44530</v>
+        <v>44531</v>
       </c>
       <c r="H135" s="73"/>
       <c r="I135" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J135" s="75"/>
       <c r="K135" s="76"/>
@@ -14701,11 +14701,11 @@
         <v>44529</v>
       </c>
       <c r="G136" s="43">
-        <v>44530</v>
+        <v>44531</v>
       </c>
       <c r="H136" s="73"/>
       <c r="I136" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J136" s="75"/>
       <c r="K136" s="76"/>
@@ -14779,7 +14779,7 @@
         <v>66</v>
       </c>
       <c r="F137" s="42">
-        <v>44529</v>
+        <v>44530</v>
       </c>
       <c r="G137" s="43">
         <v>44534</v>
@@ -14860,7 +14860,7 @@
         <v>66</v>
       </c>
       <c r="F138" s="42">
-        <v>44529</v>
+        <v>44530</v>
       </c>
       <c r="G138" s="43">
         <v>44534</v>
@@ -14941,10 +14941,10 @@
         <v>152</v>
       </c>
       <c r="F139" s="42">
-        <v>44530</v>
+        <v>44531</v>
       </c>
       <c r="G139" s="43">
-        <v>44534</v>
+        <v>44535</v>
       </c>
       <c r="H139" s="73"/>
       <c r="I139" s="26">
@@ -17972,15 +17972,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -17991,6 +17982,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I154">

</xml_diff>

<commit_message>
Removed FRED pulls from expected inflation (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B0B003-0709-4608-9029-687F05633816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7287059F-145F-4BE2-A082-D7FDE19D5DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="168">
   <si>
     <t>WBS</t>
   </si>
@@ -877,9 +877,6 @@
     <t>Model Prod (v0.17)</t>
   </si>
   <si>
-    <t>Vintage Analysis, Structural Overhaul, Website Overhaul (v0.18)</t>
-  </si>
-  <si>
     <t>Clean Folder, Improve Devops Flow</t>
   </si>
   <si>
@@ -929,6 +926,12 @@
   </si>
   <si>
     <t>Release CMEFI Structural Models On Site</t>
+  </si>
+  <si>
+    <t>Overhaul Prep (v0.18)</t>
+  </si>
+  <si>
+    <t>Vintage Analysis, Structural Overhaul, Website Overhaul (v0.19)</t>
   </si>
 </sst>
 </file>
@@ -1923,7 +1926,82 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="128">
+  <dxfs count="138">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -2981,7 +3059,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="49"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="52"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3388,10 +3466,10 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO181"/>
+  <dimension ref="A1:BO182"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G140" sqref="G140"/>
     </sheetView>
   </sheetViews>
@@ -3498,13 +3576,13 @@
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
       <c r="L4" s="79" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 49</v>
+        <v>Week 52</v>
       </c>
       <c r="M4" s="80"/>
       <c r="N4" s="80"/>
@@ -3514,7 +3592,7 @@
       <c r="R4" s="81"/>
       <c r="S4" s="79" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 50</v>
+        <v>Week 53</v>
       </c>
       <c r="T4" s="80"/>
       <c r="U4" s="80"/>
@@ -3524,7 +3602,7 @@
       <c r="Y4" s="81"/>
       <c r="Z4" s="79" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 51</v>
+        <v>Week 54</v>
       </c>
       <c r="AA4" s="80"/>
       <c r="AB4" s="80"/>
@@ -3534,7 +3612,7 @@
       <c r="AF4" s="81"/>
       <c r="AG4" s="79" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 52</v>
+        <v>Week 55</v>
       </c>
       <c r="AH4" s="80"/>
       <c r="AI4" s="80"/>
@@ -3544,7 +3622,7 @@
       <c r="AM4" s="81"/>
       <c r="AN4" s="79" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 53</v>
+        <v>Week 56</v>
       </c>
       <c r="AO4" s="80"/>
       <c r="AP4" s="80"/>
@@ -3554,7 +3632,7 @@
       <c r="AT4" s="81"/>
       <c r="AU4" s="79" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 54</v>
+        <v>Week 57</v>
       </c>
       <c r="AV4" s="80"/>
       <c r="AW4" s="80"/>
@@ -3564,7 +3642,7 @@
       <c r="BA4" s="81"/>
       <c r="BB4" s="79" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 55</v>
+        <v>Week 58</v>
       </c>
       <c r="BC4" s="80"/>
       <c r="BD4" s="80"/>
@@ -3574,7 +3652,7 @@
       <c r="BH4" s="81"/>
       <c r="BI4" s="79" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 56</v>
+        <v>Week 59</v>
       </c>
       <c r="BJ4" s="80"/>
       <c r="BK4" s="80"/>
@@ -3601,7 +3679,7 @@
       <c r="K5" s="13"/>
       <c r="L5" s="83">
         <f>L6</f>
-        <v>44529</v>
+        <v>44550</v>
       </c>
       <c r="M5" s="84"/>
       <c r="N5" s="84"/>
@@ -3611,7 +3689,7 @@
       <c r="R5" s="85"/>
       <c r="S5" s="83">
         <f>S6</f>
-        <v>44536</v>
+        <v>44557</v>
       </c>
       <c r="T5" s="84"/>
       <c r="U5" s="84"/>
@@ -3621,7 +3699,7 @@
       <c r="Y5" s="85"/>
       <c r="Z5" s="83">
         <f>Z6</f>
-        <v>44543</v>
+        <v>44564</v>
       </c>
       <c r="AA5" s="84"/>
       <c r="AB5" s="84"/>
@@ -3631,7 +3709,7 @@
       <c r="AF5" s="85"/>
       <c r="AG5" s="83">
         <f>AG6</f>
-        <v>44550</v>
+        <v>44571</v>
       </c>
       <c r="AH5" s="84"/>
       <c r="AI5" s="84"/>
@@ -3641,7 +3719,7 @@
       <c r="AM5" s="85"/>
       <c r="AN5" s="83">
         <f>AN6</f>
-        <v>44557</v>
+        <v>44578</v>
       </c>
       <c r="AO5" s="84"/>
       <c r="AP5" s="84"/>
@@ -3651,7 +3729,7 @@
       <c r="AT5" s="85"/>
       <c r="AU5" s="83">
         <f>AU6</f>
-        <v>44564</v>
+        <v>44585</v>
       </c>
       <c r="AV5" s="84"/>
       <c r="AW5" s="84"/>
@@ -3661,7 +3739,7 @@
       <c r="BA5" s="85"/>
       <c r="BB5" s="83">
         <f>BB6</f>
-        <v>44571</v>
+        <v>44592</v>
       </c>
       <c r="BC5" s="84"/>
       <c r="BD5" s="84"/>
@@ -3671,7 +3749,7 @@
       <c r="BH5" s="85"/>
       <c r="BI5" s="83">
         <f>BI6</f>
-        <v>44578</v>
+        <v>44599</v>
       </c>
       <c r="BJ5" s="84"/>
       <c r="BK5" s="84"/>
@@ -3694,227 +3772,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44529</v>
+        <v>44550</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44530</v>
+        <v>44551</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44531</v>
+        <v>44552</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44532</v>
+        <v>44553</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44533</v>
+        <v>44554</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44534</v>
+        <v>44555</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44535</v>
+        <v>44556</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44536</v>
+        <v>44557</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44537</v>
+        <v>44558</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44538</v>
+        <v>44559</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44539</v>
+        <v>44560</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44540</v>
+        <v>44561</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44541</v>
+        <v>44562</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44542</v>
+        <v>44563</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44543</v>
+        <v>44564</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44544</v>
+        <v>44565</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44545</v>
+        <v>44566</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44546</v>
+        <v>44567</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44547</v>
+        <v>44568</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44548</v>
+        <v>44569</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44549</v>
+        <v>44570</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44550</v>
+        <v>44571</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44551</v>
+        <v>44572</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44552</v>
+        <v>44573</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44553</v>
+        <v>44574</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44554</v>
+        <v>44575</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44555</v>
+        <v>44576</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44556</v>
+        <v>44577</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44557</v>
+        <v>44578</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44558</v>
+        <v>44579</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44559</v>
+        <v>44580</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44560</v>
+        <v>44581</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44561</v>
+        <v>44582</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44562</v>
+        <v>44583</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44563</v>
+        <v>44584</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44564</v>
+        <v>44585</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44565</v>
+        <v>44586</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44566</v>
+        <v>44587</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44567</v>
+        <v>44588</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44568</v>
+        <v>44589</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44569</v>
+        <v>44590</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44570</v>
+        <v>44591</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44571</v>
+        <v>44592</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44572</v>
+        <v>44593</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44573</v>
+        <v>44594</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44574</v>
+        <v>44595</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44575</v>
+        <v>44596</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44576</v>
+        <v>44597</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44577</v>
+        <v>44598</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44578</v>
+        <v>44599</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44579</v>
+        <v>44600</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44580</v>
+        <v>44601</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44581</v>
+        <v>44602</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44582</v>
+        <v>44603</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44583</v>
+        <v>44604</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44584</v>
+        <v>44605</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -8836,7 +8914,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A147" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A148" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -10167,7 +10245,7 @@
       </c>
       <c r="D80" s="70"/>
       <c r="E80" s="66" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F80" s="42">
         <v>44249</v>
@@ -12433,7 +12511,7 @@
       </c>
       <c r="D108" s="70"/>
       <c r="E108" s="66" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F108" s="42">
         <v>44383</v>
@@ -14369,7 +14447,7 @@
         <v>13</v>
       </c>
       <c r="B132" s="17" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="D132" s="19"/>
       <c r="E132" s="19"/>
@@ -14448,7 +14526,7 @@
         <v>13.1</v>
       </c>
       <c r="B133" s="65" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D133" s="70"/>
       <c r="E133" s="66" t="s">
@@ -14529,7 +14607,7 @@
         <v>13.2</v>
       </c>
       <c r="B134" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D134" s="70"/>
       <c r="E134" s="66" t="s">
@@ -14610,7 +14688,7 @@
         <v>13.3</v>
       </c>
       <c r="B135" s="65" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D135" s="70"/>
       <c r="E135" s="66" t="s">
@@ -14691,17 +14769,17 @@
         <v>13.4</v>
       </c>
       <c r="B136" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D136" s="70"/>
       <c r="E136" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F136" s="42">
-        <v>44529</v>
+        <v>44538</v>
       </c>
       <c r="G136" s="43">
-        <v>44531</v>
+        <v>44539</v>
       </c>
       <c r="H136" s="73"/>
       <c r="I136" s="26">
@@ -14766,91 +14844,89 @@
       <c r="BN136" s="46"/>
       <c r="BO136" s="46"/>
     </row>
-    <row r="137" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>13.5</v>
-      </c>
-      <c r="B137" s="65" t="s">
-        <v>161</v>
-      </c>
-      <c r="D137" s="70"/>
-      <c r="E137" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="F137" s="42">
-        <v>44530</v>
-      </c>
-      <c r="G137" s="43">
-        <v>44534</v>
-      </c>
-      <c r="H137" s="73"/>
-      <c r="I137" s="26">
-        <v>0.2</v>
-      </c>
-      <c r="J137" s="75"/>
-      <c r="K137" s="76"/>
-      <c r="L137" s="46"/>
-      <c r="M137" s="46"/>
-      <c r="N137" s="46"/>
-      <c r="O137" s="46"/>
-      <c r="P137" s="46"/>
-      <c r="Q137" s="46"/>
-      <c r="R137" s="46"/>
-      <c r="S137" s="46"/>
-      <c r="T137" s="46"/>
-      <c r="U137" s="46"/>
-      <c r="V137" s="46"/>
-      <c r="W137" s="46"/>
-      <c r="X137" s="46"/>
-      <c r="Y137" s="46"/>
-      <c r="Z137" s="46"/>
-      <c r="AA137" s="46"/>
-      <c r="AB137" s="46"/>
-      <c r="AC137" s="46"/>
-      <c r="AD137" s="46"/>
-      <c r="AE137" s="46"/>
-      <c r="AF137" s="46"/>
-      <c r="AG137" s="46"/>
-      <c r="AH137" s="46"/>
-      <c r="AI137" s="46"/>
-      <c r="AJ137" s="46"/>
-      <c r="AK137" s="46"/>
-      <c r="AL137" s="46"/>
-      <c r="AM137" s="46"/>
-      <c r="AN137" s="46"/>
-      <c r="AO137" s="46"/>
-      <c r="AP137" s="46"/>
-      <c r="AQ137" s="46"/>
-      <c r="AR137" s="46"/>
-      <c r="AS137" s="46"/>
-      <c r="AT137" s="46"/>
-      <c r="AU137" s="46"/>
-      <c r="AV137" s="46"/>
-      <c r="AW137" s="46"/>
-      <c r="AX137" s="46"/>
-      <c r="AY137" s="46"/>
-      <c r="AZ137" s="46"/>
-      <c r="BA137" s="46"/>
-      <c r="BB137" s="46"/>
-      <c r="BC137" s="46"/>
-      <c r="BD137" s="46"/>
-      <c r="BE137" s="46"/>
-      <c r="BF137" s="46"/>
-      <c r="BG137" s="46"/>
-      <c r="BH137" s="46"/>
-      <c r="BI137" s="46"/>
-      <c r="BJ137" s="46"/>
-      <c r="BK137" s="46"/>
-      <c r="BL137" s="46"/>
-      <c r="BM137" s="46"/>
-      <c r="BN137" s="46"/>
-      <c r="BO137" s="46"/>
+    <row r="137" spans="1:67" s="18" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="16" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>14</v>
+      </c>
+      <c r="B137" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D137" s="19"/>
+      <c r="E137" s="19"/>
+      <c r="F137" s="44"/>
+      <c r="G137" s="44" t="str">
+        <f t="shared" ref="G137" si="26">IF(ISBLANK(F137)," - ",IF(H137=0,F137,F137+H137-1))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="H137" s="20"/>
+      <c r="I137" s="21"/>
+      <c r="J137" s="22" t="str">
+        <f t="shared" ref="J137" si="27">IF(OR(G137=0,F137=0)," - ",NETWORKDAYS(F137,G137))</f>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="K137" s="41"/>
+      <c r="L137" s="48"/>
+      <c r="M137" s="48"/>
+      <c r="N137" s="48"/>
+      <c r="O137" s="48"/>
+      <c r="P137" s="48"/>
+      <c r="Q137" s="48"/>
+      <c r="R137" s="48"/>
+      <c r="S137" s="48"/>
+      <c r="T137" s="48"/>
+      <c r="U137" s="48"/>
+      <c r="V137" s="48"/>
+      <c r="W137" s="48"/>
+      <c r="X137" s="48"/>
+      <c r="Y137" s="48"/>
+      <c r="Z137" s="48"/>
+      <c r="AA137" s="48"/>
+      <c r="AB137" s="48"/>
+      <c r="AC137" s="48"/>
+      <c r="AD137" s="48"/>
+      <c r="AE137" s="48"/>
+      <c r="AF137" s="48"/>
+      <c r="AG137" s="48"/>
+      <c r="AH137" s="48"/>
+      <c r="AI137" s="48"/>
+      <c r="AJ137" s="48"/>
+      <c r="AK137" s="48"/>
+      <c r="AL137" s="48"/>
+      <c r="AM137" s="48"/>
+      <c r="AN137" s="48"/>
+      <c r="AO137" s="48"/>
+      <c r="AP137" s="48"/>
+      <c r="AQ137" s="48"/>
+      <c r="AR137" s="48"/>
+      <c r="AS137" s="48"/>
+      <c r="AT137" s="48"/>
+      <c r="AU137" s="48"/>
+      <c r="AV137" s="48"/>
+      <c r="AW137" s="48"/>
+      <c r="AX137" s="48"/>
+      <c r="AY137" s="48"/>
+      <c r="AZ137" s="48"/>
+      <c r="BA137" s="48"/>
+      <c r="BB137" s="48"/>
+      <c r="BC137" s="48"/>
+      <c r="BD137" s="48"/>
+      <c r="BE137" s="48"/>
+      <c r="BF137" s="48"/>
+      <c r="BG137" s="48"/>
+      <c r="BH137" s="48"/>
+      <c r="BI137" s="48"/>
+      <c r="BJ137" s="48"/>
+      <c r="BK137" s="48"/>
+      <c r="BL137" s="48"/>
+      <c r="BM137" s="48"/>
+      <c r="BN137" s="48"/>
+      <c r="BO137" s="48"/>
     </row>
     <row r="138" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.6</v>
+        <v>14.1</v>
       </c>
       <c r="B138" s="65" t="s">
         <v>160</v>
@@ -14860,14 +14936,14 @@
         <v>66</v>
       </c>
       <c r="F138" s="42">
-        <v>44530</v>
+        <v>44552</v>
       </c>
       <c r="G138" s="43">
-        <v>44534</v>
+        <v>44556</v>
       </c>
       <c r="H138" s="73"/>
       <c r="I138" s="26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J138" s="75"/>
       <c r="K138" s="76"/>
@@ -14931,20 +15007,20 @@
     <row r="139" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.7</v>
+        <v>14.2</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="D139" s="70"/>
       <c r="E139" s="66" t="s">
-        <v>152</v>
+        <v>66</v>
       </c>
       <c r="F139" s="42">
-        <v>44531</v>
+        <v>44551</v>
       </c>
       <c r="G139" s="43">
-        <v>44535</v>
+        <v>44556</v>
       </c>
       <c r="H139" s="73"/>
       <c r="I139" s="26">
@@ -15012,20 +15088,20 @@
     <row r="140" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.8</v>
+        <v>14.3</v>
       </c>
       <c r="B140" s="65" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="D140" s="70"/>
       <c r="E140" s="66" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="F140" s="42">
-        <v>44535</v>
+        <v>44551</v>
       </c>
       <c r="G140" s="43">
-        <v>44540</v>
+        <v>44556</v>
       </c>
       <c r="H140" s="73"/>
       <c r="I140" s="26">
@@ -15093,20 +15169,20 @@
     <row r="141" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.9</v>
+        <v>14.4</v>
       </c>
       <c r="B141" s="65" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D141" s="70"/>
       <c r="E141" s="66" t="s">
         <v>68</v>
       </c>
       <c r="F141" s="42">
-        <v>44535</v>
+        <v>44551</v>
       </c>
       <c r="G141" s="43">
-        <v>44540</v>
+        <v>44556</v>
       </c>
       <c r="H141" s="73"/>
       <c r="I141" s="26">
@@ -15174,20 +15250,20 @@
     <row r="142" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.10</v>
+        <v>14.5</v>
       </c>
       <c r="B142" s="65" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D142" s="70"/>
       <c r="E142" s="66" t="s">
         <v>68</v>
       </c>
       <c r="F142" s="42">
-        <v>44535</v>
+        <v>44551</v>
       </c>
       <c r="G142" s="43">
-        <v>44540</v>
+        <v>44556</v>
       </c>
       <c r="H142" s="73"/>
       <c r="I142" s="26">
@@ -15255,20 +15331,20 @@
     <row r="143" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.11</v>
+        <v>14.6</v>
       </c>
       <c r="B143" s="65" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D143" s="70"/>
       <c r="E143" s="66" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F143" s="42">
-        <v>44530</v>
+        <v>44551</v>
       </c>
       <c r="G143" s="43">
-        <v>44532</v>
+        <v>44556</v>
       </c>
       <c r="H143" s="73"/>
       <c r="I143" s="26">
@@ -15336,20 +15412,20 @@
     <row r="144" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.12</v>
+        <v>14.7</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D144" s="70"/>
       <c r="E144" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F144" s="42">
-        <v>44530</v>
+        <v>44551</v>
       </c>
       <c r="G144" s="43">
-        <v>44532</v>
+        <v>44556</v>
       </c>
       <c r="H144" s="73"/>
       <c r="I144" s="26">
@@ -15417,20 +15493,20 @@
     <row r="145" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.13</v>
+        <v>14.8</v>
       </c>
       <c r="B145" s="65" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="D145" s="70"/>
       <c r="E145" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F145" s="42">
-        <v>44520</v>
+        <v>44551</v>
       </c>
       <c r="G145" s="43">
-        <v>44525</v>
+        <v>44556</v>
       </c>
       <c r="H145" s="73"/>
       <c r="I145" s="26">
@@ -15498,23 +15574,23 @@
     <row r="146" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.14</v>
+        <v>14.9</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D146" s="70"/>
-      <c r="E146" s="70" t="s">
+      <c r="E146" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="F146" s="71">
-        <v>44520</v>
-      </c>
-      <c r="G146" s="72">
-        <v>44525</v>
+      <c r="F146" s="42">
+        <v>44551</v>
+      </c>
+      <c r="G146" s="43">
+        <v>44556</v>
       </c>
       <c r="H146" s="73"/>
-      <c r="I146" s="74">
+      <c r="I146" s="26">
         <v>0</v>
       </c>
       <c r="J146" s="75"/>
@@ -15579,27 +15655,27 @@
     <row r="147" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>13.15</v>
+        <v>14.10</v>
       </c>
       <c r="B147" s="65" t="s">
-        <v>156</v>
-      </c>
-      <c r="D147" s="66"/>
-      <c r="E147" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="D147" s="70"/>
+      <c r="E147" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="F147" s="42">
-        <v>44522</v>
-      </c>
-      <c r="G147" s="43">
-        <v>44526</v>
-      </c>
-      <c r="H147" s="25"/>
-      <c r="I147" s="26">
+      <c r="F147" s="71">
+        <v>44551</v>
+      </c>
+      <c r="G147" s="72">
+        <v>44556</v>
+      </c>
+      <c r="H147" s="73"/>
+      <c r="I147" s="74">
         <v>0</v>
       </c>
-      <c r="J147" s="27"/>
-      <c r="K147" s="40"/>
+      <c r="J147" s="75"/>
+      <c r="K147" s="76"/>
       <c r="L147" s="46"/>
       <c r="M147" s="46"/>
       <c r="N147" s="46"/>
@@ -15658,14 +15734,27 @@
       <c r="BO147" s="46"/>
     </row>
     <row r="148" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A148" s="23"/>
-      <c r="B148" s="65"/>
+      <c r="A148" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>14.11</v>
+      </c>
+      <c r="B148" s="65" t="s">
+        <v>155</v>
+      </c>
       <c r="D148" s="66"/>
-      <c r="E148" s="66"/>
-      <c r="F148" s="42"/>
-      <c r="G148" s="43"/>
+      <c r="E148" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F148" s="42">
+        <v>44551</v>
+      </c>
+      <c r="G148" s="43">
+        <v>44556</v>
+      </c>
       <c r="H148" s="25"/>
-      <c r="I148" s="26"/>
+      <c r="I148" s="26">
+        <v>0</v>
+      </c>
       <c r="J148" s="27"/>
       <c r="K148" s="40"/>
       <c r="L148" s="46"/>
@@ -15796,7 +15885,7 @@
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="23"/>
       <c r="B150" s="65"/>
-      <c r="D150" s="70"/>
+      <c r="D150" s="66"/>
       <c r="E150" s="66"/>
       <c r="F150" s="42"/>
       <c r="G150" s="43"/>
@@ -16136,7 +16225,7 @@
     <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="23"/>
       <c r="B155" s="65"/>
-      <c r="D155" s="66"/>
+      <c r="D155" s="70"/>
       <c r="E155" s="66"/>
       <c r="F155" s="42"/>
       <c r="G155" s="43"/>
@@ -16408,7 +16497,7 @@
     <row r="159" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="23"/>
       <c r="B159" s="65"/>
-      <c r="D159" s="70"/>
+      <c r="D159" s="66"/>
       <c r="E159" s="66"/>
       <c r="F159" s="42"/>
       <c r="G159" s="43"/>
@@ -16748,7 +16837,7 @@
     <row r="164" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="23"/>
       <c r="B164" s="65"/>
-      <c r="D164" s="66"/>
+      <c r="D164" s="70"/>
       <c r="E164" s="66"/>
       <c r="F164" s="42"/>
       <c r="G164" s="43"/>
@@ -17020,7 +17109,7 @@
     <row r="168" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="23"/>
       <c r="B168" s="65"/>
-      <c r="D168" s="70"/>
+      <c r="D168" s="66"/>
       <c r="E168" s="66"/>
       <c r="F168" s="42"/>
       <c r="G168" s="43"/>
@@ -17360,7 +17449,7 @@
     <row r="173" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="23"/>
       <c r="B173" s="65"/>
-      <c r="D173" s="66"/>
+      <c r="D173" s="70"/>
       <c r="E173" s="66"/>
       <c r="F173" s="42"/>
       <c r="G173" s="43"/>
@@ -17632,7 +17721,7 @@
     <row r="177" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="23"/>
       <c r="B177" s="65"/>
-      <c r="D177" s="70"/>
+      <c r="D177" s="66"/>
       <c r="E177" s="66"/>
       <c r="F177" s="42"/>
       <c r="G177" s="43"/>
@@ -17969,6 +18058,74 @@
       <c r="BN181" s="46"/>
       <c r="BO181" s="46"/>
     </row>
+    <row r="182" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="23"/>
+      <c r="B182" s="65"/>
+      <c r="D182" s="70"/>
+      <c r="E182" s="66"/>
+      <c r="F182" s="42"/>
+      <c r="G182" s="43"/>
+      <c r="H182" s="25"/>
+      <c r="I182" s="26"/>
+      <c r="J182" s="27"/>
+      <c r="K182" s="40"/>
+      <c r="L182" s="46"/>
+      <c r="M182" s="46"/>
+      <c r="N182" s="46"/>
+      <c r="O182" s="46"/>
+      <c r="P182" s="46"/>
+      <c r="Q182" s="46"/>
+      <c r="R182" s="46"/>
+      <c r="S182" s="46"/>
+      <c r="T182" s="46"/>
+      <c r="U182" s="46"/>
+      <c r="V182" s="46"/>
+      <c r="W182" s="46"/>
+      <c r="X182" s="46"/>
+      <c r="Y182" s="46"/>
+      <c r="Z182" s="46"/>
+      <c r="AA182" s="46"/>
+      <c r="AB182" s="46"/>
+      <c r="AC182" s="46"/>
+      <c r="AD182" s="46"/>
+      <c r="AE182" s="46"/>
+      <c r="AF182" s="46"/>
+      <c r="AG182" s="46"/>
+      <c r="AH182" s="46"/>
+      <c r="AI182" s="46"/>
+      <c r="AJ182" s="46"/>
+      <c r="AK182" s="46"/>
+      <c r="AL182" s="46"/>
+      <c r="AM182" s="46"/>
+      <c r="AN182" s="46"/>
+      <c r="AO182" s="46"/>
+      <c r="AP182" s="46"/>
+      <c r="AQ182" s="46"/>
+      <c r="AR182" s="46"/>
+      <c r="AS182" s="46"/>
+      <c r="AT182" s="46"/>
+      <c r="AU182" s="46"/>
+      <c r="AV182" s="46"/>
+      <c r="AW182" s="46"/>
+      <c r="AX182" s="46"/>
+      <c r="AY182" s="46"/>
+      <c r="AZ182" s="46"/>
+      <c r="BA182" s="46"/>
+      <c r="BB182" s="46"/>
+      <c r="BC182" s="46"/>
+      <c r="BD182" s="46"/>
+      <c r="BE182" s="46"/>
+      <c r="BF182" s="46"/>
+      <c r="BG182" s="46"/>
+      <c r="BH182" s="46"/>
+      <c r="BI182" s="46"/>
+      <c r="BJ182" s="46"/>
+      <c r="BK182" s="46"/>
+      <c r="BL182" s="46"/>
+      <c r="BM182" s="46"/>
+      <c r="BN182" s="46"/>
+      <c r="BO182" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
@@ -17993,8 +18150,8 @@
     <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I154">
-    <cfRule type="dataBar" priority="258">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I155">
+    <cfRule type="dataBar" priority="269">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18008,66 +18165,66 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6:BO7">
-    <cfRule type="expression" dxfId="127" priority="301">
+    <cfRule type="expression" dxfId="137" priority="312">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN131 M133:BN146 L147:BO148 M149:BN154 BO152:BO154 L155:BO157 M158:BN163 BO161:BO163 L164:BO166 M167:BN172 BO170:BO172 L173:BO175 M176:BN181 BO179:BO181">
-    <cfRule type="expression" dxfId="126" priority="304">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN131 M133:BN136 L148:BO149 M150:BN155 BO153:BO155 L156:BO158 M159:BN164 BO162:BO164 L165:BO167 M168:BN173 BO171:BO173 L174:BO176 M177:BN182 BO180:BO182 M138:BN147">
+    <cfRule type="expression" dxfId="136" priority="315">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="125" priority="305">
+    <cfRule type="expression" dxfId="135" priority="316">
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO154">
-    <cfRule type="expression" dxfId="124" priority="264">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO155">
+    <cfRule type="expression" dxfId="134" priority="275">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L63:BO73">
-    <cfRule type="expression" dxfId="123" priority="254">
+    <cfRule type="expression" dxfId="133" priority="265">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E182:E1048576 E95:E96 E98:E103 E105:E110 E112:E122 E124:E131 E133:E154">
-    <cfRule type="cellIs" dxfId="122" priority="245" operator="equal">
+  <conditionalFormatting sqref="E1:E73 E183:E1048576 E95:E96 E98:E103 E105:E110 E112:E122 E124:E131 E133:E136 E138:E155">
+    <cfRule type="cellIs" dxfId="132" priority="256" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="258" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="259" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="260" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="261" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="251" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="262" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="263" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="115" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="257" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L68:BO73">
-    <cfRule type="expression" dxfId="114" priority="310">
+    <cfRule type="expression" dxfId="124" priority="321">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="311">
+    <cfRule type="expression" dxfId="123" priority="322">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I74:I84">
-    <cfRule type="dataBar" priority="240">
+    <cfRule type="dataBar" priority="251">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18081,59 +18238,59 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO78">
-    <cfRule type="expression" dxfId="112" priority="241">
+    <cfRule type="expression" dxfId="122" priority="252">
       <formula>AND($F74&lt;=L$6,ROUNDDOWN(($G74-$F74+1)*$I74,0)+$F74-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="242">
+    <cfRule type="expression" dxfId="121" priority="253">
       <formula>AND(NOT(ISBLANK($F74)),$F74&lt;=L$6,$G74&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L74:BO84">
-    <cfRule type="expression" dxfId="110" priority="239">
+    <cfRule type="expression" dxfId="120" priority="250">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E74:E84">
-    <cfRule type="cellIs" dxfId="109" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="243" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="244" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="245" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="246" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="247" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="248" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="249" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L79:BO84">
-    <cfRule type="expression" dxfId="102" priority="243">
+    <cfRule type="expression" dxfId="112" priority="254">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="244">
+    <cfRule type="expression" dxfId="111" priority="255">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L149:BO154 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO146">
-    <cfRule type="expression" dxfId="100" priority="152">
+  <conditionalFormatting sqref="L150:BO155 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO147">
+    <cfRule type="expression" dxfId="110" priority="163">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="153">
+    <cfRule type="expression" dxfId="109" priority="164">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I155:I163">
-    <cfRule type="dataBar" priority="136">
+  <conditionalFormatting sqref="I156:I164">
+    <cfRule type="dataBar" priority="147">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18146,44 +18303,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L155:BO163">
-    <cfRule type="expression" dxfId="98" priority="135">
+  <conditionalFormatting sqref="L156:BO164">
+    <cfRule type="expression" dxfId="108" priority="146">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E155:E163">
-    <cfRule type="cellIs" dxfId="97" priority="128" operator="equal">
+  <conditionalFormatting sqref="E156:E164">
+    <cfRule type="cellIs" dxfId="107" priority="139" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="140" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="141" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="142" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="143" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="144" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="145" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L158:BO163">
-    <cfRule type="expression" dxfId="90" priority="139">
+  <conditionalFormatting sqref="L159:BO164">
+    <cfRule type="expression" dxfId="100" priority="150">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="89" priority="140">
+    <cfRule type="expression" dxfId="99" priority="151">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I164:I172">
-    <cfRule type="dataBar" priority="123">
+  <conditionalFormatting sqref="I165:I173">
+    <cfRule type="dataBar" priority="134">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18196,44 +18353,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L164:BO172">
-    <cfRule type="expression" dxfId="88" priority="122">
+  <conditionalFormatting sqref="L165:BO173">
+    <cfRule type="expression" dxfId="98" priority="133">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E164:E172">
-    <cfRule type="cellIs" dxfId="87" priority="115" operator="equal">
+  <conditionalFormatting sqref="E165:E173">
+    <cfRule type="cellIs" dxfId="97" priority="126" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="127" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="128" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="129" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="130" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="131" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="132" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L167:BO172">
-    <cfRule type="expression" dxfId="80" priority="126">
+  <conditionalFormatting sqref="L168:BO173">
+    <cfRule type="expression" dxfId="90" priority="137">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="127">
+    <cfRule type="expression" dxfId="89" priority="138">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I173:I181">
-    <cfRule type="dataBar" priority="110">
+  <conditionalFormatting sqref="I174:I182">
+    <cfRule type="dataBar" priority="121">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18246,44 +18403,44 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L173:BO181">
-    <cfRule type="expression" dxfId="78" priority="109">
+  <conditionalFormatting sqref="L174:BO182">
+    <cfRule type="expression" dxfId="88" priority="120">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E173:E181">
-    <cfRule type="cellIs" dxfId="77" priority="102" operator="equal">
+  <conditionalFormatting sqref="E174:E182">
+    <cfRule type="cellIs" dxfId="87" priority="113" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="114" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="115" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="116" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="117" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="118" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="119" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L176:BO181">
-    <cfRule type="expression" dxfId="70" priority="113">
+  <conditionalFormatting sqref="L177:BO182">
+    <cfRule type="expression" dxfId="80" priority="124">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="114">
+    <cfRule type="expression" dxfId="79" priority="125">
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I85:I86">
-    <cfRule type="dataBar" priority="97">
+    <cfRule type="dataBar" priority="108">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18297,11 +18454,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L85:BO86">
+    <cfRule type="expression" dxfId="78" priority="107">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E85:E86">
+    <cfRule type="cellIs" dxfId="77" priority="100" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="101" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="102" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="103" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="104" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="105" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="106" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
+    <cfRule type="expression" dxfId="70" priority="98">
+      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="69" priority="99">
+      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I87:I94">
+    <cfRule type="dataBar" priority="97">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L87:BO94">
     <cfRule type="expression" dxfId="68" priority="96">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E86">
+  <conditionalFormatting sqref="E87:E94">
     <cfRule type="cellIs" dxfId="67" priority="89" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18324,15 +18531,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="60" priority="87">
-      <formula>AND($F87&lt;=L$6,ROUNDDOWN(($G87-$F87+1)*$I87,0)+$F87-1&gt;=L$6)</formula>
+      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="59" priority="88">
-      <formula>AND(NOT(ISBLANK($F87)),$F87&lt;=L$6,$G87&gt;=L$6)</formula>
+      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I87:I94">
+  <conditionalFormatting sqref="I97">
     <cfRule type="dataBar" priority="86">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18341,17 +18548,17 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{2576D6AF-1BEE-4D0F-9F29-158B8510CEF5}</x14:id>
+          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L87:BO94">
+  <conditionalFormatting sqref="L97:BO97">
     <cfRule type="expression" dxfId="58" priority="85">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E94">
+  <conditionalFormatting sqref="E97">
     <cfRule type="cellIs" dxfId="57" priority="78" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18374,66 +18581,16 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO97">
-    <cfRule type="expression" dxfId="50" priority="76">
-      <formula>AND($F97&lt;=L$6,ROUNDDOWN(($G97-$F97+1)*$I97,0)+$F97-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="49" priority="77">
-      <formula>AND(NOT(ISBLANK($F97)),$F97&lt;=L$6,$G97&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I97">
-    <cfRule type="dataBar" priority="75">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{52A4FA6B-6481-4B97-9D81-1C74885277E0}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L97:BO97">
-    <cfRule type="expression" dxfId="48" priority="74">
-      <formula>L$6=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="47" priority="67" operator="equal">
-      <formula>"LINUX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="68" operator="equal">
-      <formula>"PHP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="69" operator="equal">
-      <formula>"CSS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="70" operator="equal">
-      <formula>"HTML"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="71" operator="equal">
-      <formula>"R"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="72" operator="equal">
-      <formula>"SQL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="73" operator="equal">
-      <formula>"JS"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L104:BO104">
-    <cfRule type="expression" dxfId="40" priority="43">
+    <cfRule type="expression" dxfId="50" priority="54">
       <formula>AND($F104&lt;=L$6,ROUNDDOWN(($G104-$F104+1)*$I104,0)+$F104-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="44">
+    <cfRule type="expression" dxfId="49" priority="55">
       <formula>AND(NOT(ISBLANK($F104)),$F104&lt;=L$6,$G104&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I104">
-    <cfRule type="dataBar" priority="42">
+    <cfRule type="dataBar" priority="53">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18447,11 +18604,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L104:BO104">
+    <cfRule type="expression" dxfId="48" priority="52">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E104">
+    <cfRule type="cellIs" dxfId="47" priority="45" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="48" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="51" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L111:BO111">
+    <cfRule type="expression" dxfId="40" priority="43">
+      <formula>AND($F111&lt;=L$6,ROUNDDOWN(($G111-$F111+1)*$I111,0)+$F111-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="39" priority="44">
+      <formula>AND(NOT(ISBLANK($F111)),$F111&lt;=L$6,$G111&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I111">
+    <cfRule type="dataBar" priority="42">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{90FAB54C-17F5-4636-AF91-94ADBF7BDE0D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L111:BO111">
     <cfRule type="expression" dxfId="38" priority="41">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E104">
+  <conditionalFormatting sqref="E111">
     <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18474,58 +18681,8 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L111:BO111">
-    <cfRule type="expression" dxfId="30" priority="32">
-      <formula>AND($F111&lt;=L$6,ROUNDDOWN(($G111-$F111+1)*$I111,0)+$F111-1&gt;=L$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="33">
-      <formula>AND(NOT(ISBLANK($F111)),$F111&lt;=L$6,$G111&gt;=L$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I111">
+  <conditionalFormatting sqref="I123">
     <cfRule type="dataBar" priority="31">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0" tint="-0.34998626667073579"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{90FAB54C-17F5-4636-AF91-94ADBF7BDE0D}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L111:BO111">
-    <cfRule type="expression" dxfId="28" priority="30">
-      <formula>L$6=TODAY()</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E111">
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
-      <formula>"LINUX"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="24" operator="equal">
-      <formula>"PHP"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
-      <formula>"CSS"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
-      <formula>"HTML"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
-      <formula>"R"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
-      <formula>"SQL"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
-      <formula>"JS"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I123">
-    <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -18539,11 +18696,61 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L123:BO123">
+    <cfRule type="expression" dxfId="30" priority="30">
+      <formula>L$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E123">
+    <cfRule type="cellIs" dxfId="29" priority="23" operator="equal">
+      <formula>"LINUX"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="24" operator="equal">
+      <formula>"PHP"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="25" operator="equal">
+      <formula>"CSS"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+      <formula>"HTML"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="28" operator="equal">
+      <formula>"SQL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+      <formula>"JS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L132:BO132">
+    <cfRule type="expression" dxfId="22" priority="21">
+      <formula>AND($F132&lt;=L$6,ROUNDDOWN(($G132-$F132+1)*$I132,0)+$F132-1&gt;=L$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>AND(NOT(ISBLANK($F132)),$F132&lt;=L$6,$G132&gt;=L$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I132">
+    <cfRule type="dataBar" priority="20">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{D39E3CA5-A193-489A-9A09-848BF4A69639}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L132:BO132">
     <cfRule type="expression" dxfId="20" priority="19">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E123">
+  <conditionalFormatting sqref="E132">
     <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -18566,15 +18773,15 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L132:BO132">
-    <cfRule type="expression" dxfId="12" priority="10">
-      <formula>AND($F132&lt;=L$6,ROUNDDOWN(($G132-$F132+1)*$I132,0)+$F132-1&gt;=L$6)</formula>
+  <conditionalFormatting sqref="L137:BO137">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>AND($F137&lt;=L$6,ROUNDDOWN(($G137-$F137+1)*$I137,0)+$F137-1&gt;=L$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
-      <formula>AND(NOT(ISBLANK($F132)),$F132&lt;=L$6,$G132&gt;=L$6)</formula>
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>AND(NOT(ISBLANK($F137)),$F137&lt;=L$6,$G137&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I132">
+  <conditionalFormatting sqref="I137">
     <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -18583,36 +18790,36 @@
       </dataBar>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{D39E3CA5-A193-489A-9A09-848BF4A69639}</x14:id>
+          <x14:id>{831EB1CB-C1FD-435A-B2AE-9B13F4C0A004}</x14:id>
         </ext>
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L132:BO132">
-    <cfRule type="expression" dxfId="10" priority="8">
+  <conditionalFormatting sqref="L137:BO137">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E132">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+  <conditionalFormatting sqref="E137">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"PHP"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"CSS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"HTML"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"R"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"SQL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18672,7 +18879,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I154</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I155</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -18702,7 +18909,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I155:I163</xm:sqref>
+          <xm:sqref>I156:I164</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -18717,7 +18924,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I164:I172</xm:sqref>
+          <xm:sqref>I165:I173</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -18732,7 +18939,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I173:I181</xm:sqref>
+          <xm:sqref>I174:I182</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">
@@ -18839,6 +19046,21 @@
           </x14:cfRule>
           <xm:sqref>I132</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{831EB1CB-C1FD-435A-B2AE-9B13F4C0A004}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>I137</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -19369,15 +19591,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:BN6">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>AND($E1&lt;=K$6,ROUNDDOWN(($F1-$E1+1)*$H1,0)+$E1-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>AND(NOT(ISBLANK($E1)),$E1&lt;=K$6,$F1&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:BN6">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add inf calculations by vintage date (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A310EF0-0A77-4BA5-A655-15480AC83714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD3BB2C-EE89-4051-8891-F31C206D5659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1874,6 +1874,13 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1883,6 +1890,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1891,17 +1902,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3493,8 +3493,8 @@
   <dimension ref="A1:BO194"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F147" sqref="F147"/>
+      <pane ySplit="7" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3524,27 +3524,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3589,12 +3589,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="82">
         <v>44192</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3604,183 +3604,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="77" t="str">
+      <c r="L4" s="79" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 52</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="77" t="str">
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="79" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="77" t="str">
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="79" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="78"/>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="77" t="str">
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="80"/>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="79" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="78"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="77" t="str">
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="79" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="77" t="str">
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="80"/>
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="81"/>
+      <c r="AU4" s="79" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 57</v>
       </c>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="78"/>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="77" t="str">
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="79" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 58</v>
       </c>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="78"/>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="77" t="str">
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="80"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="79" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 59</v>
       </c>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="78"/>
-      <c r="BM4" s="78"/>
-      <c r="BN4" s="78"/>
-      <c r="BO4" s="79"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="80"/>
+      <c r="BM4" s="80"/>
+      <c r="BN4" s="80"/>
+      <c r="BO4" s="81"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="80">
+      <c r="L5" s="83">
         <f>L6</f>
         <v>44550</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="80">
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="83">
         <f>S6</f>
         <v>44557</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="80">
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="83">
         <f>Z6</f>
         <v>44564</v>
       </c>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="82"/>
-      <c r="AG5" s="80">
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="84"/>
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="84"/>
+      <c r="AE5" s="84"/>
+      <c r="AF5" s="85"/>
+      <c r="AG5" s="83">
         <f>AG6</f>
         <v>44571</v>
       </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="82"/>
-      <c r="AN5" s="80">
+      <c r="AH5" s="84"/>
+      <c r="AI5" s="84"/>
+      <c r="AJ5" s="84"/>
+      <c r="AK5" s="84"/>
+      <c r="AL5" s="84"/>
+      <c r="AM5" s="85"/>
+      <c r="AN5" s="83">
         <f>AN6</f>
         <v>44578</v>
       </c>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AT5" s="82"/>
-      <c r="AU5" s="80">
+      <c r="AO5" s="84"/>
+      <c r="AP5" s="84"/>
+      <c r="AQ5" s="84"/>
+      <c r="AR5" s="84"/>
+      <c r="AS5" s="84"/>
+      <c r="AT5" s="85"/>
+      <c r="AU5" s="83">
         <f>AU6</f>
         <v>44585</v>
       </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="82"/>
-      <c r="BB5" s="80">
+      <c r="AV5" s="84"/>
+      <c r="AW5" s="84"/>
+      <c r="AX5" s="84"/>
+      <c r="AY5" s="84"/>
+      <c r="AZ5" s="84"/>
+      <c r="BA5" s="85"/>
+      <c r="BB5" s="83">
         <f>BB6</f>
         <v>44592</v>
       </c>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BH5" s="82"/>
-      <c r="BI5" s="80">
+      <c r="BC5" s="84"/>
+      <c r="BD5" s="84"/>
+      <c r="BE5" s="84"/>
+      <c r="BF5" s="84"/>
+      <c r="BG5" s="84"/>
+      <c r="BH5" s="85"/>
+      <c r="BI5" s="83">
         <f>BI6</f>
         <v>44599</v>
       </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="82"/>
+      <c r="BJ5" s="84"/>
+      <c r="BK5" s="84"/>
+      <c r="BL5" s="84"/>
+      <c r="BM5" s="84"/>
+      <c r="BN5" s="84"/>
+      <c r="BO5" s="85"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -15044,7 +15044,7 @@
         <v>44552</v>
       </c>
       <c r="G139" s="43">
-        <v>44553</v>
+        <v>44555</v>
       </c>
       <c r="H139" s="73"/>
       <c r="I139" s="26">
@@ -15122,10 +15122,10 @@
         <v>66</v>
       </c>
       <c r="F140" s="42">
-        <v>44553</v>
+        <v>44555</v>
       </c>
       <c r="G140" s="43">
-        <v>44553</v>
+        <v>44556</v>
       </c>
       <c r="H140" s="73"/>
       <c r="I140" s="26">
@@ -15203,10 +15203,10 @@
         <v>66</v>
       </c>
       <c r="F141" s="42">
-        <v>44553</v>
+        <v>44555</v>
       </c>
       <c r="G141" s="43">
-        <v>44553</v>
+        <v>44556</v>
       </c>
       <c r="H141" s="73"/>
       <c r="I141" s="26">
@@ -15284,7 +15284,7 @@
         <v>66</v>
       </c>
       <c r="F142" s="42">
-        <v>44553</v>
+        <v>44555</v>
       </c>
       <c r="G142" s="43">
         <v>44556</v>
@@ -15365,7 +15365,7 @@
         <v>66</v>
       </c>
       <c r="F143" s="42">
-        <v>44553</v>
+        <v>44555</v>
       </c>
       <c r="G143" s="43">
         <v>44556</v>
@@ -19073,15 +19073,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -19092,6 +19083,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I167">

</xml_diff>

<commit_message>
Updated PM and README (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD3BB2C-EE89-4051-8891-F31C206D5659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4624CE47-9672-4E29-B3DB-B4E5C9ED5A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -907,12 +907,6 @@
     <t>Pull all Historical Data Vintages</t>
   </si>
   <si>
-    <t>Refactor Nowcast Model to use Proper Backtesting w/Vintages</t>
-  </si>
-  <si>
-    <t>Develop Benchmark Composite Model - Optimal Model Stacking (RF/MRF)</t>
-  </si>
-  <si>
     <t>Refactor Structural Model</t>
   </si>
   <si>
@@ -937,25 +931,31 @@
     <t>Add Historical Data Calculated Variables</t>
   </si>
   <si>
-    <t>Add Historical Data Transforms</t>
-  </si>
-  <si>
-    <t>Model Overhaul - External Forecasts &amp; Web Release (v0.19)</t>
-  </si>
-  <si>
-    <t>Release Benchmark Composite Model on Website</t>
-  </si>
-  <si>
-    <t>Release External Forecasts on Website</t>
-  </si>
-  <si>
-    <t>Add Vintage External Forecast for Old Treasury Yield Forecasts</t>
-  </si>
-  <si>
     <t>Rebuild Asset Contagion Index</t>
   </si>
   <si>
     <t>Rebuild Sentiment Index</t>
+  </si>
+  <si>
+    <t>Model Overhaul - Modularization &amp; Web Release (v0.19)</t>
+  </si>
+  <si>
+    <t>Split Rate Model</t>
+  </si>
+  <si>
+    <t>Add AMERIBOR, SONIA, BSBY Rates</t>
+  </si>
+  <si>
+    <t>Update TDNS Forecasts</t>
+  </si>
+  <si>
+    <t>Update Benchmark Rate Forecasts</t>
+  </si>
+  <si>
+    <t>Develop Rate Composite Model - Optimal Model Stacking (RF/MRF)</t>
+  </si>
+  <si>
+    <t>Release Rate Forecasts on Website</t>
   </si>
 </sst>
 </file>
@@ -1874,13 +1874,6 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1890,10 +1883,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1902,6 +1891,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3494,7 +3494,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G142" sqref="G142"/>
+      <selection pane="bottomLeft" activeCell="R146" sqref="R146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3524,27 +3524,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3589,12 +3589,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="85">
         <v>44192</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3604,183 +3604,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="79" t="str">
+      <c r="L4" s="77" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 52</v>
       </c>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="79" t="str">
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="77" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="79" t="str">
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="77" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="81"/>
-      <c r="AG4" s="79" t="str">
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
+      <c r="AE4" s="78"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="77" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="80"/>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="81"/>
-      <c r="AN4" s="79" t="str">
+      <c r="AH4" s="78"/>
+      <c r="AI4" s="78"/>
+      <c r="AJ4" s="78"/>
+      <c r="AK4" s="78"/>
+      <c r="AL4" s="78"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="77" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="80"/>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="81"/>
-      <c r="AU4" s="79" t="str">
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="78"/>
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="77" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 57</v>
       </c>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="80"/>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="81"/>
-      <c r="BB4" s="79" t="str">
+      <c r="AV4" s="78"/>
+      <c r="AW4" s="78"/>
+      <c r="AX4" s="78"/>
+      <c r="AY4" s="78"/>
+      <c r="AZ4" s="78"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="77" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 58</v>
       </c>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="80"/>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="81"/>
-      <c r="BI4" s="79" t="str">
+      <c r="BC4" s="78"/>
+      <c r="BD4" s="78"/>
+      <c r="BE4" s="78"/>
+      <c r="BF4" s="78"/>
+      <c r="BG4" s="78"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="77" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 59</v>
       </c>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="80"/>
-      <c r="BM4" s="80"/>
-      <c r="BN4" s="80"/>
-      <c r="BO4" s="81"/>
+      <c r="BJ4" s="78"/>
+      <c r="BK4" s="78"/>
+      <c r="BL4" s="78"/>
+      <c r="BM4" s="78"/>
+      <c r="BN4" s="78"/>
+      <c r="BO4" s="79"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="83">
+      <c r="L5" s="80">
         <f>L6</f>
         <v>44550</v>
       </c>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="83">
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="80">
         <f>S6</f>
         <v>44557</v>
       </c>
-      <c r="T5" s="84"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="85"/>
-      <c r="Z5" s="83">
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="80">
         <f>Z6</f>
         <v>44564</v>
       </c>
-      <c r="AA5" s="84"/>
-      <c r="AB5" s="84"/>
-      <c r="AC5" s="84"/>
-      <c r="AD5" s="84"/>
-      <c r="AE5" s="84"/>
-      <c r="AF5" s="85"/>
-      <c r="AG5" s="83">
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="82"/>
+      <c r="AG5" s="80">
         <f>AG6</f>
         <v>44571</v>
       </c>
-      <c r="AH5" s="84"/>
-      <c r="AI5" s="84"/>
-      <c r="AJ5" s="84"/>
-      <c r="AK5" s="84"/>
-      <c r="AL5" s="84"/>
-      <c r="AM5" s="85"/>
-      <c r="AN5" s="83">
+      <c r="AH5" s="81"/>
+      <c r="AI5" s="81"/>
+      <c r="AJ5" s="81"/>
+      <c r="AK5" s="81"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="82"/>
+      <c r="AN5" s="80">
         <f>AN6</f>
         <v>44578</v>
       </c>
-      <c r="AO5" s="84"/>
-      <c r="AP5" s="84"/>
-      <c r="AQ5" s="84"/>
-      <c r="AR5" s="84"/>
-      <c r="AS5" s="84"/>
-      <c r="AT5" s="85"/>
-      <c r="AU5" s="83">
+      <c r="AO5" s="81"/>
+      <c r="AP5" s="81"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="81"/>
+      <c r="AS5" s="81"/>
+      <c r="AT5" s="82"/>
+      <c r="AU5" s="80">
         <f>AU6</f>
         <v>44585</v>
       </c>
-      <c r="AV5" s="84"/>
-      <c r="AW5" s="84"/>
-      <c r="AX5" s="84"/>
-      <c r="AY5" s="84"/>
-      <c r="AZ5" s="84"/>
-      <c r="BA5" s="85"/>
-      <c r="BB5" s="83">
+      <c r="AV5" s="81"/>
+      <c r="AW5" s="81"/>
+      <c r="AX5" s="81"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="81"/>
+      <c r="BA5" s="82"/>
+      <c r="BB5" s="80">
         <f>BB6</f>
         <v>44592</v>
       </c>
-      <c r="BC5" s="84"/>
-      <c r="BD5" s="84"/>
-      <c r="BE5" s="84"/>
-      <c r="BF5" s="84"/>
-      <c r="BG5" s="84"/>
-      <c r="BH5" s="85"/>
-      <c r="BI5" s="83">
+      <c r="BC5" s="81"/>
+      <c r="BD5" s="81"/>
+      <c r="BE5" s="81"/>
+      <c r="BF5" s="81"/>
+      <c r="BG5" s="81"/>
+      <c r="BH5" s="82"/>
+      <c r="BI5" s="80">
         <f>BI6</f>
         <v>44599</v>
       </c>
-      <c r="BJ5" s="84"/>
-      <c r="BK5" s="84"/>
-      <c r="BL5" s="84"/>
-      <c r="BM5" s="84"/>
-      <c r="BN5" s="84"/>
-      <c r="BO5" s="85"/>
+      <c r="BJ5" s="81"/>
+      <c r="BK5" s="81"/>
+      <c r="BL5" s="81"/>
+      <c r="BM5" s="81"/>
+      <c r="BN5" s="81"/>
+      <c r="BO5" s="82"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -14471,7 +14471,7 @@
         <v>13</v>
       </c>
       <c r="B132" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D132" s="19"/>
       <c r="E132" s="19"/>
@@ -14874,7 +14874,7 @@
         <v>14</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D137" s="19"/>
       <c r="E137" s="19"/>
@@ -14953,7 +14953,7 @@
         <v>14.1</v>
       </c>
       <c r="B138" s="65" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D138" s="70"/>
       <c r="E138" s="66" t="s">
@@ -15034,7 +15034,7 @@
         <v>14.2</v>
       </c>
       <c r="B139" s="65" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D139" s="70"/>
       <c r="E139" s="66" t="s">
@@ -15048,7 +15048,7 @@
       </c>
       <c r="H139" s="73"/>
       <c r="I139" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J139" s="75"/>
       <c r="K139" s="76"/>
@@ -15115,7 +15115,7 @@
         <v>14.3</v>
       </c>
       <c r="B140" s="65" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D140" s="70"/>
       <c r="E140" s="66" t="s">
@@ -15129,7 +15129,7 @@
       </c>
       <c r="H140" s="73"/>
       <c r="I140" s="26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J140" s="75"/>
       <c r="K140" s="76"/>
@@ -15196,7 +15196,7 @@
         <v>14.4</v>
       </c>
       <c r="B141" s="65" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D141" s="70"/>
       <c r="E141" s="66" t="s">
@@ -15210,7 +15210,7 @@
       </c>
       <c r="H141" s="73"/>
       <c r="I141" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J141" s="75"/>
       <c r="K141" s="76"/>
@@ -15277,21 +15277,21 @@
         <v>14.5</v>
       </c>
       <c r="B142" s="65" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="D142" s="70"/>
       <c r="E142" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F142" s="42">
-        <v>44555</v>
+        <v>44556</v>
       </c>
       <c r="G142" s="43">
-        <v>44556</v>
+        <v>44557</v>
       </c>
       <c r="H142" s="73"/>
       <c r="I142" s="26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J142" s="75"/>
       <c r="K142" s="76"/>
@@ -15358,21 +15358,21 @@
         <v>14.6</v>
       </c>
       <c r="B143" s="65" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="D143" s="70"/>
       <c r="E143" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F143" s="42">
-        <v>44555</v>
+        <v>44556</v>
       </c>
       <c r="G143" s="43">
-        <v>44556</v>
+        <v>44557</v>
       </c>
       <c r="H143" s="73"/>
       <c r="I143" s="26">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="J143" s="75"/>
       <c r="K143" s="76"/>
@@ -15439,17 +15439,17 @@
         <v>14.7</v>
       </c>
       <c r="B144" s="65" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D144" s="70"/>
       <c r="E144" s="66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F144" s="42">
-        <v>44557</v>
+        <v>44558</v>
       </c>
       <c r="G144" s="43">
-        <v>44561</v>
+        <v>44197</v>
       </c>
       <c r="H144" s="73"/>
       <c r="I144" s="26">
@@ -15520,17 +15520,17 @@
         <v>14.8</v>
       </c>
       <c r="B145" s="65" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D145" s="70"/>
       <c r="E145" s="66" t="s">
         <v>68</v>
       </c>
       <c r="F145" s="42">
-        <v>44557</v>
+        <v>44559</v>
       </c>
       <c r="G145" s="43">
-        <v>44562</v>
+        <v>44198</v>
       </c>
       <c r="H145" s="73"/>
       <c r="I145" s="26">
@@ -15601,17 +15601,17 @@
         <v>14.9</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D146" s="70"/>
       <c r="E146" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F146" s="42">
-        <v>44557</v>
+        <v>44561</v>
       </c>
       <c r="G146" s="43">
-        <v>44563</v>
+        <v>44198</v>
       </c>
       <c r="H146" s="73"/>
       <c r="I146" s="26">
@@ -15682,17 +15682,17 @@
         <v>14.10</v>
       </c>
       <c r="B147" s="65" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D147" s="70"/>
       <c r="E147" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F147" s="42">
-        <v>44557</v>
+        <v>44561</v>
       </c>
       <c r="G147" s="43">
-        <v>44563</v>
+        <v>44198</v>
       </c>
       <c r="H147" s="73"/>
       <c r="I147" s="26">
@@ -16116,7 +16116,7 @@
         <v>0.2</v>
       </c>
       <c r="B153" s="65" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D153" s="70"/>
       <c r="E153" s="66" t="s">
@@ -16197,7 +16197,7 @@
         <v>0.3</v>
       </c>
       <c r="B154" s="65" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D154" s="70"/>
       <c r="E154" s="66" t="s">
@@ -16278,7 +16278,7 @@
         <v>0.4</v>
       </c>
       <c r="B155" s="65" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D155" s="70"/>
       <c r="E155" s="66" t="s">
@@ -16359,7 +16359,7 @@
         <v>0.5</v>
       </c>
       <c r="B156" s="65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D156" s="70"/>
       <c r="E156" s="66" t="s">
@@ -16440,7 +16440,7 @@
         <v>0.6</v>
       </c>
       <c r="B157" s="65" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D157" s="70"/>
       <c r="E157" s="66" t="s">
@@ -19073,6 +19073,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -19083,15 +19092,6 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I167">

</xml_diff>

<commit_message>
Cleaned up folder structure (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4624CE47-9672-4E29-B3DB-B4E5C9ED5A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED08817B-D89B-4D33-848F-BB5CEE698147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1874,6 +1874,13 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1883,6 +1890,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1891,17 +1902,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3083,7 +3083,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="52"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$I$4" horiz="1" max="100" min="1" page="0" val="53"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3493,8 +3493,8 @@
   <dimension ref="A1:BO194"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R146" sqref="R146"/>
+      <pane ySplit="7" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3524,27 +3524,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3589,198 +3589,198 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="82">
         <v>44192</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
       </c>
       <c r="I4" s="67">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="77" t="str">
+      <c r="L4" s="79" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 52</v>
-      </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="77" t="str">
+        <v>Week 53</v>
+      </c>
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="79" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 53</v>
-      </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="77" t="str">
+        <v>Week 54</v>
+      </c>
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="79" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 54</v>
-      </c>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="78"/>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="77" t="str">
+        <v>Week 55</v>
+      </c>
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="80"/>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="79" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 55</v>
-      </c>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="78"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="77" t="str">
+        <v>Week 56</v>
+      </c>
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="79" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 56</v>
-      </c>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="77" t="str">
+        <v>Week 57</v>
+      </c>
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="80"/>
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="81"/>
+      <c r="AU4" s="79" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 57</v>
-      </c>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="78"/>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="77" t="str">
+        <v>Week 58</v>
+      </c>
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="79" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 58</v>
-      </c>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="78"/>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="77" t="str">
+        <v>Week 59</v>
+      </c>
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="80"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="79" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 59</v>
-      </c>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="78"/>
-      <c r="BM4" s="78"/>
-      <c r="BN4" s="78"/>
-      <c r="BO4" s="79"/>
+        <v>Week 60</v>
+      </c>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="80"/>
+      <c r="BM4" s="80"/>
+      <c r="BN4" s="80"/>
+      <c r="BO4" s="81"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="80">
+      <c r="L5" s="83">
         <f>L6</f>
-        <v>44550</v>
-      </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="80">
+        <v>44557</v>
+      </c>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="83">
         <f>S6</f>
-        <v>44557</v>
-      </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="80">
+        <v>44564</v>
+      </c>
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="83">
         <f>Z6</f>
-        <v>44564</v>
-      </c>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="82"/>
-      <c r="AG5" s="80">
+        <v>44571</v>
+      </c>
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="84"/>
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="84"/>
+      <c r="AE5" s="84"/>
+      <c r="AF5" s="85"/>
+      <c r="AG5" s="83">
         <f>AG6</f>
-        <v>44571</v>
-      </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="82"/>
-      <c r="AN5" s="80">
+        <v>44578</v>
+      </c>
+      <c r="AH5" s="84"/>
+      <c r="AI5" s="84"/>
+      <c r="AJ5" s="84"/>
+      <c r="AK5" s="84"/>
+      <c r="AL5" s="84"/>
+      <c r="AM5" s="85"/>
+      <c r="AN5" s="83">
         <f>AN6</f>
-        <v>44578</v>
-      </c>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AT5" s="82"/>
-      <c r="AU5" s="80">
+        <v>44585</v>
+      </c>
+      <c r="AO5" s="84"/>
+      <c r="AP5" s="84"/>
+      <c r="AQ5" s="84"/>
+      <c r="AR5" s="84"/>
+      <c r="AS5" s="84"/>
+      <c r="AT5" s="85"/>
+      <c r="AU5" s="83">
         <f>AU6</f>
-        <v>44585</v>
-      </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="82"/>
-      <c r="BB5" s="80">
+        <v>44592</v>
+      </c>
+      <c r="AV5" s="84"/>
+      <c r="AW5" s="84"/>
+      <c r="AX5" s="84"/>
+      <c r="AY5" s="84"/>
+      <c r="AZ5" s="84"/>
+      <c r="BA5" s="85"/>
+      <c r="BB5" s="83">
         <f>BB6</f>
-        <v>44592</v>
-      </c>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BH5" s="82"/>
-      <c r="BI5" s="80">
+        <v>44599</v>
+      </c>
+      <c r="BC5" s="84"/>
+      <c r="BD5" s="84"/>
+      <c r="BE5" s="84"/>
+      <c r="BF5" s="84"/>
+      <c r="BG5" s="84"/>
+      <c r="BH5" s="85"/>
+      <c r="BI5" s="83">
         <f>BI6</f>
-        <v>44599</v>
-      </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="82"/>
+        <v>44606</v>
+      </c>
+      <c r="BJ5" s="84"/>
+      <c r="BK5" s="84"/>
+      <c r="BL5" s="84"/>
+      <c r="BM5" s="84"/>
+      <c r="BN5" s="84"/>
+      <c r="BO5" s="85"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -3796,227 +3796,227 @@
       <c r="K6" s="13"/>
       <c r="L6" s="37">
         <f>C4-WEEKDAY(C4,1)+2+7*(I4-1)</f>
-        <v>44550</v>
+        <v>44557</v>
       </c>
       <c r="M6" s="28">
         <f t="shared" ref="M6:AR6" si="0">L6+1</f>
-        <v>44551</v>
+        <v>44558</v>
       </c>
       <c r="N6" s="28">
         <f t="shared" si="0"/>
-        <v>44552</v>
+        <v>44559</v>
       </c>
       <c r="O6" s="28">
         <f t="shared" si="0"/>
-        <v>44553</v>
+        <v>44560</v>
       </c>
       <c r="P6" s="28">
         <f t="shared" si="0"/>
-        <v>44554</v>
+        <v>44561</v>
       </c>
       <c r="Q6" s="28">
         <f t="shared" si="0"/>
-        <v>44555</v>
+        <v>44562</v>
       </c>
       <c r="R6" s="38">
         <f t="shared" si="0"/>
-        <v>44556</v>
+        <v>44563</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>44557</v>
+        <v>44564</v>
       </c>
       <c r="T6" s="28">
         <f t="shared" si="0"/>
-        <v>44558</v>
+        <v>44565</v>
       </c>
       <c r="U6" s="28">
         <f t="shared" si="0"/>
-        <v>44559</v>
+        <v>44566</v>
       </c>
       <c r="V6" s="28">
         <f t="shared" si="0"/>
-        <v>44560</v>
+        <v>44567</v>
       </c>
       <c r="W6" s="28">
         <f t="shared" si="0"/>
-        <v>44561</v>
+        <v>44568</v>
       </c>
       <c r="X6" s="28">
         <f t="shared" si="0"/>
-        <v>44562</v>
+        <v>44569</v>
       </c>
       <c r="Y6" s="38">
         <f t="shared" si="0"/>
-        <v>44563</v>
+        <v>44570</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>44564</v>
+        <v>44571</v>
       </c>
       <c r="AA6" s="28">
         <f t="shared" si="0"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="AB6" s="28">
         <f t="shared" si="0"/>
-        <v>44566</v>
+        <v>44573</v>
       </c>
       <c r="AC6" s="28">
         <f t="shared" si="0"/>
-        <v>44567</v>
+        <v>44574</v>
       </c>
       <c r="AD6" s="28">
         <f t="shared" si="0"/>
-        <v>44568</v>
+        <v>44575</v>
       </c>
       <c r="AE6" s="28">
         <f t="shared" si="0"/>
-        <v>44569</v>
+        <v>44576</v>
       </c>
       <c r="AF6" s="38">
         <f t="shared" si="0"/>
-        <v>44570</v>
+        <v>44577</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="AH6" s="28">
         <f t="shared" si="0"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="AI6" s="28">
         <f t="shared" si="0"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="AJ6" s="28">
         <f t="shared" si="0"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="AK6" s="28">
         <f t="shared" si="0"/>
-        <v>44575</v>
+        <v>44582</v>
       </c>
       <c r="AL6" s="28">
         <f t="shared" si="0"/>
-        <v>44576</v>
+        <v>44583</v>
       </c>
       <c r="AM6" s="38">
         <f t="shared" si="0"/>
-        <v>44577</v>
+        <v>44584</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>44578</v>
+        <v>44585</v>
       </c>
       <c r="AO6" s="28">
         <f t="shared" si="0"/>
-        <v>44579</v>
+        <v>44586</v>
       </c>
       <c r="AP6" s="28">
         <f t="shared" si="0"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="AQ6" s="28">
         <f t="shared" si="0"/>
-        <v>44581</v>
+        <v>44588</v>
       </c>
       <c r="AR6" s="28">
         <f t="shared" si="0"/>
-        <v>44582</v>
+        <v>44589</v>
       </c>
       <c r="AS6" s="28">
         <f t="shared" ref="AS6:BO6" si="1">AR6+1</f>
-        <v>44583</v>
+        <v>44590</v>
       </c>
       <c r="AT6" s="38">
         <f t="shared" si="1"/>
-        <v>44584</v>
+        <v>44591</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="1"/>
-        <v>44585</v>
+        <v>44592</v>
       </c>
       <c r="AV6" s="28">
         <f t="shared" si="1"/>
-        <v>44586</v>
+        <v>44593</v>
       </c>
       <c r="AW6" s="28">
         <f t="shared" si="1"/>
-        <v>44587</v>
+        <v>44594</v>
       </c>
       <c r="AX6" s="28">
         <f t="shared" si="1"/>
-        <v>44588</v>
+        <v>44595</v>
       </c>
       <c r="AY6" s="28">
         <f t="shared" si="1"/>
-        <v>44589</v>
+        <v>44596</v>
       </c>
       <c r="AZ6" s="28">
         <f t="shared" si="1"/>
-        <v>44590</v>
+        <v>44597</v>
       </c>
       <c r="BA6" s="38">
         <f t="shared" si="1"/>
-        <v>44591</v>
+        <v>44598</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="1"/>
-        <v>44592</v>
+        <v>44599</v>
       </c>
       <c r="BC6" s="28">
         <f t="shared" si="1"/>
-        <v>44593</v>
+        <v>44600</v>
       </c>
       <c r="BD6" s="28">
         <f t="shared" si="1"/>
-        <v>44594</v>
+        <v>44601</v>
       </c>
       <c r="BE6" s="28">
         <f t="shared" si="1"/>
-        <v>44595</v>
+        <v>44602</v>
       </c>
       <c r="BF6" s="28">
         <f t="shared" si="1"/>
-        <v>44596</v>
+        <v>44603</v>
       </c>
       <c r="BG6" s="28">
         <f t="shared" si="1"/>
-        <v>44597</v>
+        <v>44604</v>
       </c>
       <c r="BH6" s="38">
         <f t="shared" si="1"/>
-        <v>44598</v>
+        <v>44605</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="1"/>
-        <v>44599</v>
+        <v>44606</v>
       </c>
       <c r="BJ6" s="28">
         <f t="shared" si="1"/>
-        <v>44600</v>
+        <v>44607</v>
       </c>
       <c r="BK6" s="28">
         <f t="shared" si="1"/>
-        <v>44601</v>
+        <v>44608</v>
       </c>
       <c r="BL6" s="28">
         <f t="shared" si="1"/>
-        <v>44602</v>
+        <v>44609</v>
       </c>
       <c r="BM6" s="28">
         <f t="shared" si="1"/>
-        <v>44603</v>
+        <v>44610</v>
       </c>
       <c r="BN6" s="28">
         <f t="shared" si="1"/>
-        <v>44604</v>
+        <v>44611</v>
       </c>
       <c r="BO6" s="38">
         <f t="shared" si="1"/>
-        <v>44605</v>
+        <v>44612</v>
       </c>
     </row>
     <row r="7" spans="1:67" s="63" customFormat="1" ht="24.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -15125,7 +15125,7 @@
         <v>44555</v>
       </c>
       <c r="G140" s="43">
-        <v>44556</v>
+        <v>44557</v>
       </c>
       <c r="H140" s="73"/>
       <c r="I140" s="26">
@@ -15206,7 +15206,7 @@
         <v>44555</v>
       </c>
       <c r="G141" s="43">
-        <v>44556</v>
+        <v>44557</v>
       </c>
       <c r="H141" s="73"/>
       <c r="I141" s="26">
@@ -15287,7 +15287,7 @@
         <v>44556</v>
       </c>
       <c r="G142" s="43">
-        <v>44557</v>
+        <v>44558</v>
       </c>
       <c r="H142" s="73"/>
       <c r="I142" s="26">
@@ -15368,7 +15368,7 @@
         <v>44556</v>
       </c>
       <c r="G143" s="43">
-        <v>44557</v>
+        <v>44558</v>
       </c>
       <c r="H143" s="73"/>
       <c r="I143" s="26">
@@ -19073,15 +19073,6 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -19092,6 +19083,15 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I167">

</xml_diff>

<commit_message>
Added Ameribor forecasts (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC25201-8FC1-43DD-892D-1B4438BA3492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF095B-2C5A-4E59-B3BF-CE3454F7B3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="179">
   <si>
     <t>WBS</t>
   </si>
@@ -962,6 +962,9 @@
   </si>
   <si>
     <t>Add Raw Forecast Storage to TimescaleDB</t>
+  </si>
+  <si>
+    <t>Add BSBY Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1880,6 +1883,13 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1889,6 +1899,10 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1897,17 +1911,6 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3496,11 +3499,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO196"/>
+  <dimension ref="A1:BO197"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
+      <selection pane="bottomLeft" activeCell="I147" sqref="I147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3530,27 +3533,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="83"/>
-      <c r="T1" s="83"/>
-      <c r="U1" s="83"/>
-      <c r="V1" s="83"/>
-      <c r="W1" s="83"/>
-      <c r="X1" s="83"/>
-      <c r="Y1" s="83"/>
-      <c r="Z1" s="83"/>
-      <c r="AA1" s="83"/>
-      <c r="AB1" s="83"/>
-      <c r="AC1" s="83"/>
-      <c r="AD1" s="83"/>
-      <c r="AE1" s="83"/>
-      <c r="AF1" s="83"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3595,12 +3598,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="85">
+      <c r="C4" s="82">
         <v>44192</v>
       </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="85"/>
-      <c r="F4" s="85"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3610,183 +3613,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="77" t="str">
+      <c r="L4" s="79" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="M4" s="78"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="78"/>
-      <c r="P4" s="78"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="77" t="str">
+      <c r="M4" s="80"/>
+      <c r="N4" s="80"/>
+      <c r="O4" s="80"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="80"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="79" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="T4" s="78"/>
-      <c r="U4" s="78"/>
-      <c r="V4" s="78"/>
-      <c r="W4" s="78"/>
-      <c r="X4" s="78"/>
-      <c r="Y4" s="79"/>
-      <c r="Z4" s="77" t="str">
+      <c r="T4" s="80"/>
+      <c r="U4" s="80"/>
+      <c r="V4" s="80"/>
+      <c r="W4" s="80"/>
+      <c r="X4" s="80"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="79" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="AA4" s="78"/>
-      <c r="AB4" s="78"/>
-      <c r="AC4" s="78"/>
-      <c r="AD4" s="78"/>
-      <c r="AE4" s="78"/>
-      <c r="AF4" s="79"/>
-      <c r="AG4" s="77" t="str">
+      <c r="AA4" s="80"/>
+      <c r="AB4" s="80"/>
+      <c r="AC4" s="80"/>
+      <c r="AD4" s="80"/>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="81"/>
+      <c r="AG4" s="79" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="AH4" s="78"/>
-      <c r="AI4" s="78"/>
-      <c r="AJ4" s="78"/>
-      <c r="AK4" s="78"/>
-      <c r="AL4" s="78"/>
-      <c r="AM4" s="79"/>
-      <c r="AN4" s="77" t="str">
+      <c r="AH4" s="80"/>
+      <c r="AI4" s="80"/>
+      <c r="AJ4" s="80"/>
+      <c r="AK4" s="80"/>
+      <c r="AL4" s="80"/>
+      <c r="AM4" s="81"/>
+      <c r="AN4" s="79" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 57</v>
       </c>
-      <c r="AO4" s="78"/>
-      <c r="AP4" s="78"/>
-      <c r="AQ4" s="78"/>
-      <c r="AR4" s="78"/>
-      <c r="AS4" s="78"/>
-      <c r="AT4" s="79"/>
-      <c r="AU4" s="77" t="str">
+      <c r="AO4" s="80"/>
+      <c r="AP4" s="80"/>
+      <c r="AQ4" s="80"/>
+      <c r="AR4" s="80"/>
+      <c r="AS4" s="80"/>
+      <c r="AT4" s="81"/>
+      <c r="AU4" s="79" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 58</v>
       </c>
-      <c r="AV4" s="78"/>
-      <c r="AW4" s="78"/>
-      <c r="AX4" s="78"/>
-      <c r="AY4" s="78"/>
-      <c r="AZ4" s="78"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="77" t="str">
+      <c r="AV4" s="80"/>
+      <c r="AW4" s="80"/>
+      <c r="AX4" s="80"/>
+      <c r="AY4" s="80"/>
+      <c r="AZ4" s="80"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="79" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 59</v>
       </c>
-      <c r="BC4" s="78"/>
-      <c r="BD4" s="78"/>
-      <c r="BE4" s="78"/>
-      <c r="BF4" s="78"/>
-      <c r="BG4" s="78"/>
-      <c r="BH4" s="79"/>
-      <c r="BI4" s="77" t="str">
+      <c r="BC4" s="80"/>
+      <c r="BD4" s="80"/>
+      <c r="BE4" s="80"/>
+      <c r="BF4" s="80"/>
+      <c r="BG4" s="80"/>
+      <c r="BH4" s="81"/>
+      <c r="BI4" s="79" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 60</v>
       </c>
-      <c r="BJ4" s="78"/>
-      <c r="BK4" s="78"/>
-      <c r="BL4" s="78"/>
-      <c r="BM4" s="78"/>
-      <c r="BN4" s="78"/>
-      <c r="BO4" s="79"/>
+      <c r="BJ4" s="80"/>
+      <c r="BK4" s="80"/>
+      <c r="BL4" s="80"/>
+      <c r="BM4" s="80"/>
+      <c r="BN4" s="80"/>
+      <c r="BO4" s="81"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="84" t="s">
+      <c r="C5" s="78" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
+      <c r="D5" s="78"/>
+      <c r="E5" s="78"/>
+      <c r="F5" s="78"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="80">
+      <c r="L5" s="83">
         <f>L6</f>
         <v>44557</v>
       </c>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="82"/>
-      <c r="S5" s="80">
+      <c r="M5" s="84"/>
+      <c r="N5" s="84"/>
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="83">
         <f>S6</f>
         <v>44564</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="82"/>
-      <c r="Z5" s="80">
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="83">
         <f>Z6</f>
         <v>44571</v>
       </c>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AF5" s="82"/>
-      <c r="AG5" s="80">
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="84"/>
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="84"/>
+      <c r="AE5" s="84"/>
+      <c r="AF5" s="85"/>
+      <c r="AG5" s="83">
         <f>AG6</f>
         <v>44578</v>
       </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="82"/>
-      <c r="AN5" s="80">
+      <c r="AH5" s="84"/>
+      <c r="AI5" s="84"/>
+      <c r="AJ5" s="84"/>
+      <c r="AK5" s="84"/>
+      <c r="AL5" s="84"/>
+      <c r="AM5" s="85"/>
+      <c r="AN5" s="83">
         <f>AN6</f>
         <v>44585</v>
       </c>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AT5" s="82"/>
-      <c r="AU5" s="80">
+      <c r="AO5" s="84"/>
+      <c r="AP5" s="84"/>
+      <c r="AQ5" s="84"/>
+      <c r="AR5" s="84"/>
+      <c r="AS5" s="84"/>
+      <c r="AT5" s="85"/>
+      <c r="AU5" s="83">
         <f>AU6</f>
         <v>44592</v>
       </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="82"/>
-      <c r="BB5" s="80">
+      <c r="AV5" s="84"/>
+      <c r="AW5" s="84"/>
+      <c r="AX5" s="84"/>
+      <c r="AY5" s="84"/>
+      <c r="AZ5" s="84"/>
+      <c r="BA5" s="85"/>
+      <c r="BB5" s="83">
         <f>BB6</f>
         <v>44599</v>
       </c>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BH5" s="82"/>
-      <c r="BI5" s="80">
+      <c r="BC5" s="84"/>
+      <c r="BD5" s="84"/>
+      <c r="BE5" s="84"/>
+      <c r="BF5" s="84"/>
+      <c r="BG5" s="84"/>
+      <c r="BH5" s="85"/>
+      <c r="BI5" s="83">
         <f>BI6</f>
         <v>44606</v>
       </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="82"/>
+      <c r="BJ5" s="84"/>
+      <c r="BK5" s="84"/>
+      <c r="BL5" s="84"/>
+      <c r="BM5" s="84"/>
+      <c r="BN5" s="84"/>
+      <c r="BO5" s="85"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8944,7 +8947,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A162" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A163" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -15459,7 +15462,7 @@
       </c>
       <c r="H144" s="73"/>
       <c r="I144" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J144" s="75"/>
       <c r="K144" s="76"/>
@@ -15536,11 +15539,11 @@
         <v>44558</v>
       </c>
       <c r="G145" s="43">
-        <v>44558</v>
+        <v>44559</v>
       </c>
       <c r="H145" s="73"/>
       <c r="I145" s="26">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J145" s="75"/>
       <c r="K145" s="76"/>
@@ -15607,21 +15610,21 @@
         <v>14.9</v>
       </c>
       <c r="B146" s="65" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="D146" s="70"/>
       <c r="E146" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F146" s="42">
-        <v>44558</v>
+        <v>44559</v>
       </c>
       <c r="G146" s="43">
-        <v>44560</v>
+        <v>44559</v>
       </c>
       <c r="H146" s="73"/>
       <c r="I146" s="26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J146" s="75"/>
       <c r="K146" s="76"/>
@@ -15688,17 +15691,17 @@
         <v>14.10</v>
       </c>
       <c r="B147" s="65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D147" s="70"/>
       <c r="E147" s="66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F147" s="42">
+        <v>44559</v>
+      </c>
+      <c r="G147" s="43">
         <v>44560</v>
-      </c>
-      <c r="G147" s="43">
-        <v>44563</v>
       </c>
       <c r="H147" s="73"/>
       <c r="I147" s="26">
@@ -15769,17 +15772,17 @@
         <v>14.11</v>
       </c>
       <c r="B148" s="65" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D148" s="70"/>
       <c r="E148" s="66" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F148" s="42">
-        <v>44561</v>
+        <v>44560</v>
       </c>
       <c r="G148" s="43">
-        <v>44564</v>
+        <v>44563</v>
       </c>
       <c r="H148" s="73"/>
       <c r="I148" s="26">
@@ -15850,7 +15853,7 @@
         <v>14.12</v>
       </c>
       <c r="B149" s="65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D149" s="70"/>
       <c r="E149" s="66" t="s">
@@ -15926,14 +15929,27 @@
       <c r="BO149" s="46"/>
     </row>
     <row r="150" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="23"/>
-      <c r="B150" s="65"/>
+      <c r="A150" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>14.13</v>
+      </c>
+      <c r="B150" s="65" t="s">
+        <v>168</v>
+      </c>
       <c r="D150" s="70"/>
-      <c r="E150" s="66"/>
-      <c r="F150" s="42"/>
-      <c r="G150" s="43"/>
+      <c r="E150" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F150" s="42">
+        <v>44561</v>
+      </c>
+      <c r="G150" s="43">
+        <v>44564</v>
+      </c>
       <c r="H150" s="73"/>
-      <c r="I150" s="26"/>
+      <c r="I150" s="26">
+        <v>0</v>
+      </c>
       <c r="J150" s="75"/>
       <c r="K150" s="76"/>
       <c r="L150" s="46"/>
@@ -16198,27 +16214,14 @@
       <c r="BO153" s="46"/>
     </row>
     <row r="154" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>0.1</v>
-      </c>
-      <c r="B154" s="65" t="s">
-        <v>150</v>
-      </c>
+      <c r="A154" s="23"/>
+      <c r="B154" s="65"/>
       <c r="D154" s="70"/>
-      <c r="E154" s="66" t="s">
-        <v>151</v>
-      </c>
-      <c r="F154" s="42">
-        <v>44557</v>
-      </c>
-      <c r="G154" s="43">
-        <v>44561</v>
-      </c>
+      <c r="E154" s="66"/>
+      <c r="F154" s="42"/>
+      <c r="G154" s="43"/>
       <c r="H154" s="73"/>
-      <c r="I154" s="26">
-        <v>0</v>
-      </c>
+      <c r="I154" s="26"/>
       <c r="J154" s="75"/>
       <c r="K154" s="76"/>
       <c r="L154" s="46"/>
@@ -16281,17 +16284,17 @@
     <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="B155" s="65" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D155" s="70"/>
       <c r="E155" s="66" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="F155" s="42">
-        <v>44561</v>
+        <v>44557</v>
       </c>
       <c r="G155" s="43">
         <v>44561</v>
@@ -16362,17 +16365,17 @@
     <row r="156" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="B156" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D156" s="70"/>
       <c r="E156" s="66" t="s">
         <v>68</v>
       </c>
       <c r="F156" s="42">
-        <v>44551</v>
+        <v>44561</v>
       </c>
       <c r="G156" s="43">
         <v>44561</v>
@@ -16443,10 +16446,10 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="B157" s="65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D157" s="70"/>
       <c r="E157" s="66" t="s">
@@ -16456,7 +16459,7 @@
         <v>44551</v>
       </c>
       <c r="G157" s="43">
-        <v>44556</v>
+        <v>44561</v>
       </c>
       <c r="H157" s="73"/>
       <c r="I157" s="26">
@@ -16524,14 +16527,14 @@
     <row r="158" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="B158" s="65" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D158" s="70"/>
       <c r="E158" s="66" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F158" s="42">
         <v>44551</v>
@@ -16605,10 +16608,10 @@
     <row r="159" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="B159" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D159" s="70"/>
       <c r="E159" s="66" t="s">
@@ -16686,10 +16689,10 @@
     <row r="160" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="B160" s="65" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D160" s="70"/>
       <c r="E160" s="66" t="s">
@@ -16767,23 +16770,23 @@
     <row r="161" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="B161" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D161" s="70"/>
-      <c r="E161" s="70" t="s">
+      <c r="E161" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="F161" s="71">
+      <c r="F161" s="42">
         <v>44551</v>
       </c>
-      <c r="G161" s="72">
+      <c r="G161" s="43">
         <v>44556</v>
       </c>
       <c r="H161" s="73"/>
-      <c r="I161" s="74">
+      <c r="I161" s="26">
         <v>0</v>
       </c>
       <c r="J161" s="75"/>
@@ -16848,27 +16851,27 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="B162" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="D162" s="66"/>
-      <c r="E162" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="D162" s="70"/>
+      <c r="E162" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="F162" s="42">
+      <c r="F162" s="71">
         <v>44551</v>
       </c>
-      <c r="G162" s="43">
+      <c r="G162" s="72">
         <v>44556</v>
       </c>
-      <c r="H162" s="25"/>
-      <c r="I162" s="26">
+      <c r="H162" s="73"/>
+      <c r="I162" s="74">
         <v>0</v>
       </c>
-      <c r="J162" s="27"/>
-      <c r="K162" s="40"/>
+      <c r="J162" s="75"/>
+      <c r="K162" s="76"/>
       <c r="L162" s="46"/>
       <c r="M162" s="46"/>
       <c r="N162" s="46"/>
@@ -16927,14 +16930,27 @@
       <c r="BO162" s="46"/>
     </row>
     <row r="163" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A163" s="23"/>
-      <c r="B163" s="65"/>
+      <c r="A163" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>0.9</v>
+      </c>
+      <c r="B163" s="65" t="s">
+        <v>155</v>
+      </c>
       <c r="D163" s="66"/>
-      <c r="E163" s="66"/>
-      <c r="F163" s="42"/>
-      <c r="G163" s="43"/>
+      <c r="E163" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F163" s="42">
+        <v>44551</v>
+      </c>
+      <c r="G163" s="43">
+        <v>44556</v>
+      </c>
       <c r="H163" s="25"/>
-      <c r="I163" s="26"/>
+      <c r="I163" s="26">
+        <v>0</v>
+      </c>
       <c r="J163" s="27"/>
       <c r="K163" s="40"/>
       <c r="L163" s="46"/>
@@ -17065,7 +17081,7 @@
     <row r="165" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="23"/>
       <c r="B165" s="65"/>
-      <c r="D165" s="70"/>
+      <c r="D165" s="66"/>
       <c r="E165" s="66"/>
       <c r="F165" s="42"/>
       <c r="G165" s="43"/>
@@ -17405,7 +17421,7 @@
     <row r="170" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="23"/>
       <c r="B170" s="65"/>
-      <c r="D170" s="66"/>
+      <c r="D170" s="70"/>
       <c r="E170" s="66"/>
       <c r="F170" s="42"/>
       <c r="G170" s="43"/>
@@ -17677,7 +17693,7 @@
     <row r="174" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="23"/>
       <c r="B174" s="65"/>
-      <c r="D174" s="70"/>
+      <c r="D174" s="66"/>
       <c r="E174" s="66"/>
       <c r="F174" s="42"/>
       <c r="G174" s="43"/>
@@ -18017,7 +18033,7 @@
     <row r="179" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="23"/>
       <c r="B179" s="65"/>
-      <c r="D179" s="66"/>
+      <c r="D179" s="70"/>
       <c r="E179" s="66"/>
       <c r="F179" s="42"/>
       <c r="G179" s="43"/>
@@ -18289,7 +18305,7 @@
     <row r="183" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="23"/>
       <c r="B183" s="65"/>
-      <c r="D183" s="70"/>
+      <c r="D183" s="66"/>
       <c r="E183" s="66"/>
       <c r="F183" s="42"/>
       <c r="G183" s="43"/>
@@ -18629,7 +18645,7 @@
     <row r="188" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="23"/>
       <c r="B188" s="65"/>
-      <c r="D188" s="66"/>
+      <c r="D188" s="70"/>
       <c r="E188" s="66"/>
       <c r="F188" s="42"/>
       <c r="G188" s="43"/>
@@ -18901,7 +18917,7 @@
     <row r="192" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A192" s="23"/>
       <c r="B192" s="65"/>
-      <c r="D192" s="70"/>
+      <c r="D192" s="66"/>
       <c r="E192" s="66"/>
       <c r="F192" s="42"/>
       <c r="G192" s="43"/>
@@ -19238,18 +19254,77 @@
       <c r="BN196" s="46"/>
       <c r="BO196" s="46"/>
     </row>
+    <row r="197" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="23"/>
+      <c r="B197" s="65"/>
+      <c r="D197" s="70"/>
+      <c r="E197" s="66"/>
+      <c r="F197" s="42"/>
+      <c r="G197" s="43"/>
+      <c r="H197" s="25"/>
+      <c r="I197" s="26"/>
+      <c r="J197" s="27"/>
+      <c r="K197" s="40"/>
+      <c r="L197" s="46"/>
+      <c r="M197" s="46"/>
+      <c r="N197" s="46"/>
+      <c r="O197" s="46"/>
+      <c r="P197" s="46"/>
+      <c r="Q197" s="46"/>
+      <c r="R197" s="46"/>
+      <c r="S197" s="46"/>
+      <c r="T197" s="46"/>
+      <c r="U197" s="46"/>
+      <c r="V197" s="46"/>
+      <c r="W197" s="46"/>
+      <c r="X197" s="46"/>
+      <c r="Y197" s="46"/>
+      <c r="Z197" s="46"/>
+      <c r="AA197" s="46"/>
+      <c r="AB197" s="46"/>
+      <c r="AC197" s="46"/>
+      <c r="AD197" s="46"/>
+      <c r="AE197" s="46"/>
+      <c r="AF197" s="46"/>
+      <c r="AG197" s="46"/>
+      <c r="AH197" s="46"/>
+      <c r="AI197" s="46"/>
+      <c r="AJ197" s="46"/>
+      <c r="AK197" s="46"/>
+      <c r="AL197" s="46"/>
+      <c r="AM197" s="46"/>
+      <c r="AN197" s="46"/>
+      <c r="AO197" s="46"/>
+      <c r="AP197" s="46"/>
+      <c r="AQ197" s="46"/>
+      <c r="AR197" s="46"/>
+      <c r="AS197" s="46"/>
+      <c r="AT197" s="46"/>
+      <c r="AU197" s="46"/>
+      <c r="AV197" s="46"/>
+      <c r="AW197" s="46"/>
+      <c r="AX197" s="46"/>
+      <c r="AY197" s="46"/>
+      <c r="AZ197" s="46"/>
+      <c r="BA197" s="46"/>
+      <c r="BB197" s="46"/>
+      <c r="BC197" s="46"/>
+      <c r="BD197" s="46"/>
+      <c r="BE197" s="46"/>
+      <c r="BF197" s="46"/>
+      <c r="BG197" s="46"/>
+      <c r="BH197" s="46"/>
+      <c r="BI197" s="46"/>
+      <c r="BJ197" s="46"/>
+      <c r="BK197" s="46"/>
+      <c r="BL197" s="46"/>
+      <c r="BM197" s="46"/>
+      <c r="BN197" s="46"/>
+      <c r="BO197" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -19260,9 +19335,18 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I169">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I170">
     <cfRule type="dataBar" priority="269">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19281,7 +19365,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN131 M133:BN136 L162:BO163 M164:BN169 BO167:BO169 L170:BO172 M173:BN178 BO176:BO178 L179:BO181 M182:BN187 BO185:BO187 L188:BO190 M191:BN196 BO194:BO196 M138:BN161">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN131 M133:BN136 L163:BO164 M165:BN170 BO168:BO170 L171:BO173 M174:BN179 BO177:BO179 L180:BO182 M183:BN188 BO186:BO188 L189:BO191 M192:BN197 BO195:BO197 M138:BN162">
     <cfRule type="expression" dxfId="136" priority="315">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -19289,7 +19373,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO169">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO170">
     <cfRule type="expression" dxfId="134" priority="275">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -19299,7 +19383,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E197:E1048576 E95:E96 E98:E103 E105:E110 E112:E122 E124:E131 E133:E136 E138:E169">
+  <conditionalFormatting sqref="E1:E73 E198:E1048576 E95:E96 E98:E103 E105:E110 E112:E122 E124:E131 E133:E136 E138:E170">
     <cfRule type="cellIs" dxfId="132" priority="256" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19393,7 +19477,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L164:BO169 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO161">
+  <conditionalFormatting sqref="L165:BO170 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO162">
     <cfRule type="expression" dxfId="110" priority="163">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19401,7 +19485,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I170:I178">
+  <conditionalFormatting sqref="I171:I179">
     <cfRule type="dataBar" priority="147">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19415,12 +19499,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L170:BO178">
+  <conditionalFormatting sqref="L171:BO179">
     <cfRule type="expression" dxfId="108" priority="146">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E170:E178">
+  <conditionalFormatting sqref="E171:E179">
     <cfRule type="cellIs" dxfId="107" priority="139" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19443,7 +19527,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L173:BO178">
+  <conditionalFormatting sqref="L174:BO179">
     <cfRule type="expression" dxfId="100" priority="150">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19451,7 +19535,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I179:I187">
+  <conditionalFormatting sqref="I180:I188">
     <cfRule type="dataBar" priority="134">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19465,12 +19549,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L179:BO187">
+  <conditionalFormatting sqref="L180:BO188">
     <cfRule type="expression" dxfId="98" priority="133">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E179:E187">
+  <conditionalFormatting sqref="E180:E188">
     <cfRule type="cellIs" dxfId="97" priority="126" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19493,7 +19577,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L182:BO187">
+  <conditionalFormatting sqref="L183:BO188">
     <cfRule type="expression" dxfId="90" priority="137">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19501,7 +19585,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I188:I196">
+  <conditionalFormatting sqref="I189:I197">
     <cfRule type="dataBar" priority="121">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19515,12 +19599,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L188:BO196">
+  <conditionalFormatting sqref="L189:BO197">
     <cfRule type="expression" dxfId="88" priority="120">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E188:E196">
+  <conditionalFormatting sqref="E189:E197">
     <cfRule type="cellIs" dxfId="87" priority="113" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19543,7 +19627,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L191:BO196">
+  <conditionalFormatting sqref="L192:BO197">
     <cfRule type="expression" dxfId="80" priority="124">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19991,7 +20075,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I169</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I170</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -20021,7 +20105,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I170:I178</xm:sqref>
+          <xm:sqref>I171:I179</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -20036,7 +20120,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I179:I187</xm:sqref>
+          <xm:sqref>I180:I188</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -20051,7 +20135,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I188:I196</xm:sqref>
+          <xm:sqref>I189:I197</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">

</xml_diff>

<commit_message>
Added BSBY forecasts (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDF095B-2C5A-4E59-B3BF-CE3454F7B3E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE240E17-E04C-4615-9370-FC567221016F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -428,7 +428,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="180">
   <si>
     <t>WBS</t>
   </si>
@@ -965,6 +965,9 @@
   </si>
   <si>
     <t>Add BSBY Forecasts</t>
+  </si>
+  <si>
+    <t>Add Inflation Forecasts</t>
   </si>
 </sst>
 </file>
@@ -1883,13 +1886,6 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1899,10 +1895,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1911,6 +1903,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3499,11 +3502,11 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO197"/>
+  <dimension ref="A1:BO198"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I147" sqref="I147"/>
+      <selection pane="bottomLeft" activeCell="I148" sqref="I148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3533,27 +3536,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3598,12 +3601,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="85">
         <v>44192</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3613,183 +3616,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="79" t="str">
+      <c r="L4" s="77" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="79" t="str">
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="77" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="79" t="str">
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="77" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="81"/>
-      <c r="AG4" s="79" t="str">
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
+      <c r="AE4" s="78"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="77" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="80"/>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="81"/>
-      <c r="AN4" s="79" t="str">
+      <c r="AH4" s="78"/>
+      <c r="AI4" s="78"/>
+      <c r="AJ4" s="78"/>
+      <c r="AK4" s="78"/>
+      <c r="AL4" s="78"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="77" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 57</v>
       </c>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="80"/>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="81"/>
-      <c r="AU4" s="79" t="str">
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="78"/>
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="77" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 58</v>
       </c>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="80"/>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="81"/>
-      <c r="BB4" s="79" t="str">
+      <c r="AV4" s="78"/>
+      <c r="AW4" s="78"/>
+      <c r="AX4" s="78"/>
+      <c r="AY4" s="78"/>
+      <c r="AZ4" s="78"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="77" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 59</v>
       </c>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="80"/>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="81"/>
-      <c r="BI4" s="79" t="str">
+      <c r="BC4" s="78"/>
+      <c r="BD4" s="78"/>
+      <c r="BE4" s="78"/>
+      <c r="BF4" s="78"/>
+      <c r="BG4" s="78"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="77" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 60</v>
       </c>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="80"/>
-      <c r="BM4" s="80"/>
-      <c r="BN4" s="80"/>
-      <c r="BO4" s="81"/>
+      <c r="BJ4" s="78"/>
+      <c r="BK4" s="78"/>
+      <c r="BL4" s="78"/>
+      <c r="BM4" s="78"/>
+      <c r="BN4" s="78"/>
+      <c r="BO4" s="79"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="83">
+      <c r="L5" s="80">
         <f>L6</f>
         <v>44557</v>
       </c>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="83">
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="80">
         <f>S6</f>
         <v>44564</v>
       </c>
-      <c r="T5" s="84"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="85"/>
-      <c r="Z5" s="83">
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="80">
         <f>Z6</f>
         <v>44571</v>
       </c>
-      <c r="AA5" s="84"/>
-      <c r="AB5" s="84"/>
-      <c r="AC5" s="84"/>
-      <c r="AD5" s="84"/>
-      <c r="AE5" s="84"/>
-      <c r="AF5" s="85"/>
-      <c r="AG5" s="83">
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="82"/>
+      <c r="AG5" s="80">
         <f>AG6</f>
         <v>44578</v>
       </c>
-      <c r="AH5" s="84"/>
-      <c r="AI5" s="84"/>
-      <c r="AJ5" s="84"/>
-      <c r="AK5" s="84"/>
-      <c r="AL5" s="84"/>
-      <c r="AM5" s="85"/>
-      <c r="AN5" s="83">
+      <c r="AH5" s="81"/>
+      <c r="AI5" s="81"/>
+      <c r="AJ5" s="81"/>
+      <c r="AK5" s="81"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="82"/>
+      <c r="AN5" s="80">
         <f>AN6</f>
         <v>44585</v>
       </c>
-      <c r="AO5" s="84"/>
-      <c r="AP5" s="84"/>
-      <c r="AQ5" s="84"/>
-      <c r="AR5" s="84"/>
-      <c r="AS5" s="84"/>
-      <c r="AT5" s="85"/>
-      <c r="AU5" s="83">
+      <c r="AO5" s="81"/>
+      <c r="AP5" s="81"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="81"/>
+      <c r="AS5" s="81"/>
+      <c r="AT5" s="82"/>
+      <c r="AU5" s="80">
         <f>AU6</f>
         <v>44592</v>
       </c>
-      <c r="AV5" s="84"/>
-      <c r="AW5" s="84"/>
-      <c r="AX5" s="84"/>
-      <c r="AY5" s="84"/>
-      <c r="AZ5" s="84"/>
-      <c r="BA5" s="85"/>
-      <c r="BB5" s="83">
+      <c r="AV5" s="81"/>
+      <c r="AW5" s="81"/>
+      <c r="AX5" s="81"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="81"/>
+      <c r="BA5" s="82"/>
+      <c r="BB5" s="80">
         <f>BB6</f>
         <v>44599</v>
       </c>
-      <c r="BC5" s="84"/>
-      <c r="BD5" s="84"/>
-      <c r="BE5" s="84"/>
-      <c r="BF5" s="84"/>
-      <c r="BG5" s="84"/>
-      <c r="BH5" s="85"/>
-      <c r="BI5" s="83">
+      <c r="BC5" s="81"/>
+      <c r="BD5" s="81"/>
+      <c r="BE5" s="81"/>
+      <c r="BF5" s="81"/>
+      <c r="BG5" s="81"/>
+      <c r="BH5" s="82"/>
+      <c r="BI5" s="80">
         <f>BI6</f>
         <v>44606</v>
       </c>
-      <c r="BJ5" s="84"/>
-      <c r="BK5" s="84"/>
-      <c r="BL5" s="84"/>
-      <c r="BM5" s="84"/>
-      <c r="BN5" s="84"/>
-      <c r="BO5" s="85"/>
+      <c r="BJ5" s="81"/>
+      <c r="BK5" s="81"/>
+      <c r="BL5" s="81"/>
+      <c r="BM5" s="81"/>
+      <c r="BN5" s="81"/>
+      <c r="BO5" s="82"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -8947,7 +8950,7 @@
     </row>
     <row r="64" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="23" t="str">
-        <f t="shared" ref="A64:A163" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A64:A164" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>5.1</v>
       </c>
       <c r="B64" s="65" t="s">
@@ -15624,7 +15627,7 @@
       </c>
       <c r="H146" s="73"/>
       <c r="I146" s="26">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="J146" s="75"/>
       <c r="K146" s="76"/>
@@ -15691,14 +15694,14 @@
         <v>14.10</v>
       </c>
       <c r="B147" s="65" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="D147" s="70"/>
       <c r="E147" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F147" s="42">
-        <v>44559</v>
+        <v>44560</v>
       </c>
       <c r="G147" s="43">
         <v>44560</v>
@@ -15772,17 +15775,17 @@
         <v>14.11</v>
       </c>
       <c r="B148" s="65" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D148" s="70"/>
       <c r="E148" s="66" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F148" s="42">
         <v>44560</v>
       </c>
       <c r="G148" s="43">
-        <v>44563</v>
+        <v>44562</v>
       </c>
       <c r="H148" s="73"/>
       <c r="I148" s="26">
@@ -15853,14 +15856,14 @@
         <v>14.12</v>
       </c>
       <c r="B149" s="65" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D149" s="70"/>
       <c r="E149" s="66" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F149" s="42">
-        <v>44561</v>
+        <v>44562</v>
       </c>
       <c r="G149" s="43">
         <v>44564</v>
@@ -15934,17 +15937,17 @@
         <v>14.13</v>
       </c>
       <c r="B150" s="65" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D150" s="70"/>
       <c r="E150" s="66" t="s">
         <v>66</v>
       </c>
       <c r="F150" s="42">
-        <v>44561</v>
+        <v>44563</v>
       </c>
       <c r="G150" s="43">
-        <v>44564</v>
+        <v>44571</v>
       </c>
       <c r="H150" s="73"/>
       <c r="I150" s="26">
@@ -16010,14 +16013,27 @@
       <c r="BO150" s="46"/>
     </row>
     <row r="151" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A151" s="23"/>
-      <c r="B151" s="65"/>
+      <c r="A151" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>14.14</v>
+      </c>
+      <c r="B151" s="65" t="s">
+        <v>168</v>
+      </c>
       <c r="D151" s="70"/>
-      <c r="E151" s="66"/>
-      <c r="F151" s="42"/>
-      <c r="G151" s="43"/>
+      <c r="E151" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F151" s="42">
+        <v>44563</v>
+      </c>
+      <c r="G151" s="43">
+        <v>44571</v>
+      </c>
       <c r="H151" s="73"/>
-      <c r="I151" s="26"/>
+      <c r="I151" s="26">
+        <v>0</v>
+      </c>
       <c r="J151" s="75"/>
       <c r="K151" s="76"/>
       <c r="L151" s="46"/>
@@ -16282,27 +16298,14 @@
       <c r="BO154" s="46"/>
     </row>
     <row r="155" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="23" t="str">
-        <f t="shared" si="9"/>
-        <v>0.1</v>
-      </c>
-      <c r="B155" s="65" t="s">
-        <v>150</v>
-      </c>
+      <c r="A155" s="23"/>
+      <c r="B155" s="65"/>
       <c r="D155" s="70"/>
-      <c r="E155" s="66" t="s">
-        <v>151</v>
-      </c>
-      <c r="F155" s="42">
-        <v>44557</v>
-      </c>
-      <c r="G155" s="43">
-        <v>44561</v>
-      </c>
+      <c r="E155" s="66"/>
+      <c r="F155" s="42"/>
+      <c r="G155" s="43"/>
       <c r="H155" s="73"/>
-      <c r="I155" s="26">
-        <v>0</v>
-      </c>
+      <c r="I155" s="26"/>
       <c r="J155" s="75"/>
       <c r="K155" s="76"/>
       <c r="L155" s="46"/>
@@ -16365,17 +16368,17 @@
     <row r="156" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="B156" s="65" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D156" s="70"/>
       <c r="E156" s="66" t="s">
-        <v>68</v>
+        <v>151</v>
       </c>
       <c r="F156" s="42">
-        <v>44561</v>
+        <v>44557</v>
       </c>
       <c r="G156" s="43">
         <v>44561</v>
@@ -16446,17 +16449,17 @@
     <row r="157" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="B157" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D157" s="70"/>
       <c r="E157" s="66" t="s">
         <v>68</v>
       </c>
       <c r="F157" s="42">
-        <v>44551</v>
+        <v>44561</v>
       </c>
       <c r="G157" s="43">
         <v>44561</v>
@@ -16527,10 +16530,10 @@
     <row r="158" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="B158" s="65" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D158" s="70"/>
       <c r="E158" s="66" t="s">
@@ -16540,7 +16543,7 @@
         <v>44551</v>
       </c>
       <c r="G158" s="43">
-        <v>44556</v>
+        <v>44561</v>
       </c>
       <c r="H158" s="73"/>
       <c r="I158" s="26">
@@ -16608,14 +16611,14 @@
     <row r="159" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="B159" s="65" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D159" s="70"/>
       <c r="E159" s="66" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F159" s="42">
         <v>44551</v>
@@ -16689,10 +16692,10 @@
     <row r="160" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="B160" s="65" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D160" s="70"/>
       <c r="E160" s="66" t="s">
@@ -16770,10 +16773,10 @@
     <row r="161" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="B161" s="65" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="D161" s="70"/>
       <c r="E161" s="66" t="s">
@@ -16851,23 +16854,23 @@
     <row r="162" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="B162" s="65" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D162" s="70"/>
-      <c r="E162" s="70" t="s">
+      <c r="E162" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="F162" s="71">
+      <c r="F162" s="42">
         <v>44551</v>
       </c>
-      <c r="G162" s="72">
+      <c r="G162" s="43">
         <v>44556</v>
       </c>
       <c r="H162" s="73"/>
-      <c r="I162" s="74">
+      <c r="I162" s="26">
         <v>0</v>
       </c>
       <c r="J162" s="75"/>
@@ -16932,27 +16935,27 @@
     <row r="163" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="23" t="str">
         <f t="shared" si="9"/>
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="B163" s="65" t="s">
-        <v>155</v>
-      </c>
-      <c r="D163" s="66"/>
-      <c r="E163" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="D163" s="70"/>
+      <c r="E163" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="F163" s="42">
+      <c r="F163" s="71">
         <v>44551</v>
       </c>
-      <c r="G163" s="43">
+      <c r="G163" s="72">
         <v>44556</v>
       </c>
-      <c r="H163" s="25"/>
-      <c r="I163" s="26">
+      <c r="H163" s="73"/>
+      <c r="I163" s="74">
         <v>0</v>
       </c>
-      <c r="J163" s="27"/>
-      <c r="K163" s="40"/>
+      <c r="J163" s="75"/>
+      <c r="K163" s="76"/>
       <c r="L163" s="46"/>
       <c r="M163" s="46"/>
       <c r="N163" s="46"/>
@@ -17011,14 +17014,27 @@
       <c r="BO163" s="46"/>
     </row>
     <row r="164" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A164" s="23"/>
-      <c r="B164" s="65"/>
+      <c r="A164" s="23" t="str">
+        <f t="shared" si="9"/>
+        <v>0.9</v>
+      </c>
+      <c r="B164" s="65" t="s">
+        <v>155</v>
+      </c>
       <c r="D164" s="66"/>
-      <c r="E164" s="66"/>
-      <c r="F164" s="42"/>
-      <c r="G164" s="43"/>
+      <c r="E164" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="F164" s="42">
+        <v>44551</v>
+      </c>
+      <c r="G164" s="43">
+        <v>44556</v>
+      </c>
       <c r="H164" s="25"/>
-      <c r="I164" s="26"/>
+      <c r="I164" s="26">
+        <v>0</v>
+      </c>
       <c r="J164" s="27"/>
       <c r="K164" s="40"/>
       <c r="L164" s="46"/>
@@ -17149,7 +17165,7 @@
     <row r="166" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="23"/>
       <c r="B166" s="65"/>
-      <c r="D166" s="70"/>
+      <c r="D166" s="66"/>
       <c r="E166" s="66"/>
       <c r="F166" s="42"/>
       <c r="G166" s="43"/>
@@ -17489,7 +17505,7 @@
     <row r="171" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="23"/>
       <c r="B171" s="65"/>
-      <c r="D171" s="66"/>
+      <c r="D171" s="70"/>
       <c r="E171" s="66"/>
       <c r="F171" s="42"/>
       <c r="G171" s="43"/>
@@ -17761,7 +17777,7 @@
     <row r="175" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="23"/>
       <c r="B175" s="65"/>
-      <c r="D175" s="70"/>
+      <c r="D175" s="66"/>
       <c r="E175" s="66"/>
       <c r="F175" s="42"/>
       <c r="G175" s="43"/>
@@ -18101,7 +18117,7 @@
     <row r="180" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A180" s="23"/>
       <c r="B180" s="65"/>
-      <c r="D180" s="66"/>
+      <c r="D180" s="70"/>
       <c r="E180" s="66"/>
       <c r="F180" s="42"/>
       <c r="G180" s="43"/>
@@ -18373,7 +18389,7 @@
     <row r="184" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="23"/>
       <c r="B184" s="65"/>
-      <c r="D184" s="70"/>
+      <c r="D184" s="66"/>
       <c r="E184" s="66"/>
       <c r="F184" s="42"/>
       <c r="G184" s="43"/>
@@ -18713,7 +18729,7 @@
     <row r="189" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="23"/>
       <c r="B189" s="65"/>
-      <c r="D189" s="66"/>
+      <c r="D189" s="70"/>
       <c r="E189" s="66"/>
       <c r="F189" s="42"/>
       <c r="G189" s="43"/>
@@ -18985,7 +19001,7 @@
     <row r="193" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="23"/>
       <c r="B193" s="65"/>
-      <c r="D193" s="70"/>
+      <c r="D193" s="66"/>
       <c r="E193" s="66"/>
       <c r="F193" s="42"/>
       <c r="G193" s="43"/>
@@ -19322,9 +19338,86 @@
       <c r="BN197" s="46"/>
       <c r="BO197" s="46"/>
     </row>
+    <row r="198" spans="1:67" s="24" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="23"/>
+      <c r="B198" s="65"/>
+      <c r="D198" s="70"/>
+      <c r="E198" s="66"/>
+      <c r="F198" s="42"/>
+      <c r="G198" s="43"/>
+      <c r="H198" s="25"/>
+      <c r="I198" s="26"/>
+      <c r="J198" s="27"/>
+      <c r="K198" s="40"/>
+      <c r="L198" s="46"/>
+      <c r="M198" s="46"/>
+      <c r="N198" s="46"/>
+      <c r="O198" s="46"/>
+      <c r="P198" s="46"/>
+      <c r="Q198" s="46"/>
+      <c r="R198" s="46"/>
+      <c r="S198" s="46"/>
+      <c r="T198" s="46"/>
+      <c r="U198" s="46"/>
+      <c r="V198" s="46"/>
+      <c r="W198" s="46"/>
+      <c r="X198" s="46"/>
+      <c r="Y198" s="46"/>
+      <c r="Z198" s="46"/>
+      <c r="AA198" s="46"/>
+      <c r="AB198" s="46"/>
+      <c r="AC198" s="46"/>
+      <c r="AD198" s="46"/>
+      <c r="AE198" s="46"/>
+      <c r="AF198" s="46"/>
+      <c r="AG198" s="46"/>
+      <c r="AH198" s="46"/>
+      <c r="AI198" s="46"/>
+      <c r="AJ198" s="46"/>
+      <c r="AK198" s="46"/>
+      <c r="AL198" s="46"/>
+      <c r="AM198" s="46"/>
+      <c r="AN198" s="46"/>
+      <c r="AO198" s="46"/>
+      <c r="AP198" s="46"/>
+      <c r="AQ198" s="46"/>
+      <c r="AR198" s="46"/>
+      <c r="AS198" s="46"/>
+      <c r="AT198" s="46"/>
+      <c r="AU198" s="46"/>
+      <c r="AV198" s="46"/>
+      <c r="AW198" s="46"/>
+      <c r="AX198" s="46"/>
+      <c r="AY198" s="46"/>
+      <c r="AZ198" s="46"/>
+      <c r="BA198" s="46"/>
+      <c r="BB198" s="46"/>
+      <c r="BC198" s="46"/>
+      <c r="BD198" s="46"/>
+      <c r="BE198" s="46"/>
+      <c r="BF198" s="46"/>
+      <c r="BG198" s="46"/>
+      <c r="BH198" s="46"/>
+      <c r="BI198" s="46"/>
+      <c r="BJ198" s="46"/>
+      <c r="BK198" s="46"/>
+      <c r="BL198" s="46"/>
+      <c r="BM198" s="46"/>
+      <c r="BN198" s="46"/>
+      <c r="BO198" s="46"/>
+    </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -19335,18 +19428,9 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I170">
+  <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I171">
     <cfRule type="dataBar" priority="269">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19365,7 +19449,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN131 M133:BN136 L163:BO164 M165:BN170 BO168:BO170 L171:BO173 M174:BN179 BO177:BO179 L180:BO182 M183:BN188 BO186:BO188 L189:BO191 M192:BN197 BO195:BO197 M138:BN162">
+  <conditionalFormatting sqref="L8:BO67 M68:BN73 R71:BO73 M79:BN84 BO82:BO84 L85:BO86 L95:BO96 M98:BN103 M105:BN110 M112:BN122 L123:BO123 M124:BN131 M133:BN136 L164:BO165 M166:BN171 BO169:BO171 L172:BO174 M175:BN180 BO178:BO180 L181:BO183 M184:BN189 BO187:BO189 L190:BO192 M193:BN198 BO196:BO198 M138:BN163">
     <cfRule type="expression" dxfId="136" priority="315">
       <formula>AND($F8&lt;=L$6,ROUNDDOWN(($G8-$F8+1)*$I8,0)+$F8-1&gt;=L$6)</formula>
     </cfRule>
@@ -19373,7 +19457,7 @@
       <formula>AND(NOT(ISBLANK($F8)),$F8&lt;=L$6,$G8&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO170">
+  <conditionalFormatting sqref="L6:BO62 L95:BO96 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO171">
     <cfRule type="expression" dxfId="134" priority="275">
       <formula>L$6=TODAY()</formula>
     </cfRule>
@@ -19383,7 +19467,7 @@
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:E73 E198:E1048576 E95:E96 E98:E103 E105:E110 E112:E122 E124:E131 E133:E136 E138:E170">
+  <conditionalFormatting sqref="E1:E73 E199:E1048576 E95:E96 E98:E103 E105:E110 E112:E122 E124:E131 E133:E136 E138:E171">
     <cfRule type="cellIs" dxfId="132" priority="256" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19477,7 +19561,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L165:BO170 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO162">
+  <conditionalFormatting sqref="L166:BO171 L98:BO103 L105:BO110 L112:BO122 L124:BO131 L133:BO136 L138:BO163">
     <cfRule type="expression" dxfId="110" priority="163">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19485,7 +19569,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I171:I179">
+  <conditionalFormatting sqref="I172:I180">
     <cfRule type="dataBar" priority="147">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19499,12 +19583,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L171:BO179">
+  <conditionalFormatting sqref="L172:BO180">
     <cfRule type="expression" dxfId="108" priority="146">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E171:E179">
+  <conditionalFormatting sqref="E172:E180">
     <cfRule type="cellIs" dxfId="107" priority="139" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19527,7 +19611,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L174:BO179">
+  <conditionalFormatting sqref="L175:BO180">
     <cfRule type="expression" dxfId="100" priority="150">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19535,7 +19619,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I180:I188">
+  <conditionalFormatting sqref="I181:I189">
     <cfRule type="dataBar" priority="134">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19549,12 +19633,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L180:BO188">
+  <conditionalFormatting sqref="L181:BO189">
     <cfRule type="expression" dxfId="98" priority="133">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E180:E188">
+  <conditionalFormatting sqref="E181:E189">
     <cfRule type="cellIs" dxfId="97" priority="126" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19577,7 +19661,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L183:BO188">
+  <conditionalFormatting sqref="L184:BO189">
     <cfRule type="expression" dxfId="90" priority="137">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -19585,7 +19669,7 @@
       <formula>AND(NOT(ISBLANK(#REF!)),#REF!&lt;=L$6,#REF!&gt;=L$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I189:I197">
+  <conditionalFormatting sqref="I190:I198">
     <cfRule type="dataBar" priority="121">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -19599,12 +19683,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L189:BO197">
+  <conditionalFormatting sqref="L190:BO198">
     <cfRule type="expression" dxfId="88" priority="120">
       <formula>L$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E189:E197">
+  <conditionalFormatting sqref="E190:E198">
     <cfRule type="cellIs" dxfId="87" priority="113" operator="equal">
       <formula>"LINUX"</formula>
     </cfRule>
@@ -19627,7 +19711,7 @@
       <formula>"JS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L192:BO197">
+  <conditionalFormatting sqref="L193:BO198">
     <cfRule type="expression" dxfId="80" priority="124">
       <formula>AND(#REF!&lt;=L$6,ROUNDDOWN((#REF!-#REF!+1)*#REF!,0)+#REF!-1&gt;=L$6)</formula>
     </cfRule>
@@ -20075,7 +20159,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I170</xm:sqref>
+          <xm:sqref>I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I171</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{BFFF36CC-68C1-40BD-B8E2-86AEDBB6FF36}">
@@ -20105,7 +20189,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I171:I179</xm:sqref>
+          <xm:sqref>I172:I180</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6615FE7E-0BE8-4AD8-A679-1083F0182AAC}">
@@ -20120,7 +20204,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I180:I188</xm:sqref>
+          <xm:sqref>I181:I189</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C53AC685-AE5A-453B-B781-EF3C7745AAB5}">
@@ -20135,7 +20219,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>I189:I197</xm:sqref>
+          <xm:sqref>I190:I198</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{09CDF19A-9118-4777-8CA8-000A1FFBD033}">

</xml_diff>

<commit_message>
Fixed Bloomberg rates parsing issue (v0.19)
</commit_message>
<xml_diff>
--- a/ECONFORECASTING PM.xlsx
+++ b/ECONFORECASTING PM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3207AFDA-5ABB-4422-8F59-71B751FD08F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB08D537-C8B2-49B3-B1BA-858C2A1D6397}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1859,13 +1859,6 @@
     <xf numFmtId="1" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1875,10 +1868,6 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1887,6 +1876,17 @@
     </xf>
     <xf numFmtId="167" fontId="33" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -3479,7 +3479,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B140" sqref="B140"/>
+      <selection pane="bottomLeft" activeCell="U160" sqref="U160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3509,27 +3509,27 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="J1" s="68"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
-      <c r="X1" s="77"/>
-      <c r="Y1" s="77"/>
-      <c r="Z1" s="77"/>
-      <c r="AA1" s="77"/>
-      <c r="AB1" s="77"/>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="77"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
+      <c r="S1" s="83"/>
+      <c r="T1" s="83"/>
+      <c r="U1" s="83"/>
+      <c r="V1" s="83"/>
+      <c r="W1" s="83"/>
+      <c r="X1" s="83"/>
+      <c r="Y1" s="83"/>
+      <c r="Z1" s="83"/>
+      <c r="AA1" s="83"/>
+      <c r="AB1" s="83"/>
+      <c r="AC1" s="83"/>
+      <c r="AD1" s="83"/>
+      <c r="AE1" s="83"/>
+      <c r="AF1" s="83"/>
     </row>
     <row r="2" spans="1:67" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15"/>
@@ -3574,12 +3574,12 @@
       <c r="B4" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="82">
+      <c r="C4" s="85">
         <v>44192</v>
       </c>
-      <c r="D4" s="82"/>
-      <c r="E4" s="82"/>
-      <c r="F4" s="82"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
       <c r="G4" s="50"/>
       <c r="H4" s="53" t="s">
         <v>10</v>
@@ -3589,183 +3589,183 @@
       </c>
       <c r="J4" s="51"/>
       <c r="K4" s="13"/>
-      <c r="L4" s="79" t="str">
+      <c r="L4" s="77" t="str">
         <f>"Week "&amp;(L6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 53</v>
       </c>
-      <c r="M4" s="80"/>
-      <c r="N4" s="80"/>
-      <c r="O4" s="80"/>
-      <c r="P4" s="80"/>
-      <c r="Q4" s="80"/>
-      <c r="R4" s="81"/>
-      <c r="S4" s="79" t="str">
+      <c r="M4" s="78"/>
+      <c r="N4" s="78"/>
+      <c r="O4" s="78"/>
+      <c r="P4" s="78"/>
+      <c r="Q4" s="78"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="77" t="str">
         <f>"Week "&amp;(S6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 54</v>
       </c>
-      <c r="T4" s="80"/>
-      <c r="U4" s="80"/>
-      <c r="V4" s="80"/>
-      <c r="W4" s="80"/>
-      <c r="X4" s="80"/>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="79" t="str">
+      <c r="T4" s="78"/>
+      <c r="U4" s="78"/>
+      <c r="V4" s="78"/>
+      <c r="W4" s="78"/>
+      <c r="X4" s="78"/>
+      <c r="Y4" s="79"/>
+      <c r="Z4" s="77" t="str">
         <f>"Week "&amp;(Z6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 55</v>
       </c>
-      <c r="AA4" s="80"/>
-      <c r="AB4" s="80"/>
-      <c r="AC4" s="80"/>
-      <c r="AD4" s="80"/>
-      <c r="AE4" s="80"/>
-      <c r="AF4" s="81"/>
-      <c r="AG4" s="79" t="str">
+      <c r="AA4" s="78"/>
+      <c r="AB4" s="78"/>
+      <c r="AC4" s="78"/>
+      <c r="AD4" s="78"/>
+      <c r="AE4" s="78"/>
+      <c r="AF4" s="79"/>
+      <c r="AG4" s="77" t="str">
         <f>"Week "&amp;(AG6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 56</v>
       </c>
-      <c r="AH4" s="80"/>
-      <c r="AI4" s="80"/>
-      <c r="AJ4" s="80"/>
-      <c r="AK4" s="80"/>
-      <c r="AL4" s="80"/>
-      <c r="AM4" s="81"/>
-      <c r="AN4" s="79" t="str">
+      <c r="AH4" s="78"/>
+      <c r="AI4" s="78"/>
+      <c r="AJ4" s="78"/>
+      <c r="AK4" s="78"/>
+      <c r="AL4" s="78"/>
+      <c r="AM4" s="79"/>
+      <c r="AN4" s="77" t="str">
         <f>"Week "&amp;(AN6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 57</v>
       </c>
-      <c r="AO4" s="80"/>
-      <c r="AP4" s="80"/>
-      <c r="AQ4" s="80"/>
-      <c r="AR4" s="80"/>
-      <c r="AS4" s="80"/>
-      <c r="AT4" s="81"/>
-      <c r="AU4" s="79" t="str">
+      <c r="AO4" s="78"/>
+      <c r="AP4" s="78"/>
+      <c r="AQ4" s="78"/>
+      <c r="AR4" s="78"/>
+      <c r="AS4" s="78"/>
+      <c r="AT4" s="79"/>
+      <c r="AU4" s="77" t="str">
         <f>"Week "&amp;(AU6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 58</v>
       </c>
-      <c r="AV4" s="80"/>
-      <c r="AW4" s="80"/>
-      <c r="AX4" s="80"/>
-      <c r="AY4" s="80"/>
-      <c r="AZ4" s="80"/>
-      <c r="BA4" s="81"/>
-      <c r="BB4" s="79" t="str">
+      <c r="AV4" s="78"/>
+      <c r="AW4" s="78"/>
+      <c r="AX4" s="78"/>
+      <c r="AY4" s="78"/>
+      <c r="AZ4" s="78"/>
+      <c r="BA4" s="79"/>
+      <c r="BB4" s="77" t="str">
         <f>"Week "&amp;(BB6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 59</v>
       </c>
-      <c r="BC4" s="80"/>
-      <c r="BD4" s="80"/>
-      <c r="BE4" s="80"/>
-      <c r="BF4" s="80"/>
-      <c r="BG4" s="80"/>
-      <c r="BH4" s="81"/>
-      <c r="BI4" s="79" t="str">
+      <c r="BC4" s="78"/>
+      <c r="BD4" s="78"/>
+      <c r="BE4" s="78"/>
+      <c r="BF4" s="78"/>
+      <c r="BG4" s="78"/>
+      <c r="BH4" s="79"/>
+      <c r="BI4" s="77" t="str">
         <f>"Week "&amp;(BI6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 60</v>
       </c>
-      <c r="BJ4" s="80"/>
-      <c r="BK4" s="80"/>
-      <c r="BL4" s="80"/>
-      <c r="BM4" s="80"/>
-      <c r="BN4" s="80"/>
-      <c r="BO4" s="81"/>
+      <c r="BJ4" s="78"/>
+      <c r="BK4" s="78"/>
+      <c r="BL4" s="78"/>
+      <c r="BM4" s="78"/>
+      <c r="BN4" s="78"/>
+      <c r="BO4" s="79"/>
     </row>
     <row r="5" spans="1:67" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="49"/>
       <c r="B5" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="84" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="78"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
       <c r="G5" s="52"/>
       <c r="H5" s="52"/>
       <c r="I5" s="52"/>
       <c r="J5" s="52"/>
       <c r="K5" s="13"/>
-      <c r="L5" s="83">
+      <c r="L5" s="80">
         <f>L6</f>
         <v>44557</v>
       </c>
-      <c r="M5" s="84"/>
-      <c r="N5" s="84"/>
-      <c r="O5" s="84"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="84"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="83">
+      <c r="M5" s="81"/>
+      <c r="N5" s="81"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="80">
         <f>S6</f>
         <v>44564</v>
       </c>
-      <c r="T5" s="84"/>
-      <c r="U5" s="84"/>
-      <c r="V5" s="84"/>
-      <c r="W5" s="84"/>
-      <c r="X5" s="84"/>
-      <c r="Y5" s="85"/>
-      <c r="Z5" s="83">
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="81"/>
+      <c r="W5" s="81"/>
+      <c r="X5" s="81"/>
+      <c r="Y5" s="82"/>
+      <c r="Z5" s="80">
         <f>Z6</f>
         <v>44571</v>
       </c>
-      <c r="AA5" s="84"/>
-      <c r="AB5" s="84"/>
-      <c r="AC5" s="84"/>
-      <c r="AD5" s="84"/>
-      <c r="AE5" s="84"/>
-      <c r="AF5" s="85"/>
-      <c r="AG5" s="83">
+      <c r="AA5" s="81"/>
+      <c r="AB5" s="81"/>
+      <c r="AC5" s="81"/>
+      <c r="AD5" s="81"/>
+      <c r="AE5" s="81"/>
+      <c r="AF5" s="82"/>
+      <c r="AG5" s="80">
         <f>AG6</f>
         <v>44578</v>
       </c>
-      <c r="AH5" s="84"/>
-      <c r="AI5" s="84"/>
-      <c r="AJ5" s="84"/>
-      <c r="AK5" s="84"/>
-      <c r="AL5" s="84"/>
-      <c r="AM5" s="85"/>
-      <c r="AN5" s="83">
+      <c r="AH5" s="81"/>
+      <c r="AI5" s="81"/>
+      <c r="AJ5" s="81"/>
+      <c r="AK5" s="81"/>
+      <c r="AL5" s="81"/>
+      <c r="AM5" s="82"/>
+      <c r="AN5" s="80">
         <f>AN6</f>
         <v>44585</v>
       </c>
-      <c r="AO5" s="84"/>
-      <c r="AP5" s="84"/>
-      <c r="AQ5" s="84"/>
-      <c r="AR5" s="84"/>
-      <c r="AS5" s="84"/>
-      <c r="AT5" s="85"/>
-      <c r="AU5" s="83">
+      <c r="AO5" s="81"/>
+      <c r="AP5" s="81"/>
+      <c r="AQ5" s="81"/>
+      <c r="AR5" s="81"/>
+      <c r="AS5" s="81"/>
+      <c r="AT5" s="82"/>
+      <c r="AU5" s="80">
         <f>AU6</f>
         <v>44592</v>
       </c>
-      <c r="AV5" s="84"/>
-      <c r="AW5" s="84"/>
-      <c r="AX5" s="84"/>
-      <c r="AY5" s="84"/>
-      <c r="AZ5" s="84"/>
-      <c r="BA5" s="85"/>
-      <c r="BB5" s="83">
+      <c r="AV5" s="81"/>
+      <c r="AW5" s="81"/>
+      <c r="AX5" s="81"/>
+      <c r="AY5" s="81"/>
+      <c r="AZ5" s="81"/>
+      <c r="BA5" s="82"/>
+      <c r="BB5" s="80">
         <f>BB6</f>
         <v>44599</v>
       </c>
-      <c r="BC5" s="84"/>
-      <c r="BD5" s="84"/>
-      <c r="BE5" s="84"/>
-      <c r="BF5" s="84"/>
-      <c r="BG5" s="84"/>
-      <c r="BH5" s="85"/>
-      <c r="BI5" s="83">
+      <c r="BC5" s="81"/>
+      <c r="BD5" s="81"/>
+      <c r="BE5" s="81"/>
+      <c r="BF5" s="81"/>
+      <c r="BG5" s="81"/>
+      <c r="BH5" s="82"/>
+      <c r="BI5" s="80">
         <f>BI6</f>
         <v>44606</v>
       </c>
-      <c r="BJ5" s="84"/>
-      <c r="BK5" s="84"/>
-      <c r="BL5" s="84"/>
-      <c r="BM5" s="84"/>
-      <c r="BN5" s="84"/>
-      <c r="BO5" s="85"/>
+      <c r="BJ5" s="81"/>
+      <c r="BK5" s="81"/>
+      <c r="BL5" s="81"/>
+      <c r="BM5" s="81"/>
+      <c r="BN5" s="81"/>
+      <c r="BO5" s="82"/>
     </row>
     <row r="6" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
@@ -18653,6 +18653,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="L1:AF1"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="S4:Y4"/>
+    <mergeCell ref="L4:R4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="S5:Y5"/>
+    <mergeCell ref="L5:R5"/>
+    <mergeCell ref="Z4:AF4"/>
+    <mergeCell ref="Z5:AF5"/>
     <mergeCell ref="AG4:AM4"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="BI4:BO4"/>
@@ -18663,15 +18672,6 @@
     <mergeCell ref="AN4:AT4"/>
     <mergeCell ref="BB4:BH4"/>
     <mergeCell ref="BB5:BH5"/>
-    <mergeCell ref="L1:AF1"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="S4:Y4"/>
-    <mergeCell ref="L4:R4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="S5:Y5"/>
-    <mergeCell ref="L5:R5"/>
-    <mergeCell ref="Z4:AF4"/>
-    <mergeCell ref="Z5:AF5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="I8:I73 I95:I96 I98:I103 I105:I110 I112:I122 I124:I131 I133:I136 I138:I162">

</xml_diff>